<commit_message>
actualiza provincias 2020.08.19. Recupera NA del agregado por CCAA
</commit_message>
<xml_diff>
--- a/data/output/covid19-spain_consolidated.xlsx
+++ b/data/output/covid19-spain_consolidated.xlsx
@@ -1484,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G32" t="n">
         <v>12</v>
@@ -1519,7 +1519,7 @@
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G33" t="n">
         <v>12</v>
@@ -1554,7 +1554,7 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="G34" t="n">
         <v>13</v>
@@ -1589,7 +1589,7 @@
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="G35" t="n">
         <v>15</v>
@@ -1624,7 +1624,7 @@
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G36" t="n">
         <v>16</v>
@@ -1659,7 +1659,7 @@
         <v>8</v>
       </c>
       <c r="F37" t="n">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G37" t="n">
         <v>15</v>
@@ -1694,7 +1694,7 @@
         <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="G38" t="n">
         <v>16</v>
@@ -1729,7 +1729,7 @@
         <v>19</v>
       </c>
       <c r="F39" t="n">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G39" t="n">
         <v>18</v>
@@ -1764,7 +1764,7 @@
         <v>28</v>
       </c>
       <c r="F40" t="n">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="G40" t="n">
         <v>20</v>
@@ -1799,7 +1799,7 @@
         <v>33</v>
       </c>
       <c r="F41" t="n">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="G41" t="n">
         <v>26</v>
@@ -1834,7 +1834,7 @@
         <v>43</v>
       </c>
       <c r="F42" t="n">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="G42" t="n">
         <v>31</v>
@@ -1869,7 +1869,7 @@
         <v>54</v>
       </c>
       <c r="F43" t="n">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="G43" t="n">
         <v>37</v>
@@ -1904,7 +1904,7 @@
         <v>68</v>
       </c>
       <c r="F44" t="n">
-        <v>1873</v>
+        <v>1875</v>
       </c>
       <c r="G44" t="n">
         <v>218</v>
@@ -1939,7 +1939,7 @@
         <v>109</v>
       </c>
       <c r="F45" t="n">
-        <v>2167</v>
+        <v>2169</v>
       </c>
       <c r="G45" t="n">
         <v>229</v>
@@ -1974,7 +1974,7 @@
         <v>123</v>
       </c>
       <c r="F46" t="n">
-        <v>3047</v>
+        <v>3049</v>
       </c>
       <c r="G46" t="n">
         <v>317</v>
@@ -2009,7 +2009,7 @@
         <v>134</v>
       </c>
       <c r="F47" t="n">
-        <v>3180</v>
+        <v>3182</v>
       </c>
       <c r="G47" t="n">
         <v>345</v>
@@ -2044,7 +2044,7 @@
         <v>152</v>
       </c>
       <c r="F48" t="n">
-        <v>4780</v>
+        <v>4781</v>
       </c>
       <c r="G48" t="n">
         <v>481</v>
@@ -2056,7 +2056,7 @@
         <v>17583</v>
       </c>
       <c r="J48" t="n">
-        <v>14243</v>
+        <v>14244</v>
       </c>
       <c r="K48" t="n">
         <v>34</v>
@@ -2079,7 +2079,7 @@
         <v>168</v>
       </c>
       <c r="F49" t="n">
-        <v>5275</v>
+        <v>5276</v>
       </c>
       <c r="G49" t="n">
         <v>680</v>
@@ -2091,7 +2091,7 @@
         <v>20761</v>
       </c>
       <c r="J49" t="n">
-        <v>17323</v>
+        <v>17324</v>
       </c>
       <c r="K49" t="n">
         <v>43</v>
@@ -2114,7 +2114,7 @@
         <v>3103</v>
       </c>
       <c r="F50" t="n">
-        <v>6987</v>
+        <v>6988</v>
       </c>
       <c r="G50" t="n">
         <v>830</v>
@@ -2126,7 +2126,7 @@
         <v>26438</v>
       </c>
       <c r="J50" t="n">
-        <v>21077</v>
+        <v>21079</v>
       </c>
       <c r="K50" t="n">
         <v>121</v>
@@ -2140,7 +2140,7 @@
         <v>2285</v>
       </c>
       <c r="C51" t="n">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D51" t="n">
         <v>1</v>
@@ -2149,7 +2149,7 @@
         <v>3956</v>
       </c>
       <c r="F51" t="n">
-        <v>8573</v>
+        <v>8574</v>
       </c>
       <c r="G51" t="n">
         <v>976</v>
@@ -2158,10 +2158,10 @@
         <v>1696</v>
       </c>
       <c r="I51" t="n">
-        <v>32043</v>
+        <v>32044</v>
       </c>
       <c r="J51" t="n">
-        <v>25317</v>
+        <v>25320</v>
       </c>
       <c r="K51" t="n">
         <v>84</v>
@@ -2184,7 +2184,7 @@
         <v>4713</v>
       </c>
       <c r="F52" t="n">
-        <v>10121</v>
+        <v>10122</v>
       </c>
       <c r="G52" t="n">
         <v>1124</v>
@@ -2193,10 +2193,10 @@
         <v>2127</v>
       </c>
       <c r="I52" t="n">
-        <v>36738</v>
+        <v>36739</v>
       </c>
       <c r="J52" t="n">
-        <v>28692</v>
+        <v>28693</v>
       </c>
       <c r="K52" t="n">
         <v>120</v>
@@ -2219,7 +2219,7 @@
         <v>5164</v>
       </c>
       <c r="F53" t="n">
-        <v>11723</v>
+        <v>11724</v>
       </c>
       <c r="G53" t="n">
         <v>1285</v>
@@ -2228,10 +2228,10 @@
         <v>2625</v>
       </c>
       <c r="I53" t="n">
-        <v>40705</v>
+        <v>40706</v>
       </c>
       <c r="J53" t="n">
-        <v>31646</v>
+        <v>31647</v>
       </c>
       <c r="K53" t="n">
         <v>204</v>
@@ -2254,7 +2254,7 @@
         <v>5942</v>
       </c>
       <c r="F54" t="n">
-        <v>13363</v>
+        <v>13364</v>
       </c>
       <c r="G54" t="n">
         <v>1489</v>
@@ -2263,10 +2263,10 @@
         <v>3217</v>
       </c>
       <c r="I54" t="n">
-        <v>47099</v>
+        <v>47100</v>
       </c>
       <c r="J54" t="n">
-        <v>36445</v>
+        <v>36446</v>
       </c>
       <c r="K54" t="n">
         <v>251</v>
@@ -2289,7 +2289,7 @@
         <v>6463</v>
       </c>
       <c r="F55" t="n">
-        <v>15343</v>
+        <v>15344</v>
       </c>
       <c r="G55" t="n">
         <v>1808</v>
@@ -2298,7 +2298,7 @@
         <v>3973</v>
       </c>
       <c r="I55" t="n">
-        <v>52406</v>
+        <v>52407</v>
       </c>
       <c r="J55" t="n">
         <v>41979</v>
@@ -2324,7 +2324,7 @@
         <v>8924</v>
       </c>
       <c r="F56" t="n">
-        <v>17033</v>
+        <v>17034</v>
       </c>
       <c r="G56" t="n">
         <v>2051</v>
@@ -2333,7 +2333,7 @@
         <v>4728</v>
       </c>
       <c r="I56" t="n">
-        <v>63098</v>
+        <v>63099</v>
       </c>
       <c r="J56" t="n">
         <v>46855</v>
@@ -2368,7 +2368,7 @@
         <v>5591</v>
       </c>
       <c r="I57" t="n">
-        <v>72675</v>
+        <v>72676</v>
       </c>
       <c r="J57" t="n">
         <v>54309</v>
@@ -2403,10 +2403,10 @@
         <v>6575</v>
       </c>
       <c r="I58" t="n">
-        <v>81187</v>
+        <v>81188</v>
       </c>
       <c r="J58" t="n">
-        <v>59282</v>
+        <v>59281</v>
       </c>
       <c r="K58" t="n">
         <v>926</v>
@@ -2438,10 +2438,10 @@
         <v>7628</v>
       </c>
       <c r="I59" t="n">
-        <v>89779</v>
+        <v>89780</v>
       </c>
       <c r="J59" t="n">
-        <v>62626</v>
+        <v>62627</v>
       </c>
       <c r="K59" t="n">
         <v>1281</v>
@@ -2473,10 +2473,10 @@
         <v>8602</v>
       </c>
       <c r="I60" t="n">
-        <v>96083</v>
+        <v>96084</v>
       </c>
       <c r="J60" t="n">
-        <v>65300</v>
+        <v>65301</v>
       </c>
       <c r="K60" t="n">
         <v>1818</v>
@@ -2508,7 +2508,7 @@
         <v>9548</v>
       </c>
       <c r="I61" t="n">
-        <v>103275</v>
+        <v>103276</v>
       </c>
       <c r="J61" t="n">
         <v>70156</v>
@@ -2543,7 +2543,7 @@
         <v>10614</v>
       </c>
       <c r="I62" t="n">
-        <v>108823</v>
+        <v>108824</v>
       </c>
       <c r="J62" t="n">
         <v>74422</v>
@@ -2578,10 +2578,10 @@
         <v>11637</v>
       </c>
       <c r="I63" t="n">
-        <v>117175</v>
+        <v>117176</v>
       </c>
       <c r="J63" t="n">
-        <v>78243</v>
+        <v>78245</v>
       </c>
       <c r="K63" t="n">
         <v>2687</v>
@@ -2595,7 +2595,7 @@
         <v>5257</v>
       </c>
       <c r="C64" t="n">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="D64" t="n">
         <v>0</v>
@@ -2613,10 +2613,10 @@
         <v>12719</v>
       </c>
       <c r="I64" t="n">
-        <v>123949</v>
+        <v>123951</v>
       </c>
       <c r="J64" t="n">
-        <v>82058</v>
+        <v>82060</v>
       </c>
       <c r="K64" t="n">
         <v>3377</v>
@@ -2648,10 +2648,10 @@
         <v>13731</v>
       </c>
       <c r="I65" t="n">
-        <v>130637</v>
+        <v>130639</v>
       </c>
       <c r="J65" t="n">
-        <v>85926</v>
+        <v>85929</v>
       </c>
       <c r="K65" t="n">
         <v>4274</v>
@@ -2683,10 +2683,10 @@
         <v>14646</v>
       </c>
       <c r="I66" t="n">
-        <v>135946</v>
+        <v>135948</v>
       </c>
       <c r="J66" t="n">
-        <v>88355</v>
+        <v>88359</v>
       </c>
       <c r="K66" t="n">
         <v>5120</v>
@@ -2718,10 +2718,10 @@
         <v>15502</v>
       </c>
       <c r="I67" t="n">
-        <v>139708</v>
+        <v>139710</v>
       </c>
       <c r="J67" t="n">
-        <v>90012</v>
+        <v>90016</v>
       </c>
       <c r="K67" t="n">
         <v>5738</v>
@@ -2753,10 +2753,10 @@
         <v>16424</v>
       </c>
       <c r="I68" t="n">
-        <v>144594</v>
+        <v>144596</v>
       </c>
       <c r="J68" t="n">
-        <v>93223</v>
+        <v>93228</v>
       </c>
       <c r="K68" t="n">
         <v>6269</v>
@@ -2779,7 +2779,7 @@
         <v>4856</v>
       </c>
       <c r="F69" t="n">
-        <v>28789</v>
+        <v>28790</v>
       </c>
       <c r="G69" t="n">
         <v>3409</v>
@@ -2788,10 +2788,10 @@
         <v>17320</v>
       </c>
       <c r="I69" t="n">
-        <v>149514</v>
+        <v>149516</v>
       </c>
       <c r="J69" t="n">
-        <v>96280</v>
+        <v>96288</v>
       </c>
       <c r="K69" t="n">
         <v>6996</v>
@@ -2805,7 +2805,7 @@
         <v>2507</v>
       </c>
       <c r="C70" t="n">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="D70" t="n">
         <v>119</v>
@@ -2814,7 +2814,7 @@
         <v>4806</v>
       </c>
       <c r="F70" t="n">
-        <v>27695</v>
+        <v>27696</v>
       </c>
       <c r="G70" t="n">
         <v>3324</v>
@@ -2823,10 +2823,10 @@
         <v>18293</v>
       </c>
       <c r="I70" t="n">
-        <v>154913</v>
+        <v>154914</v>
       </c>
       <c r="J70" t="n">
-        <v>99401</v>
+        <v>99408</v>
       </c>
       <c r="K70" t="n">
         <v>7921</v>
@@ -2849,7 +2849,7 @@
         <v>4827</v>
       </c>
       <c r="F71" t="n">
-        <v>26327</v>
+        <v>26328</v>
       </c>
       <c r="G71" t="n">
         <v>3283</v>
@@ -2858,10 +2858,10 @@
         <v>19161</v>
       </c>
       <c r="I71" t="n">
-        <v>159905</v>
+        <v>159906</v>
       </c>
       <c r="J71" t="n">
-        <v>102014</v>
+        <v>102022</v>
       </c>
       <c r="K71" t="n">
         <v>9123</v>
@@ -2884,7 +2884,7 @@
         <v>4970</v>
       </c>
       <c r="F72" t="n">
-        <v>25943</v>
+        <v>25944</v>
       </c>
       <c r="G72" t="n">
         <v>3202</v>
@@ -2893,10 +2893,10 @@
         <v>19957</v>
       </c>
       <c r="I72" t="n">
-        <v>165060</v>
+        <v>165061</v>
       </c>
       <c r="J72" t="n">
-        <v>104298</v>
+        <v>104306</v>
       </c>
       <c r="K72" t="n">
         <v>10149</v>
@@ -2919,7 +2919,7 @@
         <v>5059</v>
       </c>
       <c r="F73" t="n">
-        <v>25140</v>
+        <v>25141</v>
       </c>
       <c r="G73" t="n">
         <v>3158</v>
@@ -2928,10 +2928,10 @@
         <v>20759</v>
       </c>
       <c r="I73" t="n">
-        <v>168829</v>
+        <v>168830</v>
       </c>
       <c r="J73" t="n">
-        <v>106067</v>
+        <v>106075</v>
       </c>
       <c r="K73" t="n">
         <v>11000</v>
@@ -2945,7 +2945,7 @@
         <v>2259</v>
       </c>
       <c r="C74" t="n">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="D74" t="n">
         <v>485</v>
@@ -2954,7 +2954,7 @@
         <v>5050</v>
       </c>
       <c r="F74" t="n">
-        <v>24499</v>
+        <v>24500</v>
       </c>
       <c r="G74" t="n">
         <v>3092</v>
@@ -2963,10 +2963,10 @@
         <v>21448</v>
       </c>
       <c r="I74" t="n">
-        <v>171872</v>
+        <v>171874</v>
       </c>
       <c r="J74" t="n">
-        <v>107318</v>
+        <v>107327</v>
       </c>
       <c r="K74" t="n">
         <v>11810</v>
@@ -2989,7 +2989,7 @@
         <v>5082</v>
       </c>
       <c r="F75" t="n">
-        <v>24210</v>
+        <v>24211</v>
       </c>
       <c r="G75" t="n">
         <v>3054</v>
@@ -2998,10 +2998,10 @@
         <v>22136</v>
       </c>
       <c r="I75" t="n">
-        <v>175374</v>
+        <v>175376</v>
       </c>
       <c r="J75" t="n">
-        <v>109243</v>
+        <v>109253</v>
       </c>
       <c r="K75" t="n">
         <v>12310</v>
@@ -3033,10 +3033,10 @@
         <v>22863</v>
       </c>
       <c r="I76" t="n">
-        <v>179702</v>
+        <v>179704</v>
       </c>
       <c r="J76" t="n">
-        <v>111774</v>
+        <v>111784</v>
       </c>
       <c r="K76" t="n">
         <v>13129</v>
@@ -3068,10 +3068,10 @@
         <v>23565</v>
       </c>
       <c r="I77" t="n">
-        <v>184103</v>
+        <v>184105</v>
       </c>
       <c r="J77" t="n">
-        <v>116797</v>
+        <v>116807</v>
       </c>
       <c r="K77" t="n">
         <v>14225</v>
@@ -3103,10 +3103,10 @@
         <v>24244</v>
       </c>
       <c r="I78" t="n">
-        <v>188812</v>
+        <v>188814</v>
       </c>
       <c r="J78" t="n">
-        <v>119149</v>
+        <v>119159</v>
       </c>
       <c r="K78" t="n">
         <v>15159</v>
@@ -3120,10 +3120,10 @@
         <v>3676</v>
       </c>
       <c r="C79" t="n">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="D79" t="n">
-        <v>1537</v>
+        <v>1535</v>
       </c>
       <c r="E79" t="n">
         <v>5378</v>
@@ -3138,10 +3138,10 @@
         <v>24855</v>
       </c>
       <c r="I79" t="n">
-        <v>193917</v>
+        <v>193916</v>
       </c>
       <c r="J79" t="n">
-        <v>121434</v>
+        <v>121445</v>
       </c>
       <c r="K79" t="n">
         <v>17293</v>
@@ -3164,7 +3164,7 @@
         <v>10437</v>
       </c>
       <c r="F80" t="n">
-        <v>19643</v>
+        <v>19644</v>
       </c>
       <c r="G80" t="n">
         <v>2522</v>
@@ -3173,10 +3173,10 @@
         <v>25458</v>
       </c>
       <c r="I80" t="n">
-        <v>199799</v>
+        <v>199798</v>
       </c>
       <c r="J80" t="n">
-        <v>122903</v>
+        <v>122915</v>
       </c>
       <c r="K80" t="n">
         <v>17184</v>
@@ -3199,7 +3199,7 @@
         <v>10241</v>
       </c>
       <c r="F81" t="n">
-        <v>19205</v>
+        <v>19206</v>
       </c>
       <c r="G81" t="n">
         <v>2536</v>
@@ -3208,10 +3208,10 @@
         <v>25986</v>
       </c>
       <c r="I81" t="n">
-        <v>202026</v>
+        <v>202025</v>
       </c>
       <c r="J81" t="n">
-        <v>123773</v>
+        <v>123785</v>
       </c>
       <c r="K81" t="n">
         <v>17825</v>
@@ -3234,7 +3234,7 @@
         <v>10220</v>
       </c>
       <c r="F82" t="n">
-        <v>19024</v>
+        <v>19025</v>
       </c>
       <c r="G82" t="n">
         <v>2481</v>
@@ -3243,10 +3243,10 @@
         <v>26480</v>
       </c>
       <c r="I82" t="n">
-        <v>204949</v>
+        <v>204948</v>
       </c>
       <c r="J82" t="n">
-        <v>125485</v>
+        <v>125499</v>
       </c>
       <c r="K82" t="n">
         <v>19791</v>
@@ -3269,7 +3269,7 @@
         <v>10149</v>
       </c>
       <c r="F83" t="n">
-        <v>18579</v>
+        <v>18580</v>
       </c>
       <c r="G83" t="n">
         <v>2408</v>
@@ -3278,10 +3278,10 @@
         <v>26988</v>
       </c>
       <c r="I83" t="n">
-        <v>208702</v>
+        <v>208701</v>
       </c>
       <c r="J83" t="n">
-        <v>127270</v>
+        <v>127285</v>
       </c>
       <c r="K83" t="n">
         <v>20567</v>
@@ -3304,7 +3304,7 @@
         <v>9642</v>
       </c>
       <c r="F84" t="n">
-        <v>17873</v>
+        <v>17877</v>
       </c>
       <c r="G84" t="n">
         <v>2316</v>
@@ -3313,10 +3313,10 @@
         <v>27474</v>
       </c>
       <c r="I84" t="n">
-        <v>213319</v>
+        <v>213318</v>
       </c>
       <c r="J84" t="n">
-        <v>126501</v>
+        <v>126517</v>
       </c>
       <c r="K84" t="n">
         <v>21163</v>
@@ -3339,7 +3339,7 @@
         <v>9325</v>
       </c>
       <c r="F85" t="n">
-        <v>17133</v>
+        <v>17137</v>
       </c>
       <c r="G85" t="n">
         <v>2261</v>
@@ -3348,10 +3348,10 @@
         <v>27906</v>
       </c>
       <c r="I85" t="n">
-        <v>217041</v>
+        <v>217040</v>
       </c>
       <c r="J85" t="n">
-        <v>127839</v>
+        <v>127857</v>
       </c>
       <c r="K85" t="n">
         <v>23466</v>
@@ -3374,7 +3374,7 @@
         <v>19892</v>
       </c>
       <c r="F86" t="n">
-        <v>16360</v>
+        <v>16364</v>
       </c>
       <c r="G86" t="n">
         <v>2177</v>
@@ -3383,10 +3383,10 @@
         <v>28345</v>
       </c>
       <c r="I86" t="n">
-        <v>220702</v>
+        <v>220701</v>
       </c>
       <c r="J86" t="n">
-        <v>129294</v>
+        <v>129319</v>
       </c>
       <c r="K86" t="n">
         <v>26642.89</v>
@@ -3409,7 +3409,7 @@
         <v>20059</v>
       </c>
       <c r="F87" t="n">
-        <v>16659</v>
+        <v>16663</v>
       </c>
       <c r="G87" t="n">
         <v>2304</v>
@@ -3418,10 +3418,10 @@
         <v>28716</v>
       </c>
       <c r="I87" t="n">
-        <v>223316</v>
+        <v>223315</v>
       </c>
       <c r="J87" t="n">
-        <v>130071</v>
+        <v>130097</v>
       </c>
       <c r="K87" t="n">
         <v>26800.966</v>
@@ -3438,13 +3438,13 @@
         <v>303</v>
       </c>
       <c r="D88" t="n">
-        <v>6988</v>
+        <v>6987</v>
       </c>
       <c r="E88" t="n">
         <v>20137</v>
       </c>
       <c r="F88" t="n">
-        <v>16174</v>
+        <v>16177</v>
       </c>
       <c r="G88" t="n">
         <v>2254</v>
@@ -3453,10 +3453,10 @@
         <v>29039</v>
       </c>
       <c r="I88" t="n">
-        <v>225695</v>
+        <v>225693</v>
       </c>
       <c r="J88" t="n">
-        <v>130582</v>
+        <v>130608</v>
       </c>
       <c r="K88" t="n">
         <v>30332</v>
@@ -3479,7 +3479,7 @@
         <v>20114</v>
       </c>
       <c r="F89" t="n">
-        <v>16061</v>
+        <v>16064</v>
       </c>
       <c r="G89" t="n">
         <v>2258</v>
@@ -3488,10 +3488,10 @@
         <v>29343</v>
       </c>
       <c r="I89" t="n">
-        <v>228391</v>
+        <v>228389</v>
       </c>
       <c r="J89" t="n">
-        <v>131628</v>
+        <v>131668</v>
       </c>
       <c r="K89" t="n">
         <v>31464</v>
@@ -3514,7 +3514,7 @@
         <v>19056</v>
       </c>
       <c r="F90" t="n">
-        <v>15543</v>
+        <v>15546</v>
       </c>
       <c r="G90" t="n">
         <v>2112</v>
@@ -3523,10 +3523,10 @@
         <v>29683</v>
       </c>
       <c r="I90" t="n">
-        <v>228193</v>
+        <v>228191</v>
       </c>
       <c r="J90" t="n">
-        <v>135579</v>
+        <v>135621</v>
       </c>
       <c r="K90" t="n">
         <v>33093</v>
@@ -3549,7 +3549,7 @@
         <v>20627</v>
       </c>
       <c r="F91" t="n">
-        <v>14967</v>
+        <v>14970</v>
       </c>
       <c r="G91" t="n">
         <v>2048</v>
@@ -3558,10 +3558,10 @@
         <v>29996</v>
       </c>
       <c r="I91" t="n">
-        <v>231083</v>
+        <v>231081</v>
       </c>
       <c r="J91" t="n">
-        <v>136521</v>
+        <v>136565</v>
       </c>
       <c r="K91" t="n">
         <v>35180</v>
@@ -3584,7 +3584,7 @@
         <v>19386</v>
       </c>
       <c r="F92" t="n">
-        <v>14348</v>
+        <v>14351</v>
       </c>
       <c r="G92" t="n">
         <v>1941</v>
@@ -3593,10 +3593,10 @@
         <v>30273</v>
       </c>
       <c r="I92" t="n">
-        <v>234305</v>
+        <v>234303</v>
       </c>
       <c r="J92" t="n">
-        <v>137364</v>
+        <v>137412</v>
       </c>
       <c r="K92" t="n">
         <v>33061</v>
@@ -3619,7 +3619,7 @@
         <v>19654</v>
       </c>
       <c r="F93" t="n">
-        <v>15160</v>
+        <v>15163</v>
       </c>
       <c r="G93" t="n">
         <v>2267</v>
@@ -3628,10 +3628,10 @@
         <v>30557</v>
       </c>
       <c r="I93" t="n">
-        <v>236456</v>
+        <v>236454</v>
       </c>
       <c r="J93" t="n">
-        <v>137867</v>
+        <v>137917</v>
       </c>
       <c r="K93" t="n">
         <v>34222</v>
@@ -3654,7 +3654,7 @@
         <v>20056</v>
       </c>
       <c r="F94" t="n">
-        <v>14913</v>
+        <v>14916</v>
       </c>
       <c r="G94" t="n">
         <v>2277</v>
@@ -3663,10 +3663,10 @@
         <v>30786</v>
       </c>
       <c r="I94" t="n">
-        <v>238115</v>
+        <v>238113</v>
       </c>
       <c r="J94" t="n">
-        <v>138199</v>
+        <v>138249</v>
       </c>
       <c r="K94" t="n">
         <v>34923</v>
@@ -3689,7 +3689,7 @@
         <v>20206</v>
       </c>
       <c r="F95" t="n">
-        <v>14827</v>
+        <v>14830</v>
       </c>
       <c r="G95" t="n">
         <v>2228</v>
@@ -3698,10 +3698,10 @@
         <v>31007</v>
       </c>
       <c r="I95" t="n">
-        <v>239210</v>
+        <v>239208</v>
       </c>
       <c r="J95" t="n">
-        <v>138455</v>
+        <v>138505</v>
       </c>
       <c r="K95" t="n">
         <v>35437</v>
@@ -3724,7 +3724,7 @@
         <v>20387</v>
       </c>
       <c r="F96" t="n">
-        <v>14552</v>
+        <v>14555</v>
       </c>
       <c r="G96" t="n">
         <v>2135</v>
@@ -3733,10 +3733,10 @@
         <v>31210</v>
       </c>
       <c r="I96" t="n">
-        <v>240960</v>
+        <v>240958</v>
       </c>
       <c r="J96" t="n">
-        <v>139220</v>
+        <v>139270</v>
       </c>
       <c r="K96" t="n">
         <v>36006</v>
@@ -3759,7 +3759,7 @@
         <v>16370</v>
       </c>
       <c r="F97" t="n">
-        <v>14228</v>
+        <v>14231</v>
       </c>
       <c r="G97" t="n">
         <v>2085</v>
@@ -3768,10 +3768,10 @@
         <v>31441</v>
       </c>
       <c r="I97" t="n">
-        <v>243015</v>
+        <v>243013</v>
       </c>
       <c r="J97" t="n">
-        <v>152214</v>
+        <v>152268</v>
       </c>
       <c r="K97" t="n">
         <v>36965</v>
@@ -3794,7 +3794,7 @@
         <v>16806</v>
       </c>
       <c r="F98" t="n">
-        <v>13671</v>
+        <v>13673</v>
       </c>
       <c r="G98" t="n">
         <v>1977</v>
@@ -3803,10 +3803,10 @@
         <v>31685</v>
       </c>
       <c r="I98" t="n">
-        <v>245962</v>
+        <v>245960</v>
       </c>
       <c r="J98" t="n">
-        <v>153010</v>
+        <v>153064</v>
       </c>
       <c r="K98" t="n">
         <v>37943</v>
@@ -3829,7 +3829,7 @@
         <v>17160</v>
       </c>
       <c r="F99" t="n">
-        <v>13076</v>
+        <v>13079</v>
       </c>
       <c r="G99" t="n">
         <v>1901</v>
@@ -3838,10 +3838,10 @@
         <v>31768</v>
       </c>
       <c r="I99" t="n">
-        <v>246338</v>
+        <v>246336</v>
       </c>
       <c r="J99" t="n">
-        <v>151457</v>
+        <v>151514</v>
       </c>
       <c r="K99" t="n">
         <v>38932</v>
@@ -3864,7 +3864,7 @@
         <v>17322</v>
       </c>
       <c r="F100" t="n">
-        <v>12195</v>
+        <v>12197</v>
       </c>
       <c r="G100" t="n">
         <v>1837</v>
@@ -3873,10 +3873,10 @@
         <v>32122</v>
       </c>
       <c r="I100" t="n">
-        <v>250875</v>
+        <v>250873</v>
       </c>
       <c r="J100" t="n">
-        <v>154335</v>
+        <v>154393</v>
       </c>
       <c r="K100" t="n">
         <v>39875</v>
@@ -3899,7 +3899,7 @@
         <v>17603</v>
       </c>
       <c r="F101" t="n">
-        <v>12054</v>
+        <v>12056</v>
       </c>
       <c r="G101" t="n">
         <v>1760</v>
@@ -3908,10 +3908,10 @@
         <v>32296</v>
       </c>
       <c r="I101" t="n">
-        <v>252693</v>
+        <v>252691</v>
       </c>
       <c r="J101" t="n">
-        <v>154625</v>
+        <v>154683</v>
       </c>
       <c r="K101" t="n">
         <v>41086</v>
@@ -3934,7 +3934,7 @@
         <v>17854</v>
       </c>
       <c r="F102" t="n">
-        <v>11676</v>
+        <v>11678</v>
       </c>
       <c r="G102" t="n">
         <v>1699</v>
@@ -3943,10 +3943,10 @@
         <v>32293</v>
       </c>
       <c r="I102" t="n">
-        <v>251651</v>
+        <v>251649</v>
       </c>
       <c r="J102" t="n">
-        <v>152592</v>
+        <v>152650</v>
       </c>
       <c r="K102" t="n">
         <v>41579</v>
@@ -3969,7 +3969,7 @@
         <v>17973</v>
       </c>
       <c r="F103" t="n">
-        <v>11595</v>
+        <v>11597</v>
       </c>
       <c r="G103" t="n">
         <v>1642</v>
@@ -3978,10 +3978,10 @@
         <v>32603</v>
       </c>
       <c r="I103" t="n">
-        <v>255277</v>
+        <v>255275</v>
       </c>
       <c r="J103" t="n">
-        <v>155405</v>
+        <v>155464</v>
       </c>
       <c r="K103" t="n">
         <v>41920</v>
@@ -4004,7 +4004,7 @@
         <v>18099</v>
       </c>
       <c r="F104" t="n">
-        <v>11254</v>
+        <v>11255</v>
       </c>
       <c r="G104" t="n">
         <v>1574</v>
@@ -4013,10 +4013,10 @@
         <v>32753</v>
       </c>
       <c r="I104" t="n">
-        <v>256957</v>
+        <v>256955</v>
       </c>
       <c r="J104" t="n">
-        <v>156046</v>
+        <v>156106</v>
       </c>
       <c r="K104" t="n">
         <v>42608</v>
@@ -4039,7 +4039,7 @@
         <v>18076</v>
       </c>
       <c r="F105" t="n">
-        <v>10849</v>
+        <v>10850</v>
       </c>
       <c r="G105" t="n">
         <v>1495</v>
@@ -4048,10 +4048,10 @@
         <v>32872</v>
       </c>
       <c r="I105" t="n">
-        <v>258557</v>
+        <v>258555</v>
       </c>
       <c r="J105" t="n">
-        <v>156715</v>
+        <v>156777</v>
       </c>
       <c r="K105" t="n">
         <v>43586</v>
@@ -4074,7 +4074,7 @@
         <v>2826</v>
       </c>
       <c r="F106" t="n">
-        <v>10433</v>
+        <v>10434</v>
       </c>
       <c r="G106" t="n">
         <v>1459</v>
@@ -4083,10 +4083,10 @@
         <v>31536</v>
       </c>
       <c r="I106" t="n">
-        <v>203341</v>
+        <v>203339</v>
       </c>
       <c r="J106" t="n">
-        <v>184620</v>
+        <v>184683</v>
       </c>
       <c r="K106" t="n">
         <v>44466</v>
@@ -4109,7 +4109,7 @@
         <v>2826</v>
       </c>
       <c r="F107" t="n">
-        <v>10014</v>
+        <v>10016</v>
       </c>
       <c r="G107" t="n">
         <v>1469</v>
@@ -4118,10 +4118,10 @@
         <v>31649</v>
       </c>
       <c r="I107" t="n">
-        <v>204636</v>
+        <v>204634</v>
       </c>
       <c r="J107" t="n">
-        <v>198026</v>
+        <v>198089</v>
       </c>
       <c r="K107" t="n">
         <v>45150</v>
@@ -4144,7 +4144,7 @@
         <v>2823</v>
       </c>
       <c r="F108" t="n">
-        <v>9734</v>
+        <v>9736</v>
       </c>
       <c r="G108" t="n">
         <v>1432</v>
@@ -4153,10 +4153,10 @@
         <v>31739</v>
       </c>
       <c r="I108" t="n">
-        <v>205249</v>
+        <v>205247</v>
       </c>
       <c r="J108" t="n">
-        <v>198342</v>
+        <v>198407</v>
       </c>
       <c r="K108" t="n">
         <v>45881</v>
@@ -4179,7 +4179,7 @@
         <v>2809</v>
       </c>
       <c r="F109" t="n">
-        <v>9605</v>
+        <v>9607</v>
       </c>
       <c r="G109" t="n">
         <v>1397</v>
@@ -4188,10 +4188,10 @@
         <v>31810</v>
       </c>
       <c r="I109" t="n">
-        <v>205599</v>
+        <v>205597</v>
       </c>
       <c r="J109" t="n">
-        <v>198585</v>
+        <v>198651</v>
       </c>
       <c r="K109" t="n">
         <v>46333</v>
@@ -4214,7 +4214,7 @@
         <v>2784</v>
       </c>
       <c r="F110" t="n">
-        <v>9523</v>
+        <v>9524</v>
       </c>
       <c r="G110" t="n">
         <v>1379</v>
@@ -4223,10 +4223,10 @@
         <v>31728</v>
       </c>
       <c r="I110" t="n">
-        <v>179083</v>
+        <v>179081</v>
       </c>
       <c r="J110" t="n">
-        <v>221589</v>
+        <v>221658</v>
       </c>
       <c r="K110" t="n">
         <v>40246</v>
@@ -4249,7 +4249,7 @@
         <v>1564</v>
       </c>
       <c r="F111" t="n">
-        <v>9230</v>
+        <v>9231</v>
       </c>
       <c r="G111" t="n">
         <v>1308</v>
@@ -4258,10 +4258,10 @@
         <v>31961</v>
       </c>
       <c r="I111" t="n">
-        <v>174988</v>
+        <v>174986</v>
       </c>
       <c r="J111" t="n">
-        <v>230117</v>
+        <v>230186</v>
       </c>
       <c r="K111" t="n">
         <v>40464</v>
@@ -4275,7 +4275,7 @@
         <v>53</v>
       </c>
       <c r="C112" t="n">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D112" t="n">
         <v>12514</v>
@@ -4284,7 +4284,7 @@
         <v>1370</v>
       </c>
       <c r="F112" t="n">
-        <v>8929</v>
+        <v>8930</v>
       </c>
       <c r="G112" t="n">
         <v>1241</v>
@@ -4293,10 +4293,10 @@
         <v>32052</v>
       </c>
       <c r="I112" t="n">
-        <v>175551</v>
+        <v>175550</v>
       </c>
       <c r="J112" t="n">
-        <v>230859</v>
+        <v>230933</v>
       </c>
       <c r="K112" t="n">
         <v>46183</v>
@@ -4319,7 +4319,7 @@
         <v>1344</v>
       </c>
       <c r="F113" t="n">
-        <v>4303</v>
+        <v>4304</v>
       </c>
       <c r="G113" t="n">
         <v>762</v>
@@ -4328,10 +4328,10 @@
         <v>32114</v>
       </c>
       <c r="I113" t="n">
-        <v>83722</v>
+        <v>83721</v>
       </c>
       <c r="J113" t="n">
-        <v>231704</v>
+        <v>231780</v>
       </c>
       <c r="K113" t="n">
         <v>49016</v>
@@ -4354,7 +4354,7 @@
         <v>1338</v>
       </c>
       <c r="F114" t="n">
-        <v>3744</v>
+        <v>3746</v>
       </c>
       <c r="G114" t="n">
         <v>695</v>
@@ -4363,10 +4363,10 @@
         <v>32184</v>
       </c>
       <c r="I114" t="n">
-        <v>84209</v>
+        <v>84208</v>
       </c>
       <c r="J114" t="n">
-        <v>232545</v>
+        <v>232622</v>
       </c>
       <c r="K114" t="n">
         <v>49577</v>
@@ -4389,7 +4389,7 @@
         <v>1322</v>
       </c>
       <c r="F115" t="n">
-        <v>3756</v>
+        <v>3758</v>
       </c>
       <c r="G115" t="n">
         <v>703</v>
@@ -4398,10 +4398,10 @@
         <v>32261</v>
       </c>
       <c r="I115" t="n">
-        <v>84424</v>
+        <v>84423</v>
       </c>
       <c r="J115" t="n">
-        <v>232869</v>
+        <v>232946</v>
       </c>
       <c r="K115" t="n">
         <v>39307</v>
@@ -4424,7 +4424,7 @@
         <v>1322</v>
       </c>
       <c r="F116" t="n">
-        <v>3668</v>
+        <v>3670</v>
       </c>
       <c r="G116" t="n">
         <v>681</v>
@@ -4433,10 +4433,10 @@
         <v>32312</v>
       </c>
       <c r="I116" t="n">
-        <v>84586</v>
+        <v>84585</v>
       </c>
       <c r="J116" t="n">
-        <v>233156</v>
+        <v>233234</v>
       </c>
       <c r="K116" t="n">
         <v>40488</v>
@@ -4459,7 +4459,7 @@
         <v>1647</v>
       </c>
       <c r="F117" t="n">
-        <v>3566</v>
+        <v>3568</v>
       </c>
       <c r="G117" t="n">
         <v>652</v>
@@ -4468,10 +4468,10 @@
         <v>29426</v>
       </c>
       <c r="I117" t="n">
-        <v>84932</v>
+        <v>84931</v>
       </c>
       <c r="J117" t="n">
-        <v>216783</v>
+        <v>216863</v>
       </c>
       <c r="K117" t="n">
         <v>40512</v>
@@ -4494,7 +4494,7 @@
         <v>1213</v>
       </c>
       <c r="F118" t="n">
-        <v>3436</v>
+        <v>3438</v>
       </c>
       <c r="G118" t="n">
         <v>643</v>
@@ -4503,10 +4503,10 @@
         <v>29486</v>
       </c>
       <c r="I118" t="n">
-        <v>85309</v>
+        <v>85308</v>
       </c>
       <c r="J118" t="n">
-        <v>217444</v>
+        <v>217527</v>
       </c>
       <c r="K118" t="n">
         <v>53170</v>
@@ -4529,7 +4529,7 @@
         <v>1143</v>
       </c>
       <c r="F119" t="n">
-        <v>3230</v>
+        <v>3232</v>
       </c>
       <c r="G119" t="n">
         <v>596</v>
@@ -4538,10 +4538,10 @@
         <v>32486</v>
       </c>
       <c r="I119" t="n">
-        <v>85703</v>
+        <v>85702</v>
       </c>
       <c r="J119" t="n">
-        <v>235060</v>
+        <v>235146</v>
       </c>
       <c r="K119" t="n">
         <v>53883</v>
@@ -4564,7 +4564,7 @@
         <v>859</v>
       </c>
       <c r="F120" t="n">
-        <v>2925</v>
+        <v>2927</v>
       </c>
       <c r="G120" t="n">
         <v>532</v>
@@ -4573,10 +4573,10 @@
         <v>32304</v>
       </c>
       <c r="I120" t="n">
-        <v>83919</v>
+        <v>83918</v>
       </c>
       <c r="J120" t="n">
-        <v>235706</v>
+        <v>235797</v>
       </c>
       <c r="K120" t="n">
         <v>52897</v>
@@ -4590,7 +4590,7 @@
         <v>74</v>
       </c>
       <c r="C121" t="n">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D121" t="n">
         <v>26</v>
@@ -4599,10 +4599,10 @@
         <v>1652</v>
       </c>
       <c r="F121" t="n">
-        <v>2863</v>
+        <v>2865</v>
       </c>
       <c r="G121" t="n">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="H121" t="n">
         <v>32742</v>
@@ -4611,7 +4611,7 @@
         <v>86303</v>
       </c>
       <c r="J121" t="n">
-        <v>236388</v>
+        <v>236487</v>
       </c>
       <c r="K121" t="n">
         <v>60941</v>
@@ -4634,10 +4634,10 @@
         <v>1595</v>
       </c>
       <c r="F122" t="n">
-        <v>2725</v>
+        <v>2727</v>
       </c>
       <c r="G122" t="n">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="H122" t="n">
         <v>32783</v>
@@ -4646,7 +4646,7 @@
         <v>86445</v>
       </c>
       <c r="J122" t="n">
-        <v>236735</v>
+        <v>236835</v>
       </c>
       <c r="K122" t="n">
         <v>61527</v>
@@ -4669,7 +4669,7 @@
         <v>1565</v>
       </c>
       <c r="F123" t="n">
-        <v>2665</v>
+        <v>2668</v>
       </c>
       <c r="G123" t="n">
         <v>512</v>
@@ -4681,7 +4681,7 @@
         <v>86492</v>
       </c>
       <c r="J123" t="n">
-        <v>236997</v>
+        <v>237101</v>
       </c>
       <c r="K123" t="n">
         <v>61840</v>
@@ -4704,7 +4704,7 @@
         <v>1513</v>
       </c>
       <c r="F124" t="n">
-        <v>2692</v>
+        <v>2695</v>
       </c>
       <c r="G124" t="n">
         <v>507</v>
@@ -4716,7 +4716,7 @@
         <v>86568</v>
       </c>
       <c r="J124" t="n">
-        <v>237331</v>
+        <v>237436</v>
       </c>
       <c r="K124" t="n">
         <v>62091</v>
@@ -4739,7 +4739,7 @@
         <v>1321</v>
       </c>
       <c r="F125" t="n">
-        <v>2427</v>
+        <v>2430</v>
       </c>
       <c r="G125" t="n">
         <v>469</v>
@@ -4751,7 +4751,7 @@
         <v>84747</v>
       </c>
       <c r="J125" t="n">
-        <v>237894</v>
+        <v>238003</v>
       </c>
       <c r="K125" t="n">
         <v>60998</v>
@@ -4774,7 +4774,7 @@
         <v>1537</v>
       </c>
       <c r="F126" t="n">
-        <v>2336</v>
+        <v>2338</v>
       </c>
       <c r="G126" t="n">
         <v>443</v>
@@ -4786,7 +4786,7 @@
         <v>87079</v>
       </c>
       <c r="J126" t="n">
-        <v>238503</v>
+        <v>238615</v>
       </c>
       <c r="K126" t="n">
         <v>63197</v>
@@ -4809,7 +4809,7 @@
         <v>402</v>
       </c>
       <c r="F127" t="n">
-        <v>2101</v>
+        <v>2103</v>
       </c>
       <c r="G127" t="n">
         <v>421</v>
@@ -4821,7 +4821,7 @@
         <v>94549</v>
       </c>
       <c r="J127" t="n">
-        <v>239038</v>
+        <v>239153</v>
       </c>
       <c r="K127" t="n">
         <v>56161</v>
@@ -4844,7 +4844,7 @@
         <v>357</v>
       </c>
       <c r="F128" t="n">
-        <v>1933</v>
+        <v>1934</v>
       </c>
       <c r="G128" t="n">
         <v>399</v>
@@ -4856,7 +4856,7 @@
         <v>97061</v>
       </c>
       <c r="J128" t="n">
-        <v>241714</v>
+        <v>241832</v>
       </c>
       <c r="K128" t="n">
         <v>58166</v>
@@ -4879,7 +4879,7 @@
         <v>356</v>
       </c>
       <c r="F129" t="n">
-        <v>1854</v>
+        <v>1855</v>
       </c>
       <c r="G129" t="n">
         <v>400</v>
@@ -4891,7 +4891,7 @@
         <v>97053</v>
       </c>
       <c r="J129" t="n">
-        <v>242048</v>
+        <v>242168</v>
       </c>
       <c r="K129" t="n">
         <v>58388</v>
@@ -4914,7 +4914,7 @@
         <v>360</v>
       </c>
       <c r="F130" t="n">
-        <v>1842</v>
+        <v>1843</v>
       </c>
       <c r="G130" t="n">
         <v>398</v>
@@ -4926,7 +4926,7 @@
         <v>97210</v>
       </c>
       <c r="J130" t="n">
-        <v>242638</v>
+        <v>242759</v>
       </c>
       <c r="K130" t="n">
         <v>58665</v>
@@ -4961,7 +4961,7 @@
         <v>97355</v>
       </c>
       <c r="J131" t="n">
-        <v>242944</v>
+        <v>243068</v>
       </c>
       <c r="K131" t="n">
         <v>58766</v>
@@ -4984,7 +4984,7 @@
         <v>1022</v>
       </c>
       <c r="F132" t="n">
-        <v>1750</v>
+        <v>1752</v>
       </c>
       <c r="G132" t="n">
         <v>370</v>
@@ -4996,7 +4996,7 @@
         <v>97527</v>
       </c>
       <c r="J132" t="n">
-        <v>243347</v>
+        <v>243472</v>
       </c>
       <c r="K132" t="n">
         <v>59174</v>
@@ -5019,7 +5019,7 @@
         <v>986</v>
       </c>
       <c r="F133" t="n">
-        <v>1613</v>
+        <v>1615</v>
       </c>
       <c r="G133" t="n">
         <v>332</v>
@@ -5031,7 +5031,7 @@
         <v>97733</v>
       </c>
       <c r="J133" t="n">
-        <v>241638</v>
+        <v>241765</v>
       </c>
       <c r="K133" t="n">
         <v>59613</v>
@@ -5054,7 +5054,7 @@
         <v>945</v>
       </c>
       <c r="F134" t="n">
-        <v>1522</v>
+        <v>1524</v>
       </c>
       <c r="G134" t="n">
         <v>331</v>
@@ -5066,7 +5066,7 @@
         <v>97886</v>
       </c>
       <c r="J134" t="n">
-        <v>242043</v>
+        <v>242174</v>
       </c>
       <c r="K134" t="n">
         <v>59932</v>
@@ -5089,7 +5089,7 @@
         <v>300</v>
       </c>
       <c r="F135" t="n">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="G135" t="n">
         <v>321</v>
@@ -5101,7 +5101,7 @@
         <v>98094</v>
       </c>
       <c r="J135" t="n">
-        <v>242506</v>
+        <v>242637</v>
       </c>
       <c r="K135" t="n">
         <v>60275</v>
@@ -5124,7 +5124,7 @@
         <v>308</v>
       </c>
       <c r="F136" t="n">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="G136" t="n">
         <v>290</v>
@@ -5136,7 +5136,7 @@
         <v>98151</v>
       </c>
       <c r="J136" t="n">
-        <v>216584</v>
+        <v>216716</v>
       </c>
       <c r="K136" t="n">
         <v>52176</v>
@@ -5159,7 +5159,7 @@
         <v>299</v>
       </c>
       <c r="F137" t="n">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="G137" t="n">
         <v>282</v>
@@ -5171,7 +5171,7 @@
         <v>98187</v>
       </c>
       <c r="J137" t="n">
-        <v>216682</v>
+        <v>216815</v>
       </c>
       <c r="K137" t="n">
         <v>52241</v>
@@ -5194,7 +5194,7 @@
         <v>866</v>
       </c>
       <c r="F138" t="n">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="G138" t="n">
         <v>297</v>
@@ -5206,7 +5206,7 @@
         <v>98299</v>
       </c>
       <c r="J138" t="n">
-        <v>243067</v>
+        <v>243202</v>
       </c>
       <c r="K138" t="n">
         <v>60802</v>
@@ -5229,7 +5229,7 @@
         <v>267</v>
       </c>
       <c r="F139" t="n">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="G139" t="n">
         <v>287</v>
@@ -5241,7 +5241,7 @@
         <v>98475</v>
       </c>
       <c r="J139" t="n">
-        <v>243362</v>
+        <v>243497</v>
       </c>
       <c r="K139" t="n">
         <v>61114</v>
@@ -5264,7 +5264,7 @@
         <v>237</v>
       </c>
       <c r="F140" t="n">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="G140" t="n">
         <v>275</v>
@@ -5276,7 +5276,7 @@
         <v>98615</v>
       </c>
       <c r="J140" t="n">
-        <v>243693</v>
+        <v>243829</v>
       </c>
       <c r="K140" t="n">
         <v>61436</v>
@@ -5299,7 +5299,7 @@
         <v>775</v>
       </c>
       <c r="F141" t="n">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="G141" t="n">
         <v>260</v>
@@ -5311,7 +5311,7 @@
         <v>98828</v>
       </c>
       <c r="J141" t="n">
-        <v>244188</v>
+        <v>244325</v>
       </c>
       <c r="K141" t="n">
         <v>61810</v>
@@ -5334,7 +5334,7 @@
         <v>226</v>
       </c>
       <c r="F142" t="n">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="G142" t="n">
         <v>237</v>
@@ -5346,7 +5346,7 @@
         <v>99014</v>
       </c>
       <c r="J142" t="n">
-        <v>244559</v>
+        <v>244698</v>
       </c>
       <c r="K142" t="n">
         <v>62041</v>
@@ -5369,7 +5369,7 @@
         <v>223</v>
       </c>
       <c r="F143" t="n">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="G143" t="n">
         <v>225</v>
@@ -5381,7 +5381,7 @@
         <v>99097</v>
       </c>
       <c r="J143" t="n">
-        <v>244783</v>
+        <v>244923</v>
       </c>
       <c r="K143" t="n">
         <v>62244</v>
@@ -5404,10 +5404,10 @@
         <v>238</v>
       </c>
       <c r="F144" t="n">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="G144" t="n">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H144" t="n">
         <v>33417</v>
@@ -5416,7 +5416,7 @@
         <v>99153</v>
       </c>
       <c r="J144" t="n">
-        <v>244974</v>
+        <v>245115</v>
       </c>
       <c r="K144" t="n">
         <v>62289</v>
@@ -5439,10 +5439,10 @@
         <v>821</v>
       </c>
       <c r="F145" t="n">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="G145" t="n">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H145" t="n">
         <v>33640</v>
@@ -5451,7 +5451,7 @@
         <v>99277</v>
       </c>
       <c r="J145" t="n">
-        <v>245204</v>
+        <v>245346</v>
       </c>
       <c r="K145" t="n">
         <v>62351</v>
@@ -5474,10 +5474,10 @@
         <v>838</v>
       </c>
       <c r="F146" t="n">
-        <v>1075</v>
+        <v>1077</v>
       </c>
       <c r="G146" t="n">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H146" t="n">
         <v>33652</v>
@@ -5486,7 +5486,7 @@
         <v>99346</v>
       </c>
       <c r="J146" t="n">
-        <v>245560</v>
+        <v>245705</v>
       </c>
       <c r="K146" t="n">
         <v>62507</v>
@@ -5509,10 +5509,10 @@
         <v>78</v>
       </c>
       <c r="F147" t="n">
-        <v>1082</v>
+        <v>1085</v>
       </c>
       <c r="G147" t="n">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H147" t="n">
         <v>33230</v>
@@ -5521,7 +5521,7 @@
         <v>97269</v>
       </c>
       <c r="J147" t="n">
-        <v>245874</v>
+        <v>246023</v>
       </c>
       <c r="K147" t="n">
         <v>60872</v>
@@ -5544,7 +5544,7 @@
         <v>896</v>
       </c>
       <c r="F148" t="n">
-        <v>1069</v>
+        <v>1073</v>
       </c>
       <c r="G148" t="n">
         <v>204</v>
@@ -5556,7 +5556,7 @@
         <v>99723</v>
       </c>
       <c r="J148" t="n">
-        <v>246257</v>
+        <v>246407</v>
       </c>
       <c r="K148" t="n">
         <v>62979</v>
@@ -5570,7 +5570,7 @@
         <v>23</v>
       </c>
       <c r="C149" t="n">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D149" t="n">
         <v>31</v>
@@ -5579,7 +5579,7 @@
         <v>216</v>
       </c>
       <c r="F149" t="n">
-        <v>1004</v>
+        <v>1008</v>
       </c>
       <c r="G149" t="n">
         <v>188</v>
@@ -5588,10 +5588,10 @@
         <v>33480</v>
       </c>
       <c r="I149" t="n">
-        <v>100011</v>
+        <v>100012</v>
       </c>
       <c r="J149" t="n">
-        <v>246803</v>
+        <v>246955</v>
       </c>
       <c r="K149" t="n">
         <v>63184</v>
@@ -5614,7 +5614,7 @@
         <v>76</v>
       </c>
       <c r="F150" t="n">
-        <v>982</v>
+        <v>986</v>
       </c>
       <c r="G150" t="n">
         <v>179</v>
@@ -5623,10 +5623,10 @@
         <v>33264</v>
       </c>
       <c r="I150" t="n">
-        <v>97841</v>
+        <v>97842</v>
       </c>
       <c r="J150" t="n">
-        <v>247059</v>
+        <v>247211</v>
       </c>
       <c r="K150" t="n">
         <v>61363</v>
@@ -5649,7 +5649,7 @@
         <v>76</v>
       </c>
       <c r="F151" t="n">
-        <v>890</v>
+        <v>894</v>
       </c>
       <c r="G151" t="n">
         <v>146</v>
@@ -5658,10 +5658,10 @@
         <v>33271</v>
       </c>
       <c r="I151" t="n">
-        <v>97936</v>
+        <v>97937</v>
       </c>
       <c r="J151" t="n">
-        <v>247252</v>
+        <v>247405</v>
       </c>
       <c r="K151" t="n">
         <v>60427</v>
@@ -5684,19 +5684,19 @@
         <v>211</v>
       </c>
       <c r="F152" t="n">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="G152" t="n">
         <v>177</v>
       </c>
       <c r="H152" t="n">
-        <v>33455</v>
+        <v>33503</v>
       </c>
       <c r="I152" t="n">
-        <v>100430</v>
+        <v>100431</v>
       </c>
       <c r="J152" t="n">
-        <v>247499</v>
+        <v>247654</v>
       </c>
       <c r="K152" t="n">
         <v>63416</v>
@@ -5719,7 +5719,7 @@
         <v>203</v>
       </c>
       <c r="F153" t="n">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="G153" t="n">
         <v>174</v>
@@ -5728,10 +5728,10 @@
         <v>33522</v>
       </c>
       <c r="I153" t="n">
-        <v>100737</v>
+        <v>100738</v>
       </c>
       <c r="J153" t="n">
-        <v>247916</v>
+        <v>248072</v>
       </c>
       <c r="K153" t="n">
         <v>58247</v>
@@ -5754,7 +5754,7 @@
         <v>207</v>
       </c>
       <c r="F154" t="n">
-        <v>962</v>
+        <v>965</v>
       </c>
       <c r="G154" t="n">
         <v>170</v>
@@ -5763,10 +5763,10 @@
         <v>33536</v>
       </c>
       <c r="I154" t="n">
-        <v>101135</v>
+        <v>101136</v>
       </c>
       <c r="J154" t="n">
-        <v>248332</v>
+        <v>248492</v>
       </c>
       <c r="K154" t="n">
         <v>65597</v>
@@ -5789,7 +5789,7 @@
         <v>205</v>
       </c>
       <c r="F155" t="n">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="G155" t="n">
         <v>159</v>
@@ -5798,10 +5798,10 @@
         <v>33753</v>
       </c>
       <c r="I155" t="n">
-        <v>101537</v>
+        <v>101538</v>
       </c>
       <c r="J155" t="n">
-        <v>248790</v>
+        <v>248955</v>
       </c>
       <c r="K155" t="n">
         <v>65782</v>
@@ -5824,7 +5824,7 @@
         <v>203</v>
       </c>
       <c r="F156" t="n">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="G156" t="n">
         <v>153</v>
@@ -5833,10 +5833,10 @@
         <v>33551</v>
       </c>
       <c r="I156" t="n">
-        <v>101985</v>
+        <v>101986</v>
       </c>
       <c r="J156" t="n">
-        <v>243003</v>
+        <v>243172</v>
       </c>
       <c r="K156" t="n">
         <v>61385</v>
@@ -5859,7 +5859,7 @@
         <v>63</v>
       </c>
       <c r="F157" t="n">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="G157" t="n">
         <v>73</v>
@@ -5868,10 +5868,10 @@
         <v>28096</v>
       </c>
       <c r="I157" t="n">
-        <v>99815</v>
+        <v>99816</v>
       </c>
       <c r="J157" t="n">
-        <v>213337</v>
+        <v>213506</v>
       </c>
       <c r="K157" t="n">
         <v>35399</v>
@@ -5894,7 +5894,7 @@
         <v>63</v>
       </c>
       <c r="F158" t="n">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="G158" t="n">
         <v>61</v>
@@ -5903,10 +5903,10 @@
         <v>28102</v>
       </c>
       <c r="I158" t="n">
-        <v>99996</v>
+        <v>99997</v>
       </c>
       <c r="J158" t="n">
-        <v>213493</v>
+        <v>213663</v>
       </c>
       <c r="K158" t="n">
         <v>35407</v>
@@ -5929,7 +5929,7 @@
         <v>205</v>
       </c>
       <c r="F159" t="n">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="G159" t="n">
         <v>150</v>
@@ -5938,10 +5938,10 @@
         <v>32864</v>
       </c>
       <c r="I159" t="n">
-        <v>102633</v>
+        <v>102634</v>
       </c>
       <c r="J159" t="n">
-        <v>239598</v>
+        <v>239768</v>
       </c>
       <c r="K159" t="n">
         <v>61621</v>
@@ -5964,7 +5964,7 @@
         <v>200</v>
       </c>
       <c r="F160" t="n">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="G160" t="n">
         <v>144</v>
@@ -5973,10 +5973,10 @@
         <v>33588</v>
       </c>
       <c r="I160" t="n">
-        <v>103193</v>
+        <v>103194</v>
       </c>
       <c r="J160" t="n">
-        <v>240206</v>
+        <v>240379</v>
       </c>
       <c r="K160" t="n">
         <v>61735</v>
@@ -5999,7 +5999,7 @@
         <v>198</v>
       </c>
       <c r="F161" t="n">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="G161" t="n">
         <v>131</v>
@@ -6008,10 +6008,10 @@
         <v>33597</v>
       </c>
       <c r="I161" t="n">
-        <v>103871</v>
+        <v>103872</v>
       </c>
       <c r="J161" t="n">
-        <v>233563</v>
+        <v>233738</v>
       </c>
       <c r="K161" t="n">
         <v>61867</v>
@@ -6034,7 +6034,7 @@
         <v>1091</v>
       </c>
       <c r="F162" t="n">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="G162" t="n">
         <v>128</v>
@@ -6043,10 +6043,10 @@
         <v>33822</v>
       </c>
       <c r="I162" t="n">
-        <v>104643</v>
+        <v>104644</v>
       </c>
       <c r="J162" t="n">
-        <v>248034</v>
+        <v>248214</v>
       </c>
       <c r="K162" t="n">
         <v>66701</v>
@@ -6069,7 +6069,7 @@
         <v>198</v>
       </c>
       <c r="F163" t="n">
-        <v>823</v>
+        <v>826</v>
       </c>
       <c r="G163" t="n">
         <v>123</v>
@@ -6078,10 +6078,10 @@
         <v>32931</v>
       </c>
       <c r="I163" t="n">
-        <v>105647</v>
+        <v>105648</v>
       </c>
       <c r="J163" t="n">
-        <v>234988</v>
+        <v>235169</v>
       </c>
       <c r="K163" t="n">
         <v>62159</v>
@@ -6104,7 +6104,7 @@
         <v>73</v>
       </c>
       <c r="F164" t="n">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="G164" t="n">
         <v>65</v>
@@ -6113,10 +6113,10 @@
         <v>28849</v>
       </c>
       <c r="I164" t="n">
-        <v>103626</v>
+        <v>103627</v>
       </c>
       <c r="J164" t="n">
-        <v>215193</v>
+        <v>215374</v>
       </c>
       <c r="K164" t="n">
         <v>35724</v>
@@ -6130,7 +6130,7 @@
         <v>18</v>
       </c>
       <c r="C165" t="n">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D165" t="n">
         <v>1</v>
@@ -6139,7 +6139,7 @@
         <v>1073</v>
       </c>
       <c r="F165" t="n">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="G165" t="n">
         <v>65</v>
@@ -6148,10 +6148,10 @@
         <v>27008</v>
       </c>
       <c r="I165" t="n">
-        <v>110633</v>
+        <v>110635</v>
       </c>
       <c r="J165" t="n">
-        <v>224021</v>
+        <v>224202</v>
       </c>
       <c r="K165" t="n">
         <v>31920</v>
@@ -6174,7 +6174,7 @@
         <v>1250</v>
       </c>
       <c r="F166" t="n">
-        <v>919</v>
+        <v>922</v>
       </c>
       <c r="G166" t="n">
         <v>135</v>
@@ -6183,10 +6183,10 @@
         <v>33852</v>
       </c>
       <c r="I166" t="n">
-        <v>114036</v>
+        <v>114038</v>
       </c>
       <c r="J166" t="n">
-        <v>254924</v>
+        <v>255107</v>
       </c>
       <c r="K166" t="n">
         <v>67236</v>
@@ -6209,7 +6209,7 @@
         <v>1355</v>
       </c>
       <c r="F167" t="n">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="G167" t="n">
         <v>125</v>
@@ -6218,10 +6218,10 @@
         <v>33858</v>
       </c>
       <c r="I167" t="n">
-        <v>115321</v>
+        <v>115323</v>
       </c>
       <c r="J167" t="n">
-        <v>256062</v>
+        <v>256244</v>
       </c>
       <c r="K167" t="n">
         <v>67415</v>
@@ -6235,7 +6235,7 @@
         <v>23</v>
       </c>
       <c r="C168" t="n">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="D168" t="n">
         <v>523</v>
@@ -6244,7 +6244,7 @@
         <v>1591</v>
       </c>
       <c r="F168" t="n">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="G168" t="n">
         <v>132</v>
@@ -6253,10 +6253,10 @@
         <v>33864</v>
       </c>
       <c r="I168" t="n">
-        <v>109686</v>
+        <v>109689</v>
       </c>
       <c r="J168" t="n">
-        <v>257398</v>
+        <v>257582</v>
       </c>
       <c r="K168" t="n">
         <v>67567</v>
@@ -6279,7 +6279,7 @@
         <v>192</v>
       </c>
       <c r="F169" t="n">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="G169" t="n">
         <v>129</v>
@@ -6288,10 +6288,10 @@
         <v>33657</v>
       </c>
       <c r="I169" t="n">
-        <v>111003</v>
+        <v>111006</v>
       </c>
       <c r="J169" t="n">
-        <v>258934</v>
+        <v>259120</v>
       </c>
       <c r="K169" t="n">
         <v>62774</v>
@@ -6308,13 +6308,13 @@
         <v>1554</v>
       </c>
       <c r="D170" t="n">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E170" t="n">
         <v>304</v>
       </c>
       <c r="F170" t="n">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="G170" t="n">
         <v>128</v>
@@ -6323,10 +6323,10 @@
         <v>33298</v>
       </c>
       <c r="I170" t="n">
-        <v>116101</v>
+        <v>116103</v>
       </c>
       <c r="J170" t="n">
-        <v>256707</v>
+        <v>256896</v>
       </c>
       <c r="K170" t="n">
         <v>66142</v>
@@ -6349,7 +6349,7 @@
         <v>218</v>
       </c>
       <c r="F171" t="n">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="G171" t="n">
         <v>75</v>
@@ -6358,10 +6358,10 @@
         <v>19297</v>
       </c>
       <c r="I171" t="n">
-        <v>114410</v>
+        <v>114412</v>
       </c>
       <c r="J171" t="n">
-        <v>227562</v>
+        <v>227752</v>
       </c>
       <c r="K171" t="n">
         <v>35666</v>
@@ -6384,7 +6384,7 @@
         <v>2675</v>
       </c>
       <c r="F172" t="n">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="G172" t="n">
         <v>78</v>
@@ -6393,10 +6393,10 @@
         <v>26675</v>
       </c>
       <c r="I172" t="n">
-        <v>123311</v>
+        <v>123313</v>
       </c>
       <c r="J172" t="n">
-        <v>228606</v>
+        <v>228797</v>
       </c>
       <c r="K172" t="n">
         <v>32040</v>
@@ -6419,7 +6419,7 @@
         <v>3040</v>
       </c>
       <c r="F173" t="n">
-        <v>1080</v>
+        <v>1082</v>
       </c>
       <c r="G173" t="n">
         <v>138</v>
@@ -6428,10 +6428,10 @@
         <v>33899</v>
       </c>
       <c r="I173" t="n">
-        <v>127462</v>
+        <v>127464</v>
       </c>
       <c r="J173" t="n">
-        <v>262467</v>
+        <v>262661</v>
       </c>
       <c r="K173" t="n">
         <v>65273</v>
@@ -6445,7 +6445,7 @@
         <v>69</v>
       </c>
       <c r="C174" t="n">
-        <v>1877</v>
+        <v>1878</v>
       </c>
       <c r="D174" t="n">
         <v>350</v>
@@ -6454,7 +6454,7 @@
         <v>3339</v>
       </c>
       <c r="F174" t="n">
-        <v>1119</v>
+        <v>1121</v>
       </c>
       <c r="G174" t="n">
         <v>143</v>
@@ -6463,10 +6463,10 @@
         <v>33915</v>
       </c>
       <c r="I174" t="n">
-        <v>129221</v>
+        <v>129224</v>
       </c>
       <c r="J174" t="n">
-        <v>264545</v>
+        <v>264742</v>
       </c>
       <c r="K174" t="n">
         <v>63702</v>
@@ -6489,7 +6489,7 @@
         <v>3762</v>
       </c>
       <c r="F175" t="n">
-        <v>1128</v>
+        <v>1130</v>
       </c>
       <c r="G175" t="n">
         <v>156</v>
@@ -6498,10 +6498,10 @@
         <v>33923</v>
       </c>
       <c r="I175" t="n">
-        <v>131487</v>
+        <v>131490</v>
       </c>
       <c r="J175" t="n">
-        <v>266936</v>
+        <v>267137</v>
       </c>
       <c r="K175" t="n">
         <v>71182</v>
@@ -6524,7 +6524,7 @@
         <v>4087</v>
       </c>
       <c r="F176" t="n">
-        <v>1129</v>
+        <v>1131</v>
       </c>
       <c r="G176" t="n">
         <v>157</v>
@@ -6533,10 +6533,10 @@
         <v>30850</v>
       </c>
       <c r="I176" t="n">
-        <v>133397</v>
+        <v>133400</v>
       </c>
       <c r="J176" t="n">
-        <v>250505</v>
+        <v>250708</v>
       </c>
       <c r="K176" t="n">
         <v>63993</v>
@@ -6559,7 +6559,7 @@
         <v>602</v>
       </c>
       <c r="F177" t="n">
-        <v>1191</v>
+        <v>1193</v>
       </c>
       <c r="G177" t="n">
         <v>175</v>
@@ -6568,10 +6568,10 @@
         <v>33725</v>
       </c>
       <c r="I177" t="n">
-        <v>125390</v>
+        <v>125393</v>
       </c>
       <c r="J177" t="n">
-        <v>271672</v>
+        <v>271879</v>
       </c>
       <c r="K177" t="n">
         <v>66390</v>
@@ -6594,7 +6594,7 @@
         <v>601</v>
       </c>
       <c r="F178" t="n">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="G178" t="n">
         <v>114</v>
@@ -6603,10 +6603,10 @@
         <v>19378</v>
       </c>
       <c r="I178" t="n">
-        <v>104392</v>
+        <v>104395</v>
       </c>
       <c r="J178" t="n">
-        <v>239612</v>
+        <v>239819</v>
       </c>
       <c r="K178" t="n">
         <v>37038</v>
@@ -6629,19 +6629,19 @@
         <v>4916</v>
       </c>
       <c r="F179" t="n">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="G179" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H179" t="n">
         <v>19607</v>
       </c>
       <c r="I179" t="n">
-        <v>115724</v>
+        <v>115727</v>
       </c>
       <c r="J179" t="n">
-        <v>240935</v>
+        <v>241142</v>
       </c>
       <c r="K179" t="n">
         <v>38920</v>
@@ -6655,7 +6655,7 @@
         <v>13</v>
       </c>
       <c r="C180" t="n">
-        <v>1749</v>
+        <v>1750</v>
       </c>
       <c r="D180" t="n">
         <v>151</v>
@@ -6664,19 +6664,19 @@
         <v>5373</v>
       </c>
       <c r="F180" t="n">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="G180" t="n">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H180" t="n">
         <v>33832</v>
       </c>
       <c r="I180" t="n">
-        <v>115714</v>
+        <v>115718</v>
       </c>
       <c r="J180" t="n">
-        <v>274335</v>
+        <v>274546</v>
       </c>
       <c r="K180" t="n">
         <v>68557</v>
@@ -6699,19 +6699,19 @@
         <v>815</v>
       </c>
       <c r="F181" t="n">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="G181" t="n">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H181" t="n">
         <v>33779</v>
       </c>
       <c r="I181" t="n">
-        <v>110031</v>
+        <v>110035</v>
       </c>
       <c r="J181" t="n">
-        <v>272737</v>
+        <v>272949</v>
       </c>
       <c r="K181" t="n">
         <v>66832</v>
@@ -6734,19 +6734,19 @@
         <v>6579</v>
       </c>
       <c r="F182" t="n">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="G182" t="n">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H182" t="n">
         <v>34012</v>
       </c>
       <c r="I182" t="n">
-        <v>123586</v>
+        <v>123590</v>
       </c>
       <c r="J182" t="n">
-        <v>282012</v>
+        <v>282227</v>
       </c>
       <c r="K182" t="n">
         <v>72283</v>
@@ -6769,19 +6769,19 @@
         <v>914</v>
       </c>
       <c r="F183" t="n">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="G183" t="n">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="H183" t="n">
         <v>33813</v>
       </c>
       <c r="I183" t="n">
-        <v>113121</v>
+        <v>113125</v>
       </c>
       <c r="J183" t="n">
-        <v>287700</v>
+        <v>287920</v>
       </c>
       <c r="K183" t="n">
         <v>67291</v>
@@ -6804,19 +6804,19 @@
         <v>1063</v>
       </c>
       <c r="F184" t="n">
-        <v>1661</v>
+        <v>1663</v>
       </c>
       <c r="G184" t="n">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H184" t="n">
         <v>33826</v>
       </c>
       <c r="I184" t="n">
-        <v>114766</v>
+        <v>114770</v>
       </c>
       <c r="J184" t="n">
-        <v>291186</v>
+        <v>291411</v>
       </c>
       <c r="K184" t="n">
         <v>67449</v>
@@ -6839,19 +6839,19 @@
         <v>11</v>
       </c>
       <c r="F185" t="n">
-        <v>1354</v>
+        <v>1356</v>
       </c>
       <c r="G185" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H185" t="n">
         <v>19303</v>
       </c>
       <c r="I185" t="n">
-        <v>110215</v>
+        <v>110219</v>
       </c>
       <c r="J185" t="n">
-        <v>254041</v>
+        <v>254269</v>
       </c>
       <c r="K185" t="n">
         <v>31834</v>
@@ -6874,19 +6874,19 @@
         <v>8526</v>
       </c>
       <c r="F186" t="n">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="G186" t="n">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H186" t="n">
         <v>19553</v>
       </c>
       <c r="I186" t="n">
-        <v>123742</v>
+        <v>123746</v>
       </c>
       <c r="J186" t="n">
-        <v>255671</v>
+        <v>255899</v>
       </c>
       <c r="K186" t="n">
         <v>39603</v>
@@ -6903,25 +6903,25 @@
         <v>2162</v>
       </c>
       <c r="D187" t="n">
-        <v>63873</v>
+        <v>63872</v>
       </c>
       <c r="E187" t="n">
         <v>9811</v>
       </c>
       <c r="F187" t="n">
-        <v>2075</v>
+        <v>2077</v>
       </c>
       <c r="G187" t="n">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H187" t="n">
         <v>31009</v>
       </c>
       <c r="I187" t="n">
-        <v>132176</v>
+        <v>132179</v>
       </c>
       <c r="J187" t="n">
-        <v>298316</v>
+        <v>298549</v>
       </c>
       <c r="K187" t="n">
         <v>73439</v>
@@ -6944,19 +6944,19 @@
         <v>10355</v>
       </c>
       <c r="F188" t="n">
-        <v>2135</v>
+        <v>2137</v>
       </c>
       <c r="G188" t="n">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H188" t="n">
         <v>34118</v>
       </c>
       <c r="I188" t="n">
-        <v>134092</v>
+        <v>134095</v>
       </c>
       <c r="J188" t="n">
-        <v>302038</v>
+        <v>302280</v>
       </c>
       <c r="K188" t="n">
         <v>73686</v>
@@ -6970,7 +6970,7 @@
         <v>230</v>
       </c>
       <c r="C189" t="n">
-        <v>2316</v>
+        <v>2317</v>
       </c>
       <c r="D189" t="n">
         <v>63930</v>
@@ -6979,19 +6979,19 @@
         <v>10698</v>
       </c>
       <c r="F189" t="n">
-        <v>2140</v>
+        <v>2142</v>
       </c>
       <c r="G189" t="n">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H189" t="n">
         <v>34135</v>
       </c>
       <c r="I189" t="n">
-        <v>136044</v>
+        <v>136048</v>
       </c>
       <c r="J189" t="n">
-        <v>305955</v>
+        <v>306199</v>
       </c>
       <c r="K189" t="n">
         <v>74403</v>
@@ -7014,19 +7014,19 @@
         <v>11367</v>
       </c>
       <c r="F190" t="n">
-        <v>2186</v>
+        <v>2187</v>
       </c>
       <c r="G190" t="n">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="H190" t="n">
         <v>34155</v>
       </c>
       <c r="I190" t="n">
-        <v>138075</v>
+        <v>138079</v>
       </c>
       <c r="J190" t="n">
-        <v>310293</v>
+        <v>310541</v>
       </c>
       <c r="K190" t="n">
         <v>74743</v>
@@ -7040,7 +7040,7 @@
         <v>461</v>
       </c>
       <c r="C191" t="n">
-        <v>2845</v>
+        <v>2846</v>
       </c>
       <c r="D191" t="n">
         <v>63997</v>
@@ -7049,19 +7049,19 @@
         <v>1997</v>
       </c>
       <c r="F191" t="n">
-        <v>2234</v>
+        <v>2236</v>
       </c>
       <c r="G191" t="n">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="H191" t="n">
         <v>33933</v>
       </c>
       <c r="I191" t="n">
-        <v>122584</v>
+        <v>122589</v>
       </c>
       <c r="J191" t="n">
-        <v>315201</v>
+        <v>315463</v>
       </c>
       <c r="K191" t="n">
         <v>68675</v>
@@ -7075,7 +7075,7 @@
         <v>282</v>
       </c>
       <c r="C192" t="n">
-        <v>1602</v>
+        <v>1603</v>
       </c>
       <c r="D192" t="n">
         <v>64006</v>
@@ -7084,19 +7084,19 @@
         <v>344</v>
       </c>
       <c r="F192" t="n">
-        <v>1493</v>
+        <v>1495</v>
       </c>
       <c r="G192" t="n">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H192" t="n">
         <v>19557</v>
       </c>
       <c r="I192" t="n">
-        <v>120519</v>
+        <v>120525</v>
       </c>
       <c r="J192" t="n">
-        <v>281080</v>
+        <v>281345</v>
       </c>
       <c r="K192" t="n">
         <v>34613</v>
@@ -7119,19 +7119,19 @@
         <v>11209</v>
       </c>
       <c r="F193" t="n">
-        <v>1665</v>
+        <v>1667</v>
       </c>
       <c r="G193" t="n">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H193" t="n">
         <v>19826</v>
       </c>
       <c r="I193" t="n">
-        <v>139285</v>
+        <v>139291</v>
       </c>
       <c r="J193" t="n">
-        <v>280213</v>
+        <v>280480</v>
       </c>
       <c r="K193" t="n">
         <v>41061</v>
@@ -7145,28 +7145,28 @@
         <v>311</v>
       </c>
       <c r="C194" t="n">
-        <v>2982</v>
+        <v>2983</v>
       </c>
       <c r="D194" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E194" t="n">
         <v>12286</v>
       </c>
       <c r="F194" t="n">
-        <v>2472</v>
+        <v>2473</v>
       </c>
       <c r="G194" t="n">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="H194" t="n">
         <v>33749</v>
       </c>
       <c r="I194" t="n">
-        <v>139732</v>
+        <v>139738</v>
       </c>
       <c r="J194" t="n">
-        <v>321040</v>
+        <v>321325</v>
       </c>
       <c r="K194" t="n">
         <v>65579</v>
@@ -7180,7 +7180,7 @@
         <v>951</v>
       </c>
       <c r="C195" t="n">
-        <v>2597</v>
+        <v>2598</v>
       </c>
       <c r="D195" t="n">
         <v>64117</v>
@@ -7189,19 +7189,19 @@
         <v>13771</v>
       </c>
       <c r="F195" t="n">
-        <v>2656</v>
+        <v>2657</v>
       </c>
       <c r="G195" t="n">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="H195" t="n">
         <v>34294</v>
       </c>
       <c r="I195" t="n">
-        <v>146395</v>
+        <v>146402</v>
       </c>
       <c r="J195" t="n">
-        <v>329543</v>
+        <v>329858</v>
       </c>
       <c r="K195" t="n">
         <v>69652</v>
@@ -7215,7 +7215,7 @@
         <v>579</v>
       </c>
       <c r="C196" t="n">
-        <v>2922</v>
+        <v>2921</v>
       </c>
       <c r="D196" t="n">
         <v>64155</v>
@@ -7224,19 +7224,19 @@
         <v>14167</v>
       </c>
       <c r="F196" t="n">
-        <v>2704</v>
+        <v>2705</v>
       </c>
       <c r="G196" t="n">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="H196" t="n">
-        <v>34325</v>
+        <v>34324</v>
       </c>
       <c r="I196" t="n">
-        <v>148527</v>
+        <v>148533</v>
       </c>
       <c r="J196" t="n">
-        <v>334860</v>
+        <v>335198</v>
       </c>
       <c r="K196" t="n">
         <v>70569</v>
@@ -7250,7 +7250,7 @@
         <v>660</v>
       </c>
       <c r="C197" t="n">
-        <v>3038</v>
+        <v>3037</v>
       </c>
       <c r="D197" t="n">
         <v>64225</v>
@@ -7259,19 +7259,19 @@
         <v>14874</v>
       </c>
       <c r="F197" t="n">
-        <v>2837</v>
+        <v>2838</v>
       </c>
       <c r="G197" t="n">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="H197" t="n">
-        <v>34351</v>
+        <v>34349</v>
       </c>
       <c r="I197" t="n">
-        <v>150807</v>
+        <v>150812</v>
       </c>
       <c r="J197" t="n">
-        <v>340781</v>
+        <v>341141</v>
       </c>
       <c r="K197" t="n">
         <v>71202</v>
@@ -7285,28 +7285,28 @@
         <v>579</v>
       </c>
       <c r="C198" t="n">
-        <v>3459</v>
+        <v>3449</v>
       </c>
       <c r="D198" t="n">
-        <v>64232</v>
+        <v>64231</v>
       </c>
       <c r="E198" t="n">
         <v>3729</v>
       </c>
       <c r="F198" t="n">
-        <v>2957</v>
+        <v>2419</v>
       </c>
       <c r="G198" t="n">
-        <v>381</v>
+        <v>272</v>
       </c>
       <c r="H198" t="n">
-        <v>33313</v>
+        <v>20542</v>
       </c>
       <c r="I198" t="n">
-        <v>132450</v>
+        <v>132444</v>
       </c>
       <c r="J198" t="n">
-        <v>347465</v>
+        <v>347945</v>
       </c>
       <c r="K198" t="n">
         <v>63953</v>
@@ -7320,7 +7320,7 @@
         <v>539</v>
       </c>
       <c r="C199" t="n">
-        <v>1942</v>
+        <v>1907</v>
       </c>
       <c r="D199" t="n">
         <v>64260</v>
@@ -7329,19 +7329,19 @@
         <v>962</v>
       </c>
       <c r="F199" t="n">
-        <v>1876</v>
+        <v>1301</v>
       </c>
       <c r="G199" t="n">
-        <v>250</v>
+        <v>139</v>
       </c>
       <c r="H199" t="n">
-        <v>18898</v>
+        <v>6120</v>
       </c>
       <c r="I199" t="n">
-        <v>129347</v>
+        <v>129306</v>
       </c>
       <c r="J199" t="n">
-        <v>307218</v>
+        <v>307722</v>
       </c>
       <c r="K199" t="n">
         <v>35129</v>
@@ -7355,7 +7355,7 @@
         <v>273</v>
       </c>
       <c r="C200" t="n">
-        <v>1288</v>
+        <v>1265</v>
       </c>
       <c r="D200" t="n">
         <v>64261</v>
@@ -7364,19 +7364,19 @@
         <v>1103</v>
       </c>
       <c r="F200" t="n">
-        <v>1987</v>
+        <v>1370</v>
       </c>
       <c r="G200" t="n">
-        <v>271</v>
+        <v>152</v>
       </c>
       <c r="H200" t="n">
-        <v>18907</v>
+        <v>6126</v>
       </c>
       <c r="I200" t="n">
-        <v>130170</v>
+        <v>130106</v>
       </c>
       <c r="J200" t="n">
-        <v>309636</v>
+        <v>310128</v>
       </c>
       <c r="K200" t="n">
         <v>35293</v>
@@ -7390,7 +7390,7 @@
         <v>415</v>
       </c>
       <c r="C201" t="n">
-        <v>3054</v>
+        <v>3306</v>
       </c>
       <c r="D201" t="n">
         <v>64345</v>
@@ -7399,19 +7399,19 @@
         <v>16406</v>
       </c>
       <c r="F201" t="n">
-        <v>2885</v>
+        <v>2888</v>
       </c>
       <c r="G201" t="n">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="H201" t="n">
         <v>21147</v>
       </c>
       <c r="I201" t="n">
-        <v>157930</v>
+        <v>158118</v>
       </c>
       <c r="J201" t="n">
-        <v>354547</v>
+        <v>355332</v>
       </c>
       <c r="K201" t="n">
         <v>69386</v>
@@ -7425,31 +7425,31 @@
         <v>912</v>
       </c>
       <c r="C202" t="n">
-        <v>1779</v>
+        <v>2710</v>
       </c>
       <c r="D202" t="n">
-        <v>58</v>
+        <v>64395</v>
       </c>
       <c r="E202" t="n">
-        <v>2753</v>
+        <v>4479</v>
       </c>
       <c r="F202" t="n">
-        <v>2784</v>
+        <v>3008</v>
       </c>
       <c r="G202" t="n">
-        <v>304</v>
+        <v>334</v>
       </c>
       <c r="H202" t="n">
-        <v>16611</v>
+        <v>20078</v>
       </c>
       <c r="I202" t="n">
-        <v>126856</v>
+        <v>137552</v>
       </c>
       <c r="J202" t="n">
-        <v>311038</v>
+        <v>338889</v>
       </c>
       <c r="K202" t="n">
-        <v>57258</v>
+        <v>61111</v>
       </c>
     </row>
     <row r="203">
@@ -7460,31 +7460,66 @@
         <v>670</v>
       </c>
       <c r="C203" t="n">
-        <v>932</v>
+        <v>1678</v>
       </c>
       <c r="D203" t="n">
-        <v>0</v>
+        <v>64473</v>
       </c>
       <c r="E203" t="n">
         <v>2978</v>
       </c>
       <c r="F203" t="n">
-        <v>2526</v>
+        <v>3166</v>
       </c>
       <c r="G203" t="n">
-        <v>280</v>
+        <v>338</v>
       </c>
       <c r="H203" t="n">
-        <v>16084</v>
+        <v>20092</v>
       </c>
       <c r="I203" t="n">
-        <v>22904</v>
+        <v>138343</v>
       </c>
       <c r="J203" t="n">
-        <v>86672</v>
+        <v>319449</v>
       </c>
       <c r="K203" t="n">
-        <v>57259</v>
+        <v>57789</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="n">
+        <v>44063</v>
+      </c>
+      <c r="B204" t="n">
+        <v>781</v>
+      </c>
+      <c r="C204" t="n">
+        <v>544</v>
+      </c>
+      <c r="D204" t="n">
+        <v>0</v>
+      </c>
+      <c r="E204" t="n">
+        <v>3160</v>
+      </c>
+      <c r="F204" t="n">
+        <v>2343</v>
+      </c>
+      <c r="G204" t="n">
+        <v>261</v>
+      </c>
+      <c r="H204" t="n">
+        <v>15477</v>
+      </c>
+      <c r="I204" t="n">
+        <v>9590</v>
+      </c>
+      <c r="J204" t="n">
+        <v>89275</v>
+      </c>
+      <c r="K204" t="n">
+        <v>56406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualiza provincias 2002.08.27 I
</commit_message>
<xml_diff>
--- a/data/output/covid19-spain_consolidated.xlsx
+++ b/data/output/covid19-spain_consolidated.xlsx
@@ -2664,7 +2664,7 @@
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G33" t="n">
         <v>12</v>
@@ -2738,7 +2738,7 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="G34" t="n">
         <v>13</v>
@@ -2812,7 +2812,7 @@
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="G35" t="n">
         <v>15</v>
@@ -2886,7 +2886,7 @@
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G36" t="n">
         <v>16</v>
@@ -2960,7 +2960,7 @@
         <v>8</v>
       </c>
       <c r="F37" t="n">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G37" t="n">
         <v>15</v>
@@ -3034,7 +3034,7 @@
         <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G38" t="n">
         <v>16</v>
@@ -3108,7 +3108,7 @@
         <v>19</v>
       </c>
       <c r="F39" t="n">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="G39" t="n">
         <v>18</v>
@@ -3182,7 +3182,7 @@
         <v>28</v>
       </c>
       <c r="F40" t="n">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="G40" t="n">
         <v>20</v>
@@ -3256,7 +3256,7 @@
         <v>33</v>
       </c>
       <c r="F41" t="n">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="G41" t="n">
         <v>27</v>
@@ -3330,7 +3330,7 @@
         <v>43</v>
       </c>
       <c r="F42" t="n">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="G42" t="n">
         <v>33</v>
@@ -3404,7 +3404,7 @@
         <v>54</v>
       </c>
       <c r="F43" t="n">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="G43" t="n">
         <v>38</v>
@@ -6142,7 +6142,7 @@
         <v>10437</v>
       </c>
       <c r="F80" t="n">
-        <v>19979</v>
+        <v>19980</v>
       </c>
       <c r="G80" t="n">
         <v>2464</v>
@@ -6216,7 +6216,7 @@
         <v>10241</v>
       </c>
       <c r="F81" t="n">
-        <v>19541</v>
+        <v>19542</v>
       </c>
       <c r="G81" t="n">
         <v>2475</v>
@@ -6364,7 +6364,7 @@
         <v>10149</v>
       </c>
       <c r="F83" t="n">
-        <v>18917</v>
+        <v>18918</v>
       </c>
       <c r="G83" t="n">
         <v>2348</v>
@@ -6438,7 +6438,7 @@
         <v>9642</v>
       </c>
       <c r="F84" t="n">
-        <v>18032</v>
+        <v>18033</v>
       </c>
       <c r="G84" t="n">
         <v>2255</v>
@@ -6512,7 +6512,7 @@
         <v>9325</v>
       </c>
       <c r="F85" t="n">
-        <v>17140</v>
+        <v>17141</v>
       </c>
       <c r="G85" t="n">
         <v>2194</v>
@@ -6586,7 +6586,7 @@
         <v>19892</v>
       </c>
       <c r="F86" t="n">
-        <v>16368</v>
+        <v>16369</v>
       </c>
       <c r="G86" t="n">
         <v>2108</v>
@@ -6660,7 +6660,7 @@
         <v>20059</v>
       </c>
       <c r="F87" t="n">
-        <v>16667</v>
+        <v>16668</v>
       </c>
       <c r="G87" t="n">
         <v>2235</v>
@@ -6734,7 +6734,7 @@
         <v>20137</v>
       </c>
       <c r="F88" t="n">
-        <v>16181</v>
+        <v>16182</v>
       </c>
       <c r="G88" t="n">
         <v>2185</v>
@@ -6808,7 +6808,7 @@
         <v>20114</v>
       </c>
       <c r="F89" t="n">
-        <v>16069</v>
+        <v>16070</v>
       </c>
       <c r="G89" t="n">
         <v>2188</v>
@@ -6882,7 +6882,7 @@
         <v>19056</v>
       </c>
       <c r="F90" t="n">
-        <v>15550</v>
+        <v>15551</v>
       </c>
       <c r="G90" t="n">
         <v>2042</v>
@@ -6956,7 +6956,7 @@
         <v>20627</v>
       </c>
       <c r="F91" t="n">
-        <v>14974</v>
+        <v>14975</v>
       </c>
       <c r="G91" t="n">
         <v>1975</v>
@@ -7030,7 +7030,7 @@
         <v>19386</v>
       </c>
       <c r="F92" t="n">
-        <v>14353</v>
+        <v>14354</v>
       </c>
       <c r="G92" t="n">
         <v>1868</v>
@@ -7474,7 +7474,7 @@
         <v>16806</v>
       </c>
       <c r="F98" t="n">
-        <v>13679</v>
+        <v>13680</v>
       </c>
       <c r="G98" t="n">
         <v>1901</v>
@@ -8436,7 +8436,7 @@
         <v>1564</v>
       </c>
       <c r="F111" t="n">
-        <v>9238</v>
+        <v>9239</v>
       </c>
       <c r="G111" t="n">
         <v>1231</v>
@@ -8732,7 +8732,7 @@
         <v>1322</v>
       </c>
       <c r="F115" t="n">
-        <v>8054</v>
+        <v>8055</v>
       </c>
       <c r="G115" t="n">
         <v>704</v>
@@ -8806,7 +8806,7 @@
         <v>1322</v>
       </c>
       <c r="F116" t="n">
-        <v>7942</v>
+        <v>7943</v>
       </c>
       <c r="G116" t="n">
         <v>677</v>
@@ -8880,7 +8880,7 @@
         <v>1647</v>
       </c>
       <c r="F117" t="n">
-        <v>7885</v>
+        <v>7886</v>
       </c>
       <c r="G117" t="n">
         <v>658</v>
@@ -8954,7 +8954,7 @@
         <v>1213</v>
       </c>
       <c r="F118" t="n">
-        <v>7731</v>
+        <v>7732</v>
       </c>
       <c r="G118" t="n">
         <v>644</v>
@@ -9028,7 +9028,7 @@
         <v>1143</v>
       </c>
       <c r="F119" t="n">
-        <v>3239</v>
+        <v>3241</v>
       </c>
       <c r="G119" t="n">
         <v>597</v>
@@ -9102,7 +9102,7 @@
         <v>859</v>
       </c>
       <c r="F120" t="n">
-        <v>3042</v>
+        <v>3044</v>
       </c>
       <c r="G120" t="n">
         <v>534</v>
@@ -9176,7 +9176,7 @@
         <v>1652</v>
       </c>
       <c r="F121" t="n">
-        <v>2868</v>
+        <v>2869</v>
       </c>
       <c r="G121" t="n">
         <v>529</v>
@@ -9250,7 +9250,7 @@
         <v>1595</v>
       </c>
       <c r="F122" t="n">
-        <v>2731</v>
+        <v>2732</v>
       </c>
       <c r="G122" t="n">
         <v>508</v>
@@ -9324,7 +9324,7 @@
         <v>1565</v>
       </c>
       <c r="F123" t="n">
-        <v>2672</v>
+        <v>2673</v>
       </c>
       <c r="G123" t="n">
         <v>513</v>
@@ -9398,7 +9398,7 @@
         <v>1513</v>
       </c>
       <c r="F124" t="n">
-        <v>2697</v>
+        <v>2699</v>
       </c>
       <c r="G124" t="n">
         <v>508</v>
@@ -9472,7 +9472,7 @@
         <v>1321</v>
       </c>
       <c r="F125" t="n">
-        <v>2534</v>
+        <v>2535</v>
       </c>
       <c r="G125" t="n">
         <v>470</v>
@@ -9546,7 +9546,7 @@
         <v>1537</v>
       </c>
       <c r="F126" t="n">
-        <v>2342</v>
+        <v>2343</v>
       </c>
       <c r="G126" t="n">
         <v>444</v>
@@ -9620,7 +9620,7 @@
         <v>402</v>
       </c>
       <c r="F127" t="n">
-        <v>2106</v>
+        <v>2107</v>
       </c>
       <c r="G127" t="n">
         <v>422</v>
@@ -9694,7 +9694,7 @@
         <v>357</v>
       </c>
       <c r="F128" t="n">
-        <v>1937</v>
+        <v>1939</v>
       </c>
       <c r="G128" t="n">
         <v>400</v>
@@ -9768,7 +9768,7 @@
         <v>356</v>
       </c>
       <c r="F129" t="n">
-        <v>1859</v>
+        <v>1861</v>
       </c>
       <c r="G129" t="n">
         <v>401</v>
@@ -9842,7 +9842,7 @@
         <v>360</v>
       </c>
       <c r="F130" t="n">
-        <v>1846</v>
+        <v>1848</v>
       </c>
       <c r="G130" t="n">
         <v>400</v>
@@ -9916,7 +9916,7 @@
         <v>1085</v>
       </c>
       <c r="F131" t="n">
-        <v>1822</v>
+        <v>1825</v>
       </c>
       <c r="G131" t="n">
         <v>391</v>
@@ -9990,7 +9990,7 @@
         <v>1022</v>
       </c>
       <c r="F132" t="n">
-        <v>1757</v>
+        <v>1760</v>
       </c>
       <c r="G132" t="n">
         <v>372</v>
@@ -10064,7 +10064,7 @@
         <v>986</v>
       </c>
       <c r="F133" t="n">
-        <v>1688</v>
+        <v>1691</v>
       </c>
       <c r="G133" t="n">
         <v>334</v>
@@ -10138,7 +10138,7 @@
         <v>945</v>
       </c>
       <c r="F134" t="n">
-        <v>1528</v>
+        <v>1530</v>
       </c>
       <c r="G134" t="n">
         <v>333</v>
@@ -10212,7 +10212,7 @@
         <v>300</v>
       </c>
       <c r="F135" t="n">
-        <v>1437</v>
+        <v>1439</v>
       </c>
       <c r="G135" t="n">
         <v>322</v>
@@ -10286,7 +10286,7 @@
         <v>308</v>
       </c>
       <c r="F136" t="n">
-        <v>1379</v>
+        <v>1381</v>
       </c>
       <c r="G136" t="n">
         <v>292</v>
@@ -10360,7 +10360,7 @@
         <v>299</v>
       </c>
       <c r="F137" t="n">
-        <v>1380</v>
+        <v>1382</v>
       </c>
       <c r="G137" t="n">
         <v>284</v>
@@ -10434,7 +10434,7 @@
         <v>866</v>
       </c>
       <c r="F138" t="n">
-        <v>1373</v>
+        <v>1375</v>
       </c>
       <c r="G138" t="n">
         <v>299</v>
@@ -10508,7 +10508,7 @@
         <v>267</v>
       </c>
       <c r="F139" t="n">
-        <v>1363</v>
+        <v>1365</v>
       </c>
       <c r="G139" t="n">
         <v>288</v>
@@ -10582,10 +10582,10 @@
         <v>237</v>
       </c>
       <c r="F140" t="n">
-        <v>1291</v>
+        <v>1293</v>
       </c>
       <c r="G140" t="n">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="H140" t="n">
         <v>33553</v>
@@ -10656,10 +10656,10 @@
         <v>775</v>
       </c>
       <c r="F141" t="n">
-        <v>1260</v>
+        <v>1262</v>
       </c>
       <c r="G141" t="n">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H141" t="n">
         <v>33589</v>
@@ -10730,10 +10730,10 @@
         <v>226</v>
       </c>
       <c r="F142" t="n">
-        <v>1180</v>
+        <v>1183</v>
       </c>
       <c r="G142" t="n">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H142" t="n">
         <v>33596</v>
@@ -10804,7 +10804,7 @@
         <v>223</v>
       </c>
       <c r="F143" t="n">
-        <v>1166</v>
+        <v>1170</v>
       </c>
       <c r="G143" t="n">
         <v>225</v>
@@ -10878,7 +10878,7 @@
         <v>238</v>
       </c>
       <c r="F144" t="n">
-        <v>1156</v>
+        <v>1160</v>
       </c>
       <c r="G144" t="n">
         <v>230</v>
@@ -10952,7 +10952,7 @@
         <v>821</v>
       </c>
       <c r="F145" t="n">
-        <v>1165</v>
+        <v>1169</v>
       </c>
       <c r="G145" t="n">
         <v>212</v>
@@ -11026,7 +11026,7 @@
         <v>838</v>
       </c>
       <c r="F146" t="n">
-        <v>1133</v>
+        <v>1136</v>
       </c>
       <c r="G146" t="n">
         <v>203</v>
@@ -11100,7 +11100,7 @@
         <v>78</v>
       </c>
       <c r="F147" t="n">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="G147" t="n">
         <v>203</v>
@@ -11174,7 +11174,7 @@
         <v>896</v>
       </c>
       <c r="F148" t="n">
-        <v>1081</v>
+        <v>1084</v>
       </c>
       <c r="G148" t="n">
         <v>204</v>
@@ -11248,7 +11248,7 @@
         <v>216</v>
       </c>
       <c r="F149" t="n">
-        <v>1018</v>
+        <v>1021</v>
       </c>
       <c r="G149" t="n">
         <v>188</v>
@@ -11322,7 +11322,7 @@
         <v>76</v>
       </c>
       <c r="F150" t="n">
-        <v>1024</v>
+        <v>1027</v>
       </c>
       <c r="G150" t="n">
         <v>179</v>
@@ -11396,7 +11396,7 @@
         <v>76</v>
       </c>
       <c r="F151" t="n">
-        <v>1039</v>
+        <v>1042</v>
       </c>
       <c r="G151" t="n">
         <v>146</v>
@@ -11470,7 +11470,7 @@
         <v>211</v>
       </c>
       <c r="F152" t="n">
-        <v>1023</v>
+        <v>1026</v>
       </c>
       <c r="G152" t="n">
         <v>177</v>
@@ -11544,7 +11544,7 @@
         <v>203</v>
       </c>
       <c r="F153" t="n">
-        <v>1008</v>
+        <v>1011</v>
       </c>
       <c r="G153" t="n">
         <v>174</v>
@@ -11618,10 +11618,10 @@
         <v>207</v>
       </c>
       <c r="F154" t="n">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="G154" t="n">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H154" t="n">
         <v>33742</v>
@@ -11692,10 +11692,10 @@
         <v>205</v>
       </c>
       <c r="F155" t="n">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="G155" t="n">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H155" t="n">
         <v>33753</v>
@@ -11766,7 +11766,7 @@
         <v>203</v>
       </c>
       <c r="F156" t="n">
-        <v>893</v>
+        <v>896</v>
       </c>
       <c r="G156" t="n">
         <v>153</v>
@@ -11840,7 +11840,7 @@
         <v>63</v>
       </c>
       <c r="F157" t="n">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c r="G157" t="n">
         <v>73</v>
@@ -11914,7 +11914,7 @@
         <v>63</v>
       </c>
       <c r="F158" t="n">
-        <v>931</v>
+        <v>934</v>
       </c>
       <c r="G158" t="n">
         <v>61</v>
@@ -11988,7 +11988,7 @@
         <v>205</v>
       </c>
       <c r="F159" t="n">
-        <v>931</v>
+        <v>934</v>
       </c>
       <c r="G159" t="n">
         <v>146</v>
@@ -12062,7 +12062,7 @@
         <v>200</v>
       </c>
       <c r="F160" t="n">
-        <v>899</v>
+        <v>902</v>
       </c>
       <c r="G160" t="n">
         <v>144</v>
@@ -12136,7 +12136,7 @@
         <v>198</v>
       </c>
       <c r="F161" t="n">
-        <v>889</v>
+        <v>893</v>
       </c>
       <c r="G161" t="n">
         <v>132</v>
@@ -12210,7 +12210,7 @@
         <v>1091</v>
       </c>
       <c r="F162" t="n">
-        <v>860</v>
+        <v>864</v>
       </c>
       <c r="G162" t="n">
         <v>128</v>
@@ -12284,7 +12284,7 @@
         <v>198</v>
       </c>
       <c r="F163" t="n">
-        <v>831</v>
+        <v>836</v>
       </c>
       <c r="G163" t="n">
         <v>123</v>
@@ -12358,7 +12358,7 @@
         <v>73</v>
       </c>
       <c r="F164" t="n">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="G164" t="n">
         <v>65</v>
@@ -12432,7 +12432,7 @@
         <v>1073</v>
       </c>
       <c r="F165" t="n">
-        <v>886</v>
+        <v>890</v>
       </c>
       <c r="G165" t="n">
         <v>65</v>
@@ -12506,7 +12506,7 @@
         <v>1250</v>
       </c>
       <c r="F166" t="n">
-        <v>929</v>
+        <v>933</v>
       </c>
       <c r="G166" t="n">
         <v>135</v>
@@ -12580,7 +12580,7 @@
         <v>1355</v>
       </c>
       <c r="F167" t="n">
-        <v>955</v>
+        <v>959</v>
       </c>
       <c r="G167" t="n">
         <v>125</v>
@@ -12654,7 +12654,7 @@
         <v>1591</v>
       </c>
       <c r="F168" t="n">
-        <v>973</v>
+        <v>977</v>
       </c>
       <c r="G168" t="n">
         <v>132</v>
@@ -12728,7 +12728,7 @@
         <v>192</v>
       </c>
       <c r="F169" t="n">
-        <v>936</v>
+        <v>939</v>
       </c>
       <c r="G169" t="n">
         <v>129</v>
@@ -12802,7 +12802,7 @@
         <v>304</v>
       </c>
       <c r="F170" t="n">
-        <v>968</v>
+        <v>971</v>
       </c>
       <c r="G170" t="n">
         <v>128</v>
@@ -12876,7 +12876,7 @@
         <v>218</v>
       </c>
       <c r="F171" t="n">
-        <v>1018</v>
+        <v>1021</v>
       </c>
       <c r="G171" t="n">
         <v>75</v>
@@ -12950,7 +12950,7 @@
         <v>2675</v>
       </c>
       <c r="F172" t="n">
-        <v>1047</v>
+        <v>1051</v>
       </c>
       <c r="G172" t="n">
         <v>78</v>
@@ -13024,7 +13024,7 @@
         <v>3040</v>
       </c>
       <c r="F173" t="n">
-        <v>1087</v>
+        <v>1091</v>
       </c>
       <c r="G173" t="n">
         <v>138</v>
@@ -13098,7 +13098,7 @@
         <v>3339</v>
       </c>
       <c r="F174" t="n">
-        <v>1125</v>
+        <v>1129</v>
       </c>
       <c r="G174" t="n">
         <v>144</v>
@@ -13172,7 +13172,7 @@
         <v>3762</v>
       </c>
       <c r="F175" t="n">
-        <v>1134</v>
+        <v>1138</v>
       </c>
       <c r="G175" t="n">
         <v>157</v>
@@ -13246,7 +13246,7 @@
         <v>4087</v>
       </c>
       <c r="F176" t="n">
-        <v>1184</v>
+        <v>1186</v>
       </c>
       <c r="G176" t="n">
         <v>158</v>
@@ -13320,7 +13320,7 @@
         <v>602</v>
       </c>
       <c r="F177" t="n">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="G177" t="n">
         <v>176</v>
@@ -13394,7 +13394,7 @@
         <v>601</v>
       </c>
       <c r="F178" t="n">
-        <v>1257</v>
+        <v>1259</v>
       </c>
       <c r="G178" t="n">
         <v>115</v>
@@ -13468,7 +13468,7 @@
         <v>4916</v>
       </c>
       <c r="F179" t="n">
-        <v>1305</v>
+        <v>1307</v>
       </c>
       <c r="G179" t="n">
         <v>107</v>
@@ -13542,7 +13542,7 @@
         <v>5373</v>
       </c>
       <c r="F180" t="n">
-        <v>1411</v>
+        <v>1413</v>
       </c>
       <c r="G180" t="n">
         <v>198</v>
@@ -13616,7 +13616,7 @@
         <v>815</v>
       </c>
       <c r="F181" t="n">
-        <v>1510</v>
+        <v>1512</v>
       </c>
       <c r="G181" t="n">
         <v>214</v>
@@ -13690,7 +13690,7 @@
         <v>6579</v>
       </c>
       <c r="F182" t="n">
-        <v>1542</v>
+        <v>1544</v>
       </c>
       <c r="G182" t="n">
         <v>206</v>
@@ -13764,7 +13764,7 @@
         <v>914</v>
       </c>
       <c r="F183" t="n">
-        <v>1605</v>
+        <v>1607</v>
       </c>
       <c r="G183" t="n">
         <v>214</v>
@@ -13838,7 +13838,7 @@
         <v>1063</v>
       </c>
       <c r="F184" t="n">
-        <v>1670</v>
+        <v>1672</v>
       </c>
       <c r="G184" t="n">
         <v>216</v>
@@ -13912,7 +13912,7 @@
         <v>11</v>
       </c>
       <c r="F185" t="n">
-        <v>1745</v>
+        <v>1747</v>
       </c>
       <c r="G185" t="n">
         <v>155</v>
@@ -13986,7 +13986,7 @@
         <v>8526</v>
       </c>
       <c r="F186" t="n">
-        <v>1807</v>
+        <v>1809</v>
       </c>
       <c r="G186" t="n">
         <v>129</v>
@@ -14060,7 +14060,7 @@
         <v>9811</v>
       </c>
       <c r="F187" t="n">
-        <v>2085</v>
+        <v>2087</v>
       </c>
       <c r="G187" t="n">
         <v>255</v>
@@ -14134,7 +14134,7 @@
         <v>10355</v>
       </c>
       <c r="F188" t="n">
-        <v>2145</v>
+        <v>2147</v>
       </c>
       <c r="G188" t="n">
         <v>258</v>
@@ -14208,7 +14208,7 @@
         <v>10698</v>
       </c>
       <c r="F189" t="n">
-        <v>2150</v>
+        <v>2152</v>
       </c>
       <c r="G189" t="n">
         <v>262</v>
@@ -14282,7 +14282,7 @@
         <v>11367</v>
       </c>
       <c r="F190" t="n">
-        <v>2195</v>
+        <v>2197</v>
       </c>
       <c r="G190" t="n">
         <v>266</v>
@@ -14356,7 +14356,7 @@
         <v>1997</v>
       </c>
       <c r="F191" t="n">
-        <v>2244</v>
+        <v>2246</v>
       </c>
       <c r="G191" t="n">
         <v>277</v>
@@ -14430,7 +14430,7 @@
         <v>344</v>
       </c>
       <c r="F192" t="n">
-        <v>2271</v>
+        <v>2272</v>
       </c>
       <c r="G192" t="n">
         <v>189</v>
@@ -14504,7 +14504,7 @@
         <v>11209</v>
       </c>
       <c r="F193" t="n">
-        <v>2344</v>
+        <v>2346</v>
       </c>
       <c r="G193" t="n">
         <v>219</v>
@@ -14578,7 +14578,7 @@
         <v>12286</v>
       </c>
       <c r="F194" t="n">
-        <v>2553</v>
+        <v>2555</v>
       </c>
       <c r="G194" t="n">
         <v>318</v>
@@ -14652,7 +14652,7 @@
         <v>13771</v>
       </c>
       <c r="F195" t="n">
-        <v>2669</v>
+        <v>2671</v>
       </c>
       <c r="G195" t="n">
         <v>341</v>
@@ -14726,7 +14726,7 @@
         <v>14167</v>
       </c>
       <c r="F196" t="n">
-        <v>2713</v>
+        <v>2715</v>
       </c>
       <c r="G196" t="n">
         <v>350</v>
@@ -14800,7 +14800,7 @@
         <v>15048</v>
       </c>
       <c r="F197" t="n">
-        <v>2853</v>
+        <v>2855</v>
       </c>
       <c r="G197" t="n">
         <v>368</v>
@@ -14874,7 +14874,7 @@
         <v>3952</v>
       </c>
       <c r="F198" t="n">
-        <v>2968</v>
+        <v>2970</v>
       </c>
       <c r="G198" t="n">
         <v>384</v>
@@ -14948,7 +14948,7 @@
         <v>962</v>
       </c>
       <c r="F199" t="n">
-        <v>3025</v>
+        <v>3027</v>
       </c>
       <c r="G199" t="n">
         <v>253</v>
@@ -15022,7 +15022,7 @@
         <v>1396</v>
       </c>
       <c r="F200" t="n">
-        <v>3139</v>
+        <v>3141</v>
       </c>
       <c r="G200" t="n">
         <v>275</v>
@@ -15096,7 +15096,7 @@
         <v>16780</v>
       </c>
       <c r="F201" t="n">
-        <v>3556</v>
+        <v>3558</v>
       </c>
       <c r="G201" t="n">
         <v>451</v>
@@ -15170,7 +15170,7 @@
         <v>16980</v>
       </c>
       <c r="F202" t="n">
-        <v>3692</v>
+        <v>3694</v>
       </c>
       <c r="G202" t="n">
         <v>463</v>
@@ -15244,7 +15244,7 @@
         <v>15371</v>
       </c>
       <c r="F203" t="n">
-        <v>3863</v>
+        <v>3865</v>
       </c>
       <c r="G203" t="n">
         <v>464</v>
@@ -15318,13 +15318,13 @@
         <v>3714</v>
       </c>
       <c r="F204" t="n">
-        <v>3993</v>
+        <v>3995</v>
       </c>
       <c r="G204" t="n">
         <v>487</v>
       </c>
       <c r="H204" t="n">
-        <v>34571</v>
+        <v>34572</v>
       </c>
       <c r="I204" t="n">
         <v>142968</v>
@@ -15360,19 +15360,19 @@
         <v>5827.6</v>
       </c>
       <c r="T204" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="U204" t="n">
         <v>0.1</v>
       </c>
       <c r="V204" t="n">
-        <v>35</v>
+        <v>35.3</v>
       </c>
       <c r="W204" t="n">
-        <v>31.1</v>
+        <v>31.3</v>
       </c>
       <c r="X204" t="n">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="205">
@@ -15392,13 +15392,13 @@
         <v>3984</v>
       </c>
       <c r="F205" t="n">
-        <v>4066</v>
+        <v>4069</v>
       </c>
       <c r="G205" t="n">
         <v>512</v>
       </c>
       <c r="H205" t="n">
-        <v>34599</v>
+        <v>34600</v>
       </c>
       <c r="I205" t="n">
         <v>145373</v>
@@ -15440,13 +15440,13 @@
         <v>0.1</v>
       </c>
       <c r="V205" t="n">
-        <v>29.7</v>
+        <v>30</v>
       </c>
       <c r="W205" t="n">
-        <v>31.6</v>
+        <v>31.7</v>
       </c>
       <c r="X205" t="n">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="206">
@@ -15466,13 +15466,13 @@
         <v>2562</v>
       </c>
       <c r="F206" t="n">
-        <v>4073</v>
+        <v>4075</v>
       </c>
       <c r="G206" t="n">
         <v>312</v>
       </c>
       <c r="H206" t="n">
-        <v>34612</v>
+        <v>34614</v>
       </c>
       <c r="I206" t="n">
         <v>141301</v>
@@ -15508,19 +15508,19 @@
         <v>6172.3</v>
       </c>
       <c r="T206" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U206" t="n">
         <v>0</v>
       </c>
       <c r="V206" t="n">
-        <v>20.7</v>
+        <v>21.3</v>
       </c>
       <c r="W206" t="n">
-        <v>31.3</v>
+        <v>31.6</v>
       </c>
       <c r="X206" t="n">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="207">
@@ -15540,13 +15540,13 @@
         <v>14504</v>
       </c>
       <c r="F207" t="n">
-        <v>4136</v>
+        <v>4138</v>
       </c>
       <c r="G207" t="n">
         <v>318</v>
       </c>
       <c r="H207" t="n">
-        <v>34673</v>
+        <v>34675</v>
       </c>
       <c r="I207" t="n">
         <v>167082</v>
@@ -15588,13 +15588,13 @@
         <v>0.2</v>
       </c>
       <c r="V207" t="n">
-        <v>34</v>
+        <v>34.3</v>
       </c>
       <c r="W207" t="n">
-        <v>38.3</v>
+        <v>38.6</v>
       </c>
       <c r="X207" t="n">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="208">
@@ -15614,13 +15614,13 @@
         <v>15874</v>
       </c>
       <c r="F208" t="n">
-        <v>4689</v>
+        <v>4696</v>
       </c>
       <c r="G208" t="n">
-        <v>454</v>
+        <v>581</v>
       </c>
       <c r="H208" t="n">
-        <v>34730</v>
+        <v>34746</v>
       </c>
       <c r="I208" t="n">
         <v>174869</v>
@@ -15656,19 +15656,19 @@
         <v>6345.6</v>
       </c>
       <c r="T208" t="n">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="U208" t="n">
         <v>0.2</v>
       </c>
       <c r="V208" t="n">
-        <v>43.7</v>
+        <v>48.7</v>
       </c>
       <c r="W208" t="n">
-        <v>37.7</v>
+        <v>40</v>
       </c>
       <c r="X208" t="n">
-        <v>264</v>
+        <v>280</v>
       </c>
     </row>
     <row r="209">
@@ -15688,13 +15688,13 @@
         <v>5565</v>
       </c>
       <c r="F209" t="n">
-        <v>4852</v>
+        <v>4859</v>
       </c>
       <c r="G209" t="n">
         <v>481</v>
       </c>
       <c r="H209" t="n">
-        <v>34759</v>
+        <v>34775</v>
       </c>
       <c r="I209" t="n">
         <v>153174</v>
@@ -15736,13 +15736,13 @@
         <v>0.1</v>
       </c>
       <c r="V209" t="n">
-        <v>49</v>
+        <v>53.7</v>
       </c>
       <c r="W209" t="n">
-        <v>35.6</v>
+        <v>37.9</v>
       </c>
       <c r="X209" t="n">
-        <v>249</v>
+        <v>265</v>
       </c>
     </row>
     <row r="210">
@@ -15750,73 +15750,73 @@
         <v>44069</v>
       </c>
       <c r="B210" t="n">
-        <v>1100</v>
+        <v>1332</v>
       </c>
       <c r="C210" t="n">
         <v>3726</v>
       </c>
       <c r="D210" t="n">
-        <v>55</v>
+        <v>64782</v>
       </c>
       <c r="E210" t="n">
         <v>5968</v>
       </c>
       <c r="F210" t="n">
-        <v>4746</v>
+        <v>4920</v>
       </c>
       <c r="G210" t="n">
-        <v>483</v>
+        <v>507</v>
       </c>
       <c r="H210" t="n">
-        <v>33882</v>
+        <v>34056</v>
       </c>
       <c r="I210" t="n">
-        <v>143136</v>
+        <v>150505</v>
       </c>
       <c r="J210" t="n">
-        <v>410614</v>
+        <v>416277</v>
       </c>
       <c r="K210" t="n">
         <v>61777</v>
       </c>
       <c r="L210" t="n">
-        <v>-8379</v>
+        <v>-1010</v>
       </c>
       <c r="M210" t="n">
-        <v>168</v>
+        <v>7537</v>
       </c>
       <c r="N210" t="n">
-        <v>63958</v>
+        <v>69621</v>
       </c>
       <c r="O210" t="n">
-        <v>23165</v>
+        <v>28828</v>
       </c>
       <c r="P210" t="n">
-        <v>-10038</v>
+        <v>-2669</v>
       </c>
       <c r="Q210" t="n">
-        <v>-2986.6</v>
+        <v>-1933.9</v>
       </c>
       <c r="R210" t="n">
-        <v>-7821</v>
+        <v>-2158</v>
       </c>
       <c r="S210" t="n">
-        <v>4374.4</v>
+        <v>5183.4</v>
       </c>
       <c r="T210" t="n">
-        <v>-877</v>
+        <v>-719</v>
       </c>
       <c r="U210" t="n">
-        <v>-2.5</v>
+        <v>-2.1</v>
       </c>
       <c r="V210" t="n">
-        <v>-263.7</v>
+        <v>-206.3</v>
       </c>
       <c r="W210" t="n">
-        <v>-95.4</v>
+        <v>-70.6</v>
       </c>
       <c r="X210" t="n">
-        <v>-668</v>
+        <v>-494</v>
       </c>
     </row>
     <row r="211">
@@ -15824,73 +15824,147 @@
         <v>44070</v>
       </c>
       <c r="B211" t="n">
-        <v>1024</v>
+        <v>1362</v>
       </c>
       <c r="C211" t="n">
-        <v>991</v>
+        <v>2566</v>
       </c>
       <c r="D211" t="n">
         <v>10</v>
       </c>
       <c r="E211" t="n">
-        <v>3442</v>
+        <v>6566</v>
       </c>
       <c r="F211" t="n">
-        <v>3720</v>
+        <v>4311</v>
       </c>
       <c r="G211" t="n">
-        <v>353</v>
+        <v>415</v>
       </c>
       <c r="H211" t="n">
-        <v>32168</v>
+        <v>32223</v>
       </c>
       <c r="I211" t="n">
-        <v>138396</v>
+        <v>144264</v>
       </c>
       <c r="J211" t="n">
-        <v>322000</v>
+        <v>380034</v>
       </c>
       <c r="K211" t="n">
-        <v>60103</v>
+        <v>62676</v>
       </c>
       <c r="L211" t="n">
-        <v>5187</v>
+        <v>11055</v>
       </c>
       <c r="M211" t="n">
-        <v>-6977</v>
+        <v>-1109</v>
       </c>
       <c r="N211" t="n">
-        <v>-31710</v>
+        <v>26324</v>
       </c>
       <c r="O211" t="n">
-        <v>-73964</v>
+        <v>-15930</v>
       </c>
       <c r="P211" t="n">
-        <v>-4740</v>
+        <v>-6241</v>
       </c>
       <c r="Q211" t="n">
-        <v>-653.1</v>
+        <v>185.1</v>
       </c>
       <c r="R211" t="n">
-        <v>-88614</v>
+        <v>-36243</v>
       </c>
       <c r="S211" t="n">
-        <v>-9349.9</v>
+        <v>-1059.3</v>
       </c>
       <c r="T211" t="n">
-        <v>-1714</v>
+        <v>-1833</v>
       </c>
       <c r="U211" t="n">
-        <v>-5.1</v>
+        <v>-5.4</v>
       </c>
       <c r="V211" t="n">
-        <v>-854</v>
+        <v>-841</v>
       </c>
       <c r="W211" t="n">
-        <v>-343.3</v>
+        <v>-335.6</v>
       </c>
       <c r="X211" t="n">
-        <v>-2403</v>
+        <v>-2349</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="1" t="n">
+        <v>44071</v>
+      </c>
+      <c r="B212" t="n">
+        <v>454</v>
+      </c>
+      <c r="C212" t="n">
+        <v>0</v>
+      </c>
+      <c r="D212" t="n">
+        <v>0</v>
+      </c>
+      <c r="E212" t="n">
+        <v>0</v>
+      </c>
+      <c r="F212" t="n">
+        <v>724</v>
+      </c>
+      <c r="G212" t="n">
+        <v>37</v>
+      </c>
+      <c r="H212" t="n">
+        <v>4231</v>
+      </c>
+      <c r="I212" t="n">
+        <v>16066</v>
+      </c>
+      <c r="J212" t="n">
+        <v>62027</v>
+      </c>
+      <c r="K212" t="n">
+        <v>28830</v>
+      </c>
+      <c r="L212" t="n">
+        <v>-114011</v>
+      </c>
+      <c r="M212" t="n">
+        <v>-125235</v>
+      </c>
+      <c r="N212" t="n">
+        <v>-295628</v>
+      </c>
+      <c r="O212" t="n">
+        <v>-338834</v>
+      </c>
+      <c r="P212" t="n">
+        <v>-128198</v>
+      </c>
+      <c r="Q212" t="n">
+        <v>-18472.4</v>
+      </c>
+      <c r="R212" t="n">
+        <v>-318007</v>
+      </c>
+      <c r="S212" t="n">
+        <v>-47705.3</v>
+      </c>
+      <c r="T212" t="n">
+        <v>-27992</v>
+      </c>
+      <c r="U212" t="n">
+        <v>-86.9</v>
+      </c>
+      <c r="V212" t="n">
+        <v>-10181.3</v>
+      </c>
+      <c r="W212" t="n">
+        <v>-4338.4</v>
+      </c>
+      <c r="X212" t="n">
+        <v>-30369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
arregla datos errores transcripción
</commit_message>
<xml_diff>
--- a/data/output/covid19-spain_consolidated.xlsx
+++ b/data/output/covid19-spain_consolidated.xlsx
@@ -14063,7 +14063,7 @@
         <v>2113</v>
       </c>
       <c r="G187" t="n">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="H187" t="n">
         <v>34095</v>
@@ -15765,7 +15765,7 @@
         <v>5080</v>
       </c>
       <c r="G210" t="n">
-        <v>535</v>
+        <v>515</v>
       </c>
       <c r="H210" t="n">
         <v>34288</v>
@@ -15910,10 +15910,10 @@
         <v>6856</v>
       </c>
       <c r="F212" t="n">
-        <v>4332</v>
+        <v>4353</v>
       </c>
       <c r="G212" t="n">
-        <v>323</v>
+        <v>377</v>
       </c>
       <c r="H212" t="n">
         <v>29152</v>
@@ -15984,19 +15984,19 @@
         <v>0</v>
       </c>
       <c r="F213" t="n">
-        <v>371</v>
+        <v>787</v>
       </c>
       <c r="G213" t="n">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="H213" t="n">
-        <v>2748</v>
+        <v>4243</v>
       </c>
       <c r="I213" t="n">
         <v>16370</v>
       </c>
       <c r="J213" t="n">
-        <v>34801</v>
+        <v>62542</v>
       </c>
       <c r="K213" t="n">
         <v>11046</v>
@@ -16008,10 +16008,10 @@
         <v>-150729</v>
       </c>
       <c r="N213" t="n">
-        <v>-325593</v>
+        <v>-297852</v>
       </c>
       <c r="O213" t="n">
-        <v>-369885</v>
+        <v>-342144</v>
       </c>
       <c r="P213" t="n">
         <v>-130144</v>
@@ -16020,25 +16020,25 @@
         <v>-17850.1</v>
       </c>
       <c r="R213" t="n">
-        <v>-328533</v>
+        <v>-300792</v>
       </c>
       <c r="S213" t="n">
-        <v>-52424.6</v>
+        <v>-48461.6</v>
       </c>
       <c r="T213" t="n">
-        <v>-26404</v>
+        <v>-24909</v>
       </c>
       <c r="U213" t="n">
-        <v>-90.6</v>
+        <v>-85.4</v>
       </c>
       <c r="V213" t="n">
-        <v>-10513.3</v>
+        <v>-10015</v>
       </c>
       <c r="W213" t="n">
-        <v>-4552.3</v>
+        <v>-4338.7</v>
       </c>
       <c r="X213" t="n">
-        <v>-31866</v>
+        <v>-30371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recupera la fuente de los datos para muchas CCAA (perdidas por fallo del script)
</commit_message>
<xml_diff>
--- a/data/output/covid19-spain_consolidated.xlsx
+++ b/data/output/covid19-spain_consolidated.xlsx
@@ -2582,7 +2582,7 @@
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="G32" t="n">
         <v>12</v>
@@ -2878,7 +2878,7 @@
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G36" t="n">
         <v>16</v>
@@ -4941,7 +4941,7 @@
         <v>3472</v>
       </c>
       <c r="C64" t="n">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D64" t="n">
         <v>0</v>
@@ -4959,37 +4959,37 @@
         <v>12722</v>
       </c>
       <c r="I64" t="n">
-        <v>123989</v>
+        <v>123990</v>
       </c>
       <c r="J64" t="n">
-        <v>82431</v>
+        <v>82432</v>
       </c>
       <c r="K64" t="n">
         <v>3363</v>
       </c>
       <c r="L64" t="n">
-        <v>97535</v>
+        <v>97536</v>
       </c>
       <c r="M64" t="n">
-        <v>51240</v>
+        <v>51241</v>
       </c>
       <c r="N64" t="n">
-        <v>61174</v>
+        <v>61175</v>
       </c>
       <c r="O64" t="n">
-        <v>27867</v>
+        <v>27868</v>
       </c>
       <c r="P64" t="n">
-        <v>6694</v>
+        <v>6695</v>
       </c>
       <c r="Q64" t="n">
-        <v>7320</v>
+        <v>7320.1</v>
       </c>
       <c r="R64" t="n">
-        <v>3843</v>
+        <v>3844</v>
       </c>
       <c r="S64" t="n">
-        <v>3981</v>
+        <v>3981.1</v>
       </c>
       <c r="T64" t="n">
         <v>1082</v>
@@ -5033,37 +5033,37 @@
         <v>13732</v>
       </c>
       <c r="I65" t="n">
-        <v>130856</v>
+        <v>130857</v>
       </c>
       <c r="J65" t="n">
-        <v>86326</v>
+        <v>86327</v>
       </c>
       <c r="K65" t="n">
         <v>4285</v>
       </c>
       <c r="L65" t="n">
-        <v>98801</v>
+        <v>98802</v>
       </c>
       <c r="M65" t="n">
-        <v>49592</v>
+        <v>49593</v>
       </c>
       <c r="N65" t="n">
-        <v>60818</v>
+        <v>60819</v>
       </c>
       <c r="O65" t="n">
-        <v>26773</v>
+        <v>26774</v>
       </c>
       <c r="P65" t="n">
         <v>6867</v>
       </c>
       <c r="Q65" t="n">
-        <v>7084.6</v>
+        <v>7084.7</v>
       </c>
       <c r="R65" t="n">
         <v>3895</v>
       </c>
       <c r="S65" t="n">
-        <v>3824.7</v>
+        <v>3824.9</v>
       </c>
       <c r="T65" t="n">
         <v>1010</v>
@@ -5107,37 +5107,37 @@
         <v>14651</v>
       </c>
       <c r="I66" t="n">
-        <v>136014</v>
+        <v>136015</v>
       </c>
       <c r="J66" t="n">
-        <v>88766</v>
+        <v>88767</v>
       </c>
       <c r="K66" t="n">
         <v>5112</v>
       </c>
       <c r="L66" t="n">
-        <v>99254</v>
+        <v>99255</v>
       </c>
       <c r="M66" t="n">
-        <v>46188</v>
+        <v>46189</v>
       </c>
       <c r="N66" t="n">
-        <v>59879</v>
+        <v>59880</v>
       </c>
       <c r="O66" t="n">
-        <v>25856</v>
+        <v>25857</v>
       </c>
       <c r="P66" t="n">
         <v>5158</v>
       </c>
       <c r="Q66" t="n">
-        <v>6598.3</v>
+        <v>6598.4</v>
       </c>
       <c r="R66" t="n">
         <v>2440</v>
       </c>
       <c r="S66" t="n">
-        <v>3693.7</v>
+        <v>3693.9</v>
       </c>
       <c r="T66" t="n">
         <v>919</v>
@@ -5181,37 +5181,37 @@
         <v>15505</v>
       </c>
       <c r="I67" t="n">
-        <v>139790</v>
+        <v>139791</v>
       </c>
       <c r="J67" t="n">
-        <v>90445</v>
+        <v>90446</v>
       </c>
       <c r="K67" t="n">
         <v>5716</v>
       </c>
       <c r="L67" t="n">
-        <v>99034</v>
+        <v>99035</v>
       </c>
       <c r="M67" t="n">
-        <v>43639</v>
+        <v>43640</v>
       </c>
       <c r="N67" t="n">
-        <v>58595</v>
+        <v>58596</v>
       </c>
       <c r="O67" t="n">
-        <v>24857</v>
+        <v>24858</v>
       </c>
       <c r="P67" t="n">
         <v>3776</v>
       </c>
       <c r="Q67" t="n">
-        <v>6234.1</v>
+        <v>6234.3</v>
       </c>
       <c r="R67" t="n">
         <v>1679</v>
       </c>
       <c r="S67" t="n">
-        <v>3551</v>
+        <v>3551.1</v>
       </c>
       <c r="T67" t="n">
         <v>854</v>
@@ -5255,37 +5255,37 @@
         <v>16425</v>
       </c>
       <c r="I68" t="n">
-        <v>144612</v>
+        <v>144613</v>
       </c>
       <c r="J68" t="n">
-        <v>93687</v>
+        <v>93688</v>
       </c>
       <c r="K68" t="n">
         <v>6241</v>
       </c>
       <c r="L68" t="n">
-        <v>97501</v>
+        <v>97502</v>
       </c>
       <c r="M68" t="n">
-        <v>41290</v>
+        <v>41291</v>
       </c>
       <c r="N68" t="n">
-        <v>57028</v>
+        <v>57029</v>
       </c>
       <c r="O68" t="n">
-        <v>23233</v>
+        <v>23234</v>
       </c>
       <c r="P68" t="n">
         <v>4822</v>
       </c>
       <c r="Q68" t="n">
-        <v>5898.6</v>
+        <v>5898.7</v>
       </c>
       <c r="R68" t="n">
         <v>3242</v>
       </c>
       <c r="S68" t="n">
-        <v>3319</v>
+        <v>3319.1</v>
       </c>
       <c r="T68" t="n">
         <v>920</v>
@@ -5329,37 +5329,37 @@
         <v>17336</v>
       </c>
       <c r="I69" t="n">
-        <v>149553</v>
+        <v>149554</v>
       </c>
       <c r="J69" t="n">
-        <v>96780</v>
+        <v>96781</v>
       </c>
       <c r="K69" t="n">
         <v>6969</v>
       </c>
       <c r="L69" t="n">
-        <v>97111</v>
+        <v>97112</v>
       </c>
       <c r="M69" t="n">
-        <v>40684</v>
+        <v>40685</v>
       </c>
       <c r="N69" t="n">
-        <v>54577</v>
+        <v>54578</v>
       </c>
       <c r="O69" t="n">
-        <v>22038</v>
+        <v>22039</v>
       </c>
       <c r="P69" t="n">
         <v>4941</v>
       </c>
       <c r="Q69" t="n">
-        <v>5812</v>
+        <v>5812.1</v>
       </c>
       <c r="R69" t="n">
         <v>3093</v>
       </c>
       <c r="S69" t="n">
-        <v>3148.3</v>
+        <v>3148.4</v>
       </c>
       <c r="T69" t="n">
         <v>911</v>
@@ -5403,37 +5403,37 @@
         <v>18299</v>
       </c>
       <c r="I70" t="n">
-        <v>154981</v>
+        <v>154982</v>
       </c>
       <c r="J70" t="n">
-        <v>99937</v>
+        <v>99938</v>
       </c>
       <c r="K70" t="n">
         <v>7881</v>
       </c>
       <c r="L70" t="n">
-        <v>91835</v>
+        <v>91836</v>
       </c>
       <c r="M70" t="n">
-        <v>37686</v>
+        <v>37687</v>
       </c>
       <c r="N70" t="n">
-        <v>52187</v>
+        <v>52188</v>
       </c>
       <c r="O70" t="n">
-        <v>21349</v>
+        <v>21350</v>
       </c>
       <c r="P70" t="n">
         <v>5428</v>
       </c>
       <c r="Q70" t="n">
-        <v>5383.7</v>
+        <v>5383.9</v>
       </c>
       <c r="R70" t="n">
         <v>3157</v>
       </c>
       <c r="S70" t="n">
-        <v>3049.9</v>
+        <v>3050</v>
       </c>
       <c r="T70" t="n">
         <v>963</v>
@@ -5477,22 +5477,22 @@
         <v>19169</v>
       </c>
       <c r="I71" t="n">
-        <v>159971</v>
+        <v>159972</v>
       </c>
       <c r="J71" t="n">
-        <v>102597</v>
+        <v>102598</v>
       </c>
       <c r="K71" t="n">
         <v>9073</v>
       </c>
       <c r="L71" t="n">
-        <v>87222</v>
+        <v>87223</v>
       </c>
       <c r="M71" t="n">
         <v>35982</v>
       </c>
       <c r="N71" t="n">
-        <v>48033</v>
+        <v>48034</v>
       </c>
       <c r="O71" t="n">
         <v>20166</v>
@@ -5542,7 +5542,7 @@
         <v>4970</v>
       </c>
       <c r="F72" t="n">
-        <v>26364</v>
+        <v>26365</v>
       </c>
       <c r="G72" t="n">
         <v>3269</v>
@@ -5551,22 +5551,22 @@
         <v>19964</v>
       </c>
       <c r="I72" t="n">
-        <v>165127</v>
+        <v>165128</v>
       </c>
       <c r="J72" t="n">
-        <v>104919</v>
+        <v>104920</v>
       </c>
       <c r="K72" t="n">
         <v>10089</v>
       </c>
       <c r="L72" t="n">
-        <v>83863</v>
+        <v>83864</v>
       </c>
       <c r="M72" t="n">
         <v>34271</v>
       </c>
       <c r="N72" t="n">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="O72" t="n">
         <v>18593</v>
@@ -5625,22 +5625,22 @@
         <v>20764</v>
       </c>
       <c r="I73" t="n">
-        <v>168872</v>
+        <v>168873</v>
       </c>
       <c r="J73" t="n">
-        <v>106706</v>
+        <v>106707</v>
       </c>
       <c r="K73" t="n">
         <v>10942</v>
       </c>
       <c r="L73" t="n">
-        <v>79046</v>
+        <v>79047</v>
       </c>
       <c r="M73" t="n">
         <v>32858</v>
       </c>
       <c r="N73" t="n">
-        <v>43796</v>
+        <v>43797</v>
       </c>
       <c r="O73" t="n">
         <v>17940</v>
@@ -5699,22 +5699,22 @@
         <v>21450</v>
       </c>
       <c r="I74" t="n">
-        <v>171907</v>
+        <v>171908</v>
       </c>
       <c r="J74" t="n">
-        <v>107976</v>
+        <v>107977</v>
       </c>
       <c r="K74" t="n">
         <v>11757</v>
       </c>
       <c r="L74" t="n">
-        <v>75756</v>
+        <v>75757</v>
       </c>
       <c r="M74" t="n">
         <v>32117</v>
       </c>
       <c r="N74" t="n">
-        <v>42388</v>
+        <v>42389</v>
       </c>
       <c r="O74" t="n">
         <v>17531</v>
@@ -5773,22 +5773,22 @@
         <v>22140</v>
       </c>
       <c r="I75" t="n">
-        <v>175401</v>
+        <v>175402</v>
       </c>
       <c r="J75" t="n">
-        <v>109940</v>
+        <v>109941</v>
       </c>
       <c r="K75" t="n">
         <v>12234</v>
       </c>
       <c r="L75" t="n">
-        <v>72079</v>
+        <v>72080</v>
       </c>
       <c r="M75" t="n">
         <v>30789</v>
       </c>
       <c r="N75" t="n">
-        <v>39486</v>
+        <v>39487</v>
       </c>
       <c r="O75" t="n">
         <v>16253</v>
@@ -5847,22 +5847,22 @@
         <v>22865</v>
       </c>
       <c r="I76" t="n">
-        <v>179715</v>
+        <v>179716</v>
       </c>
       <c r="J76" t="n">
-        <v>112524</v>
+        <v>112525</v>
       </c>
       <c r="K76" t="n">
         <v>13046</v>
       </c>
       <c r="L76" t="n">
-        <v>70846</v>
+        <v>70847</v>
       </c>
       <c r="M76" t="n">
         <v>30162</v>
       </c>
       <c r="N76" t="n">
-        <v>37782</v>
+        <v>37783</v>
       </c>
       <c r="O76" t="n">
         <v>15744</v>
@@ -5903,7 +5903,7 @@
         <v>2828</v>
       </c>
       <c r="C77" t="n">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D77" t="n">
         <v>779</v>
@@ -5921,37 +5921,37 @@
         <v>23568</v>
       </c>
       <c r="I77" t="n">
-        <v>184115</v>
+        <v>184117</v>
       </c>
       <c r="J77" t="n">
-        <v>117603</v>
+        <v>117605</v>
       </c>
       <c r="K77" t="n">
         <v>14124</v>
       </c>
       <c r="L77" t="n">
-        <v>66820</v>
+        <v>66822</v>
       </c>
       <c r="M77" t="n">
-        <v>29134</v>
+        <v>29135</v>
       </c>
       <c r="N77" t="n">
-        <v>39015</v>
+        <v>39017</v>
       </c>
       <c r="O77" t="n">
-        <v>17666</v>
+        <v>17667</v>
       </c>
       <c r="P77" t="n">
-        <v>4400</v>
+        <v>4401</v>
       </c>
       <c r="Q77" t="n">
-        <v>4162</v>
+        <v>4162.1</v>
       </c>
       <c r="R77" t="n">
-        <v>5079</v>
+        <v>5080</v>
       </c>
       <c r="S77" t="n">
-        <v>2523.7</v>
+        <v>2523.9</v>
       </c>
       <c r="T77" t="n">
         <v>703</v>
@@ -5995,37 +5995,37 @@
         <v>24246</v>
       </c>
       <c r="I78" t="n">
-        <v>188826</v>
+        <v>188828</v>
       </c>
       <c r="J78" t="n">
-        <v>120003</v>
+        <v>120005</v>
       </c>
       <c r="K78" t="n">
         <v>15049</v>
       </c>
       <c r="L78" t="n">
-        <v>64837</v>
+        <v>64838</v>
       </c>
       <c r="M78" t="n">
-        <v>28855</v>
+        <v>28856</v>
       </c>
       <c r="N78" t="n">
-        <v>37572</v>
+        <v>37573</v>
       </c>
       <c r="O78" t="n">
-        <v>17406</v>
+        <v>17407</v>
       </c>
       <c r="P78" t="n">
         <v>4711</v>
       </c>
       <c r="Q78" t="n">
-        <v>4122.1</v>
+        <v>4122.3</v>
       </c>
       <c r="R78" t="n">
         <v>2400</v>
       </c>
       <c r="S78" t="n">
-        <v>2486.6</v>
+        <v>2486.7</v>
       </c>
       <c r="T78" t="n">
         <v>678</v>
@@ -6069,37 +6069,37 @@
         <v>24859</v>
       </c>
       <c r="I79" t="n">
-        <v>193909</v>
+        <v>193911</v>
       </c>
       <c r="J79" t="n">
-        <v>122344</v>
+        <v>122346</v>
       </c>
       <c r="K79" t="n">
         <v>17165</v>
       </c>
       <c r="L79" t="n">
-        <v>63053</v>
+        <v>63054</v>
       </c>
       <c r="M79" t="n">
-        <v>28782</v>
+        <v>28783</v>
       </c>
       <c r="N79" t="n">
-        <v>36018</v>
+        <v>36019</v>
       </c>
       <c r="O79" t="n">
-        <v>17425</v>
+        <v>17426</v>
       </c>
       <c r="P79" t="n">
         <v>5083</v>
       </c>
       <c r="Q79" t="n">
-        <v>4111.7</v>
+        <v>4111.9</v>
       </c>
       <c r="R79" t="n">
         <v>2341</v>
       </c>
       <c r="S79" t="n">
-        <v>2489.3</v>
+        <v>2489.4</v>
       </c>
       <c r="T79" t="n">
         <v>613</v>
@@ -6143,37 +6143,37 @@
         <v>25465</v>
       </c>
       <c r="I80" t="n">
-        <v>199818</v>
+        <v>199820</v>
       </c>
       <c r="J80" t="n">
-        <v>123849</v>
+        <v>123851</v>
       </c>
       <c r="K80" t="n">
         <v>17041</v>
       </c>
       <c r="L80" t="n">
-        <v>63804</v>
+        <v>63805</v>
       </c>
       <c r="M80" t="n">
-        <v>30946</v>
+        <v>30947</v>
       </c>
       <c r="N80" t="n">
-        <v>35083</v>
+        <v>35084</v>
       </c>
       <c r="O80" t="n">
-        <v>17143</v>
+        <v>17144</v>
       </c>
       <c r="P80" t="n">
         <v>5909</v>
       </c>
       <c r="Q80" t="n">
-        <v>4420.9</v>
+        <v>4421</v>
       </c>
       <c r="R80" t="n">
         <v>1505</v>
       </c>
       <c r="S80" t="n">
-        <v>2449</v>
+        <v>2449.1</v>
       </c>
       <c r="T80" t="n">
         <v>606</v>
@@ -6217,37 +6217,37 @@
         <v>25989</v>
       </c>
       <c r="I81" t="n">
-        <v>202017</v>
+        <v>202019</v>
       </c>
       <c r="J81" t="n">
-        <v>124736</v>
+        <v>124738</v>
       </c>
       <c r="K81" t="n">
         <v>17680</v>
       </c>
       <c r="L81" t="n">
-        <v>62227</v>
+        <v>62228</v>
       </c>
       <c r="M81" t="n">
-        <v>30110</v>
+        <v>30111</v>
       </c>
       <c r="N81" t="n">
-        <v>34291</v>
+        <v>34292</v>
       </c>
       <c r="O81" t="n">
-        <v>16760</v>
+        <v>16761</v>
       </c>
       <c r="P81" t="n">
         <v>2199</v>
       </c>
       <c r="Q81" t="n">
-        <v>4301.4</v>
+        <v>4301.6</v>
       </c>
       <c r="R81" t="n">
         <v>887</v>
       </c>
       <c r="S81" t="n">
-        <v>2394.3</v>
+        <v>2394.4</v>
       </c>
       <c r="T81" t="n">
         <v>524</v>
@@ -6291,37 +6291,37 @@
         <v>26485</v>
       </c>
       <c r="I82" t="n">
-        <v>204986</v>
+        <v>204988</v>
       </c>
       <c r="J82" t="n">
-        <v>126494</v>
+        <v>126496</v>
       </c>
       <c r="K82" t="n">
         <v>19637</v>
       </c>
       <c r="L82" t="n">
-        <v>60374</v>
+        <v>60375</v>
       </c>
       <c r="M82" t="n">
-        <v>29585</v>
+        <v>29586</v>
       </c>
       <c r="N82" t="n">
-        <v>32807</v>
+        <v>32808</v>
       </c>
       <c r="O82" t="n">
-        <v>16554</v>
+        <v>16555</v>
       </c>
       <c r="P82" t="n">
         <v>2969</v>
       </c>
       <c r="Q82" t="n">
-        <v>4226.4</v>
+        <v>4226.6</v>
       </c>
       <c r="R82" t="n">
         <v>1758</v>
       </c>
       <c r="S82" t="n">
-        <v>2364.9</v>
+        <v>2365</v>
       </c>
       <c r="T82" t="n">
         <v>496</v>
@@ -6365,37 +6365,37 @@
         <v>26990</v>
       </c>
       <c r="I83" t="n">
-        <v>208720</v>
+        <v>208722</v>
       </c>
       <c r="J83" t="n">
-        <v>128376</v>
+        <v>128378</v>
       </c>
       <c r="K83" t="n">
         <v>20400</v>
       </c>
       <c r="L83" t="n">
-        <v>59167</v>
+        <v>59168</v>
       </c>
       <c r="M83" t="n">
-        <v>29005</v>
+        <v>29006</v>
       </c>
       <c r="N83" t="n">
-        <v>31596</v>
+        <v>31597</v>
       </c>
       <c r="O83" t="n">
-        <v>15852</v>
+        <v>15853</v>
       </c>
       <c r="P83" t="n">
         <v>3734</v>
       </c>
       <c r="Q83" t="n">
-        <v>4143.6</v>
+        <v>4143.7</v>
       </c>
       <c r="R83" t="n">
         <v>1882</v>
       </c>
       <c r="S83" t="n">
-        <v>2264.6</v>
+        <v>2264.7</v>
       </c>
       <c r="T83" t="n">
         <v>505</v>
@@ -6439,22 +6439,22 @@
         <v>27480</v>
       </c>
       <c r="I84" t="n">
-        <v>213321</v>
+        <v>213323</v>
       </c>
       <c r="J84" t="n">
-        <v>130370</v>
+        <v>130372</v>
       </c>
       <c r="K84" t="n">
         <v>20967</v>
       </c>
       <c r="L84" t="n">
-        <v>58340</v>
+        <v>58341</v>
       </c>
       <c r="M84" t="n">
         <v>29206</v>
       </c>
       <c r="N84" t="n">
-        <v>30433</v>
+        <v>30434</v>
       </c>
       <c r="O84" t="n">
         <v>12767</v>
@@ -6513,22 +6513,22 @@
         <v>27911</v>
       </c>
       <c r="I85" t="n">
-        <v>217034</v>
+        <v>217036</v>
       </c>
       <c r="J85" t="n">
-        <v>131778</v>
+        <v>131780</v>
       </c>
       <c r="K85" t="n">
         <v>23252</v>
       </c>
       <c r="L85" t="n">
-        <v>57063</v>
+        <v>57064</v>
       </c>
       <c r="M85" t="n">
         <v>28208</v>
       </c>
       <c r="N85" t="n">
-        <v>29181</v>
+        <v>29182</v>
       </c>
       <c r="O85" t="n">
         <v>11775</v>
@@ -6587,22 +6587,22 @@
         <v>28349</v>
       </c>
       <c r="I86" t="n">
-        <v>220703</v>
+        <v>220705</v>
       </c>
       <c r="J86" t="n">
-        <v>133331</v>
+        <v>133333</v>
       </c>
       <c r="K86" t="n">
         <v>26414.89</v>
       </c>
       <c r="L86" t="n">
-        <v>55576</v>
+        <v>55577</v>
       </c>
       <c r="M86" t="n">
         <v>26794</v>
       </c>
       <c r="N86" t="n">
-        <v>28412</v>
+        <v>28413</v>
       </c>
       <c r="O86" t="n">
         <v>10987</v>
@@ -6661,22 +6661,22 @@
         <v>28719</v>
       </c>
       <c r="I87" t="n">
-        <v>223317</v>
+        <v>223319</v>
       </c>
       <c r="J87" t="n">
-        <v>134154</v>
+        <v>134156</v>
       </c>
       <c r="K87" t="n">
         <v>26531.966</v>
       </c>
       <c r="L87" t="n">
-        <v>54445</v>
+        <v>54446</v>
       </c>
       <c r="M87" t="n">
         <v>23499</v>
       </c>
       <c r="N87" t="n">
-        <v>27448</v>
+        <v>27449</v>
       </c>
       <c r="O87" t="n">
         <v>10305</v>
@@ -6735,22 +6735,22 @@
         <v>29045</v>
       </c>
       <c r="I88" t="n">
-        <v>225702</v>
+        <v>225704</v>
       </c>
       <c r="J88" t="n">
-        <v>134677</v>
+        <v>134679</v>
       </c>
       <c r="K88" t="n">
         <v>30059</v>
       </c>
       <c r="L88" t="n">
-        <v>53795</v>
+        <v>53796</v>
       </c>
       <c r="M88" t="n">
         <v>23685</v>
       </c>
       <c r="N88" t="n">
-        <v>26701</v>
+        <v>26702</v>
       </c>
       <c r="O88" t="n">
         <v>9941</v>
@@ -6800,7 +6800,7 @@
         <v>20114</v>
       </c>
       <c r="F89" t="n">
-        <v>15930</v>
+        <v>15931</v>
       </c>
       <c r="G89" t="n">
         <v>2215</v>
@@ -6809,22 +6809,22 @@
         <v>29344</v>
       </c>
       <c r="I89" t="n">
-        <v>228383</v>
+        <v>228385</v>
       </c>
       <c r="J89" t="n">
-        <v>135819</v>
+        <v>135821</v>
       </c>
       <c r="K89" t="n">
         <v>31157</v>
       </c>
       <c r="L89" t="n">
-        <v>52982</v>
+        <v>52983</v>
       </c>
       <c r="M89" t="n">
         <v>23397</v>
       </c>
       <c r="N89" t="n">
-        <v>25879</v>
+        <v>25880</v>
       </c>
       <c r="O89" t="n">
         <v>9325</v>
@@ -6874,7 +6874,7 @@
         <v>19056</v>
       </c>
       <c r="F90" t="n">
-        <v>15371</v>
+        <v>15372</v>
       </c>
       <c r="G90" t="n">
         <v>2052</v>
@@ -6883,22 +6883,22 @@
         <v>29685</v>
       </c>
       <c r="I90" t="n">
-        <v>228216</v>
+        <v>228218</v>
       </c>
       <c r="J90" t="n">
-        <v>137169</v>
+        <v>137171</v>
       </c>
       <c r="K90" t="n">
         <v>33387</v>
       </c>
       <c r="L90" t="n">
-        <v>48501</v>
+        <v>48502</v>
       </c>
       <c r="M90" t="n">
         <v>19496</v>
       </c>
       <c r="N90" t="n">
-        <v>24645</v>
+        <v>24646</v>
       </c>
       <c r="O90" t="n">
         <v>8793</v>
@@ -6948,7 +6948,7 @@
         <v>20627</v>
       </c>
       <c r="F91" t="n">
-        <v>14852</v>
+        <v>14853</v>
       </c>
       <c r="G91" t="n">
         <v>1981</v>
@@ -6957,10 +6957,10 @@
         <v>29997</v>
       </c>
       <c r="I91" t="n">
-        <v>231085</v>
+        <v>231087</v>
       </c>
       <c r="J91" t="n">
-        <v>138222</v>
+        <v>138224</v>
       </c>
       <c r="K91" t="n">
         <v>34830</v>
@@ -7031,10 +7031,10 @@
         <v>30277</v>
       </c>
       <c r="I92" t="n">
-        <v>234309</v>
+        <v>234311</v>
       </c>
       <c r="J92" t="n">
-        <v>139160</v>
+        <v>139162</v>
       </c>
       <c r="K92" t="n">
         <v>32719</v>
@@ -7105,10 +7105,10 @@
         <v>30557</v>
       </c>
       <c r="I93" t="n">
-        <v>236468</v>
+        <v>236470</v>
       </c>
       <c r="J93" t="n">
-        <v>139727</v>
+        <v>139729</v>
       </c>
       <c r="K93" t="n">
         <v>33871</v>
@@ -7170,7 +7170,7 @@
         <v>20056</v>
       </c>
       <c r="F94" t="n">
-        <v>15007</v>
+        <v>15008</v>
       </c>
       <c r="G94" t="n">
         <v>2249</v>
@@ -7179,10 +7179,10 @@
         <v>30790</v>
       </c>
       <c r="I94" t="n">
-        <v>238131</v>
+        <v>238133</v>
       </c>
       <c r="J94" t="n">
-        <v>140096</v>
+        <v>140098</v>
       </c>
       <c r="K94" t="n">
         <v>34531</v>
@@ -7244,7 +7244,7 @@
         <v>20206</v>
       </c>
       <c r="F95" t="n">
-        <v>14975</v>
+        <v>14976</v>
       </c>
       <c r="G95" t="n">
         <v>2195</v>
@@ -7253,10 +7253,10 @@
         <v>31009</v>
       </c>
       <c r="I95" t="n">
-        <v>239223</v>
+        <v>239225</v>
       </c>
       <c r="J95" t="n">
-        <v>140380</v>
+        <v>140382</v>
       </c>
       <c r="K95" t="n">
         <v>35049</v>
@@ -7309,7 +7309,7 @@
         <v>567</v>
       </c>
       <c r="C96" t="n">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D96" t="n">
         <v>9480</v>
@@ -7318,7 +7318,7 @@
         <v>20387</v>
       </c>
       <c r="F96" t="n">
-        <v>14572</v>
+        <v>14573</v>
       </c>
       <c r="G96" t="n">
         <v>2099</v>
@@ -7327,37 +7327,37 @@
         <v>31212</v>
       </c>
       <c r="I96" t="n">
-        <v>240992</v>
+        <v>240993</v>
       </c>
       <c r="J96" t="n">
-        <v>141250</v>
+        <v>141251</v>
       </c>
       <c r="K96" t="n">
         <v>35634</v>
       </c>
       <c r="L96" t="n">
-        <v>36006</v>
+        <v>36005</v>
       </c>
       <c r="M96" t="n">
-        <v>12609</v>
+        <v>12608</v>
       </c>
       <c r="N96" t="n">
-        <v>14756</v>
+        <v>14755</v>
       </c>
       <c r="O96" t="n">
-        <v>5431</v>
+        <v>5430</v>
       </c>
       <c r="P96" t="n">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="Q96" t="n">
-        <v>1801.3</v>
+        <v>1801.1</v>
       </c>
       <c r="R96" t="n">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="S96" t="n">
-        <v>775.9</v>
+        <v>775.7</v>
       </c>
       <c r="T96" t="n">
         <v>203</v>
@@ -7392,7 +7392,7 @@
         <v>16370</v>
       </c>
       <c r="F97" t="n">
-        <v>14169</v>
+        <v>14170</v>
       </c>
       <c r="G97" t="n">
         <v>2013</v>
@@ -7401,37 +7401,37 @@
         <v>31445</v>
       </c>
       <c r="I97" t="n">
-        <v>243055</v>
+        <v>243056</v>
       </c>
       <c r="J97" t="n">
-        <v>154351</v>
+        <v>154352</v>
       </c>
       <c r="K97" t="n">
         <v>36619</v>
       </c>
       <c r="L97" t="n">
-        <v>34335</v>
+        <v>34334</v>
       </c>
       <c r="M97" t="n">
-        <v>14839</v>
+        <v>14838</v>
       </c>
       <c r="N97" t="n">
-        <v>25975</v>
+        <v>25974</v>
       </c>
       <c r="O97" t="n">
-        <v>17182</v>
+        <v>17181</v>
       </c>
       <c r="P97" t="n">
         <v>2063</v>
       </c>
       <c r="Q97" t="n">
-        <v>2119.9</v>
+        <v>2119.7</v>
       </c>
       <c r="R97" t="n">
         <v>13101</v>
       </c>
       <c r="S97" t="n">
-        <v>2454.6</v>
+        <v>2454.4</v>
       </c>
       <c r="T97" t="n">
         <v>233</v>
@@ -7475,37 +7475,37 @@
         <v>31688</v>
       </c>
       <c r="I98" t="n">
-        <v>246001</v>
+        <v>246002</v>
       </c>
       <c r="J98" t="n">
-        <v>155232</v>
+        <v>155233</v>
       </c>
       <c r="K98" t="n">
         <v>37508</v>
       </c>
       <c r="L98" t="n">
-        <v>32680</v>
+        <v>32679</v>
       </c>
       <c r="M98" t="n">
-        <v>14916</v>
+        <v>14915</v>
       </c>
       <c r="N98" t="n">
-        <v>24862</v>
+        <v>24861</v>
       </c>
       <c r="O98" t="n">
-        <v>17010</v>
+        <v>17009</v>
       </c>
       <c r="P98" t="n">
         <v>2946</v>
       </c>
       <c r="Q98" t="n">
-        <v>2130.9</v>
+        <v>2130.7</v>
       </c>
       <c r="R98" t="n">
         <v>881</v>
       </c>
       <c r="S98" t="n">
-        <v>2430</v>
+        <v>2429.9</v>
       </c>
       <c r="T98" t="n">
         <v>243</v>
@@ -7549,37 +7549,37 @@
         <v>31915</v>
       </c>
       <c r="I99" t="n">
-        <v>246367</v>
+        <v>246368</v>
       </c>
       <c r="J99" t="n">
-        <v>155993</v>
+        <v>155994</v>
       </c>
       <c r="K99" t="n">
         <v>38473</v>
       </c>
       <c r="L99" t="n">
-        <v>29333</v>
+        <v>29332</v>
       </c>
       <c r="M99" t="n">
-        <v>12058</v>
+        <v>12057</v>
       </c>
       <c r="N99" t="n">
-        <v>24215</v>
+        <v>24214</v>
       </c>
       <c r="O99" t="n">
-        <v>16833</v>
+        <v>16832</v>
       </c>
       <c r="P99" t="n">
         <v>366</v>
       </c>
       <c r="Q99" t="n">
-        <v>1722.6</v>
+        <v>1722.4</v>
       </c>
       <c r="R99" t="n">
         <v>761</v>
       </c>
       <c r="S99" t="n">
-        <v>2404.7</v>
+        <v>2404.6</v>
       </c>
       <c r="T99" t="n">
         <v>227</v>
@@ -7623,37 +7623,37 @@
         <v>32125</v>
       </c>
       <c r="I100" t="n">
-        <v>250894</v>
+        <v>250895</v>
       </c>
       <c r="J100" t="n">
-        <v>156731</v>
+        <v>156732</v>
       </c>
       <c r="K100" t="n">
         <v>39370</v>
       </c>
       <c r="L100" t="n">
-        <v>30191</v>
+        <v>30190</v>
       </c>
       <c r="M100" t="n">
-        <v>14426</v>
+        <v>14425</v>
       </c>
       <c r="N100" t="n">
-        <v>23400</v>
+        <v>23399</v>
       </c>
       <c r="O100" t="n">
-        <v>17004</v>
+        <v>17003</v>
       </c>
       <c r="P100" t="n">
         <v>4527</v>
       </c>
       <c r="Q100" t="n">
-        <v>2060.9</v>
+        <v>2060.7</v>
       </c>
       <c r="R100" t="n">
         <v>738</v>
       </c>
       <c r="S100" t="n">
-        <v>2429.1</v>
+        <v>2429</v>
       </c>
       <c r="T100" t="n">
         <v>210</v>
@@ -7697,37 +7697,37 @@
         <v>32298</v>
       </c>
       <c r="I101" t="n">
-        <v>252714</v>
+        <v>252715</v>
       </c>
       <c r="J101" t="n">
-        <v>157058</v>
+        <v>157059</v>
       </c>
       <c r="K101" t="n">
         <v>40573</v>
       </c>
       <c r="L101" t="n">
-        <v>29397</v>
+        <v>29396</v>
       </c>
       <c r="M101" t="n">
-        <v>14583</v>
+        <v>14582</v>
       </c>
       <c r="N101" t="n">
-        <v>22904</v>
+        <v>22903</v>
       </c>
       <c r="O101" t="n">
-        <v>16962</v>
+        <v>16961</v>
       </c>
       <c r="P101" t="n">
         <v>1820</v>
       </c>
       <c r="Q101" t="n">
-        <v>2083.3</v>
+        <v>2083.1</v>
       </c>
       <c r="R101" t="n">
         <v>327</v>
       </c>
       <c r="S101" t="n">
-        <v>2423.1</v>
+        <v>2423</v>
       </c>
       <c r="T101" t="n">
         <v>173</v>
@@ -7771,37 +7771,37 @@
         <v>32445</v>
       </c>
       <c r="I102" t="n">
-        <v>251674</v>
+        <v>251675</v>
       </c>
       <c r="J102" t="n">
-        <v>157308</v>
+        <v>157309</v>
       </c>
       <c r="K102" t="n">
         <v>41048</v>
       </c>
       <c r="L102" t="n">
-        <v>25972</v>
+        <v>25971</v>
       </c>
       <c r="M102" t="n">
-        <v>12451</v>
+        <v>12450</v>
       </c>
       <c r="N102" t="n">
-        <v>22631</v>
+        <v>22630</v>
       </c>
       <c r="O102" t="n">
-        <v>16928</v>
+        <v>16927</v>
       </c>
       <c r="P102" t="n">
         <v>-1040</v>
       </c>
       <c r="Q102" t="n">
-        <v>1778.7</v>
+        <v>1778.6</v>
       </c>
       <c r="R102" t="n">
         <v>250</v>
       </c>
       <c r="S102" t="n">
-        <v>2418.3</v>
+        <v>2418.1</v>
       </c>
       <c r="T102" t="n">
         <v>147</v>
@@ -7845,22 +7845,22 @@
         <v>32606</v>
       </c>
       <c r="I103" t="n">
-        <v>255294</v>
+        <v>255295</v>
       </c>
       <c r="J103" t="n">
-        <v>157957</v>
+        <v>157958</v>
       </c>
       <c r="K103" t="n">
         <v>41415</v>
       </c>
       <c r="L103" t="n">
-        <v>26911</v>
+        <v>26910</v>
       </c>
       <c r="M103" t="n">
         <v>14302</v>
       </c>
       <c r="N103" t="n">
-        <v>22138</v>
+        <v>22137</v>
       </c>
       <c r="O103" t="n">
         <v>16707</v>
@@ -7919,22 +7919,22 @@
         <v>32756</v>
       </c>
       <c r="I104" t="n">
-        <v>256972</v>
+        <v>256973</v>
       </c>
       <c r="J104" t="n">
-        <v>158710</v>
+        <v>158711</v>
       </c>
       <c r="K104" t="n">
         <v>42045</v>
       </c>
       <c r="L104" t="n">
-        <v>28756</v>
+        <v>28755</v>
       </c>
       <c r="M104" t="n">
         <v>13917</v>
       </c>
       <c r="N104" t="n">
-        <v>21541</v>
+        <v>21540</v>
       </c>
       <c r="O104" t="n">
         <v>4359</v>
@@ -7993,22 +7993,22 @@
         <v>32876</v>
       </c>
       <c r="I105" t="n">
-        <v>258579</v>
+        <v>258580</v>
       </c>
       <c r="J105" t="n">
-        <v>159503</v>
+        <v>159504</v>
       </c>
       <c r="K105" t="n">
         <v>42997</v>
       </c>
       <c r="L105" t="n">
-        <v>27494</v>
+        <v>27493</v>
       </c>
       <c r="M105" t="n">
         <v>12578</v>
       </c>
       <c r="N105" t="n">
-        <v>21281</v>
+        <v>21280</v>
       </c>
       <c r="O105" t="n">
         <v>4271</v>
@@ -8067,22 +8067,22 @@
         <v>32992</v>
       </c>
       <c r="I106" t="n">
-        <v>203368</v>
+        <v>203369</v>
       </c>
       <c r="J106" t="n">
-        <v>187558</v>
+        <v>187559</v>
       </c>
       <c r="K106" t="n">
         <v>43872</v>
       </c>
       <c r="L106" t="n">
-        <v>-30941</v>
+        <v>-30942</v>
       </c>
       <c r="M106" t="n">
         <v>-42999</v>
       </c>
       <c r="N106" t="n">
-        <v>48398</v>
+        <v>48397</v>
       </c>
       <c r="O106" t="n">
         <v>31565</v>
@@ -8141,22 +8141,22 @@
         <v>33105</v>
       </c>
       <c r="I107" t="n">
-        <v>204656</v>
+        <v>204657</v>
       </c>
       <c r="J107" t="n">
-        <v>201036</v>
+        <v>201037</v>
       </c>
       <c r="K107" t="n">
         <v>44569</v>
       </c>
       <c r="L107" t="n">
-        <v>-31812</v>
+        <v>-31813</v>
       </c>
       <c r="M107" t="n">
         <v>-46238</v>
       </c>
       <c r="N107" t="n">
-        <v>61309</v>
+        <v>61308</v>
       </c>
       <c r="O107" t="n">
         <v>44305</v>
@@ -8215,22 +8215,22 @@
         <v>33196</v>
       </c>
       <c r="I108" t="n">
-        <v>205264</v>
+        <v>205265</v>
       </c>
       <c r="J108" t="n">
-        <v>201379</v>
+        <v>201380</v>
       </c>
       <c r="K108" t="n">
         <v>45287</v>
       </c>
       <c r="L108" t="n">
-        <v>-32867</v>
+        <v>-32868</v>
       </c>
       <c r="M108" t="n">
         <v>-47450</v>
       </c>
       <c r="N108" t="n">
-        <v>61283</v>
+        <v>61282</v>
       </c>
       <c r="O108" t="n">
         <v>44321</v>
@@ -8289,22 +8289,22 @@
         <v>33266</v>
       </c>
       <c r="I109" t="n">
-        <v>205609</v>
+        <v>205610</v>
       </c>
       <c r="J109" t="n">
-        <v>201644</v>
+        <v>201645</v>
       </c>
       <c r="K109" t="n">
         <v>45664</v>
       </c>
       <c r="L109" t="n">
-        <v>-33614</v>
+        <v>-33615</v>
       </c>
       <c r="M109" t="n">
         <v>-46065</v>
       </c>
       <c r="N109" t="n">
-        <v>61264</v>
+        <v>61263</v>
       </c>
       <c r="O109" t="n">
         <v>44336</v>
@@ -8363,10 +8363,10 @@
         <v>33338</v>
       </c>
       <c r="I110" t="n">
-        <v>179096</v>
+        <v>179097</v>
       </c>
       <c r="J110" t="n">
-        <v>227030</v>
+        <v>227031</v>
       </c>
       <c r="K110" t="n">
         <v>39588</v>
@@ -8437,10 +8437,10 @@
         <v>33417</v>
       </c>
       <c r="I111" t="n">
-        <v>175000</v>
+        <v>175001</v>
       </c>
       <c r="J111" t="n">
-        <v>233372</v>
+        <v>233373</v>
       </c>
       <c r="K111" t="n">
         <v>39801</v>
@@ -8511,10 +8511,10 @@
         <v>32054</v>
       </c>
       <c r="I112" t="n">
-        <v>175560</v>
+        <v>175561</v>
       </c>
       <c r="J112" t="n">
-        <v>234252</v>
+        <v>234253</v>
       </c>
       <c r="K112" t="n">
         <v>45485</v>
@@ -8585,10 +8585,10 @@
         <v>32116</v>
       </c>
       <c r="I113" t="n">
-        <v>83728</v>
+        <v>83729</v>
       </c>
       <c r="J113" t="n">
-        <v>235190</v>
+        <v>235191</v>
       </c>
       <c r="K113" t="n">
         <v>48306</v>
@@ -8659,10 +8659,10 @@
         <v>32187</v>
       </c>
       <c r="I114" t="n">
-        <v>84217</v>
+        <v>84218</v>
       </c>
       <c r="J114" t="n">
-        <v>236171</v>
+        <v>236172</v>
       </c>
       <c r="K114" t="n">
         <v>48852</v>
@@ -8733,10 +8733,10 @@
         <v>32263</v>
       </c>
       <c r="I115" t="n">
-        <v>84432</v>
+        <v>84433</v>
       </c>
       <c r="J115" t="n">
-        <v>236534</v>
+        <v>236535</v>
       </c>
       <c r="K115" t="n">
         <v>38560</v>
@@ -8807,10 +8807,10 @@
         <v>32315</v>
       </c>
       <c r="I116" t="n">
-        <v>84595</v>
+        <v>84596</v>
       </c>
       <c r="J116" t="n">
-        <v>236850</v>
+        <v>236851</v>
       </c>
       <c r="K116" t="n">
         <v>38749</v>
@@ -8881,10 +8881,10 @@
         <v>32368</v>
       </c>
       <c r="I117" t="n">
-        <v>84923</v>
+        <v>84924</v>
       </c>
       <c r="J117" t="n">
-        <v>237446</v>
+        <v>237447</v>
       </c>
       <c r="K117" t="n">
         <v>40726</v>
@@ -8955,10 +8955,10 @@
         <v>32428</v>
       </c>
       <c r="I118" t="n">
-        <v>85295</v>
+        <v>85296</v>
       </c>
       <c r="J118" t="n">
-        <v>238244</v>
+        <v>238245</v>
       </c>
       <c r="K118" t="n">
         <v>52399</v>
@@ -9029,10 +9029,10 @@
         <v>32488</v>
       </c>
       <c r="I119" t="n">
-        <v>85702</v>
+        <v>85703</v>
       </c>
       <c r="J119" t="n">
-        <v>239136</v>
+        <v>239137</v>
       </c>
       <c r="K119" t="n">
         <v>53095</v>
@@ -9103,10 +9103,10 @@
         <v>32530</v>
       </c>
       <c r="I120" t="n">
-        <v>83918</v>
+        <v>83919</v>
       </c>
       <c r="J120" t="n">
-        <v>239907</v>
+        <v>239908</v>
       </c>
       <c r="K120" t="n">
         <v>52089</v>
@@ -9177,10 +9177,10 @@
         <v>32744</v>
       </c>
       <c r="I121" t="n">
-        <v>86302</v>
+        <v>86303</v>
       </c>
       <c r="J121" t="n">
-        <v>240724</v>
+        <v>240725</v>
       </c>
       <c r="K121" t="n">
         <v>60099</v>
@@ -9233,7 +9233,7 @@
         <v>73</v>
       </c>
       <c r="C122" t="n">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D122" t="n">
         <v>5</v>
@@ -9260,28 +9260,28 @@
         <v>60670</v>
       </c>
       <c r="L122" t="n">
-        <v>-118823</v>
+        <v>-118824</v>
       </c>
       <c r="M122" t="n">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="N122" t="n">
-        <v>39744</v>
+        <v>39743</v>
       </c>
       <c r="O122" t="n">
-        <v>4589</v>
+        <v>4588</v>
       </c>
       <c r="P122" t="n">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q122" t="n">
-        <v>287</v>
+        <v>286.9</v>
       </c>
       <c r="R122" t="n">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="S122" t="n">
-        <v>655.6</v>
+        <v>655.4</v>
       </c>
       <c r="T122" t="n">
         <v>41</v>
@@ -9334,28 +9334,28 @@
         <v>60974</v>
       </c>
       <c r="L123" t="n">
-        <v>-119120</v>
+        <v>-119121</v>
       </c>
       <c r="M123" t="n">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="N123" t="n">
-        <v>39773</v>
+        <v>39772</v>
       </c>
       <c r="O123" t="n">
-        <v>4567</v>
+        <v>4566</v>
       </c>
       <c r="P123" t="n">
         <v>48</v>
       </c>
       <c r="Q123" t="n">
-        <v>270.6</v>
+        <v>270.4</v>
       </c>
       <c r="R123" t="n">
         <v>294</v>
       </c>
       <c r="S123" t="n">
-        <v>652.4</v>
+        <v>652.3</v>
       </c>
       <c r="T123" t="n">
         <v>34</v>
@@ -9408,28 +9408,28 @@
         <v>61236</v>
       </c>
       <c r="L124" t="n">
-        <v>-92528</v>
+        <v>-92529</v>
       </c>
       <c r="M124" t="n">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="N124" t="n">
-        <v>14836</v>
+        <v>14835</v>
       </c>
       <c r="O124" t="n">
-        <v>4420</v>
+        <v>4419</v>
       </c>
       <c r="P124" t="n">
         <v>79</v>
       </c>
       <c r="Q124" t="n">
-        <v>235</v>
+        <v>234.9</v>
       </c>
       <c r="R124" t="n">
         <v>449</v>
       </c>
       <c r="S124" t="n">
-        <v>631.4</v>
+        <v>631.3</v>
       </c>
       <c r="T124" t="n">
         <v>29</v>
@@ -9482,28 +9482,28 @@
         <v>61862</v>
       </c>
       <c r="L125" t="n">
-        <v>-88068</v>
+        <v>-88069</v>
       </c>
       <c r="M125" t="n">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="N125" t="n">
-        <v>11274</v>
+        <v>11273</v>
       </c>
       <c r="O125" t="n">
-        <v>6402</v>
+        <v>6401</v>
       </c>
       <c r="P125" t="n">
         <v>364</v>
       </c>
       <c r="Q125" t="n">
-        <v>233.9</v>
+        <v>233.7</v>
       </c>
       <c r="R125" t="n">
         <v>2780</v>
       </c>
       <c r="S125" t="n">
-        <v>914.6</v>
+        <v>914.4</v>
       </c>
       <c r="T125" t="n">
         <v>10</v>
@@ -9556,28 +9556,28 @@
         <v>62353</v>
       </c>
       <c r="L126" t="n">
-        <v>-88490</v>
+        <v>-88491</v>
       </c>
       <c r="M126" t="n">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="N126" t="n">
-        <v>11143</v>
+        <v>11142</v>
       </c>
       <c r="O126" t="n">
-        <v>6259</v>
+        <v>6258</v>
       </c>
       <c r="P126" t="n">
         <v>138</v>
       </c>
       <c r="Q126" t="n">
-        <v>195.4</v>
+        <v>195.3</v>
       </c>
       <c r="R126" t="n">
         <v>749</v>
       </c>
       <c r="S126" t="n">
-        <v>894.1</v>
+        <v>894</v>
       </c>
       <c r="T126" t="n">
         <v>71</v>
@@ -9630,28 +9630,28 @@
         <v>55303</v>
       </c>
       <c r="L127" t="n">
+        <v>10838</v>
+      </c>
+      <c r="M127" t="n">
+        <v>10648</v>
+      </c>
+      <c r="N127" t="n">
         <v>10839</v>
       </c>
-      <c r="M127" t="n">
-        <v>10649</v>
-      </c>
-      <c r="N127" t="n">
-        <v>10840</v>
-      </c>
       <c r="O127" t="n">
-        <v>6123</v>
+        <v>6122</v>
       </c>
       <c r="P127" t="n">
         <v>7497</v>
       </c>
       <c r="Q127" t="n">
-        <v>1521.3</v>
+        <v>1521.1</v>
       </c>
       <c r="R127" t="n">
         <v>635</v>
       </c>
       <c r="S127" t="n">
-        <v>874.7</v>
+        <v>874.6</v>
       </c>
       <c r="T127" t="n">
         <v>364</v>
@@ -9704,28 +9704,28 @@
         <v>57316</v>
       </c>
       <c r="L128" t="n">
-        <v>12859</v>
+        <v>12858</v>
       </c>
       <c r="M128" t="n">
-        <v>10774</v>
+        <v>10773</v>
       </c>
       <c r="N128" t="n">
-        <v>10598</v>
+        <v>10597</v>
       </c>
       <c r="O128" t="n">
-        <v>6045</v>
+        <v>6044</v>
       </c>
       <c r="P128" t="n">
         <v>2509</v>
       </c>
       <c r="Q128" t="n">
-        <v>1539.1</v>
+        <v>1539</v>
       </c>
       <c r="R128" t="n">
         <v>739</v>
       </c>
       <c r="S128" t="n">
-        <v>863.6</v>
+        <v>863.4</v>
       </c>
       <c r="T128" t="n">
         <v>24</v>
@@ -9778,13 +9778,13 @@
         <v>57539</v>
       </c>
       <c r="L129" t="n">
-        <v>12616</v>
+        <v>12615</v>
       </c>
       <c r="M129" t="n">
         <v>10607</v>
       </c>
       <c r="N129" t="n">
-        <v>10627</v>
+        <v>10626</v>
       </c>
       <c r="O129" t="n">
         <v>6038</v>
@@ -9852,13 +9852,13 @@
         <v>57815</v>
       </c>
       <c r="L130" t="n">
-        <v>12609</v>
+        <v>12608</v>
       </c>
       <c r="M130" t="n">
         <v>10715</v>
       </c>
       <c r="N130" t="n">
-        <v>10923</v>
+        <v>10922</v>
       </c>
       <c r="O130" t="n">
         <v>6356</v>
@@ -9926,13 +9926,13 @@
         <v>57932</v>
       </c>
       <c r="L131" t="n">
-        <v>12434</v>
+        <v>12433</v>
       </c>
       <c r="M131" t="n">
         <v>10789</v>
       </c>
       <c r="N131" t="n">
-        <v>10714</v>
+        <v>10713</v>
       </c>
       <c r="O131" t="n">
         <v>6294</v>
@@ -10000,13 +10000,13 @@
         <v>58347</v>
       </c>
       <c r="L132" t="n">
-        <v>12260</v>
+        <v>12259</v>
       </c>
       <c r="M132" t="n">
         <v>10623</v>
       </c>
       <c r="N132" t="n">
-        <v>10420</v>
+        <v>10419</v>
       </c>
       <c r="O132" t="n">
         <v>4018</v>
@@ -10074,13 +10074,13 @@
         <v>58779</v>
       </c>
       <c r="L133" t="n">
-        <v>12032</v>
+        <v>12031</v>
       </c>
       <c r="M133" t="n">
         <v>10664</v>
       </c>
       <c r="N133" t="n">
-        <v>10046</v>
+        <v>10045</v>
       </c>
       <c r="O133" t="n">
         <v>3787</v>
@@ -10148,13 +10148,13 @@
         <v>59109</v>
       </c>
       <c r="L134" t="n">
-        <v>13969</v>
+        <v>13968</v>
       </c>
       <c r="M134" t="n">
         <v>3320</v>
       </c>
       <c r="N134" t="n">
-        <v>9790</v>
+        <v>9789</v>
       </c>
       <c r="O134" t="n">
         <v>3667</v>
@@ -10222,13 +10222,13 @@
         <v>59457</v>
       </c>
       <c r="L135" t="n">
-        <v>11794</v>
+        <v>11793</v>
       </c>
       <c r="M135" t="n">
         <v>1020</v>
       </c>
       <c r="N135" t="n">
-        <v>9565</v>
+        <v>9564</v>
       </c>
       <c r="O135" t="n">
         <v>3520</v>
@@ -11536,7 +11536,7 @@
         <v>203</v>
       </c>
       <c r="F153" t="n">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="G153" t="n">
         <v>178</v>
@@ -11980,7 +11980,7 @@
         <v>1036</v>
       </c>
       <c r="F159" t="n">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="G159" t="n">
         <v>150</v>
@@ -12054,7 +12054,7 @@
         <v>1056</v>
       </c>
       <c r="F160" t="n">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="G160" t="n">
         <v>140</v>
@@ -16041,7 +16041,7 @@
         <v>1300</v>
       </c>
       <c r="C214" t="n">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="D214" t="n">
         <v>64890</v>
@@ -16059,37 +16059,37 @@
         <v>35024</v>
       </c>
       <c r="I214" t="n">
-        <v>184197</v>
+        <v>184196</v>
       </c>
       <c r="J214" t="n">
-        <v>472286</v>
+        <v>472285</v>
       </c>
       <c r="K214" t="n">
         <v>58181</v>
       </c>
       <c r="L214" t="n">
-        <v>52516</v>
+        <v>52515</v>
       </c>
       <c r="M214" t="n">
-        <v>16180</v>
+        <v>16179</v>
       </c>
       <c r="N214" t="n">
-        <v>101273</v>
+        <v>101272</v>
       </c>
       <c r="O214" t="n">
-        <v>55181</v>
+        <v>55180</v>
       </c>
       <c r="P214" t="n">
-        <v>27791</v>
+        <v>27790</v>
       </c>
       <c r="Q214" t="n">
-        <v>2311.4</v>
+        <v>2311.3</v>
       </c>
       <c r="R214" t="n">
-        <v>3816</v>
+        <v>3815</v>
       </c>
       <c r="S214" t="n">
-        <v>7883</v>
+        <v>7882.9</v>
       </c>
       <c r="T214" t="n">
         <v>82</v>
@@ -16133,37 +16133,37 @@
         <v>35074</v>
       </c>
       <c r="I215" t="n">
-        <v>194775</v>
+        <v>194774</v>
       </c>
       <c r="J215" t="n">
-        <v>480432</v>
+        <v>480431</v>
       </c>
       <c r="K215" t="n">
         <v>89628</v>
       </c>
       <c r="L215" t="n">
-        <v>35064</v>
+        <v>35063</v>
       </c>
       <c r="M215" t="n">
-        <v>18993</v>
+        <v>18992</v>
       </c>
       <c r="N215" t="n">
-        <v>104184</v>
+        <v>104183</v>
       </c>
       <c r="O215" t="n">
-        <v>57089</v>
+        <v>57088</v>
       </c>
       <c r="P215" t="n">
         <v>10578</v>
       </c>
       <c r="Q215" t="n">
-        <v>2713.3</v>
+        <v>2713.1</v>
       </c>
       <c r="R215" t="n">
         <v>8146</v>
       </c>
       <c r="S215" t="n">
-        <v>8155.6</v>
+        <v>8155.4</v>
       </c>
       <c r="T215" t="n">
         <v>50</v>
@@ -16207,37 +16207,37 @@
         <v>35155</v>
       </c>
       <c r="I216" t="n">
-        <v>197465</v>
+        <v>197464</v>
       </c>
       <c r="J216" t="n">
-        <v>490060</v>
+        <v>490059</v>
       </c>
       <c r="K216" t="n">
         <v>92049</v>
       </c>
       <c r="L216" t="n">
-        <v>35262</v>
+        <v>35261</v>
       </c>
       <c r="M216" t="n">
-        <v>18077</v>
+        <v>18076</v>
       </c>
       <c r="N216" t="n">
-        <v>106104</v>
+        <v>106103</v>
       </c>
       <c r="O216" t="n">
-        <v>56308</v>
+        <v>56307</v>
       </c>
       <c r="P216" t="n">
         <v>2690</v>
       </c>
       <c r="Q216" t="n">
-        <v>2582.4</v>
+        <v>2582.3</v>
       </c>
       <c r="R216" t="n">
         <v>9628</v>
       </c>
       <c r="S216" t="n">
-        <v>8044</v>
+        <v>8043.9</v>
       </c>
       <c r="T216" t="n">
         <v>81</v>
@@ -16281,37 +16281,37 @@
         <v>35210</v>
       </c>
       <c r="I217" t="n">
-        <v>200332</v>
+        <v>200331</v>
       </c>
       <c r="J217" t="n">
-        <v>499158</v>
+        <v>499157</v>
       </c>
       <c r="K217" t="n">
         <v>68476</v>
       </c>
       <c r="L217" t="n">
-        <v>35391</v>
+        <v>35390</v>
       </c>
       <c r="M217" t="n">
-        <v>17875</v>
+        <v>17874</v>
       </c>
       <c r="N217" t="n">
-        <v>107413</v>
+        <v>107412</v>
       </c>
       <c r="O217" t="n">
-        <v>55897</v>
+        <v>55896</v>
       </c>
       <c r="P217" t="n">
         <v>2867</v>
       </c>
       <c r="Q217" t="n">
-        <v>2553.6</v>
+        <v>2553.4</v>
       </c>
       <c r="R217" t="n">
         <v>9098</v>
       </c>
       <c r="S217" t="n">
-        <v>7985.3</v>
+        <v>7985.1</v>
       </c>
       <c r="T217" t="n">
         <v>55</v>
@@ -16355,37 +16355,37 @@
         <v>35283</v>
       </c>
       <c r="I218" t="n">
-        <v>203461</v>
+        <v>203460</v>
       </c>
       <c r="J218" t="n">
-        <v>508836</v>
+        <v>508835</v>
       </c>
       <c r="K218" t="n">
         <v>95317</v>
       </c>
       <c r="L218" t="n">
-        <v>59525</v>
+        <v>59524</v>
       </c>
       <c r="M218" t="n">
-        <v>43435</v>
+        <v>43434</v>
       </c>
       <c r="N218" t="n">
-        <v>109165</v>
+        <v>109164</v>
       </c>
       <c r="O218" t="n">
-        <v>56246</v>
+        <v>56245</v>
       </c>
       <c r="P218" t="n">
         <v>3129</v>
       </c>
       <c r="Q218" t="n">
-        <v>6205</v>
+        <v>6204.9</v>
       </c>
       <c r="R218" t="n">
         <v>9678</v>
       </c>
       <c r="S218" t="n">
-        <v>8035.1</v>
+        <v>8035</v>
       </c>
       <c r="T218" t="n">
         <v>73</v>
@@ -16429,37 +16429,37 @@
         <v>35330</v>
       </c>
       <c r="I219" t="n">
-        <v>178988</v>
+        <v>178987</v>
       </c>
       <c r="J219" t="n">
-        <v>520425</v>
+        <v>520424</v>
       </c>
       <c r="K219" t="n">
         <v>77034</v>
       </c>
       <c r="L219" t="n">
-        <v>32665</v>
+        <v>32664</v>
       </c>
       <c r="M219" t="n">
-        <v>16336</v>
+        <v>16335</v>
       </c>
       <c r="N219" t="n">
-        <v>111441</v>
+        <v>111440</v>
       </c>
       <c r="O219" t="n">
-        <v>57334</v>
+        <v>57333</v>
       </c>
       <c r="P219" t="n">
         <v>-24473</v>
       </c>
       <c r="Q219" t="n">
-        <v>2333.7</v>
+        <v>2333.6</v>
       </c>
       <c r="R219" t="n">
         <v>11589</v>
       </c>
       <c r="S219" t="n">
-        <v>8190.6</v>
+        <v>8190.4</v>
       </c>
       <c r="T219" t="n">
         <v>47</v>
@@ -16503,37 +16503,37 @@
         <v>35355</v>
       </c>
       <c r="I220" t="n">
-        <v>171388</v>
+        <v>171387</v>
       </c>
       <c r="J220" t="n">
-        <v>526980</v>
+        <v>526979</v>
       </c>
       <c r="K220" t="n">
         <v>42820</v>
       </c>
       <c r="L220" t="n">
-        <v>29134</v>
+        <v>29133</v>
       </c>
       <c r="M220" t="n">
-        <v>14982</v>
+        <v>14981</v>
       </c>
       <c r="N220" t="n">
-        <v>112853</v>
+        <v>112852</v>
       </c>
       <c r="O220" t="n">
-        <v>58510</v>
+        <v>58509</v>
       </c>
       <c r="P220" t="n">
         <v>-7600</v>
       </c>
       <c r="Q220" t="n">
-        <v>2140.3</v>
+        <v>2140.1</v>
       </c>
       <c r="R220" t="n">
         <v>6555</v>
       </c>
       <c r="S220" t="n">
-        <v>8358.6</v>
+        <v>8358.4</v>
       </c>
       <c r="T220" t="n">
         <v>25</v>
@@ -16568,7 +16568,7 @@
         <v>16009</v>
       </c>
       <c r="F221" t="n">
-        <v>7033</v>
+        <v>7034</v>
       </c>
       <c r="G221" t="n">
         <v>810</v>
@@ -16577,22 +16577,22 @@
         <v>35446</v>
       </c>
       <c r="I221" t="n">
-        <v>200956</v>
+        <v>200955</v>
       </c>
       <c r="J221" t="n">
-        <v>531287</v>
+        <v>531286</v>
       </c>
       <c r="K221" t="n">
         <v>63593</v>
       </c>
       <c r="L221" t="n">
-        <v>32939</v>
+        <v>32938</v>
       </c>
       <c r="M221" t="n">
         <v>16759</v>
       </c>
       <c r="N221" t="n">
-        <v>114182</v>
+        <v>114181</v>
       </c>
       <c r="O221" t="n">
         <v>59001</v>
@@ -16642,7 +16642,7 @@
         <v>17779</v>
       </c>
       <c r="F222" t="n">
-        <v>7269</v>
+        <v>7270</v>
       </c>
       <c r="G222" t="n">
         <v>1027</v>
@@ -16651,22 +16651,22 @@
         <v>35529</v>
       </c>
       <c r="I222" t="n">
-        <v>212527</v>
+        <v>212526</v>
       </c>
       <c r="J222" t="n">
-        <v>539478</v>
+        <v>539477</v>
       </c>
       <c r="K222" t="n">
         <v>101199</v>
       </c>
       <c r="L222" t="n">
-        <v>36745</v>
+        <v>36744</v>
       </c>
       <c r="M222" t="n">
         <v>17752</v>
       </c>
       <c r="N222" t="n">
-        <v>116135</v>
+        <v>116134</v>
       </c>
       <c r="O222" t="n">
         <v>59046</v>
@@ -16716,7 +16716,7 @@
         <v>17840</v>
       </c>
       <c r="F223" t="n">
-        <v>7384</v>
+        <v>7386</v>
       </c>
       <c r="G223" t="n">
         <v>1052</v>
@@ -16725,22 +16725,22 @@
         <v>35609</v>
       </c>
       <c r="I223" t="n">
-        <v>215435</v>
+        <v>215434</v>
       </c>
       <c r="J223" t="n">
-        <v>550295</v>
+        <v>550294</v>
       </c>
       <c r="K223" t="n">
         <v>103135</v>
       </c>
       <c r="L223" t="n">
-        <v>36047</v>
+        <v>36046</v>
       </c>
       <c r="M223" t="n">
         <v>17970</v>
       </c>
       <c r="N223" t="n">
-        <v>116543</v>
+        <v>116542</v>
       </c>
       <c r="O223" t="n">
         <v>60235</v>
@@ -16790,7 +16790,7 @@
         <v>18013</v>
       </c>
       <c r="F224" t="n">
-        <v>7522</v>
+        <v>7524</v>
       </c>
       <c r="G224" t="n">
         <v>1053</v>
@@ -16799,22 +16799,22 @@
         <v>35682</v>
       </c>
       <c r="I224" t="n">
-        <v>218503</v>
+        <v>218502</v>
       </c>
       <c r="J224" t="n">
-        <v>560943</v>
+        <v>560942</v>
       </c>
       <c r="K224" t="n">
         <v>104838</v>
       </c>
       <c r="L224" t="n">
-        <v>36046</v>
+        <v>36045</v>
       </c>
       <c r="M224" t="n">
         <v>18171</v>
       </c>
       <c r="N224" t="n">
-        <v>117682</v>
+        <v>117681</v>
       </c>
       <c r="O224" t="n">
         <v>61785</v>
@@ -16864,7 +16864,7 @@
         <v>17776</v>
       </c>
       <c r="F225" t="n">
-        <v>7591</v>
+        <v>7593</v>
       </c>
       <c r="G225" t="n">
         <v>1080</v>
@@ -16873,22 +16873,22 @@
         <v>35774</v>
       </c>
       <c r="I225" t="n">
-        <v>221594</v>
+        <v>221593</v>
       </c>
       <c r="J225" t="n">
-        <v>572233</v>
+        <v>572232</v>
       </c>
       <c r="K225" t="n">
         <v>106912</v>
       </c>
       <c r="L225" t="n">
-        <v>61568</v>
+        <v>61567</v>
       </c>
       <c r="M225" t="n">
         <v>18133</v>
       </c>
       <c r="N225" t="n">
-        <v>119643</v>
+        <v>119642</v>
       </c>
       <c r="O225" t="n">
         <v>63397</v>
@@ -16938,7 +16938,7 @@
         <v>9661</v>
       </c>
       <c r="F226" t="n">
-        <v>7644</v>
+        <v>7645</v>
       </c>
       <c r="G226" t="n">
         <v>775</v>
@@ -16947,22 +16947,22 @@
         <v>35813</v>
       </c>
       <c r="I226" t="n">
-        <v>194046</v>
+        <v>194045</v>
       </c>
       <c r="J226" t="n">
-        <v>584421</v>
+        <v>584420</v>
       </c>
       <c r="K226" t="n">
         <v>86255</v>
       </c>
       <c r="L226" t="n">
-        <v>31394</v>
+        <v>31393</v>
       </c>
       <c r="M226" t="n">
         <v>15058</v>
       </c>
       <c r="N226" t="n">
-        <v>121330</v>
+        <v>121329</v>
       </c>
       <c r="O226" t="n">
         <v>63996</v>
@@ -17012,7 +17012,7 @@
         <v>7801</v>
       </c>
       <c r="F227" t="n">
-        <v>7708</v>
+        <v>7709</v>
       </c>
       <c r="G227" t="n">
         <v>666</v>
@@ -17021,22 +17021,22 @@
         <v>35849</v>
       </c>
       <c r="I227" t="n">
-        <v>195751</v>
+        <v>195750</v>
       </c>
       <c r="J227" t="n">
-        <v>591683</v>
+        <v>591682</v>
       </c>
       <c r="K227" t="n">
         <v>55418</v>
       </c>
       <c r="L227" t="n">
-        <v>39345</v>
+        <v>39344</v>
       </c>
       <c r="M227" t="n">
         <v>24363</v>
       </c>
       <c r="N227" t="n">
-        <v>123213</v>
+        <v>123212</v>
       </c>
       <c r="O227" t="n">
         <v>64703</v>
@@ -17086,7 +17086,7 @@
         <v>16919</v>
       </c>
       <c r="F228" t="n">
-        <v>8308</v>
+        <v>8309</v>
       </c>
       <c r="G228" t="n">
         <v>1036</v>
@@ -17095,10 +17095,10 @@
         <v>35987</v>
       </c>
       <c r="I228" t="n">
-        <v>228030</v>
+        <v>228029</v>
       </c>
       <c r="J228" t="n">
-        <v>596959</v>
+        <v>596958</v>
       </c>
       <c r="K228" t="n">
         <v>78986</v>
@@ -17160,7 +17160,7 @@
         <v>16881</v>
       </c>
       <c r="F229" t="n">
-        <v>8491</v>
+        <v>8492</v>
       </c>
       <c r="G229" t="n">
         <v>1036</v>
@@ -17169,10 +17169,10 @@
         <v>36092</v>
       </c>
       <c r="I229" t="n">
-        <v>230701</v>
+        <v>230700</v>
       </c>
       <c r="J229" t="n">
-        <v>606146</v>
+        <v>606145</v>
       </c>
       <c r="K229" t="n">
         <v>113177</v>
@@ -17225,7 +17225,7 @@
         <v>1637</v>
       </c>
       <c r="C230" t="n">
-        <v>4386</v>
+        <v>4408</v>
       </c>
       <c r="D230" t="n">
         <v>66230</v>
@@ -17243,37 +17243,37 @@
         <v>36197</v>
       </c>
       <c r="I230" t="n">
-        <v>233502</v>
+        <v>233523</v>
       </c>
       <c r="J230" t="n">
-        <v>617903</v>
+        <v>617924</v>
       </c>
       <c r="K230" t="n">
         <v>115493</v>
       </c>
       <c r="L230" t="n">
-        <v>36037</v>
+        <v>36059</v>
       </c>
       <c r="M230" t="n">
-        <v>18067</v>
+        <v>18089</v>
       </c>
       <c r="N230" t="n">
-        <v>127843</v>
+        <v>127865</v>
       </c>
       <c r="O230" t="n">
-        <v>67608</v>
+        <v>67630</v>
       </c>
       <c r="P230" t="n">
-        <v>2801</v>
+        <v>2823</v>
       </c>
       <c r="Q230" t="n">
-        <v>2581</v>
+        <v>2584.1</v>
       </c>
       <c r="R230" t="n">
-        <v>11757</v>
+        <v>11779</v>
       </c>
       <c r="S230" t="n">
-        <v>9658.3</v>
+        <v>9661.4</v>
       </c>
       <c r="T230" t="n">
         <v>105</v>
@@ -17299,7 +17299,7 @@
         <v>1837</v>
       </c>
       <c r="C231" t="n">
-        <v>4303</v>
+        <v>4340</v>
       </c>
       <c r="D231" t="n">
         <v>66498</v>
@@ -17317,37 +17317,37 @@
         <v>36308</v>
       </c>
       <c r="I231" t="n">
-        <v>236271</v>
+        <v>236329</v>
       </c>
       <c r="J231" t="n">
-        <v>628502</v>
+        <v>628560</v>
       </c>
       <c r="K231" t="n">
         <v>83274</v>
       </c>
       <c r="L231" t="n">
-        <v>35939</v>
+        <v>35998</v>
       </c>
       <c r="M231" t="n">
-        <v>17768</v>
+        <v>17827</v>
       </c>
       <c r="N231" t="n">
-        <v>129344</v>
+        <v>129403</v>
       </c>
       <c r="O231" t="n">
-        <v>67559</v>
+        <v>67618</v>
       </c>
       <c r="P231" t="n">
-        <v>2769</v>
+        <v>2806</v>
       </c>
       <c r="Q231" t="n">
-        <v>2538.3</v>
+        <v>2546.7</v>
       </c>
       <c r="R231" t="n">
-        <v>10599</v>
+        <v>10636</v>
       </c>
       <c r="S231" t="n">
-        <v>9651.3</v>
+        <v>9659.7</v>
       </c>
       <c r="T231" t="n">
         <v>111</v>
@@ -17373,7 +17373,7 @@
         <v>1873</v>
       </c>
       <c r="C232" t="n">
-        <v>4599</v>
+        <v>4611</v>
       </c>
       <c r="D232" t="n">
         <v>67048</v>
@@ -17388,55 +17388,55 @@
         <v>1248</v>
       </c>
       <c r="H232" t="n">
-        <v>36429</v>
+        <v>36430</v>
       </c>
       <c r="I232" t="n">
-        <v>239309</v>
+        <v>239379</v>
       </c>
       <c r="J232" t="n">
-        <v>639079</v>
+        <v>639149</v>
       </c>
       <c r="K232" t="n">
         <v>119087</v>
       </c>
       <c r="L232" t="n">
-        <v>35848</v>
+        <v>35919</v>
       </c>
       <c r="M232" t="n">
-        <v>17715</v>
+        <v>17786</v>
       </c>
       <c r="N232" t="n">
-        <v>130243</v>
+        <v>130314</v>
       </c>
       <c r="O232" t="n">
-        <v>66846</v>
+        <v>66917</v>
       </c>
       <c r="P232" t="n">
-        <v>3038</v>
+        <v>3050</v>
       </c>
       <c r="Q232" t="n">
-        <v>2530.7</v>
+        <v>2540.9</v>
       </c>
       <c r="R232" t="n">
-        <v>10577</v>
+        <v>10589</v>
       </c>
       <c r="S232" t="n">
-        <v>9549.4</v>
+        <v>9559.6</v>
       </c>
       <c r="T232" t="n">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="U232" t="n">
         <v>0.3</v>
       </c>
       <c r="V232" t="n">
-        <v>112.3</v>
+        <v>112.7</v>
       </c>
       <c r="W232" t="n">
-        <v>93.6</v>
+        <v>93.7</v>
       </c>
       <c r="X232" t="n">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="233">
@@ -17447,7 +17447,7 @@
         <v>2255</v>
       </c>
       <c r="C233" t="n">
-        <v>4907</v>
+        <v>4988</v>
       </c>
       <c r="D233" t="n">
         <v>67317</v>
@@ -17462,40 +17462,40 @@
         <v>831</v>
       </c>
       <c r="H233" t="n">
-        <v>36476</v>
+        <v>36477</v>
       </c>
       <c r="I233" t="n">
-        <v>209984</v>
+        <v>210135</v>
       </c>
       <c r="J233" t="n">
-        <v>639337</v>
+        <v>639495</v>
       </c>
       <c r="K233" t="n">
         <v>97749</v>
       </c>
       <c r="L233" t="n">
-        <v>30996</v>
+        <v>31148</v>
       </c>
       <c r="M233" t="n">
-        <v>15938</v>
+        <v>16090</v>
       </c>
       <c r="N233" t="n">
-        <v>118912</v>
+        <v>119071</v>
       </c>
       <c r="O233" t="n">
-        <v>54916</v>
+        <v>55075</v>
       </c>
       <c r="P233" t="n">
-        <v>-29325</v>
+        <v>-29244</v>
       </c>
       <c r="Q233" t="n">
-        <v>2276.9</v>
+        <v>2298.6</v>
       </c>
       <c r="R233" t="n">
-        <v>258</v>
+        <v>346</v>
       </c>
       <c r="S233" t="n">
-        <v>7845.1</v>
+        <v>7867.9</v>
       </c>
       <c r="T233" t="n">
         <v>47</v>
@@ -17504,13 +17504,13 @@
         <v>0.1</v>
       </c>
       <c r="V233" t="n">
-        <v>93</v>
+        <v>93.3</v>
       </c>
       <c r="W233" t="n">
-        <v>94.7</v>
+        <v>94.9</v>
       </c>
       <c r="X233" t="n">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="234">
@@ -17521,7 +17521,7 @@
         <v>2203</v>
       </c>
       <c r="C234" t="n">
-        <v>2514</v>
+        <v>2617</v>
       </c>
       <c r="D234" t="n">
         <v>67317</v>
@@ -17530,61 +17530,61 @@
         <v>8367</v>
       </c>
       <c r="F234" t="n">
-        <v>8828</v>
+        <v>8825</v>
       </c>
       <c r="G234" t="n">
-        <v>661</v>
+        <v>717</v>
       </c>
       <c r="H234" t="n">
-        <v>36507</v>
+        <v>36513</v>
       </c>
       <c r="I234" t="n">
-        <v>211445</v>
+        <v>211699</v>
       </c>
       <c r="J234" t="n">
-        <v>646049</v>
+        <v>646253</v>
       </c>
       <c r="K234" t="n">
         <v>63482</v>
       </c>
       <c r="L234" t="n">
-        <v>40057</v>
+        <v>40312</v>
       </c>
       <c r="M234" t="n">
-        <v>15694</v>
+        <v>15949</v>
       </c>
       <c r="N234" t="n">
-        <v>119069</v>
+        <v>119274</v>
       </c>
       <c r="O234" t="n">
-        <v>54366</v>
+        <v>54571</v>
       </c>
       <c r="P234" t="n">
-        <v>1461</v>
+        <v>1564</v>
       </c>
       <c r="Q234" t="n">
-        <v>2242</v>
+        <v>2278.4</v>
       </c>
       <c r="R234" t="n">
-        <v>6712</v>
+        <v>6758</v>
       </c>
       <c r="S234" t="n">
-        <v>7766.6</v>
+        <v>7795.9</v>
       </c>
       <c r="T234" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="U234" t="n">
         <v>0.1</v>
       </c>
       <c r="V234" t="n">
-        <v>66.3</v>
+        <v>68.3</v>
       </c>
       <c r="W234" t="n">
-        <v>94</v>
+        <v>94.9</v>
       </c>
       <c r="X234" t="n">
-        <v>658</v>
+        <v>664</v>
       </c>
     </row>
     <row r="235">
@@ -17592,10 +17592,10 @@
         <v>44094</v>
       </c>
       <c r="B235" t="n">
-        <v>1124</v>
+        <v>1300</v>
       </c>
       <c r="C235" t="n">
-        <v>1427</v>
+        <v>2075</v>
       </c>
       <c r="D235" t="n">
         <v>67352</v>
@@ -17604,61 +17604,61 @@
         <v>8572</v>
       </c>
       <c r="F235" t="n">
-        <v>9195</v>
+        <v>9234</v>
       </c>
       <c r="G235" t="n">
-        <v>827</v>
+        <v>972</v>
       </c>
       <c r="H235" t="n">
-        <v>36642</v>
+        <v>36652</v>
       </c>
       <c r="I235" t="n">
-        <v>212216</v>
+        <v>212740</v>
       </c>
       <c r="J235" t="n">
-        <v>649529</v>
+        <v>650557</v>
       </c>
       <c r="K235" t="n">
-        <v>60034</v>
+        <v>66432</v>
       </c>
       <c r="L235" t="n">
-        <v>11260</v>
+        <v>11785</v>
       </c>
       <c r="M235" t="n">
-        <v>-15814</v>
+        <v>-15289</v>
       </c>
       <c r="N235" t="n">
-        <v>118242</v>
+        <v>119271</v>
       </c>
       <c r="O235" t="n">
-        <v>52570</v>
+        <v>53599</v>
       </c>
       <c r="P235" t="n">
-        <v>771</v>
+        <v>1041</v>
       </c>
       <c r="Q235" t="n">
-        <v>-2259.1</v>
+        <v>-2184.1</v>
       </c>
       <c r="R235" t="n">
-        <v>3480</v>
+        <v>4304</v>
       </c>
       <c r="S235" t="n">
-        <v>7510</v>
+        <v>7657</v>
       </c>
       <c r="T235" t="n">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="U235" t="n">
         <v>0.4</v>
       </c>
       <c r="V235" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="W235" t="n">
-        <v>93.6</v>
+        <v>95</v>
       </c>
       <c r="X235" t="n">
-        <v>655</v>
+        <v>665</v>
       </c>
     </row>
     <row r="236">
@@ -17669,70 +17669,144 @@
         <v>717</v>
       </c>
       <c r="C236" t="n">
-        <v>3041</v>
+        <v>3417</v>
       </c>
       <c r="D236" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E236" t="n">
-        <v>6972</v>
+        <v>8141</v>
       </c>
       <c r="F236" t="n">
-        <v>9298</v>
+        <v>9338</v>
       </c>
       <c r="G236" t="n">
-        <v>286</v>
+        <v>586</v>
       </c>
       <c r="H236" t="n">
-        <v>36694</v>
+        <v>36714</v>
       </c>
       <c r="I236" t="n">
-        <v>25332</v>
+        <v>189367</v>
       </c>
       <c r="J236" t="n">
-        <v>653788</v>
+        <v>655551</v>
       </c>
       <c r="K236" t="n">
-        <v>87572</v>
+        <v>89986</v>
       </c>
       <c r="L236" t="n">
-        <v>-187195</v>
+        <v>-23159</v>
       </c>
       <c r="M236" t="n">
-        <v>-205369</v>
+        <v>-41333</v>
       </c>
       <c r="N236" t="n">
-        <v>114310</v>
+        <v>116074</v>
       </c>
       <c r="O236" t="n">
-        <v>47642</v>
+        <v>49406</v>
       </c>
       <c r="P236" t="n">
-        <v>-186884</v>
+        <v>-23373</v>
       </c>
       <c r="Q236" t="n">
-        <v>-29338.4</v>
+        <v>-5904.7</v>
       </c>
       <c r="R236" t="n">
-        <v>4259</v>
+        <v>4994</v>
       </c>
       <c r="S236" t="n">
-        <v>6806</v>
+        <v>7058</v>
       </c>
       <c r="T236" t="n">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="U236" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="V236" t="n">
-        <v>72.7</v>
+        <v>79</v>
       </c>
       <c r="W236" t="n">
-        <v>86</v>
+        <v>88.9</v>
       </c>
       <c r="X236" t="n">
-        <v>602</v>
+        <v>622</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="n">
+        <v>44096</v>
+      </c>
+      <c r="B237" t="n">
+        <v>723</v>
+      </c>
+      <c r="C237" t="n">
+        <v>0</v>
+      </c>
+      <c r="D237" t="n">
+        <v>0</v>
+      </c>
+      <c r="E237" t="n">
+        <v>0</v>
+      </c>
+      <c r="F237" t="n">
+        <v>556</v>
+      </c>
+      <c r="G237" t="n">
+        <v>80</v>
+      </c>
+      <c r="H237" t="n">
+        <v>2236</v>
+      </c>
+      <c r="I237" t="n">
+        <v>0</v>
+      </c>
+      <c r="J237" t="n">
+        <v>48784</v>
+      </c>
+      <c r="K237" t="n">
+        <v>9946</v>
+      </c>
+      <c r="L237" t="n">
+        <v>-215434</v>
+      </c>
+      <c r="M237" t="n">
+        <v>-233523</v>
+      </c>
+      <c r="N237" t="n">
+        <v>-501510</v>
+      </c>
+      <c r="O237" t="n">
+        <v>-569140</v>
+      </c>
+      <c r="P237" t="n">
+        <v>-189367</v>
+      </c>
+      <c r="Q237" t="n">
+        <v>-33360.4</v>
+      </c>
+      <c r="R237" t="n">
+        <v>-606767</v>
+      </c>
+      <c r="S237" t="n">
+        <v>-81305.7</v>
+      </c>
+      <c r="T237" t="n">
+        <v>-34478</v>
+      </c>
+      <c r="U237" t="n">
+        <v>-93.9</v>
+      </c>
+      <c r="V237" t="n">
+        <v>-11425.7</v>
+      </c>
+      <c r="W237" t="n">
+        <v>-4851.6</v>
+      </c>
+      <c r="X237" t="n">
+        <v>-33961</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualiza provincias 2º 2020-11-23. Corrige erratas README #22
</commit_message>
<xml_diff>
--- a/data/output/covid19-spain_consolidated.xlsx
+++ b/data/output/covid19-spain_consolidated.xlsx
@@ -14860,7 +14860,7 @@
         <v>1220</v>
       </c>
       <c r="D198" t="n">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E198" t="n">
         <v>1591</v>
@@ -14875,7 +14875,7 @@
         <v>35466</v>
       </c>
       <c r="I198" t="n">
-        <v>114606</v>
+        <v>114605</v>
       </c>
       <c r="J198" t="n">
         <v>277536</v>
@@ -14884,10 +14884,10 @@
         <v>67569</v>
       </c>
       <c r="L198" t="n">
-        <v>9464</v>
+        <v>9463</v>
       </c>
       <c r="M198" t="n">
-        <v>6502</v>
+        <v>6501</v>
       </c>
       <c r="N198" t="n">
         <v>11901</v>
@@ -14896,10 +14896,10 @@
         <v>7679</v>
       </c>
       <c r="P198" t="n">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="Q198" t="n">
-        <v>928.9</v>
+        <v>928.7</v>
       </c>
       <c r="R198" t="n">
         <v>1629</v>
@@ -14949,7 +14949,7 @@
         <v>35473</v>
       </c>
       <c r="I199" t="n">
-        <v>115996</v>
+        <v>115995</v>
       </c>
       <c r="J199" t="n">
         <v>279342</v>
@@ -14958,10 +14958,10 @@
         <v>62774</v>
       </c>
       <c r="L199" t="n">
-        <v>10441</v>
+        <v>10440</v>
       </c>
       <c r="M199" t="n">
-        <v>7092</v>
+        <v>7091</v>
       </c>
       <c r="N199" t="n">
         <v>13051</v>
@@ -14973,7 +14973,7 @@
         <v>1390</v>
       </c>
       <c r="Q199" t="n">
-        <v>1013.1</v>
+        <v>1013</v>
       </c>
       <c r="R199" t="n">
         <v>1806</v>
@@ -15023,7 +15023,7 @@
         <v>35480</v>
       </c>
       <c r="I200" t="n">
-        <v>121121</v>
+        <v>121120</v>
       </c>
       <c r="J200" t="n">
         <v>281528</v>
@@ -15032,10 +15032,10 @@
         <v>66142</v>
       </c>
       <c r="L200" t="n">
-        <v>15130</v>
+        <v>15129</v>
       </c>
       <c r="M200" t="n">
-        <v>11212</v>
+        <v>11211</v>
       </c>
       <c r="N200" t="n">
         <v>14432</v>
@@ -15047,7 +15047,7 @@
         <v>5125</v>
       </c>
       <c r="Q200" t="n">
-        <v>1601.7</v>
+        <v>1601.6</v>
       </c>
       <c r="R200" t="n">
         <v>2186</v>
@@ -15097,7 +15097,7 @@
         <v>35484</v>
       </c>
       <c r="I201" t="n">
-        <v>121890</v>
+        <v>121889</v>
       </c>
       <c r="J201" t="n">
         <v>282984</v>
@@ -15106,10 +15106,10 @@
         <v>35666</v>
       </c>
       <c r="L201" t="n">
-        <v>15691</v>
+        <v>15690</v>
       </c>
       <c r="M201" t="n">
-        <v>11654</v>
+        <v>11653</v>
       </c>
       <c r="N201" t="n">
         <v>15600</v>
@@ -15121,7 +15121,7 @@
         <v>769</v>
       </c>
       <c r="Q201" t="n">
-        <v>1664.9</v>
+        <v>1664.7</v>
       </c>
       <c r="R201" t="n">
         <v>1456</v>
@@ -15171,7 +15171,7 @@
         <v>35490</v>
       </c>
       <c r="I202" t="n">
-        <v>123786</v>
+        <v>123785</v>
       </c>
       <c r="J202" t="n">
         <v>284076</v>
@@ -15180,10 +15180,10 @@
         <v>32040</v>
       </c>
       <c r="L202" t="n">
-        <v>17400</v>
+        <v>17399</v>
       </c>
       <c r="M202" t="n">
-        <v>13073</v>
+        <v>13072</v>
       </c>
       <c r="N202" t="n">
         <v>16458</v>
@@ -15195,7 +15195,7 @@
         <v>1896</v>
       </c>
       <c r="Q202" t="n">
-        <v>1867.6</v>
+        <v>1867.4</v>
       </c>
       <c r="R202" t="n">
         <v>1092</v>
@@ -15245,7 +15245,7 @@
         <v>35505</v>
       </c>
       <c r="I203" t="n">
-        <v>125531</v>
+        <v>125530</v>
       </c>
       <c r="J203" t="n">
         <v>285968</v>
@@ -15254,10 +15254,10 @@
         <v>68199</v>
       </c>
       <c r="L203" t="n">
-        <v>18807</v>
+        <v>18806</v>
       </c>
       <c r="M203" t="n">
-        <v>13738</v>
+        <v>13737</v>
       </c>
       <c r="N203" t="n">
         <v>17867</v>
@@ -15269,7 +15269,7 @@
         <v>1745</v>
       </c>
       <c r="Q203" t="n">
-        <v>1962.6</v>
+        <v>1962.4</v>
       </c>
       <c r="R203" t="n">
         <v>1892</v>
@@ -15319,7 +15319,7 @@
         <v>35522</v>
       </c>
       <c r="I204" t="n">
-        <v>127541</v>
+        <v>127540</v>
       </c>
       <c r="J204" t="n">
         <v>288499</v>
@@ -15328,10 +15328,10 @@
         <v>66625</v>
       </c>
       <c r="L204" t="n">
-        <v>20202</v>
+        <v>20201</v>
       </c>
       <c r="M204" t="n">
-        <v>14377</v>
+        <v>14376</v>
       </c>
       <c r="N204" t="n">
         <v>19500</v>
@@ -15343,7 +15343,7 @@
         <v>2010</v>
       </c>
       <c r="Q204" t="n">
-        <v>2053.9</v>
+        <v>2053.7</v>
       </c>
       <c r="R204" t="n">
         <v>2531</v>
@@ -15393,7 +15393,7 @@
         <v>35530</v>
       </c>
       <c r="I205" t="n">
-        <v>129603</v>
+        <v>129602</v>
       </c>
       <c r="J205" t="n">
         <v>290966</v>
@@ -15402,7 +15402,7 @@
         <v>74114</v>
       </c>
       <c r="L205" t="n">
-        <v>21499</v>
+        <v>21498</v>
       </c>
       <c r="M205" t="n">
         <v>14997</v>
@@ -15467,7 +15467,7 @@
         <v>35536</v>
       </c>
       <c r="I206" t="n">
-        <v>131444</v>
+        <v>131443</v>
       </c>
       <c r="J206" t="n">
         <v>293281</v>
@@ -15476,7 +15476,7 @@
         <v>66928</v>
       </c>
       <c r="L206" t="n">
-        <v>22540</v>
+        <v>22539</v>
       </c>
       <c r="M206" t="n">
         <v>15448</v>
@@ -15541,7 +15541,7 @@
         <v>35544</v>
       </c>
       <c r="I207" t="n">
-        <v>132980</v>
+        <v>132979</v>
       </c>
       <c r="J207" t="n">
         <v>296138</v>
@@ -15550,7 +15550,7 @@
         <v>67255</v>
       </c>
       <c r="L207" t="n">
-        <v>23071</v>
+        <v>23070</v>
       </c>
       <c r="M207" t="n">
         <v>11859</v>
@@ -15615,7 +15615,7 @@
         <v>35556</v>
       </c>
       <c r="I208" t="n">
-        <v>133740</v>
+        <v>133739</v>
       </c>
       <c r="J208" t="n">
         <v>297682</v>
@@ -15624,7 +15624,7 @@
         <v>39981</v>
       </c>
       <c r="L208" t="n">
-        <v>23504</v>
+        <v>23503</v>
       </c>
       <c r="M208" t="n">
         <v>11850</v>
@@ -15689,7 +15689,7 @@
         <v>35572</v>
       </c>
       <c r="I209" t="n">
-        <v>135583</v>
+        <v>135582</v>
       </c>
       <c r="J209" t="n">
         <v>299087</v>
@@ -15698,7 +15698,7 @@
         <v>43941</v>
       </c>
       <c r="L209" t="n">
-        <v>24870</v>
+        <v>24869</v>
       </c>
       <c r="M209" t="n">
         <v>11797</v>
@@ -15763,7 +15763,7 @@
         <v>35588</v>
       </c>
       <c r="I210" t="n">
-        <v>137069</v>
+        <v>137068</v>
       </c>
       <c r="J210" t="n">
         <v>301344</v>
@@ -15772,7 +15772,7 @@
         <v>71506</v>
       </c>
       <c r="L210" t="n">
-        <v>25276</v>
+        <v>25275</v>
       </c>
       <c r="M210" t="n">
         <v>11538</v>
@@ -15837,7 +15837,7 @@
         <v>35603</v>
       </c>
       <c r="I211" t="n">
-        <v>139094</v>
+        <v>139093</v>
       </c>
       <c r="J211" t="n">
         <v>304329</v>
@@ -15846,7 +15846,7 @@
         <v>75012</v>
       </c>
       <c r="L211" t="n">
-        <v>25930</v>
+        <v>25929</v>
       </c>
       <c r="M211" t="n">
         <v>11553</v>
@@ -15911,7 +15911,7 @@
         <v>35621</v>
       </c>
       <c r="I212" t="n">
-        <v>141094</v>
+        <v>141093</v>
       </c>
       <c r="J212" t="n">
         <v>307330</v>
@@ -15985,7 +15985,7 @@
         <v>35638</v>
       </c>
       <c r="I213" t="n">
-        <v>142675</v>
+        <v>142674</v>
       </c>
       <c r="J213" t="n">
         <v>310902</v>
@@ -16059,7 +16059,7 @@
         <v>35649</v>
       </c>
       <c r="I214" t="n">
-        <v>144465</v>
+        <v>144464</v>
       </c>
       <c r="J214" t="n">
         <v>314839</v>
@@ -16133,7 +16133,7 @@
         <v>35660</v>
       </c>
       <c r="I215" t="n">
-        <v>145356</v>
+        <v>145355</v>
       </c>
       <c r="J215" t="n">
         <v>317725</v>
@@ -16207,7 +16207,7 @@
         <v>35685</v>
       </c>
       <c r="I216" t="n">
-        <v>148726</v>
+        <v>148725</v>
       </c>
       <c r="J216" t="n">
         <v>319370</v>
@@ -16281,7 +16281,7 @@
         <v>35706</v>
       </c>
       <c r="I217" t="n">
-        <v>150397</v>
+        <v>150396</v>
       </c>
       <c r="J217" t="n">
         <v>322512</v>
@@ -16355,7 +16355,7 @@
         <v>35734</v>
       </c>
       <c r="I218" t="n">
-        <v>152738</v>
+        <v>152737</v>
       </c>
       <c r="J218" t="n">
         <v>326837</v>
@@ -16429,7 +16429,7 @@
         <v>35748</v>
       </c>
       <c r="I219" t="n">
-        <v>154680</v>
+        <v>154679</v>
       </c>
       <c r="J219" t="n">
         <v>330943</v>
@@ -16503,7 +16503,7 @@
         <v>35769</v>
       </c>
       <c r="I220" t="n">
-        <v>157099</v>
+        <v>157098</v>
       </c>
       <c r="J220" t="n">
         <v>335740</v>
@@ -16577,7 +16577,7 @@
         <v>35781</v>
       </c>
       <c r="I221" t="n">
-        <v>159094</v>
+        <v>159093</v>
       </c>
       <c r="J221" t="n">
         <v>341388</v>
@@ -16651,7 +16651,7 @@
         <v>35790</v>
       </c>
       <c r="I222" t="n">
-        <v>160296</v>
+        <v>160295</v>
       </c>
       <c r="J222" t="n">
         <v>344401</v>
@@ -16725,7 +16725,7 @@
         <v>35841</v>
       </c>
       <c r="I223" t="n">
-        <v>162798</v>
+        <v>162797</v>
       </c>
       <c r="J223" t="n">
         <v>346560</v>
@@ -16799,7 +16799,7 @@
         <v>35887</v>
       </c>
       <c r="I224" t="n">
-        <v>164866</v>
+        <v>164865</v>
       </c>
       <c r="J224" t="n">
         <v>350793</v>
@@ -16873,7 +16873,7 @@
         <v>35920</v>
       </c>
       <c r="I225" t="n">
-        <v>167156</v>
+        <v>167155</v>
       </c>
       <c r="J225" t="n">
         <v>356967</v>
@@ -16947,7 +16947,7 @@
         <v>35950</v>
       </c>
       <c r="I226" t="n">
-        <v>169675</v>
+        <v>169674</v>
       </c>
       <c r="J226" t="n">
         <v>362848</v>
@@ -17021,7 +17021,7 @@
         <v>35982</v>
       </c>
       <c r="I227" t="n">
-        <v>172450</v>
+        <v>172449</v>
       </c>
       <c r="J227" t="n">
         <v>369340</v>
@@ -17095,7 +17095,7 @@
         <v>35997</v>
       </c>
       <c r="I228" t="n">
-        <v>174761</v>
+        <v>174760</v>
       </c>
       <c r="J228" t="n">
         <v>377072</v>
@@ -17169,7 +17169,7 @@
         <v>36013</v>
       </c>
       <c r="I229" t="n">
-        <v>176473</v>
+        <v>176472</v>
       </c>
       <c r="J229" t="n">
         <v>381198</v>
@@ -17243,7 +17243,7 @@
         <v>36042</v>
       </c>
       <c r="I230" t="n">
-        <v>177722</v>
+        <v>177721</v>
       </c>
       <c r="J230" t="n">
         <v>383644</v>
@@ -17317,7 +17317,7 @@
         <v>36105</v>
       </c>
       <c r="I231" t="n">
-        <v>181783</v>
+        <v>181782</v>
       </c>
       <c r="J231" t="n">
         <v>389031</v>
@@ -17391,7 +17391,7 @@
         <v>36146</v>
       </c>
       <c r="I232" t="n">
-        <v>184671</v>
+        <v>184670</v>
       </c>
       <c r="J232" t="n">
         <v>396991</v>
@@ -17465,7 +17465,7 @@
         <v>36185</v>
       </c>
       <c r="I233" t="n">
-        <v>187974</v>
+        <v>187973</v>
       </c>
       <c r="J233" t="n">
         <v>405093</v>
@@ -17539,7 +17539,7 @@
         <v>36214</v>
       </c>
       <c r="I234" t="n">
-        <v>190793</v>
+        <v>190792</v>
       </c>
       <c r="J234" t="n">
         <v>413314</v>
@@ -17613,7 +17613,7 @@
         <v>36231</v>
       </c>
       <c r="I235" t="n">
-        <v>193879</v>
+        <v>193878</v>
       </c>
       <c r="J235" t="n">
         <v>423040</v>
@@ -17687,7 +17687,7 @@
         <v>36247</v>
       </c>
       <c r="I236" t="n">
-        <v>195900</v>
+        <v>195899</v>
       </c>
       <c r="J236" t="n">
         <v>428327</v>
@@ -17761,7 +17761,7 @@
         <v>36335</v>
       </c>
       <c r="I237" t="n">
-        <v>198997</v>
+        <v>198996</v>
       </c>
       <c r="J237" t="n">
         <v>431356</v>
@@ -17835,7 +17835,7 @@
         <v>36415</v>
       </c>
       <c r="I238" t="n">
-        <v>201852</v>
+        <v>201851</v>
       </c>
       <c r="J238" t="n">
         <v>437765</v>
@@ -17909,7 +17909,7 @@
         <v>36454</v>
       </c>
       <c r="I239" t="n">
-        <v>206055</v>
+        <v>206054</v>
       </c>
       <c r="J239" t="n">
         <v>448513</v>
@@ -17983,7 +17983,7 @@
         <v>36498</v>
       </c>
       <c r="I240" t="n">
-        <v>209932</v>
+        <v>209931</v>
       </c>
       <c r="J240" t="n">
         <v>458331</v>
@@ -18057,7 +18057,7 @@
         <v>36537</v>
       </c>
       <c r="I241" t="n">
-        <v>213672</v>
+        <v>213671</v>
       </c>
       <c r="J241" t="n">
         <v>468028</v>
@@ -18131,7 +18131,7 @@
         <v>36565</v>
       </c>
       <c r="I242" t="n">
-        <v>217181</v>
+        <v>217180</v>
       </c>
       <c r="J242" t="n">
         <v>479052</v>
@@ -18205,7 +18205,7 @@
         <v>36595</v>
       </c>
       <c r="I243" t="n">
-        <v>219547</v>
+        <v>219546</v>
       </c>
       <c r="J243" t="n">
         <v>484575</v>
@@ -18279,7 +18279,7 @@
         <v>36677</v>
       </c>
       <c r="I244" t="n">
-        <v>222584</v>
+        <v>222583</v>
       </c>
       <c r="J244" t="n">
         <v>488489</v>
@@ -18353,7 +18353,7 @@
         <v>36767</v>
       </c>
       <c r="I245" t="n">
-        <v>225986</v>
+        <v>225985</v>
       </c>
       <c r="J245" t="n">
         <v>496880</v>
@@ -18427,7 +18427,7 @@
         <v>36850</v>
       </c>
       <c r="I246" t="n">
-        <v>229581</v>
+        <v>229580</v>
       </c>
       <c r="J246" t="n">
         <v>506971</v>
@@ -18501,7 +18501,7 @@
         <v>36905</v>
       </c>
       <c r="I247" t="n">
-        <v>233289</v>
+        <v>233288</v>
       </c>
       <c r="J247" t="n">
         <v>516488</v>
@@ -18575,7 +18575,7 @@
         <v>36978</v>
       </c>
       <c r="I248" t="n">
-        <v>237419</v>
+        <v>237418</v>
       </c>
       <c r="J248" t="n">
         <v>526618</v>
@@ -18649,7 +18649,7 @@
         <v>37025</v>
       </c>
       <c r="I249" t="n">
-        <v>241305</v>
+        <v>241304</v>
       </c>
       <c r="J249" t="n">
         <v>538653</v>
@@ -18723,7 +18723,7 @@
         <v>37050</v>
       </c>
       <c r="I250" t="n">
-        <v>244012</v>
+        <v>244011</v>
       </c>
       <c r="J250" t="n">
         <v>545306</v>
@@ -18797,7 +18797,7 @@
         <v>37141</v>
       </c>
       <c r="I251" t="n">
-        <v>246847</v>
+        <v>246846</v>
       </c>
       <c r="J251" t="n">
         <v>549674</v>
@@ -18871,7 +18871,7 @@
         <v>37270</v>
       </c>
       <c r="I252" t="n">
-        <v>249766</v>
+        <v>249765</v>
       </c>
       <c r="J252" t="n">
         <v>558042</v>
@@ -18945,7 +18945,7 @@
         <v>37350</v>
       </c>
       <c r="I253" t="n">
-        <v>253681</v>
+        <v>253680</v>
       </c>
       <c r="J253" t="n">
         <v>569343</v>
@@ -19019,7 +19019,7 @@
         <v>37424</v>
       </c>
       <c r="I254" t="n">
-        <v>257513</v>
+        <v>257512</v>
       </c>
       <c r="J254" t="n">
         <v>580470</v>
@@ -19093,7 +19093,7 @@
         <v>37517</v>
       </c>
       <c r="I255" t="n">
-        <v>261562</v>
+        <v>261561</v>
       </c>
       <c r="J255" t="n">
         <v>592282</v>
@@ -19167,7 +19167,7 @@
         <v>37557</v>
       </c>
       <c r="I256" t="n">
-        <v>264830</v>
+        <v>264829</v>
       </c>
       <c r="J256" t="n">
         <v>605107</v>
@@ -19241,7 +19241,7 @@
         <v>37593</v>
       </c>
       <c r="I257" t="n">
-        <v>267668</v>
+        <v>267667</v>
       </c>
       <c r="J257" t="n">
         <v>612490</v>
@@ -19315,7 +19315,7 @@
         <v>37731</v>
       </c>
       <c r="I258" t="n">
-        <v>271110</v>
+        <v>271109</v>
       </c>
       <c r="J258" t="n">
         <v>617869</v>
@@ -19389,7 +19389,7 @@
         <v>37893</v>
       </c>
       <c r="I259" t="n">
-        <v>274414</v>
+        <v>274413</v>
       </c>
       <c r="J259" t="n">
         <v>627232</v>
@@ -19463,7 +19463,7 @@
         <v>37998</v>
       </c>
       <c r="I260" t="n">
-        <v>278360</v>
+        <v>278359</v>
       </c>
       <c r="J260" t="n">
         <v>639701</v>
@@ -19537,7 +19537,7 @@
         <v>38110</v>
       </c>
       <c r="I261" t="n">
-        <v>282198</v>
+        <v>282197</v>
       </c>
       <c r="J261" t="n">
         <v>651612</v>
@@ -19611,7 +19611,7 @@
         <v>38230</v>
       </c>
       <c r="I262" t="n">
-        <v>286730</v>
+        <v>286729</v>
       </c>
       <c r="J262" t="n">
         <v>664099</v>
@@ -19685,7 +19685,7 @@
         <v>38280</v>
       </c>
       <c r="I263" t="n">
-        <v>291299</v>
+        <v>291298</v>
       </c>
       <c r="J263" t="n">
         <v>668581</v>
@@ -19759,7 +19759,7 @@
         <v>38322</v>
       </c>
       <c r="I264" t="n">
-        <v>294369</v>
+        <v>294368</v>
       </c>
       <c r="J264" t="n">
         <v>676033</v>
@@ -19833,7 +19833,7 @@
         <v>38487</v>
       </c>
       <c r="I265" t="n">
-        <v>297387</v>
+        <v>297386</v>
       </c>
       <c r="J265" t="n">
         <v>680869</v>
@@ -19907,7 +19907,7 @@
         <v>38701</v>
       </c>
       <c r="I266" t="n">
-        <v>301057</v>
+        <v>301056</v>
       </c>
       <c r="J266" t="n">
         <v>690487</v>
@@ -19981,7 +19981,7 @@
         <v>38829</v>
       </c>
       <c r="I267" t="n">
-        <v>305379</v>
+        <v>305378</v>
       </c>
       <c r="J267" t="n">
         <v>702488</v>
@@ -20055,7 +20055,7 @@
         <v>38946</v>
       </c>
       <c r="I268" t="n">
-        <v>309553</v>
+        <v>309552</v>
       </c>
       <c r="J268" t="n">
         <v>714067</v>
@@ -20129,7 +20129,7 @@
         <v>39058</v>
       </c>
       <c r="I269" t="n">
-        <v>313135</v>
+        <v>313134</v>
       </c>
       <c r="J269" t="n">
         <v>725424</v>
@@ -20203,7 +20203,7 @@
         <v>39131</v>
       </c>
       <c r="I270" t="n">
-        <v>317033</v>
+        <v>317032</v>
       </c>
       <c r="J270" t="n">
         <v>738328</v>
@@ -20277,7 +20277,7 @@
         <v>39185</v>
       </c>
       <c r="I271" t="n">
-        <v>320034</v>
+        <v>320033</v>
       </c>
       <c r="J271" t="n">
         <v>745269</v>
@@ -20351,7 +20351,7 @@
         <v>39451</v>
       </c>
       <c r="I272" t="n">
-        <v>323503</v>
+        <v>323502</v>
       </c>
       <c r="J272" t="n">
         <v>749739</v>
@@ -20425,7 +20425,7 @@
         <v>39586</v>
       </c>
       <c r="I273" t="n">
-        <v>326793</v>
+        <v>326792</v>
       </c>
       <c r="J273" t="n">
         <v>758068</v>
@@ -20499,7 +20499,7 @@
         <v>39733</v>
       </c>
       <c r="I274" t="n">
-        <v>330651</v>
+        <v>330650</v>
       </c>
       <c r="J274" t="n">
         <v>768892</v>
@@ -20573,7 +20573,7 @@
         <v>39881</v>
       </c>
       <c r="I275" t="n">
-        <v>334448</v>
+        <v>334447</v>
       </c>
       <c r="J275" t="n">
         <v>778438</v>
@@ -20647,7 +20647,7 @@
         <v>40022</v>
       </c>
       <c r="I276" t="n">
-        <v>338357</v>
+        <v>338356</v>
       </c>
       <c r="J276" t="n">
         <v>788418</v>
@@ -20721,7 +20721,7 @@
         <v>40104</v>
       </c>
       <c r="I277" t="n">
-        <v>342765</v>
+        <v>342764</v>
       </c>
       <c r="J277" t="n">
         <v>799693</v>
@@ -20795,7 +20795,7 @@
         <v>40151</v>
       </c>
       <c r="I278" t="n">
-        <v>345854</v>
+        <v>345853</v>
       </c>
       <c r="J278" t="n">
         <v>804657</v>
@@ -20869,7 +20869,7 @@
         <v>40353</v>
       </c>
       <c r="I279" t="n">
-        <v>348436</v>
+        <v>348435</v>
       </c>
       <c r="J279" t="n">
         <v>807991</v>
@@ -20943,7 +20943,7 @@
         <v>40499</v>
       </c>
       <c r="I280" t="n">
-        <v>351671</v>
+        <v>351670</v>
       </c>
       <c r="J280" t="n">
         <v>815858</v>
@@ -20999,7 +20999,7 @@
         <v>1546</v>
       </c>
       <c r="C281" t="n">
-        <v>4480</v>
+        <v>4481</v>
       </c>
       <c r="D281" t="n">
         <v>69901</v>
@@ -21020,34 +21020,34 @@
         <v>356151</v>
       </c>
       <c r="J281" t="n">
-        <v>824572</v>
+        <v>824573</v>
       </c>
       <c r="K281" t="n">
         <v>132359</v>
       </c>
       <c r="L281" t="n">
-        <v>50772</v>
+        <v>50773</v>
       </c>
       <c r="M281" t="n">
-        <v>25500</v>
+        <v>25501</v>
       </c>
       <c r="N281" t="n">
-        <v>122084</v>
+        <v>122085</v>
       </c>
       <c r="O281" t="n">
-        <v>55680</v>
+        <v>55681</v>
       </c>
       <c r="P281" t="n">
-        <v>4480</v>
+        <v>4481</v>
       </c>
       <c r="Q281" t="n">
-        <v>3642.9</v>
+        <v>3643</v>
       </c>
       <c r="R281" t="n">
-        <v>8714</v>
+        <v>8715</v>
       </c>
       <c r="S281" t="n">
-        <v>7954.3</v>
+        <v>7954.4</v>
       </c>
       <c r="T281" t="n">
         <v>166</v>
@@ -21094,34 +21094,34 @@
         <v>363757</v>
       </c>
       <c r="J282" t="n">
-        <v>833915</v>
+        <v>833916</v>
       </c>
       <c r="K282" t="n">
         <v>163200</v>
       </c>
       <c r="L282" t="n">
-        <v>54204</v>
+        <v>54205</v>
       </c>
       <c r="M282" t="n">
-        <v>29309</v>
+        <v>29310</v>
       </c>
       <c r="N282" t="n">
-        <v>119848</v>
+        <v>119849</v>
       </c>
       <c r="O282" t="n">
-        <v>55477</v>
+        <v>55478</v>
       </c>
       <c r="P282" t="n">
         <v>7606</v>
       </c>
       <c r="Q282" t="n">
-        <v>4187</v>
+        <v>4187.1</v>
       </c>
       <c r="R282" t="n">
         <v>9343</v>
       </c>
       <c r="S282" t="n">
-        <v>7925.3</v>
+        <v>7925.4</v>
       </c>
       <c r="T282" t="n">
         <v>109</v>
@@ -21168,34 +21168,34 @@
         <v>369311</v>
       </c>
       <c r="J283" t="n">
-        <v>843596</v>
+        <v>843597</v>
       </c>
       <c r="K283" t="n">
         <v>136604</v>
       </c>
       <c r="L283" t="n">
-        <v>56176</v>
+        <v>56177</v>
       </c>
       <c r="M283" t="n">
-        <v>30954</v>
+        <v>30955</v>
       </c>
       <c r="N283" t="n">
-        <v>118172</v>
+        <v>118173</v>
       </c>
       <c r="O283" t="n">
-        <v>55178</v>
+        <v>55179</v>
       </c>
       <c r="P283" t="n">
         <v>5554</v>
       </c>
       <c r="Q283" t="n">
-        <v>4422</v>
+        <v>4422.1</v>
       </c>
       <c r="R283" t="n">
         <v>9681</v>
       </c>
       <c r="S283" t="n">
-        <v>7882.6</v>
+        <v>7882.7</v>
       </c>
       <c r="T283" t="n">
         <v>128</v>
@@ -21221,7 +21221,7 @@
         <v>1991</v>
       </c>
       <c r="C284" t="n">
-        <v>6238</v>
+        <v>6242</v>
       </c>
       <c r="D284" t="n">
         <v>70337</v>
@@ -21239,37 +21239,37 @@
         <v>40994</v>
       </c>
       <c r="I284" t="n">
-        <v>375511</v>
+        <v>375515</v>
       </c>
       <c r="J284" t="n">
-        <v>789473</v>
+        <v>789478</v>
       </c>
       <c r="K284" t="n">
         <v>123923</v>
       </c>
       <c r="L284" t="n">
-        <v>58478</v>
+        <v>58483</v>
       </c>
       <c r="M284" t="n">
-        <v>32746</v>
+        <v>32751</v>
       </c>
       <c r="N284" t="n">
-        <v>51145</v>
+        <v>51150</v>
       </c>
       <c r="O284" t="n">
-        <v>-10220</v>
+        <v>-10215</v>
       </c>
       <c r="P284" t="n">
-        <v>6200</v>
+        <v>6204</v>
       </c>
       <c r="Q284" t="n">
-        <v>4678</v>
+        <v>4678.7</v>
       </c>
       <c r="R284" t="n">
-        <v>-54123</v>
+        <v>-54119</v>
       </c>
       <c r="S284" t="n">
-        <v>-1460</v>
+        <v>-1459.3</v>
       </c>
       <c r="T284" t="n">
         <v>92</v>
@@ -21313,37 +21313,37 @@
         <v>41070</v>
       </c>
       <c r="I285" t="n">
-        <v>379501</v>
+        <v>379505</v>
       </c>
       <c r="J285" t="n">
-        <v>794460</v>
+        <v>794465</v>
       </c>
       <c r="K285" t="n">
         <v>77366</v>
       </c>
       <c r="L285" t="n">
-        <v>59467</v>
+        <v>59472</v>
       </c>
       <c r="M285" t="n">
-        <v>33647</v>
+        <v>33652</v>
       </c>
       <c r="N285" t="n">
-        <v>49191</v>
+        <v>49196</v>
       </c>
       <c r="O285" t="n">
-        <v>-10197</v>
+        <v>-10192</v>
       </c>
       <c r="P285" t="n">
         <v>3990</v>
       </c>
       <c r="Q285" t="n">
-        <v>4806.7</v>
+        <v>4807.4</v>
       </c>
       <c r="R285" t="n">
         <v>4987</v>
       </c>
       <c r="S285" t="n">
-        <v>-1456.7</v>
+        <v>-1456</v>
       </c>
       <c r="T285" t="n">
         <v>76</v>
@@ -21387,37 +21387,37 @@
         <v>41174</v>
       </c>
       <c r="I286" t="n">
-        <v>382750</v>
+        <v>382754</v>
       </c>
       <c r="J286" t="n">
-        <v>799035</v>
+        <v>799040</v>
       </c>
       <c r="K286" t="n">
         <v>77950</v>
       </c>
       <c r="L286" t="n">
-        <v>59247</v>
+        <v>59252</v>
       </c>
       <c r="M286" t="n">
-        <v>34314</v>
+        <v>34319</v>
       </c>
       <c r="N286" t="n">
-        <v>49296</v>
+        <v>49301</v>
       </c>
       <c r="O286" t="n">
-        <v>-8956</v>
+        <v>-8951</v>
       </c>
       <c r="P286" t="n">
         <v>3249</v>
       </c>
       <c r="Q286" t="n">
-        <v>4902</v>
+        <v>4902.7</v>
       </c>
       <c r="R286" t="n">
         <v>4575</v>
       </c>
       <c r="S286" t="n">
-        <v>-1279.4</v>
+        <v>-1278.7</v>
       </c>
       <c r="T286" t="n">
         <v>104</v>
@@ -21461,37 +21461,37 @@
         <v>41379</v>
       </c>
       <c r="I287" t="n">
-        <v>386222</v>
+        <v>386226</v>
       </c>
       <c r="J287" t="n">
-        <v>804851</v>
+        <v>804856</v>
       </c>
       <c r="K287" t="n">
         <v>142144</v>
       </c>
       <c r="L287" t="n">
-        <v>59429</v>
+        <v>59434</v>
       </c>
       <c r="M287" t="n">
-        <v>34551</v>
+        <v>34556</v>
       </c>
       <c r="N287" t="n">
-        <v>46783</v>
+        <v>46788</v>
       </c>
       <c r="O287" t="n">
-        <v>-11007</v>
+        <v>-11002</v>
       </c>
       <c r="P287" t="n">
         <v>3472</v>
       </c>
       <c r="Q287" t="n">
-        <v>4935.9</v>
+        <v>4936.6</v>
       </c>
       <c r="R287" t="n">
         <v>5816</v>
       </c>
       <c r="S287" t="n">
-        <v>-1572.4</v>
+        <v>-1571.7</v>
       </c>
       <c r="T287" t="n">
         <v>205</v>
@@ -21535,37 +21535,37 @@
         <v>41572</v>
       </c>
       <c r="I288" t="n">
-        <v>391314</v>
+        <v>391318</v>
       </c>
       <c r="J288" t="n">
-        <v>815236</v>
+        <v>815241</v>
       </c>
       <c r="K288" t="n">
         <v>143911</v>
       </c>
       <c r="L288" t="n">
-        <v>60663</v>
+        <v>60668</v>
       </c>
       <c r="M288" t="n">
-        <v>35163</v>
+        <v>35167</v>
       </c>
       <c r="N288" t="n">
-        <v>46344</v>
+        <v>46349</v>
       </c>
       <c r="O288" t="n">
-        <v>-9336</v>
+        <v>-9332</v>
       </c>
       <c r="P288" t="n">
         <v>5092</v>
       </c>
       <c r="Q288" t="n">
-        <v>5023.3</v>
+        <v>5023.9</v>
       </c>
       <c r="R288" t="n">
         <v>10385</v>
       </c>
       <c r="S288" t="n">
-        <v>-1333.7</v>
+        <v>-1333.1</v>
       </c>
       <c r="T288" t="n">
         <v>193</v>
@@ -21609,37 +21609,37 @@
         <v>41705</v>
       </c>
       <c r="I289" t="n">
-        <v>358832</v>
+        <v>358836</v>
       </c>
       <c r="J289" t="n">
-        <v>826592</v>
+        <v>826597</v>
       </c>
       <c r="K289" t="n">
         <v>145437</v>
       </c>
       <c r="L289" t="n">
-        <v>24384</v>
+        <v>24389</v>
       </c>
       <c r="M289" t="n">
-        <v>-4925</v>
+        <v>-4921</v>
       </c>
       <c r="N289" t="n">
-        <v>48154</v>
+        <v>48159</v>
       </c>
       <c r="O289" t="n">
-        <v>-7323</v>
+        <v>-7319</v>
       </c>
       <c r="P289" t="n">
         <v>-32482</v>
       </c>
       <c r="Q289" t="n">
-        <v>-703.6</v>
+        <v>-703</v>
       </c>
       <c r="R289" t="n">
         <v>11356</v>
       </c>
       <c r="S289" t="n">
-        <v>-1046.1</v>
+        <v>-1045.6</v>
       </c>
       <c r="T289" t="n">
         <v>133</v>
@@ -21683,37 +21683,37 @@
         <v>41845</v>
       </c>
       <c r="I290" t="n">
-        <v>366022</v>
+        <v>366026</v>
       </c>
       <c r="J290" t="n">
-        <v>838781</v>
+        <v>838786</v>
       </c>
       <c r="K290" t="n">
         <v>147892</v>
       </c>
       <c r="L290" t="n">
-        <v>27665</v>
+        <v>27670</v>
       </c>
       <c r="M290" t="n">
-        <v>-3289</v>
+        <v>-3285</v>
       </c>
       <c r="N290" t="n">
-        <v>50363</v>
+        <v>50368</v>
       </c>
       <c r="O290" t="n">
-        <v>-4815</v>
+        <v>-4811</v>
       </c>
       <c r="P290" t="n">
         <v>7190</v>
       </c>
       <c r="Q290" t="n">
-        <v>-469.9</v>
+        <v>-469.3</v>
       </c>
       <c r="R290" t="n">
         <v>12189</v>
       </c>
       <c r="S290" t="n">
-        <v>-687.9</v>
+        <v>-687.3</v>
       </c>
       <c r="T290" t="n">
         <v>140</v>
@@ -21757,22 +21757,22 @@
         <v>41964</v>
       </c>
       <c r="I291" t="n">
-        <v>374468</v>
+        <v>374472</v>
       </c>
       <c r="J291" t="n">
-        <v>851803</v>
+        <v>851808</v>
       </c>
       <c r="K291" t="n">
         <v>134525</v>
       </c>
       <c r="L291" t="n">
-        <v>31703</v>
+        <v>31708</v>
       </c>
       <c r="M291" t="n">
         <v>-1043</v>
       </c>
       <c r="N291" t="n">
-        <v>52110</v>
+        <v>52115</v>
       </c>
       <c r="O291" t="n">
         <v>62330</v>
@@ -21813,7 +21813,7 @@
         <v>3523</v>
       </c>
       <c r="C292" t="n">
-        <v>4143</v>
+        <v>4142</v>
       </c>
       <c r="D292" t="n">
         <v>71067</v>
@@ -21831,37 +21831,37 @@
         <v>42057</v>
       </c>
       <c r="I292" t="n">
-        <v>429841</v>
+        <v>429844</v>
       </c>
       <c r="J292" t="n">
-        <v>858721</v>
+        <v>858725</v>
       </c>
       <c r="K292" t="n">
         <v>85296</v>
       </c>
       <c r="L292" t="n">
-        <v>83987</v>
+        <v>83991</v>
       </c>
       <c r="M292" t="n">
-        <v>50340</v>
+        <v>50339</v>
       </c>
       <c r="N292" t="n">
-        <v>54064</v>
+        <v>54068</v>
       </c>
       <c r="O292" t="n">
-        <v>64261</v>
+        <v>64260</v>
       </c>
       <c r="P292" t="n">
-        <v>55373</v>
+        <v>55372</v>
       </c>
       <c r="Q292" t="n">
-        <v>7191.4</v>
+        <v>7191.3</v>
       </c>
       <c r="R292" t="n">
-        <v>6918</v>
+        <v>6917</v>
       </c>
       <c r="S292" t="n">
-        <v>9180.1</v>
+        <v>9180</v>
       </c>
       <c r="T292" t="n">
         <v>93</v>
@@ -21905,37 +21905,37 @@
         <v>42279</v>
       </c>
       <c r="I293" t="n">
-        <v>434756</v>
+        <v>434759</v>
       </c>
       <c r="J293" t="n">
-        <v>865225</v>
+        <v>865229</v>
       </c>
       <c r="K293" t="n">
         <v>88553</v>
       </c>
       <c r="L293" t="n">
-        <v>86320</v>
+        <v>86324</v>
       </c>
       <c r="M293" t="n">
-        <v>52006</v>
+        <v>52005</v>
       </c>
       <c r="N293" t="n">
-        <v>57234</v>
+        <v>57238</v>
       </c>
       <c r="O293" t="n">
-        <v>66190</v>
+        <v>66189</v>
       </c>
       <c r="P293" t="n">
         <v>4915</v>
       </c>
       <c r="Q293" t="n">
-        <v>7429.4</v>
+        <v>7429.3</v>
       </c>
       <c r="R293" t="n">
         <v>6504</v>
       </c>
       <c r="S293" t="n">
-        <v>9455.7</v>
+        <v>9455.6</v>
       </c>
       <c r="T293" t="n">
         <v>222</v>
@@ -21979,37 +21979,37 @@
         <v>42447</v>
       </c>
       <c r="I294" t="n">
-        <v>442150</v>
+        <v>442153</v>
       </c>
       <c r="J294" t="n">
-        <v>877680</v>
+        <v>877684</v>
       </c>
       <c r="K294" t="n">
         <v>154543</v>
       </c>
       <c r="L294" t="n">
-        <v>90479</v>
+        <v>90483</v>
       </c>
       <c r="M294" t="n">
-        <v>55928</v>
+        <v>55927</v>
       </c>
       <c r="N294" t="n">
-        <v>61822</v>
+        <v>61826</v>
       </c>
       <c r="O294" t="n">
-        <v>72829</v>
+        <v>72828</v>
       </c>
       <c r="P294" t="n">
         <v>7394</v>
       </c>
       <c r="Q294" t="n">
-        <v>7989.7</v>
+        <v>7989.6</v>
       </c>
       <c r="R294" t="n">
         <v>12455</v>
       </c>
       <c r="S294" t="n">
-        <v>10404.1</v>
+        <v>10404</v>
       </c>
       <c r="T294" t="n">
         <v>168</v>
@@ -22053,37 +22053,37 @@
         <v>42640</v>
       </c>
       <c r="I295" t="n">
-        <v>499148</v>
+        <v>499151</v>
       </c>
       <c r="J295" t="n">
-        <v>890310</v>
+        <v>890314</v>
       </c>
       <c r="K295" t="n">
         <v>156839</v>
       </c>
       <c r="L295" t="n">
-        <v>142997</v>
+        <v>143000</v>
       </c>
       <c r="M295" t="n">
-        <v>107834</v>
+        <v>107833</v>
       </c>
       <c r="N295" t="n">
-        <v>65738</v>
+        <v>65741</v>
       </c>
       <c r="O295" t="n">
-        <v>75074</v>
+        <v>75073</v>
       </c>
       <c r="P295" t="n">
         <v>56998</v>
       </c>
       <c r="Q295" t="n">
-        <v>15404.9</v>
+        <v>15404.7</v>
       </c>
       <c r="R295" t="n">
         <v>12630</v>
       </c>
       <c r="S295" t="n">
-        <v>10724.9</v>
+        <v>10724.7</v>
       </c>
       <c r="T295" t="n">
         <v>193</v>
@@ -22127,37 +22127,37 @@
         <v>42791</v>
       </c>
       <c r="I296" t="n">
-        <v>508613</v>
+        <v>508616</v>
       </c>
       <c r="J296" t="n">
-        <v>904385</v>
+        <v>904389</v>
       </c>
       <c r="K296" t="n">
         <v>148998</v>
       </c>
       <c r="L296" t="n">
-        <v>144856</v>
+        <v>144859</v>
       </c>
       <c r="M296" t="n">
-        <v>149781</v>
+        <v>149780</v>
       </c>
       <c r="N296" t="n">
-        <v>70470</v>
+        <v>70473</v>
       </c>
       <c r="O296" t="n">
-        <v>77793</v>
+        <v>77792</v>
       </c>
       <c r="P296" t="n">
         <v>9465</v>
       </c>
       <c r="Q296" t="n">
-        <v>21397.3</v>
+        <v>21397.1</v>
       </c>
       <c r="R296" t="n">
         <v>14075</v>
       </c>
       <c r="S296" t="n">
-        <v>11113.3</v>
+        <v>11113.1</v>
       </c>
       <c r="T296" t="n">
         <v>151</v>
@@ -22201,37 +22201,37 @@
         <v>43012</v>
       </c>
       <c r="I297" t="n">
-        <v>581700</v>
+        <v>581703</v>
       </c>
       <c r="J297" t="n">
-        <v>917439</v>
+        <v>917443</v>
       </c>
       <c r="K297" t="n">
         <v>161976</v>
       </c>
       <c r="L297" t="n">
-        <v>212389</v>
+        <v>212392</v>
       </c>
       <c r="M297" t="n">
-        <v>215678</v>
+        <v>215677</v>
       </c>
       <c r="N297" t="n">
-        <v>73843</v>
+        <v>73846</v>
       </c>
       <c r="O297" t="n">
-        <v>78658</v>
+        <v>78657</v>
       </c>
       <c r="P297" t="n">
         <v>73087</v>
       </c>
       <c r="Q297" t="n">
-        <v>30811.1</v>
+        <v>30811</v>
       </c>
       <c r="R297" t="n">
         <v>13054</v>
       </c>
       <c r="S297" t="n">
-        <v>11236.9</v>
+        <v>11236.7</v>
       </c>
       <c r="T297" t="n">
         <v>221</v>
@@ -22275,37 +22275,37 @@
         <v>43177</v>
       </c>
       <c r="I298" t="n">
-        <v>596933</v>
+        <v>596936</v>
       </c>
       <c r="J298" t="n">
-        <v>882305</v>
+        <v>882309</v>
       </c>
       <c r="K298" t="n">
         <v>147923</v>
       </c>
       <c r="L298" t="n">
-        <v>221422</v>
+        <v>221421</v>
       </c>
       <c r="M298" t="n">
-        <v>222465</v>
+        <v>222464</v>
       </c>
       <c r="N298" t="n">
-        <v>92832</v>
+        <v>92831</v>
       </c>
       <c r="O298" t="n">
-        <v>30502</v>
+        <v>30501</v>
       </c>
       <c r="P298" t="n">
         <v>15233</v>
       </c>
       <c r="Q298" t="n">
-        <v>31780.7</v>
+        <v>31780.6</v>
       </c>
       <c r="R298" t="n">
         <v>-35134</v>
       </c>
       <c r="S298" t="n">
-        <v>4357.4</v>
+        <v>4357.3</v>
       </c>
       <c r="T298" t="n">
         <v>165</v>
@@ -22349,22 +22349,22 @@
         <v>43287</v>
       </c>
       <c r="I299" t="n">
-        <v>608264</v>
+        <v>608267</v>
       </c>
       <c r="J299" t="n">
-        <v>889650</v>
+        <v>889654</v>
       </c>
       <c r="K299" t="n">
         <v>94944</v>
       </c>
       <c r="L299" t="n">
-        <v>228763</v>
+        <v>228762</v>
       </c>
       <c r="M299" t="n">
         <v>178423</v>
       </c>
       <c r="N299" t="n">
-        <v>95190</v>
+        <v>95189</v>
       </c>
       <c r="O299" t="n">
         <v>30929</v>
@@ -22423,22 +22423,22 @@
         <v>43565</v>
       </c>
       <c r="I300" t="n">
-        <v>617143</v>
+        <v>617146</v>
       </c>
       <c r="J300" t="n">
-        <v>896825</v>
+        <v>896829</v>
       </c>
       <c r="K300" t="n">
         <v>112307</v>
       </c>
       <c r="L300" t="n">
-        <v>234393</v>
+        <v>234392</v>
       </c>
       <c r="M300" t="n">
         <v>182387</v>
       </c>
       <c r="N300" t="n">
-        <v>97790</v>
+        <v>97789</v>
       </c>
       <c r="O300" t="n">
         <v>31600</v>
@@ -22497,22 +22497,22 @@
         <v>43793</v>
       </c>
       <c r="I301" t="n">
-        <v>628939</v>
+        <v>628942</v>
       </c>
       <c r="J301" t="n">
-        <v>865188</v>
+        <v>865192</v>
       </c>
       <c r="K301" t="n">
         <v>154374</v>
       </c>
       <c r="L301" t="n">
-        <v>242717</v>
+        <v>242716</v>
       </c>
       <c r="M301" t="n">
         <v>186789</v>
       </c>
       <c r="N301" t="n">
-        <v>60337</v>
+        <v>60336</v>
       </c>
       <c r="O301" t="n">
         <v>-12492</v>
@@ -22571,22 +22571,22 @@
         <v>44031</v>
       </c>
       <c r="I302" t="n">
-        <v>643333</v>
+        <v>643336</v>
       </c>
       <c r="J302" t="n">
-        <v>877885</v>
+        <v>877889</v>
       </c>
       <c r="K302" t="n">
         <v>171541</v>
       </c>
       <c r="L302" t="n">
-        <v>252019</v>
+        <v>252018</v>
       </c>
       <c r="M302" t="n">
         <v>144185</v>
       </c>
       <c r="N302" t="n">
-        <v>62649</v>
+        <v>62648</v>
       </c>
       <c r="O302" t="n">
         <v>-12425</v>
@@ -22645,22 +22645,22 @@
         <v>44243</v>
       </c>
       <c r="I303" t="n">
-        <v>656919</v>
+        <v>656922</v>
       </c>
       <c r="J303" t="n">
-        <v>834875</v>
+        <v>834879</v>
       </c>
       <c r="K303" t="n">
         <v>210391</v>
       </c>
       <c r="L303" t="n">
-        <v>298087</v>
+        <v>298086</v>
       </c>
       <c r="M303" t="n">
         <v>148306</v>
       </c>
       <c r="N303" t="n">
-        <v>8283</v>
+        <v>8282</v>
       </c>
       <c r="O303" t="n">
         <v>-69510</v>
@@ -22719,22 +22719,22 @@
         <v>44486</v>
       </c>
       <c r="I304" t="n">
-        <v>673050</v>
+        <v>673053</v>
       </c>
       <c r="J304" t="n">
-        <v>847675</v>
+        <v>847679</v>
       </c>
       <c r="K304" t="n">
         <v>163222</v>
       </c>
       <c r="L304" t="n">
-        <v>307028</v>
+        <v>307027</v>
       </c>
       <c r="M304" t="n">
         <v>91350</v>
       </c>
       <c r="N304" t="n">
-        <v>8894</v>
+        <v>8893</v>
       </c>
       <c r="O304" t="n">
         <v>-69764</v>
@@ -22793,22 +22793,22 @@
         <v>44735</v>
       </c>
       <c r="I305" t="n">
-        <v>689897</v>
+        <v>689900</v>
       </c>
       <c r="J305" t="n">
-        <v>861335</v>
+        <v>861339</v>
       </c>
       <c r="K305" t="n">
         <v>164037</v>
       </c>
       <c r="L305" t="n">
-        <v>315429</v>
+        <v>315428</v>
       </c>
       <c r="M305" t="n">
         <v>92964</v>
       </c>
       <c r="N305" t="n">
-        <v>9532</v>
+        <v>9531</v>
       </c>
       <c r="O305" t="n">
         <v>-20970</v>
@@ -22867,10 +22867,10 @@
         <v>44971</v>
       </c>
       <c r="I306" t="n">
-        <v>703421</v>
+        <v>703424</v>
       </c>
       <c r="J306" t="n">
-        <v>869425</v>
+        <v>869429</v>
       </c>
       <c r="K306" t="n">
         <v>108164</v>
@@ -22941,10 +22941,10 @@
         <v>45252</v>
       </c>
       <c r="I307" t="n">
-        <v>713656</v>
+        <v>713659</v>
       </c>
       <c r="J307" t="n">
-        <v>877026</v>
+        <v>877030</v>
       </c>
       <c r="K307" t="n">
         <v>112065</v>
@@ -23015,10 +23015,10 @@
         <v>45537</v>
       </c>
       <c r="I308" t="n">
-        <v>726973</v>
+        <v>726976</v>
       </c>
       <c r="J308" t="n">
-        <v>886298</v>
+        <v>886302</v>
       </c>
       <c r="K308" t="n">
         <v>190101</v>
@@ -23089,10 +23089,10 @@
         <v>45842</v>
       </c>
       <c r="I309" t="n">
-        <v>742384</v>
+        <v>742387</v>
       </c>
       <c r="J309" t="n">
-        <v>897648</v>
+        <v>897652</v>
       </c>
       <c r="K309" t="n">
         <v>180262</v>
@@ -23163,10 +23163,10 @@
         <v>46164</v>
       </c>
       <c r="I310" t="n">
-        <v>755753</v>
+        <v>755756</v>
       </c>
       <c r="J310" t="n">
-        <v>909726</v>
+        <v>909730</v>
       </c>
       <c r="K310" t="n">
         <v>236358</v>
@@ -23237,10 +23237,10 @@
         <v>46501</v>
       </c>
       <c r="I311" t="n">
-        <v>769845</v>
+        <v>769848</v>
       </c>
       <c r="J311" t="n">
-        <v>921284</v>
+        <v>921288</v>
       </c>
       <c r="K311" t="n">
         <v>201952</v>
@@ -23311,10 +23311,10 @@
         <v>46786</v>
       </c>
       <c r="I312" t="n">
-        <v>784382</v>
+        <v>784385</v>
       </c>
       <c r="J312" t="n">
-        <v>932490</v>
+        <v>932494</v>
       </c>
       <c r="K312" t="n">
         <v>187772</v>
@@ -23385,10 +23385,10 @@
         <v>47036</v>
       </c>
       <c r="I313" t="n">
-        <v>797265</v>
+        <v>797268</v>
       </c>
       <c r="J313" t="n">
-        <v>939452</v>
+        <v>939456</v>
       </c>
       <c r="K313" t="n">
         <v>125410</v>
@@ -23459,10 +23459,10 @@
         <v>47389</v>
       </c>
       <c r="I314" t="n">
-        <v>805000</v>
+        <v>805003</v>
       </c>
       <c r="J314" t="n">
-        <v>945984</v>
+        <v>945988</v>
       </c>
       <c r="K314" t="n">
         <v>145156</v>
@@ -23533,10 +23533,10 @@
         <v>47673</v>
       </c>
       <c r="I315" t="n">
-        <v>816440</v>
+        <v>816443</v>
       </c>
       <c r="J315" t="n">
-        <v>954122</v>
+        <v>954126</v>
       </c>
       <c r="K315" t="n">
         <v>216037</v>
@@ -23607,10 +23607,10 @@
         <v>48069</v>
       </c>
       <c r="I316" t="n">
-        <v>829517</v>
+        <v>829520</v>
       </c>
       <c r="J316" t="n">
-        <v>964319</v>
+        <v>964323</v>
       </c>
       <c r="K316" t="n">
         <v>220703</v>
@@ -23681,10 +23681,10 @@
         <v>48387</v>
       </c>
       <c r="I317" t="n">
-        <v>841853</v>
+        <v>841856</v>
       </c>
       <c r="J317" t="n">
-        <v>974112</v>
+        <v>974116</v>
       </c>
       <c r="K317" t="n">
         <v>272009</v>
@@ -23755,10 +23755,10 @@
         <v>48693</v>
       </c>
       <c r="I318" t="n">
-        <v>855266</v>
+        <v>855269</v>
       </c>
       <c r="J318" t="n">
-        <v>982747</v>
+        <v>982751</v>
       </c>
       <c r="K318" t="n">
         <v>228971</v>
@@ -23829,10 +23829,10 @@
         <v>49001</v>
       </c>
       <c r="I319" t="n">
-        <v>868071</v>
+        <v>868074</v>
       </c>
       <c r="J319" t="n">
-        <v>990614</v>
+        <v>990618</v>
       </c>
       <c r="K319" t="n">
         <v>217812</v>
@@ -23903,10 +23903,10 @@
         <v>49200</v>
       </c>
       <c r="I320" t="n">
-        <v>877613</v>
+        <v>877616</v>
       </c>
       <c r="J320" t="n">
-        <v>996065</v>
+        <v>996069</v>
       </c>
       <c r="K320" t="n">
         <v>148078</v>
@@ -23959,7 +23959,7 @@
         <v>2533</v>
       </c>
       <c r="C321" t="n">
-        <v>3818</v>
+        <v>3819</v>
       </c>
       <c r="D321" t="n">
         <v>197302</v>
@@ -23977,37 +23977,37 @@
         <v>49585</v>
       </c>
       <c r="I321" t="n">
-        <v>883780</v>
+        <v>883784</v>
       </c>
       <c r="J321" t="n">
-        <v>1001489</v>
+        <v>1001494</v>
       </c>
       <c r="K321" t="n">
         <v>171000</v>
       </c>
       <c r="L321" t="n">
-        <v>170124</v>
+        <v>170125</v>
       </c>
       <c r="M321" t="n">
-        <v>78780</v>
+        <v>78781</v>
       </c>
       <c r="N321" t="n">
-        <v>124463</v>
+        <v>124464</v>
       </c>
       <c r="O321" t="n">
-        <v>55505</v>
+        <v>55506</v>
       </c>
       <c r="P321" t="n">
-        <v>6167</v>
+        <v>6168</v>
       </c>
       <c r="Q321" t="n">
-        <v>11254.3</v>
+        <v>11254.4</v>
       </c>
       <c r="R321" t="n">
-        <v>5424</v>
+        <v>5425</v>
       </c>
       <c r="S321" t="n">
-        <v>7929.3</v>
+        <v>7929.4</v>
       </c>
       <c r="T321" t="n">
         <v>385</v>
@@ -24051,37 +24051,37 @@
         <v>49849</v>
       </c>
       <c r="I322" t="n">
-        <v>892758</v>
+        <v>892762</v>
       </c>
       <c r="J322" t="n">
-        <v>1008668</v>
+        <v>1008673</v>
       </c>
       <c r="K322" t="n">
         <v>250897</v>
       </c>
       <c r="L322" t="n">
-        <v>165785</v>
+        <v>165786</v>
       </c>
       <c r="M322" t="n">
-        <v>76318</v>
+        <v>76319</v>
       </c>
       <c r="N322" t="n">
-        <v>122370</v>
+        <v>122371</v>
       </c>
       <c r="O322" t="n">
-        <v>54546</v>
+        <v>54547</v>
       </c>
       <c r="P322" t="n">
         <v>8978</v>
       </c>
       <c r="Q322" t="n">
-        <v>10902.6</v>
+        <v>10902.7</v>
       </c>
       <c r="R322" t="n">
         <v>7179</v>
       </c>
       <c r="S322" t="n">
-        <v>7792.3</v>
+        <v>7792.4</v>
       </c>
       <c r="T322" t="n">
         <v>264</v>
@@ -24107,7 +24107,7 @@
         <v>5337</v>
       </c>
       <c r="C323" t="n">
-        <v>4175</v>
+        <v>4176</v>
       </c>
       <c r="D323" t="n">
         <v>77549</v>
@@ -24125,37 +24125,37 @@
         <v>50214</v>
       </c>
       <c r="I323" t="n">
-        <v>901999</v>
+        <v>902004</v>
       </c>
       <c r="J323" t="n">
-        <v>1015744</v>
+        <v>1015750</v>
       </c>
       <c r="K323" t="n">
         <v>256196</v>
       </c>
       <c r="L323" t="n">
-        <v>159615</v>
+        <v>159617</v>
       </c>
       <c r="M323" t="n">
-        <v>72482</v>
+        <v>72484</v>
       </c>
       <c r="N323" t="n">
-        <v>118096</v>
+        <v>118098</v>
       </c>
       <c r="O323" t="n">
-        <v>51425</v>
+        <v>51427</v>
       </c>
       <c r="P323" t="n">
-        <v>9241</v>
+        <v>9242</v>
       </c>
       <c r="Q323" t="n">
-        <v>10354.6</v>
+        <v>10354.9</v>
       </c>
       <c r="R323" t="n">
-        <v>7076</v>
+        <v>7077</v>
       </c>
       <c r="S323" t="n">
-        <v>7346.4</v>
+        <v>7346.7</v>
       </c>
       <c r="T323" t="n">
         <v>365</v>
@@ -24199,37 +24199,37 @@
         <v>50549</v>
       </c>
       <c r="I324" t="n">
-        <v>912071</v>
+        <v>912076</v>
       </c>
       <c r="J324" t="n">
-        <v>1022579</v>
+        <v>1022585</v>
       </c>
       <c r="K324" t="n">
         <v>315618</v>
       </c>
       <c r="L324" t="n">
-        <v>156318</v>
+        <v>156320</v>
       </c>
       <c r="M324" t="n">
-        <v>70218</v>
+        <v>70220</v>
       </c>
       <c r="N324" t="n">
-        <v>112853</v>
+        <v>112855</v>
       </c>
       <c r="O324" t="n">
-        <v>48467</v>
+        <v>48469</v>
       </c>
       <c r="P324" t="n">
         <v>10072</v>
       </c>
       <c r="Q324" t="n">
-        <v>10031.1</v>
+        <v>10031.4</v>
       </c>
       <c r="R324" t="n">
         <v>6835</v>
       </c>
       <c r="S324" t="n">
-        <v>6923.9</v>
+        <v>6924.1</v>
       </c>
       <c r="T324" t="n">
         <v>335</v>
@@ -24255,7 +24255,7 @@
         <v>6079</v>
       </c>
       <c r="C325" t="n">
-        <v>3584</v>
+        <v>3587</v>
       </c>
       <c r="D325" t="n">
         <v>78567</v>
@@ -24273,37 +24273,37 @@
         <v>50839</v>
       </c>
       <c r="I325" t="n">
-        <v>922144</v>
+        <v>922152</v>
       </c>
       <c r="J325" t="n">
-        <v>1029351</v>
+        <v>1029360</v>
       </c>
       <c r="K325" t="n">
         <v>323180</v>
       </c>
       <c r="L325" t="n">
-        <v>152299</v>
+        <v>152304</v>
       </c>
       <c r="M325" t="n">
-        <v>66878</v>
+        <v>66883</v>
       </c>
       <c r="N325" t="n">
-        <v>108067</v>
+        <v>108072</v>
       </c>
       <c r="O325" t="n">
-        <v>46604</v>
+        <v>46609</v>
       </c>
       <c r="P325" t="n">
-        <v>10073</v>
+        <v>10076</v>
       </c>
       <c r="Q325" t="n">
-        <v>9554</v>
+        <v>9554.7</v>
       </c>
       <c r="R325" t="n">
-        <v>6772</v>
+        <v>6775</v>
       </c>
       <c r="S325" t="n">
-        <v>6657.7</v>
+        <v>6658.4</v>
       </c>
       <c r="T325" t="n">
         <v>290</v>
@@ -24329,7 +24329,7 @@
         <v>5245</v>
       </c>
       <c r="C326" t="n">
-        <v>2782</v>
+        <v>2804</v>
       </c>
       <c r="D326" t="n">
         <v>78970</v>
@@ -24338,61 +24338,61 @@
         <v>19962</v>
       </c>
       <c r="F326" t="n">
-        <v>13925</v>
+        <v>14729</v>
       </c>
       <c r="G326" t="n">
-        <v>2120</v>
+        <v>2164</v>
       </c>
       <c r="H326" t="n">
-        <v>50310</v>
+        <v>51112</v>
       </c>
       <c r="I326" t="n">
-        <v>931805</v>
+        <v>931835</v>
       </c>
       <c r="J326" t="n">
-        <v>1014194</v>
+        <v>1034861</v>
       </c>
       <c r="K326" t="n">
         <v>309034</v>
       </c>
       <c r="L326" t="n">
-        <v>147423</v>
+        <v>147450</v>
       </c>
       <c r="M326" t="n">
-        <v>63734</v>
+        <v>63761</v>
       </c>
       <c r="N326" t="n">
-        <v>81704</v>
+        <v>102367</v>
       </c>
       <c r="O326" t="n">
-        <v>23580</v>
+        <v>44243</v>
       </c>
       <c r="P326" t="n">
-        <v>9661</v>
+        <v>9683</v>
       </c>
       <c r="Q326" t="n">
-        <v>9104.9</v>
+        <v>9108.7</v>
       </c>
       <c r="R326" t="n">
-        <v>-15157</v>
+        <v>5501</v>
       </c>
       <c r="S326" t="n">
-        <v>3368.6</v>
+        <v>6320.4</v>
       </c>
       <c r="T326" t="n">
-        <v>-529</v>
+        <v>273</v>
       </c>
       <c r="U326" t="n">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="V326" t="n">
-        <v>32</v>
+        <v>299.3</v>
       </c>
       <c r="W326" t="n">
-        <v>187</v>
+        <v>301.6</v>
       </c>
       <c r="X326" t="n">
-        <v>1309</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="327">
@@ -24403,7 +24403,7 @@
         <v>4315</v>
       </c>
       <c r="C327" t="n">
-        <v>1642</v>
+        <v>1694</v>
       </c>
       <c r="D327" t="n">
         <v>78991</v>
@@ -24412,46 +24412,46 @@
         <v>18304</v>
       </c>
       <c r="F327" t="n">
-        <v>13389</v>
+        <v>14206</v>
       </c>
       <c r="G327" t="n">
-        <v>2574</v>
+        <v>2617</v>
       </c>
       <c r="H327" t="n">
-        <v>50495</v>
+        <v>51297</v>
       </c>
       <c r="I327" t="n">
-        <v>939978</v>
+        <v>940060</v>
       </c>
       <c r="J327" t="n">
-        <v>1017612</v>
+        <v>1038331</v>
       </c>
       <c r="K327" t="n">
         <v>229606</v>
       </c>
       <c r="L327" t="n">
-        <v>142713</v>
+        <v>142792</v>
       </c>
       <c r="M327" t="n">
-        <v>62365</v>
+        <v>62444</v>
       </c>
       <c r="N327" t="n">
-        <v>78160</v>
+        <v>98875</v>
       </c>
       <c r="O327" t="n">
-        <v>21547</v>
+        <v>42262</v>
       </c>
       <c r="P327" t="n">
-        <v>8173</v>
+        <v>8225</v>
       </c>
       <c r="Q327" t="n">
-        <v>8909.3</v>
+        <v>8920.6</v>
       </c>
       <c r="R327" t="n">
-        <v>3418</v>
+        <v>3470</v>
       </c>
       <c r="S327" t="n">
-        <v>3078.1</v>
+        <v>6037.4</v>
       </c>
       <c r="T327" t="n">
         <v>185</v>
@@ -24460,13 +24460,13 @@
         <v>0.4</v>
       </c>
       <c r="V327" t="n">
-        <v>-18</v>
+        <v>249.3</v>
       </c>
       <c r="W327" t="n">
-        <v>185</v>
+        <v>299.6</v>
       </c>
       <c r="X327" t="n">
-        <v>1295</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="328">
@@ -24474,73 +24474,73 @@
         <v>44157</v>
       </c>
       <c r="B328" t="n">
-        <v>1670</v>
+        <v>1771</v>
       </c>
       <c r="C328" t="n">
-        <v>862</v>
+        <v>2216</v>
       </c>
       <c r="D328" t="n">
         <v>78993</v>
       </c>
       <c r="E328" t="n">
-        <v>17577</v>
+        <v>23138</v>
       </c>
       <c r="F328" t="n">
-        <v>13280</v>
+        <v>14374</v>
       </c>
       <c r="G328" t="n">
-        <v>1658</v>
+        <v>2374</v>
       </c>
       <c r="H328" t="n">
-        <v>49726</v>
+        <v>51470</v>
       </c>
       <c r="I328" t="n">
-        <v>943950</v>
+        <v>944332</v>
       </c>
       <c r="J328" t="n">
-        <v>976936</v>
+        <v>1041467</v>
       </c>
       <c r="K328" t="n">
-        <v>234175</v>
+        <v>254889</v>
       </c>
       <c r="L328" t="n">
-        <v>138950</v>
+        <v>139329</v>
       </c>
       <c r="M328" t="n">
-        <v>60170</v>
+        <v>60548</v>
       </c>
       <c r="N328" t="n">
-        <v>30952</v>
+        <v>95479</v>
       </c>
       <c r="O328" t="n">
-        <v>-24553</v>
+        <v>39973</v>
       </c>
       <c r="P328" t="n">
-        <v>3972</v>
+        <v>4272</v>
       </c>
       <c r="Q328" t="n">
-        <v>8595.7</v>
+        <v>8649.7</v>
       </c>
       <c r="R328" t="n">
-        <v>-40676</v>
+        <v>3136</v>
       </c>
       <c r="S328" t="n">
-        <v>-3507.6</v>
+        <v>5710.4</v>
       </c>
       <c r="T328" t="n">
-        <v>-769</v>
+        <v>173</v>
       </c>
       <c r="U328" t="n">
-        <v>-1.5</v>
+        <v>0.3</v>
       </c>
       <c r="V328" t="n">
-        <v>-371</v>
+        <v>210.3</v>
       </c>
       <c r="W328" t="n">
-        <v>20.1</v>
+        <v>269.3</v>
       </c>
       <c r="X328" t="n">
-        <v>141</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="329">
@@ -24548,73 +24548,73 @@
         <v>44158</v>
       </c>
       <c r="B329" t="n">
-        <v>1265</v>
+        <v>1362</v>
       </c>
       <c r="C329" t="n">
-        <v>111</v>
+        <v>870</v>
       </c>
       <c r="D329" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E329" t="n">
-        <v>1128</v>
+        <v>5756</v>
       </c>
       <c r="F329" t="n">
-        <v>5804</v>
+        <v>14500</v>
       </c>
       <c r="G329" t="n">
-        <v>626</v>
+        <v>633</v>
       </c>
       <c r="H329" t="n">
-        <v>10702</v>
+        <v>51596</v>
       </c>
       <c r="I329" t="n">
-        <v>361447</v>
+        <v>947311</v>
       </c>
       <c r="J329" t="n">
-        <v>158888</v>
+        <v>1042885</v>
       </c>
       <c r="K329" t="n">
-        <v>206148</v>
+        <v>223717</v>
       </c>
       <c r="L329" t="n">
-        <v>-454993</v>
+        <v>130868</v>
       </c>
       <c r="M329" t="n">
-        <v>-531311</v>
+        <v>54549</v>
       </c>
       <c r="N329" t="n">
-        <v>-795234</v>
+        <v>88759</v>
       </c>
       <c r="O329" t="n">
-        <v>-849780</v>
+        <v>34212</v>
       </c>
       <c r="P329" t="n">
-        <v>-582503</v>
+        <v>2979</v>
       </c>
       <c r="Q329" t="n">
-        <v>-75901.6</v>
+        <v>7792.7</v>
       </c>
       <c r="R329" t="n">
-        <v>-818048</v>
+        <v>1418</v>
       </c>
       <c r="S329" t="n">
-        <v>-121397.1</v>
+        <v>4887.4</v>
       </c>
       <c r="T329" t="n">
-        <v>-39024</v>
+        <v>126</v>
       </c>
       <c r="U329" t="n">
-        <v>-78.5</v>
+        <v>0.2</v>
       </c>
       <c r="V329" t="n">
-        <v>-13202.7</v>
+        <v>161.3</v>
       </c>
       <c r="W329" t="n">
-        <v>-5592.4</v>
+        <v>249.6</v>
       </c>
       <c r="X329" t="n">
-        <v>-39147</v>
+        <v>1747</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualiza extremadura últimos días
</commit_message>
<xml_diff>
--- a/data/output/covid19-spain_consolidated.xlsx
+++ b/data/output/covid19-spain_consolidated.xlsx
@@ -29562,7 +29562,7 @@
         <v>44196</v>
       </c>
       <c r="B367" t="n">
-        <v>4357</v>
+        <v>4900</v>
       </c>
       <c r="C367" t="n">
         <v>4071</v>
@@ -29574,7 +29574,7 @@
         <v>6022</v>
       </c>
       <c r="F367" t="n">
-        <v>7707</v>
+        <v>7926</v>
       </c>
       <c r="G367" t="n">
         <v>0</v>
@@ -29583,58 +29583,58 @@
         <v>2352</v>
       </c>
       <c r="I367" t="n">
-        <v>1030</v>
+        <v>1058</v>
       </c>
       <c r="J367" t="n">
-        <v>52252</v>
+        <v>53324</v>
       </c>
       <c r="K367" t="n">
-        <v>1694385</v>
+        <v>1732186</v>
       </c>
       <c r="L367" t="n">
-        <v>975467</v>
+        <v>1013268</v>
       </c>
       <c r="M367" t="n">
-        <v>357456</v>
+        <v>389243</v>
       </c>
       <c r="N367" t="n">
-        <v>-133301</v>
+        <v>-95500</v>
       </c>
       <c r="O367" t="n">
-        <v>-56416</v>
+        <v>-18615</v>
       </c>
       <c r="P367" t="n">
-        <v>-133081</v>
+        <v>-95280</v>
       </c>
       <c r="Q367" t="n">
-        <v>-166962</v>
+        <v>-129161</v>
       </c>
       <c r="R367" t="n">
-        <v>-154515</v>
+        <v>-116714</v>
       </c>
       <c r="S367" t="n">
-        <v>-8059.4</v>
+        <v>-2659.3</v>
       </c>
       <c r="T367" t="n">
-        <v>-177603</v>
+        <v>-139802</v>
       </c>
       <c r="U367" t="n">
-        <v>-23851.7</v>
+        <v>-18451.6</v>
       </c>
       <c r="V367" t="n">
-        <v>-6375</v>
+        <v>-5303</v>
       </c>
       <c r="W367" t="n">
-        <v>-10.9</v>
+        <v>-9</v>
       </c>
       <c r="X367" t="n">
-        <v>-2373.7</v>
+        <v>-2016.3</v>
       </c>
       <c r="Y367" t="n">
-        <v>-933.1</v>
+        <v>-780</v>
       </c>
       <c r="Z367" t="n">
-        <v>-6532</v>
+        <v>-5460</v>
       </c>
     </row>
     <row r="368">
@@ -29642,7 +29642,7 @@
         <v>44197</v>
       </c>
       <c r="B368" t="n">
-        <v>958</v>
+        <v>1340</v>
       </c>
       <c r="C368" t="n">
         <v>1167</v>
@@ -29654,7 +29654,7 @@
         <v>5976</v>
       </c>
       <c r="F368" t="n">
-        <v>7871</v>
+        <v>8116</v>
       </c>
       <c r="G368" t="n">
         <v>352</v>
@@ -29663,58 +29663,58 @@
         <v>77406</v>
       </c>
       <c r="I368" t="n">
-        <v>1168</v>
+        <v>1197</v>
       </c>
       <c r="J368" t="n">
-        <v>53275</v>
+        <v>54349</v>
       </c>
       <c r="K368" t="n">
-        <v>1740206</v>
+        <v>1778389</v>
       </c>
       <c r="L368" t="n">
-        <v>1020397</v>
+        <v>1058580</v>
       </c>
       <c r="M368" t="n">
-        <v>124843</v>
+        <v>156697</v>
       </c>
       <c r="N368" t="n">
-        <v>-98049</v>
+        <v>-59866</v>
       </c>
       <c r="O368" t="n">
-        <v>-37285</v>
+        <v>898</v>
       </c>
       <c r="P368" t="n">
-        <v>-93646</v>
+        <v>-55463</v>
       </c>
       <c r="Q368" t="n">
-        <v>-124056</v>
+        <v>-85873</v>
       </c>
       <c r="R368" t="n">
-        <v>45821</v>
+        <v>46203</v>
       </c>
       <c r="S368" t="n">
-        <v>-5326.4</v>
+        <v>128.3</v>
       </c>
       <c r="T368" t="n">
-        <v>44930</v>
+        <v>45312</v>
       </c>
       <c r="U368" t="n">
-        <v>-17722.3</v>
+        <v>-12267.6</v>
       </c>
       <c r="V368" t="n">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="W368" t="n">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="X368" t="n">
-        <v>-2102.7</v>
+        <v>-1744.7</v>
       </c>
       <c r="Y368" t="n">
-        <v>-801</v>
+        <v>-647.6</v>
       </c>
       <c r="Z368" t="n">
-        <v>-5607</v>
+        <v>-4533</v>
       </c>
     </row>
     <row r="369">
@@ -29722,7 +29722,7 @@
         <v>44198</v>
       </c>
       <c r="B369" t="n">
-        <v>1958</v>
+        <v>2584</v>
       </c>
       <c r="C369" t="n">
         <v>1100</v>
@@ -29734,7 +29734,7 @@
         <v>5174</v>
       </c>
       <c r="F369" t="n">
-        <v>7124</v>
+        <v>7394</v>
       </c>
       <c r="G369" t="n">
         <v>205</v>
@@ -29743,58 +29743,58 @@
         <v>77607</v>
       </c>
       <c r="I369" t="n">
-        <v>1014</v>
+        <v>1042</v>
       </c>
       <c r="J369" t="n">
-        <v>46750</v>
+        <v>47829</v>
       </c>
       <c r="K369" t="n">
-        <v>1430416</v>
+        <v>1469225</v>
       </c>
       <c r="L369" t="n">
-        <v>992959</v>
+        <v>1031768</v>
       </c>
       <c r="M369" t="n">
-        <v>122651</v>
+        <v>155249</v>
       </c>
       <c r="N369" t="n">
-        <v>-300628</v>
+        <v>-261819</v>
       </c>
       <c r="O369" t="n">
-        <v>-353586</v>
+        <v>-314777</v>
       </c>
       <c r="P369" t="n">
-        <v>-123500</v>
+        <v>-84691</v>
       </c>
       <c r="Q369" t="n">
-        <v>-153930</v>
+        <v>-115121</v>
       </c>
       <c r="R369" t="n">
-        <v>-309790</v>
+        <v>-309164</v>
       </c>
       <c r="S369" t="n">
-        <v>-50512.3</v>
+        <v>-44968.1</v>
       </c>
       <c r="T369" t="n">
-        <v>-27438</v>
+        <v>-26812</v>
       </c>
       <c r="U369" t="n">
-        <v>-21990</v>
+        <v>-16445.9</v>
       </c>
       <c r="V369" t="n">
-        <v>-6525</v>
+        <v>-6520</v>
       </c>
       <c r="W369" t="n">
-        <v>-12.2</v>
+        <v>-12</v>
       </c>
       <c r="X369" t="n">
-        <v>-3959</v>
+        <v>-3599.3</v>
       </c>
       <c r="Y369" t="n">
-        <v>-1751.7</v>
+        <v>-1597.6</v>
       </c>
       <c r="Z369" t="n">
-        <v>-12262</v>
+        <v>-11183</v>
       </c>
     </row>
     <row r="370">
@@ -29850,25 +29850,25 @@
         <v>-989017</v>
       </c>
       <c r="R370" t="n">
-        <v>-1102483</v>
+        <v>-1141292</v>
       </c>
       <c r="S370" t="n">
         <v>-208650.7</v>
       </c>
       <c r="T370" t="n">
-        <v>-832655</v>
+        <v>-871464</v>
       </c>
       <c r="U370" t="n">
         <v>-141288.1</v>
       </c>
       <c r="V370" t="n">
-        <v>-38466</v>
+        <v>-39545</v>
       </c>
       <c r="W370" t="n">
-        <v>-82.3</v>
+        <v>-82.7</v>
       </c>
       <c r="X370" t="n">
-        <v>-14656</v>
+        <v>-15013.3</v>
       </c>
       <c r="Y370" t="n">
         <v>-7261.4</v>

</xml_diff>

<commit_message>
actualiza 2 datos provincias 2021-01-21
</commit_message>
<xml_diff>
--- a/data/output/covid19-spain_consolidated.xlsx
+++ b/data/output/covid19-spain_consolidated.xlsx
@@ -22051,7 +22051,7 @@
         <v>68782</v>
       </c>
       <c r="E273" t="n">
-        <v>15656</v>
+        <v>15655</v>
       </c>
       <c r="F273" t="n">
         <v>9896</v>
@@ -22075,7 +22075,7 @@
         <v>773288</v>
       </c>
       <c r="M273" t="n">
-        <v>131929</v>
+        <v>131930</v>
       </c>
       <c r="N273" t="n">
         <v>150399</v>
@@ -22131,7 +22131,7 @@
         <v>68955</v>
       </c>
       <c r="E274" t="n">
-        <v>15468</v>
+        <v>15467</v>
       </c>
       <c r="F274" t="n">
         <v>9639</v>
@@ -22155,7 +22155,7 @@
         <v>784298</v>
       </c>
       <c r="M274" t="n">
-        <v>135502</v>
+        <v>135503</v>
       </c>
       <c r="N274" t="n">
         <v>148733</v>
@@ -22211,7 +22211,7 @@
         <v>69217</v>
       </c>
       <c r="E275" t="n">
-        <v>15189</v>
+        <v>15188</v>
       </c>
       <c r="F275" t="n">
         <v>9378</v>
@@ -22235,7 +22235,7 @@
         <v>793999</v>
       </c>
       <c r="M275" t="n">
-        <v>138356</v>
+        <v>138357</v>
       </c>
       <c r="N275" t="n">
         <v>146348</v>
@@ -22291,7 +22291,7 @@
         <v>69363</v>
       </c>
       <c r="E276" t="n">
-        <v>6221</v>
+        <v>6220</v>
       </c>
       <c r="F276" t="n">
         <v>9278</v>
@@ -22315,7 +22315,7 @@
         <v>804191</v>
       </c>
       <c r="M276" t="n">
-        <v>114526</v>
+        <v>114527</v>
       </c>
       <c r="N276" t="n">
         <v>143710</v>
@@ -22371,7 +22371,7 @@
         <v>69576</v>
       </c>
       <c r="E277" t="n">
-        <v>3570</v>
+        <v>3569</v>
       </c>
       <c r="F277" t="n">
         <v>9159</v>
@@ -22395,7 +22395,7 @@
         <v>815612</v>
       </c>
       <c r="M277" t="n">
-        <v>116473</v>
+        <v>116474</v>
       </c>
       <c r="N277" t="n">
         <v>139657</v>
@@ -22451,7 +22451,7 @@
         <v>69591</v>
       </c>
       <c r="E278" t="n">
-        <v>3659</v>
+        <v>3658</v>
       </c>
       <c r="F278" t="n">
         <v>9172</v>
@@ -22475,7 +22475,7 @@
         <v>820776</v>
       </c>
       <c r="M278" t="n">
-        <v>73807</v>
+        <v>73808</v>
       </c>
       <c r="N278" t="n">
         <v>138777</v>
@@ -22531,7 +22531,7 @@
         <v>69609</v>
       </c>
       <c r="E279" t="n">
-        <v>6070</v>
+        <v>6069</v>
       </c>
       <c r="F279" t="n">
         <v>9479</v>
@@ -22555,7 +22555,7 @@
         <v>823908</v>
       </c>
       <c r="M279" t="n">
-        <v>74529</v>
+        <v>74530</v>
       </c>
       <c r="N279" t="n">
         <v>138540</v>
@@ -22611,7 +22611,7 @@
         <v>69710</v>
       </c>
       <c r="E280" t="n">
-        <v>3468</v>
+        <v>3466</v>
       </c>
       <c r="F280" t="n">
         <v>9568</v>
@@ -22635,7 +22635,7 @@
         <v>832295</v>
       </c>
       <c r="M280" t="n">
-        <v>120670</v>
+        <v>120672</v>
       </c>
       <c r="N280" t="n">
         <v>137172</v>
@@ -22691,7 +22691,7 @@
         <v>69856</v>
       </c>
       <c r="E281" t="n">
-        <v>5791</v>
+        <v>5789</v>
       </c>
       <c r="F281" t="n">
         <v>9375</v>
@@ -22715,7 +22715,7 @@
         <v>841157</v>
       </c>
       <c r="M281" t="n">
-        <v>135135</v>
+        <v>135137</v>
       </c>
       <c r="N281" t="n">
         <v>135241</v>
@@ -22771,7 +22771,7 @@
         <v>69961</v>
       </c>
       <c r="E282" t="n">
-        <v>14713</v>
+        <v>14711</v>
       </c>
       <c r="F282" t="n">
         <v>9216</v>
@@ -22795,7 +22795,7 @@
         <v>850758</v>
       </c>
       <c r="M282" t="n">
-        <v>165997</v>
+        <v>165999</v>
       </c>
       <c r="N282" t="n">
         <v>135027</v>
@@ -22851,7 +22851,7 @@
         <v>70155</v>
       </c>
       <c r="E283" t="n">
-        <v>5866</v>
+        <v>5864</v>
       </c>
       <c r="F283" t="n">
         <v>9163</v>
@@ -22875,7 +22875,7 @@
         <v>860648</v>
       </c>
       <c r="M283" t="n">
-        <v>139333</v>
+        <v>139335</v>
       </c>
       <c r="N283" t="n">
         <v>135360</v>
@@ -22931,7 +22931,7 @@
         <v>70276</v>
       </c>
       <c r="E284" t="n">
-        <v>3446</v>
+        <v>3444</v>
       </c>
       <c r="F284" t="n">
         <v>9091</v>
@@ -22955,7 +22955,7 @@
         <v>806765</v>
       </c>
       <c r="M284" t="n">
-        <v>128891</v>
+        <v>128893</v>
       </c>
       <c r="N284" t="n">
         <v>135267</v>
@@ -23011,7 +23011,7 @@
         <v>70280</v>
       </c>
       <c r="E285" t="n">
-        <v>3515</v>
+        <v>3512</v>
       </c>
       <c r="F285" t="n">
         <v>9115</v>
@@ -23035,7 +23035,7 @@
         <v>812135</v>
       </c>
       <c r="M285" t="n">
-        <v>82444</v>
+        <v>82447</v>
       </c>
       <c r="N285" t="n">
         <v>135567</v>
@@ -23091,7 +23091,7 @@
         <v>70283</v>
       </c>
       <c r="E286" t="n">
-        <v>3590</v>
+        <v>3587</v>
       </c>
       <c r="F286" t="n">
         <v>9427</v>
@@ -23115,7 +23115,7 @@
         <v>817014</v>
       </c>
       <c r="M286" t="n">
-        <v>83115</v>
+        <v>83118</v>
       </c>
       <c r="N286" t="n">
         <v>137641</v>
@@ -23171,7 +23171,7 @@
         <v>70291</v>
       </c>
       <c r="E287" t="n">
-        <v>6198</v>
+        <v>6195</v>
       </c>
       <c r="F287" t="n">
         <v>9814</v>
@@ -23195,7 +23195,7 @@
         <v>822411</v>
       </c>
       <c r="M287" t="n">
-        <v>145025</v>
+        <v>145028</v>
       </c>
       <c r="N287" t="n">
         <v>135754</v>
@@ -23251,7 +23251,7 @@
         <v>70544</v>
       </c>
       <c r="E288" t="n">
-        <v>6043</v>
+        <v>6040</v>
       </c>
       <c r="F288" t="n">
         <v>10083</v>
@@ -23275,7 +23275,7 @@
         <v>833621</v>
       </c>
       <c r="M288" t="n">
-        <v>146816</v>
+        <v>146819</v>
       </c>
       <c r="N288" t="n">
         <v>137294</v>
@@ -23331,7 +23331,7 @@
         <v>70684</v>
       </c>
       <c r="E289" t="n">
-        <v>6171</v>
+        <v>6168</v>
       </c>
       <c r="F289" t="n">
         <v>10095</v>
@@ -23355,7 +23355,7 @@
         <v>845266</v>
       </c>
       <c r="M289" t="n">
-        <v>148228</v>
+        <v>148231</v>
       </c>
       <c r="N289" t="n">
         <v>141172</v>
@@ -23411,7 +23411,7 @@
         <v>70924</v>
       </c>
       <c r="E290" t="n">
-        <v>6177</v>
+        <v>6174</v>
       </c>
       <c r="F290" t="n">
         <v>10192</v>
@@ -23435,7 +23435,7 @@
         <v>857470</v>
       </c>
       <c r="M290" t="n">
-        <v>150750</v>
+        <v>150753</v>
       </c>
       <c r="N290" t="n">
         <v>145228</v>
@@ -23491,7 +23491,7 @@
         <v>71056</v>
       </c>
       <c r="E291" t="n">
-        <v>3599</v>
+        <v>3596</v>
       </c>
       <c r="F291" t="n">
         <v>10185</v>
@@ -23515,7 +23515,7 @@
         <v>870669</v>
       </c>
       <c r="M291" t="n">
-        <v>139603</v>
+        <v>139606</v>
       </c>
       <c r="N291" t="n">
         <v>149944</v>
@@ -23571,7 +23571,7 @@
         <v>71063</v>
       </c>
       <c r="E292" t="n">
-        <v>3896</v>
+        <v>3893</v>
       </c>
       <c r="F292" t="n">
         <v>10406</v>
@@ -23595,7 +23595,7 @@
         <v>877957</v>
       </c>
       <c r="M292" t="n">
-        <v>90471</v>
+        <v>90474</v>
       </c>
       <c r="N292" t="n">
         <v>153407</v>
@@ -23651,7 +23651,7 @@
         <v>71066</v>
       </c>
       <c r="E293" t="n">
-        <v>3990</v>
+        <v>3987</v>
       </c>
       <c r="F293" t="n">
         <v>10941</v>
@@ -23675,7 +23675,7 @@
         <v>884311</v>
       </c>
       <c r="M293" t="n">
-        <v>91347</v>
+        <v>91350</v>
       </c>
       <c r="N293" t="n">
         <v>158185</v>
@@ -23731,7 +23731,7 @@
         <v>71296</v>
       </c>
       <c r="E294" t="n">
-        <v>6705</v>
+        <v>6702</v>
       </c>
       <c r="F294" t="n">
         <v>11344</v>
@@ -23755,7 +23755,7 @@
         <v>898407</v>
       </c>
       <c r="M294" t="n">
-        <v>157320</v>
+        <v>157323</v>
       </c>
       <c r="N294" t="n">
         <v>165232</v>
@@ -23811,7 +23811,7 @@
         <v>71456</v>
       </c>
       <c r="E295" t="n">
-        <v>6872</v>
+        <v>6869</v>
       </c>
       <c r="F295" t="n">
         <v>11580</v>
@@ -23835,7 +23835,7 @@
         <v>911162</v>
       </c>
       <c r="M295" t="n">
-        <v>159391</v>
+        <v>159394</v>
       </c>
       <c r="N295" t="n">
         <v>170356</v>
@@ -23891,7 +23891,7 @@
         <v>71641</v>
       </c>
       <c r="E296" t="n">
-        <v>19227</v>
+        <v>19223</v>
       </c>
       <c r="F296" t="n">
         <v>11940</v>
@@ -23915,7 +23915,7 @@
         <v>925228</v>
       </c>
       <c r="M296" t="n">
-        <v>151407</v>
+        <v>151411</v>
       </c>
       <c r="N296" t="n">
         <v>173141</v>
@@ -23971,7 +23971,7 @@
         <v>72051</v>
       </c>
       <c r="E297" t="n">
-        <v>7420</v>
+        <v>7416</v>
       </c>
       <c r="F297" t="n">
         <v>12376</v>
@@ -23995,7 +23995,7 @@
         <v>938306</v>
       </c>
       <c r="M297" t="n">
-        <v>164243</v>
+        <v>164247</v>
       </c>
       <c r="N297" t="n">
         <v>180771</v>
@@ -24051,7 +24051,7 @@
         <v>72461</v>
       </c>
       <c r="E298" t="n">
-        <v>4676</v>
+        <v>4672</v>
       </c>
       <c r="F298" t="n">
         <v>12743</v>
@@ -24075,7 +24075,7 @@
         <v>903555</v>
       </c>
       <c r="M298" t="n">
-        <v>152504</v>
+        <v>152508</v>
       </c>
       <c r="N298" t="n">
         <v>190933</v>
@@ -24131,7 +24131,7 @@
         <v>72472</v>
       </c>
       <c r="E299" t="n">
-        <v>4897</v>
+        <v>4893</v>
       </c>
       <c r="F299" t="n">
         <v>13087</v>
@@ -24155,7 +24155,7 @@
         <v>911253</v>
       </c>
       <c r="M299" t="n">
-        <v>99583</v>
+        <v>99587</v>
       </c>
       <c r="N299" t="n">
         <v>196602</v>
@@ -24211,7 +24211,7 @@
         <v>72476</v>
       </c>
       <c r="E300" t="n">
-        <v>7929</v>
+        <v>7925</v>
       </c>
       <c r="F300" t="n">
         <v>13735</v>
@@ -24235,7 +24235,7 @@
         <v>917669</v>
       </c>
       <c r="M300" t="n">
-        <v>114635</v>
+        <v>114639</v>
       </c>
       <c r="N300" t="n">
         <v>200760</v>
@@ -24282,16 +24282,16 @@
         <v>44130</v>
       </c>
       <c r="B301" t="n">
-        <v>4819</v>
+        <v>4820</v>
       </c>
       <c r="C301" t="n">
-        <v>7546.266</v>
+        <v>7547.266</v>
       </c>
       <c r="D301" t="n">
         <v>72687</v>
       </c>
       <c r="E301" t="n">
-        <v>4875</v>
+        <v>4872</v>
       </c>
       <c r="F301" t="n">
         <v>14225</v>
@@ -24309,37 +24309,37 @@
         <v>43937</v>
       </c>
       <c r="K301" t="n">
-        <v>1194209</v>
+        <v>1194210</v>
       </c>
       <c r="L301" t="n">
-        <v>887167</v>
+        <v>887168</v>
       </c>
       <c r="M301" t="n">
-        <v>156717</v>
+        <v>156721</v>
       </c>
       <c r="N301" t="n">
-        <v>219104</v>
+        <v>219105</v>
       </c>
       <c r="O301" t="n">
-        <v>124278</v>
+        <v>124279</v>
       </c>
       <c r="P301" t="n">
-        <v>64756</v>
+        <v>64757</v>
       </c>
       <c r="Q301" t="n">
-        <v>-11240</v>
+        <v>-11239</v>
       </c>
       <c r="R301" t="n">
-        <v>25681</v>
+        <v>25682</v>
       </c>
       <c r="S301" t="n">
-        <v>17754</v>
+        <v>17754.1</v>
       </c>
       <c r="T301" t="n">
-        <v>-30502</v>
+        <v>-30501</v>
       </c>
       <c r="U301" t="n">
-        <v>-1605.7</v>
+        <v>-1605.6</v>
       </c>
       <c r="V301" t="n">
         <v>291</v>
@@ -24371,7 +24371,7 @@
         <v>72928</v>
       </c>
       <c r="E302" t="n">
-        <v>8123</v>
+        <v>8120</v>
       </c>
       <c r="F302" t="n">
         <v>14388</v>
@@ -24389,37 +24389,37 @@
         <v>44176</v>
       </c>
       <c r="K302" t="n">
-        <v>1213170</v>
+        <v>1213171</v>
       </c>
       <c r="L302" t="n">
-        <v>899891</v>
+        <v>899892</v>
       </c>
       <c r="M302" t="n">
-        <v>173797</v>
+        <v>173801</v>
       </c>
       <c r="N302" t="n">
-        <v>225151</v>
+        <v>225152</v>
       </c>
       <c r="O302" t="n">
-        <v>127405</v>
+        <v>127406</v>
       </c>
       <c r="P302" t="n">
-        <v>66270</v>
+        <v>66271</v>
       </c>
       <c r="Q302" t="n">
-        <v>-11271</v>
+        <v>-11270</v>
       </c>
       <c r="R302" t="n">
         <v>18961</v>
       </c>
       <c r="S302" t="n">
-        <v>18200.7</v>
+        <v>18200.9</v>
       </c>
       <c r="T302" t="n">
         <v>12724</v>
       </c>
       <c r="U302" t="n">
-        <v>-1610.1</v>
+        <v>-1610</v>
       </c>
       <c r="V302" t="n">
         <v>239</v>
@@ -24451,7 +24451,7 @@
         <v>73142</v>
       </c>
       <c r="E303" t="n">
-        <v>25701</v>
+        <v>25698</v>
       </c>
       <c r="F303" t="n">
         <v>14624</v>
@@ -24469,37 +24469,37 @@
         <v>44387</v>
       </c>
       <c r="K303" t="n">
-        <v>1239468</v>
+        <v>1239469</v>
       </c>
       <c r="L303" t="n">
-        <v>856971</v>
+        <v>856972</v>
       </c>
       <c r="M303" t="n">
-        <v>212459</v>
+        <v>212463</v>
       </c>
       <c r="N303" t="n">
-        <v>237432</v>
+        <v>237433</v>
       </c>
       <c r="O303" t="n">
-        <v>138896</v>
+        <v>138897</v>
       </c>
       <c r="P303" t="n">
-        <v>11705</v>
+        <v>11706</v>
       </c>
       <c r="Q303" t="n">
-        <v>-68257</v>
+        <v>-68256</v>
       </c>
       <c r="R303" t="n">
         <v>26298</v>
       </c>
       <c r="S303" t="n">
-        <v>19842.3</v>
+        <v>19842.4</v>
       </c>
       <c r="T303" t="n">
         <v>-42920</v>
       </c>
       <c r="U303" t="n">
-        <v>-9751</v>
+        <v>-9750.9</v>
       </c>
       <c r="V303" t="n">
         <v>211</v>
@@ -24531,7 +24531,7 @@
         <v>73357</v>
       </c>
       <c r="E304" t="n">
-        <v>5152</v>
+        <v>5149</v>
       </c>
       <c r="F304" t="n">
         <v>14931</v>
@@ -24549,37 +24549,37 @@
         <v>44630</v>
       </c>
       <c r="K304" t="n">
-        <v>1262342</v>
+        <v>1262343</v>
       </c>
       <c r="L304" t="n">
-        <v>869606</v>
+        <v>869607</v>
       </c>
       <c r="M304" t="n">
-        <v>165282</v>
+        <v>165286</v>
       </c>
       <c r="N304" t="n">
-        <v>245585</v>
+        <v>245586</v>
       </c>
       <c r="O304" t="n">
-        <v>141635</v>
+        <v>141636</v>
       </c>
       <c r="P304" t="n">
-        <v>12136</v>
+        <v>12137</v>
       </c>
       <c r="Q304" t="n">
-        <v>-68700</v>
+        <v>-68699</v>
       </c>
       <c r="R304" t="n">
         <v>22874</v>
       </c>
       <c r="S304" t="n">
-        <v>20233.6</v>
+        <v>20233.7</v>
       </c>
       <c r="T304" t="n">
         <v>12635</v>
       </c>
       <c r="U304" t="n">
-        <v>-9814.3</v>
+        <v>-9814.1</v>
       </c>
       <c r="V304" t="n">
         <v>243</v>
@@ -24611,7 +24611,7 @@
         <v>73514</v>
       </c>
       <c r="E305" t="n">
-        <v>5219</v>
+        <v>5216</v>
       </c>
       <c r="F305" t="n">
         <v>14922</v>
@@ -24629,37 +24629,37 @@
         <v>44886</v>
       </c>
       <c r="K305" t="n">
-        <v>1286833</v>
+        <v>1286834</v>
       </c>
       <c r="L305" t="n">
-        <v>883554</v>
+        <v>883555</v>
       </c>
       <c r="M305" t="n">
-        <v>168455</v>
+        <v>168459</v>
       </c>
       <c r="N305" t="n">
-        <v>253370</v>
+        <v>253371</v>
       </c>
       <c r="O305" t="n">
-        <v>142430</v>
+        <v>142431</v>
       </c>
       <c r="P305" t="n">
-        <v>12885</v>
+        <v>12886</v>
       </c>
       <c r="Q305" t="n">
-        <v>-20001</v>
+        <v>-20000</v>
       </c>
       <c r="R305" t="n">
         <v>24491</v>
       </c>
       <c r="S305" t="n">
-        <v>20347.1</v>
+        <v>20347.3</v>
       </c>
       <c r="T305" t="n">
         <v>13948</v>
       </c>
       <c r="U305" t="n">
-        <v>-2857.3</v>
+        <v>-2857.1</v>
       </c>
       <c r="V305" t="n">
         <v>256</v>
@@ -24691,7 +24691,7 @@
         <v>73528</v>
       </c>
       <c r="E306" t="n">
-        <v>5462</v>
+        <v>5459</v>
       </c>
       <c r="F306" t="n">
         <v>15299</v>
@@ -24709,37 +24709,37 @@
         <v>45137</v>
       </c>
       <c r="K306" t="n">
-        <v>1305275</v>
+        <v>1305276</v>
       </c>
       <c r="L306" t="n">
-        <v>891939</v>
+        <v>891940</v>
       </c>
       <c r="M306" t="n">
-        <v>112632</v>
+        <v>112636</v>
       </c>
       <c r="N306" t="n">
-        <v>261311</v>
+        <v>261312</v>
       </c>
       <c r="O306" t="n">
-        <v>147446</v>
+        <v>147447</v>
       </c>
       <c r="P306" t="n">
-        <v>13982</v>
+        <v>13983</v>
       </c>
       <c r="Q306" t="n">
-        <v>-19314</v>
+        <v>-19313</v>
       </c>
       <c r="R306" t="n">
         <v>18442</v>
       </c>
       <c r="S306" t="n">
-        <v>21063.7</v>
+        <v>21063.9</v>
       </c>
       <c r="T306" t="n">
         <v>8385</v>
       </c>
       <c r="U306" t="n">
-        <v>-2759.1</v>
+        <v>-2759</v>
       </c>
       <c r="V306" t="n">
         <v>251</v>
@@ -24771,7 +24771,7 @@
         <v>73536</v>
       </c>
       <c r="E307" t="n">
-        <v>5433</v>
+        <v>5430</v>
       </c>
       <c r="F307" t="n">
         <v>16089</v>
@@ -24789,37 +24789,37 @@
         <v>45344</v>
       </c>
       <c r="K307" t="n">
-        <v>1320284</v>
+        <v>1320285</v>
       </c>
       <c r="L307" t="n">
-        <v>899000</v>
+        <v>899001</v>
       </c>
       <c r="M307" t="n">
-        <v>114165</v>
+        <v>114169</v>
       </c>
       <c r="N307" t="n">
-        <v>266941</v>
+        <v>266942</v>
       </c>
       <c r="O307" t="n">
-        <v>151756</v>
+        <v>151757</v>
       </c>
       <c r="P307" t="n">
-        <v>14689</v>
+        <v>14690</v>
       </c>
       <c r="Q307" t="n">
-        <v>-18669</v>
+        <v>-18668</v>
       </c>
       <c r="R307" t="n">
         <v>15009</v>
       </c>
       <c r="S307" t="n">
-        <v>21679.4</v>
+        <v>21679.6</v>
       </c>
       <c r="T307" t="n">
         <v>7061</v>
       </c>
       <c r="U307" t="n">
-        <v>-2667</v>
+        <v>-2666.9</v>
       </c>
       <c r="V307" t="n">
         <v>207</v>
@@ -24851,7 +24851,7 @@
         <v>73652</v>
       </c>
       <c r="E308" t="n">
-        <v>8974</v>
+        <v>8971</v>
       </c>
       <c r="F308" t="n">
         <v>16701</v>
@@ -24869,22 +24869,22 @@
         <v>45715</v>
       </c>
       <c r="K308" t="n">
-        <v>1337766</v>
+        <v>1337767</v>
       </c>
       <c r="L308" t="n">
-        <v>909052</v>
+        <v>909053</v>
       </c>
       <c r="M308" t="n">
-        <v>192115</v>
+        <v>192119</v>
       </c>
       <c r="N308" t="n">
-        <v>267835</v>
+        <v>267836</v>
       </c>
       <c r="O308" t="n">
         <v>143557</v>
       </c>
       <c r="P308" t="n">
-        <v>10645</v>
+        <v>10646</v>
       </c>
       <c r="Q308" t="n">
         <v>21885</v>
@@ -24931,7 +24931,7 @@
         <v>73966</v>
       </c>
       <c r="E309" t="n">
-        <v>5357</v>
+        <v>5354</v>
       </c>
       <c r="F309" t="n">
         <v>16995</v>
@@ -24949,22 +24949,22 @@
         <v>46022</v>
       </c>
       <c r="K309" t="n">
-        <v>1358066</v>
+        <v>1358067</v>
       </c>
       <c r="L309" t="n">
-        <v>920389</v>
+        <v>920390</v>
       </c>
       <c r="M309" t="n">
-        <v>182003</v>
+        <v>182007</v>
       </c>
       <c r="N309" t="n">
-        <v>272301</v>
+        <v>272302</v>
       </c>
       <c r="O309" t="n">
         <v>144896</v>
       </c>
       <c r="P309" t="n">
-        <v>9227</v>
+        <v>9228</v>
       </c>
       <c r="Q309" t="n">
         <v>20498</v>
@@ -25011,7 +25011,7 @@
         <v>74233</v>
       </c>
       <c r="E310" t="n">
-        <v>30291</v>
+        <v>30288</v>
       </c>
       <c r="F310" t="n">
         <v>17176</v>
@@ -25029,22 +25029,22 @@
         <v>46351</v>
       </c>
       <c r="K310" t="n">
-        <v>1377733</v>
+        <v>1377734</v>
       </c>
       <c r="L310" t="n">
-        <v>932272</v>
+        <v>932273</v>
       </c>
       <c r="M310" t="n">
-        <v>237916</v>
+        <v>237920</v>
       </c>
       <c r="N310" t="n">
-        <v>277161</v>
+        <v>277162</v>
       </c>
       <c r="O310" t="n">
         <v>138265</v>
       </c>
       <c r="P310" t="n">
-        <v>7044</v>
+        <v>7045</v>
       </c>
       <c r="Q310" t="n">
         <v>75301</v>
@@ -25091,7 +25091,7 @@
         <v>74451</v>
       </c>
       <c r="E311" t="n">
-        <v>9530</v>
+        <v>9527</v>
       </c>
       <c r="F311" t="n">
         <v>16996</v>
@@ -25109,22 +25109,22 @@
         <v>46694</v>
       </c>
       <c r="K311" t="n">
-        <v>1397858</v>
+        <v>1397859</v>
       </c>
       <c r="L311" t="n">
-        <v>943809</v>
+        <v>943810</v>
       </c>
       <c r="M311" t="n">
-        <v>203258</v>
+        <v>203262</v>
       </c>
       <c r="N311" t="n">
-        <v>277151</v>
+        <v>277152</v>
       </c>
       <c r="O311" t="n">
         <v>135516</v>
       </c>
       <c r="P311" t="n">
-        <v>5503</v>
+        <v>5504</v>
       </c>
       <c r="Q311" t="n">
         <v>74203</v>
@@ -25171,7 +25171,7 @@
         <v>74801</v>
       </c>
       <c r="E312" t="n">
-        <v>5856</v>
+        <v>5853</v>
       </c>
       <c r="F312" t="n">
         <v>16614</v>
@@ -25189,22 +25189,22 @@
         <v>47005</v>
       </c>
       <c r="K312" t="n">
-        <v>1418715</v>
+        <v>1418716</v>
       </c>
       <c r="L312" t="n">
-        <v>955463</v>
+        <v>955464</v>
       </c>
       <c r="M312" t="n">
-        <v>191439</v>
+        <v>191443</v>
       </c>
       <c r="N312" t="n">
-        <v>274312</v>
+        <v>274313</v>
       </c>
       <c r="O312" t="n">
         <v>131882</v>
       </c>
       <c r="P312" t="n">
-        <v>51908</v>
+        <v>51909</v>
       </c>
       <c r="Q312" t="n">
         <v>71909</v>
@@ -25251,7 +25251,7 @@
         <v>74843</v>
       </c>
       <c r="E313" t="n">
-        <v>6120</v>
+        <v>6117</v>
       </c>
       <c r="F313" t="n">
         <v>16665</v>
@@ -25269,22 +25269,22 @@
         <v>47278</v>
       </c>
       <c r="K313" t="n">
-        <v>1436139</v>
+        <v>1436140</v>
       </c>
       <c r="L313" t="n">
-        <v>962801</v>
+        <v>962802</v>
       </c>
       <c r="M313" t="n">
-        <v>129052</v>
+        <v>129056</v>
       </c>
       <c r="N313" t="n">
-        <v>278310</v>
+        <v>278311</v>
       </c>
       <c r="O313" t="n">
         <v>130864</v>
       </c>
       <c r="P313" t="n">
-        <v>51548</v>
+        <v>51549</v>
       </c>
       <c r="Q313" t="n">
         <v>70862</v>
@@ -25331,7 +25331,7 @@
         <v>74845</v>
       </c>
       <c r="E314" t="n">
-        <v>9974</v>
+        <v>9971</v>
       </c>
       <c r="F314" t="n">
         <v>17324</v>
@@ -25349,22 +25349,22 @@
         <v>47513</v>
       </c>
       <c r="K314" t="n">
-        <v>1447832</v>
+        <v>1447833</v>
       </c>
       <c r="L314" t="n">
-        <v>968467</v>
+        <v>968468</v>
       </c>
       <c r="M314" t="n">
-        <v>146313</v>
+        <v>146317</v>
       </c>
       <c r="N314" t="n">
-        <v>279304</v>
+        <v>279305</v>
       </c>
       <c r="O314" t="n">
         <v>127548</v>
       </c>
       <c r="P314" t="n">
-        <v>50798</v>
+        <v>50799</v>
       </c>
       <c r="Q314" t="n">
         <v>69467</v>
@@ -25411,7 +25411,7 @@
         <v>75126</v>
       </c>
       <c r="E315" t="n">
-        <v>9742</v>
+        <v>9739</v>
       </c>
       <c r="F315" t="n">
         <v>17774</v>
@@ -25429,13 +25429,13 @@
         <v>47904</v>
       </c>
       <c r="K315" t="n">
-        <v>1463068</v>
+        <v>1463069</v>
       </c>
       <c r="L315" t="n">
-        <v>976956</v>
+        <v>976957</v>
       </c>
       <c r="M315" t="n">
-        <v>217085</v>
+        <v>217089</v>
       </c>
       <c r="N315" t="n">
         <v>268859</v>
@@ -25491,7 +25491,7 @@
         <v>75422</v>
       </c>
       <c r="E316" t="n">
-        <v>9723</v>
+        <v>9720</v>
       </c>
       <c r="F316" t="n">
         <v>17586</v>
@@ -25509,13 +25509,13 @@
         <v>48292</v>
       </c>
       <c r="K316" t="n">
-        <v>1481453</v>
+        <v>1481454</v>
       </c>
       <c r="L316" t="n">
-        <v>987062</v>
+        <v>987063</v>
       </c>
       <c r="M316" t="n">
-        <v>221574</v>
+        <v>221578</v>
       </c>
       <c r="N316" t="n">
         <v>268283</v>
@@ -25571,7 +25571,7 @@
         <v>75758</v>
       </c>
       <c r="E317" t="n">
-        <v>28646</v>
+        <v>28643</v>
       </c>
       <c r="F317" t="n">
         <v>17432</v>
@@ -25589,13 +25589,13 @@
         <v>48604</v>
       </c>
       <c r="K317" t="n">
-        <v>1499591</v>
+        <v>1499592</v>
       </c>
       <c r="L317" t="n">
-        <v>996921</v>
+        <v>996922</v>
       </c>
       <c r="M317" t="n">
-        <v>272682</v>
+        <v>272686</v>
       </c>
       <c r="N317" t="n">
         <v>260123</v>
@@ -25651,7 +25651,7 @@
         <v>75988</v>
       </c>
       <c r="E318" t="n">
-        <v>9569</v>
+        <v>9566</v>
       </c>
       <c r="F318" t="n">
         <v>17367</v>
@@ -25669,13 +25669,13 @@
         <v>48927</v>
       </c>
       <c r="K318" t="n">
-        <v>1518770</v>
+        <v>1518771</v>
       </c>
       <c r="L318" t="n">
-        <v>1006294</v>
+        <v>1006295</v>
       </c>
       <c r="M318" t="n">
-        <v>231894</v>
+        <v>231898</v>
       </c>
       <c r="N318" t="n">
         <v>256428</v>
@@ -25731,7 +25731,7 @@
         <v>76433</v>
       </c>
       <c r="E319" t="n">
-        <v>4998</v>
+        <v>4995</v>
       </c>
       <c r="F319" t="n">
         <v>16753</v>
@@ -25749,13 +25749,13 @@
         <v>49259</v>
       </c>
       <c r="K319" t="n">
-        <v>1537009</v>
+        <v>1537010</v>
       </c>
       <c r="L319" t="n">
-        <v>1015059</v>
+        <v>1015060</v>
       </c>
       <c r="M319" t="n">
-        <v>220717</v>
+        <v>220721</v>
       </c>
       <c r="N319" t="n">
         <v>250176</v>
@@ -25811,7 +25811,7 @@
         <v>76450</v>
       </c>
       <c r="E320" t="n">
-        <v>5049</v>
+        <v>5046</v>
       </c>
       <c r="F320" t="n">
         <v>16591</v>
@@ -25829,13 +25829,13 @@
         <v>49502</v>
       </c>
       <c r="K320" t="n">
-        <v>1550765</v>
+        <v>1550766</v>
       </c>
       <c r="L320" t="n">
-        <v>1021010</v>
+        <v>1021011</v>
       </c>
       <c r="M320" t="n">
-        <v>151061</v>
+        <v>151065</v>
       </c>
       <c r="N320" t="n">
         <v>245490</v>
@@ -25891,7 +25891,7 @@
         <v>76468</v>
       </c>
       <c r="E321" t="n">
-        <v>8879</v>
+        <v>8876</v>
       </c>
       <c r="F321" t="n">
         <v>16959</v>
@@ -25909,13 +25909,13 @@
         <v>49741</v>
       </c>
       <c r="K321" t="n">
-        <v>1559503</v>
+        <v>1559504</v>
       </c>
       <c r="L321" t="n">
-        <v>1024632</v>
+        <v>1024633</v>
       </c>
       <c r="M321" t="n">
-        <v>171450</v>
+        <v>171454</v>
       </c>
       <c r="N321" t="n">
         <v>239219</v>
@@ -25971,7 +25971,7 @@
         <v>76960</v>
       </c>
       <c r="E322" t="n">
-        <v>8482</v>
+        <v>8479</v>
       </c>
       <c r="F322" t="n">
         <v>17149</v>
@@ -25989,13 +25989,13 @@
         <v>50136</v>
       </c>
       <c r="K322" t="n">
-        <v>1572032</v>
+        <v>1572033</v>
       </c>
       <c r="L322" t="n">
-        <v>1032094</v>
+        <v>1032095</v>
       </c>
       <c r="M322" t="n">
-        <v>251352</v>
+        <v>251356</v>
       </c>
       <c r="N322" t="n">
         <v>234266</v>
@@ -26051,7 +26051,7 @@
         <v>77566</v>
       </c>
       <c r="E323" t="n">
-        <v>8239</v>
+        <v>8236</v>
       </c>
       <c r="F323" t="n">
         <v>16719</v>
@@ -26069,13 +26069,13 @@
         <v>50509</v>
       </c>
       <c r="K323" t="n">
-        <v>1585258</v>
+        <v>1585259</v>
       </c>
       <c r="L323" t="n">
-        <v>1039243</v>
+        <v>1039244</v>
       </c>
       <c r="M323" t="n">
-        <v>256638</v>
+        <v>256642</v>
       </c>
       <c r="N323" t="n">
         <v>227192</v>
@@ -26131,7 +26131,7 @@
         <v>78000</v>
       </c>
       <c r="E324" t="n">
-        <v>22604</v>
+        <v>22601</v>
       </c>
       <c r="F324" t="n">
         <v>16165</v>
@@ -26149,13 +26149,13 @@
         <v>50839</v>
       </c>
       <c r="K324" t="n">
-        <v>1599569</v>
+        <v>1599570</v>
       </c>
       <c r="L324" t="n">
-        <v>1046217</v>
+        <v>1046218</v>
       </c>
       <c r="M324" t="n">
-        <v>316024</v>
+        <v>316028</v>
       </c>
       <c r="N324" t="n">
         <v>221836</v>
@@ -26211,7 +26211,7 @@
         <v>78567</v>
       </c>
       <c r="E325" t="n">
-        <v>21768</v>
+        <v>21765</v>
       </c>
       <c r="F325" t="n">
         <v>15543</v>
@@ -26229,13 +26229,13 @@
         <v>51147</v>
       </c>
       <c r="K325" t="n">
-        <v>1614334</v>
+        <v>1614335</v>
       </c>
       <c r="L325" t="n">
-        <v>1053121</v>
+        <v>1053122</v>
       </c>
       <c r="M325" t="n">
-        <v>323537</v>
+        <v>323541</v>
       </c>
       <c r="N325" t="n">
         <v>216476</v>
@@ -26291,7 +26291,7 @@
         <v>78969</v>
       </c>
       <c r="E326" t="n">
-        <v>17163</v>
+        <v>17158</v>
       </c>
       <c r="F326" t="n">
         <v>14830</v>
@@ -26309,13 +26309,13 @@
         <v>51454</v>
       </c>
       <c r="K326" t="n">
-        <v>1628100</v>
+        <v>1628101</v>
       </c>
       <c r="L326" t="n">
-        <v>1059250</v>
+        <v>1059251</v>
       </c>
       <c r="M326" t="n">
-        <v>311962</v>
+        <v>311968</v>
       </c>
       <c r="N326" t="n">
         <v>209385</v>
@@ -26371,7 +26371,7 @@
         <v>78992</v>
       </c>
       <c r="E327" t="n">
-        <v>15400</v>
+        <v>15395</v>
       </c>
       <c r="F327" t="n">
         <v>14342</v>
@@ -26389,13 +26389,13 @@
         <v>51682</v>
       </c>
       <c r="K327" t="n">
-        <v>1638874</v>
+        <v>1638875</v>
       </c>
       <c r="L327" t="n">
-        <v>1063238</v>
+        <v>1063239</v>
       </c>
       <c r="M327" t="n">
-        <v>232616</v>
+        <v>232622</v>
       </c>
       <c r="N327" t="n">
         <v>202735</v>
@@ -26451,7 +26451,7 @@
         <v>79003</v>
       </c>
       <c r="E328" t="n">
-        <v>20133</v>
+        <v>20128</v>
       </c>
       <c r="F328" t="n">
         <v>14561</v>
@@ -26469,13 +26469,13 @@
         <v>51861</v>
       </c>
       <c r="K328" t="n">
-        <v>1645373</v>
+        <v>1645374</v>
       </c>
       <c r="L328" t="n">
-        <v>1066109</v>
+        <v>1066110</v>
       </c>
       <c r="M328" t="n">
-        <v>255369</v>
+        <v>255375</v>
       </c>
       <c r="N328" t="n">
         <v>197541</v>
@@ -26531,7 +26531,7 @@
         <v>79403</v>
       </c>
       <c r="E329" t="n">
-        <v>16063</v>
+        <v>16057</v>
       </c>
       <c r="F329" t="n">
         <v>14447</v>
@@ -26549,13 +26549,13 @@
         <v>52276</v>
       </c>
       <c r="K329" t="n">
-        <v>1653392</v>
+        <v>1653393</v>
       </c>
       <c r="L329" t="n">
-        <v>1070670</v>
+        <v>1070671</v>
       </c>
       <c r="M329" t="n">
-        <v>328136</v>
+        <v>328143</v>
       </c>
       <c r="N329" t="n">
         <v>190324</v>
@@ -26611,7 +26611,7 @@
         <v>79948</v>
       </c>
       <c r="E330" t="n">
-        <v>15263</v>
+        <v>15257</v>
       </c>
       <c r="F330" t="n">
         <v>13826</v>
@@ -26629,13 +26629,13 @@
         <v>52565</v>
       </c>
       <c r="K330" t="n">
-        <v>1664489</v>
+        <v>1664490</v>
       </c>
       <c r="L330" t="n">
-        <v>1075581</v>
+        <v>1075582</v>
       </c>
       <c r="M330" t="n">
-        <v>335594</v>
+        <v>335601</v>
       </c>
       <c r="N330" t="n">
         <v>183036</v>
@@ -26691,7 +26691,7 @@
         <v>80350</v>
       </c>
       <c r="E331" t="n">
-        <v>14248</v>
+        <v>14240</v>
       </c>
       <c r="F331" t="n">
         <v>13161</v>
@@ -26709,13 +26709,13 @@
         <v>52867</v>
       </c>
       <c r="K331" t="n">
-        <v>1673727</v>
+        <v>1673728</v>
       </c>
       <c r="L331" t="n">
-        <v>1080479</v>
+        <v>1080480</v>
       </c>
       <c r="M331" t="n">
-        <v>343019</v>
+        <v>343028</v>
       </c>
       <c r="N331" t="n">
         <v>174136</v>
@@ -26771,7 +26771,7 @@
         <v>80632</v>
       </c>
       <c r="E332" t="n">
-        <v>13471</v>
+        <v>13460</v>
       </c>
       <c r="F332" t="n">
         <v>12601</v>
@@ -26789,13 +26789,13 @@
         <v>53156</v>
       </c>
       <c r="K332" t="n">
-        <v>1685503</v>
+        <v>1685504</v>
       </c>
       <c r="L332" t="n">
-        <v>1085517</v>
+        <v>1085518</v>
       </c>
       <c r="M332" t="n">
-        <v>349877</v>
+        <v>349889</v>
       </c>
       <c r="N332" t="n">
         <v>166733</v>
@@ -26851,7 +26851,7 @@
         <v>80963</v>
       </c>
       <c r="E333" t="n">
-        <v>12687</v>
+        <v>12675</v>
       </c>
       <c r="F333" t="n">
         <v>11955</v>
@@ -26869,13 +26869,13 @@
         <v>53425</v>
       </c>
       <c r="K333" t="n">
-        <v>1695568</v>
+        <v>1695569</v>
       </c>
       <c r="L333" t="n">
-        <v>1090534</v>
+        <v>1090535</v>
       </c>
       <c r="M333" t="n">
-        <v>356620</v>
+        <v>356633</v>
       </c>
       <c r="N333" t="n">
         <v>158559</v>
@@ -26931,7 +26931,7 @@
         <v>80956</v>
       </c>
       <c r="E334" t="n">
-        <v>11478</v>
+        <v>11465</v>
       </c>
       <c r="F334" t="n">
         <v>11739</v>
@@ -26949,13 +26949,13 @@
         <v>53646</v>
       </c>
       <c r="K334" t="n">
-        <v>1703360</v>
+        <v>1703361</v>
       </c>
       <c r="L334" t="n">
-        <v>1093890</v>
+        <v>1093891</v>
       </c>
       <c r="M334" t="n">
-        <v>266993</v>
+        <v>267007</v>
       </c>
       <c r="N334" t="n">
         <v>152595</v>
@@ -27011,7 +27011,7 @@
         <v>80978</v>
       </c>
       <c r="E335" t="n">
-        <v>16228</v>
+        <v>16215</v>
       </c>
       <c r="F335" t="n">
         <v>11959</v>
@@ -27029,13 +27029,13 @@
         <v>53822</v>
       </c>
       <c r="K335" t="n">
-        <v>1708288</v>
+        <v>1708289</v>
       </c>
       <c r="L335" t="n">
-        <v>1096102</v>
+        <v>1096103</v>
       </c>
       <c r="M335" t="n">
-        <v>290549</v>
+        <v>290563</v>
       </c>
       <c r="N335" t="n">
         <v>148785</v>
@@ -27091,7 +27091,7 @@
         <v>81284</v>
       </c>
       <c r="E336" t="n">
-        <v>15697</v>
+        <v>15683</v>
       </c>
       <c r="F336" t="n">
         <v>11981</v>
@@ -27109,13 +27109,13 @@
         <v>54120</v>
       </c>
       <c r="K336" t="n">
-        <v>1714307</v>
+        <v>1714308</v>
       </c>
       <c r="L336" t="n">
-        <v>1099846</v>
+        <v>1099847</v>
       </c>
       <c r="M336" t="n">
-        <v>371012</v>
+        <v>371027</v>
       </c>
       <c r="N336" t="n">
         <v>142275</v>
@@ -27171,7 +27171,7 @@
         <v>81549</v>
       </c>
       <c r="E337" t="n">
-        <v>15216</v>
+        <v>15201</v>
       </c>
       <c r="F337" t="n">
         <v>11475</v>
@@ -27189,13 +27189,13 @@
         <v>54413</v>
       </c>
       <c r="K337" t="n">
-        <v>1722132</v>
+        <v>1722133</v>
       </c>
       <c r="L337" t="n">
-        <v>1104461</v>
+        <v>1104462</v>
       </c>
       <c r="M337" t="n">
-        <v>398136</v>
+        <v>398152</v>
       </c>
       <c r="N337" t="n">
         <v>136874</v>
@@ -27251,7 +27251,7 @@
         <v>81788</v>
       </c>
       <c r="E338" t="n">
-        <v>14854</v>
+        <v>14837</v>
       </c>
       <c r="F338" t="n">
         <v>11004</v>
@@ -27269,13 +27269,13 @@
         <v>54678</v>
       </c>
       <c r="K338" t="n">
-        <v>1732135</v>
+        <v>1732136</v>
       </c>
       <c r="L338" t="n">
-        <v>1109169</v>
+        <v>1109170</v>
       </c>
       <c r="M338" t="n">
-        <v>404843</v>
+        <v>404861</v>
       </c>
       <c r="N338" t="n">
         <v>132566</v>
@@ -27331,7 +27331,7 @@
         <v>81907</v>
       </c>
       <c r="E339" t="n">
-        <v>14584</v>
+        <v>14563</v>
       </c>
       <c r="F339" t="n">
         <v>10673</v>
@@ -27349,13 +27349,13 @@
         <v>54934</v>
       </c>
       <c r="K339" t="n">
-        <v>1740900</v>
+        <v>1740901</v>
       </c>
       <c r="L339" t="n">
-        <v>1113238</v>
+        <v>1113239</v>
       </c>
       <c r="M339" t="n">
-        <v>411522</v>
+        <v>411544</v>
       </c>
       <c r="N339" t="n">
         <v>126566</v>
@@ -27411,7 +27411,7 @@
         <v>82183</v>
       </c>
       <c r="E340" t="n">
-        <v>10095</v>
+        <v>10074</v>
       </c>
       <c r="F340" t="n">
         <v>10174</v>
@@ -27429,13 +27429,13 @@
         <v>55141</v>
       </c>
       <c r="K340" t="n">
-        <v>1748956</v>
+        <v>1748957</v>
       </c>
       <c r="L340" t="n">
-        <v>1117086</v>
+        <v>1117087</v>
       </c>
       <c r="M340" t="n">
-        <v>397761</v>
+        <v>397783</v>
       </c>
       <c r="N340" t="n">
         <v>120856</v>
@@ -27491,7 +27491,7 @@
         <v>82200</v>
       </c>
       <c r="E341" t="n">
-        <v>9982</v>
+        <v>9958</v>
       </c>
       <c r="F341" t="n">
         <v>9881</v>
@@ -27509,13 +27509,13 @@
         <v>55296</v>
       </c>
       <c r="K341" t="n">
-        <v>1753957</v>
+        <v>1753958</v>
       </c>
       <c r="L341" t="n">
-        <v>1119127</v>
+        <v>1119128</v>
       </c>
       <c r="M341" t="n">
-        <v>298656</v>
+        <v>298681</v>
       </c>
       <c r="N341" t="n">
         <v>115083</v>
@@ -27571,7 +27571,7 @@
         <v>82214</v>
       </c>
       <c r="E342" t="n">
-        <v>9921</v>
+        <v>9897</v>
       </c>
       <c r="F342" t="n">
         <v>9964</v>
@@ -27589,13 +27589,13 @@
         <v>55439</v>
       </c>
       <c r="K342" t="n">
-        <v>1757335</v>
+        <v>1757336</v>
       </c>
       <c r="L342" t="n">
-        <v>1120555</v>
+        <v>1120556</v>
       </c>
       <c r="M342" t="n">
-        <v>303102</v>
+        <v>303127</v>
       </c>
       <c r="N342" t="n">
         <v>111962</v>
@@ -27651,7 +27651,7 @@
         <v>82229</v>
       </c>
       <c r="E343" t="n">
-        <v>9514</v>
+        <v>9487</v>
       </c>
       <c r="F343" t="n">
         <v>9949</v>
@@ -27669,13 +27669,13 @@
         <v>55750</v>
       </c>
       <c r="K343" t="n">
-        <v>1765338</v>
+        <v>1765339</v>
       </c>
       <c r="L343" t="n">
-        <v>1124650</v>
+        <v>1124651</v>
       </c>
       <c r="M343" t="n">
-        <v>414756</v>
+        <v>414784</v>
       </c>
       <c r="N343" t="n">
         <v>111946</v>
@@ -27731,7 +27731,7 @@
         <v>82241</v>
       </c>
       <c r="E344" t="n">
-        <v>13307</v>
+        <v>13280</v>
       </c>
       <c r="F344" t="n">
         <v>9483</v>
@@ -27749,13 +27749,13 @@
         <v>55897</v>
       </c>
       <c r="K344" t="n">
-        <v>1768587</v>
+        <v>1768588</v>
       </c>
       <c r="L344" t="n">
-        <v>1126198</v>
+        <v>1126199</v>
       </c>
       <c r="M344" t="n">
-        <v>334678</v>
+        <v>334706</v>
       </c>
       <c r="N344" t="n">
         <v>104098</v>
@@ -27811,7 +27811,7 @@
         <v>82456</v>
       </c>
       <c r="E345" t="n">
-        <v>12473</v>
+        <v>12446</v>
       </c>
       <c r="F345" t="n">
         <v>9373</v>
@@ -27829,13 +27829,13 @@
         <v>56135</v>
       </c>
       <c r="K345" t="n">
-        <v>1776741</v>
+        <v>1776742</v>
       </c>
       <c r="L345" t="n">
-        <v>1078416</v>
+        <v>1078417</v>
       </c>
       <c r="M345" t="n">
-        <v>353134</v>
+        <v>353162</v>
       </c>
       <c r="N345" t="n">
         <v>103014</v>
@@ -27891,7 +27891,7 @@
         <v>82645</v>
       </c>
       <c r="E346" t="n">
-        <v>13131</v>
+        <v>13104</v>
       </c>
       <c r="F346" t="n">
         <v>9178</v>
@@ -27909,13 +27909,13 @@
         <v>56356</v>
       </c>
       <c r="K346" t="n">
-        <v>1785774</v>
+        <v>1785775</v>
       </c>
       <c r="L346" t="n">
-        <v>1083361</v>
+        <v>1083362</v>
       </c>
       <c r="M346" t="n">
-        <v>457148</v>
+        <v>457176</v>
       </c>
       <c r="N346" t="n">
         <v>100271</v>
@@ -27971,7 +27971,7 @@
         <v>82867</v>
       </c>
       <c r="E347" t="n">
-        <v>8416</v>
+        <v>8387</v>
       </c>
       <c r="F347" t="n">
         <v>8855</v>
@@ -27989,13 +27989,13 @@
         <v>56564</v>
       </c>
       <c r="K347" t="n">
-        <v>1795710</v>
+        <v>1795711</v>
       </c>
       <c r="L347" t="n">
-        <v>1088998</v>
+        <v>1088999</v>
       </c>
       <c r="M347" t="n">
-        <v>443166</v>
+        <v>443196</v>
       </c>
       <c r="N347" t="n">
         <v>100142</v>
@@ -28051,7 +28051,7 @@
         <v>82902</v>
       </c>
       <c r="E348" t="n">
-        <v>8731</v>
+        <v>8702</v>
       </c>
       <c r="F348" t="n">
         <v>8715</v>
@@ -28069,13 +28069,13 @@
         <v>56704</v>
       </c>
       <c r="K348" t="n">
-        <v>1801173</v>
+        <v>1801174</v>
       </c>
       <c r="L348" t="n">
-        <v>1091536</v>
+        <v>1091537</v>
       </c>
       <c r="M348" t="n">
-        <v>335591</v>
+        <v>335621</v>
       </c>
       <c r="N348" t="n">
         <v>97813</v>
@@ -28131,7 +28131,7 @@
         <v>82934</v>
       </c>
       <c r="E349" t="n">
-        <v>13965</v>
+        <v>13936</v>
       </c>
       <c r="F349" t="n">
         <v>8969</v>
@@ -28149,13 +28149,13 @@
         <v>56809</v>
       </c>
       <c r="K349" t="n">
-        <v>1805461</v>
+        <v>1805462</v>
       </c>
       <c r="L349" t="n">
-        <v>1093265</v>
+        <v>1093266</v>
       </c>
       <c r="M349" t="n">
-        <v>361412</v>
+        <v>361442</v>
       </c>
       <c r="N349" t="n">
         <v>97173</v>
@@ -28211,7 +28211,7 @@
         <v>83133</v>
       </c>
       <c r="E350" t="n">
-        <v>13797</v>
+        <v>13765</v>
       </c>
       <c r="F350" t="n">
         <v>9116</v>
@@ -28229,13 +28229,13 @@
         <v>57118</v>
       </c>
       <c r="K350" t="n">
-        <v>1815831</v>
+        <v>1815832</v>
       </c>
       <c r="L350" t="n">
-        <v>1099364</v>
+        <v>1099365</v>
       </c>
       <c r="M350" t="n">
-        <v>483678</v>
+        <v>483711</v>
       </c>
       <c r="N350" t="n">
         <v>101524</v>
@@ -28291,7 +28291,7 @@
         <v>83827</v>
       </c>
       <c r="E351" t="n">
-        <v>13753</v>
+        <v>13718</v>
       </c>
       <c r="F351" t="n">
         <v>8940</v>
@@ -28309,13 +28309,13 @@
         <v>57319</v>
       </c>
       <c r="K351" t="n">
-        <v>1826624</v>
+        <v>1826625</v>
       </c>
       <c r="L351" t="n">
-        <v>1104853</v>
+        <v>1104854</v>
       </c>
       <c r="M351" t="n">
-        <v>491846</v>
+        <v>491882</v>
       </c>
       <c r="N351" t="n">
         <v>104492</v>
@@ -28371,7 +28371,7 @@
         <v>83468</v>
       </c>
       <c r="E352" t="n">
-        <v>13837</v>
+        <v>13796</v>
       </c>
       <c r="F352" t="n">
         <v>8856</v>
@@ -28389,13 +28389,13 @@
         <v>57493</v>
       </c>
       <c r="K352" t="n">
-        <v>1837316</v>
+        <v>1837317</v>
       </c>
       <c r="L352" t="n">
-        <v>1110695</v>
+        <v>1110696</v>
       </c>
       <c r="M352" t="n">
-        <v>499085</v>
+        <v>499127</v>
       </c>
       <c r="N352" t="n">
         <v>105181</v>
@@ -28451,7 +28451,7 @@
         <v>83643</v>
       </c>
       <c r="E353" t="n">
-        <v>13942</v>
+        <v>13897</v>
       </c>
       <c r="F353" t="n">
         <v>8709</v>
@@ -28469,13 +28469,13 @@
         <v>57656</v>
       </c>
       <c r="K353" t="n">
-        <v>1847757</v>
+        <v>1847758</v>
       </c>
       <c r="L353" t="n">
-        <v>1116176</v>
+        <v>1116177</v>
       </c>
       <c r="M353" t="n">
-        <v>506894</v>
+        <v>506940</v>
       </c>
       <c r="N353" t="n">
         <v>106857</v>
@@ -28531,7 +28531,7 @@
         <v>83780</v>
       </c>
       <c r="E354" t="n">
-        <v>8382</v>
+        <v>8327</v>
       </c>
       <c r="F354" t="n">
         <v>8492</v>
@@ -28549,13 +28549,13 @@
         <v>57846</v>
       </c>
       <c r="K354" t="n">
-        <v>1858354</v>
+        <v>1858355</v>
       </c>
       <c r="L354" t="n">
-        <v>1121663</v>
+        <v>1121664</v>
       </c>
       <c r="M354" t="n">
-        <v>490881</v>
+        <v>490937</v>
       </c>
       <c r="N354" t="n">
         <v>109398</v>
@@ -28611,7 +28611,7 @@
         <v>83791</v>
       </c>
       <c r="E355" t="n">
-        <v>8601</v>
+        <v>8538</v>
       </c>
       <c r="F355" t="n">
         <v>8466</v>
@@ -28629,13 +28629,13 @@
         <v>57996</v>
       </c>
       <c r="K355" t="n">
-        <v>1865786</v>
+        <v>1865787</v>
       </c>
       <c r="L355" t="n">
-        <v>1124152</v>
+        <v>1124153</v>
       </c>
       <c r="M355" t="n">
-        <v>370702</v>
+        <v>370766</v>
       </c>
       <c r="N355" t="n">
         <v>111829</v>
@@ -28691,7 +28691,7 @@
         <v>83799</v>
       </c>
       <c r="E356" t="n">
-        <v>15042</v>
+        <v>14966</v>
       </c>
       <c r="F356" t="n">
         <v>8684</v>
@@ -28709,13 +28709,13 @@
         <v>58125</v>
       </c>
       <c r="K356" t="n">
-        <v>1870157</v>
+        <v>1870158</v>
       </c>
       <c r="L356" t="n">
-        <v>1125988</v>
+        <v>1125989</v>
       </c>
       <c r="M356" t="n">
-        <v>400991</v>
+        <v>401068</v>
       </c>
       <c r="N356" t="n">
         <v>112822</v>
@@ -28771,7 +28771,7 @@
         <v>84050</v>
       </c>
       <c r="E357" t="n">
-        <v>14989</v>
+        <v>14888</v>
       </c>
       <c r="F357" t="n">
         <v>9011</v>
@@ -28789,13 +28789,13 @@
         <v>58390</v>
       </c>
       <c r="K357" t="n">
-        <v>1879467</v>
+        <v>1879468</v>
       </c>
       <c r="L357" t="n">
-        <v>1132663</v>
+        <v>1132664</v>
       </c>
       <c r="M357" t="n">
-        <v>529767</v>
+        <v>529869</v>
       </c>
       <c r="N357" t="n">
         <v>114129</v>
@@ -28851,7 +28851,7 @@
         <v>84237</v>
       </c>
       <c r="E358" t="n">
-        <v>15176</v>
+        <v>15062</v>
       </c>
       <c r="F358" t="n">
         <v>8884</v>
@@ -28869,13 +28869,13 @@
         <v>58574</v>
       </c>
       <c r="K358" t="n">
-        <v>1890129</v>
+        <v>1890130</v>
       </c>
       <c r="L358" t="n">
-        <v>1138534</v>
+        <v>1138535</v>
       </c>
       <c r="M358" t="n">
-        <v>537033</v>
+        <v>537148</v>
       </c>
       <c r="N358" t="n">
         <v>121542</v>
@@ -28931,7 +28931,7 @@
         <v>84439</v>
       </c>
       <c r="E359" t="n">
-        <v>8451</v>
+        <v>8332</v>
       </c>
       <c r="F359" t="n">
         <v>8528</v>
@@ -28949,13 +28949,13 @@
         <v>58749</v>
       </c>
       <c r="K359" t="n">
-        <v>1902989</v>
+        <v>1902990</v>
       </c>
       <c r="L359" t="n">
-        <v>1146302</v>
+        <v>1146303</v>
       </c>
       <c r="M359" t="n">
-        <v>518269</v>
+        <v>518389</v>
       </c>
       <c r="N359" t="n">
         <v>126248</v>
@@ -29011,7 +29011,7 @@
         <v>84449</v>
       </c>
       <c r="E360" t="n">
-        <v>8698</v>
+        <v>8578</v>
       </c>
       <c r="F360" t="n">
         <v>8369</v>
@@ -29029,13 +29029,13 @@
         <v>58862</v>
       </c>
       <c r="K360" t="n">
-        <v>1912726</v>
+        <v>1912727</v>
       </c>
       <c r="L360" t="n">
-        <v>1150521</v>
+        <v>1150522</v>
       </c>
       <c r="M360" t="n">
-        <v>396849</v>
+        <v>396970</v>
       </c>
       <c r="N360" t="n">
         <v>126952</v>
@@ -29091,7 +29091,7 @@
         <v>84455</v>
       </c>
       <c r="E361" t="n">
-        <v>8652</v>
+        <v>8529</v>
       </c>
       <c r="F361" t="n">
         <v>8405</v>
@@ -29109,13 +29109,13 @@
         <v>58961</v>
       </c>
       <c r="K361" t="n">
-        <v>1915753</v>
+        <v>1915754</v>
       </c>
       <c r="L361" t="n">
-        <v>1152681</v>
+        <v>1152682</v>
       </c>
       <c r="M361" t="n">
-        <v>172550</v>
+        <v>172674</v>
       </c>
       <c r="N361" t="n">
         <v>120043</v>
@@ -29171,7 +29171,7 @@
         <v>84474</v>
       </c>
       <c r="E362" t="n">
-        <v>8786</v>
+        <v>8662</v>
       </c>
       <c r="F362" t="n">
         <v>8772</v>
@@ -29189,13 +29189,13 @@
         <v>59093</v>
       </c>
       <c r="K362" t="n">
-        <v>1922457</v>
+        <v>1922458</v>
       </c>
       <c r="L362" t="n">
-        <v>1155304</v>
+        <v>1155305</v>
       </c>
       <c r="M362" t="n">
-        <v>400695</v>
+        <v>400820</v>
       </c>
       <c r="N362" t="n">
         <v>121284</v>
@@ -29251,7 +29251,7 @@
         <v>84485</v>
       </c>
       <c r="E363" t="n">
-        <v>15977</v>
+        <v>15852</v>
       </c>
       <c r="F363" t="n">
         <v>8965</v>
@@ -29269,13 +29269,13 @@
         <v>59197</v>
       </c>
       <c r="K363" t="n">
-        <v>1927228</v>
+        <v>1927229</v>
       </c>
       <c r="L363" t="n">
-        <v>1158019</v>
+        <v>1158020</v>
       </c>
       <c r="M363" t="n">
-        <v>429384</v>
+        <v>429510</v>
       </c>
       <c r="N363" t="n">
         <v>121767</v>
@@ -29331,7 +29331,7 @@
         <v>84643</v>
       </c>
       <c r="E364" t="n">
-        <v>16497</v>
+        <v>16366</v>
       </c>
       <c r="F364" t="n">
         <v>9332</v>
@@ -29349,13 +29349,13 @@
         <v>59533</v>
       </c>
       <c r="K364" t="n">
-        <v>1941267</v>
+        <v>1941268</v>
       </c>
       <c r="L364" t="n">
-        <v>1168847</v>
+        <v>1168848</v>
       </c>
       <c r="M364" t="n">
-        <v>562782</v>
+        <v>562914</v>
       </c>
       <c r="N364" t="n">
         <v>125436</v>
@@ -29411,7 +29411,7 @@
         <v>84813</v>
       </c>
       <c r="E365" t="n">
-        <v>16975</v>
+        <v>16843</v>
       </c>
       <c r="F365" t="n">
         <v>9356</v>
@@ -29429,13 +29429,13 @@
         <v>59755</v>
       </c>
       <c r="K365" t="n">
-        <v>1959409</v>
+        <v>1959410</v>
       </c>
       <c r="L365" t="n">
-        <v>1179153</v>
+        <v>1179154</v>
       </c>
       <c r="M365" t="n">
-        <v>567442</v>
+        <v>567575</v>
       </c>
       <c r="N365" t="n">
         <v>132785</v>
@@ -29491,7 +29491,7 @@
         <v>85021</v>
       </c>
       <c r="E366" t="n">
-        <v>9952</v>
+        <v>9816</v>
       </c>
       <c r="F366" t="n">
         <v>9130</v>
@@ -29509,13 +29509,13 @@
         <v>59970</v>
       </c>
       <c r="K366" t="n">
-        <v>1977063</v>
+        <v>1977064</v>
       </c>
       <c r="L366" t="n">
-        <v>1190528</v>
+        <v>1190529</v>
       </c>
       <c r="M366" t="n">
-        <v>544917</v>
+        <v>545054</v>
       </c>
       <c r="N366" t="n">
         <v>139747</v>
@@ -29571,7 +29571,7 @@
         <v>85023</v>
       </c>
       <c r="E367" t="n">
-        <v>10376</v>
+        <v>10238</v>
       </c>
       <c r="F367" t="n">
         <v>8971</v>
@@ -29589,13 +29589,13 @@
         <v>60087</v>
       </c>
       <c r="K367" t="n">
-        <v>1988932</v>
+        <v>1988933</v>
       </c>
       <c r="L367" t="n">
-        <v>1196876</v>
+        <v>1196877</v>
       </c>
       <c r="M367" t="n">
-        <v>411882</v>
+        <v>412021</v>
       </c>
       <c r="N367" t="n">
         <v>141175</v>
@@ -29651,7 +29651,7 @@
         <v>85055</v>
       </c>
       <c r="E368" t="n">
-        <v>10431</v>
+        <v>10293</v>
       </c>
       <c r="F368" t="n">
         <v>9142</v>
@@ -29669,13 +29669,13 @@
         <v>60197</v>
       </c>
       <c r="K368" t="n">
-        <v>1994638</v>
+        <v>1994639</v>
       </c>
       <c r="L368" t="n">
-        <v>1200298</v>
+        <v>1200299</v>
       </c>
       <c r="M368" t="n">
-        <v>413818</v>
+        <v>413957</v>
       </c>
       <c r="N368" t="n">
         <v>136284</v>
@@ -29731,7 +29731,7 @@
         <v>85072</v>
       </c>
       <c r="E369" t="n">
-        <v>9760</v>
+        <v>9622</v>
       </c>
       <c r="F369" t="n">
         <v>9669</v>
@@ -29749,13 +29749,13 @@
         <v>60307</v>
       </c>
       <c r="K369" t="n">
-        <v>2004325</v>
+        <v>2004326</v>
       </c>
       <c r="L369" t="n">
-        <v>1204534</v>
+        <v>1204535</v>
       </c>
       <c r="M369" t="n">
-        <v>412912</v>
+        <v>413051</v>
       </c>
       <c r="N369" t="n">
         <v>138539</v>
@@ -29811,7 +29811,7 @@
         <v>85085</v>
       </c>
       <c r="E370" t="n">
-        <v>19859</v>
+        <v>19721</v>
       </c>
       <c r="F370" t="n">
         <v>10100</v>
@@ -29829,13 +29829,13 @@
         <v>60385</v>
       </c>
       <c r="K370" t="n">
-        <v>2012314</v>
+        <v>2012315</v>
       </c>
       <c r="L370" t="n">
-        <v>1208633</v>
+        <v>1208634</v>
       </c>
       <c r="M370" t="n">
-        <v>444091</v>
+        <v>444230</v>
       </c>
       <c r="N370" t="n">
         <v>142157</v>
@@ -29891,7 +29891,7 @@
         <v>85296</v>
       </c>
       <c r="E371" t="n">
-        <v>19001</v>
+        <v>18862</v>
       </c>
       <c r="F371" t="n">
         <v>10678</v>
@@ -29909,13 +29909,13 @@
         <v>60707</v>
       </c>
       <c r="K371" t="n">
-        <v>2032715</v>
+        <v>2032716</v>
       </c>
       <c r="L371" t="n">
-        <v>1223493</v>
+        <v>1223494</v>
       </c>
       <c r="M371" t="n">
-        <v>589442</v>
+        <v>589582</v>
       </c>
       <c r="N371" t="n">
         <v>153248</v>
@@ -29971,7 +29971,7 @@
         <v>85519</v>
       </c>
       <c r="E372" t="n">
-        <v>11789</v>
+        <v>11647</v>
       </c>
       <c r="F372" t="n">
         <v>10699</v>
@@ -29989,13 +29989,13 @@
         <v>60981</v>
       </c>
       <c r="K372" t="n">
-        <v>2056808</v>
+        <v>2056809</v>
       </c>
       <c r="L372" t="n">
-        <v>1239145</v>
+        <v>1239146</v>
       </c>
       <c r="M372" t="n">
-        <v>563508</v>
+        <v>563651</v>
       </c>
       <c r="N372" t="n">
         <v>166679</v>
@@ -30051,7 +30051,7 @@
         <v>85533</v>
       </c>
       <c r="E373" t="n">
-        <v>20823</v>
+        <v>20680</v>
       </c>
       <c r="F373" t="n">
         <v>11006</v>
@@ -30069,13 +30069,13 @@
         <v>61164</v>
       </c>
       <c r="K373" t="n">
-        <v>2069544</v>
+        <v>2069545</v>
       </c>
       <c r="L373" t="n">
-        <v>1246285</v>
+        <v>1246286</v>
       </c>
       <c r="M373" t="n">
-        <v>449531</v>
+        <v>449675</v>
       </c>
       <c r="N373" t="n">
         <v>166555</v>
@@ -30131,7 +30131,7 @@
         <v>85777</v>
       </c>
       <c r="E374" t="n">
-        <v>21185</v>
+        <v>21041</v>
       </c>
       <c r="F374" t="n">
         <v>11597</v>
@@ -30149,13 +30149,13 @@
         <v>61376</v>
       </c>
       <c r="K374" t="n">
-        <v>2093418</v>
+        <v>2093419</v>
       </c>
       <c r="L374" t="n">
-        <v>1260120</v>
+        <v>1260121</v>
       </c>
       <c r="M374" t="n">
-        <v>600558</v>
+        <v>600703</v>
       </c>
       <c r="N374" t="n">
         <v>180692</v>
@@ -30211,7 +30211,7 @@
         <v>86036</v>
       </c>
       <c r="E375" t="n">
-        <v>13612</v>
+        <v>13468</v>
       </c>
       <c r="F375" t="n">
         <v>12005</v>
@@ -30229,13 +30229,13 @@
         <v>61644</v>
       </c>
       <c r="K375" t="n">
-        <v>2119167</v>
+        <v>2119168</v>
       </c>
       <c r="L375" t="n">
-        <v>1275609</v>
+        <v>1275610</v>
       </c>
       <c r="M375" t="n">
-        <v>571983</v>
+        <v>572128</v>
       </c>
       <c r="N375" t="n">
         <v>203414</v>
@@ -30291,7 +30291,7 @@
         <v>86049</v>
       </c>
       <c r="E376" t="n">
-        <v>14393</v>
+        <v>14249</v>
       </c>
       <c r="F376" t="n">
         <v>12264</v>
@@ -30309,13 +30309,13 @@
         <v>61847</v>
       </c>
       <c r="K376" t="n">
-        <v>2138519</v>
+        <v>2138520</v>
       </c>
       <c r="L376" t="n">
-        <v>1281579</v>
+        <v>1281580</v>
       </c>
       <c r="M376" t="n">
-        <v>422204</v>
+        <v>422349</v>
       </c>
       <c r="N376" t="n">
         <v>216062</v>
@@ -30362,16 +30362,16 @@
         <v>44206</v>
       </c>
       <c r="B377" t="n">
-        <v>5237</v>
+        <v>5238</v>
       </c>
       <c r="C377" t="n">
-        <v>1816</v>
+        <v>1817</v>
       </c>
       <c r="D377" t="n">
         <v>86076</v>
       </c>
       <c r="E377" t="n">
-        <v>23965</v>
+        <v>23822</v>
       </c>
       <c r="F377" t="n">
         <v>12678</v>
@@ -30389,37 +30389,37 @@
         <v>61997</v>
       </c>
       <c r="K377" t="n">
-        <v>2149017</v>
+        <v>2149019</v>
       </c>
       <c r="L377" t="n">
-        <v>1286269</v>
+        <v>1286271</v>
       </c>
       <c r="M377" t="n">
-        <v>454958</v>
+        <v>455103</v>
       </c>
       <c r="N377" t="n">
-        <v>221789</v>
+        <v>221790</v>
       </c>
       <c r="O377" t="n">
-        <v>136703</v>
+        <v>136704</v>
       </c>
       <c r="P377" t="n">
-        <v>128250</v>
+        <v>128251</v>
       </c>
       <c r="Q377" t="n">
-        <v>77636</v>
+        <v>77637</v>
       </c>
       <c r="R377" t="n">
-        <v>10498</v>
+        <v>10499</v>
       </c>
       <c r="S377" t="n">
-        <v>19529</v>
+        <v>19529.1</v>
       </c>
       <c r="T377" t="n">
-        <v>4690</v>
+        <v>4691</v>
       </c>
       <c r="U377" t="n">
-        <v>11090.9</v>
+        <v>11091</v>
       </c>
       <c r="V377" t="n">
         <v>150</v>
@@ -30451,7 +30451,7 @@
         <v>86381</v>
       </c>
       <c r="E378" t="n">
-        <v>24453</v>
+        <v>24308</v>
       </c>
       <c r="F378" t="n">
         <v>13695</v>
@@ -30469,37 +30469,37 @@
         <v>62338</v>
       </c>
       <c r="K378" t="n">
-        <v>2178498</v>
+        <v>2178500</v>
       </c>
       <c r="L378" t="n">
-        <v>1304060</v>
+        <v>1304062</v>
       </c>
       <c r="M378" t="n">
-        <v>611397</v>
+        <v>611544</v>
       </c>
       <c r="N378" t="n">
-        <v>237231</v>
+        <v>237232</v>
       </c>
       <c r="O378" t="n">
-        <v>145783</v>
+        <v>145784</v>
       </c>
       <c r="P378" t="n">
-        <v>135213</v>
+        <v>135214</v>
       </c>
       <c r="Q378" t="n">
-        <v>80567</v>
+        <v>80568</v>
       </c>
       <c r="R378" t="n">
         <v>29481</v>
       </c>
       <c r="S378" t="n">
-        <v>20826.1</v>
+        <v>20826.3</v>
       </c>
       <c r="T378" t="n">
         <v>17791</v>
       </c>
       <c r="U378" t="n">
-        <v>11509.6</v>
+        <v>11509.7</v>
       </c>
       <c r="V378" t="n">
         <v>341</v>
@@ -30531,7 +30531,7 @@
         <v>86610</v>
       </c>
       <c r="E379" t="n">
-        <v>25731</v>
+        <v>25585</v>
       </c>
       <c r="F379" t="n">
         <v>14239</v>
@@ -30549,37 +30549,37 @@
         <v>62652</v>
       </c>
       <c r="K379" t="n">
-        <v>2205762</v>
+        <v>2205764</v>
       </c>
       <c r="L379" t="n">
-        <v>1318799</v>
+        <v>1318801</v>
       </c>
       <c r="M379" t="n">
-        <v>615341</v>
+        <v>615489</v>
       </c>
       <c r="N379" t="n">
-        <v>246353</v>
+        <v>246354</v>
       </c>
       <c r="O379" t="n">
-        <v>148954</v>
+        <v>148955</v>
       </c>
       <c r="P379" t="n">
-        <v>139646</v>
+        <v>139647</v>
       </c>
       <c r="Q379" t="n">
-        <v>79654</v>
+        <v>79655</v>
       </c>
       <c r="R379" t="n">
         <v>27264</v>
       </c>
       <c r="S379" t="n">
-        <v>21279.1</v>
+        <v>21279.3</v>
       </c>
       <c r="T379" t="n">
         <v>14739</v>
       </c>
       <c r="U379" t="n">
-        <v>11379.1</v>
+        <v>11379.3</v>
       </c>
       <c r="V379" t="n">
         <v>314</v>
@@ -30611,7 +30611,7 @@
         <v>86835</v>
       </c>
       <c r="E380" t="n">
-        <v>27306</v>
+        <v>27158</v>
       </c>
       <c r="F380" t="n">
         <v>14736</v>
@@ -30629,37 +30629,37 @@
         <v>62912</v>
       </c>
       <c r="K380" t="n">
-        <v>2238130</v>
+        <v>2238132</v>
       </c>
       <c r="L380" t="n">
-        <v>1335561</v>
+        <v>1335563</v>
       </c>
       <c r="M380" t="n">
-        <v>620389</v>
+        <v>620539</v>
       </c>
       <c r="N380" t="n">
-        <v>261067</v>
+        <v>261068</v>
       </c>
       <c r="O380" t="n">
-        <v>168586</v>
+        <v>168587</v>
       </c>
       <c r="P380" t="n">
-        <v>145033</v>
+        <v>145034</v>
       </c>
       <c r="Q380" t="n">
-        <v>89276</v>
+        <v>89277</v>
       </c>
       <c r="R380" t="n">
         <v>32368</v>
       </c>
       <c r="S380" t="n">
-        <v>24083.7</v>
+        <v>24083.9</v>
       </c>
       <c r="T380" t="n">
         <v>16762</v>
       </c>
       <c r="U380" t="n">
-        <v>12753.7</v>
+        <v>12753.9</v>
       </c>
       <c r="V380" t="n">
         <v>260</v>
@@ -30691,7 +30691,7 @@
         <v>87140</v>
       </c>
       <c r="E381" t="n">
-        <v>28772</v>
+        <v>28624</v>
       </c>
       <c r="F381" t="n">
         <v>15413</v>
@@ -30709,37 +30709,37 @@
         <v>63180</v>
       </c>
       <c r="K381" t="n">
-        <v>2272663</v>
+        <v>2272665</v>
       </c>
       <c r="L381" t="n">
-        <v>1352808</v>
+        <v>1352810</v>
       </c>
       <c r="M381" t="n">
-        <v>625372</v>
+        <v>625522</v>
       </c>
       <c r="N381" t="n">
-        <v>283731</v>
+        <v>283732</v>
       </c>
       <c r="O381" t="n">
-        <v>179245</v>
+        <v>179246</v>
       </c>
       <c r="P381" t="n">
-        <v>155932</v>
+        <v>155933</v>
       </c>
       <c r="Q381" t="n">
-        <v>92688</v>
+        <v>92689</v>
       </c>
       <c r="R381" t="n">
         <v>34533</v>
       </c>
       <c r="S381" t="n">
-        <v>25606.4</v>
+        <v>25606.6</v>
       </c>
       <c r="T381" t="n">
         <v>17247</v>
       </c>
       <c r="U381" t="n">
-        <v>13241.1</v>
+        <v>13241.3</v>
       </c>
       <c r="V381" t="n">
         <v>268</v>
@@ -30771,7 +30771,7 @@
         <v>87337</v>
       </c>
       <c r="E382" t="n">
-        <v>19590</v>
+        <v>19439</v>
       </c>
       <c r="F382" t="n">
         <v>15862</v>
@@ -30789,37 +30789,37 @@
         <v>63444</v>
       </c>
       <c r="K382" t="n">
-        <v>2310043</v>
+        <v>2310045</v>
       </c>
       <c r="L382" t="n">
-        <v>1370969</v>
+        <v>1370971</v>
       </c>
       <c r="M382" t="n">
-        <v>595857</v>
+        <v>596010</v>
       </c>
       <c r="N382" t="n">
-        <v>315405</v>
+        <v>315406</v>
       </c>
       <c r="O382" t="n">
-        <v>190876</v>
+        <v>190877</v>
       </c>
       <c r="P382" t="n">
-        <v>170671</v>
+        <v>170672</v>
       </c>
       <c r="Q382" t="n">
-        <v>95360</v>
+        <v>95361</v>
       </c>
       <c r="R382" t="n">
         <v>37380</v>
       </c>
       <c r="S382" t="n">
-        <v>27268</v>
+        <v>27268.1</v>
       </c>
       <c r="T382" t="n">
         <v>18161</v>
       </c>
       <c r="U382" t="n">
-        <v>13622.9</v>
+        <v>13623</v>
       </c>
       <c r="V382" t="n">
         <v>264</v>
@@ -30842,16 +30842,16 @@
         <v>44212</v>
       </c>
       <c r="B383" t="n">
-        <v>15145</v>
+        <v>15146</v>
       </c>
       <c r="C383" t="n">
-        <v>2571</v>
+        <v>2572</v>
       </c>
       <c r="D383" t="n">
         <v>87366</v>
       </c>
       <c r="E383" t="n">
-        <v>20638</v>
+        <v>20488</v>
       </c>
       <c r="F383" t="n">
         <v>16878</v>
@@ -30869,37 +30869,37 @@
         <v>63663</v>
       </c>
       <c r="K383" t="n">
-        <v>2337174</v>
+        <v>2337177</v>
       </c>
       <c r="L383" t="n">
-        <v>1379156</v>
+        <v>1379159</v>
       </c>
       <c r="M383" t="n">
-        <v>431822</v>
+        <v>431975</v>
       </c>
       <c r="N383" t="n">
-        <v>332849</v>
+        <v>332851</v>
       </c>
       <c r="O383" t="n">
-        <v>198655</v>
+        <v>198657</v>
       </c>
       <c r="P383" t="n">
-        <v>174622</v>
+        <v>174624</v>
       </c>
       <c r="Q383" t="n">
-        <v>97577</v>
+        <v>97579</v>
       </c>
       <c r="R383" t="n">
-        <v>27131</v>
+        <v>27132</v>
       </c>
       <c r="S383" t="n">
-        <v>28379.3</v>
+        <v>28379.6</v>
       </c>
       <c r="T383" t="n">
-        <v>8187</v>
+        <v>8188</v>
       </c>
       <c r="U383" t="n">
-        <v>13939.6</v>
+        <v>13939.9</v>
       </c>
       <c r="V383" t="n">
         <v>219</v>
@@ -30931,7 +30931,7 @@
         <v>87402</v>
       </c>
       <c r="E384" t="n">
-        <v>31093</v>
+        <v>30943</v>
       </c>
       <c r="F384" t="n">
         <v>18141</v>
@@ -30949,37 +30949,37 @@
         <v>63882</v>
       </c>
       <c r="K384" t="n">
-        <v>2355547</v>
+        <v>2355550</v>
       </c>
       <c r="L384" t="n">
-        <v>1385061</v>
+        <v>1385064</v>
       </c>
       <c r="M384" t="n">
-        <v>468456</v>
+        <v>468609</v>
       </c>
       <c r="N384" t="n">
-        <v>343233</v>
+        <v>343235</v>
       </c>
       <c r="O384" t="n">
-        <v>206530</v>
+        <v>206531</v>
       </c>
       <c r="P384" t="n">
-        <v>176428</v>
+        <v>176430</v>
       </c>
       <c r="Q384" t="n">
-        <v>98792</v>
+        <v>98793</v>
       </c>
       <c r="R384" t="n">
         <v>18373</v>
       </c>
       <c r="S384" t="n">
-        <v>29504.3</v>
+        <v>29504.4</v>
       </c>
       <c r="T384" t="n">
         <v>5905</v>
       </c>
       <c r="U384" t="n">
-        <v>14113.1</v>
+        <v>14113.3</v>
       </c>
       <c r="V384" t="n">
         <v>219</v>
@@ -31002,16 +31002,16 @@
         <v>44214</v>
       </c>
       <c r="B385" t="n">
-        <v>8871</v>
+        <v>8874</v>
       </c>
       <c r="C385" t="n">
-        <v>10184</v>
+        <v>10187</v>
       </c>
       <c r="D385" t="n">
         <v>87722</v>
       </c>
       <c r="E385" t="n">
-        <v>31410</v>
+        <v>31260</v>
       </c>
       <c r="F385" t="n">
         <v>19443</v>
@@ -31029,37 +31029,37 @@
         <v>64291</v>
       </c>
       <c r="K385" t="n">
-        <v>2388775</v>
+        <v>2388781</v>
       </c>
       <c r="L385" t="n">
-        <v>1406520</v>
+        <v>1406526</v>
       </c>
       <c r="M385" t="n">
-        <v>643473</v>
+        <v>643629</v>
       </c>
       <c r="N385" t="n">
-        <v>356060</v>
+        <v>356065</v>
       </c>
       <c r="O385" t="n">
-        <v>210277</v>
+        <v>210281</v>
       </c>
       <c r="P385" t="n">
-        <v>183027</v>
+        <v>183032</v>
       </c>
       <c r="Q385" t="n">
-        <v>102460</v>
+        <v>102464</v>
       </c>
       <c r="R385" t="n">
-        <v>33228</v>
+        <v>33231</v>
       </c>
       <c r="S385" t="n">
-        <v>30039.6</v>
+        <v>30040.1</v>
       </c>
       <c r="T385" t="n">
-        <v>21459</v>
+        <v>21462</v>
       </c>
       <c r="U385" t="n">
-        <v>14637.1</v>
+        <v>14637.7</v>
       </c>
       <c r="V385" t="n">
         <v>409</v>
@@ -31082,16 +31082,16 @@
         <v>44215</v>
       </c>
       <c r="B386" t="n">
-        <v>15982</v>
+        <v>15984</v>
       </c>
       <c r="C386" t="n">
-        <v>5225</v>
+        <v>5227</v>
       </c>
       <c r="D386" t="n">
         <v>88034</v>
       </c>
       <c r="E386" t="n">
-        <v>22308</v>
+        <v>22150</v>
       </c>
       <c r="F386" t="n">
         <v>20431</v>
@@ -31109,37 +31109,37 @@
         <v>64708</v>
       </c>
       <c r="K386" t="n">
-        <v>2423740</v>
+        <v>2423748</v>
       </c>
       <c r="L386" t="n">
-        <v>1424463</v>
+        <v>1424471</v>
       </c>
       <c r="M386" t="n">
-        <v>615526</v>
+        <v>615692</v>
       </c>
       <c r="N386" t="n">
-        <v>366932</v>
+        <v>366939</v>
       </c>
       <c r="O386" t="n">
-        <v>217978</v>
+        <v>217984</v>
       </c>
       <c r="P386" t="n">
-        <v>185318</v>
+        <v>185325</v>
       </c>
       <c r="Q386" t="n">
-        <v>105664</v>
+        <v>105670</v>
       </c>
       <c r="R386" t="n">
-        <v>34965</v>
+        <v>34967</v>
       </c>
       <c r="S386" t="n">
-        <v>31139.7</v>
+        <v>31140.6</v>
       </c>
       <c r="T386" t="n">
-        <v>17943</v>
+        <v>17945</v>
       </c>
       <c r="U386" t="n">
-        <v>15094.9</v>
+        <v>15095.7</v>
       </c>
       <c r="V386" t="n">
         <v>417</v>
@@ -31162,16 +31162,16 @@
         <v>44216</v>
       </c>
       <c r="B387" t="n">
-        <v>18338</v>
+        <v>18350</v>
       </c>
       <c r="C387" t="n">
-        <v>5384</v>
+        <v>5396</v>
       </c>
       <c r="D387" t="n">
         <v>88431</v>
       </c>
       <c r="E387" t="n">
-        <v>32966</v>
+        <v>32817</v>
       </c>
       <c r="F387" t="n">
         <v>21085</v>
@@ -31189,37 +31189,37 @@
         <v>65119</v>
       </c>
       <c r="K387" t="n">
-        <v>2462824</v>
+        <v>2462844</v>
       </c>
       <c r="L387" t="n">
-        <v>1441217</v>
+        <v>1441237</v>
       </c>
       <c r="M387" t="n">
-        <v>657696</v>
+        <v>657865</v>
       </c>
       <c r="N387" t="n">
-        <v>393280</v>
+        <v>393299</v>
       </c>
       <c r="O387" t="n">
-        <v>224694</v>
+        <v>224712</v>
       </c>
       <c r="P387" t="n">
-        <v>194932</v>
+        <v>194951</v>
       </c>
       <c r="Q387" t="n">
-        <v>105656</v>
+        <v>105674</v>
       </c>
       <c r="R387" t="n">
-        <v>39084</v>
+        <v>39096</v>
       </c>
       <c r="S387" t="n">
-        <v>32099.1</v>
+        <v>32101.7</v>
       </c>
       <c r="T387" t="n">
-        <v>16754</v>
+        <v>16766</v>
       </c>
       <c r="U387" t="n">
-        <v>15093.7</v>
+        <v>15096.3</v>
       </c>
       <c r="V387" t="n">
         <v>411</v>
@@ -31242,79 +31242,79 @@
         <v>44217</v>
       </c>
       <c r="B388" t="n">
-        <v>15106</v>
+        <v>16165</v>
       </c>
       <c r="C388" t="n">
-        <v>4115</v>
+        <v>4427</v>
       </c>
       <c r="D388" t="n">
         <v>88723</v>
       </c>
       <c r="E388" t="n">
-        <v>3875</v>
+        <v>23892</v>
       </c>
       <c r="F388" t="n">
-        <v>21953</v>
+        <v>21952</v>
       </c>
       <c r="G388" t="n">
-        <v>579</v>
+        <v>10090</v>
       </c>
       <c r="H388" t="n">
-        <v>87755</v>
+        <v>97266</v>
       </c>
       <c r="I388" t="n">
-        <v>3129</v>
+        <v>3258</v>
       </c>
       <c r="J388" t="n">
-        <v>65453</v>
+        <v>65471</v>
       </c>
       <c r="K388" t="n">
-        <v>2497227</v>
+        <v>2498306</v>
       </c>
       <c r="L388" t="n">
-        <v>1455269</v>
+        <v>1455601</v>
       </c>
       <c r="M388" t="n">
-        <v>527248</v>
+        <v>628749</v>
       </c>
       <c r="N388" t="n">
-        <v>403809</v>
+        <v>404887</v>
       </c>
       <c r="O388" t="n">
-        <v>224564</v>
+        <v>225641</v>
       </c>
       <c r="P388" t="n">
-        <v>195149</v>
+        <v>195480</v>
       </c>
       <c r="Q388" t="n">
-        <v>102461</v>
+        <v>102791</v>
       </c>
       <c r="R388" t="n">
-        <v>34403</v>
+        <v>35462</v>
       </c>
       <c r="S388" t="n">
-        <v>32080.6</v>
+        <v>32234.4</v>
       </c>
       <c r="T388" t="n">
-        <v>14052</v>
+        <v>14364</v>
       </c>
       <c r="U388" t="n">
-        <v>14637.3</v>
+        <v>14684.4</v>
       </c>
       <c r="V388" t="n">
-        <v>334</v>
+        <v>352</v>
       </c>
       <c r="W388" t="n">
         <v>0.5</v>
       </c>
       <c r="X388" t="n">
-        <v>387.3</v>
+        <v>393.3</v>
       </c>
       <c r="Y388" t="n">
-        <v>324.7</v>
+        <v>327.3</v>
       </c>
       <c r="Z388" t="n">
-        <v>2273</v>
+        <v>2291</v>
       </c>
     </row>
     <row r="389">
@@ -31322,7 +31322,7 @@
         <v>44218</v>
       </c>
       <c r="B389" t="n">
-        <v>2929</v>
+        <v>11556</v>
       </c>
       <c r="C389" t="n">
         <v>691</v>
@@ -31334,7 +31334,7 @@
         <v>3255</v>
       </c>
       <c r="F389" t="n">
-        <v>5460</v>
+        <v>9058</v>
       </c>
       <c r="G389" t="n">
         <v>2</v>
@@ -31343,58 +31343,58 @@
         <v>27</v>
       </c>
       <c r="I389" t="n">
-        <v>383</v>
+        <v>960</v>
       </c>
       <c r="J389" t="n">
-        <v>11495</v>
+        <v>15532</v>
       </c>
       <c r="K389" t="n">
-        <v>598264</v>
+        <v>843120</v>
       </c>
       <c r="L389" t="n">
         <v>198634</v>
       </c>
       <c r="M389" t="n">
-        <v>269486</v>
+        <v>460372</v>
       </c>
       <c r="N389" t="n">
-        <v>-1520903</v>
+        <v>-1276048</v>
       </c>
       <c r="O389" t="n">
-        <v>-1711779</v>
+        <v>-1466925</v>
       </c>
       <c r="P389" t="n">
-        <v>-1076975</v>
+        <v>-1076976</v>
       </c>
       <c r="Q389" t="n">
-        <v>-1172335</v>
+        <v>-1172337</v>
       </c>
       <c r="R389" t="n">
-        <v>-1898963</v>
+        <v>-1655186</v>
       </c>
       <c r="S389" t="n">
-        <v>-244539.9</v>
+        <v>-209560.7</v>
       </c>
       <c r="T389" t="n">
-        <v>-1256635</v>
+        <v>-1256967</v>
       </c>
       <c r="U389" t="n">
-        <v>-167476.4</v>
+        <v>-167476.7</v>
       </c>
       <c r="V389" t="n">
-        <v>-53958</v>
+        <v>-49939</v>
       </c>
       <c r="W389" t="n">
-        <v>-82.4</v>
+        <v>-76.3</v>
       </c>
       <c r="X389" t="n">
-        <v>-17737.7</v>
+        <v>-16392</v>
       </c>
       <c r="Y389" t="n">
-        <v>-7421.3</v>
+        <v>-6844.6</v>
       </c>
       <c r="Z389" t="n">
-        <v>-51949</v>
+        <v>-47912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrige datos gráficos provincias 2021-09-15
</commit_message>
<xml_diff>
--- a/data/output/covid19-spain_consolidated.xlsx
+++ b/data/output/covid19-spain_consolidated.xlsx
@@ -50294,7 +50294,7 @@
         <v>191</v>
       </c>
       <c r="F626" t="n">
-        <v>1285</v>
+        <v>3260</v>
       </c>
       <c r="G626" t="n">
         <v>0</v>
@@ -50306,55 +50306,55 @@
         <v>251</v>
       </c>
       <c r="J626" t="n">
-        <v>43889</v>
+        <v>99686</v>
       </c>
       <c r="K626" t="n">
-        <v>2245849</v>
+        <v>4941266</v>
       </c>
       <c r="L626" t="n">
-        <v>539805</v>
+        <v>2722533</v>
       </c>
       <c r="M626" t="n">
         <v>0</v>
       </c>
       <c r="N626" t="n">
-        <v>-2650479</v>
+        <v>44938</v>
       </c>
       <c r="O626" t="n">
-        <v>-2678456</v>
+        <v>16961</v>
       </c>
       <c r="P626" t="n">
-        <v>-2161299</v>
+        <v>21429</v>
       </c>
       <c r="Q626" t="n">
-        <v>-2174757</v>
+        <v>7971</v>
       </c>
       <c r="R626" t="n">
-        <v>-2694005</v>
+        <v>1412</v>
       </c>
       <c r="S626" t="n">
-        <v>-382636.6</v>
+        <v>2423</v>
       </c>
       <c r="T626" t="n">
-        <v>-2182462</v>
+        <v>266</v>
       </c>
       <c r="U626" t="n">
-        <v>-310679.6</v>
+        <v>1138.7</v>
       </c>
       <c r="V626" t="n">
-        <v>-55771</v>
+        <v>26</v>
       </c>
       <c r="W626" t="n">
-        <v>-56</v>
+        <v>0</v>
       </c>
       <c r="X626" t="n">
-        <v>-18539</v>
+        <v>60</v>
       </c>
       <c r="Y626" t="n">
-        <v>-7921.3</v>
+        <v>49.7</v>
       </c>
       <c r="Z626" t="n">
-        <v>-55449</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualiza datos provincias 2021-12-05
</commit_message>
<xml_diff>
--- a/data/output/covid19-spain_consolidated.xlsx
+++ b/data/output/covid19-spain_consolidated.xlsx
@@ -12786,7 +12786,7 @@
         <v>409</v>
       </c>
       <c r="J157" t="n">
-        <v>34904</v>
+        <v>36358</v>
       </c>
       <c r="K157" t="n">
         <v>289029</v>
@@ -12822,19 +12822,19 @@
         <v>1029.7</v>
       </c>
       <c r="V157" t="n">
-        <v>-1067</v>
+        <v>387</v>
       </c>
       <c r="W157" t="n">
-        <v>-3</v>
+        <v>1.1</v>
       </c>
       <c r="X157" t="n">
-        <v>-323</v>
+        <v>161.7</v>
       </c>
       <c r="Y157" t="n">
-        <v>-83.6</v>
+        <v>124.1</v>
       </c>
       <c r="Z157" t="n">
-        <v>-585</v>
+        <v>869</v>
       </c>
     </row>
     <row r="158">
@@ -12866,7 +12866,7 @@
         <v>401</v>
       </c>
       <c r="J158" t="n">
-        <v>34945</v>
+        <v>36399</v>
       </c>
       <c r="K158" t="n">
         <v>290205</v>
@@ -12908,13 +12908,13 @@
         <v>0.1</v>
       </c>
       <c r="X158" t="n">
-        <v>-316.7</v>
+        <v>168</v>
       </c>
       <c r="Y158" t="n">
-        <v>-110.3</v>
+        <v>97.4</v>
       </c>
       <c r="Z158" t="n">
-        <v>-772</v>
+        <v>682</v>
       </c>
     </row>
     <row r="159">
@@ -12946,7 +12946,7 @@
         <v>392</v>
       </c>
       <c r="J159" t="n">
-        <v>34980</v>
+        <v>36434</v>
       </c>
       <c r="K159" t="n">
         <v>290737</v>
@@ -12988,13 +12988,13 @@
         <v>0.1</v>
       </c>
       <c r="X159" t="n">
-        <v>-330.3</v>
+        <v>154.3</v>
       </c>
       <c r="Y159" t="n">
-        <v>-116.3</v>
+        <v>91.4</v>
       </c>
       <c r="Z159" t="n">
-        <v>-814</v>
+        <v>640</v>
       </c>
     </row>
     <row r="160">
@@ -13026,7 +13026,7 @@
         <v>402</v>
       </c>
       <c r="J160" t="n">
-        <v>35012</v>
+        <v>36466</v>
       </c>
       <c r="K160" t="n">
         <v>291557</v>
@@ -13071,10 +13071,10 @@
         <v>36</v>
       </c>
       <c r="Y160" t="n">
-        <v>-117.9</v>
+        <v>89.9</v>
       </c>
       <c r="Z160" t="n">
-        <v>-825</v>
+        <v>629</v>
       </c>
     </row>
     <row r="161">
@@ -13106,7 +13106,7 @@
         <v>383</v>
       </c>
       <c r="J161" t="n">
-        <v>35037</v>
+        <v>36491</v>
       </c>
       <c r="K161" t="n">
         <v>292302</v>
@@ -13151,10 +13151,10 @@
         <v>30.7</v>
       </c>
       <c r="Y161" t="n">
-        <v>-119.4</v>
+        <v>88.3</v>
       </c>
       <c r="Z161" t="n">
-        <v>-836</v>
+        <v>618</v>
       </c>
     </row>
     <row r="162">
@@ -13186,7 +13186,7 @@
         <v>336</v>
       </c>
       <c r="J162" t="n">
-        <v>35078</v>
+        <v>36532</v>
       </c>
       <c r="K162" t="n">
         <v>293136</v>
@@ -13231,10 +13231,10 @@
         <v>32.7</v>
       </c>
       <c r="Y162" t="n">
-        <v>-116.7</v>
+        <v>91</v>
       </c>
       <c r="Z162" t="n">
-        <v>-817</v>
+        <v>637</v>
       </c>
     </row>
     <row r="163">
@@ -13266,7 +13266,7 @@
         <v>340</v>
       </c>
       <c r="J163" t="n">
-        <v>35111</v>
+        <v>36565</v>
       </c>
       <c r="K163" t="n">
         <v>294029</v>
@@ -13311,10 +13311,10 @@
         <v>33</v>
       </c>
       <c r="Y163" t="n">
-        <v>-122.9</v>
+        <v>84.9</v>
       </c>
       <c r="Z163" t="n">
-        <v>-860</v>
+        <v>594</v>
       </c>
     </row>
     <row r="164">
@@ -13346,7 +13346,7 @@
         <v>322</v>
       </c>
       <c r="J164" t="n">
-        <v>35148</v>
+        <v>36602</v>
       </c>
       <c r="K164" t="n">
         <v>294950</v>
@@ -13426,7 +13426,7 @@
         <v>314</v>
       </c>
       <c r="J165" t="n">
-        <v>35161</v>
+        <v>36615</v>
       </c>
       <c r="K165" t="n">
         <v>295923</v>
@@ -13506,7 +13506,7 @@
         <v>282</v>
       </c>
       <c r="J166" t="n">
-        <v>35173</v>
+        <v>36627</v>
       </c>
       <c r="K166" t="n">
         <v>296328</v>
@@ -13586,7 +13586,7 @@
         <v>277</v>
       </c>
       <c r="J167" t="n">
-        <v>35194</v>
+        <v>36648</v>
       </c>
       <c r="K167" t="n">
         <v>296515</v>
@@ -13702,19 +13702,19 @@
         <v>564.3</v>
       </c>
       <c r="V168" t="n">
-        <v>1644</v>
+        <v>190</v>
       </c>
       <c r="W168" t="n">
-        <v>4.7</v>
+        <v>0.5</v>
       </c>
       <c r="X168" t="n">
-        <v>559</v>
+        <v>74.3</v>
       </c>
       <c r="Y168" t="n">
-        <v>257.3</v>
+        <v>49.6</v>
       </c>
       <c r="Z168" t="n">
-        <v>1801</v>
+        <v>347</v>
       </c>
     </row>
     <row r="169">
@@ -13788,13 +13788,13 @@
         <v>0.1</v>
       </c>
       <c r="X169" t="n">
-        <v>564.7</v>
+        <v>80</v>
       </c>
       <c r="Y169" t="n">
-        <v>255.6</v>
+        <v>47.9</v>
       </c>
       <c r="Z169" t="n">
-        <v>1789</v>
+        <v>335</v>
       </c>
     </row>
     <row r="170">
@@ -13868,13 +13868,13 @@
         <v>0.1</v>
       </c>
       <c r="X170" t="n">
-        <v>565</v>
+        <v>80.3</v>
       </c>
       <c r="Y170" t="n">
-        <v>254</v>
+        <v>46.3</v>
       </c>
       <c r="Z170" t="n">
-        <v>1778</v>
+        <v>324</v>
       </c>
     </row>
     <row r="171">
@@ -13951,10 +13951,10 @@
         <v>32</v>
       </c>
       <c r="Y171" t="n">
-        <v>255.1</v>
+        <v>47.4</v>
       </c>
       <c r="Z171" t="n">
-        <v>1786</v>
+        <v>332</v>
       </c>
     </row>
     <row r="172">
@@ -14031,10 +14031,10 @@
         <v>29</v>
       </c>
       <c r="Y172" t="n">
-        <v>256.1</v>
+        <v>48.4</v>
       </c>
       <c r="Z172" t="n">
-        <v>1793</v>
+        <v>339</v>
       </c>
     </row>
     <row r="173">
@@ -14111,10 +14111,10 @@
         <v>31.3</v>
       </c>
       <c r="Y173" t="n">
-        <v>258.6</v>
+        <v>50.9</v>
       </c>
       <c r="Z173" t="n">
-        <v>1810</v>
+        <v>356</v>
       </c>
     </row>
     <row r="174">
@@ -14191,10 +14191,10 @@
         <v>19.3</v>
       </c>
       <c r="Y174" t="n">
-        <v>256.9</v>
+        <v>49.1</v>
       </c>
       <c r="Z174" t="n">
-        <v>1798</v>
+        <v>344</v>
       </c>
     </row>
     <row r="175">
@@ -53506,7 +53506,7 @@
         <v>347</v>
       </c>
       <c r="J666" t="n">
-        <v>96379</v>
+        <v>101105</v>
       </c>
       <c r="K666" t="n">
         <v>5069193</v>
@@ -53542,19 +53542,19 @@
         <v>908.9</v>
       </c>
       <c r="V666" t="n">
-        <v>-4685</v>
+        <v>41</v>
       </c>
       <c r="W666" t="n">
-        <v>-4.6</v>
+        <v>0</v>
       </c>
       <c r="X666" t="n">
-        <v>-1555</v>
+        <v>20.3</v>
       </c>
       <c r="Y666" t="n">
-        <v>-653.3</v>
+        <v>21.9</v>
       </c>
       <c r="Z666" t="n">
-        <v>-4573</v>
+        <v>153</v>
       </c>
     </row>
     <row r="667">
@@ -53586,7 +53586,7 @@
         <v>374</v>
       </c>
       <c r="J667" t="n">
-        <v>96397</v>
+        <v>101123</v>
       </c>
       <c r="K667" t="n">
         <v>5071356</v>
@@ -53628,13 +53628,13 @@
         <v>0</v>
       </c>
       <c r="X667" t="n">
-        <v>-1552</v>
+        <v>23.3</v>
       </c>
       <c r="Y667" t="n">
-        <v>-655.6</v>
+        <v>19.6</v>
       </c>
       <c r="Z667" t="n">
-        <v>-4589</v>
+        <v>137</v>
       </c>
     </row>
     <row r="668">
@@ -53666,7 +53666,7 @@
         <v>366</v>
       </c>
       <c r="J668" t="n">
-        <v>96411</v>
+        <v>101137</v>
       </c>
       <c r="K668" t="n">
         <v>5073432</v>
@@ -53708,13 +53708,13 @@
         <v>0</v>
       </c>
       <c r="X668" t="n">
-        <v>-1551</v>
+        <v>24.3</v>
       </c>
       <c r="Y668" t="n">
-        <v>-656.7</v>
+        <v>18.4</v>
       </c>
       <c r="Z668" t="n">
-        <v>-4597</v>
+        <v>129</v>
       </c>
     </row>
     <row r="669">
@@ -53746,7 +53746,7 @@
         <v>347</v>
       </c>
       <c r="J669" t="n">
-        <v>96419</v>
+        <v>101145</v>
       </c>
       <c r="K669" t="n">
         <v>5075622</v>
@@ -53791,10 +53791,10 @@
         <v>13.3</v>
       </c>
       <c r="Y669" t="n">
-        <v>-658.7</v>
+        <v>16.4</v>
       </c>
       <c r="Z669" t="n">
-        <v>-4611</v>
+        <v>115</v>
       </c>
     </row>
     <row r="670">
@@ -53826,7 +53826,7 @@
         <v>220</v>
       </c>
       <c r="J670" t="n">
-        <v>96428</v>
+        <v>101154</v>
       </c>
       <c r="K670" t="n">
         <v>5076578</v>
@@ -53871,10 +53871,10 @@
         <v>10.3</v>
       </c>
       <c r="Y670" t="n">
-        <v>-659.4</v>
+        <v>15.7</v>
       </c>
       <c r="Z670" t="n">
-        <v>-4616</v>
+        <v>110</v>
       </c>
     </row>
     <row r="671">
@@ -53906,7 +53906,7 @@
         <v>256</v>
       </c>
       <c r="J671" t="n">
-        <v>96433</v>
+        <v>101159</v>
       </c>
       <c r="K671" t="n">
         <v>5077163</v>
@@ -53951,10 +53951,10 @@
         <v>7.3</v>
       </c>
       <c r="Y671" t="n">
-        <v>-660</v>
+        <v>15.1</v>
       </c>
       <c r="Z671" t="n">
-        <v>-4620</v>
+        <v>106</v>
       </c>
     </row>
     <row r="672">
@@ -53986,7 +53986,7 @@
         <v>235</v>
       </c>
       <c r="J672" t="n">
-        <v>96439</v>
+        <v>101165</v>
       </c>
       <c r="K672" t="n">
         <v>5078403</v>
@@ -54031,10 +54031,10 @@
         <v>6.7</v>
       </c>
       <c r="Y672" t="n">
-        <v>-660.7</v>
+        <v>14.4</v>
       </c>
       <c r="Z672" t="n">
-        <v>-4625</v>
+        <v>101</v>
       </c>
     </row>
     <row r="673">
@@ -54066,7 +54066,7 @@
         <v>359</v>
       </c>
       <c r="J673" t="n">
-        <v>96473</v>
+        <v>101199</v>
       </c>
       <c r="K673" t="n">
         <v>5081721</v>
@@ -54146,7 +54146,7 @@
         <v>362</v>
       </c>
       <c r="J674" t="n">
-        <v>96498</v>
+        <v>101224</v>
       </c>
       <c r="K674" t="n">
         <v>5084300</v>
@@ -54226,7 +54226,7 @@
         <v>352</v>
       </c>
       <c r="J675" t="n">
-        <v>96507</v>
+        <v>101233</v>
       </c>
       <c r="K675" t="n">
         <v>5087132</v>
@@ -54306,7 +54306,7 @@
         <v>333</v>
       </c>
       <c r="J676" t="n">
-        <v>96525</v>
+        <v>101251</v>
       </c>
       <c r="K676" t="n">
         <v>5090113</v>
@@ -54386,7 +54386,7 @@
         <v>212</v>
       </c>
       <c r="J677" t="n">
-        <v>96532</v>
+        <v>101258</v>
       </c>
       <c r="K677" t="n">
         <v>5091474</v>
@@ -54466,7 +54466,7 @@
         <v>261</v>
       </c>
       <c r="J678" t="n">
-        <v>96540</v>
+        <v>101266</v>
       </c>
       <c r="K678" t="n">
         <v>5092650</v>
@@ -54546,7 +54546,7 @@
         <v>350</v>
       </c>
       <c r="J679" t="n">
-        <v>96563</v>
+        <v>101289</v>
       </c>
       <c r="K679" t="n">
         <v>5096630</v>
@@ -54626,7 +54626,7 @@
         <v>368</v>
       </c>
       <c r="J680" t="n">
-        <v>96619</v>
+        <v>101345</v>
       </c>
       <c r="K680" t="n">
         <v>5099964</v>
@@ -54706,7 +54706,7 @@
         <v>366</v>
       </c>
       <c r="J681" t="n">
-        <v>96639</v>
+        <v>101365</v>
       </c>
       <c r="K681" t="n">
         <v>5103608</v>
@@ -54786,7 +54786,7 @@
         <v>370</v>
       </c>
       <c r="J682" t="n">
-        <v>96674</v>
+        <v>101400</v>
       </c>
       <c r="K682" t="n">
         <v>5107754</v>
@@ -54866,7 +54866,7 @@
         <v>338</v>
       </c>
       <c r="J683" t="n">
-        <v>96693</v>
+        <v>101419</v>
       </c>
       <c r="K683" t="n">
         <v>5112008</v>
@@ -54946,7 +54946,7 @@
         <v>224</v>
       </c>
       <c r="J684" t="n">
-        <v>96704</v>
+        <v>101430</v>
       </c>
       <c r="K684" t="n">
         <v>5114326</v>
@@ -55026,7 +55026,7 @@
         <v>285</v>
       </c>
       <c r="J685" t="n">
-        <v>96716</v>
+        <v>101442</v>
       </c>
       <c r="K685" t="n">
         <v>5116491</v>
@@ -55106,7 +55106,7 @@
         <v>395</v>
       </c>
       <c r="J686" t="n">
-        <v>96738</v>
+        <v>101464</v>
       </c>
       <c r="K686" t="n">
         <v>5122152</v>
@@ -55186,7 +55186,7 @@
         <v>340</v>
       </c>
       <c r="J687" t="n">
-        <v>96779</v>
+        <v>101505</v>
       </c>
       <c r="K687" t="n">
         <v>5127159</v>
@@ -55266,7 +55266,7 @@
         <v>416</v>
       </c>
       <c r="J688" t="n">
-        <v>96807</v>
+        <v>101533</v>
       </c>
       <c r="K688" t="n">
         <v>5133873</v>
@@ -55346,7 +55346,7 @@
         <v>402</v>
       </c>
       <c r="J689" t="n">
-        <v>96827</v>
+        <v>101553</v>
       </c>
       <c r="K689" t="n">
         <v>5140265</v>
@@ -55426,7 +55426,7 @@
         <v>376</v>
       </c>
       <c r="J690" t="n">
-        <v>96844</v>
+        <v>101570</v>
       </c>
       <c r="K690" t="n">
         <v>5146922</v>
@@ -55506,7 +55506,7 @@
         <v>243</v>
       </c>
       <c r="J691" t="n">
-        <v>96854</v>
+        <v>101580</v>
       </c>
       <c r="K691" t="n">
         <v>5150823</v>
@@ -55586,7 +55586,7 @@
         <v>322</v>
       </c>
       <c r="J692" t="n">
-        <v>96865</v>
+        <v>101591</v>
       </c>
       <c r="K692" t="n">
         <v>5154227</v>
@@ -55666,7 +55666,7 @@
         <v>473</v>
       </c>
       <c r="J693" t="n">
-        <v>96895</v>
+        <v>101621</v>
       </c>
       <c r="K693" t="n">
         <v>5163313</v>
@@ -55746,7 +55746,7 @@
         <v>495</v>
       </c>
       <c r="J694" t="n">
-        <v>96954</v>
+        <v>101680</v>
       </c>
       <c r="K694" t="n">
         <v>5170962</v>
@@ -55826,7 +55826,7 @@
         <v>503</v>
       </c>
       <c r="J695" t="n">
-        <v>96974</v>
+        <v>101700</v>
       </c>
       <c r="K695" t="n">
         <v>5180129</v>
@@ -55906,7 +55906,7 @@
         <v>506</v>
       </c>
       <c r="J696" t="n">
-        <v>96999</v>
+        <v>101725</v>
       </c>
       <c r="K696" t="n">
         <v>5189976</v>
@@ -55986,7 +55986,7 @@
         <v>446</v>
       </c>
       <c r="J697" t="n">
-        <v>97021</v>
+        <v>101747</v>
       </c>
       <c r="K697" t="n">
         <v>5199478</v>
@@ -56066,7 +56066,7 @@
         <v>340</v>
       </c>
       <c r="J698" t="n">
-        <v>97026</v>
+        <v>101752</v>
       </c>
       <c r="K698" t="n">
         <v>5204773</v>
@@ -56146,7 +56146,7 @@
         <v>440</v>
       </c>
       <c r="J699" t="n">
-        <v>97039</v>
+        <v>101765</v>
       </c>
       <c r="K699" t="n">
         <v>5209676</v>
@@ -56226,7 +56226,7 @@
         <v>611</v>
       </c>
       <c r="J700" t="n">
-        <v>97077</v>
+        <v>101803</v>
       </c>
       <c r="K700" t="n">
         <v>5222532</v>
@@ -56306,7 +56306,7 @@
         <v>641</v>
       </c>
       <c r="J701" t="n">
-        <v>97159</v>
+        <v>101885</v>
       </c>
       <c r="K701" t="n">
         <v>5234310</v>
@@ -56386,7 +56386,7 @@
         <v>646</v>
       </c>
       <c r="J702" t="n">
-        <v>97191</v>
+        <v>101917</v>
       </c>
       <c r="K702" t="n">
         <v>5246869</v>
@@ -56466,7 +56466,7 @@
         <v>674</v>
       </c>
       <c r="J703" t="n">
-        <v>97227</v>
+        <v>101953</v>
       </c>
       <c r="K703" t="n">
         <v>5260493</v>
@@ -56546,7 +56546,7 @@
         <v>608</v>
       </c>
       <c r="J704" t="n">
-        <v>93201</v>
+        <v>97927</v>
       </c>
       <c r="K704" t="n">
         <v>5093079</v>
@@ -56585,7 +56585,7 @@
         <v>-4026</v>
       </c>
       <c r="W704" t="n">
-        <v>-4.1</v>
+        <v>-3.9</v>
       </c>
       <c r="X704" t="n">
         <v>-1319.3</v>
@@ -56626,7 +56626,7 @@
         <v>338</v>
       </c>
       <c r="J705" t="n">
-        <v>69965</v>
+        <v>74691</v>
       </c>
       <c r="K705" t="n">
         <v>3947797</v>
@@ -56665,7 +56665,7 @@
         <v>-23236</v>
       </c>
       <c r="W705" t="n">
-        <v>-24.9</v>
+        <v>-23.7</v>
       </c>
       <c r="X705" t="n">
         <v>-9075.3</v>
@@ -56706,7 +56706,7 @@
         <v>289</v>
       </c>
       <c r="J706" t="n">
-        <v>63110</v>
+        <v>67836</v>
       </c>
       <c r="K706" t="n">
         <v>3846416</v>
@@ -56745,7 +56745,7 @@
         <v>-6855</v>
       </c>
       <c r="W706" t="n">
-        <v>-9.8</v>
+        <v>-9.2</v>
       </c>
       <c r="X706" t="n">
         <v>-11372.3</v>
@@ -56822,19 +56822,19 @@
         <v>-372067.6</v>
       </c>
       <c r="V707" t="n">
-        <v>-46930</v>
+        <v>-51656</v>
       </c>
       <c r="W707" t="n">
-        <v>-74.4</v>
+        <v>-76.1</v>
       </c>
       <c r="X707" t="n">
-        <v>-25673.7</v>
+        <v>-27249</v>
       </c>
       <c r="Y707" t="n">
-        <v>-11556.7</v>
+        <v>-12231.9</v>
       </c>
       <c r="Z707" t="n">
-        <v>-80897</v>
+        <v>-85623</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualiza datos provincias 2021-12-06
</commit_message>
<xml_diff>
--- a/data/output/covid19-spain_consolidated.xlsx
+++ b/data/output/covid19-spain_consolidated.xlsx
@@ -53669,37 +53669,37 @@
         <v>101137</v>
       </c>
       <c r="K668" t="n">
-        <v>5073432</v>
+        <v>5073433</v>
       </c>
       <c r="L668" t="n">
-        <v>2811134</v>
+        <v>2811135</v>
       </c>
       <c r="M668" t="n">
         <v>10912</v>
       </c>
       <c r="N668" t="n">
-        <v>23882</v>
+        <v>23883</v>
       </c>
       <c r="O668" t="n">
-        <v>12192</v>
+        <v>12193</v>
       </c>
       <c r="P668" t="n">
-        <v>12663</v>
+        <v>12664</v>
       </c>
       <c r="Q668" t="n">
-        <v>6495</v>
+        <v>6496</v>
       </c>
       <c r="R668" t="n">
-        <v>2076</v>
+        <v>2077</v>
       </c>
       <c r="S668" t="n">
-        <v>1741.7</v>
+        <v>1741.9</v>
       </c>
       <c r="T668" t="n">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="U668" t="n">
-        <v>927.9</v>
+        <v>928</v>
       </c>
       <c r="V668" t="n">
         <v>14</v>
@@ -53749,37 +53749,37 @@
         <v>101145</v>
       </c>
       <c r="K669" t="n">
-        <v>5075622</v>
+        <v>5075623</v>
       </c>
       <c r="L669" t="n">
-        <v>2812277</v>
+        <v>2812278</v>
       </c>
       <c r="M669" t="n">
         <v>10914</v>
       </c>
       <c r="N669" t="n">
-        <v>24309</v>
+        <v>24310</v>
       </c>
       <c r="O669" t="n">
-        <v>12518</v>
+        <v>12519</v>
       </c>
       <c r="P669" t="n">
-        <v>12823</v>
+        <v>12824</v>
       </c>
       <c r="Q669" t="n">
-        <v>6588</v>
+        <v>6589</v>
       </c>
       <c r="R669" t="n">
         <v>2190</v>
       </c>
       <c r="S669" t="n">
-        <v>1788.3</v>
+        <v>1788.4</v>
       </c>
       <c r="T669" t="n">
         <v>1143</v>
       </c>
       <c r="U669" t="n">
-        <v>941.1</v>
+        <v>941.3</v>
       </c>
       <c r="V669" t="n">
         <v>8</v>
@@ -53829,37 +53829,37 @@
         <v>101154</v>
       </c>
       <c r="K670" t="n">
-        <v>5076578</v>
+        <v>5076579</v>
       </c>
       <c r="L670" t="n">
-        <v>2812724</v>
+        <v>2812725</v>
       </c>
       <c r="M670" t="n">
         <v>10914</v>
       </c>
       <c r="N670" t="n">
-        <v>24443</v>
+        <v>24444</v>
       </c>
       <c r="O670" t="n">
-        <v>12617</v>
+        <v>12618</v>
       </c>
       <c r="P670" t="n">
-        <v>12923</v>
+        <v>12924</v>
       </c>
       <c r="Q670" t="n">
-        <v>6647</v>
+        <v>6648</v>
       </c>
       <c r="R670" t="n">
         <v>956</v>
       </c>
       <c r="S670" t="n">
-        <v>1802.4</v>
+        <v>1802.6</v>
       </c>
       <c r="T670" t="n">
         <v>447</v>
       </c>
       <c r="U670" t="n">
-        <v>949.6</v>
+        <v>949.7</v>
       </c>
       <c r="V670" t="n">
         <v>9</v>
@@ -53909,37 +53909,37 @@
         <v>101159</v>
       </c>
       <c r="K671" t="n">
-        <v>5077163</v>
+        <v>5077164</v>
       </c>
       <c r="L671" t="n">
-        <v>2813088</v>
+        <v>2813089</v>
       </c>
       <c r="M671" t="n">
         <v>10914</v>
       </c>
       <c r="N671" t="n">
-        <v>24284</v>
+        <v>24285</v>
       </c>
       <c r="O671" t="n">
-        <v>12428</v>
+        <v>12429</v>
       </c>
       <c r="P671" t="n">
-        <v>12878</v>
+        <v>12879</v>
       </c>
       <c r="Q671" t="n">
-        <v>6584</v>
+        <v>6585</v>
       </c>
       <c r="R671" t="n">
         <v>585</v>
       </c>
       <c r="S671" t="n">
-        <v>1775.4</v>
+        <v>1775.6</v>
       </c>
       <c r="T671" t="n">
         <v>364</v>
       </c>
       <c r="U671" t="n">
-        <v>940.6</v>
+        <v>940.7</v>
       </c>
       <c r="V671" t="n">
         <v>5</v>
@@ -53989,37 +53989,37 @@
         <v>101165</v>
       </c>
       <c r="K672" t="n">
-        <v>5078403</v>
+        <v>5078404</v>
       </c>
       <c r="L672" t="n">
-        <v>2813692</v>
+        <v>2813693</v>
       </c>
       <c r="M672" t="n">
         <v>10914</v>
       </c>
       <c r="N672" t="n">
-        <v>23147</v>
+        <v>23148</v>
       </c>
       <c r="O672" t="n">
-        <v>11170</v>
+        <v>11171</v>
       </c>
       <c r="P672" t="n">
-        <v>12236</v>
+        <v>12237</v>
       </c>
       <c r="Q672" t="n">
-        <v>5864</v>
+        <v>5865</v>
       </c>
       <c r="R672" t="n">
         <v>1240</v>
       </c>
       <c r="S672" t="n">
-        <v>1595.7</v>
+        <v>1595.9</v>
       </c>
       <c r="T672" t="n">
         <v>604</v>
       </c>
       <c r="U672" t="n">
-        <v>837.7</v>
+        <v>837.9</v>
       </c>
       <c r="V672" t="n">
         <v>6</v>
@@ -54069,37 +54069,37 @@
         <v>101199</v>
       </c>
       <c r="K673" t="n">
-        <v>5081721</v>
+        <v>5081722</v>
       </c>
       <c r="L673" t="n">
-        <v>2815533</v>
+        <v>2815534</v>
       </c>
       <c r="M673" t="n">
         <v>10915</v>
       </c>
       <c r="N673" t="n">
-        <v>24594</v>
+        <v>24595</v>
       </c>
       <c r="O673" t="n">
-        <v>12528</v>
+        <v>12529</v>
       </c>
       <c r="P673" t="n">
-        <v>13026</v>
+        <v>13027</v>
       </c>
       <c r="Q673" t="n">
-        <v>6664</v>
+        <v>6665</v>
       </c>
       <c r="R673" t="n">
         <v>3318</v>
       </c>
       <c r="S673" t="n">
-        <v>1789.7</v>
+        <v>1789.9</v>
       </c>
       <c r="T673" t="n">
         <v>1841</v>
       </c>
       <c r="U673" t="n">
-        <v>952</v>
+        <v>952.1</v>
       </c>
       <c r="V673" t="n">
         <v>34</v>
@@ -54149,37 +54149,37 @@
         <v>101224</v>
       </c>
       <c r="K674" t="n">
-        <v>5084300</v>
+        <v>5084301</v>
       </c>
       <c r="L674" t="n">
-        <v>2816980</v>
+        <v>2816981</v>
       </c>
       <c r="M674" t="n">
         <v>10918</v>
       </c>
       <c r="N674" t="n">
-        <v>25078</v>
+        <v>25079</v>
       </c>
       <c r="O674" t="n">
-        <v>12944</v>
+        <v>12945</v>
       </c>
       <c r="P674" t="n">
-        <v>13334</v>
+        <v>13335</v>
       </c>
       <c r="Q674" t="n">
-        <v>6951</v>
+        <v>6952</v>
       </c>
       <c r="R674" t="n">
         <v>2579</v>
       </c>
       <c r="S674" t="n">
-        <v>1849.1</v>
+        <v>1849.3</v>
       </c>
       <c r="T674" t="n">
         <v>1447</v>
       </c>
       <c r="U674" t="n">
-        <v>993</v>
+        <v>993.1</v>
       </c>
       <c r="V674" t="n">
         <v>25</v>
@@ -54229,22 +54229,22 @@
         <v>101233</v>
       </c>
       <c r="K675" t="n">
-        <v>5087132</v>
+        <v>5087133</v>
       </c>
       <c r="L675" t="n">
-        <v>2818506</v>
+        <v>2818507</v>
       </c>
       <c r="M675" t="n">
         <v>10918</v>
       </c>
       <c r="N675" t="n">
-        <v>25892</v>
+        <v>25893</v>
       </c>
       <c r="O675" t="n">
         <v>13700</v>
       </c>
       <c r="P675" t="n">
-        <v>13867</v>
+        <v>13868</v>
       </c>
       <c r="Q675" t="n">
         <v>7372</v>
@@ -54309,22 +54309,22 @@
         <v>101251</v>
       </c>
       <c r="K676" t="n">
-        <v>5090113</v>
+        <v>5090114</v>
       </c>
       <c r="L676" t="n">
-        <v>2820031</v>
+        <v>2820032</v>
       </c>
       <c r="M676" t="n">
         <v>10920</v>
       </c>
       <c r="N676" t="n">
-        <v>27009</v>
+        <v>27010</v>
       </c>
       <c r="O676" t="n">
         <v>14491</v>
       </c>
       <c r="P676" t="n">
-        <v>14342</v>
+        <v>14343</v>
       </c>
       <c r="Q676" t="n">
         <v>7754</v>
@@ -54389,22 +54389,22 @@
         <v>101258</v>
       </c>
       <c r="K677" t="n">
-        <v>5091474</v>
+        <v>5091475</v>
       </c>
       <c r="L677" t="n">
-        <v>2820706</v>
+        <v>2820707</v>
       </c>
       <c r="M677" t="n">
         <v>10923</v>
       </c>
       <c r="N677" t="n">
-        <v>27513</v>
+        <v>27514</v>
       </c>
       <c r="O677" t="n">
         <v>14896</v>
       </c>
       <c r="P677" t="n">
-        <v>14629</v>
+        <v>14630</v>
       </c>
       <c r="Q677" t="n">
         <v>7982</v>
@@ -54469,22 +54469,22 @@
         <v>101266</v>
       </c>
       <c r="K678" t="n">
-        <v>5092650</v>
+        <v>5092651</v>
       </c>
       <c r="L678" t="n">
-        <v>2821441</v>
+        <v>2821442</v>
       </c>
       <c r="M678" t="n">
         <v>10923</v>
       </c>
       <c r="N678" t="n">
-        <v>27915</v>
+        <v>27916</v>
       </c>
       <c r="O678" t="n">
         <v>15487</v>
       </c>
       <c r="P678" t="n">
-        <v>14937</v>
+        <v>14938</v>
       </c>
       <c r="Q678" t="n">
         <v>8353</v>
@@ -54549,22 +54549,22 @@
         <v>101289</v>
       </c>
       <c r="K679" t="n">
-        <v>5096630</v>
+        <v>5096631</v>
       </c>
       <c r="L679" t="n">
-        <v>2823475</v>
+        <v>2823476</v>
       </c>
       <c r="M679" t="n">
         <v>10926</v>
       </c>
       <c r="N679" t="n">
-        <v>29397</v>
+        <v>29398</v>
       </c>
       <c r="O679" t="n">
         <v>18227</v>
       </c>
       <c r="P679" t="n">
-        <v>15647</v>
+        <v>15648</v>
       </c>
       <c r="Q679" t="n">
         <v>9783</v>
@@ -54629,22 +54629,22 @@
         <v>101345</v>
       </c>
       <c r="K680" t="n">
-        <v>5099964</v>
+        <v>5099965</v>
       </c>
       <c r="L680" t="n">
-        <v>2825476</v>
+        <v>2825477</v>
       </c>
       <c r="M680" t="n">
         <v>10929</v>
       </c>
       <c r="N680" t="n">
-        <v>30771</v>
+        <v>30772</v>
       </c>
       <c r="O680" t="n">
         <v>18243</v>
       </c>
       <c r="P680" t="n">
-        <v>16607</v>
+        <v>16608</v>
       </c>
       <c r="Q680" t="n">
         <v>9943</v>
@@ -54709,22 +54709,22 @@
         <v>101365</v>
       </c>
       <c r="K681" t="n">
-        <v>5103608</v>
+        <v>5103609</v>
       </c>
       <c r="L681" t="n">
-        <v>2827476</v>
+        <v>2827477</v>
       </c>
       <c r="M681" t="n">
         <v>10932</v>
       </c>
       <c r="N681" t="n">
-        <v>32252</v>
+        <v>32253</v>
       </c>
       <c r="O681" t="n">
         <v>19308</v>
       </c>
       <c r="P681" t="n">
-        <v>17447</v>
+        <v>17448</v>
       </c>
       <c r="Q681" t="n">
         <v>10496</v>
@@ -54789,10 +54789,10 @@
         <v>101400</v>
       </c>
       <c r="K682" t="n">
-        <v>5107754</v>
+        <v>5107755</v>
       </c>
       <c r="L682" t="n">
-        <v>2829679</v>
+        <v>2829680</v>
       </c>
       <c r="M682" t="n">
         <v>10933</v>
@@ -54869,10 +54869,10 @@
         <v>101419</v>
       </c>
       <c r="K683" t="n">
-        <v>5112008</v>
+        <v>5112009</v>
       </c>
       <c r="L683" t="n">
-        <v>2832159</v>
+        <v>2832160</v>
       </c>
       <c r="M683" t="n">
         <v>10936</v>
@@ -54949,10 +54949,10 @@
         <v>101430</v>
       </c>
       <c r="K684" t="n">
-        <v>5114326</v>
+        <v>5114327</v>
       </c>
       <c r="L684" t="n">
-        <v>2833379</v>
+        <v>2833380</v>
       </c>
       <c r="M684" t="n">
         <v>10936</v>
@@ -55029,10 +55029,10 @@
         <v>101442</v>
       </c>
       <c r="K685" t="n">
-        <v>5116491</v>
+        <v>5116492</v>
       </c>
       <c r="L685" t="n">
-        <v>2834726</v>
+        <v>2834727</v>
       </c>
       <c r="M685" t="n">
         <v>10936</v>
@@ -55109,10 +55109,10 @@
         <v>101464</v>
       </c>
       <c r="K686" t="n">
-        <v>5122152</v>
+        <v>5122153</v>
       </c>
       <c r="L686" t="n">
-        <v>2837607</v>
+        <v>2837608</v>
       </c>
       <c r="M686" t="n">
         <v>10941</v>
@@ -55189,10 +55189,10 @@
         <v>101505</v>
       </c>
       <c r="K687" t="n">
-        <v>5127159</v>
+        <v>5127160</v>
       </c>
       <c r="L687" t="n">
-        <v>2840762</v>
+        <v>2840763</v>
       </c>
       <c r="M687" t="n">
         <v>10941</v>
@@ -55269,37 +55269,37 @@
         <v>101533</v>
       </c>
       <c r="K688" t="n">
-        <v>5133873</v>
+        <v>5133875</v>
       </c>
       <c r="L688" t="n">
-        <v>2844086</v>
+        <v>2844088</v>
       </c>
       <c r="M688" t="n">
         <v>10842</v>
       </c>
       <c r="N688" t="n">
-        <v>49573</v>
+        <v>49574</v>
       </c>
       <c r="O688" t="n">
-        <v>30265</v>
+        <v>30266</v>
       </c>
       <c r="P688" t="n">
-        <v>27106</v>
+        <v>27107</v>
       </c>
       <c r="Q688" t="n">
-        <v>16610</v>
+        <v>16611</v>
       </c>
       <c r="R688" t="n">
-        <v>6714</v>
+        <v>6715</v>
       </c>
       <c r="S688" t="n">
-        <v>4323.6</v>
+        <v>4323.7</v>
       </c>
       <c r="T688" t="n">
-        <v>3324</v>
+        <v>3325</v>
       </c>
       <c r="U688" t="n">
-        <v>2372.9</v>
+        <v>2373</v>
       </c>
       <c r="V688" t="n">
         <v>28</v>
@@ -55349,37 +55349,37 @@
         <v>101553</v>
       </c>
       <c r="K689" t="n">
-        <v>5140265</v>
+        <v>5140267</v>
       </c>
       <c r="L689" t="n">
-        <v>2847429</v>
+        <v>2847431</v>
       </c>
       <c r="M689" t="n">
         <v>10954</v>
       </c>
       <c r="N689" t="n">
-        <v>53133</v>
+        <v>53134</v>
       </c>
       <c r="O689" t="n">
-        <v>32511</v>
+        <v>32512</v>
       </c>
       <c r="P689" t="n">
-        <v>28923</v>
+        <v>28924</v>
       </c>
       <c r="Q689" t="n">
-        <v>17750</v>
+        <v>17751</v>
       </c>
       <c r="R689" t="n">
         <v>6392</v>
       </c>
       <c r="S689" t="n">
-        <v>4644.4</v>
+        <v>4644.6</v>
       </c>
       <c r="T689" t="n">
         <v>3343</v>
       </c>
       <c r="U689" t="n">
-        <v>2535.7</v>
+        <v>2535.9</v>
       </c>
       <c r="V689" t="n">
         <v>20</v>
@@ -55429,37 +55429,37 @@
         <v>101570</v>
       </c>
       <c r="K690" t="n">
-        <v>5146922</v>
+        <v>5146924</v>
       </c>
       <c r="L690" t="n">
-        <v>2851106</v>
+        <v>2851108</v>
       </c>
       <c r="M690" t="n">
         <v>10958</v>
       </c>
       <c r="N690" t="n">
-        <v>56809</v>
+        <v>56810</v>
       </c>
       <c r="O690" t="n">
-        <v>34914</v>
+        <v>34915</v>
       </c>
       <c r="P690" t="n">
-        <v>31075</v>
+        <v>31076</v>
       </c>
       <c r="Q690" t="n">
-        <v>18947</v>
+        <v>18948</v>
       </c>
       <c r="R690" t="n">
         <v>6657</v>
       </c>
       <c r="S690" t="n">
-        <v>4987.7</v>
+        <v>4987.9</v>
       </c>
       <c r="T690" t="n">
         <v>3677</v>
       </c>
       <c r="U690" t="n">
-        <v>2706.7</v>
+        <v>2706.9</v>
       </c>
       <c r="V690" t="n">
         <v>17</v>
@@ -55509,37 +55509,37 @@
         <v>101580</v>
       </c>
       <c r="K691" t="n">
-        <v>5150823</v>
+        <v>5150825</v>
       </c>
       <c r="L691" t="n">
-        <v>2853086</v>
+        <v>2853088</v>
       </c>
       <c r="M691" t="n">
         <v>10958</v>
       </c>
       <c r="N691" t="n">
-        <v>59349</v>
+        <v>59350</v>
       </c>
       <c r="O691" t="n">
-        <v>36497</v>
+        <v>36498</v>
       </c>
       <c r="P691" t="n">
-        <v>32380</v>
+        <v>32381</v>
       </c>
       <c r="Q691" t="n">
-        <v>19707</v>
+        <v>19708</v>
       </c>
       <c r="R691" t="n">
         <v>3901</v>
       </c>
       <c r="S691" t="n">
-        <v>5213.9</v>
+        <v>5214</v>
       </c>
       <c r="T691" t="n">
         <v>1980</v>
       </c>
       <c r="U691" t="n">
-        <v>2815.3</v>
+        <v>2815.4</v>
       </c>
       <c r="V691" t="n">
         <v>10</v>
@@ -55589,37 +55589,37 @@
         <v>101591</v>
       </c>
       <c r="K692" t="n">
-        <v>5154227</v>
+        <v>5154229</v>
       </c>
       <c r="L692" t="n">
-        <v>2855075</v>
+        <v>2855077</v>
       </c>
       <c r="M692" t="n">
         <v>10964</v>
       </c>
       <c r="N692" t="n">
-        <v>61577</v>
+        <v>61578</v>
       </c>
       <c r="O692" t="n">
-        <v>37736</v>
+        <v>37737</v>
       </c>
       <c r="P692" t="n">
-        <v>33634</v>
+        <v>33635</v>
       </c>
       <c r="Q692" t="n">
-        <v>20349</v>
+        <v>20350</v>
       </c>
       <c r="R692" t="n">
         <v>3404</v>
       </c>
       <c r="S692" t="n">
-        <v>5390.9</v>
+        <v>5391</v>
       </c>
       <c r="T692" t="n">
         <v>1989</v>
       </c>
       <c r="U692" t="n">
-        <v>2907</v>
+        <v>2907.1</v>
       </c>
       <c r="V692" t="n">
         <v>11</v>
@@ -55669,37 +55669,37 @@
         <v>101621</v>
       </c>
       <c r="K693" t="n">
-        <v>5163313</v>
+        <v>5163316</v>
       </c>
       <c r="L693" t="n">
-        <v>2859541</v>
+        <v>2859544</v>
       </c>
       <c r="M693" t="n">
         <v>10965</v>
       </c>
       <c r="N693" t="n">
-        <v>66683</v>
+        <v>66685</v>
       </c>
       <c r="O693" t="n">
-        <v>41161</v>
+        <v>41163</v>
       </c>
       <c r="P693" t="n">
-        <v>36066</v>
+        <v>36068</v>
       </c>
       <c r="Q693" t="n">
-        <v>21934</v>
+        <v>21936</v>
       </c>
       <c r="R693" t="n">
-        <v>9086</v>
+        <v>9087</v>
       </c>
       <c r="S693" t="n">
-        <v>5880.1</v>
+        <v>5880.4</v>
       </c>
       <c r="T693" t="n">
-        <v>4466</v>
+        <v>4467</v>
       </c>
       <c r="U693" t="n">
-        <v>3133.4</v>
+        <v>3133.7</v>
       </c>
       <c r="V693" t="n">
         <v>30</v>
@@ -55749,37 +55749,37 @@
         <v>101680</v>
       </c>
       <c r="K694" t="n">
-        <v>5170962</v>
+        <v>5170967</v>
       </c>
       <c r="L694" t="n">
-        <v>2863958</v>
+        <v>2863963</v>
       </c>
       <c r="M694" t="n">
         <v>10972</v>
       </c>
       <c r="N694" t="n">
-        <v>70998</v>
+        <v>71002</v>
       </c>
       <c r="O694" t="n">
-        <v>43803</v>
+        <v>43807</v>
       </c>
       <c r="P694" t="n">
-        <v>38482</v>
+        <v>38486</v>
       </c>
       <c r="Q694" t="n">
-        <v>23196</v>
+        <v>23200</v>
       </c>
       <c r="R694" t="n">
-        <v>7649</v>
+        <v>7651</v>
       </c>
       <c r="S694" t="n">
-        <v>6257.6</v>
+        <v>6258.1</v>
       </c>
       <c r="T694" t="n">
-        <v>4417</v>
+        <v>4419</v>
       </c>
       <c r="U694" t="n">
-        <v>3313.7</v>
+        <v>3314.3</v>
       </c>
       <c r="V694" t="n">
         <v>59</v>
@@ -55829,37 +55829,37 @@
         <v>101700</v>
       </c>
       <c r="K695" t="n">
-        <v>5180129</v>
+        <v>5180136</v>
       </c>
       <c r="L695" t="n">
-        <v>2868739</v>
+        <v>2868746</v>
       </c>
       <c r="M695" t="n">
         <v>10975</v>
       </c>
       <c r="N695" t="n">
-        <v>76521</v>
+        <v>76527</v>
       </c>
       <c r="O695" t="n">
-        <v>46256</v>
+        <v>46261</v>
       </c>
       <c r="P695" t="n">
-        <v>41263</v>
+        <v>41269</v>
       </c>
       <c r="Q695" t="n">
-        <v>24653</v>
+        <v>24658</v>
       </c>
       <c r="R695" t="n">
-        <v>9167</v>
+        <v>9169</v>
       </c>
       <c r="S695" t="n">
-        <v>6608</v>
+        <v>6608.7</v>
       </c>
       <c r="T695" t="n">
-        <v>4781</v>
+        <v>4783</v>
       </c>
       <c r="U695" t="n">
-        <v>3521.9</v>
+        <v>3522.6</v>
       </c>
       <c r="V695" t="n">
         <v>20</v>
@@ -55909,37 +55909,37 @@
         <v>101725</v>
       </c>
       <c r="K696" t="n">
-        <v>5189976</v>
+        <v>5189993</v>
       </c>
       <c r="L696" t="n">
-        <v>2873544</v>
+        <v>2873561</v>
       </c>
       <c r="M696" t="n">
         <v>10979</v>
       </c>
       <c r="N696" t="n">
-        <v>82222</v>
+        <v>82238</v>
       </c>
       <c r="O696" t="n">
-        <v>49711</v>
+        <v>49726</v>
       </c>
       <c r="P696" t="n">
-        <v>43865</v>
+        <v>43881</v>
       </c>
       <c r="Q696" t="n">
-        <v>26115</v>
+        <v>26130</v>
       </c>
       <c r="R696" t="n">
-        <v>9847</v>
+        <v>9857</v>
       </c>
       <c r="S696" t="n">
-        <v>7101.6</v>
+        <v>7103.7</v>
       </c>
       <c r="T696" t="n">
-        <v>4805</v>
+        <v>4815</v>
       </c>
       <c r="U696" t="n">
-        <v>3730.7</v>
+        <v>3732.9</v>
       </c>
       <c r="V696" t="n">
         <v>25</v>
@@ -55989,37 +55989,37 @@
         <v>101747</v>
       </c>
       <c r="K697" t="n">
-        <v>5199478</v>
+        <v>5199505</v>
       </c>
       <c r="L697" t="n">
-        <v>2878542</v>
+        <v>2878569</v>
       </c>
       <c r="M697" t="n">
         <v>10990</v>
       </c>
       <c r="N697" t="n">
-        <v>87470</v>
+        <v>87496</v>
       </c>
       <c r="O697" t="n">
-        <v>52556</v>
+        <v>52581</v>
       </c>
       <c r="P697" t="n">
-        <v>46383</v>
+        <v>46409</v>
       </c>
       <c r="Q697" t="n">
-        <v>27436</v>
+        <v>27461</v>
       </c>
       <c r="R697" t="n">
-        <v>9502</v>
+        <v>9512</v>
       </c>
       <c r="S697" t="n">
-        <v>7508</v>
+        <v>7511.6</v>
       </c>
       <c r="T697" t="n">
-        <v>4998</v>
+        <v>5008</v>
       </c>
       <c r="U697" t="n">
-        <v>3919.4</v>
+        <v>3923</v>
       </c>
       <c r="V697" t="n">
         <v>22</v>
@@ -56069,37 +56069,37 @@
         <v>101752</v>
       </c>
       <c r="K698" t="n">
-        <v>5204773</v>
+        <v>5204804</v>
       </c>
       <c r="L698" t="n">
-        <v>2881244</v>
+        <v>2881275</v>
       </c>
       <c r="M698" t="n">
         <v>10994</v>
       </c>
       <c r="N698" t="n">
-        <v>90447</v>
+        <v>90477</v>
       </c>
       <c r="O698" t="n">
-        <v>53950</v>
+        <v>53979</v>
       </c>
       <c r="P698" t="n">
-        <v>47865</v>
+        <v>47895</v>
       </c>
       <c r="Q698" t="n">
-        <v>28158</v>
+        <v>28187</v>
       </c>
       <c r="R698" t="n">
-        <v>5295</v>
+        <v>5299</v>
       </c>
       <c r="S698" t="n">
-        <v>7707.1</v>
+        <v>7711.3</v>
       </c>
       <c r="T698" t="n">
-        <v>2702</v>
+        <v>2706</v>
       </c>
       <c r="U698" t="n">
-        <v>4022.6</v>
+        <v>4026.7</v>
       </c>
       <c r="V698" t="n">
         <v>5</v>
@@ -56149,37 +56149,37 @@
         <v>101765</v>
       </c>
       <c r="K699" t="n">
-        <v>5209676</v>
+        <v>5209694</v>
       </c>
       <c r="L699" t="n">
-        <v>2884065</v>
+        <v>2884083</v>
       </c>
       <c r="M699" t="n">
         <v>10997</v>
       </c>
       <c r="N699" t="n">
-        <v>93185</v>
+        <v>93202</v>
       </c>
       <c r="O699" t="n">
-        <v>55449</v>
+        <v>55465</v>
       </c>
       <c r="P699" t="n">
-        <v>49339</v>
+        <v>49356</v>
       </c>
       <c r="Q699" t="n">
-        <v>28990</v>
+        <v>29006</v>
       </c>
       <c r="R699" t="n">
-        <v>4903</v>
+        <v>4890</v>
       </c>
       <c r="S699" t="n">
-        <v>7921.3</v>
+        <v>7923.6</v>
       </c>
       <c r="T699" t="n">
-        <v>2821</v>
+        <v>2808</v>
       </c>
       <c r="U699" t="n">
-        <v>4141.4</v>
+        <v>4143.7</v>
       </c>
       <c r="V699" t="n">
         <v>13</v>
@@ -56229,37 +56229,37 @@
         <v>101803</v>
       </c>
       <c r="K700" t="n">
-        <v>5222532</v>
+        <v>5222596</v>
       </c>
       <c r="L700" t="n">
-        <v>2889897</v>
+        <v>2889961</v>
       </c>
       <c r="M700" t="n">
         <v>11007</v>
       </c>
       <c r="N700" t="n">
-        <v>100380</v>
+        <v>100443</v>
       </c>
       <c r="O700" t="n">
-        <v>59219</v>
+        <v>59280</v>
       </c>
       <c r="P700" t="n">
-        <v>52290</v>
+        <v>52353</v>
       </c>
       <c r="Q700" t="n">
-        <v>30356</v>
+        <v>30417</v>
       </c>
       <c r="R700" t="n">
-        <v>12856</v>
+        <v>12902</v>
       </c>
       <c r="S700" t="n">
-        <v>8459.9</v>
+        <v>8468.6</v>
       </c>
       <c r="T700" t="n">
-        <v>5832</v>
+        <v>5878</v>
       </c>
       <c r="U700" t="n">
-        <v>4336.6</v>
+        <v>4345.3</v>
       </c>
       <c r="V700" t="n">
         <v>38</v>
@@ -56309,37 +56309,37 @@
         <v>101885</v>
       </c>
       <c r="K701" t="n">
-        <v>5234310</v>
+        <v>5234463</v>
       </c>
       <c r="L701" t="n">
-        <v>2896040</v>
+        <v>2896193</v>
       </c>
       <c r="M701" t="n">
         <v>11013</v>
       </c>
       <c r="N701" t="n">
-        <v>107151</v>
+        <v>107303</v>
       </c>
       <c r="O701" t="n">
-        <v>63348</v>
+        <v>63496</v>
       </c>
       <c r="P701" t="n">
-        <v>55278</v>
+        <v>55430</v>
       </c>
       <c r="Q701" t="n">
-        <v>32082</v>
+        <v>32230</v>
       </c>
       <c r="R701" t="n">
-        <v>11778</v>
+        <v>11867</v>
       </c>
       <c r="S701" t="n">
-        <v>9049.7</v>
+        <v>9070.9</v>
       </c>
       <c r="T701" t="n">
-        <v>6143</v>
+        <v>6232</v>
       </c>
       <c r="U701" t="n">
-        <v>4583.1</v>
+        <v>4604.3</v>
       </c>
       <c r="V701" t="n">
         <v>82</v>
@@ -56389,37 +56389,37 @@
         <v>101917</v>
       </c>
       <c r="K702" t="n">
-        <v>5246869</v>
+        <v>5247098</v>
       </c>
       <c r="L702" t="n">
-        <v>2902869</v>
+        <v>2903098</v>
       </c>
       <c r="M702" t="n">
         <v>11021</v>
       </c>
       <c r="N702" t="n">
-        <v>112996</v>
+        <v>113223</v>
       </c>
       <c r="O702" t="n">
-        <v>66740</v>
+        <v>66962</v>
       </c>
       <c r="P702" t="n">
-        <v>58783</v>
+        <v>59010</v>
       </c>
       <c r="Q702" t="n">
-        <v>34130</v>
+        <v>34352</v>
       </c>
       <c r="R702" t="n">
-        <v>12559</v>
+        <v>12635</v>
       </c>
       <c r="S702" t="n">
-        <v>9534.3</v>
+        <v>9566</v>
       </c>
       <c r="T702" t="n">
-        <v>6829</v>
+        <v>6905</v>
       </c>
       <c r="U702" t="n">
-        <v>4875.7</v>
+        <v>4907.4</v>
       </c>
       <c r="V702" t="n">
         <v>32</v>
@@ -56469,37 +56469,37 @@
         <v>101953</v>
       </c>
       <c r="K703" t="n">
-        <v>5260493</v>
+        <v>5260787</v>
       </c>
       <c r="L703" t="n">
-        <v>2909604</v>
+        <v>2909898</v>
       </c>
       <c r="M703" t="n">
         <v>11032</v>
       </c>
       <c r="N703" t="n">
-        <v>120228</v>
+        <v>120520</v>
       </c>
       <c r="O703" t="n">
-        <v>70517</v>
+        <v>70794</v>
       </c>
       <c r="P703" t="n">
-        <v>62175</v>
+        <v>62467</v>
       </c>
       <c r="Q703" t="n">
-        <v>36060</v>
+        <v>36337</v>
       </c>
       <c r="R703" t="n">
-        <v>13624</v>
+        <v>13689</v>
       </c>
       <c r="S703" t="n">
-        <v>10073.9</v>
+        <v>10113.4</v>
       </c>
       <c r="T703" t="n">
-        <v>6735</v>
+        <v>6800</v>
       </c>
       <c r="U703" t="n">
-        <v>5151.4</v>
+        <v>5191</v>
       </c>
       <c r="V703" t="n">
         <v>36</v>
@@ -56534,7 +56534,7 @@
         <v>14296</v>
       </c>
       <c r="F704" t="n">
-        <v>3274</v>
+        <v>3407</v>
       </c>
       <c r="G704" t="n">
         <v>6348</v>
@@ -56546,55 +56546,55 @@
         <v>608</v>
       </c>
       <c r="J704" t="n">
-        <v>97927</v>
+        <v>101983</v>
       </c>
       <c r="K704" t="n">
-        <v>5093079</v>
+        <v>5273411</v>
       </c>
       <c r="L704" t="n">
-        <v>2741316</v>
+        <v>2916123</v>
       </c>
       <c r="M704" t="n">
         <v>11038</v>
       </c>
       <c r="N704" t="n">
-        <v>-53843</v>
+        <v>126487</v>
       </c>
       <c r="O704" t="n">
-        <v>-106399</v>
+        <v>73906</v>
       </c>
       <c r="P704" t="n">
-        <v>-109790</v>
+        <v>65015</v>
       </c>
       <c r="Q704" t="n">
-        <v>-137226</v>
+        <v>37554</v>
       </c>
       <c r="R704" t="n">
-        <v>-167414</v>
+        <v>12624</v>
       </c>
       <c r="S704" t="n">
-        <v>-15199.9</v>
+        <v>10558</v>
       </c>
       <c r="T704" t="n">
-        <v>-168288</v>
+        <v>6225</v>
       </c>
       <c r="U704" t="n">
-        <v>-19603.7</v>
+        <v>5364.9</v>
       </c>
       <c r="V704" t="n">
-        <v>-4026</v>
+        <v>30</v>
       </c>
       <c r="W704" t="n">
-        <v>-3.9</v>
+        <v>0</v>
       </c>
       <c r="X704" t="n">
-        <v>-1319.3</v>
+        <v>32.7</v>
       </c>
       <c r="Y704" t="n">
-        <v>-545.7</v>
+        <v>33.7</v>
       </c>
       <c r="Z704" t="n">
-        <v>-3820</v>
+        <v>236</v>
       </c>
     </row>
     <row r="705">
@@ -56602,7 +56602,7 @@
         <v>44534</v>
       </c>
       <c r="B705" t="n">
-        <v>2608</v>
+        <v>3324</v>
       </c>
       <c r="C705" t="n">
         <v>837</v>
@@ -56614,7 +56614,7 @@
         <v>14506</v>
       </c>
       <c r="F705" t="n">
-        <v>2763</v>
+        <v>3438</v>
       </c>
       <c r="G705" t="n">
         <v>6341</v>
@@ -56623,58 +56623,58 @@
         <v>134038</v>
       </c>
       <c r="I705" t="n">
-        <v>338</v>
+        <v>422</v>
       </c>
       <c r="J705" t="n">
-        <v>74691</v>
+        <v>101998</v>
       </c>
       <c r="K705" t="n">
-        <v>3947797</v>
+        <v>5280088</v>
       </c>
       <c r="L705" t="n">
-        <v>2424931</v>
+        <v>2918688</v>
       </c>
       <c r="M705" t="n">
         <v>11040</v>
       </c>
       <c r="N705" t="n">
-        <v>-1203026</v>
+        <v>129263</v>
       </c>
       <c r="O705" t="n">
-        <v>-1256976</v>
+        <v>75284</v>
       </c>
       <c r="P705" t="n">
-        <v>-428155</v>
+        <v>65600</v>
       </c>
       <c r="Q705" t="n">
-        <v>-456313</v>
+        <v>37413</v>
       </c>
       <c r="R705" t="n">
-        <v>-1145282</v>
+        <v>6677</v>
       </c>
       <c r="S705" t="n">
-        <v>-179568</v>
+        <v>10754.9</v>
       </c>
       <c r="T705" t="n">
-        <v>-316385</v>
+        <v>2565</v>
       </c>
       <c r="U705" t="n">
-        <v>-65187.6</v>
+        <v>5344.7</v>
       </c>
       <c r="V705" t="n">
-        <v>-23236</v>
+        <v>15</v>
       </c>
       <c r="W705" t="n">
-        <v>-23.7</v>
+        <v>0</v>
       </c>
       <c r="X705" t="n">
-        <v>-9075.3</v>
+        <v>27</v>
       </c>
       <c r="Y705" t="n">
-        <v>-3865.9</v>
+        <v>35.1</v>
       </c>
       <c r="Z705" t="n">
-        <v>-27061</v>
+        <v>246</v>
       </c>
     </row>
     <row r="706">
@@ -56682,7 +56682,7 @@
         <v>44535</v>
       </c>
       <c r="B706" t="n">
-        <v>1909</v>
+        <v>2541</v>
       </c>
       <c r="C706" t="n">
         <v>457</v>
@@ -56694,7 +56694,7 @@
         <v>15047</v>
       </c>
       <c r="F706" t="n">
-        <v>2595</v>
+        <v>3527</v>
       </c>
       <c r="G706" t="n">
         <v>6316</v>
@@ -56703,58 +56703,58 @@
         <v>6316</v>
       </c>
       <c r="I706" t="n">
-        <v>289</v>
+        <v>372</v>
       </c>
       <c r="J706" t="n">
-        <v>67836</v>
+        <v>102003</v>
       </c>
       <c r="K706" t="n">
-        <v>3846416</v>
+        <v>5284100</v>
       </c>
       <c r="L706" t="n">
-        <v>1489596</v>
+        <v>2920521</v>
       </c>
       <c r="M706" t="n">
         <v>11042</v>
       </c>
       <c r="N706" t="n">
-        <v>-1307811</v>
+        <v>129871</v>
       </c>
       <c r="O706" t="n">
-        <v>-1363260</v>
+        <v>74406</v>
       </c>
       <c r="P706" t="n">
-        <v>-1365479</v>
+        <v>65444</v>
       </c>
       <c r="Q706" t="n">
-        <v>-1394469</v>
+        <v>36438</v>
       </c>
       <c r="R706" t="n">
-        <v>-101381</v>
+        <v>4012</v>
       </c>
       <c r="S706" t="n">
-        <v>-194751.4</v>
+        <v>10629.4</v>
       </c>
       <c r="T706" t="n">
-        <v>-935335</v>
+        <v>1833</v>
       </c>
       <c r="U706" t="n">
-        <v>-199209.9</v>
+        <v>5205.4</v>
       </c>
       <c r="V706" t="n">
-        <v>-6855</v>
+        <v>5</v>
       </c>
       <c r="W706" t="n">
-        <v>-9.2</v>
+        <v>0</v>
       </c>
       <c r="X706" t="n">
-        <v>-11372.3</v>
+        <v>16.7</v>
       </c>
       <c r="Y706" t="n">
-        <v>-4847</v>
+        <v>34</v>
       </c>
       <c r="Z706" t="n">
-        <v>-33929</v>
+        <v>238</v>
       </c>
     </row>
     <row r="707">
@@ -56762,79 +56762,159 @@
         <v>44536</v>
       </c>
       <c r="B707" t="n">
-        <v>0</v>
+        <v>719</v>
       </c>
       <c r="C707" t="n">
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="D707" t="n">
-        <v>0</v>
+        <v>119864</v>
       </c>
       <c r="E707" t="n">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="F707" t="n">
-        <v>566</v>
+        <v>3670</v>
       </c>
       <c r="G707" t="n">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="H707" t="n">
-        <v>0</v>
+        <v>127817</v>
       </c>
       <c r="I707" t="n">
-        <v>0</v>
+        <v>379</v>
       </c>
       <c r="J707" t="n">
-        <v>16180</v>
+        <v>102018</v>
       </c>
       <c r="K707" t="n">
-        <v>929296</v>
+        <v>5288442</v>
       </c>
       <c r="L707" t="n">
-        <v>285424</v>
+        <v>2921450</v>
       </c>
       <c r="M707" t="n">
-        <v>0</v>
+        <v>11064</v>
       </c>
       <c r="N707" t="n">
-        <v>-4234017</v>
+        <v>125126</v>
       </c>
       <c r="O707" t="n">
-        <v>-4293236</v>
+        <v>65846</v>
       </c>
       <c r="P707" t="n">
-        <v>-2574117</v>
+        <v>61906</v>
       </c>
       <c r="Q707" t="n">
-        <v>-2604473</v>
+        <v>31489</v>
       </c>
       <c r="R707" t="n">
-        <v>-2917120</v>
+        <v>4342</v>
       </c>
       <c r="S707" t="n">
-        <v>-613319.4</v>
+        <v>9406.6</v>
       </c>
       <c r="T707" t="n">
-        <v>-1204172</v>
+        <v>929</v>
       </c>
       <c r="U707" t="n">
-        <v>-372067.6</v>
+        <v>4498.4</v>
       </c>
       <c r="V707" t="n">
-        <v>-51656</v>
+        <v>15</v>
       </c>
       <c r="W707" t="n">
-        <v>-76.1</v>
+        <v>0</v>
       </c>
       <c r="X707" t="n">
-        <v>-27249</v>
+        <v>11.7</v>
       </c>
       <c r="Y707" t="n">
-        <v>-12231.9</v>
+        <v>30.7</v>
       </c>
       <c r="Z707" t="n">
-        <v>-85623</v>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" s="1" t="n">
+        <v>44537</v>
+      </c>
+      <c r="B708" t="n">
+        <v>3953</v>
+      </c>
+      <c r="C708" t="n">
+        <v>1284</v>
+      </c>
+      <c r="D708" t="n">
+        <v>0</v>
+      </c>
+      <c r="E708" t="n">
+        <v>0</v>
+      </c>
+      <c r="F708" t="n">
+        <v>3812</v>
+      </c>
+      <c r="G708" t="n">
+        <v>0</v>
+      </c>
+      <c r="H708" t="n">
+        <v>0</v>
+      </c>
+      <c r="I708" t="n">
+        <v>245</v>
+      </c>
+      <c r="J708" t="n">
+        <v>102028</v>
+      </c>
+      <c r="K708" t="n">
+        <v>5297852</v>
+      </c>
+      <c r="L708" t="n">
+        <v>2923257</v>
+      </c>
+      <c r="M708" t="n">
+        <v>0</v>
+      </c>
+      <c r="N708" t="n">
+        <v>126885</v>
+      </c>
+      <c r="O708" t="n">
+        <v>63389</v>
+      </c>
+      <c r="P708" t="n">
+        <v>59294</v>
+      </c>
+      <c r="Q708" t="n">
+        <v>27064</v>
+      </c>
+      <c r="R708" t="n">
+        <v>9410</v>
+      </c>
+      <c r="S708" t="n">
+        <v>9055.6</v>
+      </c>
+      <c r="T708" t="n">
+        <v>1807</v>
+      </c>
+      <c r="U708" t="n">
+        <v>3866.3</v>
+      </c>
+      <c r="V708" t="n">
+        <v>10</v>
+      </c>
+      <c r="W708" t="n">
+        <v>0</v>
+      </c>
+      <c r="X708" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y708" t="n">
+        <v>20.4</v>
+      </c>
+      <c r="Z708" t="n">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrige datos CLM 2021-12-22
</commit_message>
<xml_diff>
--- a/data/output/covid19-spain_consolidated.xlsx
+++ b/data/output/covid19-spain_consolidated.xlsx
@@ -57965,7 +57965,7 @@
         <v>17233</v>
       </c>
       <c r="C722" t="n">
-        <v>253915</v>
+        <v>7840</v>
       </c>
       <c r="D722" t="n">
         <v>120664</v>
@@ -57974,7 +57974,7 @@
         <v>38804</v>
       </c>
       <c r="F722" t="n">
-        <v>38424</v>
+        <v>6039</v>
       </c>
       <c r="G722" t="n">
         <v>6765</v>
@@ -57983,58 +57983,58 @@
         <v>135703</v>
       </c>
       <c r="I722" t="n">
-        <v>11168</v>
+        <v>1223</v>
       </c>
       <c r="J722" t="n">
-        <v>1736788</v>
+        <v>103003</v>
       </c>
       <c r="K722" t="n">
-        <v>70758132</v>
+        <v>5720892</v>
       </c>
       <c r="L722" t="n">
-        <v>68216171</v>
+        <v>3178931</v>
       </c>
       <c r="M722" t="n">
         <v>11475</v>
       </c>
       <c r="N722" t="n">
-        <v>65433881</v>
+        <v>396641</v>
       </c>
       <c r="O722" t="n">
-        <v>65295616</v>
+        <v>258376</v>
       </c>
       <c r="P722" t="n">
-        <v>65272502</v>
+        <v>235262</v>
       </c>
       <c r="Q722" t="n">
-        <v>65194769</v>
+        <v>157529</v>
       </c>
       <c r="R722" t="n">
-        <v>65089733</v>
+        <v>52493</v>
       </c>
       <c r="S722" t="n">
-        <v>9327945.1</v>
+        <v>36910.9</v>
       </c>
       <c r="T722" t="n">
-        <v>65072110</v>
+        <v>34870</v>
       </c>
       <c r="U722" t="n">
-        <v>9313538.4</v>
+        <v>22504.1</v>
       </c>
       <c r="V722" t="n">
-        <v>1633907</v>
+        <v>122</v>
       </c>
       <c r="W722" t="n">
-        <v>1588.2</v>
+        <v>0.1</v>
       </c>
       <c r="X722" t="n">
-        <v>544676.3</v>
+        <v>81.3</v>
       </c>
       <c r="Y722" t="n">
-        <v>233467.9</v>
+        <v>70</v>
       </c>
       <c r="Z722" t="n">
-        <v>1634275</v>
+        <v>490</v>
       </c>
     </row>
     <row r="723">
@@ -58045,7 +58045,7 @@
         <v>16588</v>
       </c>
       <c r="C723" t="n">
-        <v>532582</v>
+        <v>10087</v>
       </c>
       <c r="D723" t="n">
         <v>120830</v>
@@ -58054,7 +58054,7 @@
         <v>45695</v>
       </c>
       <c r="F723" t="n">
-        <v>39473</v>
+        <v>6068</v>
       </c>
       <c r="G723" t="n">
         <v>6757</v>
@@ -58063,58 +58063,58 @@
         <v>135866</v>
       </c>
       <c r="I723" t="n">
-        <v>10553</v>
+        <v>1118</v>
       </c>
       <c r="J723" t="n">
-        <v>1737338</v>
+        <v>103043</v>
       </c>
       <c r="K723" t="n">
-        <v>71332521</v>
+        <v>5772786</v>
       </c>
       <c r="L723" t="n">
-        <v>68772199</v>
+        <v>3212464</v>
       </c>
       <c r="M723" t="n">
         <v>0</v>
       </c>
       <c r="N723" t="n">
-        <v>65996578</v>
+        <v>436843</v>
       </c>
       <c r="O723" t="n">
-        <v>65836360</v>
+        <v>276625</v>
       </c>
       <c r="P723" t="n">
-        <v>65822316</v>
+        <v>262581</v>
       </c>
       <c r="Q723" t="n">
-        <v>65730031</v>
+        <v>170296</v>
       </c>
       <c r="R723" t="n">
-        <v>574389</v>
+        <v>51894</v>
       </c>
       <c r="S723" t="n">
-        <v>9405194.3</v>
+        <v>39517.9</v>
       </c>
       <c r="T723" t="n">
-        <v>556028</v>
+        <v>33533</v>
       </c>
       <c r="U723" t="n">
-        <v>9390004.4</v>
+        <v>24328</v>
       </c>
       <c r="V723" t="n">
-        <v>550</v>
+        <v>40</v>
       </c>
       <c r="W723" t="n">
         <v>0</v>
       </c>
       <c r="X723" t="n">
-        <v>544847.7</v>
+        <v>82.7</v>
       </c>
       <c r="Y723" t="n">
-        <v>233535</v>
+        <v>64.3</v>
       </c>
       <c r="Z723" t="n">
-        <v>1634745</v>
+        <v>450</v>
       </c>
     </row>
     <row r="724">
@@ -58125,7 +58125,7 @@
         <v>5002</v>
       </c>
       <c r="C724" t="n">
-        <v>628788</v>
+        <v>3528</v>
       </c>
       <c r="D724" t="n">
         <v>0</v>
@@ -58134,7 +58134,7 @@
         <v>4078</v>
       </c>
       <c r="F724" t="n">
-        <v>34705</v>
+        <v>1810</v>
       </c>
       <c r="G724" t="n">
         <v>0</v>
@@ -58143,58 +58143,58 @@
         <v>0</v>
       </c>
       <c r="I724" t="n">
-        <v>9927</v>
+        <v>237</v>
       </c>
       <c r="J724" t="n">
-        <v>1670823</v>
+        <v>35763</v>
       </c>
       <c r="K724" t="n">
-        <v>68041150</v>
+        <v>1856155</v>
       </c>
       <c r="L724" t="n">
-        <v>66842765</v>
+        <v>657770</v>
       </c>
       <c r="M724" t="n">
         <v>0</v>
       </c>
       <c r="N724" t="n">
-        <v>62685319</v>
+        <v>-3499676</v>
       </c>
       <c r="O724" t="n">
-        <v>62508312</v>
+        <v>-3676683</v>
       </c>
       <c r="P724" t="n">
-        <v>63881578</v>
+        <v>-2303417</v>
       </c>
       <c r="Q724" t="n">
-        <v>63779211</v>
+        <v>-2405784</v>
       </c>
       <c r="R724" t="n">
-        <v>-3291371</v>
+        <v>-3916631</v>
       </c>
       <c r="S724" t="n">
-        <v>8929758.9</v>
+        <v>-525240.4</v>
       </c>
       <c r="T724" t="n">
-        <v>-1929434</v>
+        <v>-2554694</v>
       </c>
       <c r="U724" t="n">
-        <v>9111315.9</v>
+        <v>-343683.4</v>
       </c>
       <c r="V724" t="n">
-        <v>-66515</v>
+        <v>-67280</v>
       </c>
       <c r="W724" t="n">
-        <v>-3.8</v>
+        <v>-65.3</v>
       </c>
       <c r="X724" t="n">
-        <v>522647.3</v>
+        <v>-22372.7</v>
       </c>
       <c r="Y724" t="n">
-        <v>224022.9</v>
+        <v>-9557.1</v>
       </c>
       <c r="Z724" t="n">
-        <v>1568160</v>
+        <v>-66900</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualiza datos provincias 2022-03-14
</commit_message>
<xml_diff>
--- a/data/output/covid19-spain_consolidated.xlsx
+++ b/data/output/covid19-spain_consolidated.xlsx
@@ -58069,37 +58069,37 @@
         <v>110093</v>
       </c>
       <c r="K723" t="n">
-        <v>6589176</v>
+        <v>6589175</v>
       </c>
       <c r="L723" t="n">
-        <v>4023235</v>
+        <v>4023234</v>
       </c>
       <c r="M723" t="n">
         <v>11527</v>
       </c>
       <c r="N723" t="n">
-        <v>600923</v>
+        <v>600922</v>
       </c>
       <c r="O723" t="n">
-        <v>404133</v>
+        <v>404132</v>
       </c>
       <c r="P723" t="n">
-        <v>422454</v>
+        <v>422453</v>
       </c>
       <c r="Q723" t="n">
-        <v>293745</v>
+        <v>293744</v>
       </c>
       <c r="R723" t="n">
-        <v>93725</v>
+        <v>93724</v>
       </c>
       <c r="S723" t="n">
-        <v>57733.3</v>
+        <v>57733.1</v>
       </c>
       <c r="T723" t="n">
-        <v>71543</v>
+        <v>71542</v>
       </c>
       <c r="U723" t="n">
-        <v>41963.6</v>
+        <v>41963.4</v>
       </c>
       <c r="V723" t="n">
         <v>123</v>
@@ -58149,37 +58149,37 @@
         <v>110189</v>
       </c>
       <c r="K724" t="n">
-        <v>6690996</v>
+        <v>6690995</v>
       </c>
       <c r="L724" t="n">
-        <v>4099857</v>
+        <v>4099856</v>
       </c>
       <c r="M724" t="n">
         <v>11573</v>
       </c>
       <c r="N724" t="n">
-        <v>679790</v>
+        <v>679789</v>
       </c>
       <c r="O724" t="n">
-        <v>458271</v>
+        <v>458270</v>
       </c>
       <c r="P724" t="n">
-        <v>484719</v>
+        <v>484718</v>
       </c>
       <c r="Q724" t="n">
-        <v>338018</v>
+        <v>338017</v>
       </c>
       <c r="R724" t="n">
         <v>101820</v>
       </c>
       <c r="S724" t="n">
-        <v>65467.3</v>
+        <v>65467.1</v>
       </c>
       <c r="T724" t="n">
         <v>76622</v>
       </c>
       <c r="U724" t="n">
-        <v>48288.3</v>
+        <v>48288.1</v>
       </c>
       <c r="V724" t="n">
         <v>96</v>
@@ -58229,37 +58229,37 @@
         <v>110259</v>
       </c>
       <c r="K725" t="n">
-        <v>6768700</v>
+        <v>6768699</v>
       </c>
       <c r="L725" t="n">
-        <v>4155926</v>
+        <v>4155925</v>
       </c>
       <c r="M725" t="n">
         <v>11575</v>
       </c>
       <c r="N725" t="n">
-        <v>731157</v>
+        <v>731156</v>
       </c>
       <c r="O725" t="n">
-        <v>486022</v>
+        <v>486021</v>
       </c>
       <c r="P725" t="n">
-        <v>524232</v>
+        <v>524231</v>
       </c>
       <c r="Q725" t="n">
-        <v>358383</v>
+        <v>358382</v>
       </c>
       <c r="R725" t="n">
         <v>77704</v>
       </c>
       <c r="S725" t="n">
-        <v>69431.7</v>
+        <v>69431.6</v>
       </c>
       <c r="T725" t="n">
         <v>56069</v>
       </c>
       <c r="U725" t="n">
-        <v>51197.6</v>
+        <v>51197.4</v>
       </c>
       <c r="V725" t="n">
         <v>70</v>
@@ -58309,37 +58309,37 @@
         <v>110342</v>
       </c>
       <c r="K726" t="n">
-        <v>6811396</v>
+        <v>6811395</v>
       </c>
       <c r="L726" t="n">
-        <v>4190199</v>
+        <v>4190198</v>
       </c>
       <c r="M726" t="n">
         <v>11580</v>
       </c>
       <c r="N726" t="n">
-        <v>758790</v>
+        <v>758789</v>
       </c>
       <c r="O726" t="n">
-        <v>499556</v>
+        <v>499555</v>
       </c>
       <c r="P726" t="n">
-        <v>547711</v>
+        <v>547710</v>
       </c>
       <c r="Q726" t="n">
-        <v>370863</v>
+        <v>370862</v>
       </c>
       <c r="R726" t="n">
         <v>42696</v>
       </c>
       <c r="S726" t="n">
-        <v>71365.1</v>
+        <v>71365</v>
       </c>
       <c r="T726" t="n">
         <v>34273</v>
       </c>
       <c r="U726" t="n">
-        <v>52980.4</v>
+        <v>52980.3</v>
       </c>
       <c r="V726" t="n">
         <v>83</v>
@@ -58389,37 +58389,37 @@
         <v>110417</v>
       </c>
       <c r="K727" t="n">
-        <v>6871575</v>
+        <v>6871574</v>
       </c>
       <c r="L727" t="n">
-        <v>4236470</v>
+        <v>4236469</v>
       </c>
       <c r="M727" t="n">
         <v>11614</v>
       </c>
       <c r="N727" t="n">
-        <v>803010</v>
+        <v>803009</v>
       </c>
       <c r="O727" t="n">
-        <v>531973</v>
+        <v>531972</v>
       </c>
       <c r="P727" t="n">
-        <v>583508</v>
+        <v>583507</v>
       </c>
       <c r="Q727" t="n">
-        <v>396415</v>
+        <v>396414</v>
       </c>
       <c r="R727" t="n">
         <v>60179</v>
       </c>
       <c r="S727" t="n">
-        <v>75996.1</v>
+        <v>75996</v>
       </c>
       <c r="T727" t="n">
         <v>46271</v>
       </c>
       <c r="U727" t="n">
-        <v>56630.7</v>
+        <v>56630.6</v>
       </c>
       <c r="V727" t="n">
         <v>75</v>
@@ -58469,37 +58469,37 @@
         <v>110543</v>
       </c>
       <c r="K728" t="n">
-        <v>7032708</v>
+        <v>7032707</v>
       </c>
       <c r="L728" t="n">
-        <v>4340252</v>
+        <v>4340251</v>
       </c>
       <c r="M728" t="n">
         <v>11689</v>
       </c>
       <c r="N728" t="n">
-        <v>928081</v>
+        <v>928080</v>
       </c>
       <c r="O728" t="n">
-        <v>616404</v>
+        <v>616403</v>
       </c>
       <c r="P728" t="n">
-        <v>666728</v>
+        <v>666727</v>
       </c>
       <c r="Q728" t="n">
-        <v>450016</v>
+        <v>450015</v>
       </c>
       <c r="R728" t="n">
         <v>161133</v>
       </c>
       <c r="S728" t="n">
-        <v>88057.7</v>
+        <v>88057.6</v>
       </c>
       <c r="T728" t="n">
         <v>103782</v>
       </c>
       <c r="U728" t="n">
-        <v>64288</v>
+        <v>64287.9</v>
       </c>
       <c r="V728" t="n">
         <v>126</v>
@@ -58549,37 +58549,37 @@
         <v>110747</v>
       </c>
       <c r="K729" t="n">
-        <v>7181393</v>
+        <v>7181392</v>
       </c>
       <c r="L729" t="n">
-        <v>4451754</v>
+        <v>4451753</v>
       </c>
       <c r="M729" t="n">
         <v>11761</v>
       </c>
       <c r="N729" t="n">
-        <v>1039811</v>
+        <v>1039810</v>
       </c>
       <c r="O729" t="n">
-        <v>685942</v>
+        <v>685941</v>
       </c>
       <c r="P729" t="n">
-        <v>752816</v>
+        <v>752815</v>
       </c>
       <c r="Q729" t="n">
-        <v>500062</v>
+        <v>500061</v>
       </c>
       <c r="R729" t="n">
         <v>148685</v>
       </c>
       <c r="S729" t="n">
-        <v>97991.7</v>
+        <v>97991.6</v>
       </c>
       <c r="T729" t="n">
         <v>111502</v>
       </c>
       <c r="U729" t="n">
-        <v>71437.4</v>
+        <v>71437.3</v>
       </c>
       <c r="V729" t="n">
         <v>204</v>
@@ -58629,22 +58629,22 @@
         <v>110877</v>
       </c>
       <c r="K730" t="n">
-        <v>7342427</v>
+        <v>7342426</v>
       </c>
       <c r="L730" t="n">
-        <v>4564308</v>
+        <v>4564307</v>
       </c>
       <c r="M730" t="n">
         <v>11818</v>
       </c>
       <c r="N730" t="n">
-        <v>1157384</v>
+        <v>1157383</v>
       </c>
       <c r="O730" t="n">
         <v>753251</v>
       </c>
       <c r="P730" t="n">
-        <v>834818</v>
+        <v>834817</v>
       </c>
       <c r="Q730" t="n">
         <v>541073</v>
@@ -58709,22 +58709,22 @@
         <v>111027</v>
       </c>
       <c r="K731" t="n">
-        <v>7495020</v>
+        <v>7495019</v>
       </c>
       <c r="L731" t="n">
-        <v>4667589</v>
+        <v>4667588</v>
       </c>
       <c r="M731" t="n">
         <v>11883</v>
       </c>
       <c r="N731" t="n">
-        <v>1262295</v>
+        <v>1262294</v>
       </c>
       <c r="O731" t="n">
         <v>804024</v>
       </c>
       <c r="P731" t="n">
-        <v>905750</v>
+        <v>905749</v>
       </c>
       <c r="Q731" t="n">
         <v>567732</v>
@@ -58789,22 +58789,22 @@
         <v>111113</v>
       </c>
       <c r="K732" t="n">
-        <v>7603140</v>
+        <v>7603139</v>
       </c>
       <c r="L732" t="n">
-        <v>4736592</v>
+        <v>4736591</v>
       </c>
       <c r="M732" t="n">
         <v>11888</v>
       </c>
       <c r="N732" t="n">
-        <v>1320462</v>
+        <v>1320461</v>
       </c>
       <c r="O732" t="n">
         <v>834440</v>
       </c>
       <c r="P732" t="n">
-        <v>939049</v>
+        <v>939048</v>
       </c>
       <c r="Q732" t="n">
         <v>580666</v>
@@ -58869,22 +58869,22 @@
         <v>111235</v>
       </c>
       <c r="K733" t="n">
-        <v>7655578</v>
+        <v>7655577</v>
       </c>
       <c r="L733" t="n">
-        <v>4774089</v>
+        <v>4774088</v>
       </c>
       <c r="M733" t="n">
         <v>11905</v>
       </c>
       <c r="N733" t="n">
-        <v>1343738</v>
+        <v>1343737</v>
       </c>
       <c r="O733" t="n">
         <v>844182</v>
       </c>
       <c r="P733" t="n">
-        <v>954753</v>
+        <v>954752</v>
       </c>
       <c r="Q733" t="n">
         <v>583890</v>
@@ -58949,22 +58949,22 @@
         <v>111326</v>
       </c>
       <c r="K734" t="n">
-        <v>7740673</v>
+        <v>7740672</v>
       </c>
       <c r="L734" t="n">
-        <v>4831943</v>
+        <v>4831942</v>
       </c>
       <c r="M734" t="n">
         <v>11939</v>
       </c>
       <c r="N734" t="n">
-        <v>1401071</v>
+        <v>1401070</v>
       </c>
       <c r="O734" t="n">
         <v>869098</v>
       </c>
       <c r="P734" t="n">
-        <v>991888</v>
+        <v>991887</v>
       </c>
       <c r="Q734" t="n">
         <v>595473</v>
@@ -59029,22 +59029,22 @@
         <v>111527</v>
       </c>
       <c r="K735" t="n">
-        <v>7965218</v>
+        <v>7965217</v>
       </c>
       <c r="L735" t="n">
-        <v>4956554</v>
+        <v>4956553</v>
       </c>
       <c r="M735" t="n">
         <v>12076</v>
       </c>
       <c r="N735" t="n">
-        <v>1548914</v>
+        <v>1548913</v>
       </c>
       <c r="O735" t="n">
         <v>932510</v>
       </c>
       <c r="P735" t="n">
-        <v>1066318</v>
+        <v>1066317</v>
       </c>
       <c r="Q735" t="n">
         <v>616302</v>
@@ -59109,22 +59109,22 @@
         <v>111828</v>
       </c>
       <c r="K736" t="n">
-        <v>8137408</v>
+        <v>8137407</v>
       </c>
       <c r="L736" t="n">
-        <v>5073963</v>
+        <v>5073962</v>
       </c>
       <c r="M736" t="n">
         <v>12163</v>
       </c>
       <c r="N736" t="n">
-        <v>1641957</v>
+        <v>1641956</v>
       </c>
       <c r="O736" t="n">
         <v>956015</v>
       </c>
       <c r="P736" t="n">
-        <v>1122271</v>
+        <v>1122270</v>
       </c>
       <c r="Q736" t="n">
         <v>622209</v>
@@ -59189,37 +59189,37 @@
         <v>111989</v>
       </c>
       <c r="K737" t="n">
-        <v>8300701</v>
+        <v>8300699</v>
       </c>
       <c r="L737" t="n">
-        <v>5187773</v>
+        <v>5187771</v>
       </c>
       <c r="M737" t="n">
         <v>12259</v>
       </c>
       <c r="N737" t="n">
-        <v>1711525</v>
+        <v>1711524</v>
       </c>
       <c r="O737" t="n">
-        <v>958274</v>
+        <v>958273</v>
       </c>
       <c r="P737" t="n">
-        <v>1164538</v>
+        <v>1164537</v>
       </c>
       <c r="Q737" t="n">
-        <v>623465</v>
+        <v>623464</v>
       </c>
       <c r="R737" t="n">
-        <v>163293</v>
+        <v>163292</v>
       </c>
       <c r="S737" t="n">
-        <v>136896.3</v>
+        <v>136896.1</v>
       </c>
       <c r="T737" t="n">
-        <v>113810</v>
+        <v>113809</v>
       </c>
       <c r="U737" t="n">
-        <v>89066.4</v>
+        <v>89066.3</v>
       </c>
       <c r="V737" t="n">
         <v>161</v>
@@ -59269,37 +59269,37 @@
         <v>112177</v>
       </c>
       <c r="K738" t="n">
-        <v>8398615</v>
+        <v>8398613</v>
       </c>
       <c r="L738" t="n">
-        <v>5248778</v>
+        <v>5248776</v>
       </c>
       <c r="M738" t="n">
         <v>12325</v>
       </c>
       <c r="N738" t="n">
-        <v>1707619</v>
+        <v>1707618</v>
       </c>
       <c r="O738" t="n">
-        <v>903595</v>
+        <v>903594</v>
       </c>
       <c r="P738" t="n">
-        <v>1148921</v>
+        <v>1148920</v>
       </c>
       <c r="Q738" t="n">
-        <v>581189</v>
+        <v>581188</v>
       </c>
       <c r="R738" t="n">
         <v>97914</v>
       </c>
       <c r="S738" t="n">
-        <v>129085</v>
+        <v>129084.9</v>
       </c>
       <c r="T738" t="n">
         <v>61005</v>
       </c>
       <c r="U738" t="n">
-        <v>83027</v>
+        <v>83026.9</v>
       </c>
       <c r="V738" t="n">
         <v>188</v>
@@ -59349,37 +59349,37 @@
         <v>112372</v>
       </c>
       <c r="K739" t="n">
-        <v>8582673</v>
+        <v>8582671</v>
       </c>
       <c r="L739" t="n">
-        <v>5363835</v>
+        <v>5363833</v>
       </c>
       <c r="M739" t="n">
         <v>12463</v>
       </c>
       <c r="N739" t="n">
-        <v>1813973</v>
+        <v>1813972</v>
       </c>
       <c r="O739" t="n">
-        <v>979533</v>
+        <v>979532</v>
       </c>
       <c r="P739" t="n">
-        <v>1207909</v>
+        <v>1207908</v>
       </c>
       <c r="Q739" t="n">
-        <v>627243</v>
+        <v>627242</v>
       </c>
       <c r="R739" t="n">
         <v>184058</v>
       </c>
       <c r="S739" t="n">
-        <v>139933.3</v>
+        <v>139933.1</v>
       </c>
       <c r="T739" t="n">
         <v>115057</v>
       </c>
       <c r="U739" t="n">
-        <v>89606.1</v>
+        <v>89606</v>
       </c>
       <c r="V739" t="n">
         <v>195</v>
@@ -59429,37 +59429,37 @@
         <v>112545</v>
       </c>
       <c r="K740" t="n">
-        <v>8680099</v>
+        <v>8680097</v>
       </c>
       <c r="L740" t="n">
-        <v>5427912</v>
+        <v>5427910</v>
       </c>
       <c r="M740" t="n">
         <v>12514</v>
       </c>
       <c r="N740" t="n">
-        <v>1868703</v>
+        <v>1868702</v>
       </c>
       <c r="O740" t="n">
-        <v>1024521</v>
+        <v>1024520</v>
       </c>
       <c r="P740" t="n">
-        <v>1237713</v>
+        <v>1237712</v>
       </c>
       <c r="Q740" t="n">
-        <v>653823</v>
+        <v>653822</v>
       </c>
       <c r="R740" t="n">
         <v>97426</v>
       </c>
       <c r="S740" t="n">
-        <v>146360.1</v>
+        <v>146360</v>
       </c>
       <c r="T740" t="n">
         <v>64077</v>
       </c>
       <c r="U740" t="n">
-        <v>93403.3</v>
+        <v>93403.1</v>
       </c>
       <c r="V740" t="n">
         <v>173</v>
@@ -59509,37 +59509,37 @@
         <v>112707</v>
       </c>
       <c r="K741" t="n">
-        <v>8780692</v>
+        <v>8780690</v>
       </c>
       <c r="L741" t="n">
-        <v>5497681</v>
+        <v>5497679</v>
       </c>
       <c r="M741" t="n">
         <v>12587</v>
       </c>
       <c r="N741" t="n">
-        <v>1909117</v>
+        <v>1909116</v>
       </c>
       <c r="O741" t="n">
-        <v>1040019</v>
+        <v>1040018</v>
       </c>
       <c r="P741" t="n">
-        <v>1261211</v>
+        <v>1261210</v>
       </c>
       <c r="Q741" t="n">
-        <v>665738</v>
+        <v>665737</v>
       </c>
       <c r="R741" t="n">
         <v>100593</v>
       </c>
       <c r="S741" t="n">
-        <v>148574.1</v>
+        <v>148574</v>
       </c>
       <c r="T741" t="n">
         <v>69769</v>
       </c>
       <c r="U741" t="n">
-        <v>95105.4</v>
+        <v>95105.3</v>
       </c>
       <c r="V741" t="n">
         <v>162</v>
@@ -59589,37 +59589,37 @@
         <v>112964</v>
       </c>
       <c r="K742" t="n">
-        <v>9004996</v>
+        <v>9004994</v>
       </c>
       <c r="L742" t="n">
-        <v>5639338</v>
+        <v>5639336</v>
       </c>
       <c r="M742" t="n">
         <v>12758</v>
       </c>
       <c r="N742" t="n">
-        <v>1972288</v>
+        <v>1972287</v>
       </c>
       <c r="O742" t="n">
-        <v>1039778</v>
+        <v>1039777</v>
       </c>
       <c r="P742" t="n">
-        <v>1299086</v>
+        <v>1299085</v>
       </c>
       <c r="Q742" t="n">
-        <v>682784</v>
+        <v>682783</v>
       </c>
       <c r="R742" t="n">
         <v>224304</v>
       </c>
       <c r="S742" t="n">
-        <v>148539.7</v>
+        <v>148539.6</v>
       </c>
       <c r="T742" t="n">
         <v>141657</v>
       </c>
       <c r="U742" t="n">
-        <v>97540.6</v>
+        <v>97540.4</v>
       </c>
       <c r="V742" t="n">
         <v>257</v>
@@ -59669,37 +59669,37 @@
         <v>113293</v>
       </c>
       <c r="K743" t="n">
-        <v>9201577</v>
+        <v>9201575</v>
       </c>
       <c r="L743" t="n">
-        <v>5770092</v>
+        <v>5770090</v>
       </c>
       <c r="M743" t="n">
         <v>12957</v>
       </c>
       <c r="N743" t="n">
-        <v>2020184</v>
+        <v>2020183</v>
       </c>
       <c r="O743" t="n">
-        <v>1064169</v>
+        <v>1064168</v>
       </c>
       <c r="P743" t="n">
-        <v>1318338</v>
+        <v>1318337</v>
       </c>
       <c r="Q743" t="n">
-        <v>696129</v>
+        <v>696128</v>
       </c>
       <c r="R743" t="n">
         <v>196581</v>
       </c>
       <c r="S743" t="n">
-        <v>152024.1</v>
+        <v>152024</v>
       </c>
       <c r="T743" t="n">
         <v>130754</v>
       </c>
       <c r="U743" t="n">
-        <v>99447</v>
+        <v>99446.9</v>
       </c>
       <c r="V743" t="n">
         <v>329</v>
@@ -59749,22 +59749,22 @@
         <v>113580</v>
       </c>
       <c r="K744" t="n">
-        <v>9394232</v>
+        <v>9394230</v>
       </c>
       <c r="L744" t="n">
-        <v>5897695</v>
+        <v>5897693</v>
       </c>
       <c r="M744" t="n">
         <v>13206</v>
       </c>
       <c r="N744" t="n">
-        <v>2051805</v>
+        <v>2051804</v>
       </c>
       <c r="O744" t="n">
         <v>1093531</v>
       </c>
       <c r="P744" t="n">
-        <v>1333387</v>
+        <v>1333386</v>
       </c>
       <c r="Q744" t="n">
         <v>709922</v>
@@ -59829,22 +59829,22 @@
         <v>113843</v>
       </c>
       <c r="K745" t="n">
-        <v>9568224</v>
+        <v>9568222</v>
       </c>
       <c r="L745" t="n">
-        <v>6005455</v>
+        <v>6005453</v>
       </c>
       <c r="M745" t="n">
         <v>13428</v>
       </c>
       <c r="N745" t="n">
-        <v>2073204</v>
+        <v>2073203</v>
       </c>
       <c r="O745" t="n">
         <v>1169609</v>
       </c>
       <c r="P745" t="n">
-        <v>1337866</v>
+        <v>1337865</v>
       </c>
       <c r="Q745" t="n">
         <v>756677</v>
@@ -59909,22 +59909,22 @@
         <v>114094</v>
       </c>
       <c r="K746" t="n">
-        <v>9744944</v>
+        <v>9744942</v>
       </c>
       <c r="L746" t="n">
-        <v>6118771</v>
+        <v>6118769</v>
       </c>
       <c r="M746" t="n">
         <v>13681</v>
       </c>
       <c r="N746" t="n">
-        <v>2141804</v>
+        <v>2141803</v>
       </c>
       <c r="O746" t="n">
         <v>1162271</v>
       </c>
       <c r="P746" t="n">
-        <v>1382179</v>
+        <v>1382178</v>
       </c>
       <c r="Q746" t="n">
         <v>754936</v>
@@ -59989,22 +59989,22 @@
         <v>114299</v>
       </c>
       <c r="K747" t="n">
-        <v>9830550</v>
+        <v>9830548</v>
       </c>
       <c r="L747" t="n">
-        <v>6176811</v>
+        <v>6176809</v>
       </c>
       <c r="M747" t="n">
         <v>13093</v>
       </c>
       <c r="N747" t="n">
-        <v>2174972</v>
+        <v>2174971</v>
       </c>
       <c r="O747" t="n">
         <v>1150451</v>
       </c>
       <c r="P747" t="n">
-        <v>1402722</v>
+        <v>1402721</v>
       </c>
       <c r="Q747" t="n">
         <v>748899</v>
@@ -60069,22 +60069,22 @@
         <v>114478</v>
       </c>
       <c r="K748" t="n">
-        <v>9924717</v>
+        <v>9924715</v>
       </c>
       <c r="L748" t="n">
-        <v>6239641</v>
+        <v>6239639</v>
       </c>
       <c r="M748" t="n">
         <v>13828</v>
       </c>
       <c r="N748" t="n">
-        <v>2184044</v>
+        <v>2184043</v>
       </c>
       <c r="O748" t="n">
         <v>1144025</v>
       </c>
       <c r="P748" t="n">
-        <v>1407698</v>
+        <v>1407697</v>
       </c>
       <c r="Q748" t="n">
         <v>741960</v>
@@ -60149,22 +60149,22 @@
         <v>114747</v>
       </c>
       <c r="K749" t="n">
-        <v>10136661</v>
+        <v>10136659</v>
       </c>
       <c r="L749" t="n">
-        <v>6367530</v>
+        <v>6367528</v>
       </c>
       <c r="M749" t="n">
         <v>14239</v>
       </c>
       <c r="N749" t="n">
-        <v>2171443</v>
+        <v>2171442</v>
       </c>
       <c r="O749" t="n">
         <v>1131665</v>
       </c>
       <c r="P749" t="n">
-        <v>1410976</v>
+        <v>1410975</v>
       </c>
       <c r="Q749" t="n">
         <v>728192</v>
@@ -60229,22 +60229,22 @@
         <v>115159</v>
       </c>
       <c r="K750" t="n">
-        <v>10300776</v>
+        <v>10300774</v>
       </c>
       <c r="L750" t="n">
-        <v>6478569</v>
+        <v>6478567</v>
       </c>
       <c r="M750" t="n">
         <v>14647</v>
       </c>
       <c r="N750" t="n">
-        <v>2163368</v>
+        <v>2163367</v>
       </c>
       <c r="O750" t="n">
         <v>1099199</v>
       </c>
       <c r="P750" t="n">
-        <v>1404606</v>
+        <v>1404605</v>
       </c>
       <c r="Q750" t="n">
         <v>708477</v>
@@ -60309,10 +60309,10 @@
         <v>115487</v>
       </c>
       <c r="K751" t="n">
-        <v>10458354</v>
+        <v>10458352</v>
       </c>
       <c r="L751" t="n">
-        <v>6577453</v>
+        <v>6577451</v>
       </c>
       <c r="M751" t="n">
         <v>14843</v>
@@ -60389,10 +60389,10 @@
         <v>115788</v>
       </c>
       <c r="K752" t="n">
-        <v>10617169</v>
+        <v>10617167</v>
       </c>
       <c r="L752" t="n">
-        <v>6663377</v>
+        <v>6663375</v>
       </c>
       <c r="M752" t="n">
         <v>15126</v>
@@ -60469,10 +60469,10 @@
         <v>116076</v>
       </c>
       <c r="K753" t="n">
-        <v>10751482</v>
+        <v>10751480</v>
       </c>
       <c r="L753" t="n">
-        <v>6746581</v>
+        <v>6746579</v>
       </c>
       <c r="M753" t="n">
         <v>15336</v>
@@ -60549,10 +60549,10 @@
         <v>116298</v>
       </c>
       <c r="K754" t="n">
-        <v>10828127</v>
+        <v>10828125</v>
       </c>
       <c r="L754" t="n">
-        <v>6793925</v>
+        <v>6793923</v>
       </c>
       <c r="M754" t="n">
         <v>15351</v>
@@ -60629,10 +60629,10 @@
         <v>116484</v>
       </c>
       <c r="K755" t="n">
-        <v>10896791</v>
+        <v>10896789</v>
       </c>
       <c r="L755" t="n">
-        <v>6839716</v>
+        <v>6839714</v>
       </c>
       <c r="M755" t="n">
         <v>15511</v>
@@ -60709,10 +60709,10 @@
         <v>116814</v>
       </c>
       <c r="K756" t="n">
-        <v>11075197</v>
+        <v>11075195</v>
       </c>
       <c r="L756" t="n">
-        <v>6927251</v>
+        <v>6927249</v>
       </c>
       <c r="M756" t="n">
         <v>15855</v>
@@ -60789,10 +60789,10 @@
         <v>117315</v>
       </c>
       <c r="K757" t="n">
-        <v>11211092</v>
+        <v>11211090</v>
       </c>
       <c r="L757" t="n">
-        <v>6999392</v>
+        <v>6999390</v>
       </c>
       <c r="M757" t="n">
         <v>16098</v>
@@ -60869,10 +60869,10 @@
         <v>117632</v>
       </c>
       <c r="K758" t="n">
-        <v>11134930</v>
+        <v>11134928</v>
       </c>
       <c r="L758" t="n">
-        <v>7065269</v>
+        <v>7065267</v>
       </c>
       <c r="M758" t="n">
         <v>16324</v>
@@ -60949,10 +60949,10 @@
         <v>117943</v>
       </c>
       <c r="K759" t="n">
-        <v>11255964</v>
+        <v>11255962</v>
       </c>
       <c r="L759" t="n">
-        <v>7124745</v>
+        <v>7124743</v>
       </c>
       <c r="M759" t="n">
         <v>16580</v>
@@ -61029,10 +61029,10 @@
         <v>118259</v>
       </c>
       <c r="K760" t="n">
-        <v>11355678</v>
+        <v>11355676</v>
       </c>
       <c r="L760" t="n">
-        <v>7175650</v>
+        <v>7175648</v>
       </c>
       <c r="M760" t="n">
         <v>16755</v>
@@ -61109,10 +61109,10 @@
         <v>118483</v>
       </c>
       <c r="K761" t="n">
-        <v>11403058</v>
+        <v>11403056</v>
       </c>
       <c r="L761" t="n">
-        <v>7203519</v>
+        <v>7203517</v>
       </c>
       <c r="M761" t="n">
         <v>16756</v>
@@ -61189,10 +61189,10 @@
         <v>118656</v>
       </c>
       <c r="K762" t="n">
-        <v>11445324</v>
+        <v>11445322</v>
       </c>
       <c r="L762" t="n">
-        <v>7230088</v>
+        <v>7230086</v>
       </c>
       <c r="M762" t="n">
         <v>16849</v>
@@ -61269,10 +61269,10 @@
         <v>118976</v>
       </c>
       <c r="K763" t="n">
-        <v>11543015</v>
+        <v>11543013</v>
       </c>
       <c r="L763" t="n">
-        <v>7282820</v>
+        <v>7282818</v>
       </c>
       <c r="M763" t="n">
         <v>17075</v>
@@ -61349,10 +61349,10 @@
         <v>119485</v>
       </c>
       <c r="K764" t="n">
-        <v>11621941</v>
+        <v>11621939</v>
       </c>
       <c r="L764" t="n">
-        <v>7130276</v>
+        <v>7130274</v>
       </c>
       <c r="M764" t="n">
         <v>17226</v>
@@ -61429,10 +61429,10 @@
         <v>119786</v>
       </c>
       <c r="K765" t="n">
-        <v>11701239</v>
+        <v>11701237</v>
       </c>
       <c r="L765" t="n">
-        <v>7169198</v>
+        <v>7169196</v>
       </c>
       <c r="M765" t="n">
         <v>17408</v>
@@ -61509,10 +61509,10 @@
         <v>120147</v>
       </c>
       <c r="K766" t="n">
-        <v>11773572</v>
+        <v>11773570</v>
       </c>
       <c r="L766" t="n">
-        <v>7206202</v>
+        <v>7206200</v>
       </c>
       <c r="M766" t="n">
         <v>17548</v>
@@ -61589,10 +61589,10 @@
         <v>120408</v>
       </c>
       <c r="K767" t="n">
-        <v>11837016</v>
+        <v>11837014</v>
       </c>
       <c r="L767" t="n">
-        <v>7239283</v>
+        <v>7239281</v>
       </c>
       <c r="M767" t="n">
         <v>17735</v>
@@ -61669,37 +61669,37 @@
         <v>120638</v>
       </c>
       <c r="K768" t="n">
-        <v>11865671</v>
+        <v>11865668</v>
       </c>
       <c r="L768" t="n">
-        <v>7255625</v>
+        <v>7255622</v>
       </c>
       <c r="M768" t="n">
         <v>17784</v>
       </c>
       <c r="N768" t="n">
-        <v>1037544</v>
+        <v>1037543</v>
       </c>
       <c r="O768" t="n">
-        <v>462613</v>
+        <v>462612</v>
       </c>
       <c r="P768" t="n">
-        <v>461700</v>
+        <v>461699</v>
       </c>
       <c r="Q768" t="n">
-        <v>52106</v>
+        <v>52105</v>
       </c>
       <c r="R768" t="n">
-        <v>28655</v>
+        <v>28654</v>
       </c>
       <c r="S768" t="n">
-        <v>66087.6</v>
+        <v>66087.4</v>
       </c>
       <c r="T768" t="n">
-        <v>16342</v>
+        <v>16341</v>
       </c>
       <c r="U768" t="n">
-        <v>7443.7</v>
+        <v>7443.6</v>
       </c>
       <c r="V768" t="n">
         <v>230</v>
@@ -61749,37 +61749,37 @@
         <v>120803</v>
       </c>
       <c r="K769" t="n">
-        <v>11898197</v>
+        <v>11898194</v>
       </c>
       <c r="L769" t="n">
-        <v>7270759</v>
+        <v>7270756</v>
       </c>
       <c r="M769" t="n">
         <v>17862</v>
       </c>
       <c r="N769" t="n">
-        <v>1001406</v>
+        <v>1001405</v>
       </c>
       <c r="O769" t="n">
-        <v>452873</v>
+        <v>452872</v>
       </c>
       <c r="P769" t="n">
-        <v>431043</v>
+        <v>431042</v>
       </c>
       <c r="Q769" t="n">
-        <v>40671</v>
+        <v>40670</v>
       </c>
       <c r="R769" t="n">
         <v>32526</v>
       </c>
       <c r="S769" t="n">
-        <v>64696.1</v>
+        <v>64696</v>
       </c>
       <c r="T769" t="n">
         <v>15134</v>
       </c>
       <c r="U769" t="n">
-        <v>5810.1</v>
+        <v>5810</v>
       </c>
       <c r="V769" t="n">
         <v>165</v>
@@ -61829,37 +61829,37 @@
         <v>121060</v>
       </c>
       <c r="K770" t="n">
-        <v>11968017</v>
+        <v>11968014</v>
       </c>
       <c r="L770" t="n">
-        <v>7306319</v>
+        <v>7306316</v>
       </c>
       <c r="M770" t="n">
         <v>18016</v>
       </c>
       <c r="N770" t="n">
-        <v>892820</v>
+        <v>892819</v>
       </c>
       <c r="O770" t="n">
-        <v>425002</v>
+        <v>425001</v>
       </c>
       <c r="P770" t="n">
-        <v>379068</v>
+        <v>379067</v>
       </c>
       <c r="Q770" t="n">
-        <v>23499</v>
+        <v>23498</v>
       </c>
       <c r="R770" t="n">
         <v>69820</v>
       </c>
       <c r="S770" t="n">
-        <v>60714.6</v>
+        <v>60714.4</v>
       </c>
       <c r="T770" t="n">
         <v>35560</v>
       </c>
       <c r="U770" t="n">
-        <v>3357</v>
+        <v>3356.9</v>
       </c>
       <c r="V770" t="n">
         <v>257</v>
@@ -61909,37 +61909,37 @@
         <v>121569</v>
       </c>
       <c r="K771" t="n">
-        <v>12016645</v>
+        <v>12016642</v>
       </c>
       <c r="L771" t="n">
-        <v>7333462</v>
+        <v>7333459</v>
       </c>
       <c r="M771" t="n">
         <v>18104</v>
       </c>
       <c r="N771" t="n">
-        <v>805553</v>
+        <v>805552</v>
       </c>
       <c r="O771" t="n">
-        <v>394704</v>
+        <v>394703</v>
       </c>
       <c r="P771" t="n">
-        <v>334070</v>
+        <v>334069</v>
       </c>
       <c r="Q771" t="n">
-        <v>203186</v>
+        <v>203185</v>
       </c>
       <c r="R771" t="n">
         <v>48628</v>
       </c>
       <c r="S771" t="n">
-        <v>56386.3</v>
+        <v>56386.1</v>
       </c>
       <c r="T771" t="n">
         <v>27143</v>
       </c>
       <c r="U771" t="n">
-        <v>29026.6</v>
+        <v>29026.4</v>
       </c>
       <c r="V771" t="n">
         <v>509</v>
@@ -61989,37 +61989,37 @@
         <v>121833</v>
       </c>
       <c r="K772" t="n">
-        <v>12064819</v>
+        <v>12064816</v>
       </c>
       <c r="L772" t="n">
-        <v>7359625</v>
+        <v>7359622</v>
       </c>
       <c r="M772" t="n">
         <v>18194</v>
       </c>
       <c r="N772" t="n">
-        <v>929889</v>
+        <v>929888</v>
       </c>
       <c r="O772" t="n">
-        <v>363580</v>
+        <v>363579</v>
       </c>
       <c r="P772" t="n">
-        <v>294356</v>
+        <v>294355</v>
       </c>
       <c r="Q772" t="n">
-        <v>190427</v>
+        <v>190426</v>
       </c>
       <c r="R772" t="n">
         <v>48174</v>
       </c>
       <c r="S772" t="n">
-        <v>51940</v>
+        <v>51939.9</v>
       </c>
       <c r="T772" t="n">
         <v>26163</v>
       </c>
       <c r="U772" t="n">
-        <v>27203.9</v>
+        <v>27203.7</v>
       </c>
       <c r="V772" t="n">
         <v>264</v>
@@ -62069,37 +62069,37 @@
         <v>122055</v>
       </c>
       <c r="K773" t="n">
-        <v>12114396</v>
+        <v>12114393</v>
       </c>
       <c r="L773" t="n">
-        <v>7381451</v>
+        <v>7381448</v>
       </c>
       <c r="M773" t="n">
         <v>18284</v>
       </c>
       <c r="N773" t="n">
-        <v>858432</v>
+        <v>858431</v>
       </c>
       <c r="O773" t="n">
-        <v>340824</v>
+        <v>340823</v>
       </c>
       <c r="P773" t="n">
-        <v>256706</v>
+        <v>256705</v>
       </c>
       <c r="Q773" t="n">
-        <v>175249</v>
+        <v>175248</v>
       </c>
       <c r="R773" t="n">
         <v>49577</v>
       </c>
       <c r="S773" t="n">
-        <v>48689.1</v>
+        <v>48689</v>
       </c>
       <c r="T773" t="n">
         <v>21826</v>
       </c>
       <c r="U773" t="n">
-        <v>25035.6</v>
+        <v>25035.4</v>
       </c>
       <c r="V773" t="n">
         <v>222</v>
@@ -62149,37 +62149,37 @@
         <v>122369</v>
       </c>
       <c r="K774" t="n">
-        <v>12156614</v>
+        <v>12156611</v>
       </c>
       <c r="L774" t="n">
-        <v>7402829</v>
+        <v>7402826</v>
       </c>
       <c r="M774" t="n">
         <v>18316</v>
       </c>
       <c r="N774" t="n">
-        <v>800936</v>
+        <v>800935</v>
       </c>
       <c r="O774" t="n">
-        <v>319598</v>
+        <v>319597</v>
       </c>
       <c r="P774" t="n">
-        <v>227179</v>
+        <v>227178</v>
       </c>
       <c r="Q774" t="n">
-        <v>163546</v>
+        <v>163545</v>
       </c>
       <c r="R774" t="n">
         <v>42218</v>
       </c>
       <c r="S774" t="n">
-        <v>45656.9</v>
+        <v>45656.7</v>
       </c>
       <c r="T774" t="n">
         <v>21378</v>
       </c>
       <c r="U774" t="n">
-        <v>23363.7</v>
+        <v>23363.6</v>
       </c>
       <c r="V774" t="n">
         <v>314</v>
@@ -62229,22 +62229,22 @@
         <v>122492</v>
       </c>
       <c r="K775" t="n">
-        <v>12171555</v>
+        <v>12171552</v>
       </c>
       <c r="L775" t="n">
-        <v>7413304</v>
+        <v>7413301</v>
       </c>
       <c r="M775" t="n">
         <v>18348</v>
       </c>
       <c r="N775" t="n">
-        <v>768497</v>
+        <v>768496</v>
       </c>
       <c r="O775" t="n">
         <v>305884</v>
       </c>
       <c r="P775" t="n">
-        <v>209785</v>
+        <v>209784</v>
       </c>
       <c r="Q775" t="n">
         <v>157679</v>
@@ -62309,22 +62309,22 @@
         <v>122656</v>
       </c>
       <c r="K776" t="n">
-        <v>12193916</v>
+        <v>12193913</v>
       </c>
       <c r="L776" t="n">
-        <v>7423145</v>
+        <v>7423142</v>
       </c>
       <c r="M776" t="n">
         <v>18427</v>
       </c>
       <c r="N776" t="n">
-        <v>748592</v>
+        <v>748591</v>
       </c>
       <c r="O776" t="n">
         <v>295719</v>
       </c>
       <c r="P776" t="n">
-        <v>193057</v>
+        <v>193056</v>
       </c>
       <c r="Q776" t="n">
         <v>152386</v>
@@ -62389,22 +62389,22 @@
         <v>122919</v>
       </c>
       <c r="K777" t="n">
-        <v>12242913</v>
+        <v>12242910</v>
       </c>
       <c r="L777" t="n">
-        <v>7446757</v>
+        <v>7446754</v>
       </c>
       <c r="M777" t="n">
         <v>18553</v>
       </c>
       <c r="N777" t="n">
-        <v>699898</v>
+        <v>699897</v>
       </c>
       <c r="O777" t="n">
         <v>274896</v>
       </c>
       <c r="P777" t="n">
-        <v>163937</v>
+        <v>163936</v>
       </c>
       <c r="Q777" t="n">
         <v>140438</v>
@@ -62469,22 +62469,22 @@
         <v>123354</v>
       </c>
       <c r="K778" t="n">
-        <v>12278148</v>
+        <v>12278145</v>
       </c>
       <c r="L778" t="n">
-        <v>7466615</v>
+        <v>7466612</v>
       </c>
       <c r="M778" t="n">
         <v>18626</v>
       </c>
       <c r="N778" t="n">
-        <v>656207</v>
+        <v>656206</v>
       </c>
       <c r="O778" t="n">
         <v>261503</v>
       </c>
       <c r="P778" t="n">
-        <v>336339</v>
+        <v>336338</v>
       </c>
       <c r="Q778" t="n">
         <v>133153</v>
@@ -62549,22 +62549,22 @@
         <v>123601</v>
       </c>
       <c r="K779" t="n">
-        <v>12312036</v>
+        <v>12312033</v>
       </c>
       <c r="L779" t="n">
-        <v>7485442</v>
+        <v>7485439</v>
       </c>
       <c r="M779" t="n">
         <v>18798</v>
       </c>
       <c r="N779" t="n">
-        <v>610797</v>
+        <v>610796</v>
       </c>
       <c r="O779" t="n">
         <v>247217</v>
       </c>
       <c r="P779" t="n">
-        <v>316244</v>
+        <v>316243</v>
       </c>
       <c r="Q779" t="n">
         <v>125817</v>
@@ -62629,22 +62629,22 @@
         <v>123818</v>
       </c>
       <c r="K780" t="n">
-        <v>12345183</v>
+        <v>12345180</v>
       </c>
       <c r="L780" t="n">
-        <v>7503508</v>
+        <v>7503505</v>
       </c>
       <c r="M780" t="n">
         <v>18954</v>
       </c>
       <c r="N780" t="n">
-        <v>571611</v>
+        <v>571610</v>
       </c>
       <c r="O780" t="n">
         <v>230787</v>
       </c>
       <c r="P780" t="n">
-        <v>297306</v>
+        <v>297305</v>
       </c>
       <c r="Q780" t="n">
         <v>122057</v>
@@ -62709,22 +62709,22 @@
         <v>123933</v>
       </c>
       <c r="K781" t="n">
-        <v>12377021</v>
+        <v>12377018</v>
       </c>
       <c r="L781" t="n">
-        <v>7522360</v>
+        <v>7522357</v>
       </c>
       <c r="M781" t="n">
         <v>19068</v>
       </c>
       <c r="N781" t="n">
-        <v>540005</v>
+        <v>540004</v>
       </c>
       <c r="O781" t="n">
         <v>220407</v>
       </c>
       <c r="P781" t="n">
-        <v>283077</v>
+        <v>283076</v>
       </c>
       <c r="Q781" t="n">
         <v>119531</v>
@@ -62789,10 +62789,10 @@
         <v>124017</v>
       </c>
       <c r="K782" t="n">
-        <v>12388846</v>
+        <v>12388843</v>
       </c>
       <c r="L782" t="n">
-        <v>7531211</v>
+        <v>7531208</v>
       </c>
       <c r="M782" t="n">
         <v>19145</v>
@@ -62869,10 +62869,10 @@
         <v>124107</v>
       </c>
       <c r="K783" t="n">
-        <v>12405756</v>
+        <v>12405753</v>
       </c>
       <c r="L783" t="n">
-        <v>7539841</v>
+        <v>7539838</v>
       </c>
       <c r="M783" t="n">
         <v>0</v>
@@ -62949,10 +62949,10 @@
         <v>124296</v>
       </c>
       <c r="K784" t="n">
-        <v>12446692</v>
+        <v>12446689</v>
       </c>
       <c r="L784" t="n">
-        <v>7563972</v>
+        <v>7563969</v>
       </c>
       <c r="M784" t="n">
         <v>19284</v>
@@ -63029,10 +63029,10 @@
         <v>124583</v>
       </c>
       <c r="K785" t="n">
-        <v>12480055</v>
+        <v>12480052</v>
       </c>
       <c r="L785" t="n">
-        <v>7587031</v>
+        <v>7587028</v>
       </c>
       <c r="M785" t="n">
         <v>19350</v>
@@ -63109,10 +63109,10 @@
         <v>124698</v>
       </c>
       <c r="K786" t="n">
-        <v>12515037</v>
+        <v>12515034</v>
       </c>
       <c r="L786" t="n">
-        <v>7609100</v>
+        <v>7609097</v>
       </c>
       <c r="M786" t="n">
         <v>19370</v>
@@ -63189,10 +63189,10 @@
         <v>124850</v>
       </c>
       <c r="K787" t="n">
-        <v>12549181</v>
+        <v>12549178</v>
       </c>
       <c r="L787" t="n">
-        <v>7629452</v>
+        <v>7629449</v>
       </c>
       <c r="M787" t="n">
         <v>19395</v>
@@ -63269,10 +63269,10 @@
         <v>124984</v>
       </c>
       <c r="K788" t="n">
-        <v>12575953</v>
+        <v>12575950</v>
       </c>
       <c r="L788" t="n">
-        <v>7647269</v>
+        <v>7647266</v>
       </c>
       <c r="M788" t="n">
         <v>19460</v>
@@ -63349,10 +63349,10 @@
         <v>125036</v>
       </c>
       <c r="K789" t="n">
-        <v>12587517</v>
+        <v>12587514</v>
       </c>
       <c r="L789" t="n">
-        <v>7656649</v>
+        <v>7656646</v>
       </c>
       <c r="M789" t="n">
         <v>19460</v>
@@ -63429,10 +63429,10 @@
         <v>125113</v>
       </c>
       <c r="K790" t="n">
-        <v>12601783</v>
+        <v>12601780</v>
       </c>
       <c r="L790" t="n">
-        <v>7664931</v>
+        <v>7664928</v>
       </c>
       <c r="M790" t="n">
         <v>19471</v>
@@ -63509,10 +63509,10 @@
         <v>125245</v>
       </c>
       <c r="K791" t="n">
-        <v>12634424</v>
+        <v>12634421</v>
       </c>
       <c r="L791" t="n">
-        <v>7686045</v>
+        <v>7686042</v>
       </c>
       <c r="M791" t="n">
         <v>19515</v>
@@ -63589,10 +63589,10 @@
         <v>125493</v>
       </c>
       <c r="K792" t="n">
-        <v>12655439</v>
+        <v>12655436</v>
       </c>
       <c r="L792" t="n">
-        <v>7699968</v>
+        <v>7699965</v>
       </c>
       <c r="M792" t="n">
         <v>19545</v>
@@ -63669,10 +63669,10 @@
         <v>125583</v>
       </c>
       <c r="K793" t="n">
-        <v>12684912</v>
+        <v>12684909</v>
       </c>
       <c r="L793" t="n">
-        <v>7722145</v>
+        <v>7722142</v>
       </c>
       <c r="M793" t="n">
         <v>19608</v>
@@ -63749,10 +63749,10 @@
         <v>125711</v>
       </c>
       <c r="K794" t="n">
-        <v>12715438</v>
+        <v>12715435</v>
       </c>
       <c r="L794" t="n">
-        <v>7743486</v>
+        <v>7743483</v>
       </c>
       <c r="M794" t="n">
         <v>19632</v>
@@ -63829,10 +63829,10 @@
         <v>125802</v>
       </c>
       <c r="K795" t="n">
-        <v>12743828</v>
+        <v>12743825</v>
       </c>
       <c r="L795" t="n">
-        <v>7763212</v>
+        <v>7763209</v>
       </c>
       <c r="M795" t="n">
         <v>19702</v>
@@ -63909,10 +63909,10 @@
         <v>125840</v>
       </c>
       <c r="K796" t="n">
-        <v>12755335</v>
+        <v>12755332</v>
       </c>
       <c r="L796" t="n">
-        <v>7771393</v>
+        <v>7771390</v>
       </c>
       <c r="M796" t="n">
         <v>19702</v>
@@ -63989,10 +63989,10 @@
         <v>125920</v>
       </c>
       <c r="K797" t="n">
-        <v>12768728</v>
+        <v>12768725</v>
       </c>
       <c r="L797" t="n">
-        <v>7778985</v>
+        <v>7778982</v>
       </c>
       <c r="M797" t="n">
         <v>19748</v>
@@ -64069,37 +64069,37 @@
         <v>126024</v>
       </c>
       <c r="K798" t="n">
-        <v>12800139</v>
+        <v>12800137</v>
       </c>
       <c r="L798" t="n">
-        <v>7798248</v>
+        <v>7798246</v>
       </c>
       <c r="M798" t="n">
         <v>19763</v>
       </c>
       <c r="N798" t="n">
-        <v>353447</v>
+        <v>353448</v>
       </c>
       <c r="O798" t="n">
-        <v>165715</v>
+        <v>165716</v>
       </c>
       <c r="P798" t="n">
-        <v>234276</v>
+        <v>234277</v>
       </c>
       <c r="Q798" t="n">
-        <v>112203</v>
+        <v>112204</v>
       </c>
       <c r="R798" t="n">
-        <v>31411</v>
+        <v>31412</v>
       </c>
       <c r="S798" t="n">
-        <v>23673.6</v>
+        <v>23673.7</v>
       </c>
       <c r="T798" t="n">
-        <v>19263</v>
+        <v>19264</v>
       </c>
       <c r="U798" t="n">
-        <v>16029</v>
+        <v>16029.1</v>
       </c>
       <c r="V798" t="n">
         <v>104</v>
@@ -64149,37 +64149,37 @@
         <v>126268</v>
       </c>
       <c r="K799" t="n">
-        <v>12826729</v>
+        <v>12826728</v>
       </c>
       <c r="L799" t="n">
-        <v>7817079</v>
+        <v>7817078</v>
       </c>
       <c r="M799" t="n">
         <v>19816</v>
       </c>
       <c r="N799" t="n">
-        <v>346674</v>
+        <v>346676</v>
       </c>
       <c r="O799" t="n">
-        <v>171290</v>
+        <v>171292</v>
       </c>
       <c r="P799" t="n">
-        <v>230048</v>
+        <v>230050</v>
       </c>
       <c r="Q799" t="n">
-        <v>117111</v>
+        <v>117113</v>
       </c>
       <c r="R799" t="n">
-        <v>26590</v>
+        <v>26591</v>
       </c>
       <c r="S799" t="n">
-        <v>24470</v>
+        <v>24470.3</v>
       </c>
       <c r="T799" t="n">
-        <v>18831</v>
+        <v>18832</v>
       </c>
       <c r="U799" t="n">
-        <v>16730.1</v>
+        <v>16730.4</v>
       </c>
       <c r="V799" t="n">
         <v>244</v>
@@ -64229,37 +64229,37 @@
         <v>126340</v>
       </c>
       <c r="K800" t="n">
-        <v>12854299</v>
+        <v>12854298</v>
       </c>
       <c r="L800" t="n">
-        <v>7835262</v>
+        <v>7835261</v>
       </c>
       <c r="M800" t="n">
         <v>19879</v>
       </c>
       <c r="N800" t="n">
-        <v>339262</v>
+        <v>339264</v>
       </c>
       <c r="O800" t="n">
-        <v>169387</v>
+        <v>169389</v>
       </c>
       <c r="P800" t="n">
-        <v>226162</v>
+        <v>226164</v>
       </c>
       <c r="Q800" t="n">
-        <v>113117</v>
+        <v>113119</v>
       </c>
       <c r="R800" t="n">
         <v>27570</v>
       </c>
       <c r="S800" t="n">
-        <v>24198.1</v>
+        <v>24198.4</v>
       </c>
       <c r="T800" t="n">
         <v>18183</v>
       </c>
       <c r="U800" t="n">
-        <v>16159.6</v>
+        <v>16159.9</v>
       </c>
       <c r="V800" t="n">
         <v>72</v>
@@ -64309,37 +64309,37 @@
         <v>126450</v>
       </c>
       <c r="K801" t="n">
-        <v>12880077</v>
+        <v>12880298</v>
       </c>
       <c r="L801" t="n">
-        <v>7851993</v>
+        <v>7852214</v>
       </c>
       <c r="M801" t="n">
         <v>19892</v>
       </c>
       <c r="N801" t="n">
-        <v>330896</v>
+        <v>331120</v>
       </c>
       <c r="O801" t="n">
-        <v>164639</v>
+        <v>164863</v>
       </c>
       <c r="P801" t="n">
-        <v>222541</v>
+        <v>222765</v>
       </c>
       <c r="Q801" t="n">
-        <v>108507</v>
+        <v>108731</v>
       </c>
       <c r="R801" t="n">
-        <v>25778</v>
+        <v>26000</v>
       </c>
       <c r="S801" t="n">
-        <v>23519.9</v>
+        <v>23551.9</v>
       </c>
       <c r="T801" t="n">
-        <v>16731</v>
+        <v>16953</v>
       </c>
       <c r="U801" t="n">
-        <v>15501</v>
+        <v>15533</v>
       </c>
       <c r="V801" t="n">
         <v>110</v>
@@ -64362,7 +64362,7 @@
         <v>44631</v>
       </c>
       <c r="B802" t="n">
-        <v>15280</v>
+        <v>15282</v>
       </c>
       <c r="C802" t="n">
         <v>11949</v>
@@ -64374,7 +64374,7 @@
         <v>123757</v>
       </c>
       <c r="F802" t="n">
-        <v>3536</v>
+        <v>4218</v>
       </c>
       <c r="G802" t="n">
         <v>114</v>
@@ -64386,55 +64386,55 @@
         <v>426</v>
       </c>
       <c r="J802" t="n">
-        <v>104158</v>
+        <v>126508</v>
       </c>
       <c r="K802" t="n">
-        <v>11282426</v>
+        <v>12903405</v>
       </c>
       <c r="L802" t="n">
-        <v>6245910</v>
+        <v>7866887</v>
       </c>
       <c r="M802" t="n">
         <v>19906</v>
       </c>
       <c r="N802" t="n">
-        <v>-1293527</v>
+        <v>327455</v>
       </c>
       <c r="O802" t="n">
-        <v>-1461402</v>
+        <v>159580</v>
       </c>
       <c r="P802" t="n">
-        <v>-1401359</v>
+        <v>219621</v>
       </c>
       <c r="Q802" t="n">
-        <v>-1517302</v>
+        <v>103678</v>
       </c>
       <c r="R802" t="n">
-        <v>-1597651</v>
+        <v>23107</v>
       </c>
       <c r="S802" t="n">
-        <v>-208771.7</v>
+        <v>22797.1</v>
       </c>
       <c r="T802" t="n">
-        <v>-1606083</v>
+        <v>14673</v>
       </c>
       <c r="U802" t="n">
-        <v>-216757.4</v>
+        <v>14811.1</v>
       </c>
       <c r="V802" t="n">
-        <v>-22292</v>
+        <v>58</v>
       </c>
       <c r="W802" t="n">
-        <v>-17.6</v>
+        <v>0</v>
       </c>
       <c r="X802" t="n">
-        <v>-7370</v>
+        <v>80</v>
       </c>
       <c r="Y802" t="n">
-        <v>-3092</v>
+        <v>100.9</v>
       </c>
       <c r="Z802" t="n">
-        <v>-21644</v>
+        <v>706</v>
       </c>
     </row>
     <row r="803">
@@ -64442,22 +64442,22 @@
         <v>44632</v>
       </c>
       <c r="B803" t="n">
-        <v>6998</v>
+        <v>7002</v>
       </c>
       <c r="C803" t="n">
         <v>5414</v>
       </c>
       <c r="D803" t="n">
-        <v>6005793</v>
+        <v>6005794</v>
       </c>
       <c r="E803" t="n">
         <v>123051</v>
       </c>
       <c r="F803" t="n">
-        <v>2389</v>
+        <v>4219</v>
       </c>
       <c r="G803" t="n">
-        <v>126300</v>
+        <v>126301</v>
       </c>
       <c r="H803" t="n">
         <v>9307</v>
@@ -64466,55 +64466,55 @@
         <v>256</v>
       </c>
       <c r="J803" t="n">
-        <v>81980</v>
+        <v>126530</v>
       </c>
       <c r="K803" t="n">
-        <v>8605528</v>
+        <v>12914804</v>
       </c>
       <c r="L803" t="n">
-        <v>6252791</v>
+        <v>7873846</v>
       </c>
       <c r="M803" t="n">
         <v>19908</v>
       </c>
       <c r="N803" t="n">
-        <v>-3981989</v>
+        <v>327290</v>
       </c>
       <c r="O803" t="n">
-        <v>-4149807</v>
+        <v>159472</v>
       </c>
       <c r="P803" t="n">
-        <v>-1403858</v>
+        <v>217200</v>
       </c>
       <c r="Q803" t="n">
-        <v>-1518602</v>
+        <v>102456</v>
       </c>
       <c r="R803" t="n">
-        <v>-2676898</v>
+        <v>11399</v>
       </c>
       <c r="S803" t="n">
-        <v>-592829.6</v>
+        <v>22781.7</v>
       </c>
       <c r="T803" t="n">
-        <v>6881</v>
+        <v>6959</v>
       </c>
       <c r="U803" t="n">
-        <v>-216943.1</v>
+        <v>14636.6</v>
       </c>
       <c r="V803" t="n">
-        <v>-22178</v>
+        <v>22</v>
       </c>
       <c r="W803" t="n">
-        <v>-21.3</v>
+        <v>0</v>
       </c>
       <c r="X803" t="n">
-        <v>-14786.7</v>
+        <v>63.3</v>
       </c>
       <c r="Y803" t="n">
-        <v>-6265.7</v>
+        <v>98.6</v>
       </c>
       <c r="Z803" t="n">
-        <v>-43860</v>
+        <v>690</v>
       </c>
     </row>
     <row r="804">
@@ -64522,79 +64522,79 @@
         <v>44633</v>
       </c>
       <c r="B804" t="n">
-        <v>5453</v>
+        <v>5458</v>
       </c>
       <c r="C804" t="n">
         <v>4265</v>
       </c>
       <c r="D804" t="n">
-        <v>6008871</v>
+        <v>6008873</v>
       </c>
       <c r="E804" t="n">
         <v>114779</v>
       </c>
       <c r="F804" t="n">
-        <v>2434</v>
+        <v>4254</v>
       </c>
       <c r="G804" t="n">
-        <v>126354</v>
+        <v>126356</v>
       </c>
       <c r="H804" t="n">
         <v>9317</v>
       </c>
       <c r="I804" t="n">
-        <v>274</v>
+        <v>343</v>
       </c>
       <c r="J804" t="n">
-        <v>80485</v>
+        <v>126540</v>
       </c>
       <c r="K804" t="n">
-        <v>8388383</v>
+        <v>12923401</v>
       </c>
       <c r="L804" t="n">
-        <v>6032298</v>
+        <v>7879090</v>
       </c>
       <c r="M804" t="n">
         <v>19915</v>
       </c>
       <c r="N804" t="n">
-        <v>-4213400</v>
+        <v>321621</v>
       </c>
       <c r="O804" t="n">
-        <v>-4380345</v>
+        <v>154676</v>
       </c>
       <c r="P804" t="n">
-        <v>-1632633</v>
+        <v>214162</v>
       </c>
       <c r="Q804" t="n">
-        <v>-1746687</v>
+        <v>100108</v>
       </c>
       <c r="R804" t="n">
-        <v>-217145</v>
+        <v>8597</v>
       </c>
       <c r="S804" t="n">
-        <v>-625763.6</v>
+        <v>22096.6</v>
       </c>
       <c r="T804" t="n">
-        <v>-220493</v>
+        <v>5244</v>
       </c>
       <c r="U804" t="n">
-        <v>-249526.7</v>
+        <v>14301.1</v>
       </c>
       <c r="V804" t="n">
-        <v>-1495</v>
+        <v>10</v>
       </c>
       <c r="W804" t="n">
-        <v>-1.8</v>
+        <v>0</v>
       </c>
       <c r="X804" t="n">
-        <v>-15321.7</v>
+        <v>30</v>
       </c>
       <c r="Y804" t="n">
-        <v>-6490.7</v>
+        <v>88.6</v>
       </c>
       <c r="Z804" t="n">
-        <v>-45435</v>
+        <v>620</v>
       </c>
     </row>
     <row r="805">
@@ -64602,79 +64602,159 @@
         <v>44634</v>
       </c>
       <c r="B805" t="n">
-        <v>530</v>
+        <v>1009</v>
       </c>
       <c r="C805" t="n">
-        <v>1135</v>
+        <v>1641</v>
       </c>
       <c r="D805" t="n">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="E805" t="n">
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="F805" t="n">
-        <v>1143</v>
+        <v>4149</v>
       </c>
       <c r="G805" t="n">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="H805" t="n">
         <v>0</v>
       </c>
       <c r="I805" t="n">
-        <v>72</v>
+        <v>190</v>
       </c>
       <c r="J805" t="n">
-        <v>38377</v>
+        <v>126579</v>
       </c>
       <c r="K805" t="n">
-        <v>2925622</v>
+        <v>12931021</v>
       </c>
       <c r="L805" t="n">
-        <v>1147794</v>
+        <v>7881533</v>
       </c>
       <c r="M805" t="n">
-        <v>0</v>
+        <v>19936</v>
       </c>
       <c r="N805" t="n">
-        <v>-9708802</v>
+        <v>296600</v>
       </c>
       <c r="O805" t="n">
-        <v>-9874517</v>
+        <v>130884</v>
       </c>
       <c r="P805" t="n">
-        <v>-6538251</v>
+        <v>195491</v>
       </c>
       <c r="Q805" t="n">
-        <v>-6650454</v>
+        <v>83287</v>
       </c>
       <c r="R805" t="n">
-        <v>-5462761</v>
+        <v>7620</v>
       </c>
       <c r="S805" t="n">
-        <v>-1410645.3</v>
+        <v>18697.7</v>
       </c>
       <c r="T805" t="n">
-        <v>-4884504</v>
+        <v>2443</v>
       </c>
       <c r="U805" t="n">
-        <v>-950064.9</v>
+        <v>11898.1</v>
       </c>
       <c r="V805" t="n">
-        <v>-42108</v>
+        <v>39</v>
       </c>
       <c r="W805" t="n">
-        <v>-52.3</v>
+        <v>0</v>
       </c>
       <c r="X805" t="n">
-        <v>-21927</v>
+        <v>23.7</v>
       </c>
       <c r="Y805" t="n">
-        <v>-12521</v>
+        <v>79.3</v>
       </c>
       <c r="Z805" t="n">
-        <v>-87647</v>
+        <v>555</v>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" s="1" t="n">
+        <v>44635</v>
+      </c>
+      <c r="B806" t="n">
+        <v>6150</v>
+      </c>
+      <c r="C806" t="n">
+        <v>557</v>
+      </c>
+      <c r="D806" t="n">
+        <v>0</v>
+      </c>
+      <c r="E806" t="n">
+        <v>0</v>
+      </c>
+      <c r="F806" t="n">
+        <v>1586</v>
+      </c>
+      <c r="G806" t="n">
+        <v>0</v>
+      </c>
+      <c r="H806" t="n">
+        <v>0</v>
+      </c>
+      <c r="I806" t="n">
+        <v>129</v>
+      </c>
+      <c r="J806" t="n">
+        <v>42774</v>
+      </c>
+      <c r="K806" t="n">
+        <v>4122308</v>
+      </c>
+      <c r="L806" t="n">
+        <v>761619</v>
+      </c>
+      <c r="M806" t="n">
+        <v>0</v>
+      </c>
+      <c r="N806" t="n">
+        <v>-8533128</v>
+      </c>
+      <c r="O806" t="n">
+        <v>-8704420</v>
+      </c>
+      <c r="P806" t="n">
+        <v>-6938346</v>
+      </c>
+      <c r="Q806" t="n">
+        <v>-7055459</v>
+      </c>
+      <c r="R806" t="n">
+        <v>-8808713</v>
+      </c>
+      <c r="S806" t="n">
+        <v>-1243488.6</v>
+      </c>
+      <c r="T806" t="n">
+        <v>-7119914</v>
+      </c>
+      <c r="U806" t="n">
+        <v>-1007922.7</v>
+      </c>
+      <c r="V806" t="n">
+        <v>-83805</v>
+      </c>
+      <c r="W806" t="n">
+        <v>-66.2</v>
+      </c>
+      <c r="X806" t="n">
+        <v>-27918.7</v>
+      </c>
+      <c r="Y806" t="n">
+        <v>-11927.7</v>
+      </c>
+      <c r="Z806" t="n">
+        <v>-83494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualiza datos provincias 2022-03-26
</commit_message>
<xml_diff>
--- a/data/output/covid19-spain_consolidated.xlsx
+++ b/data/output/covid19-spain_consolidated.xlsx
@@ -65402,7 +65402,7 @@
         <v>44644</v>
       </c>
       <c r="B815" t="n">
-        <v>1533</v>
+        <v>1578</v>
       </c>
       <c r="C815" t="n">
         <v>702</v>
@@ -65414,7 +65414,7 @@
         <v>345</v>
       </c>
       <c r="F815" t="n">
-        <v>2675</v>
+        <v>2723</v>
       </c>
       <c r="G815" t="n">
         <v>80</v>
@@ -65426,55 +65426,55 @@
         <v>226</v>
       </c>
       <c r="J815" t="n">
-        <v>81616</v>
+        <v>83275</v>
       </c>
       <c r="K815" t="n">
-        <v>7714542</v>
+        <v>7963852</v>
       </c>
       <c r="L815" t="n">
-        <v>3829857</v>
+        <v>4059645</v>
       </c>
       <c r="M815" t="n">
         <v>20094</v>
       </c>
       <c r="N815" t="n">
-        <v>-3493272</v>
+        <v>-3243962</v>
       </c>
       <c r="O815" t="n">
-        <v>-1973013</v>
+        <v>-1723703</v>
       </c>
       <c r="P815" t="n">
-        <v>-2349534</v>
+        <v>-2119746</v>
       </c>
       <c r="Q815" t="n">
-        <v>-2400747</v>
+        <v>-2170959</v>
       </c>
       <c r="R815" t="n">
-        <v>-1555016</v>
+        <v>-1305706</v>
       </c>
       <c r="S815" t="n">
-        <v>-281859</v>
+        <v>-246243.3</v>
       </c>
       <c r="T815" t="n">
-        <v>-319635</v>
+        <v>-89847</v>
       </c>
       <c r="U815" t="n">
-        <v>-342963.9</v>
+        <v>-310137</v>
       </c>
       <c r="V815" t="n">
-        <v>-11990</v>
+        <v>-10331</v>
       </c>
       <c r="W815" t="n">
-        <v>-12.8</v>
+        <v>-11</v>
       </c>
       <c r="X815" t="n">
-        <v>-12201.7</v>
+        <v>-11648.7</v>
       </c>
       <c r="Y815" t="n">
-        <v>-5212.3</v>
+        <v>-4975.3</v>
       </c>
       <c r="Z815" t="n">
-        <v>-36486</v>
+        <v>-34827</v>
       </c>
     </row>
     <row r="816">
@@ -65482,10 +65482,10 @@
         <v>44645</v>
       </c>
       <c r="B816" t="n">
-        <v>11856</v>
+        <v>11901</v>
       </c>
       <c r="C816" t="n">
-        <v>2303</v>
+        <v>2472</v>
       </c>
       <c r="D816" t="n">
         <v>0</v>
@@ -65494,7 +65494,7 @@
         <v>0</v>
       </c>
       <c r="F816" t="n">
-        <v>1528</v>
+        <v>2062</v>
       </c>
       <c r="G816" t="n">
         <v>0</v>
@@ -65503,58 +65503,138 @@
         <v>0</v>
       </c>
       <c r="I816" t="n">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="J816" t="n">
-        <v>49245</v>
+        <v>55069</v>
       </c>
       <c r="K816" t="n">
-        <v>4578543</v>
+        <v>5522905</v>
       </c>
       <c r="L816" t="n">
-        <v>1166762</v>
+        <v>1546564</v>
       </c>
       <c r="M816" t="n">
         <v>0</v>
       </c>
       <c r="N816" t="n">
-        <v>-6645319</v>
+        <v>-5700957</v>
       </c>
       <c r="O816" t="n">
-        <v>-5130132</v>
+        <v>-4185770</v>
       </c>
       <c r="P816" t="n">
-        <v>-5020231</v>
+        <v>-4640429</v>
       </c>
       <c r="Q816" t="n">
-        <v>-5073072</v>
+        <v>-4693270</v>
       </c>
       <c r="R816" t="n">
-        <v>-3135999</v>
+        <v>-2440947</v>
       </c>
       <c r="S816" t="n">
-        <v>-732876</v>
+        <v>-597967.1</v>
       </c>
       <c r="T816" t="n">
-        <v>-2663095</v>
+        <v>-2513081</v>
       </c>
       <c r="U816" t="n">
-        <v>-724724.6</v>
+        <v>-670467.1</v>
       </c>
       <c r="V816" t="n">
-        <v>-32371</v>
+        <v>-28206</v>
       </c>
       <c r="W816" t="n">
-        <v>-39.7</v>
+        <v>-33.9</v>
       </c>
       <c r="X816" t="n">
-        <v>-23008.7</v>
+        <v>-21067.3</v>
       </c>
       <c r="Y816" t="n">
-        <v>-9843.1</v>
+        <v>-9011.1</v>
       </c>
       <c r="Z816" t="n">
-        <v>-68902</v>
+        <v>-63078</v>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" s="1" t="n">
+        <v>44646</v>
+      </c>
+      <c r="B817" t="n">
+        <v>45</v>
+      </c>
+      <c r="C817" t="n">
+        <v>55</v>
+      </c>
+      <c r="D817" t="n">
+        <v>0</v>
+      </c>
+      <c r="E817" t="n">
+        <v>0</v>
+      </c>
+      <c r="F817" t="n">
+        <v>96</v>
+      </c>
+      <c r="G817" t="n">
+        <v>0</v>
+      </c>
+      <c r="H817" t="n">
+        <v>0</v>
+      </c>
+      <c r="I817" t="n">
+        <v>5</v>
+      </c>
+      <c r="J817" t="n">
+        <v>2626</v>
+      </c>
+      <c r="K817" t="n">
+        <v>400934</v>
+      </c>
+      <c r="L817" t="n">
+        <v>379857</v>
+      </c>
+      <c r="M817" t="n">
+        <v>0</v>
+      </c>
+      <c r="N817" t="n">
+        <v>-10831831</v>
+      </c>
+      <c r="O817" t="n">
+        <v>-9315530</v>
+      </c>
+      <c r="P817" t="n">
+        <v>-5811592</v>
+      </c>
+      <c r="Q817" t="n">
+        <v>-5864581</v>
+      </c>
+      <c r="R817" t="n">
+        <v>-5121971</v>
+      </c>
+      <c r="S817" t="n">
+        <v>-1330790</v>
+      </c>
+      <c r="T817" t="n">
+        <v>-1166707</v>
+      </c>
+      <c r="U817" t="n">
+        <v>-837797.3</v>
+      </c>
+      <c r="V817" t="n">
+        <v>-52443</v>
+      </c>
+      <c r="W817" t="n">
+        <v>-95.2</v>
+      </c>
+      <c r="X817" t="n">
+        <v>-30326.7</v>
+      </c>
+      <c r="Y817" t="n">
+        <v>-16506.6</v>
+      </c>
+      <c r="Z817" t="n">
+        <v>-115546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualiza datos provincias 2022-04-21
</commit_message>
<xml_diff>
--- a/data/output/covid19-spain_consolidated.xlsx
+++ b/data/output/covid19-spain_consolidated.xlsx
@@ -19814,7 +19814,7 @@
         <v>16396</v>
       </c>
       <c r="F245" t="n">
-        <v>5736</v>
+        <v>5737</v>
       </c>
       <c r="G245" t="n">
         <v>65101</v>
@@ -19894,7 +19894,7 @@
         <v>15335</v>
       </c>
       <c r="F246" t="n">
-        <v>5769</v>
+        <v>5771</v>
       </c>
       <c r="G246" t="n">
         <v>65193</v>
@@ -19974,7 +19974,7 @@
         <v>15478</v>
       </c>
       <c r="F247" t="n">
-        <v>5820</v>
+        <v>5822</v>
       </c>
       <c r="G247" t="n">
         <v>65286</v>
@@ -20054,7 +20054,7 @@
         <v>15425</v>
       </c>
       <c r="F248" t="n">
-        <v>5958</v>
+        <v>5960</v>
       </c>
       <c r="G248" t="n">
         <v>65381</v>
@@ -20134,7 +20134,7 @@
         <v>6917</v>
       </c>
       <c r="F249" t="n">
-        <v>6042</v>
+        <v>6044</v>
       </c>
       <c r="G249" t="n">
         <v>65373</v>
@@ -20214,7 +20214,7 @@
         <v>4911</v>
       </c>
       <c r="F250" t="n">
-        <v>6108</v>
+        <v>6110</v>
       </c>
       <c r="G250" t="n">
         <v>65375</v>
@@ -20294,7 +20294,7 @@
         <v>13758</v>
       </c>
       <c r="F251" t="n">
-        <v>6597</v>
+        <v>6599</v>
       </c>
       <c r="G251" t="n">
         <v>65366</v>
@@ -20374,7 +20374,7 @@
         <v>15277</v>
       </c>
       <c r="F252" t="n">
-        <v>6848</v>
+        <v>6850</v>
       </c>
       <c r="G252" t="n">
         <v>65409</v>
@@ -20454,7 +20454,7 @@
         <v>15219</v>
       </c>
       <c r="F253" t="n">
-        <v>6955</v>
+        <v>6957</v>
       </c>
       <c r="G253" t="n">
         <v>65518</v>
@@ -20534,7 +20534,7 @@
         <v>15268</v>
       </c>
       <c r="F254" t="n">
-        <v>7071</v>
+        <v>7073</v>
       </c>
       <c r="G254" t="n">
         <v>65630</v>
@@ -20614,7 +20614,7 @@
         <v>14986</v>
       </c>
       <c r="F255" t="n">
-        <v>7148</v>
+        <v>7149</v>
       </c>
       <c r="G255" t="n">
         <v>65747</v>
@@ -20694,7 +20694,7 @@
         <v>6736</v>
       </c>
       <c r="F256" t="n">
-        <v>7208</v>
+        <v>7209</v>
       </c>
       <c r="G256" t="n">
         <v>65922</v>
@@ -20774,7 +20774,7 @@
         <v>4810</v>
       </c>
       <c r="F257" t="n">
-        <v>7270</v>
+        <v>7271</v>
       </c>
       <c r="G257" t="n">
         <v>65925</v>
@@ -20854,7 +20854,7 @@
         <v>13766</v>
       </c>
       <c r="F258" t="n">
-        <v>7865</v>
+        <v>7866</v>
       </c>
       <c r="G258" t="n">
         <v>65945</v>
@@ -20934,7 +20934,7 @@
         <v>13385</v>
       </c>
       <c r="F259" t="n">
-        <v>8020</v>
+        <v>8021</v>
       </c>
       <c r="G259" t="n">
         <v>66044</v>
@@ -21014,7 +21014,7 @@
         <v>13170</v>
       </c>
       <c r="F260" t="n">
-        <v>8179</v>
+        <v>8180</v>
       </c>
       <c r="G260" t="n">
         <v>66241</v>
@@ -21094,7 +21094,7 @@
         <v>12945</v>
       </c>
       <c r="F261" t="n">
-        <v>8327</v>
+        <v>8328</v>
       </c>
       <c r="G261" t="n">
         <v>66490</v>
@@ -21174,7 +21174,7 @@
         <v>13077</v>
       </c>
       <c r="F262" t="n">
-        <v>8372</v>
+        <v>8373</v>
       </c>
       <c r="G262" t="n">
         <v>67055</v>
@@ -21254,7 +21254,7 @@
         <v>4234</v>
       </c>
       <c r="F263" t="n">
-        <v>8379</v>
+        <v>8380</v>
       </c>
       <c r="G263" t="n">
         <v>67342</v>
@@ -21334,7 +21334,7 @@
         <v>4291</v>
       </c>
       <c r="F264" t="n">
-        <v>8407</v>
+        <v>8408</v>
       </c>
       <c r="G264" t="n">
         <v>67339</v>
@@ -21414,7 +21414,7 @@
         <v>13509</v>
       </c>
       <c r="F265" t="n">
-        <v>8885</v>
+        <v>8886</v>
       </c>
       <c r="G265" t="n">
         <v>67374</v>
@@ -21494,7 +21494,7 @@
         <v>13190</v>
       </c>
       <c r="F266" t="n">
-        <v>8972</v>
+        <v>8973</v>
       </c>
       <c r="G266" t="n">
         <v>67630</v>
@@ -21574,7 +21574,7 @@
         <v>12965</v>
       </c>
       <c r="F267" t="n">
-        <v>9046</v>
+        <v>9047</v>
       </c>
       <c r="G267" t="n">
         <v>67874</v>
@@ -21654,7 +21654,7 @@
         <v>12803</v>
       </c>
       <c r="F268" t="n">
-        <v>9050</v>
+        <v>9051</v>
       </c>
       <c r="G268" t="n">
         <v>68163</v>
@@ -59346,7 +59346,7 @@
         <v>1751</v>
       </c>
       <c r="J739" t="n">
-        <v>105234</v>
+        <v>105235</v>
       </c>
       <c r="K739" t="n">
         <v>7460927</v>
@@ -59382,19 +59382,19 @@
         <v>65099.9</v>
       </c>
       <c r="V739" t="n">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="W739" t="n">
         <v>0.1</v>
       </c>
       <c r="X739" t="n">
-        <v>135.7</v>
+        <v>136</v>
       </c>
       <c r="Y739" t="n">
-        <v>134.6</v>
+        <v>134.7</v>
       </c>
       <c r="Z739" t="n">
-        <v>942</v>
+        <v>943</v>
       </c>
     </row>
     <row r="740">
@@ -59426,7 +59426,7 @@
         <v>1229</v>
       </c>
       <c r="J740" t="n">
-        <v>105347</v>
+        <v>105348</v>
       </c>
       <c r="K740" t="n">
         <v>7538224</v>
@@ -59468,13 +59468,13 @@
         <v>0.1</v>
       </c>
       <c r="X740" t="n">
-        <v>135.7</v>
+        <v>136</v>
       </c>
       <c r="Y740" t="n">
-        <v>139.3</v>
+        <v>139.4</v>
       </c>
       <c r="Z740" t="n">
-        <v>975</v>
+        <v>976</v>
       </c>
     </row>
     <row r="741">
@@ -59506,7 +59506,7 @@
         <v>1606</v>
       </c>
       <c r="J741" t="n">
-        <v>105467</v>
+        <v>105468</v>
       </c>
       <c r="K741" t="n">
         <v>7621585</v>
@@ -59548,13 +59548,13 @@
         <v>0.1</v>
       </c>
       <c r="X741" t="n">
-        <v>123</v>
+        <v>123.3</v>
       </c>
       <c r="Y741" t="n">
-        <v>146.9</v>
+        <v>147</v>
       </c>
       <c r="Z741" t="n">
-        <v>1028</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="742">
@@ -59586,7 +59586,7 @@
         <v>1968</v>
       </c>
       <c r="J742" t="n">
-        <v>105676</v>
+        <v>105677</v>
       </c>
       <c r="K742" t="n">
         <v>7803413</v>
@@ -59631,10 +59631,10 @@
         <v>147.3</v>
       </c>
       <c r="Y742" t="n">
-        <v>154.9</v>
+        <v>155</v>
       </c>
       <c r="Z742" t="n">
-        <v>1084</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="743">
@@ -59666,7 +59666,7 @@
         <v>1992</v>
       </c>
       <c r="J743" t="n">
-        <v>105970</v>
+        <v>105971</v>
       </c>
       <c r="K743" t="n">
         <v>7959385</v>
@@ -59711,10 +59711,10 @@
         <v>207.7</v>
       </c>
       <c r="Y743" t="n">
-        <v>163.3</v>
+        <v>163.4</v>
       </c>
       <c r="Z743" t="n">
-        <v>1143</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="744">
@@ -59746,7 +59746,7 @@
         <v>2021</v>
       </c>
       <c r="J744" t="n">
-        <v>106174</v>
+        <v>106175</v>
       </c>
       <c r="K744" t="n">
         <v>8111529</v>
@@ -59791,10 +59791,10 @@
         <v>235.7</v>
       </c>
       <c r="Y744" t="n">
-        <v>176.3</v>
+        <v>176.4</v>
       </c>
       <c r="Z744" t="n">
-        <v>1234</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="745">
@@ -59826,7 +59826,7 @@
         <v>2008</v>
       </c>
       <c r="J745" t="n">
-        <v>106371</v>
+        <v>106372</v>
       </c>
       <c r="K745" t="n">
         <v>8255805</v>
@@ -59871,10 +59871,10 @@
         <v>231.7</v>
       </c>
       <c r="Y745" t="n">
-        <v>181.9</v>
+        <v>182</v>
       </c>
       <c r="Z745" t="n">
-        <v>1273</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="746">
@@ -59906,7 +59906,7 @@
         <v>1874</v>
       </c>
       <c r="J746" t="n">
-        <v>106538</v>
+        <v>106539</v>
       </c>
       <c r="K746" t="n">
         <v>8397622</v>
@@ -59986,7 +59986,7 @@
         <v>1315</v>
       </c>
       <c r="J747" t="n">
-        <v>106677</v>
+        <v>106678</v>
       </c>
       <c r="K747" t="n">
         <v>8466478</v>
@@ -60066,7 +60066,7 @@
         <v>1706</v>
       </c>
       <c r="J748" t="n">
-        <v>106802</v>
+        <v>106803</v>
       </c>
       <c r="K748" t="n">
         <v>8547859</v>
@@ -60146,7 +60146,7 @@
         <v>2022</v>
       </c>
       <c r="J749" t="n">
-        <v>107029</v>
+        <v>107030</v>
       </c>
       <c r="K749" t="n">
         <v>8727772</v>
@@ -60226,7 +60226,7 @@
         <v>2011</v>
       </c>
       <c r="J750" t="n">
-        <v>107383</v>
+        <v>107384</v>
       </c>
       <c r="K750" t="n">
         <v>8864970</v>
@@ -60306,7 +60306,7 @@
         <v>2023</v>
       </c>
       <c r="J751" t="n">
-        <v>107658</v>
+        <v>107660</v>
       </c>
       <c r="K751" t="n">
         <v>9003659</v>
@@ -60342,19 +60342,19 @@
         <v>72537.9</v>
       </c>
       <c r="V751" t="n">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="W751" t="n">
         <v>0.3</v>
       </c>
       <c r="X751" t="n">
-        <v>285.3</v>
+        <v>285.7</v>
       </c>
       <c r="Y751" t="n">
-        <v>212</v>
+        <v>212.1</v>
       </c>
       <c r="Z751" t="n">
-        <v>1484</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="752">
@@ -60362,10 +60362,10 @@
         <v>44581</v>
       </c>
       <c r="B752" t="n">
-        <v>54731</v>
+        <v>54730</v>
       </c>
       <c r="C752" t="n">
-        <v>21456</v>
+        <v>21455</v>
       </c>
       <c r="D752" t="n">
         <v>5629507</v>
@@ -60386,40 +60386,40 @@
         <v>1975</v>
       </c>
       <c r="J752" t="n">
-        <v>107936</v>
+        <v>107938</v>
       </c>
       <c r="K752" t="n">
-        <v>9146182</v>
+        <v>9146181</v>
       </c>
       <c r="L752" t="n">
-        <v>5190881</v>
+        <v>5190880</v>
       </c>
       <c r="M752" t="n">
         <v>15126</v>
       </c>
       <c r="N752" t="n">
-        <v>1834194</v>
+        <v>1834193</v>
       </c>
       <c r="O752" t="n">
-        <v>890377</v>
+        <v>890376</v>
       </c>
       <c r="P752" t="n">
-        <v>1030234</v>
+        <v>1030233</v>
       </c>
       <c r="Q752" t="n">
-        <v>499353</v>
+        <v>499352</v>
       </c>
       <c r="R752" t="n">
-        <v>142523</v>
+        <v>142522</v>
       </c>
       <c r="S752" t="n">
-        <v>127196.7</v>
+        <v>127196.6</v>
       </c>
       <c r="T752" t="n">
-        <v>69632</v>
+        <v>69631</v>
       </c>
       <c r="U752" t="n">
-        <v>71336.1</v>
+        <v>71336</v>
       </c>
       <c r="V752" t="n">
         <v>278</v>
@@ -60428,13 +60428,13 @@
         <v>0.3</v>
       </c>
       <c r="X752" t="n">
-        <v>302.3</v>
+        <v>302.7</v>
       </c>
       <c r="Y752" t="n">
-        <v>223.6</v>
+        <v>223.7</v>
       </c>
       <c r="Z752" t="n">
-        <v>1565</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="753">
@@ -60466,40 +60466,40 @@
         <v>1601</v>
       </c>
       <c r="J753" t="n">
-        <v>108143</v>
+        <v>108145</v>
       </c>
       <c r="K753" t="n">
-        <v>9264312</v>
+        <v>9264311</v>
       </c>
       <c r="L753" t="n">
-        <v>5257902</v>
+        <v>5257901</v>
       </c>
       <c r="M753" t="n">
         <v>15336</v>
       </c>
       <c r="N753" t="n">
-        <v>1803385</v>
+        <v>1803384</v>
       </c>
       <c r="O753" t="n">
-        <v>866690</v>
+        <v>866689</v>
       </c>
       <c r="P753" t="n">
-        <v>1017320</v>
+        <v>1017319</v>
       </c>
       <c r="Q753" t="n">
-        <v>487961</v>
+        <v>487960</v>
       </c>
       <c r="R753" t="n">
         <v>118130</v>
       </c>
       <c r="S753" t="n">
-        <v>123812.9</v>
+        <v>123812.7</v>
       </c>
       <c r="T753" t="n">
         <v>67021</v>
       </c>
       <c r="U753" t="n">
-        <v>69708.7</v>
+        <v>69708.6</v>
       </c>
       <c r="V753" t="n">
         <v>207</v>
@@ -60508,13 +60508,13 @@
         <v>0.2</v>
       </c>
       <c r="X753" t="n">
-        <v>253.3</v>
+        <v>253.7</v>
       </c>
       <c r="Y753" t="n">
-        <v>229.3</v>
+        <v>229.4</v>
       </c>
       <c r="Z753" t="n">
-        <v>1605</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="754">
@@ -60546,40 +60546,40 @@
         <v>1384</v>
       </c>
       <c r="J754" t="n">
-        <v>108300</v>
+        <v>108302</v>
       </c>
       <c r="K754" t="n">
-        <v>9331584</v>
+        <v>9331583</v>
       </c>
       <c r="L754" t="n">
-        <v>5295873</v>
+        <v>5295872</v>
       </c>
       <c r="M754" t="n">
         <v>15351</v>
       </c>
       <c r="N754" t="n">
-        <v>1793360</v>
+        <v>1793359</v>
       </c>
       <c r="O754" t="n">
-        <v>865106</v>
+        <v>865105</v>
       </c>
       <c r="P754" t="n">
-        <v>1011344</v>
+        <v>1011343</v>
       </c>
       <c r="Q754" t="n">
-        <v>484642</v>
+        <v>484641</v>
       </c>
       <c r="R754" t="n">
         <v>67272</v>
       </c>
       <c r="S754" t="n">
-        <v>123586.6</v>
+        <v>123586.4</v>
       </c>
       <c r="T754" t="n">
         <v>37971</v>
       </c>
       <c r="U754" t="n">
-        <v>69234.6</v>
+        <v>69234.4</v>
       </c>
       <c r="V754" t="n">
         <v>157</v>
@@ -60591,10 +60591,10 @@
         <v>214</v>
       </c>
       <c r="Y754" t="n">
-        <v>231.9</v>
+        <v>232</v>
       </c>
       <c r="Z754" t="n">
-        <v>1623</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="755">
@@ -60602,10 +60602,10 @@
         <v>44584</v>
       </c>
       <c r="B755" t="n">
-        <v>14375</v>
+        <v>14374</v>
       </c>
       <c r="C755" t="n">
-        <v>7813</v>
+        <v>7812</v>
       </c>
       <c r="D755" t="n">
         <v>5659967</v>
@@ -60626,40 +60626,40 @@
         <v>1740</v>
       </c>
       <c r="J755" t="n">
-        <v>108438</v>
+        <v>108440</v>
       </c>
       <c r="K755" t="n">
-        <v>9393998</v>
+        <v>9393996</v>
       </c>
       <c r="L755" t="n">
-        <v>5335413</v>
+        <v>5335411</v>
       </c>
       <c r="M755" t="n">
         <v>15511</v>
       </c>
       <c r="N755" t="n">
-        <v>1772413</v>
+        <v>1772411</v>
       </c>
       <c r="O755" t="n">
-        <v>846139</v>
+        <v>846137</v>
       </c>
       <c r="P755" t="n">
-        <v>998347</v>
+        <v>998345</v>
       </c>
       <c r="Q755" t="n">
-        <v>474138</v>
+        <v>474136</v>
       </c>
       <c r="R755" t="n">
-        <v>62414</v>
+        <v>62413</v>
       </c>
       <c r="S755" t="n">
-        <v>120877</v>
+        <v>120876.7</v>
       </c>
       <c r="T755" t="n">
-        <v>39540</v>
+        <v>39539</v>
       </c>
       <c r="U755" t="n">
-        <v>67734</v>
+        <v>67733.7</v>
       </c>
       <c r="V755" t="n">
         <v>138</v>
@@ -60671,10 +60671,10 @@
         <v>167.3</v>
       </c>
       <c r="Y755" t="n">
-        <v>233.7</v>
+        <v>233.9</v>
       </c>
       <c r="Z755" t="n">
-        <v>1636</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="756">
@@ -60706,40 +60706,40 @@
         <v>2004</v>
       </c>
       <c r="J756" t="n">
-        <v>108715</v>
+        <v>108717</v>
       </c>
       <c r="K756" t="n">
-        <v>9557674</v>
+        <v>9557672</v>
       </c>
       <c r="L756" t="n">
-        <v>5408218</v>
+        <v>5408216</v>
       </c>
       <c r="M756" t="n">
         <v>15855</v>
       </c>
       <c r="N756" t="n">
-        <v>1754261</v>
+        <v>1754259</v>
       </c>
       <c r="O756" t="n">
-        <v>829902</v>
+        <v>829900</v>
       </c>
       <c r="P756" t="n">
-        <v>971971</v>
+        <v>971969</v>
       </c>
       <c r="Q756" t="n">
-        <v>451085</v>
+        <v>451083</v>
       </c>
       <c r="R756" t="n">
         <v>163676</v>
       </c>
       <c r="S756" t="n">
-        <v>118557.4</v>
+        <v>118557.1</v>
       </c>
       <c r="T756" t="n">
         <v>72805</v>
       </c>
       <c r="U756" t="n">
-        <v>64440.7</v>
+        <v>64440.4</v>
       </c>
       <c r="V756" t="n">
         <v>277</v>
@@ -60751,10 +60751,10 @@
         <v>190.7</v>
       </c>
       <c r="Y756" t="n">
-        <v>240.9</v>
+        <v>241</v>
       </c>
       <c r="Z756" t="n">
-        <v>1686</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="757">
@@ -60786,40 +60786,40 @@
         <v>1976</v>
       </c>
       <c r="J757" t="n">
-        <v>109137</v>
+        <v>109139</v>
       </c>
       <c r="K757" t="n">
-        <v>9680313</v>
+        <v>9680311</v>
       </c>
       <c r="L757" t="n">
-        <v>5467104</v>
+        <v>5467102</v>
       </c>
       <c r="M757" t="n">
         <v>16098</v>
       </c>
       <c r="N757" t="n">
-        <v>1720928</v>
+        <v>1720926</v>
       </c>
       <c r="O757" t="n">
-        <v>815343</v>
+        <v>815341</v>
       </c>
       <c r="P757" t="n">
-        <v>940714</v>
+        <v>940712</v>
       </c>
       <c r="Q757" t="n">
-        <v>425849</v>
+        <v>425847</v>
       </c>
       <c r="R757" t="n">
         <v>122639</v>
       </c>
       <c r="S757" t="n">
-        <v>116477.6</v>
+        <v>116477.3</v>
       </c>
       <c r="T757" t="n">
         <v>58886</v>
       </c>
       <c r="U757" t="n">
-        <v>60835.6</v>
+        <v>60835.3</v>
       </c>
       <c r="V757" t="n">
         <v>422</v>
@@ -60831,10 +60831,10 @@
         <v>279</v>
       </c>
       <c r="Y757" t="n">
-        <v>250.6</v>
+        <v>250.7</v>
       </c>
       <c r="Z757" t="n">
-        <v>1754</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="758">
@@ -60866,40 +60866,40 @@
         <v>1958</v>
       </c>
       <c r="J758" t="n">
-        <v>109400</v>
+        <v>109402</v>
       </c>
       <c r="K758" t="n">
-        <v>9592485</v>
+        <v>9592483</v>
       </c>
       <c r="L758" t="n">
-        <v>5521315</v>
+        <v>5521313</v>
       </c>
       <c r="M758" t="n">
         <v>16324</v>
       </c>
       <c r="N758" t="n">
-        <v>1480956</v>
+        <v>1480954</v>
       </c>
       <c r="O758" t="n">
-        <v>588826</v>
+        <v>588824</v>
       </c>
       <c r="P758" t="n">
-        <v>907831</v>
+        <v>907829</v>
       </c>
       <c r="Q758" t="n">
-        <v>400066</v>
+        <v>400064</v>
       </c>
       <c r="R758" t="n">
         <v>-87828</v>
       </c>
       <c r="S758" t="n">
-        <v>84118</v>
+        <v>84117.7</v>
       </c>
       <c r="T758" t="n">
         <v>54211</v>
       </c>
       <c r="U758" t="n">
-        <v>57152.3</v>
+        <v>57152</v>
       </c>
       <c r="V758" t="n">
         <v>263</v>
@@ -60946,40 +60946,40 @@
         <v>1907</v>
       </c>
       <c r="J759" t="n">
-        <v>109666</v>
+        <v>109668</v>
       </c>
       <c r="K759" t="n">
-        <v>9703640</v>
+        <v>9703638</v>
       </c>
       <c r="L759" t="n">
-        <v>5570911</v>
+        <v>5570909</v>
       </c>
       <c r="M759" t="n">
         <v>16580</v>
       </c>
       <c r="N759" t="n">
-        <v>1447835</v>
+        <v>1447833</v>
       </c>
       <c r="O759" t="n">
-        <v>557458</v>
+        <v>557457</v>
       </c>
       <c r="P759" t="n">
-        <v>879383</v>
+        <v>879381</v>
       </c>
       <c r="Q759" t="n">
-        <v>380030</v>
+        <v>380029</v>
       </c>
       <c r="R759" t="n">
         <v>111155</v>
       </c>
       <c r="S759" t="n">
-        <v>79636.9</v>
+        <v>79636.7</v>
       </c>
       <c r="T759" t="n">
         <v>49596</v>
       </c>
       <c r="U759" t="n">
-        <v>54290</v>
+        <v>54289.9</v>
       </c>
       <c r="V759" t="n">
         <v>266</v>
@@ -61026,40 +61026,40 @@
         <v>1785</v>
       </c>
       <c r="J760" t="n">
-        <v>109894</v>
+        <v>109896</v>
       </c>
       <c r="K760" t="n">
-        <v>9794369</v>
+        <v>9794367</v>
       </c>
       <c r="L760" t="n">
-        <v>5612831</v>
+        <v>5612829</v>
       </c>
       <c r="M760" t="n">
         <v>16755</v>
       </c>
       <c r="N760" t="n">
-        <v>1396747</v>
+        <v>1396745</v>
       </c>
       <c r="O760" t="n">
-        <v>530057</v>
+        <v>530056</v>
       </c>
       <c r="P760" t="n">
-        <v>842890</v>
+        <v>842888</v>
       </c>
       <c r="Q760" t="n">
-        <v>354929</v>
+        <v>354928</v>
       </c>
       <c r="R760" t="n">
         <v>90729</v>
       </c>
       <c r="S760" t="n">
-        <v>75722.4</v>
+        <v>75722.3</v>
       </c>
       <c r="T760" t="n">
         <v>41920</v>
       </c>
       <c r="U760" t="n">
-        <v>50704.1</v>
+        <v>50704</v>
       </c>
       <c r="V760" t="n">
         <v>228</v>
@@ -61106,40 +61106,40 @@
         <v>1318</v>
       </c>
       <c r="J761" t="n">
-        <v>110046</v>
+        <v>110048</v>
       </c>
       <c r="K761" t="n">
-        <v>9836276</v>
+        <v>9836274</v>
       </c>
       <c r="L761" t="n">
-        <v>5635227</v>
+        <v>5635225</v>
       </c>
       <c r="M761" t="n">
         <v>16756</v>
       </c>
       <c r="N761" t="n">
-        <v>1369798</v>
+        <v>1369796</v>
       </c>
       <c r="O761" t="n">
-        <v>504692</v>
+        <v>504691</v>
       </c>
       <c r="P761" t="n">
-        <v>823996</v>
+        <v>823994</v>
       </c>
       <c r="Q761" t="n">
-        <v>339354</v>
+        <v>339353</v>
       </c>
       <c r="R761" t="n">
         <v>41907</v>
       </c>
       <c r="S761" t="n">
-        <v>72098.9</v>
+        <v>72098.7</v>
       </c>
       <c r="T761" t="n">
         <v>22396</v>
       </c>
       <c r="U761" t="n">
-        <v>48479.1</v>
+        <v>48479</v>
       </c>
       <c r="V761" t="n">
         <v>152</v>
@@ -61186,25 +61186,25 @@
         <v>1670</v>
       </c>
       <c r="J762" t="n">
-        <v>110176</v>
+        <v>110178</v>
       </c>
       <c r="K762" t="n">
-        <v>9874957</v>
+        <v>9874955</v>
       </c>
       <c r="L762" t="n">
-        <v>5658211</v>
+        <v>5658209</v>
       </c>
       <c r="M762" t="n">
         <v>16849</v>
       </c>
       <c r="N762" t="n">
-        <v>1327098</v>
+        <v>1327096</v>
       </c>
       <c r="O762" t="n">
         <v>480959</v>
       </c>
       <c r="P762" t="n">
-        <v>796936</v>
+        <v>796934</v>
       </c>
       <c r="Q762" t="n">
         <v>322798</v>
@@ -61266,25 +61266,25 @@
         <v>1878</v>
       </c>
       <c r="J763" t="n">
-        <v>110463</v>
+        <v>110465</v>
       </c>
       <c r="K763" t="n">
-        <v>9964496</v>
+        <v>9964494</v>
       </c>
       <c r="L763" t="n">
-        <v>5702792</v>
+        <v>5702790</v>
       </c>
       <c r="M763" t="n">
         <v>17075</v>
       </c>
       <c r="N763" t="n">
-        <v>1236724</v>
+        <v>1236722</v>
       </c>
       <c r="O763" t="n">
         <v>406822</v>
       </c>
       <c r="P763" t="n">
-        <v>745659</v>
+        <v>745657</v>
       </c>
       <c r="Q763" t="n">
         <v>294574</v>
@@ -61346,25 +61346,25 @@
         <v>1859</v>
       </c>
       <c r="J764" t="n">
-        <v>110927</v>
+        <v>110929</v>
       </c>
       <c r="K764" t="n">
-        <v>10035854</v>
+        <v>10035852</v>
       </c>
       <c r="L764" t="n">
-        <v>5542679</v>
+        <v>5542677</v>
       </c>
       <c r="M764" t="n">
         <v>17226</v>
       </c>
       <c r="N764" t="n">
-        <v>1170884</v>
+        <v>1170882</v>
       </c>
       <c r="O764" t="n">
         <v>355541</v>
       </c>
       <c r="P764" t="n">
-        <v>501424</v>
+        <v>501422</v>
       </c>
       <c r="Q764" t="n">
         <v>75575</v>
@@ -61426,25 +61426,25 @@
         <v>1810</v>
       </c>
       <c r="J765" t="n">
-        <v>111162</v>
+        <v>111164</v>
       </c>
       <c r="K765" t="n">
-        <v>10109440</v>
+        <v>10109438</v>
       </c>
       <c r="L765" t="n">
-        <v>5575886</v>
+        <v>5575884</v>
       </c>
       <c r="M765" t="n">
         <v>17408</v>
       </c>
       <c r="N765" t="n">
-        <v>1105781</v>
+        <v>1105779</v>
       </c>
       <c r="O765" t="n">
         <v>516955</v>
       </c>
       <c r="P765" t="n">
-        <v>454637</v>
+        <v>454635</v>
       </c>
       <c r="Q765" t="n">
         <v>54571</v>
@@ -61506,25 +61506,25 @@
         <v>1737</v>
       </c>
       <c r="J766" t="n">
-        <v>111439</v>
+        <v>111441</v>
       </c>
       <c r="K766" t="n">
-        <v>10174646</v>
+        <v>10174644</v>
       </c>
       <c r="L766" t="n">
-        <v>5605762</v>
+        <v>5605760</v>
       </c>
       <c r="M766" t="n">
         <v>17548</v>
       </c>
       <c r="N766" t="n">
-        <v>1028464</v>
+        <v>1028463</v>
       </c>
       <c r="O766" t="n">
         <v>471006</v>
       </c>
       <c r="P766" t="n">
-        <v>414881</v>
+        <v>414880</v>
       </c>
       <c r="Q766" t="n">
         <v>34851</v>
@@ -61586,25 +61586,25 @@
         <v>1588</v>
       </c>
       <c r="J767" t="n">
-        <v>111666</v>
+        <v>111668</v>
       </c>
       <c r="K767" t="n">
-        <v>10231534</v>
+        <v>10231532</v>
       </c>
       <c r="L767" t="n">
-        <v>5632287</v>
+        <v>5632285</v>
       </c>
       <c r="M767" t="n">
         <v>17735</v>
       </c>
       <c r="N767" t="n">
-        <v>967222</v>
+        <v>967221</v>
       </c>
       <c r="O767" t="n">
         <v>437165</v>
       </c>
       <c r="P767" t="n">
-        <v>374385</v>
+        <v>374384</v>
       </c>
       <c r="Q767" t="n">
         <v>19456</v>
@@ -61666,25 +61666,25 @@
         <v>1159</v>
       </c>
       <c r="J768" t="n">
-        <v>111854</v>
+        <v>111856</v>
       </c>
       <c r="K768" t="n">
-        <v>10256425</v>
+        <v>10256423</v>
       </c>
       <c r="L768" t="n">
-        <v>5644865</v>
+        <v>5644863</v>
       </c>
       <c r="M768" t="n">
         <v>17784</v>
       </c>
       <c r="N768" t="n">
-        <v>924841</v>
+        <v>924840</v>
       </c>
       <c r="O768" t="n">
         <v>420149</v>
       </c>
       <c r="P768" t="n">
-        <v>348992</v>
+        <v>348991</v>
       </c>
       <c r="Q768" t="n">
         <v>9638</v>
@@ -61746,13 +61746,13 @@
         <v>1469</v>
       </c>
       <c r="J769" t="n">
-        <v>111990</v>
+        <v>111992</v>
       </c>
       <c r="K769" t="n">
-        <v>10286373</v>
+        <v>10286371</v>
       </c>
       <c r="L769" t="n">
-        <v>5657421</v>
+        <v>5657419</v>
       </c>
       <c r="M769" t="n">
         <v>17862</v>
@@ -61826,13 +61826,13 @@
         <v>1652</v>
       </c>
       <c r="J770" t="n">
-        <v>112199</v>
+        <v>112201</v>
       </c>
       <c r="K770" t="n">
-        <v>10349145</v>
+        <v>10349143</v>
       </c>
       <c r="L770" t="n">
-        <v>5685932</v>
+        <v>5685930</v>
       </c>
       <c r="M770" t="n">
         <v>18016</v>
@@ -61906,13 +61906,13 @@
         <v>1564</v>
       </c>
       <c r="J771" t="n">
-        <v>112672</v>
+        <v>112674</v>
       </c>
       <c r="K771" t="n">
-        <v>10392328</v>
+        <v>10392326</v>
       </c>
       <c r="L771" t="n">
-        <v>5707630</v>
+        <v>5707628</v>
       </c>
       <c r="M771" t="n">
         <v>18104</v>
@@ -61986,13 +61986,13 @@
         <v>1518</v>
       </c>
       <c r="J772" t="n">
-        <v>112912</v>
+        <v>112914</v>
       </c>
       <c r="K772" t="n">
-        <v>10434469</v>
+        <v>10434467</v>
       </c>
       <c r="L772" t="n">
-        <v>5727760</v>
+        <v>5727758</v>
       </c>
       <c r="M772" t="n">
         <v>18194</v>
@@ -62066,13 +62066,13 @@
         <v>1491</v>
       </c>
       <c r="J773" t="n">
-        <v>113110</v>
+        <v>113112</v>
       </c>
       <c r="K773" t="n">
-        <v>10478992</v>
+        <v>10478990</v>
       </c>
       <c r="L773" t="n">
-        <v>5744531</v>
+        <v>5744529</v>
       </c>
       <c r="M773" t="n">
         <v>18284</v>
@@ -62146,13 +62146,13 @@
         <v>1366</v>
       </c>
       <c r="J774" t="n">
-        <v>113339</v>
+        <v>113341</v>
       </c>
       <c r="K774" t="n">
-        <v>10516255</v>
+        <v>10516253</v>
       </c>
       <c r="L774" t="n">
-        <v>5760954</v>
+        <v>5760952</v>
       </c>
       <c r="M774" t="n">
         <v>18316</v>
@@ -62226,13 +62226,13 @@
         <v>1010</v>
       </c>
       <c r="J775" t="n">
-        <v>113432</v>
+        <v>113434</v>
       </c>
       <c r="K775" t="n">
-        <v>10528193</v>
+        <v>10528191</v>
       </c>
       <c r="L775" t="n">
-        <v>5768426</v>
+        <v>5768424</v>
       </c>
       <c r="M775" t="n">
         <v>18348</v>
@@ -62306,13 +62306,13 @@
         <v>1237</v>
       </c>
       <c r="J776" t="n">
-        <v>113561</v>
+        <v>113563</v>
       </c>
       <c r="K776" t="n">
-        <v>10548091</v>
+        <v>10548089</v>
       </c>
       <c r="L776" t="n">
-        <v>5775804</v>
+        <v>5775802</v>
       </c>
       <c r="M776" t="n">
         <v>18427</v>
@@ -62386,13 +62386,13 @@
         <v>1377</v>
       </c>
       <c r="J777" t="n">
-        <v>113800</v>
+        <v>113802</v>
       </c>
       <c r="K777" t="n">
-        <v>10590615</v>
+        <v>10590613</v>
       </c>
       <c r="L777" t="n">
-        <v>5792944</v>
+        <v>5792942</v>
       </c>
       <c r="M777" t="n">
         <v>18553</v>
@@ -62466,13 +62466,13 @@
         <v>1317</v>
       </c>
       <c r="J778" t="n">
-        <v>114193</v>
+        <v>114195</v>
       </c>
       <c r="K778" t="n">
-        <v>10620332</v>
+        <v>10620330</v>
       </c>
       <c r="L778" t="n">
-        <v>5807284</v>
+        <v>5807282</v>
       </c>
       <c r="M778" t="n">
         <v>18626</v>
@@ -62546,13 +62546,13 @@
         <v>1276</v>
       </c>
       <c r="J779" t="n">
-        <v>114405</v>
+        <v>114407</v>
       </c>
       <c r="K779" t="n">
-        <v>10648997</v>
+        <v>10648995</v>
       </c>
       <c r="L779" t="n">
-        <v>5820889</v>
+        <v>5820887</v>
       </c>
       <c r="M779" t="n">
         <v>18798</v>
@@ -62626,13 +62626,13 @@
         <v>1231</v>
       </c>
       <c r="J780" t="n">
-        <v>114593</v>
+        <v>114595</v>
       </c>
       <c r="K780" t="n">
-        <v>10676304</v>
+        <v>10676302</v>
       </c>
       <c r="L780" t="n">
-        <v>5833115</v>
+        <v>5833113</v>
       </c>
       <c r="M780" t="n">
         <v>18954</v>
@@ -62706,13 +62706,13 @@
         <v>1135</v>
       </c>
       <c r="J781" t="n">
-        <v>114704</v>
+        <v>114706</v>
       </c>
       <c r="K781" t="n">
-        <v>10700242</v>
+        <v>10700240</v>
       </c>
       <c r="L781" t="n">
-        <v>5844067</v>
+        <v>5844065</v>
       </c>
       <c r="M781" t="n">
         <v>19068</v>
@@ -62786,13 +62786,13 @@
         <v>783</v>
       </c>
       <c r="J782" t="n">
-        <v>114770</v>
+        <v>114772</v>
       </c>
       <c r="K782" t="n">
-        <v>10708836</v>
+        <v>10708834</v>
       </c>
       <c r="L782" t="n">
-        <v>5849687</v>
+        <v>5849685</v>
       </c>
       <c r="M782" t="n">
         <v>19145</v>
@@ -62866,13 +62866,13 @@
         <v>955</v>
       </c>
       <c r="J783" t="n">
-        <v>114854</v>
+        <v>114856</v>
       </c>
       <c r="K783" t="n">
-        <v>10722767</v>
+        <v>10722765</v>
       </c>
       <c r="L783" t="n">
-        <v>5855337</v>
+        <v>5855335</v>
       </c>
       <c r="M783" t="n">
         <v>0</v>
@@ -62946,13 +62946,13 @@
         <v>1138</v>
       </c>
       <c r="J784" t="n">
-        <v>115008</v>
+        <v>115010</v>
       </c>
       <c r="K784" t="n">
-        <v>10752713</v>
+        <v>10752711</v>
       </c>
       <c r="L784" t="n">
-        <v>5868477</v>
+        <v>5868475</v>
       </c>
       <c r="M784" t="n">
         <v>19284</v>
@@ -63026,13 +63026,13 @@
         <v>1090</v>
       </c>
       <c r="J785" t="n">
-        <v>115267</v>
+        <v>115269</v>
       </c>
       <c r="K785" t="n">
-        <v>10774370</v>
+        <v>10774368</v>
       </c>
       <c r="L785" t="n">
-        <v>5879830</v>
+        <v>5879828</v>
       </c>
       <c r="M785" t="n">
         <v>19350</v>
@@ -63106,13 +63106,13 @@
         <v>1035</v>
       </c>
       <c r="J786" t="n">
-        <v>115373</v>
+        <v>115375</v>
       </c>
       <c r="K786" t="n">
-        <v>10798543</v>
+        <v>10798541</v>
       </c>
       <c r="L786" t="n">
-        <v>5891089</v>
+        <v>5891087</v>
       </c>
       <c r="M786" t="n">
         <v>19370</v>
@@ -63186,13 +63186,13 @@
         <v>994</v>
       </c>
       <c r="J787" t="n">
-        <v>115507</v>
+        <v>115509</v>
       </c>
       <c r="K787" t="n">
-        <v>10821943</v>
+        <v>10821941</v>
       </c>
       <c r="L787" t="n">
-        <v>5900697</v>
+        <v>5900695</v>
       </c>
       <c r="M787" t="n">
         <v>19395</v>
@@ -63266,13 +63266,13 @@
         <v>893</v>
       </c>
       <c r="J788" t="n">
-        <v>115628</v>
+        <v>115630</v>
       </c>
       <c r="K788" t="n">
-        <v>10839492</v>
+        <v>10839490</v>
       </c>
       <c r="L788" t="n">
-        <v>5909291</v>
+        <v>5909289</v>
       </c>
       <c r="M788" t="n">
         <v>19460</v>
@@ -63346,13 +63346,13 @@
         <v>627</v>
       </c>
       <c r="J789" t="n">
-        <v>115680</v>
+        <v>115682</v>
       </c>
       <c r="K789" t="n">
-        <v>10846159</v>
+        <v>10846157</v>
       </c>
       <c r="L789" t="n">
-        <v>5913774</v>
+        <v>5913772</v>
       </c>
       <c r="M789" t="n">
         <v>19460</v>
@@ -63426,13 +63426,13 @@
         <v>773</v>
       </c>
       <c r="J790" t="n">
-        <v>115733</v>
+        <v>115735</v>
       </c>
       <c r="K790" t="n">
-        <v>10856048</v>
+        <v>10856046</v>
       </c>
       <c r="L790" t="n">
-        <v>5917679</v>
+        <v>5917677</v>
       </c>
       <c r="M790" t="n">
         <v>19471</v>
@@ -63506,13 +63506,13 @@
         <v>819</v>
       </c>
       <c r="J791" t="n">
-        <v>115853</v>
+        <v>115855</v>
       </c>
       <c r="K791" t="n">
-        <v>10878596</v>
+        <v>10878594</v>
       </c>
       <c r="L791" t="n">
-        <v>5928701</v>
+        <v>5928699</v>
       </c>
       <c r="M791" t="n">
         <v>19515</v>
@@ -63586,13 +63586,13 @@
         <v>890</v>
       </c>
       <c r="J792" t="n">
-        <v>116089</v>
+        <v>116091</v>
       </c>
       <c r="K792" t="n">
-        <v>10894623</v>
+        <v>10894621</v>
       </c>
       <c r="L792" t="n">
-        <v>5937635</v>
+        <v>5937633</v>
       </c>
       <c r="M792" t="n">
         <v>19545</v>
@@ -63666,13 +63666,13 @@
         <v>796</v>
       </c>
       <c r="J793" t="n">
-        <v>116162</v>
+        <v>116164</v>
       </c>
       <c r="K793" t="n">
-        <v>10912692</v>
+        <v>10912690</v>
       </c>
       <c r="L793" t="n">
-        <v>5948407</v>
+        <v>5948405</v>
       </c>
       <c r="M793" t="n">
         <v>19608</v>
@@ -63746,13 +63746,13 @@
         <v>832</v>
       </c>
       <c r="J794" t="n">
-        <v>116269</v>
+        <v>116271</v>
       </c>
       <c r="K794" t="n">
-        <v>10931767</v>
+        <v>10931765</v>
       </c>
       <c r="L794" t="n">
-        <v>5958299</v>
+        <v>5958297</v>
       </c>
       <c r="M794" t="n">
         <v>19632</v>
@@ -63826,13 +63826,13 @@
         <v>623</v>
       </c>
       <c r="J795" t="n">
-        <v>116358</v>
+        <v>116360</v>
       </c>
       <c r="K795" t="n">
-        <v>10949345</v>
+        <v>10949343</v>
       </c>
       <c r="L795" t="n">
-        <v>5967214</v>
+        <v>5967212</v>
       </c>
       <c r="M795" t="n">
         <v>19702</v>
@@ -63906,13 +63906,13 @@
         <v>391</v>
       </c>
       <c r="J796" t="n">
-        <v>116386</v>
+        <v>116388</v>
       </c>
       <c r="K796" t="n">
-        <v>10957126</v>
+        <v>10957124</v>
       </c>
       <c r="L796" t="n">
-        <v>5971669</v>
+        <v>5971667</v>
       </c>
       <c r="M796" t="n">
         <v>19702</v>
@@ -63986,13 +63986,13 @@
         <v>647</v>
       </c>
       <c r="J797" t="n">
-        <v>116461</v>
+        <v>116463</v>
       </c>
       <c r="K797" t="n">
-        <v>10967353</v>
+        <v>10967351</v>
       </c>
       <c r="L797" t="n">
-        <v>5976095</v>
+        <v>5976093</v>
       </c>
       <c r="M797" t="n">
         <v>19748</v>
@@ -64066,13 +64066,13 @@
         <v>734</v>
       </c>
       <c r="J798" t="n">
-        <v>116561</v>
+        <v>116563</v>
       </c>
       <c r="K798" t="n">
-        <v>10989701</v>
+        <v>10989699</v>
       </c>
       <c r="L798" t="n">
-        <v>5986283</v>
+        <v>5986281</v>
       </c>
       <c r="M798" t="n">
         <v>19763</v>
@@ -64146,13 +64146,13 @@
         <v>731</v>
       </c>
       <c r="J799" t="n">
-        <v>116794</v>
+        <v>116796</v>
       </c>
       <c r="K799" t="n">
-        <v>11006652</v>
+        <v>11006650</v>
       </c>
       <c r="L799" t="n">
-        <v>5995471</v>
+        <v>5995469</v>
       </c>
       <c r="M799" t="n">
         <v>19816</v>
@@ -64226,13 +64226,13 @@
         <v>719</v>
       </c>
       <c r="J800" t="n">
-        <v>116863</v>
+        <v>116865</v>
       </c>
       <c r="K800" t="n">
-        <v>11025386</v>
+        <v>11025384</v>
       </c>
       <c r="L800" t="n">
-        <v>6004808</v>
+        <v>6004806</v>
       </c>
       <c r="M800" t="n">
         <v>19879</v>
@@ -64306,13 +64306,13 @@
         <v>689</v>
       </c>
       <c r="J801" t="n">
-        <v>116957</v>
+        <v>116959</v>
       </c>
       <c r="K801" t="n">
-        <v>11043205</v>
+        <v>11043203</v>
       </c>
       <c r="L801" t="n">
-        <v>6013555</v>
+        <v>6013553</v>
       </c>
       <c r="M801" t="n">
         <v>19892</v>
@@ -64386,13 +64386,13 @@
         <v>469</v>
       </c>
       <c r="J802" t="n">
-        <v>117028</v>
+        <v>117030</v>
       </c>
       <c r="K802" t="n">
-        <v>11058633</v>
+        <v>11058631</v>
       </c>
       <c r="L802" t="n">
-        <v>6020539</v>
+        <v>6020537</v>
       </c>
       <c r="M802" t="n">
         <v>19906</v>
@@ -64466,13 +64466,13 @@
         <v>301</v>
       </c>
       <c r="J803" t="n">
-        <v>117057</v>
+        <v>117059</v>
       </c>
       <c r="K803" t="n">
-        <v>11067191</v>
+        <v>11067189</v>
       </c>
       <c r="L803" t="n">
-        <v>6024650</v>
+        <v>6024648</v>
       </c>
       <c r="M803" t="n">
         <v>19908</v>
@@ -64546,13 +64546,13 @@
         <v>392</v>
       </c>
       <c r="J804" t="n">
-        <v>117071</v>
+        <v>117073</v>
       </c>
       <c r="K804" t="n">
-        <v>11074234</v>
+        <v>11074232</v>
       </c>
       <c r="L804" t="n">
-        <v>6028326</v>
+        <v>6028324</v>
       </c>
       <c r="M804" t="n">
         <v>19915</v>
@@ -64626,13 +64626,13 @@
         <v>420</v>
       </c>
       <c r="J805" t="n">
-        <v>117132</v>
+        <v>117134</v>
       </c>
       <c r="K805" t="n">
-        <v>11090059</v>
+        <v>11090057</v>
       </c>
       <c r="L805" t="n">
-        <v>6037581</v>
+        <v>6037579</v>
       </c>
       <c r="M805" t="n">
         <v>19936</v>
@@ -64706,13 +64706,13 @@
         <v>487</v>
       </c>
       <c r="J806" t="n">
-        <v>116862</v>
+        <v>116864</v>
       </c>
       <c r="K806" t="n">
-        <v>11111373</v>
+        <v>11111371</v>
       </c>
       <c r="L806" t="n">
-        <v>6045645</v>
+        <v>6045643</v>
       </c>
       <c r="M806" t="n">
         <v>19953</v>
@@ -64786,13 +64786,13 @@
         <v>378</v>
       </c>
       <c r="J807" t="n">
-        <v>117397</v>
+        <v>117399</v>
       </c>
       <c r="K807" t="n">
-        <v>11125362</v>
+        <v>11125360</v>
       </c>
       <c r="L807" t="n">
-        <v>6052920</v>
+        <v>6052918</v>
       </c>
       <c r="M807" t="n">
         <v>19966</v>
@@ -64866,13 +64866,13 @@
         <v>359</v>
       </c>
       <c r="J808" t="n">
-        <v>117446</v>
+        <v>117448</v>
       </c>
       <c r="K808" t="n">
-        <v>9518974</v>
+        <v>9518972</v>
       </c>
       <c r="L808" t="n">
-        <v>6060796</v>
+        <v>6060794</v>
       </c>
       <c r="M808" t="n">
         <v>19988</v>
@@ -64946,13 +64946,13 @@
         <v>348</v>
       </c>
       <c r="J809" t="n">
-        <v>117507</v>
+        <v>117510</v>
       </c>
       <c r="K809" t="n">
-        <v>9539041</v>
+        <v>9539039</v>
       </c>
       <c r="L809" t="n">
-        <v>6068973</v>
+        <v>6068971</v>
       </c>
       <c r="M809" t="n">
         <v>20016</v>
@@ -64982,19 +64982,19 @@
         <v>6919.1</v>
       </c>
       <c r="V809" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W809" t="n">
         <v>0.1</v>
       </c>
       <c r="X809" t="n">
-        <v>215</v>
+        <v>215.3</v>
       </c>
       <c r="Y809" t="n">
-        <v>68.4</v>
+        <v>68.6</v>
       </c>
       <c r="Z809" t="n">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="810">
@@ -65026,13 +65026,13 @@
         <v>244</v>
       </c>
       <c r="J810" t="n">
-        <v>117542</v>
+        <v>117545</v>
       </c>
       <c r="K810" t="n">
-        <v>9546273</v>
+        <v>9546271</v>
       </c>
       <c r="L810" t="n">
-        <v>6073023</v>
+        <v>6073021</v>
       </c>
       <c r="M810" t="n">
         <v>20016</v>
@@ -65068,13 +65068,13 @@
         <v>0</v>
       </c>
       <c r="X810" t="n">
-        <v>48.3</v>
+        <v>48.7</v>
       </c>
       <c r="Y810" t="n">
-        <v>69.3</v>
+        <v>69.4</v>
       </c>
       <c r="Z810" t="n">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="811">
@@ -65106,13 +65106,13 @@
         <v>321</v>
       </c>
       <c r="J811" t="n">
-        <v>117565</v>
+        <v>117568</v>
       </c>
       <c r="K811" t="n">
-        <v>9553554</v>
+        <v>9553552</v>
       </c>
       <c r="L811" t="n">
-        <v>6076460</v>
+        <v>6076458</v>
       </c>
       <c r="M811" t="n">
         <v>20027</v>
@@ -65148,13 +65148,13 @@
         <v>0</v>
       </c>
       <c r="X811" t="n">
-        <v>39.7</v>
+        <v>40</v>
       </c>
       <c r="Y811" t="n">
-        <v>70.6</v>
+        <v>70.7</v>
       </c>
       <c r="Z811" t="n">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="812">
@@ -65186,13 +65186,13 @@
         <v>338</v>
       </c>
       <c r="J812" t="n">
-        <v>117606</v>
+        <v>117609</v>
       </c>
       <c r="K812" t="n">
-        <v>9569017</v>
+        <v>9569015</v>
       </c>
       <c r="L812" t="n">
-        <v>6084461</v>
+        <v>6084459</v>
       </c>
       <c r="M812" t="n">
         <v>20049</v>
@@ -65231,10 +65231,10 @@
         <v>33</v>
       </c>
       <c r="Y812" t="n">
-        <v>67.7</v>
+        <v>67.9</v>
       </c>
       <c r="Z812" t="n">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="813">
@@ -65266,13 +65266,13 @@
         <v>415</v>
       </c>
       <c r="J813" t="n">
-        <v>117176</v>
+        <v>117179</v>
       </c>
       <c r="K813" t="n">
-        <v>9589516</v>
+        <v>9589514</v>
       </c>
       <c r="L813" t="n">
-        <v>6093308</v>
+        <v>6093306</v>
       </c>
       <c r="M813" t="n">
         <v>20062</v>
@@ -65311,10 +65311,10 @@
         <v>-122</v>
       </c>
       <c r="Y813" t="n">
-        <v>44.9</v>
+        <v>45</v>
       </c>
       <c r="Z813" t="n">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="814">
@@ -65346,13 +65346,13 @@
         <v>341</v>
       </c>
       <c r="J814" t="n">
-        <v>117226</v>
+        <v>117229</v>
       </c>
       <c r="K814" t="n">
-        <v>9602707</v>
+        <v>9602705</v>
       </c>
       <c r="L814" t="n">
-        <v>4480542</v>
+        <v>4480540</v>
       </c>
       <c r="M814" t="n">
         <v>20075</v>
@@ -65391,10 +65391,10 @@
         <v>-113</v>
       </c>
       <c r="Y814" t="n">
-        <v>-24.4</v>
+        <v>-24.3</v>
       </c>
       <c r="Z814" t="n">
-        <v>-171</v>
+        <v>-170</v>
       </c>
     </row>
     <row r="815">
@@ -65426,13 +65426,13 @@
         <v>307</v>
       </c>
       <c r="J815" t="n">
-        <v>117406</v>
+        <v>117409</v>
       </c>
       <c r="K815" t="n">
-        <v>9617110</v>
+        <v>9617108</v>
       </c>
       <c r="L815" t="n">
-        <v>4486097</v>
+        <v>4486095</v>
       </c>
       <c r="M815" t="n">
         <v>20094</v>
@@ -65471,10 +65471,10 @@
         <v>-66.7</v>
       </c>
       <c r="Y815" t="n">
-        <v>-5.7</v>
+        <v>-5.6</v>
       </c>
       <c r="Z815" t="n">
-        <v>-40</v>
+        <v>-39</v>
       </c>
     </row>
     <row r="816">
@@ -65506,13 +65506,13 @@
         <v>300</v>
       </c>
       <c r="J816" t="n">
-        <v>117472</v>
+        <v>117475</v>
       </c>
       <c r="K816" t="n">
-        <v>9645737</v>
+        <v>9645735</v>
       </c>
       <c r="L816" t="n">
-        <v>4493970</v>
+        <v>4493968</v>
       </c>
       <c r="M816" t="n">
         <v>0</v>
@@ -65586,13 +65586,13 @@
         <v>205</v>
       </c>
       <c r="J817" t="n">
-        <v>117495</v>
+        <v>117498</v>
       </c>
       <c r="K817" t="n">
-        <v>9652802</v>
+        <v>9652800</v>
       </c>
       <c r="L817" t="n">
-        <v>4497109</v>
+        <v>4497107</v>
       </c>
       <c r="M817" t="n">
         <v>0</v>
@@ -65666,13 +65666,13 @@
         <v>234</v>
       </c>
       <c r="J818" t="n">
-        <v>117512</v>
+        <v>117515</v>
       </c>
       <c r="K818" t="n">
-        <v>9657902</v>
+        <v>9657900</v>
       </c>
       <c r="L818" t="n">
-        <v>4499399</v>
+        <v>4499397</v>
       </c>
       <c r="M818" t="n">
         <v>0</v>
@@ -65746,13 +65746,13 @@
         <v>289</v>
       </c>
       <c r="J819" t="n">
-        <v>117530</v>
+        <v>117533</v>
       </c>
       <c r="K819" t="n">
-        <v>9666254</v>
+        <v>9666252</v>
       </c>
       <c r="L819" t="n">
-        <v>4504107</v>
+        <v>4504105</v>
       </c>
       <c r="M819" t="n">
         <v>0</v>
@@ -65826,13 +65826,13 @@
         <v>240</v>
       </c>
       <c r="J820" t="n">
-        <v>117591</v>
+        <v>117594</v>
       </c>
       <c r="K820" t="n">
-        <v>9687720</v>
+        <v>9687718</v>
       </c>
       <c r="L820" t="n">
-        <v>4507253</v>
+        <v>4507251</v>
       </c>
       <c r="M820" t="n">
         <v>0</v>
@@ -65906,13 +65906,13 @@
         <v>221</v>
       </c>
       <c r="J821" t="n">
-        <v>116000</v>
+        <v>116003</v>
       </c>
       <c r="K821" t="n">
-        <v>9361645</v>
+        <v>9361643</v>
       </c>
       <c r="L821" t="n">
-        <v>4177482</v>
+        <v>4177480</v>
       </c>
       <c r="M821" t="n">
         <v>0</v>
@@ -65986,13 +65986,13 @@
         <v>207</v>
       </c>
       <c r="J822" t="n">
-        <v>92963</v>
+        <v>92966</v>
       </c>
       <c r="K822" t="n">
-        <v>9234275</v>
+        <v>9234273</v>
       </c>
       <c r="L822" t="n">
-        <v>4049851</v>
+        <v>4049849</v>
       </c>
       <c r="M822" t="n">
         <v>0</v>
@@ -66066,13 +66066,13 @@
         <v>204</v>
       </c>
       <c r="J823" t="n">
-        <v>93047</v>
+        <v>93050</v>
       </c>
       <c r="K823" t="n">
-        <v>8766801</v>
+        <v>8766799</v>
       </c>
       <c r="L823" t="n">
-        <v>4052424</v>
+        <v>4052422</v>
       </c>
       <c r="M823" t="n">
         <v>0</v>
@@ -66146,13 +66146,13 @@
         <v>137</v>
       </c>
       <c r="J824" t="n">
-        <v>79736</v>
+        <v>79739</v>
       </c>
       <c r="K824" t="n">
-        <v>7355778</v>
+        <v>7355776</v>
       </c>
       <c r="L824" t="n">
-        <v>4054083</v>
+        <v>4054081</v>
       </c>
       <c r="M824" t="n">
         <v>0</v>
@@ -66226,13 +66226,13 @@
         <v>185</v>
       </c>
       <c r="J825" t="n">
-        <v>79765</v>
+        <v>79768</v>
       </c>
       <c r="K825" t="n">
-        <v>7359499</v>
+        <v>7359497</v>
       </c>
       <c r="L825" t="n">
-        <v>4055280</v>
+        <v>4055278</v>
       </c>
       <c r="M825" t="n">
         <v>0</v>
@@ -66306,13 +66306,13 @@
         <v>214</v>
       </c>
       <c r="J826" t="n">
-        <v>93122</v>
+        <v>93125</v>
       </c>
       <c r="K826" t="n">
-        <v>8778183</v>
+        <v>8778181</v>
       </c>
       <c r="L826" t="n">
-        <v>4058273</v>
+        <v>4058271</v>
       </c>
       <c r="M826" t="n">
         <v>0</v>
@@ -66386,13 +66386,13 @@
         <v>187</v>
       </c>
       <c r="J827" t="n">
-        <v>93198</v>
+        <v>93201</v>
       </c>
       <c r="K827" t="n">
-        <v>8792581</v>
+        <v>8792579</v>
       </c>
       <c r="L827" t="n">
-        <v>4061421</v>
+        <v>4061419</v>
       </c>
       <c r="M827" t="n">
         <v>0</v>
@@ -66466,13 +66466,13 @@
         <v>155</v>
       </c>
       <c r="J828" t="n">
-        <v>79841</v>
+        <v>79844</v>
       </c>
       <c r="K828" t="n">
-        <v>7388019</v>
+        <v>7388017</v>
       </c>
       <c r="L828" t="n">
-        <v>4064240</v>
+        <v>4064238</v>
       </c>
       <c r="M828" t="n">
         <v>0</v>
@@ -66546,13 +66546,13 @@
         <v>188</v>
       </c>
       <c r="J829" t="n">
-        <v>93353</v>
+        <v>93355</v>
       </c>
       <c r="K829" t="n">
-        <v>8811193</v>
+        <v>8811191</v>
       </c>
       <c r="L829" t="n">
-        <v>3582989</v>
+        <v>3582987</v>
       </c>
       <c r="M829" t="n">
         <v>0</v>
@@ -66582,19 +66582,19 @@
         <v>-66694.6</v>
       </c>
       <c r="V829" t="n">
-        <v>13512</v>
+        <v>13511</v>
       </c>
       <c r="W829" t="n">
         <v>16.9</v>
       </c>
       <c r="X829" t="n">
-        <v>77</v>
+        <v>76.7</v>
       </c>
       <c r="Y829" t="n">
-        <v>55.7</v>
+        <v>55.6</v>
       </c>
       <c r="Z829" t="n">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="830">
@@ -66626,13 +66626,13 @@
         <v>195</v>
       </c>
       <c r="J830" t="n">
-        <v>93427</v>
+        <v>93430</v>
       </c>
       <c r="K830" t="n">
-        <v>8827318</v>
+        <v>8827316</v>
       </c>
       <c r="L830" t="n">
-        <v>3587245</v>
+        <v>3587243</v>
       </c>
       <c r="M830" t="n">
         <v>0</v>
@@ -66662,7 +66662,7 @@
         <v>-66454.1</v>
       </c>
       <c r="V830" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="W830" t="n">
         <v>0.1</v>
@@ -66706,13 +66706,13 @@
         <v>124</v>
       </c>
       <c r="J831" t="n">
-        <v>80033</v>
+        <v>80038</v>
       </c>
       <c r="K831" t="n">
-        <v>7407119</v>
+        <v>7407117</v>
       </c>
       <c r="L831" t="n">
-        <v>3589279</v>
+        <v>3589277</v>
       </c>
       <c r="M831" t="n">
         <v>0</v>
@@ -66742,19 +66742,19 @@
         <v>-66400.6</v>
       </c>
       <c r="V831" t="n">
-        <v>-13394</v>
+        <v>-13392</v>
       </c>
       <c r="W831" t="n">
         <v>-14.3</v>
       </c>
       <c r="X831" t="n">
-        <v>64</v>
+        <v>64.7</v>
       </c>
       <c r="Y831" t="n">
-        <v>42.4</v>
+        <v>42.7</v>
       </c>
       <c r="Z831" t="n">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="832">
@@ -66762,13 +66762,13 @@
         <v>44661</v>
       </c>
       <c r="B832" t="n">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="C832" t="n">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="D832" t="n">
-        <v>6122787</v>
+        <v>6122789</v>
       </c>
       <c r="E832" t="n">
         <v>6346</v>
@@ -66777,7 +66777,7 @@
         <v>3082</v>
       </c>
       <c r="G832" t="n">
-        <v>127136</v>
+        <v>127138</v>
       </c>
       <c r="H832" t="n">
         <v>17056</v>
@@ -66786,55 +66786,55 @@
         <v>169</v>
       </c>
       <c r="J832" t="n">
-        <v>80071</v>
+        <v>80078</v>
       </c>
       <c r="K832" t="n">
-        <v>7412772</v>
+        <v>7412771</v>
       </c>
       <c r="L832" t="n">
-        <v>3497134</v>
+        <v>3497131</v>
       </c>
       <c r="M832" t="n">
         <v>0</v>
       </c>
       <c r="N832" t="n">
-        <v>-2245130</v>
+        <v>-2245129</v>
       </c>
       <c r="O832" t="n">
-        <v>53273</v>
+        <v>53274</v>
       </c>
       <c r="P832" t="n">
-        <v>-1002265</v>
+        <v>-1002266</v>
       </c>
       <c r="Q832" t="n">
-        <v>-558146</v>
+        <v>-558147</v>
       </c>
       <c r="R832" t="n">
-        <v>5653</v>
+        <v>5654</v>
       </c>
       <c r="S832" t="n">
-        <v>7610.4</v>
+        <v>7610.6</v>
       </c>
       <c r="T832" t="n">
-        <v>-92145</v>
+        <v>-92146</v>
       </c>
       <c r="U832" t="n">
-        <v>-79735.1</v>
+        <v>-79735.3</v>
       </c>
       <c r="V832" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="W832" t="n">
         <v>0</v>
       </c>
       <c r="X832" t="n">
-        <v>-4427.3</v>
+        <v>-4425.7</v>
       </c>
       <c r="Y832" t="n">
-        <v>43.7</v>
+        <v>44.3</v>
       </c>
       <c r="Z832" t="n">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="833">
@@ -66842,79 +66842,79 @@
         <v>44662</v>
       </c>
       <c r="B833" t="n">
-        <v>2718</v>
+        <v>2734</v>
       </c>
       <c r="C833" t="n">
         <v>662</v>
       </c>
       <c r="D833" t="n">
-        <v>6126664</v>
+        <v>6126680</v>
       </c>
       <c r="E833" t="n">
         <v>6116</v>
       </c>
       <c r="F833" t="n">
-        <v>3214</v>
+        <v>3698</v>
       </c>
       <c r="G833" t="n">
-        <v>127338</v>
+        <v>127354</v>
       </c>
       <c r="H833" t="n">
         <v>17069</v>
       </c>
       <c r="I833" t="n">
-        <v>161</v>
+        <v>198</v>
       </c>
       <c r="J833" t="n">
-        <v>80090</v>
+        <v>93509</v>
       </c>
       <c r="K833" t="n">
-        <v>7418668</v>
+        <v>8841478</v>
       </c>
       <c r="L833" t="n">
-        <v>3500110</v>
+        <v>3500107</v>
       </c>
       <c r="M833" t="n">
         <v>0</v>
       </c>
       <c r="N833" t="n">
-        <v>-2247586</v>
+        <v>-824774</v>
       </c>
       <c r="O833" t="n">
-        <v>-1359515</v>
+        <v>63297</v>
       </c>
       <c r="P833" t="n">
-        <v>-1003997</v>
+        <v>-1003998</v>
       </c>
       <c r="Q833" t="n">
-        <v>-558163</v>
+        <v>-558164</v>
       </c>
       <c r="R833" t="n">
-        <v>5896</v>
+        <v>1428707</v>
       </c>
       <c r="S833" t="n">
-        <v>-194216.4</v>
+        <v>9042.4</v>
       </c>
       <c r="T833" t="n">
         <v>2976</v>
       </c>
       <c r="U833" t="n">
-        <v>-79737.6</v>
+        <v>-79737.7</v>
       </c>
       <c r="V833" t="n">
-        <v>19</v>
+        <v>13431</v>
       </c>
       <c r="W833" t="n">
-        <v>0</v>
+        <v>16.8</v>
       </c>
       <c r="X833" t="n">
-        <v>-4445.7</v>
+        <v>26.3</v>
       </c>
       <c r="Y833" t="n">
-        <v>-1861.7</v>
+        <v>54.9</v>
       </c>
       <c r="Z833" t="n">
-        <v>-13032</v>
+        <v>384</v>
       </c>
     </row>
     <row r="834">
@@ -66922,22 +66922,22 @@
         <v>44663</v>
       </c>
       <c r="B834" t="n">
-        <v>7636</v>
+        <v>7650</v>
       </c>
       <c r="C834" t="n">
         <v>2576</v>
       </c>
       <c r="D834" t="n">
-        <v>6003914</v>
+        <v>6003928</v>
       </c>
       <c r="E834" t="n">
         <v>5969</v>
       </c>
       <c r="F834" t="n">
-        <v>3815</v>
+        <v>3834</v>
       </c>
       <c r="G834" t="n">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="H834" t="n">
         <v>17080</v>
@@ -66946,55 +66946,55 @@
         <v>219</v>
       </c>
       <c r="J834" t="n">
-        <v>93650</v>
+        <v>93662</v>
       </c>
       <c r="K834" t="n">
-        <v>8857305</v>
+        <v>8857334</v>
       </c>
       <c r="L834" t="n">
-        <v>3504955</v>
+        <v>3504952</v>
       </c>
       <c r="M834" t="n">
         <v>0</v>
       </c>
       <c r="N834" t="n">
-        <v>-830415</v>
+        <v>-830384</v>
       </c>
       <c r="O834" t="n">
-        <v>64724</v>
+        <v>64755</v>
       </c>
       <c r="P834" t="n">
-        <v>-1002298</v>
+        <v>-1002299</v>
       </c>
       <c r="Q834" t="n">
-        <v>-556466</v>
+        <v>-556467</v>
       </c>
       <c r="R834" t="n">
-        <v>1438637</v>
+        <v>15856</v>
       </c>
       <c r="S834" t="n">
-        <v>9246.3</v>
+        <v>9250.7</v>
       </c>
       <c r="T834" t="n">
         <v>4845</v>
       </c>
       <c r="U834" t="n">
-        <v>-79495.1</v>
+        <v>-79495.3</v>
       </c>
       <c r="V834" t="n">
-        <v>13560</v>
+        <v>153</v>
       </c>
       <c r="W834" t="n">
-        <v>16.9</v>
+        <v>0.2</v>
       </c>
       <c r="X834" t="n">
-        <v>4539</v>
+        <v>4541.3</v>
       </c>
       <c r="Y834" t="n">
-        <v>64.6</v>
+        <v>65.9</v>
       </c>
       <c r="Z834" t="n">
-        <v>452</v>
+        <v>461</v>
       </c>
     </row>
     <row r="835">
@@ -67002,13 +67002,13 @@
         <v>44664</v>
       </c>
       <c r="B835" t="n">
-        <v>3380</v>
+        <v>3387</v>
       </c>
       <c r="C835" t="n">
         <v>682</v>
       </c>
       <c r="D835" t="n">
-        <v>6007470</v>
+        <v>6007477</v>
       </c>
       <c r="E835" t="n">
         <v>5854</v>
@@ -67017,7 +67017,7 @@
         <v>3281</v>
       </c>
       <c r="G835" t="n">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="H835" t="n">
         <v>17090</v>
@@ -67026,55 +67026,55 @@
         <v>140</v>
       </c>
       <c r="J835" t="n">
-        <v>80228</v>
+        <v>80244</v>
       </c>
       <c r="K835" t="n">
-        <v>7436933</v>
+        <v>7436969</v>
       </c>
       <c r="L835" t="n">
-        <v>3508444</v>
+        <v>3508441</v>
       </c>
       <c r="M835" t="n">
         <v>0</v>
       </c>
       <c r="N835" t="n">
-        <v>-1924712</v>
+        <v>-1924674</v>
       </c>
       <c r="O835" t="n">
-        <v>48914</v>
+        <v>48952</v>
       </c>
       <c r="P835" t="n">
-        <v>-669038</v>
+        <v>-669039</v>
       </c>
       <c r="Q835" t="n">
-        <v>-555796</v>
+        <v>-555797</v>
       </c>
       <c r="R835" t="n">
-        <v>-1420372</v>
+        <v>-1420365</v>
       </c>
       <c r="S835" t="n">
-        <v>6987.7</v>
+        <v>6993.1</v>
       </c>
       <c r="T835" t="n">
         <v>3489</v>
       </c>
       <c r="U835" t="n">
-        <v>-79399.4</v>
+        <v>-79399.6</v>
       </c>
       <c r="V835" t="n">
-        <v>-13422</v>
+        <v>-13418</v>
       </c>
       <c r="W835" t="n">
         <v>-14.3</v>
       </c>
       <c r="X835" t="n">
-        <v>52.3</v>
+        <v>55.3</v>
       </c>
       <c r="Y835" t="n">
-        <v>55.3</v>
+        <v>57.1</v>
       </c>
       <c r="Z835" t="n">
-        <v>387</v>
+        <v>400</v>
       </c>
     </row>
     <row r="836">
@@ -67082,13 +67082,13 @@
         <v>44665</v>
       </c>
       <c r="B836" t="n">
-        <v>2400</v>
+        <v>2427</v>
       </c>
       <c r="C836" t="n">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="D836" t="n">
-        <v>6009444</v>
+        <v>6009468</v>
       </c>
       <c r="E836" t="n">
         <v>5538</v>
@@ -67097,7 +67097,7 @@
         <v>3250</v>
       </c>
       <c r="G836" t="n">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="H836" t="n">
         <v>17094</v>
@@ -67106,10 +67106,10 @@
         <v>103</v>
       </c>
       <c r="J836" t="n">
-        <v>80231</v>
+        <v>80254</v>
       </c>
       <c r="K836" t="n">
-        <v>7440666</v>
+        <v>7440729</v>
       </c>
       <c r="L836" t="n">
         <v>3511601</v>
@@ -67118,43 +67118,43 @@
         <v>0</v>
       </c>
       <c r="N836" t="n">
-        <v>-1793609</v>
+        <v>-1793544</v>
       </c>
       <c r="O836" t="n">
-        <v>-1370527</v>
+        <v>-1370462</v>
       </c>
       <c r="P836" t="n">
-        <v>-538250</v>
+        <v>-538248</v>
       </c>
       <c r="Q836" t="n">
-        <v>-71388</v>
+        <v>-71386</v>
       </c>
       <c r="R836" t="n">
-        <v>3733</v>
+        <v>3760</v>
       </c>
       <c r="S836" t="n">
-        <v>-195789.6</v>
+        <v>-195780.3</v>
       </c>
       <c r="T836" t="n">
-        <v>3157</v>
+        <v>3160</v>
       </c>
       <c r="U836" t="n">
-        <v>-10198.3</v>
+        <v>-10198</v>
       </c>
       <c r="V836" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="W836" t="n">
         <v>0</v>
       </c>
       <c r="X836" t="n">
-        <v>47</v>
+        <v>-4418.3</v>
       </c>
       <c r="Y836" t="n">
-        <v>-1874.6</v>
+        <v>-1871.6</v>
       </c>
       <c r="Z836" t="n">
-        <v>-13122</v>
+        <v>-13101</v>
       </c>
     </row>
     <row r="837">
@@ -67162,13 +67162,13 @@
         <v>44666</v>
       </c>
       <c r="B837" t="n">
-        <v>1727</v>
+        <v>1730</v>
       </c>
       <c r="C837" t="n">
         <v>231</v>
       </c>
       <c r="D837" t="n">
-        <v>6011289</v>
+        <v>6011292</v>
       </c>
       <c r="E837" t="n">
         <v>5273</v>
@@ -67177,7 +67177,7 @@
         <v>3330</v>
       </c>
       <c r="G837" t="n">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="H837" t="n">
         <v>17108</v>
@@ -67186,10 +67186,10 @@
         <v>105</v>
       </c>
       <c r="J837" t="n">
-        <v>80238</v>
+        <v>80270</v>
       </c>
       <c r="K837" t="n">
-        <v>7442968</v>
+        <v>7443034</v>
       </c>
       <c r="L837" t="n">
         <v>3513233</v>
@@ -67198,43 +67198,43 @@
         <v>0</v>
       </c>
       <c r="N837" t="n">
-        <v>-1323833</v>
+        <v>-1323765</v>
       </c>
       <c r="O837" t="n">
-        <v>-1384350</v>
+        <v>-1384282</v>
       </c>
       <c r="P837" t="n">
-        <v>-539191</v>
+        <v>-539189</v>
       </c>
       <c r="Q837" t="n">
-        <v>-74012</v>
+        <v>-74010</v>
       </c>
       <c r="R837" t="n">
-        <v>2302</v>
+        <v>2305</v>
       </c>
       <c r="S837" t="n">
-        <v>-197764.3</v>
+        <v>-197754.6</v>
       </c>
       <c r="T837" t="n">
         <v>1632</v>
       </c>
       <c r="U837" t="n">
-        <v>-10573.1</v>
+        <v>-10572.9</v>
       </c>
       <c r="V837" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="W837" t="n">
         <v>0</v>
       </c>
       <c r="X837" t="n">
-        <v>-4470.7</v>
+        <v>-4464</v>
       </c>
       <c r="Y837" t="n">
-        <v>-1884.1</v>
+        <v>-1880</v>
       </c>
       <c r="Z837" t="n">
-        <v>-13189</v>
+        <v>-13160</v>
       </c>
     </row>
     <row r="838">
@@ -67242,13 +67242,13 @@
         <v>44667</v>
       </c>
       <c r="B838" t="n">
-        <v>1660</v>
+        <v>1675</v>
       </c>
       <c r="C838" t="n">
         <v>317</v>
       </c>
       <c r="D838" t="n">
-        <v>6140168</v>
+        <v>6140183</v>
       </c>
       <c r="E838" t="n">
         <v>5163</v>
@@ -67257,7 +67257,7 @@
         <v>3451</v>
       </c>
       <c r="G838" t="n">
-        <v>127315</v>
+        <v>127330</v>
       </c>
       <c r="H838" t="n">
         <v>17111</v>
@@ -67266,10 +67266,10 @@
         <v>120</v>
       </c>
       <c r="J838" t="n">
-        <v>80252</v>
+        <v>80288</v>
       </c>
       <c r="K838" t="n">
-        <v>7450200</v>
+        <v>7450281</v>
       </c>
       <c r="L838" t="n">
         <v>3515086</v>
@@ -67278,43 +67278,43 @@
         <v>0</v>
       </c>
       <c r="N838" t="n">
-        <v>94422</v>
+        <v>94505</v>
       </c>
       <c r="O838" t="n">
-        <v>43081</v>
+        <v>43164</v>
       </c>
       <c r="P838" t="n">
-        <v>-538997</v>
+        <v>-538995</v>
       </c>
       <c r="Q838" t="n">
-        <v>-74193</v>
+        <v>-74191</v>
       </c>
       <c r="R838" t="n">
-        <v>7232</v>
+        <v>7247</v>
       </c>
       <c r="S838" t="n">
-        <v>6154.4</v>
+        <v>6166.3</v>
       </c>
       <c r="T838" t="n">
         <v>1853</v>
       </c>
       <c r="U838" t="n">
-        <v>-10599</v>
+        <v>-10598.7</v>
       </c>
       <c r="V838" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="W838" t="n">
         <v>0</v>
       </c>
       <c r="X838" t="n">
-        <v>8</v>
+        <v>14.7</v>
       </c>
       <c r="Y838" t="n">
-        <v>31.3</v>
+        <v>35.7</v>
       </c>
       <c r="Z838" t="n">
-        <v>219</v>
+        <v>250</v>
       </c>
     </row>
     <row r="839">
@@ -67322,13 +67322,13 @@
         <v>44668</v>
       </c>
       <c r="B839" t="n">
-        <v>2013</v>
+        <v>2023</v>
       </c>
       <c r="C839" t="n">
-        <v>2507</v>
+        <v>2508</v>
       </c>
       <c r="D839" t="n">
-        <v>6142026</v>
+        <v>6142035</v>
       </c>
       <c r="E839" t="n">
         <v>5075</v>
@@ -67337,7 +67337,7 @@
         <v>3682</v>
       </c>
       <c r="G839" t="n">
-        <v>127341</v>
+        <v>127350</v>
       </c>
       <c r="H839" t="n">
         <v>17122</v>
@@ -67346,55 +67346,55 @@
         <v>168</v>
       </c>
       <c r="J839" t="n">
-        <v>80279</v>
+        <v>80321</v>
       </c>
       <c r="K839" t="n">
-        <v>7458638</v>
+        <v>7458729</v>
       </c>
       <c r="L839" t="n">
-        <v>3517117</v>
+        <v>3517118</v>
       </c>
       <c r="M839" t="n">
         <v>0</v>
       </c>
       <c r="N839" t="n">
-        <v>99139</v>
+        <v>99232</v>
       </c>
       <c r="O839" t="n">
-        <v>45866</v>
+        <v>45958</v>
       </c>
       <c r="P839" t="n">
-        <v>-538163</v>
+        <v>-538160</v>
       </c>
       <c r="Q839" t="n">
-        <v>19983</v>
+        <v>19987</v>
       </c>
       <c r="R839" t="n">
-        <v>8438</v>
+        <v>8448</v>
       </c>
       <c r="S839" t="n">
-        <v>6552.3</v>
+        <v>6565.4</v>
       </c>
       <c r="T839" t="n">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="U839" t="n">
-        <v>2854.7</v>
+        <v>2855.3</v>
       </c>
       <c r="V839" t="n">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="W839" t="n">
         <v>0</v>
       </c>
       <c r="X839" t="n">
-        <v>16</v>
+        <v>22.3</v>
       </c>
       <c r="Y839" t="n">
-        <v>29.7</v>
+        <v>34.7</v>
       </c>
       <c r="Z839" t="n">
-        <v>208</v>
+        <v>243</v>
       </c>
     </row>
     <row r="840">
@@ -67402,79 +67402,79 @@
         <v>44669</v>
       </c>
       <c r="B840" t="n">
-        <v>2099</v>
+        <v>2755</v>
       </c>
       <c r="C840" t="n">
-        <v>195</v>
+        <v>497</v>
       </c>
       <c r="D840" t="n">
-        <v>6017115</v>
+        <v>6017469</v>
       </c>
       <c r="E840" t="n">
         <v>5305</v>
       </c>
       <c r="F840" t="n">
-        <v>3464</v>
+        <v>3802</v>
       </c>
       <c r="G840" t="n">
-        <v>36</v>
+        <v>390</v>
       </c>
       <c r="H840" t="n">
         <v>17132</v>
       </c>
       <c r="I840" t="n">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="J840" t="n">
-        <v>77639</v>
+        <v>80344</v>
       </c>
       <c r="K840" t="n">
-        <v>7249775</v>
+        <v>7464102</v>
       </c>
       <c r="L840" t="n">
-        <v>3344722</v>
+        <v>3519931</v>
       </c>
       <c r="M840" t="n">
         <v>0</v>
       </c>
       <c r="N840" t="n">
-        <v>-1528408</v>
+        <v>-1314079</v>
       </c>
       <c r="O840" t="n">
-        <v>-168893</v>
+        <v>-1377376</v>
       </c>
       <c r="P840" t="n">
-        <v>-713551</v>
+        <v>-538340</v>
       </c>
       <c r="Q840" t="n">
-        <v>-155388</v>
+        <v>19824</v>
       </c>
       <c r="R840" t="n">
-        <v>-208863</v>
+        <v>5373</v>
       </c>
       <c r="S840" t="n">
-        <v>-24127.6</v>
+        <v>-196768</v>
       </c>
       <c r="T840" t="n">
-        <v>-172395</v>
+        <v>2813</v>
       </c>
       <c r="U840" t="n">
-        <v>-22198.3</v>
+        <v>2832</v>
       </c>
       <c r="V840" t="n">
-        <v>-2640</v>
+        <v>23</v>
       </c>
       <c r="W840" t="n">
-        <v>-3.3</v>
+        <v>0</v>
       </c>
       <c r="X840" t="n">
-        <v>-866.3</v>
+        <v>24.7</v>
       </c>
       <c r="Y840" t="n">
-        <v>-350.1</v>
+        <v>-1880.7</v>
       </c>
       <c r="Z840" t="n">
-        <v>-2451</v>
+        <v>-13165</v>
       </c>
     </row>
     <row r="841">
@@ -67482,79 +67482,79 @@
         <v>44670</v>
       </c>
       <c r="B841" t="n">
-        <v>9140</v>
+        <v>9905</v>
       </c>
       <c r="C841" t="n">
-        <v>3525</v>
+        <v>3950</v>
       </c>
       <c r="D841" t="n">
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="E841" t="n">
         <v>0</v>
       </c>
       <c r="F841" t="n">
-        <v>3597</v>
+        <v>4137</v>
       </c>
       <c r="G841" t="n">
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="H841" t="n">
         <v>0</v>
       </c>
       <c r="I841" t="n">
-        <v>95</v>
+        <v>177</v>
       </c>
       <c r="J841" t="n">
-        <v>82365</v>
+        <v>87302</v>
       </c>
       <c r="K841" t="n">
-        <v>7605661</v>
+        <v>8219622</v>
       </c>
       <c r="L841" t="n">
-        <v>3350850</v>
+        <v>3526484</v>
       </c>
       <c r="M841" t="n">
         <v>0</v>
       </c>
       <c r="N841" t="n">
-        <v>-1186920</v>
+        <v>-572957</v>
       </c>
       <c r="O841" t="n">
-        <v>-1251644</v>
+        <v>-637712</v>
       </c>
       <c r="P841" t="n">
-        <v>-710571</v>
+        <v>-534935</v>
       </c>
       <c r="Q841" t="n">
-        <v>-154105</v>
+        <v>21532</v>
       </c>
       <c r="R841" t="n">
-        <v>355886</v>
+        <v>755520</v>
       </c>
       <c r="S841" t="n">
-        <v>-178806.3</v>
+        <v>-91101.7</v>
       </c>
       <c r="T841" t="n">
-        <v>6128</v>
+        <v>6553</v>
       </c>
       <c r="U841" t="n">
-        <v>-22015</v>
+        <v>3076</v>
       </c>
       <c r="V841" t="n">
-        <v>4726</v>
+        <v>6958</v>
       </c>
       <c r="W841" t="n">
-        <v>6.1</v>
+        <v>8.7</v>
       </c>
       <c r="X841" t="n">
-        <v>704.3</v>
+        <v>2338</v>
       </c>
       <c r="Y841" t="n">
-        <v>-1612.1</v>
+        <v>-908.6</v>
       </c>
       <c r="Z841" t="n">
-        <v>-11285</v>
+        <v>-6360</v>
       </c>
     </row>
     <row r="842">
@@ -67562,79 +67562,79 @@
         <v>44671</v>
       </c>
       <c r="B842" t="n">
-        <v>0</v>
+        <v>2089</v>
       </c>
       <c r="C842" t="n">
-        <v>330</v>
+        <v>696</v>
       </c>
       <c r="D842" t="n">
-        <v>0</v>
+        <v>127525</v>
       </c>
       <c r="E842" t="n">
         <v>0</v>
       </c>
       <c r="F842" t="n">
-        <v>1651</v>
+        <v>2939</v>
       </c>
       <c r="G842" t="n">
-        <v>0</v>
+        <v>127525</v>
       </c>
       <c r="H842" t="n">
         <v>0</v>
       </c>
       <c r="I842" t="n">
-        <v>27</v>
+        <v>134</v>
       </c>
       <c r="J842" t="n">
-        <v>34671</v>
+        <v>62399</v>
       </c>
       <c r="K842" t="n">
-        <v>3437967</v>
+        <v>5043112</v>
       </c>
       <c r="L842" t="n">
-        <v>2385604</v>
+        <v>3529793</v>
       </c>
       <c r="M842" t="n">
         <v>0</v>
       </c>
       <c r="N842" t="n">
-        <v>-3950052</v>
+        <v>-2344905</v>
       </c>
       <c r="O842" t="n">
-        <v>-3998966</v>
+        <v>-2393857</v>
       </c>
       <c r="P842" t="n">
-        <v>-1678636</v>
+        <v>-534445</v>
       </c>
       <c r="Q842" t="n">
-        <v>-1122840</v>
+        <v>21352</v>
       </c>
       <c r="R842" t="n">
-        <v>-4167694</v>
+        <v>-3176510</v>
       </c>
       <c r="S842" t="n">
-        <v>-571280.9</v>
+        <v>-341979.6</v>
       </c>
       <c r="T842" t="n">
-        <v>-965246</v>
+        <v>3309</v>
       </c>
       <c r="U842" t="n">
-        <v>-160405.7</v>
+        <v>3050.3</v>
       </c>
       <c r="V842" t="n">
-        <v>-47694</v>
+        <v>-24903</v>
       </c>
       <c r="W842" t="n">
-        <v>-57.9</v>
+        <v>-28.5</v>
       </c>
       <c r="X842" t="n">
-        <v>-15202.7</v>
+        <v>-5974</v>
       </c>
       <c r="Y842" t="n">
-        <v>-6508.1</v>
+        <v>-2549.3</v>
       </c>
       <c r="Z842" t="n">
-        <v>-45557</v>
+        <v>-17845</v>
       </c>
     </row>
     <row r="843">
@@ -67642,79 +67642,79 @@
         <v>44672</v>
       </c>
       <c r="B843" t="n">
-        <v>0</v>
+        <v>2176</v>
       </c>
       <c r="C843" t="n">
         <v>60</v>
       </c>
       <c r="D843" t="n">
-        <v>0</v>
+        <v>127301</v>
       </c>
       <c r="E843" t="n">
         <v>0</v>
       </c>
       <c r="F843" t="n">
-        <v>1021</v>
+        <v>3109</v>
       </c>
       <c r="G843" t="n">
-        <v>0</v>
+        <v>127301</v>
       </c>
       <c r="H843" t="n">
         <v>0</v>
       </c>
       <c r="I843" t="n">
-        <v>11</v>
+        <v>168</v>
       </c>
       <c r="J843" t="n">
-        <v>31357</v>
+        <v>73378</v>
       </c>
       <c r="K843" t="n">
-        <v>2867392</v>
+        <v>6266753</v>
       </c>
       <c r="L843" t="n">
-        <v>2386562</v>
+        <v>3356135</v>
       </c>
       <c r="M843" t="n">
         <v>0</v>
       </c>
       <c r="N843" t="n">
-        <v>-5943801</v>
+        <v>-2544438</v>
       </c>
       <c r="O843" t="n">
-        <v>-4573274</v>
+        <v>-1173976</v>
       </c>
       <c r="P843" t="n">
-        <v>-1196427</v>
+        <v>-226852</v>
       </c>
       <c r="Q843" t="n">
-        <v>-1125039</v>
+        <v>-155466</v>
       </c>
       <c r="R843" t="n">
-        <v>-570575</v>
+        <v>1223641</v>
       </c>
       <c r="S843" t="n">
-        <v>-653324.9</v>
+        <v>-167710.9</v>
       </c>
       <c r="T843" t="n">
-        <v>958</v>
+        <v>-173658</v>
       </c>
       <c r="U843" t="n">
-        <v>-160719.9</v>
+        <v>-22209.4</v>
       </c>
       <c r="V843" t="n">
-        <v>-3314</v>
+        <v>10979</v>
       </c>
       <c r="W843" t="n">
-        <v>-9.6</v>
+        <v>17.6</v>
       </c>
       <c r="X843" t="n">
-        <v>-15427.3</v>
+        <v>-2322</v>
       </c>
       <c r="Y843" t="n">
-        <v>-6982</v>
+        <v>-982.3</v>
       </c>
       <c r="Z843" t="n">
-        <v>-48874</v>
+        <v>-6876</v>
       </c>
     </row>
     <row r="844">
@@ -67722,10 +67722,10 @@
         <v>44673</v>
       </c>
       <c r="B844" t="n">
-        <v>0</v>
+        <v>5785</v>
       </c>
       <c r="C844" t="n">
-        <v>0</v>
+        <v>1441</v>
       </c>
       <c r="D844" t="n">
         <v>0</v>
@@ -67734,7 +67734,7 @@
         <v>0</v>
       </c>
       <c r="F844" t="n">
-        <v>135</v>
+        <v>2069</v>
       </c>
       <c r="G844" t="n">
         <v>0</v>
@@ -67743,58 +67743,58 @@
         <v>0</v>
       </c>
       <c r="I844" t="n">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="J844" t="n">
-        <v>4508</v>
+        <v>50220</v>
       </c>
       <c r="K844" t="n">
-        <v>412145</v>
+        <v>4229366</v>
       </c>
       <c r="L844" t="n">
-        <v>0</v>
+        <v>972970</v>
       </c>
       <c r="M844" t="n">
         <v>0</v>
       </c>
       <c r="N844" t="n">
-        <v>-8415173</v>
+        <v>-4597950</v>
       </c>
       <c r="O844" t="n">
-        <v>-7030823</v>
+        <v>-3213668</v>
       </c>
       <c r="P844" t="n">
-        <v>-3587245</v>
+        <v>-2614273</v>
       </c>
       <c r="Q844" t="n">
-        <v>-3513233</v>
+        <v>-2540263</v>
       </c>
       <c r="R844" t="n">
-        <v>-2455247</v>
+        <v>-2037387</v>
       </c>
       <c r="S844" t="n">
-        <v>-1004403.3</v>
+        <v>-459095.4</v>
       </c>
       <c r="T844" t="n">
-        <v>-2386562</v>
+        <v>-2383165</v>
       </c>
       <c r="U844" t="n">
-        <v>-501890.4</v>
+        <v>-362894.7</v>
       </c>
       <c r="V844" t="n">
-        <v>-26849</v>
+        <v>-23158</v>
       </c>
       <c r="W844" t="n">
-        <v>-85.6</v>
+        <v>-31.6</v>
       </c>
       <c r="X844" t="n">
-        <v>-25952.3</v>
+        <v>-12360.7</v>
       </c>
       <c r="Y844" t="n">
-        <v>-10818.6</v>
+        <v>-4292.9</v>
       </c>
       <c r="Z844" t="n">
-        <v>-75730</v>
+        <v>-30050</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualiza datos provincias 2022-05-03
</commit_message>
<xml_diff>
--- a/data/output/covid19-spain_consolidated.xlsx
+++ b/data/output/covid19-spain_consolidated.xlsx
@@ -66054,7 +66054,7 @@
         <v>8107</v>
       </c>
       <c r="F823" t="n">
-        <v>3992</v>
+        <v>3994</v>
       </c>
       <c r="G823" t="n">
         <v>121</v>
@@ -66066,7 +66066,7 @@
         <v>193</v>
       </c>
       <c r="J823" t="n">
-        <v>141640</v>
+        <v>141660</v>
       </c>
       <c r="K823" t="n">
         <v>8768621</v>
@@ -66102,19 +66102,19 @@
         <v>-63068.7</v>
       </c>
       <c r="V823" t="n">
-        <v>48697</v>
+        <v>48717</v>
       </c>
       <c r="W823" t="n">
         <v>52.4</v>
       </c>
       <c r="X823" t="n">
-        <v>8023</v>
+        <v>8029.7</v>
       </c>
       <c r="Y823" t="n">
-        <v>3455.4</v>
+        <v>3458.3</v>
       </c>
       <c r="Z823" t="n">
-        <v>24188</v>
+        <v>24208</v>
       </c>
     </row>
     <row r="824">
@@ -66134,7 +66134,7 @@
         <v>7946</v>
       </c>
       <c r="F824" t="n">
-        <v>2477</v>
+        <v>2969</v>
       </c>
       <c r="G824" t="n">
         <v>126811</v>
@@ -66146,7 +66146,7 @@
         <v>137</v>
       </c>
       <c r="J824" t="n">
-        <v>128329</v>
+        <v>100563</v>
       </c>
       <c r="K824" t="n">
         <v>7357607</v>
@@ -66182,19 +66182,19 @@
         <v>-63280.1</v>
       </c>
       <c r="V824" t="n">
-        <v>-13311</v>
+        <v>-41097</v>
       </c>
       <c r="W824" t="n">
-        <v>-9.4</v>
+        <v>-29</v>
       </c>
       <c r="X824" t="n">
-        <v>4116.3</v>
+        <v>-5139</v>
       </c>
       <c r="Y824" t="n">
-        <v>1550.6</v>
+        <v>-2416</v>
       </c>
       <c r="Z824" t="n">
-        <v>10854</v>
+        <v>-16912</v>
       </c>
     </row>
     <row r="825">
@@ -66226,7 +66226,7 @@
         <v>185</v>
       </c>
       <c r="J825" t="n">
-        <v>128358</v>
+        <v>100592</v>
       </c>
       <c r="K825" t="n">
         <v>7361336</v>
@@ -66268,13 +66268,13 @@
         <v>0</v>
       </c>
       <c r="X825" t="n">
-        <v>11805</v>
+        <v>2549.7</v>
       </c>
       <c r="Y825" t="n">
-        <v>1552.3</v>
+        <v>-2414.3</v>
       </c>
       <c r="Z825" t="n">
-        <v>10866</v>
+        <v>-16900</v>
       </c>
     </row>
     <row r="826">
@@ -66306,7 +66306,7 @@
         <v>214</v>
       </c>
       <c r="J826" t="n">
-        <v>141715</v>
+        <v>113949</v>
       </c>
       <c r="K826" t="n">
         <v>8780037</v>
@@ -66345,16 +66345,16 @@
         <v>13357</v>
       </c>
       <c r="W826" t="n">
-        <v>10.4</v>
+        <v>13.3</v>
       </c>
       <c r="X826" t="n">
-        <v>25</v>
+        <v>-9237</v>
       </c>
       <c r="Y826" t="n">
-        <v>3457.9</v>
+        <v>-508.7</v>
       </c>
       <c r="Z826" t="n">
-        <v>24205</v>
+        <v>-3561</v>
       </c>
     </row>
     <row r="827">
@@ -66386,7 +66386,7 @@
         <v>187</v>
       </c>
       <c r="J827" t="n">
-        <v>141791</v>
+        <v>114025</v>
       </c>
       <c r="K827" t="n">
         <v>8794444</v>
@@ -66431,10 +66431,10 @@
         <v>4487.3</v>
       </c>
       <c r="Y827" t="n">
-        <v>3460</v>
+        <v>-506.6</v>
       </c>
       <c r="Z827" t="n">
-        <v>24220</v>
+        <v>-3546</v>
       </c>
     </row>
     <row r="828">
@@ -66466,7 +66466,7 @@
         <v>155</v>
       </c>
       <c r="J828" t="n">
-        <v>128435</v>
+        <v>100669</v>
       </c>
       <c r="K828" t="n">
         <v>7389908</v>
@@ -66505,16 +66505,16 @@
         <v>-13356</v>
       </c>
       <c r="W828" t="n">
-        <v>-9.4</v>
+        <v>-11.7</v>
       </c>
       <c r="X828" t="n">
         <v>25.7</v>
       </c>
       <c r="Y828" t="n">
-        <v>1779.3</v>
+        <v>-2187.3</v>
       </c>
       <c r="Z828" t="n">
-        <v>12455</v>
+        <v>-15311</v>
       </c>
     </row>
     <row r="829">
@@ -66546,7 +66546,7 @@
         <v>188</v>
       </c>
       <c r="J829" t="n">
-        <v>141946</v>
+        <v>114180</v>
       </c>
       <c r="K829" t="n">
         <v>8813117</v>
@@ -66585,16 +66585,16 @@
         <v>13511</v>
       </c>
       <c r="W829" t="n">
-        <v>10.5</v>
+        <v>13.4</v>
       </c>
       <c r="X829" t="n">
         <v>77</v>
       </c>
       <c r="Y829" t="n">
-        <v>7000.4</v>
+        <v>3033.9</v>
       </c>
       <c r="Z829" t="n">
-        <v>49003</v>
+        <v>21237</v>
       </c>
     </row>
     <row r="830">
@@ -66626,7 +66626,7 @@
         <v>196</v>
       </c>
       <c r="J830" t="n">
-        <v>142021</v>
+        <v>114255</v>
       </c>
       <c r="K830" t="n">
         <v>8829272</v>
@@ -66671,10 +66671,10 @@
         <v>76.7</v>
       </c>
       <c r="Y830" t="n">
-        <v>54.4</v>
+        <v>-3915</v>
       </c>
       <c r="Z830" t="n">
-        <v>381</v>
+        <v>-27405</v>
       </c>
     </row>
     <row r="831">
@@ -66706,7 +66706,7 @@
         <v>125</v>
       </c>
       <c r="J831" t="n">
-        <v>128630</v>
+        <v>100864</v>
       </c>
       <c r="K831" t="n">
         <v>7409099</v>
@@ -66745,7 +66745,7 @@
         <v>-13391</v>
       </c>
       <c r="W831" t="n">
-        <v>-9.4</v>
+        <v>-11.7</v>
       </c>
       <c r="X831" t="n">
         <v>65</v>
@@ -66786,7 +66786,7 @@
         <v>170</v>
       </c>
       <c r="J832" t="n">
-        <v>128671</v>
+        <v>100905</v>
       </c>
       <c r="K832" t="n">
         <v>7414788</v>
@@ -66866,7 +66866,7 @@
         <v>198</v>
       </c>
       <c r="J833" t="n">
-        <v>142102</v>
+        <v>114336</v>
       </c>
       <c r="K833" t="n">
         <v>8843551</v>
@@ -66905,7 +66905,7 @@
         <v>13431</v>
       </c>
       <c r="W833" t="n">
-        <v>10.4</v>
+        <v>13.3</v>
       </c>
       <c r="X833" t="n">
         <v>27</v>
@@ -66946,7 +66946,7 @@
         <v>219</v>
       </c>
       <c r="J834" t="n">
-        <v>142260</v>
+        <v>114495</v>
       </c>
       <c r="K834" t="n">
         <v>8859485</v>
@@ -66982,19 +66982,19 @@
         <v>-79457.7</v>
       </c>
       <c r="V834" t="n">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="W834" t="n">
         <v>0.1</v>
       </c>
       <c r="X834" t="n">
-        <v>4543.3</v>
+        <v>4543.7</v>
       </c>
       <c r="Y834" t="n">
-        <v>67</v>
+        <v>67.1</v>
       </c>
       <c r="Z834" t="n">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="835">
@@ -67026,7 +67026,7 @@
         <v>140</v>
       </c>
       <c r="J835" t="n">
-        <v>128844</v>
+        <v>101079</v>
       </c>
       <c r="K835" t="n">
         <v>7439161</v>
@@ -67065,16 +67065,16 @@
         <v>-13416</v>
       </c>
       <c r="W835" t="n">
-        <v>-9.4</v>
+        <v>-11.7</v>
       </c>
       <c r="X835" t="n">
-        <v>57.7</v>
+        <v>58</v>
       </c>
       <c r="Y835" t="n">
-        <v>58.4</v>
+        <v>58.6</v>
       </c>
       <c r="Z835" t="n">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="836">
@@ -67106,7 +67106,7 @@
         <v>103</v>
       </c>
       <c r="J836" t="n">
-        <v>128860</v>
+        <v>101095</v>
       </c>
       <c r="K836" t="n">
         <v>7442974</v>
@@ -67148,13 +67148,13 @@
         <v>0</v>
       </c>
       <c r="X836" t="n">
-        <v>-4414</v>
+        <v>-4413.7</v>
       </c>
       <c r="Y836" t="n">
-        <v>-1869.4</v>
+        <v>-1869.3</v>
       </c>
       <c r="Z836" t="n">
-        <v>-13086</v>
+        <v>-13085</v>
       </c>
     </row>
     <row r="837">
@@ -67186,7 +67186,7 @@
         <v>105</v>
       </c>
       <c r="J837" t="n">
-        <v>128885</v>
+        <v>101121</v>
       </c>
       <c r="K837" t="n">
         <v>7445349</v>
@@ -67222,19 +67222,19 @@
         <v>-10524.1</v>
       </c>
       <c r="V837" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="W837" t="n">
         <v>0</v>
       </c>
       <c r="X837" t="n">
-        <v>-4458.3</v>
+        <v>-4458</v>
       </c>
       <c r="Y837" t="n">
-        <v>-1876.6</v>
+        <v>-1876.3</v>
       </c>
       <c r="Z837" t="n">
-        <v>-13136</v>
+        <v>-13134</v>
       </c>
     </row>
     <row r="838">
@@ -67266,7 +67266,7 @@
         <v>120</v>
       </c>
       <c r="J838" t="n">
-        <v>128911</v>
+        <v>101148</v>
       </c>
       <c r="K838" t="n">
         <v>7452665</v>
@@ -67302,19 +67302,19 @@
         <v>-10544.3</v>
       </c>
       <c r="V838" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="W838" t="n">
         <v>0</v>
       </c>
       <c r="X838" t="n">
-        <v>22.3</v>
+        <v>23</v>
       </c>
       <c r="Y838" t="n">
-        <v>40.1</v>
+        <v>40.6</v>
       </c>
       <c r="Z838" t="n">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="839">
@@ -67346,7 +67346,7 @@
         <v>168</v>
       </c>
       <c r="J839" t="n">
-        <v>128953</v>
+        <v>101192</v>
       </c>
       <c r="K839" t="n">
         <v>7461179</v>
@@ -67382,19 +67382,19 @@
         <v>2913.9</v>
       </c>
       <c r="V839" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="W839" t="n">
         <v>0</v>
       </c>
       <c r="X839" t="n">
-        <v>31</v>
+        <v>32.3</v>
       </c>
       <c r="Y839" t="n">
-        <v>40.3</v>
+        <v>41</v>
       </c>
       <c r="Z839" t="n">
-        <v>282</v>
+        <v>287</v>
       </c>
     </row>
     <row r="840">
@@ -67426,7 +67426,7 @@
         <v>151</v>
       </c>
       <c r="J840" t="n">
-        <v>128979</v>
+        <v>101217</v>
       </c>
       <c r="K840" t="n">
         <v>7466686</v>
@@ -67462,19 +67462,19 @@
         <v>2898.1</v>
       </c>
       <c r="V840" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="W840" t="n">
         <v>0</v>
       </c>
       <c r="X840" t="n">
-        <v>31.3</v>
+        <v>32</v>
       </c>
       <c r="Y840" t="n">
-        <v>-1874.7</v>
+        <v>-1874.1</v>
       </c>
       <c r="Z840" t="n">
-        <v>-13123</v>
+        <v>-13119</v>
       </c>
     </row>
     <row r="841">
@@ -67506,7 +67506,7 @@
         <v>186</v>
       </c>
       <c r="J841" t="n">
-        <v>142517</v>
+        <v>114755</v>
       </c>
       <c r="K841" t="n">
         <v>8919141</v>
@@ -67545,16 +67545,16 @@
         <v>13538</v>
       </c>
       <c r="W841" t="n">
-        <v>10.5</v>
+        <v>13.4</v>
       </c>
       <c r="X841" t="n">
-        <v>4535.3</v>
+        <v>4535.7</v>
       </c>
       <c r="Y841" t="n">
-        <v>36.7</v>
+        <v>37.1</v>
       </c>
       <c r="Z841" t="n">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="842">
@@ -67586,7 +67586,7 @@
         <v>161</v>
       </c>
       <c r="J842" t="n">
-        <v>119835</v>
+        <v>92073</v>
       </c>
       <c r="K842" t="n">
         <v>6119156</v>
@@ -67625,16 +67625,16 @@
         <v>-22682</v>
       </c>
       <c r="W842" t="n">
-        <v>-15.9</v>
+        <v>-19.8</v>
       </c>
       <c r="X842" t="n">
-        <v>-3039.3</v>
+        <v>-3039.7</v>
       </c>
       <c r="Y842" t="n">
-        <v>-1287</v>
+        <v>-1286.6</v>
       </c>
       <c r="Z842" t="n">
-        <v>-9009</v>
+        <v>-9006</v>
       </c>
     </row>
     <row r="843">
@@ -67666,7 +67666,7 @@
         <v>187</v>
       </c>
       <c r="J843" t="n">
-        <v>133497</v>
+        <v>105737</v>
       </c>
       <c r="K843" t="n">
         <v>7561116</v>
@@ -67702,19 +67702,19 @@
         <v>3196.6</v>
       </c>
       <c r="V843" t="n">
-        <v>13662</v>
+        <v>13664</v>
       </c>
       <c r="W843" t="n">
-        <v>11.4</v>
+        <v>14.8</v>
       </c>
       <c r="X843" t="n">
-        <v>1506</v>
+        <v>1506.7</v>
       </c>
       <c r="Y843" t="n">
-        <v>662.4</v>
+        <v>663.1</v>
       </c>
       <c r="Z843" t="n">
-        <v>4637</v>
+        <v>4642</v>
       </c>
     </row>
     <row r="844">
@@ -67746,7 +67746,7 @@
         <v>202</v>
       </c>
       <c r="J844" t="n">
-        <v>142802</v>
+        <v>115048</v>
       </c>
       <c r="K844" t="n">
         <v>8959268</v>
@@ -67782,19 +67782,19 @@
         <v>3715</v>
       </c>
       <c r="V844" t="n">
-        <v>9305</v>
+        <v>9311</v>
       </c>
       <c r="W844" t="n">
-        <v>7</v>
+        <v>8.8</v>
       </c>
       <c r="X844" t="n">
-        <v>95</v>
+        <v>97.7</v>
       </c>
       <c r="Y844" t="n">
-        <v>1988.1</v>
+        <v>1989.6</v>
       </c>
       <c r="Z844" t="n">
-        <v>13917</v>
+        <v>13927</v>
       </c>
     </row>
     <row r="845">
@@ -67826,7 +67826,7 @@
         <v>125</v>
       </c>
       <c r="J845" t="n">
-        <v>129282</v>
+        <v>101535</v>
       </c>
       <c r="K845" t="n">
         <v>7518888</v>
@@ -67862,19 +67862,19 @@
         <v>3814.6</v>
       </c>
       <c r="V845" t="n">
-        <v>-13520</v>
+        <v>-13513</v>
       </c>
       <c r="W845" t="n">
-        <v>-9.5</v>
+        <v>-11.7</v>
       </c>
       <c r="X845" t="n">
-        <v>3149</v>
+        <v>3154</v>
       </c>
       <c r="Y845" t="n">
-        <v>53</v>
+        <v>55.3</v>
       </c>
       <c r="Z845" t="n">
-        <v>371</v>
+        <v>387</v>
       </c>
     </row>
     <row r="846">
@@ -67906,7 +67906,7 @@
         <v>182</v>
       </c>
       <c r="J846" t="n">
-        <v>129328</v>
+        <v>101587</v>
       </c>
       <c r="K846" t="n">
         <v>7525952</v>
@@ -67942,19 +67942,19 @@
         <v>3758.1</v>
       </c>
       <c r="V846" t="n">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="W846" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="X846" t="n">
-        <v>-1389.7</v>
+        <v>-1383.3</v>
       </c>
       <c r="Y846" t="n">
-        <v>53.6</v>
+        <v>56.4</v>
       </c>
       <c r="Z846" t="n">
-        <v>375</v>
+        <v>395</v>
       </c>
     </row>
     <row r="847">
@@ -67962,34 +67962,34 @@
         <v>44676</v>
       </c>
       <c r="B847" t="n">
-        <v>2904</v>
+        <v>3832</v>
       </c>
       <c r="C847" t="n">
         <v>779</v>
       </c>
       <c r="D847" t="n">
-        <v>127673</v>
+        <v>6169077</v>
       </c>
       <c r="E847" t="n">
         <v>6874</v>
       </c>
       <c r="F847" t="n">
-        <v>4576</v>
+        <v>4839</v>
       </c>
       <c r="G847" t="n">
-        <v>127673</v>
+        <v>127721</v>
       </c>
       <c r="H847" t="n">
         <v>17234</v>
       </c>
       <c r="I847" t="n">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="J847" t="n">
-        <v>136257</v>
+        <v>115151</v>
       </c>
       <c r="K847" t="n">
-        <v>8277096</v>
+        <v>8977333</v>
       </c>
       <c r="L847" t="n">
         <v>3548934</v>
@@ -67998,10 +67998,10 @@
         <v>0</v>
       </c>
       <c r="N847" t="n">
-        <v>-566455</v>
+        <v>133782</v>
       </c>
       <c r="O847" t="n">
-        <v>810410</v>
+        <v>1510647</v>
       </c>
       <c r="P847" t="n">
         <v>46928</v>
@@ -68010,10 +68010,10 @@
         <v>26641</v>
       </c>
       <c r="R847" t="n">
-        <v>751144</v>
+        <v>1451381</v>
       </c>
       <c r="S847" t="n">
-        <v>115772.9</v>
+        <v>215806.7</v>
       </c>
       <c r="T847" t="n">
         <v>3254</v>
@@ -68022,19 +68022,19 @@
         <v>3805.9</v>
       </c>
       <c r="V847" t="n">
-        <v>6929</v>
+        <v>13564</v>
       </c>
       <c r="W847" t="n">
-        <v>5.4</v>
+        <v>13.4</v>
       </c>
       <c r="X847" t="n">
-        <v>-2181.7</v>
+        <v>34.3</v>
       </c>
       <c r="Y847" t="n">
-        <v>1039.7</v>
+        <v>1990.6</v>
       </c>
       <c r="Z847" t="n">
-        <v>7278</v>
+        <v>13934</v>
       </c>
     </row>
     <row r="848">
@@ -68042,34 +68042,34 @@
         <v>44677</v>
       </c>
       <c r="B848" t="n">
-        <v>9836</v>
+        <v>10755</v>
       </c>
       <c r="C848" t="n">
         <v>4404</v>
       </c>
       <c r="D848" t="n">
-        <v>362</v>
+        <v>6045840</v>
       </c>
       <c r="E848" t="n">
         <v>7287</v>
       </c>
       <c r="F848" t="n">
-        <v>4690</v>
+        <v>4953</v>
       </c>
       <c r="G848" t="n">
-        <v>362</v>
+        <v>415</v>
       </c>
       <c r="H848" t="n">
         <v>32733</v>
       </c>
       <c r="I848" t="n">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="J848" t="n">
-        <v>136336</v>
+        <v>115233</v>
       </c>
       <c r="K848" t="n">
-        <v>8298103</v>
+        <v>8999266</v>
       </c>
       <c r="L848" t="n">
         <v>3555033</v>
@@ -68078,10 +68078,10 @@
         <v>0</v>
       </c>
       <c r="N848" t="n">
-        <v>-561382</v>
+        <v>139781</v>
       </c>
       <c r="O848" t="n">
-        <v>-621038</v>
+        <v>80125</v>
       </c>
       <c r="P848" t="n">
         <v>48110</v>
@@ -68090,10 +68090,10 @@
         <v>25937</v>
       </c>
       <c r="R848" t="n">
-        <v>21007</v>
+        <v>21933</v>
       </c>
       <c r="S848" t="n">
-        <v>-88719.7</v>
+        <v>11446.4</v>
       </c>
       <c r="T848" t="n">
         <v>6099</v>
@@ -68102,19 +68102,19 @@
         <v>3705.3</v>
       </c>
       <c r="V848" t="n">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="W848" t="n">
         <v>0.1</v>
       </c>
       <c r="X848" t="n">
-        <v>2351.3</v>
+        <v>4566</v>
       </c>
       <c r="Y848" t="n">
-        <v>-883</v>
+        <v>68.3</v>
       </c>
       <c r="Z848" t="n">
-        <v>-6181</v>
+        <v>478</v>
       </c>
     </row>
     <row r="849">
@@ -68122,34 +68122,34 @@
         <v>44678</v>
       </c>
       <c r="B849" t="n">
-        <v>3409</v>
+        <v>4311</v>
       </c>
       <c r="C849" t="n">
         <v>2548</v>
       </c>
       <c r="D849" t="n">
-        <v>127908</v>
+        <v>6177655</v>
       </c>
       <c r="E849" t="n">
         <v>7696</v>
       </c>
       <c r="F849" t="n">
-        <v>4042</v>
+        <v>4306</v>
       </c>
       <c r="G849" t="n">
-        <v>127908</v>
+        <v>127953</v>
       </c>
       <c r="H849" t="n">
         <v>17241</v>
       </c>
       <c r="I849" t="n">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="J849" t="n">
-        <v>122811</v>
+        <v>101712</v>
       </c>
       <c r="K849" t="n">
-        <v>6859374</v>
+        <v>7561449</v>
       </c>
       <c r="L849" t="n">
         <v>3559406</v>
@@ -68158,10 +68158,10 @@
         <v>0</v>
       </c>
       <c r="N849" t="n">
-        <v>-579787</v>
+        <v>122288</v>
       </c>
       <c r="O849" t="n">
-        <v>740218</v>
+        <v>1442293</v>
       </c>
       <c r="P849" t="n">
         <v>48956</v>
@@ -68170,10 +68170,10 @@
         <v>26706</v>
       </c>
       <c r="R849" t="n">
-        <v>-1438729</v>
+        <v>-1437817</v>
       </c>
       <c r="S849" t="n">
-        <v>105745.4</v>
+        <v>206041.9</v>
       </c>
       <c r="T849" t="n">
         <v>4373</v>
@@ -68182,19 +68182,19 @@
         <v>3815.1</v>
       </c>
       <c r="V849" t="n">
-        <v>-13525</v>
+        <v>-13521</v>
       </c>
       <c r="W849" t="n">
-        <v>-9.9</v>
+        <v>-11.7</v>
       </c>
       <c r="X849" t="n">
-        <v>-2172.3</v>
+        <v>41.7</v>
       </c>
       <c r="Y849" t="n">
-        <v>425.1</v>
+        <v>1377</v>
       </c>
       <c r="Z849" t="n">
-        <v>2976</v>
+        <v>9639</v>
       </c>
     </row>
     <row r="850">
@@ -68202,34 +68202,34 @@
         <v>44679</v>
       </c>
       <c r="B850" t="n">
-        <v>3314</v>
+        <v>4170</v>
       </c>
       <c r="C850" t="n">
         <v>350</v>
       </c>
       <c r="D850" t="n">
-        <v>127547</v>
+        <v>6180726</v>
       </c>
       <c r="E850" t="n">
         <v>8009</v>
       </c>
       <c r="F850" t="n">
-        <v>4244</v>
+        <v>4523</v>
       </c>
       <c r="G850" t="n">
-        <v>127547</v>
+        <v>127599</v>
       </c>
       <c r="H850" t="n">
         <v>17250</v>
       </c>
       <c r="I850" t="n">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="J850" t="n">
-        <v>133829</v>
+        <v>112730</v>
       </c>
       <c r="K850" t="n">
-        <v>8095672</v>
+        <v>8798609</v>
       </c>
       <c r="L850" t="n">
         <v>3384732</v>
@@ -68238,10 +68238,10 @@
         <v>0</v>
       </c>
       <c r="N850" t="n">
-        <v>652698</v>
+        <v>1355635</v>
       </c>
       <c r="O850" t="n">
-        <v>534556</v>
+        <v>1237493</v>
       </c>
       <c r="P850" t="n">
         <v>-128930</v>
@@ -68250,10 +68250,10 @@
         <v>-151306</v>
       </c>
       <c r="R850" t="n">
-        <v>1236298</v>
+        <v>1237160</v>
       </c>
       <c r="S850" t="n">
-        <v>76365.1</v>
+        <v>176784.7</v>
       </c>
       <c r="T850" t="n">
         <v>-174674</v>
@@ -68265,16 +68265,16 @@
         <v>11018</v>
       </c>
       <c r="W850" t="n">
-        <v>9</v>
+        <v>10.8</v>
       </c>
       <c r="X850" t="n">
-        <v>-809.3</v>
+        <v>-807</v>
       </c>
       <c r="Y850" t="n">
-        <v>47.4</v>
+        <v>999</v>
       </c>
       <c r="Z850" t="n">
-        <v>332</v>
+        <v>6993</v>
       </c>
     </row>
     <row r="851">
@@ -68282,34 +68282,34 @@
         <v>44680</v>
       </c>
       <c r="B851" t="n">
-        <v>7074</v>
+        <v>8006</v>
       </c>
       <c r="C851" t="n">
         <v>2567</v>
       </c>
       <c r="D851" t="n">
-        <v>0</v>
+        <v>6056803</v>
       </c>
       <c r="E851" t="n">
         <v>8294</v>
       </c>
       <c r="F851" t="n">
-        <v>4177</v>
+        <v>4439</v>
       </c>
       <c r="G851" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H851" t="n">
         <v>17265</v>
       </c>
       <c r="I851" t="n">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="J851" t="n">
-        <v>133917</v>
+        <v>112818</v>
       </c>
       <c r="K851" t="n">
-        <v>8117402</v>
+        <v>8821275</v>
       </c>
       <c r="L851" t="n">
         <v>3390892</v>
@@ -68318,10 +68318,10 @@
         <v>0</v>
       </c>
       <c r="N851" t="n">
-        <v>672053</v>
+        <v>1375926</v>
       </c>
       <c r="O851" t="n">
-        <v>-841866</v>
+        <v>-137993</v>
       </c>
       <c r="P851" t="n">
         <v>-124467</v>
@@ -68330,10 +68330,10 @@
         <v>-150472</v>
       </c>
       <c r="R851" t="n">
-        <v>21730</v>
+        <v>22666</v>
       </c>
       <c r="S851" t="n">
-        <v>-120266.6</v>
+        <v>-19713.3</v>
       </c>
       <c r="T851" t="n">
         <v>6160</v>
@@ -68348,13 +68348,13 @@
         <v>0.1</v>
       </c>
       <c r="X851" t="n">
-        <v>-806.3</v>
+        <v>-805</v>
       </c>
       <c r="Y851" t="n">
-        <v>-1269.3</v>
+        <v>-318.6</v>
       </c>
       <c r="Z851" t="n">
-        <v>-8885</v>
+        <v>-2230</v>
       </c>
     </row>
     <row r="852">
@@ -68362,34 +68362,34 @@
         <v>44681</v>
       </c>
       <c r="B852" t="n">
-        <v>2000</v>
+        <v>2485</v>
       </c>
       <c r="C852" t="n">
         <v>185</v>
       </c>
       <c r="D852" t="n">
-        <v>0</v>
+        <v>6059278</v>
       </c>
       <c r="E852" t="n">
         <v>8381</v>
       </c>
       <c r="F852" t="n">
-        <v>3592</v>
+        <v>3886</v>
       </c>
       <c r="G852" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H852" t="n">
         <v>17282</v>
       </c>
       <c r="I852" t="n">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="J852" t="n">
-        <v>120308</v>
+        <v>99209</v>
       </c>
       <c r="K852" t="n">
-        <v>6661823</v>
+        <v>7366184</v>
       </c>
       <c r="L852" t="n">
         <v>3393551</v>
@@ -68398,10 +68398,10 @@
         <v>0</v>
       </c>
       <c r="N852" t="n">
-        <v>-790842</v>
+        <v>-86481</v>
       </c>
       <c r="O852" t="n">
-        <v>-857065</v>
+        <v>-152704</v>
       </c>
       <c r="P852" t="n">
         <v>-123726</v>
@@ -68410,10 +68410,10 @@
         <v>-150428</v>
       </c>
       <c r="R852" t="n">
-        <v>-1455579</v>
+        <v>-1455091</v>
       </c>
       <c r="S852" t="n">
-        <v>-122437.9</v>
+        <v>-21814.9</v>
       </c>
       <c r="T852" t="n">
         <v>2659</v>
@@ -68425,16 +68425,16 @@
         <v>-13609</v>
       </c>
       <c r="W852" t="n">
-        <v>-10.2</v>
+        <v>-12.1</v>
       </c>
       <c r="X852" t="n">
         <v>-834.3</v>
       </c>
       <c r="Y852" t="n">
-        <v>-1282</v>
+        <v>-332.3</v>
       </c>
       <c r="Z852" t="n">
-        <v>-8974</v>
+        <v>-2326</v>
       </c>
     </row>
     <row r="853">
@@ -68442,34 +68442,34 @@
         <v>44682</v>
       </c>
       <c r="B853" t="n">
-        <v>745</v>
+        <v>1156</v>
       </c>
       <c r="C853" t="n">
         <v>1413</v>
       </c>
       <c r="D853" t="n">
-        <v>127621</v>
+        <v>6189063</v>
       </c>
       <c r="E853" t="n">
         <v>8432</v>
       </c>
       <c r="F853" t="n">
-        <v>3504</v>
+        <v>3821</v>
       </c>
       <c r="G853" t="n">
-        <v>127621</v>
+        <v>127646</v>
       </c>
       <c r="H853" t="n">
         <v>17294</v>
       </c>
       <c r="I853" t="n">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="J853" t="n">
-        <v>64765</v>
+        <v>71432</v>
       </c>
       <c r="K853" t="n">
-        <v>6670357</v>
+        <v>7375133</v>
       </c>
       <c r="L853" t="n">
         <v>3395024</v>
@@ -68478,10 +68478,10 @@
         <v>0</v>
       </c>
       <c r="N853" t="n">
-        <v>-790822</v>
+        <v>-86046</v>
       </c>
       <c r="O853" t="n">
-        <v>-855595</v>
+        <v>-150819</v>
       </c>
       <c r="P853" t="n">
         <v>-124349</v>
@@ -68490,10 +68490,10 @@
         <v>-150656</v>
       </c>
       <c r="R853" t="n">
-        <v>8534</v>
+        <v>8949</v>
       </c>
       <c r="S853" t="n">
-        <v>-122227.9</v>
+        <v>-21545.6</v>
       </c>
       <c r="T853" t="n">
         <v>1473</v>
@@ -68502,19 +68502,19 @@
         <v>-21522.3</v>
       </c>
       <c r="V853" t="n">
-        <v>-55543</v>
+        <v>-27777</v>
       </c>
       <c r="W853" t="n">
-        <v>-46.2</v>
+        <v>-28</v>
       </c>
       <c r="X853" t="n">
-        <v>-23021.3</v>
+        <v>-13766</v>
       </c>
       <c r="Y853" t="n">
-        <v>-9223.3</v>
+        <v>-4307.9</v>
       </c>
       <c r="Z853" t="n">
-        <v>-64563</v>
+        <v>-30155</v>
       </c>
     </row>
     <row r="854">
@@ -68561,7 +68561,7 @@
         <v>666455</v>
       </c>
       <c r="O854" t="n">
-        <v>-143955</v>
+        <v>-844192</v>
       </c>
       <c r="P854" t="n">
         <v>-124817</v>
@@ -68570,10 +68570,10 @@
         <v>-151458</v>
       </c>
       <c r="R854" t="n">
-        <v>1462784</v>
+        <v>758008</v>
       </c>
       <c r="S854" t="n">
-        <v>-20565</v>
+        <v>-120598.9</v>
       </c>
       <c r="T854" t="n">
         <v>2452</v>
@@ -68582,19 +68582,19 @@
         <v>-21636.9</v>
       </c>
       <c r="V854" t="n">
-        <v>13628</v>
+        <v>6961</v>
       </c>
       <c r="W854" t="n">
-        <v>21</v>
+        <v>9.7</v>
       </c>
       <c r="X854" t="n">
-        <v>-18508</v>
+        <v>-11475</v>
       </c>
       <c r="Y854" t="n">
-        <v>-8266.3</v>
+        <v>-5251.1</v>
       </c>
       <c r="Z854" t="n">
-        <v>-57864</v>
+        <v>-36758</v>
       </c>
     </row>
     <row r="855">
@@ -68641,7 +68641,7 @@
         <v>-4247278</v>
       </c>
       <c r="O855" t="n">
-        <v>-3626240</v>
+        <v>-4327403</v>
       </c>
       <c r="P855" t="n">
         <v>-2535845</v>
@@ -68653,7 +68653,7 @@
         <v>-3461278</v>
       </c>
       <c r="S855" t="n">
-        <v>-518034.3</v>
+        <v>-618200.4</v>
       </c>
       <c r="T855" t="n">
         <v>-2404225</v>
@@ -68668,13 +68668,13 @@
         <v>-41.5</v>
       </c>
       <c r="X855" t="n">
-        <v>-24823</v>
+        <v>-17790</v>
       </c>
       <c r="Y855" t="n">
-        <v>-12928.1</v>
+        <v>-9913.4</v>
       </c>
       <c r="Z855" t="n">
-        <v>-90497</v>
+        <v>-69394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualiza datos provincias 2022-06-09
</commit_message>
<xml_diff>
--- a/data/output/covid19-spain_consolidated.xlsx
+++ b/data/output/covid19-spain_consolidated.xlsx
@@ -59722,10 +59722,10 @@
         <v>44573</v>
       </c>
       <c r="B744" t="n">
-        <v>65360</v>
+        <v>65358</v>
       </c>
       <c r="C744" t="n">
-        <v>29248</v>
+        <v>29246</v>
       </c>
       <c r="D744" t="n">
         <v>5499647</v>
@@ -59749,37 +59749,37 @@
         <v>105841</v>
       </c>
       <c r="K744" t="n">
-        <v>8114600</v>
+        <v>8114598</v>
       </c>
       <c r="L744" t="n">
-        <v>4614542</v>
+        <v>4614540</v>
       </c>
       <c r="M744" t="n">
         <v>13206</v>
       </c>
       <c r="N744" t="n">
-        <v>1670889</v>
+        <v>1670887</v>
       </c>
       <c r="O744" t="n">
-        <v>882547</v>
+        <v>882545</v>
       </c>
       <c r="P744" t="n">
-        <v>952770</v>
+        <v>952768</v>
       </c>
       <c r="Q744" t="n">
-        <v>499035</v>
+        <v>499033</v>
       </c>
       <c r="R744" t="n">
-        <v>152277</v>
+        <v>152275</v>
       </c>
       <c r="S744" t="n">
-        <v>126078.1</v>
+        <v>126077.9</v>
       </c>
       <c r="T744" t="n">
-        <v>87141</v>
+        <v>87139</v>
       </c>
       <c r="U744" t="n">
-        <v>71290.7</v>
+        <v>71290.4</v>
       </c>
       <c r="V744" t="n">
         <v>213</v>
@@ -59802,13 +59802,13 @@
         <v>44574</v>
       </c>
       <c r="B745" t="n">
-        <v>62529</v>
+        <v>62528</v>
       </c>
       <c r="C745" t="n">
         <v>28432</v>
       </c>
       <c r="D745" t="n">
-        <v>5522553</v>
+        <v>5522552</v>
       </c>
       <c r="E745" t="n">
         <v>159443</v>
@@ -59817,7 +59817,7 @@
         <v>15045</v>
       </c>
       <c r="G745" t="n">
-        <v>123226</v>
+        <v>123225</v>
       </c>
       <c r="H745" t="n">
         <v>144301</v>
@@ -59829,37 +59829,37 @@
         <v>106028</v>
       </c>
       <c r="K745" t="n">
-        <v>8258818</v>
+        <v>8258815</v>
       </c>
       <c r="L745" t="n">
-        <v>4692623</v>
+        <v>4692621</v>
       </c>
       <c r="M745" t="n">
         <v>13428</v>
       </c>
       <c r="N745" t="n">
-        <v>1691112</v>
+        <v>1691109</v>
       </c>
       <c r="O745" t="n">
-        <v>944065</v>
+        <v>944062</v>
       </c>
       <c r="P745" t="n">
-        <v>955806</v>
+        <v>955804</v>
       </c>
       <c r="Q745" t="n">
-        <v>531213</v>
+        <v>531211</v>
       </c>
       <c r="R745" t="n">
-        <v>144218</v>
+        <v>144217</v>
       </c>
       <c r="S745" t="n">
-        <v>134866.4</v>
+        <v>134866</v>
       </c>
       <c r="T745" t="n">
         <v>78081</v>
       </c>
       <c r="U745" t="n">
-        <v>75887.6</v>
+        <v>75887.3</v>
       </c>
       <c r="V745" t="n">
         <v>187</v>
@@ -59882,10 +59882,10 @@
         <v>44575</v>
       </c>
       <c r="B746" t="n">
-        <v>65198</v>
+        <v>65197</v>
       </c>
       <c r="C746" t="n">
-        <v>24434</v>
+        <v>24433</v>
       </c>
       <c r="D746" t="n">
         <v>5422650</v>
@@ -59909,37 +59909,37 @@
         <v>106196</v>
       </c>
       <c r="K746" t="n">
-        <v>8400710</v>
+        <v>8400706</v>
       </c>
       <c r="L746" t="n">
-        <v>4771074</v>
+        <v>4771071</v>
       </c>
       <c r="M746" t="n">
         <v>13681</v>
       </c>
       <c r="N746" t="n">
-        <v>1745199</v>
+        <v>1745195</v>
       </c>
       <c r="O746" t="n">
-        <v>936921</v>
+        <v>936917</v>
       </c>
       <c r="P746" t="n">
-        <v>985655</v>
+        <v>985652</v>
       </c>
       <c r="Q746" t="n">
-        <v>529680</v>
+        <v>529677</v>
       </c>
       <c r="R746" t="n">
-        <v>141892</v>
+        <v>141891</v>
       </c>
       <c r="S746" t="n">
-        <v>133845.9</v>
+        <v>133845.3</v>
       </c>
       <c r="T746" t="n">
-        <v>78451</v>
+        <v>78450</v>
       </c>
       <c r="U746" t="n">
-        <v>75668.6</v>
+        <v>75668.1</v>
       </c>
       <c r="V746" t="n">
         <v>168</v>
@@ -59989,37 +59989,37 @@
         <v>106339</v>
       </c>
       <c r="K747" t="n">
-        <v>8469628</v>
+        <v>8469624</v>
       </c>
       <c r="L747" t="n">
-        <v>4812414</v>
+        <v>4812411</v>
       </c>
       <c r="M747" t="n">
         <v>13093</v>
       </c>
       <c r="N747" t="n">
-        <v>1772684</v>
+        <v>1772680</v>
       </c>
       <c r="O747" t="n">
-        <v>928464</v>
+        <v>928460</v>
       </c>
       <c r="P747" t="n">
-        <v>1000546</v>
+        <v>1000543</v>
       </c>
       <c r="Q747" t="n">
-        <v>527049</v>
+        <v>527046</v>
       </c>
       <c r="R747" t="n">
         <v>68918</v>
       </c>
       <c r="S747" t="n">
-        <v>132637.7</v>
+        <v>132637.1</v>
       </c>
       <c r="T747" t="n">
         <v>41340</v>
       </c>
       <c r="U747" t="n">
-        <v>75292.7</v>
+        <v>75292.3</v>
       </c>
       <c r="V747" t="n">
         <v>143</v>
@@ -60069,37 +60069,37 @@
         <v>106481</v>
       </c>
       <c r="K748" t="n">
-        <v>8551074</v>
+        <v>8551070</v>
       </c>
       <c r="L748" t="n">
-        <v>4862481</v>
+        <v>4862478</v>
       </c>
       <c r="M748" t="n">
         <v>13828</v>
       </c>
       <c r="N748" t="n">
-        <v>1782322</v>
+        <v>1782318</v>
       </c>
       <c r="O748" t="n">
-        <v>926460</v>
+        <v>926456</v>
       </c>
       <c r="P748" t="n">
-        <v>1006117</v>
+        <v>1006114</v>
       </c>
       <c r="Q748" t="n">
-        <v>524541</v>
+        <v>524538</v>
       </c>
       <c r="R748" t="n">
         <v>81446</v>
       </c>
       <c r="S748" t="n">
-        <v>132351.4</v>
+        <v>132350.9</v>
       </c>
       <c r="T748" t="n">
         <v>50067</v>
       </c>
       <c r="U748" t="n">
-        <v>74934.4</v>
+        <v>74934</v>
       </c>
       <c r="V748" t="n">
         <v>142</v>
@@ -60122,7 +60122,7 @@
         <v>44578</v>
       </c>
       <c r="B749" t="n">
-        <v>68914</v>
+        <v>68926</v>
       </c>
       <c r="C749" t="n">
         <v>30648</v>
@@ -60149,37 +60149,37 @@
         <v>106679</v>
       </c>
       <c r="K749" t="n">
-        <v>8730992</v>
+        <v>8731000</v>
       </c>
       <c r="L749" t="n">
-        <v>4958400</v>
+        <v>4958397</v>
       </c>
       <c r="M749" t="n">
         <v>14239</v>
       </c>
       <c r="N749" t="n">
-        <v>1768075</v>
+        <v>1768083</v>
       </c>
       <c r="O749" t="n">
-        <v>924703</v>
+        <v>924711</v>
       </c>
       <c r="P749" t="n">
-        <v>1007628</v>
+        <v>1007625</v>
       </c>
       <c r="Q749" t="n">
-        <v>521201</v>
+        <v>521198</v>
       </c>
       <c r="R749" t="n">
-        <v>179918</v>
+        <v>179930</v>
       </c>
       <c r="S749" t="n">
-        <v>132100.4</v>
+        <v>132101.6</v>
       </c>
       <c r="T749" t="n">
         <v>95919</v>
       </c>
       <c r="U749" t="n">
-        <v>74457.3</v>
+        <v>74456.9</v>
       </c>
       <c r="V749" t="n">
         <v>198</v>
@@ -60202,7 +60202,7 @@
         <v>44579</v>
       </c>
       <c r="B750" t="n">
-        <v>49945</v>
+        <v>49950</v>
       </c>
       <c r="C750" t="n">
         <v>22723</v>
@@ -60229,37 +60229,37 @@
         <v>107035</v>
       </c>
       <c r="K750" t="n">
-        <v>8868284</v>
+        <v>8868297</v>
       </c>
       <c r="L750" t="n">
-        <v>5042583</v>
+        <v>5042580</v>
       </c>
       <c r="M750" t="n">
         <v>14647</v>
       </c>
       <c r="N750" t="n">
-        <v>1766273</v>
+        <v>1766286</v>
       </c>
       <c r="O750" t="n">
-        <v>905961</v>
+        <v>905974</v>
       </c>
       <c r="P750" t="n">
-        <v>1007528</v>
+        <v>1007525</v>
       </c>
       <c r="Q750" t="n">
-        <v>515182</v>
+        <v>515179</v>
       </c>
       <c r="R750" t="n">
-        <v>137292</v>
+        <v>137297</v>
       </c>
       <c r="S750" t="n">
-        <v>129423</v>
+        <v>129424.9</v>
       </c>
       <c r="T750" t="n">
         <v>84183</v>
       </c>
       <c r="U750" t="n">
-        <v>73597.4</v>
+        <v>73597</v>
       </c>
       <c r="V750" t="n">
         <v>356</v>
@@ -60282,7 +60282,7 @@
         <v>44580</v>
       </c>
       <c r="B751" t="n">
-        <v>56311</v>
+        <v>56313</v>
       </c>
       <c r="C751" t="n">
         <v>21214</v>
@@ -60309,37 +60309,37 @@
         <v>107328</v>
       </c>
       <c r="K751" t="n">
-        <v>9007105</v>
+        <v>9007120</v>
       </c>
       <c r="L751" t="n">
-        <v>5122652</v>
+        <v>5122649</v>
       </c>
       <c r="M751" t="n">
         <v>14843</v>
       </c>
       <c r="N751" t="n">
-        <v>1775052</v>
+        <v>1775067</v>
       </c>
       <c r="O751" t="n">
-        <v>892505</v>
+        <v>892522</v>
       </c>
       <c r="P751" t="n">
-        <v>1007145</v>
+        <v>1007142</v>
       </c>
       <c r="Q751" t="n">
-        <v>508110</v>
+        <v>508109</v>
       </c>
       <c r="R751" t="n">
-        <v>138821</v>
+        <v>138823</v>
       </c>
       <c r="S751" t="n">
-        <v>127500.7</v>
+        <v>127503.1</v>
       </c>
       <c r="T751" t="n">
         <v>80069</v>
       </c>
       <c r="U751" t="n">
-        <v>72587.1</v>
+        <v>72587</v>
       </c>
       <c r="V751" t="n">
         <v>293</v>
@@ -60362,7 +60362,7 @@
         <v>44581</v>
       </c>
       <c r="B752" t="n">
-        <v>54586</v>
+        <v>54590</v>
       </c>
       <c r="C752" t="n">
         <v>21461</v>
@@ -60389,37 +60389,37 @@
         <v>107592</v>
       </c>
       <c r="K752" t="n">
-        <v>9149566</v>
+        <v>9149585</v>
       </c>
       <c r="L752" t="n">
-        <v>5192364</v>
+        <v>5192361</v>
       </c>
       <c r="M752" t="n">
         <v>15126</v>
       </c>
       <c r="N752" t="n">
-        <v>1834813</v>
+        <v>1834832</v>
       </c>
       <c r="O752" t="n">
-        <v>890748</v>
+        <v>890770</v>
       </c>
       <c r="P752" t="n">
-        <v>1030954</v>
+        <v>1030951</v>
       </c>
       <c r="Q752" t="n">
-        <v>499741</v>
+        <v>499740</v>
       </c>
       <c r="R752" t="n">
-        <v>142461</v>
+        <v>142465</v>
       </c>
       <c r="S752" t="n">
-        <v>127249.7</v>
+        <v>127252.9</v>
       </c>
       <c r="T752" t="n">
         <v>69712</v>
       </c>
       <c r="U752" t="n">
-        <v>71391.6</v>
+        <v>71391.4</v>
       </c>
       <c r="V752" t="n">
         <v>264</v>
@@ -60442,10 +60442,10 @@
         <v>44582</v>
       </c>
       <c r="B753" t="n">
-        <v>49960</v>
+        <v>49962</v>
       </c>
       <c r="C753" t="n">
-        <v>19224</v>
+        <v>19226</v>
       </c>
       <c r="D753" t="n">
         <v>5520237</v>
@@ -60469,37 +60469,37 @@
         <v>107802</v>
       </c>
       <c r="K753" t="n">
-        <v>9267754</v>
+        <v>9267775</v>
       </c>
       <c r="L753" t="n">
-        <v>5259426</v>
+        <v>5259425</v>
       </c>
       <c r="M753" t="n">
         <v>15336</v>
       </c>
       <c r="N753" t="n">
-        <v>1803965</v>
+        <v>1803986</v>
       </c>
       <c r="O753" t="n">
-        <v>867044</v>
+        <v>867069</v>
       </c>
       <c r="P753" t="n">
-        <v>1018032</v>
+        <v>1018031</v>
       </c>
       <c r="Q753" t="n">
-        <v>488352</v>
+        <v>488354</v>
       </c>
       <c r="R753" t="n">
-        <v>118188</v>
+        <v>118190</v>
       </c>
       <c r="S753" t="n">
-        <v>123863.4</v>
+        <v>123867</v>
       </c>
       <c r="T753" t="n">
-        <v>67062</v>
+        <v>67064</v>
       </c>
       <c r="U753" t="n">
-        <v>69764.6</v>
+        <v>69764.9</v>
       </c>
       <c r="V753" t="n">
         <v>210</v>
@@ -60522,7 +60522,7 @@
         <v>44583</v>
       </c>
       <c r="B754" t="n">
-        <v>18687</v>
+        <v>18690</v>
       </c>
       <c r="C754" t="n">
         <v>9356</v>
@@ -60549,37 +60549,37 @@
         <v>107973</v>
       </c>
       <c r="K754" t="n">
-        <v>9335057</v>
+        <v>9335081</v>
       </c>
       <c r="L754" t="n">
-        <v>5297418</v>
+        <v>5297417</v>
       </c>
       <c r="M754" t="n">
         <v>15351</v>
       </c>
       <c r="N754" t="n">
-        <v>1793893</v>
+        <v>1793917</v>
       </c>
       <c r="O754" t="n">
-        <v>865429</v>
+        <v>865457</v>
       </c>
       <c r="P754" t="n">
-        <v>1012053</v>
+        <v>1012052</v>
       </c>
       <c r="Q754" t="n">
-        <v>485004</v>
+        <v>485006</v>
       </c>
       <c r="R754" t="n">
-        <v>67303</v>
+        <v>67306</v>
       </c>
       <c r="S754" t="n">
-        <v>123632.7</v>
+        <v>123636.7</v>
       </c>
       <c r="T754" t="n">
         <v>37992</v>
       </c>
       <c r="U754" t="n">
-        <v>69286.3</v>
+        <v>69286.6</v>
       </c>
       <c r="V754" t="n">
         <v>171</v>
@@ -60602,10 +60602,10 @@
         <v>44584</v>
       </c>
       <c r="B755" t="n">
-        <v>14384</v>
+        <v>14383</v>
       </c>
       <c r="C755" t="n">
-        <v>7815</v>
+        <v>7814</v>
       </c>
       <c r="D755" t="n">
         <v>5659967</v>
@@ -60629,37 +60629,37 @@
         <v>108124</v>
       </c>
       <c r="K755" t="n">
-        <v>9397518</v>
+        <v>9397541</v>
       </c>
       <c r="L755" t="n">
-        <v>5336994</v>
+        <v>5336992</v>
       </c>
       <c r="M755" t="n">
         <v>15511</v>
       </c>
       <c r="N755" t="n">
-        <v>1772904</v>
+        <v>1772927</v>
       </c>
       <c r="O755" t="n">
-        <v>846444</v>
+        <v>846471</v>
       </c>
       <c r="P755" t="n">
-        <v>999054</v>
+        <v>999052</v>
       </c>
       <c r="Q755" t="n">
-        <v>474513</v>
+        <v>474514</v>
       </c>
       <c r="R755" t="n">
-        <v>62461</v>
+        <v>62460</v>
       </c>
       <c r="S755" t="n">
-        <v>120920.6</v>
+        <v>120924.4</v>
       </c>
       <c r="T755" t="n">
-        <v>39576</v>
+        <v>39575</v>
       </c>
       <c r="U755" t="n">
-        <v>67787.6</v>
+        <v>67787.7</v>
       </c>
       <c r="V755" t="n">
         <v>151</v>
@@ -60709,37 +60709,37 @@
         <v>108348</v>
       </c>
       <c r="K756" t="n">
-        <v>9557836</v>
+        <v>9557859</v>
       </c>
       <c r="L756" t="n">
-        <v>5409845</v>
+        <v>5409843</v>
       </c>
       <c r="M756" t="n">
         <v>15855</v>
       </c>
       <c r="N756" t="n">
-        <v>1751547</v>
+        <v>1751570</v>
       </c>
       <c r="O756" t="n">
-        <v>826844</v>
+        <v>826859</v>
       </c>
       <c r="P756" t="n">
-        <v>972646</v>
+        <v>972644</v>
       </c>
       <c r="Q756" t="n">
-        <v>451445</v>
+        <v>451446</v>
       </c>
       <c r="R756" t="n">
         <v>160318</v>
       </c>
       <c r="S756" t="n">
-        <v>118120.6</v>
+        <v>118122.7</v>
       </c>
       <c r="T756" t="n">
         <v>72851</v>
       </c>
       <c r="U756" t="n">
-        <v>64492.1</v>
+        <v>64492.3</v>
       </c>
       <c r="V756" t="n">
         <v>224</v>
@@ -60762,13 +60762,13 @@
         <v>44586</v>
       </c>
       <c r="B757" t="n">
-        <v>60229</v>
+        <v>60228</v>
       </c>
       <c r="C757" t="n">
         <v>16584</v>
       </c>
       <c r="D757" t="n">
-        <v>5690336</v>
+        <v>5690335</v>
       </c>
       <c r="E757" t="n">
         <v>139281</v>
@@ -60777,7 +60777,7 @@
         <v>16618</v>
       </c>
       <c r="G757" t="n">
-        <v>124158</v>
+        <v>124157</v>
       </c>
       <c r="H757" t="n">
         <v>148629</v>
@@ -60789,37 +60789,37 @@
         <v>108790</v>
       </c>
       <c r="K757" t="n">
-        <v>9683885</v>
+        <v>9683907</v>
       </c>
       <c r="L757" t="n">
-        <v>5468775</v>
+        <v>5468773</v>
       </c>
       <c r="M757" t="n">
         <v>16098</v>
       </c>
       <c r="N757" t="n">
-        <v>1721562</v>
+        <v>1721584</v>
       </c>
       <c r="O757" t="n">
-        <v>815601</v>
+        <v>815610</v>
       </c>
       <c r="P757" t="n">
-        <v>941374</v>
+        <v>941372</v>
       </c>
       <c r="Q757" t="n">
-        <v>426192</v>
+        <v>426193</v>
       </c>
       <c r="R757" t="n">
-        <v>126049</v>
+        <v>126048</v>
       </c>
       <c r="S757" t="n">
-        <v>116514.4</v>
+        <v>116515.7</v>
       </c>
       <c r="T757" t="n">
         <v>58930</v>
       </c>
       <c r="U757" t="n">
-        <v>60884.6</v>
+        <v>60884.7</v>
       </c>
       <c r="V757" t="n">
         <v>442</v>
@@ -60869,37 +60869,37 @@
         <v>109070</v>
       </c>
       <c r="K758" t="n">
-        <v>9596138</v>
+        <v>9596160</v>
       </c>
       <c r="L758" t="n">
-        <v>5523034</v>
+        <v>5523032</v>
       </c>
       <c r="M758" t="n">
         <v>16324</v>
       </c>
       <c r="N758" t="n">
-        <v>1481538</v>
+        <v>1481562</v>
       </c>
       <c r="O758" t="n">
-        <v>589033</v>
+        <v>589040</v>
       </c>
       <c r="P758" t="n">
         <v>908492</v>
       </c>
       <c r="Q758" t="n">
-        <v>400382</v>
+        <v>400383</v>
       </c>
       <c r="R758" t="n">
         <v>-87747</v>
       </c>
       <c r="S758" t="n">
-        <v>84147.6</v>
+        <v>84148.6</v>
       </c>
       <c r="T758" t="n">
         <v>54259</v>
       </c>
       <c r="U758" t="n">
-        <v>57197.4</v>
+        <v>57197.6</v>
       </c>
       <c r="V758" t="n">
         <v>280</v>
@@ -60949,37 +60949,37 @@
         <v>109310</v>
       </c>
       <c r="K759" t="n">
-        <v>9707255</v>
+        <v>9707277</v>
       </c>
       <c r="L759" t="n">
-        <v>5572653</v>
+        <v>5572651</v>
       </c>
       <c r="M759" t="n">
         <v>16580</v>
       </c>
       <c r="N759" t="n">
-        <v>1448437</v>
+        <v>1448462</v>
       </c>
       <c r="O759" t="n">
-        <v>557689</v>
+        <v>557692</v>
       </c>
       <c r="P759" t="n">
         <v>880030</v>
       </c>
       <c r="Q759" t="n">
-        <v>380289</v>
+        <v>380290</v>
       </c>
       <c r="R759" t="n">
         <v>111117</v>
       </c>
       <c r="S759" t="n">
-        <v>79669.9</v>
+        <v>79670.3</v>
       </c>
       <c r="T759" t="n">
         <v>49619</v>
       </c>
       <c r="U759" t="n">
-        <v>54327</v>
+        <v>54327.1</v>
       </c>
       <c r="V759" t="n">
         <v>240</v>
@@ -61029,37 +61029,37 @@
         <v>109541</v>
       </c>
       <c r="K760" t="n">
-        <v>9798039</v>
+        <v>9798061</v>
       </c>
       <c r="L760" t="n">
-        <v>5614605</v>
+        <v>5614603</v>
       </c>
       <c r="M760" t="n">
         <v>16755</v>
       </c>
       <c r="N760" t="n">
-        <v>1397329</v>
+        <v>1397355</v>
       </c>
       <c r="O760" t="n">
-        <v>530285</v>
+        <v>530286</v>
       </c>
       <c r="P760" t="n">
-        <v>843531</v>
+        <v>843532</v>
       </c>
       <c r="Q760" t="n">
-        <v>355179</v>
+        <v>355178</v>
       </c>
       <c r="R760" t="n">
         <v>90784</v>
       </c>
       <c r="S760" t="n">
-        <v>75755</v>
+        <v>75755.1</v>
       </c>
       <c r="T760" t="n">
         <v>41952</v>
       </c>
       <c r="U760" t="n">
-        <v>50739.9</v>
+        <v>50739.7</v>
       </c>
       <c r="V760" t="n">
         <v>231</v>
@@ -61109,37 +61109,37 @@
         <v>109694</v>
       </c>
       <c r="K761" t="n">
-        <v>9839989</v>
+        <v>9840011</v>
       </c>
       <c r="L761" t="n">
-        <v>5637018</v>
+        <v>5637016</v>
       </c>
       <c r="M761" t="n">
         <v>16756</v>
       </c>
       <c r="N761" t="n">
-        <v>1370361</v>
+        <v>1370387</v>
       </c>
       <c r="O761" t="n">
-        <v>504932</v>
+        <v>504930</v>
       </c>
       <c r="P761" t="n">
-        <v>824604</v>
+        <v>824605</v>
       </c>
       <c r="Q761" t="n">
-        <v>339600</v>
+        <v>339599</v>
       </c>
       <c r="R761" t="n">
         <v>41950</v>
       </c>
       <c r="S761" t="n">
-        <v>72133.1</v>
+        <v>72132.9</v>
       </c>
       <c r="T761" t="n">
         <v>22413</v>
       </c>
       <c r="U761" t="n">
-        <v>48514.3</v>
+        <v>48514.1</v>
       </c>
       <c r="V761" t="n">
         <v>153</v>
@@ -61189,22 +61189,22 @@
         <v>109837</v>
       </c>
       <c r="K762" t="n">
-        <v>9878700</v>
+        <v>9878722</v>
       </c>
       <c r="L762" t="n">
-        <v>5660020</v>
+        <v>5660018</v>
       </c>
       <c r="M762" t="n">
         <v>16849</v>
       </c>
       <c r="N762" t="n">
-        <v>1327626</v>
+        <v>1327652</v>
       </c>
       <c r="O762" t="n">
-        <v>481182</v>
+        <v>481181</v>
       </c>
       <c r="P762" t="n">
-        <v>797539</v>
+        <v>797540</v>
       </c>
       <c r="Q762" t="n">
         <v>323026</v>
@@ -61213,7 +61213,7 @@
         <v>38711</v>
       </c>
       <c r="S762" t="n">
-        <v>68740.3</v>
+        <v>68740.1</v>
       </c>
       <c r="T762" t="n">
         <v>23002</v>
@@ -61269,22 +61269,22 @@
         <v>110097</v>
       </c>
       <c r="K763" t="n">
-        <v>9968233</v>
+        <v>9968255</v>
       </c>
       <c r="L763" t="n">
-        <v>5704648</v>
+        <v>5704646</v>
       </c>
       <c r="M763" t="n">
         <v>17075</v>
       </c>
       <c r="N763" t="n">
-        <v>1237241</v>
+        <v>1237255</v>
       </c>
       <c r="O763" t="n">
-        <v>410397</v>
+        <v>410396</v>
       </c>
       <c r="P763" t="n">
-        <v>746248</v>
+        <v>746249</v>
       </c>
       <c r="Q763" t="n">
         <v>294803</v>
@@ -61293,7 +61293,7 @@
         <v>89533</v>
       </c>
       <c r="S763" t="n">
-        <v>58628.1</v>
+        <v>58628</v>
       </c>
       <c r="T763" t="n">
         <v>44628</v>
@@ -61349,22 +61349,22 @@
         <v>110562</v>
       </c>
       <c r="K764" t="n">
-        <v>10039623</v>
+        <v>10039645</v>
       </c>
       <c r="L764" t="n">
-        <v>5544565</v>
+        <v>5544563</v>
       </c>
       <c r="M764" t="n">
         <v>17226</v>
       </c>
       <c r="N764" t="n">
-        <v>1171339</v>
+        <v>1171348</v>
       </c>
       <c r="O764" t="n">
         <v>355738</v>
       </c>
       <c r="P764" t="n">
-        <v>501982</v>
+        <v>501983</v>
       </c>
       <c r="Q764" t="n">
         <v>75790</v>
@@ -61429,22 +61429,22 @@
         <v>110805</v>
       </c>
       <c r="K765" t="n">
-        <v>10113230</v>
+        <v>10113252</v>
       </c>
       <c r="L765" t="n">
-        <v>5577793</v>
+        <v>5577791</v>
       </c>
       <c r="M765" t="n">
         <v>17408</v>
       </c>
       <c r="N765" t="n">
-        <v>1106125</v>
+        <v>1106132</v>
       </c>
       <c r="O765" t="n">
         <v>517092</v>
       </c>
       <c r="P765" t="n">
-        <v>455141</v>
+        <v>455142</v>
       </c>
       <c r="Q765" t="n">
         <v>54759</v>
@@ -61509,22 +61509,22 @@
         <v>111095</v>
       </c>
       <c r="K766" t="n">
-        <v>10178470</v>
+        <v>10178492</v>
       </c>
       <c r="L766" t="n">
-        <v>5607693</v>
+        <v>5607691</v>
       </c>
       <c r="M766" t="n">
         <v>17548</v>
       </c>
       <c r="N766" t="n">
-        <v>1028904</v>
+        <v>1028907</v>
       </c>
       <c r="O766" t="n">
         <v>471215</v>
       </c>
       <c r="P766" t="n">
-        <v>415329</v>
+        <v>415330</v>
       </c>
       <c r="Q766" t="n">
         <v>35040</v>
@@ -61589,22 +61589,22 @@
         <v>111311</v>
       </c>
       <c r="K767" t="n">
-        <v>10235362</v>
+        <v>10235384</v>
       </c>
       <c r="L767" t="n">
-        <v>5634235</v>
+        <v>5634233</v>
       </c>
       <c r="M767" t="n">
         <v>17735</v>
       </c>
       <c r="N767" t="n">
-        <v>967608</v>
+        <v>967609</v>
       </c>
       <c r="O767" t="n">
         <v>437323</v>
       </c>
       <c r="P767" t="n">
-        <v>374809</v>
+        <v>374808</v>
       </c>
       <c r="Q767" t="n">
         <v>19630</v>
@@ -61669,22 +61669,22 @@
         <v>111503</v>
       </c>
       <c r="K768" t="n">
-        <v>10260274</v>
+        <v>10260296</v>
       </c>
       <c r="L768" t="n">
-        <v>5646822</v>
+        <v>5646820</v>
       </c>
       <c r="M768" t="n">
         <v>17784</v>
       </c>
       <c r="N768" t="n">
-        <v>925217</v>
+        <v>925215</v>
       </c>
       <c r="O768" t="n">
         <v>420285</v>
       </c>
       <c r="P768" t="n">
-        <v>349404</v>
+        <v>349403</v>
       </c>
       <c r="Q768" t="n">
         <v>9804</v>
@@ -61749,16 +61749,16 @@
         <v>111651</v>
       </c>
       <c r="K769" t="n">
-        <v>10290228</v>
+        <v>10290250</v>
       </c>
       <c r="L769" t="n">
-        <v>5659385</v>
+        <v>5659383</v>
       </c>
       <c r="M769" t="n">
         <v>17862</v>
       </c>
       <c r="N769" t="n">
-        <v>892710</v>
+        <v>892709</v>
       </c>
       <c r="O769" t="n">
         <v>411528</v>
@@ -61829,16 +61829,16 @@
         <v>111831</v>
       </c>
       <c r="K770" t="n">
-        <v>10352974</v>
+        <v>10352996</v>
       </c>
       <c r="L770" t="n">
-        <v>5687924</v>
+        <v>5687922</v>
       </c>
       <c r="M770" t="n">
         <v>18016</v>
       </c>
       <c r="N770" t="n">
-        <v>795138</v>
+        <v>795137</v>
       </c>
       <c r="O770" t="n">
         <v>384741</v>
@@ -61909,10 +61909,10 @@
         <v>112306</v>
       </c>
       <c r="K771" t="n">
-        <v>10396178</v>
+        <v>10396200</v>
       </c>
       <c r="L771" t="n">
-        <v>5709635</v>
+        <v>5709633</v>
       </c>
       <c r="M771" t="n">
         <v>18104</v>
@@ -61989,10 +61989,10 @@
         <v>112550</v>
       </c>
       <c r="K772" t="n">
-        <v>10438340</v>
+        <v>10438362</v>
       </c>
       <c r="L772" t="n">
-        <v>5729790</v>
+        <v>5729788</v>
       </c>
       <c r="M772" t="n">
         <v>18194</v>
@@ -62069,10 +62069,10 @@
         <v>112757</v>
       </c>
       <c r="K773" t="n">
-        <v>10482893</v>
+        <v>10482915</v>
       </c>
       <c r="L773" t="n">
-        <v>5746582</v>
+        <v>5746580</v>
       </c>
       <c r="M773" t="n">
         <v>18284</v>
@@ -62149,10 +62149,10 @@
         <v>112973</v>
       </c>
       <c r="K774" t="n">
-        <v>10520142</v>
+        <v>10520164</v>
       </c>
       <c r="L774" t="n">
-        <v>5763011</v>
+        <v>5763009</v>
       </c>
       <c r="M774" t="n">
         <v>18316</v>
@@ -62229,10 +62229,10 @@
         <v>113067</v>
       </c>
       <c r="K775" t="n">
-        <v>10532088</v>
+        <v>10532110</v>
       </c>
       <c r="L775" t="n">
-        <v>5770492</v>
+        <v>5770490</v>
       </c>
       <c r="M775" t="n">
         <v>18348</v>
@@ -62309,10 +62309,10 @@
         <v>113207</v>
       </c>
       <c r="K776" t="n">
-        <v>10551993</v>
+        <v>10552015</v>
       </c>
       <c r="L776" t="n">
-        <v>5777876</v>
+        <v>5777874</v>
       </c>
       <c r="M776" t="n">
         <v>18427</v>
@@ -62389,10 +62389,10 @@
         <v>113416</v>
       </c>
       <c r="K777" t="n">
-        <v>10594525</v>
+        <v>10594547</v>
       </c>
       <c r="L777" t="n">
-        <v>5795036</v>
+        <v>5795034</v>
       </c>
       <c r="M777" t="n">
         <v>18553</v>
@@ -62469,10 +62469,10 @@
         <v>113811</v>
       </c>
       <c r="K778" t="n">
-        <v>10624260</v>
+        <v>10624282</v>
       </c>
       <c r="L778" t="n">
-        <v>5809391</v>
+        <v>5809389</v>
       </c>
       <c r="M778" t="n">
         <v>18626</v>
@@ -62549,10 +62549,10 @@
         <v>114031</v>
       </c>
       <c r="K779" t="n">
-        <v>10652932</v>
+        <v>10652954</v>
       </c>
       <c r="L779" t="n">
-        <v>5823007</v>
+        <v>5823005</v>
       </c>
       <c r="M779" t="n">
         <v>18798</v>
@@ -62629,10 +62629,10 @@
         <v>114200</v>
       </c>
       <c r="K780" t="n">
-        <v>10680260</v>
+        <v>10680282</v>
       </c>
       <c r="L780" t="n">
-        <v>5835250</v>
+        <v>5835248</v>
       </c>
       <c r="M780" t="n">
         <v>18954</v>
@@ -62709,10 +62709,10 @@
         <v>114316</v>
       </c>
       <c r="K781" t="n">
-        <v>10704221</v>
+        <v>10704243</v>
       </c>
       <c r="L781" t="n">
-        <v>5846220</v>
+        <v>5846218</v>
       </c>
       <c r="M781" t="n">
         <v>19068</v>
@@ -62789,10 +62789,10 @@
         <v>114382</v>
       </c>
       <c r="K782" t="n">
-        <v>10712830</v>
+        <v>10712852</v>
       </c>
       <c r="L782" t="n">
-        <v>5851848</v>
+        <v>5851846</v>
       </c>
       <c r="M782" t="n">
         <v>19145</v>
@@ -62869,10 +62869,10 @@
         <v>114472</v>
       </c>
       <c r="K783" t="n">
-        <v>10726765</v>
+        <v>10726787</v>
       </c>
       <c r="L783" t="n">
-        <v>5857505</v>
+        <v>5857503</v>
       </c>
       <c r="M783" t="n">
         <v>0</v>
@@ -62949,10 +62949,10 @@
         <v>114596</v>
       </c>
       <c r="K784" t="n">
-        <v>10756716</v>
+        <v>10756738</v>
       </c>
       <c r="L784" t="n">
-        <v>5870654</v>
+        <v>5870652</v>
       </c>
       <c r="M784" t="n">
         <v>19284</v>
@@ -63029,10 +63029,10 @@
         <v>114854</v>
       </c>
       <c r="K785" t="n">
-        <v>10778384</v>
+        <v>10778406</v>
       </c>
       <c r="L785" t="n">
-        <v>5882019</v>
+        <v>5882017</v>
       </c>
       <c r="M785" t="n">
         <v>19350</v>
@@ -63109,10 +63109,10 @@
         <v>114966</v>
       </c>
       <c r="K786" t="n">
-        <v>10802575</v>
+        <v>10802597</v>
       </c>
       <c r="L786" t="n">
-        <v>5893295</v>
+        <v>5893293</v>
       </c>
       <c r="M786" t="n">
         <v>19370</v>
@@ -63189,10 +63189,10 @@
         <v>115079</v>
       </c>
       <c r="K787" t="n">
-        <v>10825984</v>
+        <v>10826006</v>
       </c>
       <c r="L787" t="n">
-        <v>5902913</v>
+        <v>5902911</v>
       </c>
       <c r="M787" t="n">
         <v>19395</v>
@@ -63269,10 +63269,10 @@
         <v>115200</v>
       </c>
       <c r="K788" t="n">
-        <v>10843487</v>
+        <v>10843509</v>
       </c>
       <c r="L788" t="n">
-        <v>5911519</v>
+        <v>5911517</v>
       </c>
       <c r="M788" t="n">
         <v>19460</v>
@@ -63349,10 +63349,10 @@
         <v>115255</v>
       </c>
       <c r="K789" t="n">
-        <v>10850217</v>
+        <v>10850239</v>
       </c>
       <c r="L789" t="n">
-        <v>5916003</v>
+        <v>5916001</v>
       </c>
       <c r="M789" t="n">
         <v>19460</v>
@@ -63429,10 +63429,10 @@
         <v>115314</v>
       </c>
       <c r="K790" t="n">
-        <v>10860070</v>
+        <v>10860092</v>
       </c>
       <c r="L790" t="n">
-        <v>5919912</v>
+        <v>5919910</v>
       </c>
       <c r="M790" t="n">
         <v>19471</v>
@@ -63509,10 +63509,10 @@
         <v>115413</v>
       </c>
       <c r="K791" t="n">
-        <v>10882664</v>
+        <v>10882686</v>
       </c>
       <c r="L791" t="n">
-        <v>5930947</v>
+        <v>5930945</v>
       </c>
       <c r="M791" t="n">
         <v>19515</v>
@@ -63589,10 +63589,10 @@
         <v>115644</v>
       </c>
       <c r="K792" t="n">
-        <v>10898703</v>
+        <v>10898725</v>
       </c>
       <c r="L792" t="n">
-        <v>5939899</v>
+        <v>5939897</v>
       </c>
       <c r="M792" t="n">
         <v>19545</v>
@@ -63669,10 +63669,10 @@
         <v>115717</v>
       </c>
       <c r="K793" t="n">
-        <v>10916788</v>
+        <v>10916810</v>
       </c>
       <c r="L793" t="n">
-        <v>5950687</v>
+        <v>5950685</v>
       </c>
       <c r="M793" t="n">
         <v>19608</v>
@@ -63749,10 +63749,10 @@
         <v>115820</v>
       </c>
       <c r="K794" t="n">
-        <v>10935882</v>
+        <v>10935904</v>
       </c>
       <c r="L794" t="n">
-        <v>5960599</v>
+        <v>5960597</v>
       </c>
       <c r="M794" t="n">
         <v>19632</v>
@@ -63829,10 +63829,10 @@
         <v>115908</v>
       </c>
       <c r="K795" t="n">
-        <v>10953471</v>
+        <v>10953493</v>
       </c>
       <c r="L795" t="n">
-        <v>5969527</v>
+        <v>5969525</v>
       </c>
       <c r="M795" t="n">
         <v>19702</v>
@@ -63909,10 +63909,10 @@
         <v>115935</v>
       </c>
       <c r="K796" t="n">
-        <v>10961260</v>
+        <v>10961282</v>
       </c>
       <c r="L796" t="n">
-        <v>5973992</v>
+        <v>5973990</v>
       </c>
       <c r="M796" t="n">
         <v>19702</v>
@@ -63989,10 +63989,10 @@
         <v>116008</v>
       </c>
       <c r="K797" t="n">
-        <v>10971499</v>
+        <v>10971521</v>
       </c>
       <c r="L797" t="n">
-        <v>5978430</v>
+        <v>5978428</v>
       </c>
       <c r="M797" t="n">
         <v>19748</v>
@@ -64069,10 +64069,10 @@
         <v>116105</v>
       </c>
       <c r="K798" t="n">
-        <v>10993857</v>
+        <v>10993879</v>
       </c>
       <c r="L798" t="n">
-        <v>5988629</v>
+        <v>5988627</v>
       </c>
       <c r="M798" t="n">
         <v>19763</v>
@@ -64149,10 +64149,10 @@
         <v>116341</v>
       </c>
       <c r="K799" t="n">
-        <v>11010822</v>
+        <v>11010844</v>
       </c>
       <c r="L799" t="n">
-        <v>5997829</v>
+        <v>5997827</v>
       </c>
       <c r="M799" t="n">
         <v>19816</v>
@@ -64229,10 +64229,10 @@
         <v>116413</v>
       </c>
       <c r="K800" t="n">
-        <v>11029562</v>
+        <v>11029584</v>
       </c>
       <c r="L800" t="n">
-        <v>6007175</v>
+        <v>6007173</v>
       </c>
       <c r="M800" t="n">
         <v>19879</v>
@@ -64309,10 +64309,10 @@
         <v>116480</v>
       </c>
       <c r="K801" t="n">
-        <v>11047395</v>
+        <v>11047417</v>
       </c>
       <c r="L801" t="n">
-        <v>6015932</v>
+        <v>6015930</v>
       </c>
       <c r="M801" t="n">
         <v>19892</v>
@@ -64389,10 +64389,10 @@
         <v>116551</v>
       </c>
       <c r="K802" t="n">
-        <v>11062826</v>
+        <v>11062848</v>
       </c>
       <c r="L802" t="n">
-        <v>6022923</v>
+        <v>6022921</v>
       </c>
       <c r="M802" t="n">
         <v>19906</v>
@@ -64469,10 +64469,10 @@
         <v>116581</v>
       </c>
       <c r="K803" t="n">
-        <v>11071394</v>
+        <v>11071416</v>
       </c>
       <c r="L803" t="n">
-        <v>6027043</v>
+        <v>6027041</v>
       </c>
       <c r="M803" t="n">
         <v>19908</v>
@@ -64549,10 +64549,10 @@
         <v>116600</v>
       </c>
       <c r="K804" t="n">
-        <v>11078432</v>
+        <v>11078454</v>
       </c>
       <c r="L804" t="n">
-        <v>6030718</v>
+        <v>6030716</v>
       </c>
       <c r="M804" t="n">
         <v>19915</v>
@@ -64629,10 +64629,10 @@
         <v>116661</v>
       </c>
       <c r="K805" t="n">
-        <v>11094272</v>
+        <v>11094294</v>
       </c>
       <c r="L805" t="n">
-        <v>6039987</v>
+        <v>6039985</v>
       </c>
       <c r="M805" t="n">
         <v>19936</v>
@@ -64709,10 +64709,10 @@
         <v>116863</v>
       </c>
       <c r="K806" t="n">
-        <v>11115601</v>
+        <v>11115623</v>
       </c>
       <c r="L806" t="n">
-        <v>6048068</v>
+        <v>6048066</v>
       </c>
       <c r="M806" t="n">
         <v>19953</v>
@@ -64789,10 +64789,10 @@
         <v>116909</v>
       </c>
       <c r="K807" t="n">
-        <v>11129608</v>
+        <v>11129630</v>
       </c>
       <c r="L807" t="n">
-        <v>6055352</v>
+        <v>6055350</v>
       </c>
       <c r="M807" t="n">
         <v>19966</v>
@@ -64869,10 +64869,10 @@
         <v>117015</v>
       </c>
       <c r="K808" t="n">
-        <v>9523240</v>
+        <v>9523262</v>
       </c>
       <c r="L808" t="n">
-        <v>6063245</v>
+        <v>6063243</v>
       </c>
       <c r="M808" t="n">
         <v>19988</v>
@@ -64949,10 +64949,10 @@
         <v>117075</v>
       </c>
       <c r="K809" t="n">
-        <v>9543328</v>
+        <v>9543350</v>
       </c>
       <c r="L809" t="n">
-        <v>6071442</v>
+        <v>6071440</v>
       </c>
       <c r="M809" t="n">
         <v>20016</v>
@@ -65029,10 +65029,10 @@
         <v>117110</v>
       </c>
       <c r="K810" t="n">
-        <v>9550576</v>
+        <v>9550598</v>
       </c>
       <c r="L810" t="n">
-        <v>6075506</v>
+        <v>6075504</v>
       </c>
       <c r="M810" t="n">
         <v>20016</v>
@@ -65109,10 +65109,10 @@
         <v>117132</v>
       </c>
       <c r="K811" t="n">
-        <v>9557864</v>
+        <v>9557886</v>
       </c>
       <c r="L811" t="n">
-        <v>6078949</v>
+        <v>6078947</v>
       </c>
       <c r="M811" t="n">
         <v>20027</v>
@@ -65189,10 +65189,10 @@
         <v>117177</v>
       </c>
       <c r="K812" t="n">
-        <v>9573348</v>
+        <v>9573370</v>
       </c>
       <c r="L812" t="n">
-        <v>6086971</v>
+        <v>6086969</v>
       </c>
       <c r="M812" t="n">
         <v>20049</v>
@@ -65269,10 +65269,10 @@
         <v>117237</v>
       </c>
       <c r="K813" t="n">
-        <v>9593872</v>
+        <v>9593894</v>
       </c>
       <c r="L813" t="n">
-        <v>6095844</v>
+        <v>6095842</v>
       </c>
       <c r="M813" t="n">
         <v>20062</v>
@@ -65349,10 +65349,10 @@
         <v>117296</v>
       </c>
       <c r="K814" t="n">
-        <v>9607081</v>
+        <v>9607103</v>
       </c>
       <c r="L814" t="n">
-        <v>4483104</v>
+        <v>4483102</v>
       </c>
       <c r="M814" t="n">
         <v>20075</v>
@@ -65429,10 +65429,10 @@
         <v>117475</v>
       </c>
       <c r="K815" t="n">
-        <v>9621502</v>
+        <v>9621524</v>
       </c>
       <c r="L815" t="n">
-        <v>4488674</v>
+        <v>4488672</v>
       </c>
       <c r="M815" t="n">
         <v>20094</v>
@@ -65509,10 +65509,10 @@
         <v>117542</v>
       </c>
       <c r="K816" t="n">
-        <v>9650151</v>
+        <v>9650173</v>
       </c>
       <c r="L816" t="n">
-        <v>4496565</v>
+        <v>4496563</v>
       </c>
       <c r="M816" t="n">
         <v>0</v>
@@ -65589,10 +65589,10 @@
         <v>117565</v>
       </c>
       <c r="K817" t="n">
-        <v>9657231</v>
+        <v>9657253</v>
       </c>
       <c r="L817" t="n">
-        <v>4499720</v>
+        <v>4499718</v>
       </c>
       <c r="M817" t="n">
         <v>0</v>
@@ -65669,10 +65669,10 @@
         <v>117583</v>
       </c>
       <c r="K818" t="n">
-        <v>9662343</v>
+        <v>9662365</v>
       </c>
       <c r="L818" t="n">
-        <v>4502025</v>
+        <v>4502023</v>
       </c>
       <c r="M818" t="n">
         <v>0</v>
@@ -65749,10 +65749,10 @@
         <v>117601</v>
       </c>
       <c r="K819" t="n">
-        <v>9670737</v>
+        <v>9670759</v>
       </c>
       <c r="L819" t="n">
-        <v>4506768</v>
+        <v>4506766</v>
       </c>
       <c r="M819" t="n">
         <v>0</v>
@@ -65829,10 +65829,10 @@
         <v>117660</v>
       </c>
       <c r="K820" t="n">
-        <v>9692192</v>
+        <v>9692214</v>
       </c>
       <c r="L820" t="n">
-        <v>4510003</v>
+        <v>4510001</v>
       </c>
       <c r="M820" t="n">
         <v>0</v>
@@ -65909,10 +65909,10 @@
         <v>117712</v>
       </c>
       <c r="K821" t="n">
-        <v>9699388</v>
+        <v>9699410</v>
       </c>
       <c r="L821" t="n">
-        <v>4513596</v>
+        <v>4513594</v>
       </c>
       <c r="M821" t="n">
         <v>0</v>
@@ -65989,10 +65989,10 @@
         <v>117840</v>
       </c>
       <c r="K822" t="n">
-        <v>9703538</v>
+        <v>9703560</v>
       </c>
       <c r="L822" t="n">
-        <v>4516028</v>
+        <v>4516026</v>
       </c>
       <c r="M822" t="n">
         <v>0</v>
@@ -66069,10 +66069,10 @@
         <v>117922</v>
       </c>
       <c r="K823" t="n">
-        <v>9236109</v>
+        <v>9236131</v>
       </c>
       <c r="L823" t="n">
-        <v>4518685</v>
+        <v>4518683</v>
       </c>
       <c r="M823" t="n">
         <v>0</v>
@@ -66149,10 +66149,10 @@
         <v>117941</v>
       </c>
       <c r="K824" t="n">
-        <v>9238738</v>
+        <v>9238760</v>
       </c>
       <c r="L824" t="n">
-        <v>4520407</v>
+        <v>4520405</v>
       </c>
       <c r="M824" t="n">
         <v>0</v>
@@ -66229,10 +66229,10 @@
         <v>117970</v>
       </c>
       <c r="K825" t="n">
-        <v>9242475</v>
+        <v>9242497</v>
       </c>
       <c r="L825" t="n">
-        <v>4521663</v>
+        <v>4521661</v>
       </c>
       <c r="M825" t="n">
         <v>0</v>
@@ -66309,10 +66309,10 @@
         <v>117998</v>
       </c>
       <c r="K826" t="n">
-        <v>9247569</v>
+        <v>9247591</v>
       </c>
       <c r="L826" t="n">
-        <v>4524794</v>
+        <v>4524792</v>
       </c>
       <c r="M826" t="n">
         <v>0</v>
@@ -66389,10 +66389,10 @@
         <v>118073</v>
       </c>
       <c r="K827" t="n">
-        <v>9261963</v>
+        <v>9261985</v>
       </c>
       <c r="L827" t="n">
-        <v>4528055</v>
+        <v>4528053</v>
       </c>
       <c r="M827" t="n">
         <v>0</v>
@@ -66469,10 +66469,10 @@
         <v>118106</v>
       </c>
       <c r="K828" t="n">
-        <v>9275439</v>
+        <v>9275461</v>
       </c>
       <c r="L828" t="n">
-        <v>4531004</v>
+        <v>4531002</v>
       </c>
       <c r="M828" t="n">
         <v>0</v>
@@ -66549,10 +66549,10 @@
         <v>118243</v>
       </c>
       <c r="K829" t="n">
-        <v>9280667</v>
+        <v>9280689</v>
       </c>
       <c r="L829" t="n">
-        <v>4049899</v>
+        <v>4049897</v>
       </c>
       <c r="M829" t="n">
         <v>0</v>
@@ -66629,10 +66629,10 @@
         <v>118312</v>
       </c>
       <c r="K830" t="n">
-        <v>9296856</v>
+        <v>9296878</v>
       </c>
       <c r="L830" t="n">
-        <v>4054256</v>
+        <v>4054254</v>
       </c>
       <c r="M830" t="n">
         <v>0</v>
@@ -66709,10 +66709,10 @@
         <v>118331</v>
       </c>
       <c r="K831" t="n">
-        <v>9299498</v>
+        <v>9299520</v>
       </c>
       <c r="L831" t="n">
-        <v>4056399</v>
+        <v>4056397</v>
       </c>
       <c r="M831" t="n">
         <v>0</v>
@@ -66789,10 +66789,10 @@
         <v>118372</v>
       </c>
       <c r="K832" t="n">
-        <v>8971965</v>
+        <v>8971987</v>
       </c>
       <c r="L832" t="n">
-        <v>3724823</v>
+        <v>3724821</v>
       </c>
       <c r="M832" t="n">
         <v>0</v>
@@ -66869,10 +66869,10 @@
         <v>118393</v>
       </c>
       <c r="K833" t="n">
-        <v>8977960</v>
+        <v>8977982</v>
       </c>
       <c r="L833" t="n">
-        <v>3727978</v>
+        <v>3727976</v>
       </c>
       <c r="M833" t="n">
         <v>0</v>
@@ -66949,10 +66949,10 @@
         <v>118562</v>
       </c>
       <c r="K834" t="n">
-        <v>8862435</v>
+        <v>8862457</v>
       </c>
       <c r="L834" t="n">
-        <v>3603063</v>
+        <v>3603061</v>
       </c>
       <c r="M834" t="n">
         <v>0</v>
@@ -67029,10 +67029,10 @@
         <v>118588</v>
       </c>
       <c r="K835" t="n">
-        <v>8868898</v>
+        <v>8868920</v>
       </c>
       <c r="L835" t="n">
-        <v>3606709</v>
+        <v>3606707</v>
       </c>
       <c r="M835" t="n">
         <v>0</v>
@@ -67109,10 +67109,10 @@
         <v>118605</v>
       </c>
       <c r="K836" t="n">
-        <v>8872733</v>
+        <v>8872755</v>
       </c>
       <c r="L836" t="n">
-        <v>3609959</v>
+        <v>3609957</v>
       </c>
       <c r="M836" t="n">
         <v>0</v>
@@ -67189,10 +67189,10 @@
         <v>118631</v>
       </c>
       <c r="K837" t="n">
-        <v>8875142</v>
+        <v>8875164</v>
       </c>
       <c r="L837" t="n">
-        <v>3611704</v>
+        <v>3611702</v>
       </c>
       <c r="M837" t="n">
         <v>0</v>
@@ -67269,10 +67269,10 @@
         <v>118660</v>
       </c>
       <c r="K838" t="n">
-        <v>8882481</v>
+        <v>8882503</v>
       </c>
       <c r="L838" t="n">
-        <v>3613666</v>
+        <v>3613664</v>
       </c>
       <c r="M838" t="n">
         <v>0</v>
@@ -67349,10 +67349,10 @@
         <v>118703</v>
       </c>
       <c r="K839" t="n">
-        <v>8891027</v>
+        <v>8891049</v>
       </c>
       <c r="L839" t="n">
-        <v>3615882</v>
+        <v>3615880</v>
       </c>
       <c r="M839" t="n">
         <v>0</v>
@@ -67429,10 +67429,10 @@
         <v>118728</v>
       </c>
       <c r="K840" t="n">
-        <v>8896611</v>
+        <v>8896633</v>
       </c>
       <c r="L840" t="n">
-        <v>3618957</v>
+        <v>3618955</v>
       </c>
       <c r="M840" t="n">
         <v>0</v>
@@ -67509,10 +67509,10 @@
         <v>118824</v>
       </c>
       <c r="K841" t="n">
-        <v>8922326</v>
+        <v>8922348</v>
       </c>
       <c r="L841" t="n">
-        <v>3626009</v>
+        <v>3626007</v>
       </c>
       <c r="M841" t="n">
         <v>0</v>
@@ -67589,10 +67589,10 @@
         <v>118874</v>
       </c>
       <c r="K842" t="n">
-        <v>8933183</v>
+        <v>8933205</v>
       </c>
       <c r="L842" t="n">
-        <v>3629846</v>
+        <v>3629844</v>
       </c>
       <c r="M842" t="n">
         <v>0</v>
@@ -67669,10 +67669,10 @@
         <v>119043</v>
       </c>
       <c r="K843" t="n">
-        <v>8940629</v>
+        <v>8940651</v>
       </c>
       <c r="L843" t="n">
-        <v>3633367</v>
+        <v>3633365</v>
       </c>
       <c r="M843" t="n">
         <v>0</v>
@@ -67749,10 +67749,10 @@
         <v>119127</v>
       </c>
       <c r="K844" t="n">
-        <v>8962623</v>
+        <v>8962645</v>
       </c>
       <c r="L844" t="n">
-        <v>3638858</v>
+        <v>3638856</v>
       </c>
       <c r="M844" t="n">
         <v>0</v>
@@ -67802,13 +67802,13 @@
         <v>44674</v>
       </c>
       <c r="B845" t="n">
-        <v>2572</v>
+        <v>2573</v>
       </c>
       <c r="C845" t="n">
         <v>436</v>
       </c>
       <c r="D845" t="n">
-        <v>6034523</v>
+        <v>6034524</v>
       </c>
       <c r="E845" t="n">
         <v>6581</v>
@@ -67817,7 +67817,7 @@
         <v>4572</v>
       </c>
       <c r="G845" t="n">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H845" t="n">
         <v>17217</v>
@@ -67829,19 +67829,19 @@
         <v>119148</v>
       </c>
       <c r="K845" t="n">
-        <v>8966018</v>
+        <v>8966041</v>
       </c>
       <c r="L845" t="n">
-        <v>3641605</v>
+        <v>3641603</v>
       </c>
       <c r="M845" t="n">
         <v>0</v>
       </c>
       <c r="N845" t="n">
-        <v>-333480</v>
+        <v>-333479</v>
       </c>
       <c r="O845" t="n">
-        <v>83537</v>
+        <v>83538</v>
       </c>
       <c r="P845" t="n">
         <v>-414794</v>
@@ -67850,10 +67850,10 @@
         <v>27939</v>
       </c>
       <c r="R845" t="n">
-        <v>3395</v>
+        <v>3396</v>
       </c>
       <c r="S845" t="n">
-        <v>11933.9</v>
+        <v>11934</v>
       </c>
       <c r="T845" t="n">
         <v>2747</v>
@@ -67909,19 +67909,19 @@
         <v>119206</v>
       </c>
       <c r="K846" t="n">
-        <v>8973150</v>
+        <v>8973173</v>
       </c>
       <c r="L846" t="n">
-        <v>3643437</v>
+        <v>3643435</v>
       </c>
       <c r="M846" t="n">
         <v>0</v>
       </c>
       <c r="N846" t="n">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="O846" t="n">
-        <v>82123</v>
+        <v>82124</v>
       </c>
       <c r="P846" t="n">
         <v>-81386</v>
@@ -67933,7 +67933,7 @@
         <v>7132</v>
       </c>
       <c r="S846" t="n">
-        <v>11731.9</v>
+        <v>11732</v>
       </c>
       <c r="T846" t="n">
         <v>1832</v>
@@ -67989,19 +67989,19 @@
         <v>119235</v>
       </c>
       <c r="K847" t="n">
-        <v>8981119</v>
+        <v>8981142</v>
       </c>
       <c r="L847" t="n">
-        <v>3646980</v>
+        <v>3646978</v>
       </c>
       <c r="M847" t="n">
         <v>0</v>
       </c>
       <c r="N847" t="n">
-        <v>3159</v>
+        <v>3160</v>
       </c>
       <c r="O847" t="n">
-        <v>84508</v>
+        <v>84509</v>
       </c>
       <c r="P847" t="n">
         <v>-80998</v>
@@ -68013,7 +68013,7 @@
         <v>7969</v>
       </c>
       <c r="S847" t="n">
-        <v>12072.6</v>
+        <v>12072.7</v>
       </c>
       <c r="T847" t="n">
         <v>3543</v>
@@ -68069,19 +68069,19 @@
         <v>119314</v>
       </c>
       <c r="K848" t="n">
-        <v>9003177</v>
+        <v>9003200</v>
       </c>
       <c r="L848" t="n">
-        <v>3653324</v>
+        <v>3653322</v>
       </c>
       <c r="M848" t="n">
         <v>0</v>
       </c>
       <c r="N848" t="n">
-        <v>140742</v>
+        <v>140743</v>
       </c>
       <c r="O848" t="n">
-        <v>80851</v>
+        <v>80852</v>
       </c>
       <c r="P848" t="n">
         <v>50261</v>
@@ -68093,7 +68093,7 @@
         <v>22058</v>
       </c>
       <c r="S848" t="n">
-        <v>11550.1</v>
+        <v>11550.3</v>
       </c>
       <c r="T848" t="n">
         <v>6344</v>
@@ -68149,19 +68149,19 @@
         <v>119384</v>
       </c>
       <c r="K849" t="n">
-        <v>9015247</v>
+        <v>9015270</v>
       </c>
       <c r="L849" t="n">
-        <v>3658040</v>
+        <v>3658038</v>
       </c>
       <c r="M849" t="n">
         <v>0</v>
       </c>
       <c r="N849" t="n">
-        <v>146349</v>
+        <v>146350</v>
       </c>
       <c r="O849" t="n">
-        <v>82064</v>
+        <v>82065</v>
       </c>
       <c r="P849" t="n">
         <v>51331</v>
@@ -68173,7 +68173,7 @@
         <v>12070</v>
       </c>
       <c r="S849" t="n">
-        <v>11723.4</v>
+        <v>11723.6</v>
       </c>
       <c r="T849" t="n">
         <v>4716</v>
@@ -68229,19 +68229,19 @@
         <v>119539</v>
       </c>
       <c r="K850" t="n">
-        <v>9024121</v>
+        <v>9024144</v>
       </c>
       <c r="L850" t="n">
-        <v>3662552</v>
+        <v>3662550</v>
       </c>
       <c r="M850" t="n">
         <v>0</v>
       </c>
       <c r="N850" t="n">
-        <v>151388</v>
+        <v>151389</v>
       </c>
       <c r="O850" t="n">
-        <v>83492</v>
+        <v>83493</v>
       </c>
       <c r="P850" t="n">
         <v>52593</v>
@@ -68253,7 +68253,7 @@
         <v>8874</v>
       </c>
       <c r="S850" t="n">
-        <v>11927.4</v>
+        <v>11927.6</v>
       </c>
       <c r="T850" t="n">
         <v>4512</v>
@@ -68309,19 +68309,19 @@
         <v>119644</v>
       </c>
       <c r="K851" t="n">
-        <v>9047819</v>
+        <v>9047842</v>
       </c>
       <c r="L851" t="n">
-        <v>3669514</v>
+        <v>3669512</v>
       </c>
       <c r="M851" t="n">
         <v>0</v>
       </c>
       <c r="N851" t="n">
-        <v>172677</v>
+        <v>172678</v>
       </c>
       <c r="O851" t="n">
-        <v>85196</v>
+        <v>85197</v>
       </c>
       <c r="P851" t="n">
         <v>57810</v>
@@ -68333,7 +68333,7 @@
         <v>23698</v>
       </c>
       <c r="S851" t="n">
-        <v>12170.9</v>
+        <v>12171</v>
       </c>
       <c r="T851" t="n">
         <v>6962</v>
@@ -68389,16 +68389,16 @@
         <v>119669</v>
       </c>
       <c r="K852" t="n">
-        <v>9051779</v>
+        <v>9051802</v>
       </c>
       <c r="L852" t="n">
-        <v>3672775</v>
+        <v>3672773</v>
       </c>
       <c r="M852" t="n">
         <v>0</v>
       </c>
       <c r="N852" t="n">
-        <v>169298</v>
+        <v>169299</v>
       </c>
       <c r="O852" t="n">
         <v>85761</v>
@@ -68469,16 +68469,16 @@
         <v>119708</v>
       </c>
       <c r="K853" t="n">
-        <v>9061306</v>
+        <v>9061329</v>
       </c>
       <c r="L853" t="n">
-        <v>3674776</v>
+        <v>3674774</v>
       </c>
       <c r="M853" t="n">
         <v>0</v>
       </c>
       <c r="N853" t="n">
-        <v>170279</v>
+        <v>170280</v>
       </c>
       <c r="O853" t="n">
         <v>88156</v>
@@ -68549,16 +68549,16 @@
         <v>119733</v>
       </c>
       <c r="K854" t="n">
-        <v>9068487</v>
+        <v>9068510</v>
       </c>
       <c r="L854" t="n">
-        <v>3678949</v>
+        <v>3678947</v>
       </c>
       <c r="M854" t="n">
         <v>0</v>
       </c>
       <c r="N854" t="n">
-        <v>171876</v>
+        <v>171877</v>
       </c>
       <c r="O854" t="n">
         <v>87368</v>
@@ -68629,16 +68629,16 @@
         <v>119774</v>
       </c>
       <c r="K855" t="n">
-        <v>9089718</v>
+        <v>9089741</v>
       </c>
       <c r="L855" t="n">
-        <v>3684740</v>
+        <v>3684738</v>
       </c>
       <c r="M855" t="n">
         <v>0</v>
       </c>
       <c r="N855" t="n">
-        <v>167392</v>
+        <v>167393</v>
       </c>
       <c r="O855" t="n">
         <v>86541</v>
@@ -68709,16 +68709,16 @@
         <v>119825</v>
       </c>
       <c r="K856" t="n">
-        <v>9102100</v>
+        <v>9102123</v>
       </c>
       <c r="L856" t="n">
-        <v>3690009</v>
+        <v>3690007</v>
       </c>
       <c r="M856" t="n">
         <v>0</v>
       </c>
       <c r="N856" t="n">
-        <v>168917</v>
+        <v>168918</v>
       </c>
       <c r="O856" t="n">
         <v>86853</v>
@@ -68789,16 +68789,16 @@
         <v>119948</v>
       </c>
       <c r="K857" t="n">
-        <v>9111197</v>
+        <v>9111220</v>
       </c>
       <c r="L857" t="n">
-        <v>3694828</v>
+        <v>3694826</v>
       </c>
       <c r="M857" t="n">
         <v>0</v>
       </c>
       <c r="N857" t="n">
-        <v>170568</v>
+        <v>170569</v>
       </c>
       <c r="O857" t="n">
         <v>87076</v>
@@ -68869,16 +68869,16 @@
         <v>120054</v>
       </c>
       <c r="K858" t="n">
-        <v>9135648</v>
+        <v>9135671</v>
       </c>
       <c r="L858" t="n">
-        <v>3702273</v>
+        <v>3702271</v>
       </c>
       <c r="M858" t="n">
         <v>0</v>
       </c>
       <c r="N858" t="n">
-        <v>173025</v>
+        <v>173026</v>
       </c>
       <c r="O858" t="n">
         <v>87829</v>
@@ -68949,10 +68949,10 @@
         <v>120076</v>
       </c>
       <c r="K859" t="n">
-        <v>9139702</v>
+        <v>9139725</v>
       </c>
       <c r="L859" t="n">
-        <v>3705530</v>
+        <v>3705528</v>
       </c>
       <c r="M859" t="n">
         <v>0</v>
@@ -69029,10 +69029,10 @@
         <v>120108</v>
       </c>
       <c r="K860" t="n">
-        <v>9145334</v>
+        <v>9145357</v>
       </c>
       <c r="L860" t="n">
-        <v>3707551</v>
+        <v>3707549</v>
       </c>
       <c r="M860" t="n">
         <v>0</v>
@@ -69109,10 +69109,10 @@
         <v>120148</v>
       </c>
       <c r="K861" t="n">
-        <v>9155713</v>
+        <v>9155736</v>
       </c>
       <c r="L861" t="n">
-        <v>3711758</v>
+        <v>3711756</v>
       </c>
       <c r="M861" t="n">
         <v>0</v>
@@ -69189,10 +69189,10 @@
         <v>120248</v>
       </c>
       <c r="K862" t="n">
-        <v>9172198</v>
+        <v>9172221</v>
       </c>
       <c r="L862" t="n">
-        <v>3710776</v>
+        <v>3710774</v>
       </c>
       <c r="M862" t="n">
         <v>0</v>
@@ -69269,10 +69269,10 @@
         <v>120310</v>
       </c>
       <c r="K863" t="n">
-        <v>9183154</v>
+        <v>9183177</v>
       </c>
       <c r="L863" t="n">
-        <v>3715343</v>
+        <v>3715341</v>
       </c>
       <c r="M863" t="n">
         <v>0</v>
@@ -69349,10 +69349,10 @@
         <v>120495</v>
       </c>
       <c r="K864" t="n">
-        <v>9190927</v>
+        <v>9190950</v>
       </c>
       <c r="L864" t="n">
-        <v>3719454</v>
+        <v>3719452</v>
       </c>
       <c r="M864" t="n">
         <v>0</v>
@@ -69429,10 +69429,10 @@
         <v>120613</v>
       </c>
       <c r="K865" t="n">
-        <v>9216628</v>
+        <v>9216651</v>
       </c>
       <c r="L865" t="n">
-        <v>3725409</v>
+        <v>3725407</v>
       </c>
       <c r="M865" t="n">
         <v>0</v>
@@ -69509,10 +69509,10 @@
         <v>120644</v>
       </c>
       <c r="K866" t="n">
-        <v>9219764</v>
+        <v>9219787</v>
       </c>
       <c r="L866" t="n">
-        <v>3727834</v>
+        <v>3727832</v>
       </c>
       <c r="M866" t="n">
         <v>0</v>
@@ -69589,10 +69589,10 @@
         <v>120694</v>
       </c>
       <c r="K867" t="n">
-        <v>9226832</v>
+        <v>9226855</v>
       </c>
       <c r="L867" t="n">
-        <v>3729650</v>
+        <v>3729648</v>
       </c>
       <c r="M867" t="n">
         <v>0</v>
@@ -69669,10 +69669,10 @@
         <v>120732</v>
       </c>
       <c r="K868" t="n">
-        <v>9234312</v>
+        <v>9234335</v>
       </c>
       <c r="L868" t="n">
-        <v>3733690</v>
+        <v>3733688</v>
       </c>
       <c r="M868" t="n">
         <v>0</v>
@@ -69749,10 +69749,10 @@
         <v>120840</v>
       </c>
       <c r="K869" t="n">
-        <v>9254984</v>
+        <v>9255007</v>
       </c>
       <c r="L869" t="n">
-        <v>3738628</v>
+        <v>3738626</v>
       </c>
       <c r="M869" t="n">
         <v>0</v>
@@ -69829,10 +69829,10 @@
         <v>120909</v>
       </c>
       <c r="K870" t="n">
-        <v>9262624</v>
+        <v>9262647</v>
       </c>
       <c r="L870" t="n">
-        <v>3742334</v>
+        <v>3742332</v>
       </c>
       <c r="M870" t="n">
         <v>0</v>
@@ -69909,10 +69909,10 @@
         <v>121066</v>
       </c>
       <c r="K871" t="n">
-        <v>9268953</v>
+        <v>9268976</v>
       </c>
       <c r="L871" t="n">
-        <v>3745568</v>
+        <v>3745566</v>
       </c>
       <c r="M871" t="n">
         <v>0</v>
@@ -69989,10 +69989,10 @@
         <v>121174</v>
       </c>
       <c r="K872" t="n">
-        <v>9290647</v>
+        <v>9290670</v>
       </c>
       <c r="L872" t="n">
-        <v>3750370</v>
+        <v>3750368</v>
       </c>
       <c r="M872" t="n">
         <v>0</v>
@@ -70069,10 +70069,10 @@
         <v>121199</v>
       </c>
       <c r="K873" t="n">
-        <v>9292596</v>
+        <v>9292619</v>
       </c>
       <c r="L873" t="n">
-        <v>3751757</v>
+        <v>3751755</v>
       </c>
       <c r="M873" t="n">
         <v>0</v>
@@ -70149,10 +70149,10 @@
         <v>121222</v>
       </c>
       <c r="K874" t="n">
-        <v>9296497</v>
+        <v>9296520</v>
       </c>
       <c r="L874" t="n">
-        <v>3752985</v>
+        <v>3752983</v>
       </c>
       <c r="M874" t="n">
         <v>0</v>
@@ -70229,10 +70229,10 @@
         <v>121251</v>
       </c>
       <c r="K875" t="n">
-        <v>9302130</v>
+        <v>9302153</v>
       </c>
       <c r="L875" t="n">
-        <v>3756579</v>
+        <v>3756577</v>
       </c>
       <c r="M875" t="n">
         <v>0</v>
@@ -70309,10 +70309,10 @@
         <v>121340</v>
       </c>
       <c r="K876" t="n">
-        <v>9320508</v>
+        <v>9320531</v>
       </c>
       <c r="L876" t="n">
-        <v>3760501</v>
+        <v>3760499</v>
       </c>
       <c r="M876" t="n">
         <v>0</v>
@@ -70389,10 +70389,10 @@
         <v>121386</v>
       </c>
       <c r="K877" t="n">
-        <v>9326203</v>
+        <v>9326226</v>
       </c>
       <c r="L877" t="n">
-        <v>3763158</v>
+        <v>3763156</v>
       </c>
       <c r="M877" t="n">
         <v>0</v>
@@ -70469,10 +70469,10 @@
         <v>121562</v>
       </c>
       <c r="K878" t="n">
-        <v>9330184</v>
+        <v>9330207</v>
       </c>
       <c r="L878" t="n">
-        <v>3765513</v>
+        <v>3765511</v>
       </c>
       <c r="M878" t="n">
         <v>0</v>
@@ -70549,10 +70549,10 @@
         <v>121660</v>
       </c>
       <c r="K879" t="n">
-        <v>9344683</v>
+        <v>9344706</v>
       </c>
       <c r="L879" t="n">
-        <v>3769039</v>
+        <v>3769037</v>
       </c>
       <c r="M879" t="n">
         <v>0</v>
@@ -70602,13 +70602,13 @@
         <v>44709</v>
       </c>
       <c r="B880" t="n">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="C880" t="n">
         <v>241</v>
       </c>
       <c r="D880" t="n">
-        <v>6291574</v>
+        <v>6291575</v>
       </c>
       <c r="E880" t="n">
         <v>0</v>
@@ -70617,7 +70617,7 @@
         <v>4835</v>
       </c>
       <c r="G880" t="n">
-        <v>128583</v>
+        <v>128584</v>
       </c>
       <c r="H880" t="n">
         <v>0</v>
@@ -70629,19 +70629,19 @@
         <v>121690</v>
       </c>
       <c r="K880" t="n">
-        <v>9347482</v>
+        <v>9347506</v>
       </c>
       <c r="L880" t="n">
-        <v>3770167</v>
+        <v>3770165</v>
       </c>
       <c r="M880" t="n">
         <v>0</v>
       </c>
       <c r="N880" t="n">
-        <v>127718</v>
+        <v>127719</v>
       </c>
       <c r="O880" t="n">
-        <v>54886</v>
+        <v>54887</v>
       </c>
       <c r="P880" t="n">
         <v>42333</v>
@@ -70650,10 +70650,10 @@
         <v>18410</v>
       </c>
       <c r="R880" t="n">
-        <v>2799</v>
+        <v>2800</v>
       </c>
       <c r="S880" t="n">
-        <v>7840.9</v>
+        <v>7841</v>
       </c>
       <c r="T880" t="n">
         <v>1128</v>
@@ -70682,13 +70682,13 @@
         <v>44710</v>
       </c>
       <c r="B881" t="n">
-        <v>689</v>
+        <v>692</v>
       </c>
       <c r="C881" t="n">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="D881" t="n">
-        <v>6293496</v>
+        <v>6293498</v>
       </c>
       <c r="E881" t="n">
         <v>0</v>
@@ -70697,7 +70697,7 @@
         <v>4956</v>
       </c>
       <c r="G881" t="n">
-        <v>128567</v>
+        <v>128569</v>
       </c>
       <c r="H881" t="n">
         <v>0</v>
@@ -70709,37 +70709,37 @@
         <v>121710</v>
       </c>
       <c r="K881" t="n">
-        <v>9350753</v>
+        <v>9350780</v>
       </c>
       <c r="L881" t="n">
-        <v>3771350</v>
+        <v>3771349</v>
       </c>
       <c r="M881" t="n">
         <v>0</v>
       </c>
       <c r="N881" t="n">
-        <v>123921</v>
+        <v>123925</v>
       </c>
       <c r="O881" t="n">
-        <v>54256</v>
+        <v>54260</v>
       </c>
       <c r="P881" t="n">
-        <v>41700</v>
+        <v>41701</v>
       </c>
       <c r="Q881" t="n">
-        <v>18365</v>
+        <v>18366</v>
       </c>
       <c r="R881" t="n">
-        <v>3271</v>
+        <v>3274</v>
       </c>
       <c r="S881" t="n">
-        <v>7750.9</v>
+        <v>7751.4</v>
       </c>
       <c r="T881" t="n">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="U881" t="n">
-        <v>2623.6</v>
+        <v>2623.7</v>
       </c>
       <c r="V881" t="n">
         <v>20</v>
@@ -70762,13 +70762,13 @@
         <v>44711</v>
       </c>
       <c r="B882" t="n">
-        <v>1641</v>
+        <v>1643</v>
       </c>
       <c r="C882" t="n">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="D882" t="n">
-        <v>6169040</v>
+        <v>6169041</v>
       </c>
       <c r="E882" t="n">
         <v>0</v>
@@ -70777,7 +70777,7 @@
         <v>4893</v>
       </c>
       <c r="G882" t="n">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H882" t="n">
         <v>0</v>
@@ -70789,7 +70789,7 @@
         <v>121729</v>
       </c>
       <c r="K882" t="n">
-        <v>9355622</v>
+        <v>9355651</v>
       </c>
       <c r="L882" t="n">
         <v>3774626</v>
@@ -70798,28 +70798,28 @@
         <v>0</v>
       </c>
       <c r="N882" t="n">
-        <v>121310</v>
+        <v>121316</v>
       </c>
       <c r="O882" t="n">
-        <v>53492</v>
+        <v>53498</v>
       </c>
       <c r="P882" t="n">
-        <v>40936</v>
+        <v>40938</v>
       </c>
       <c r="Q882" t="n">
-        <v>18047</v>
+        <v>18049</v>
       </c>
       <c r="R882" t="n">
-        <v>4869</v>
+        <v>4871</v>
       </c>
       <c r="S882" t="n">
-        <v>7641.7</v>
+        <v>7642.6</v>
       </c>
       <c r="T882" t="n">
-        <v>3276</v>
+        <v>3277</v>
       </c>
       <c r="U882" t="n">
-        <v>2578.1</v>
+        <v>2578.4</v>
       </c>
       <c r="V882" t="n">
         <v>19</v>
@@ -70869,7 +70869,7 @@
         <v>99191</v>
       </c>
       <c r="K883" t="n">
-        <v>9368128</v>
+        <v>9368157</v>
       </c>
       <c r="L883" t="n">
         <v>3777881</v>
@@ -70878,28 +70878,28 @@
         <v>0</v>
       </c>
       <c r="N883" t="n">
-        <v>113144</v>
+        <v>113150</v>
       </c>
       <c r="O883" t="n">
-        <v>47620</v>
+        <v>47626</v>
       </c>
       <c r="P883" t="n">
-        <v>39253</v>
+        <v>39255</v>
       </c>
       <c r="Q883" t="n">
-        <v>17380</v>
+        <v>17382</v>
       </c>
       <c r="R883" t="n">
         <v>12506</v>
       </c>
       <c r="S883" t="n">
-        <v>6802.9</v>
+        <v>6803.7</v>
       </c>
       <c r="T883" t="n">
         <v>3255</v>
       </c>
       <c r="U883" t="n">
-        <v>2482.9</v>
+        <v>2483.1</v>
       </c>
       <c r="V883" t="n">
         <v>-22538</v>
@@ -70922,13 +70922,13 @@
         <v>44713</v>
       </c>
       <c r="B884" t="n">
-        <v>1841</v>
+        <v>1854</v>
       </c>
       <c r="C884" t="n">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D884" t="n">
-        <v>6305358</v>
+        <v>6305370</v>
       </c>
       <c r="E884" t="n">
         <v>0</v>
@@ -70937,7 +70937,7 @@
         <v>12387</v>
       </c>
       <c r="G884" t="n">
-        <v>128712</v>
+        <v>128724</v>
       </c>
       <c r="H884" t="n">
         <v>0</v>
@@ -70949,37 +70949,37 @@
         <v>85249</v>
       </c>
       <c r="K884" t="n">
-        <v>7855927</v>
+        <v>7855969</v>
       </c>
       <c r="L884" t="n">
-        <v>3780305</v>
+        <v>3780306</v>
       </c>
       <c r="M884" t="n">
         <v>0</v>
       </c>
       <c r="N884" t="n">
-        <v>-1406697</v>
+        <v>-1406678</v>
       </c>
       <c r="O884" t="n">
-        <v>-1470276</v>
+        <v>-1470257</v>
       </c>
       <c r="P884" t="n">
-        <v>37971</v>
+        <v>37974</v>
       </c>
       <c r="Q884" t="n">
-        <v>17147</v>
+        <v>17150</v>
       </c>
       <c r="R884" t="n">
-        <v>-1512201</v>
+        <v>-1512188</v>
       </c>
       <c r="S884" t="n">
-        <v>-210039.4</v>
+        <v>-210036.7</v>
       </c>
       <c r="T884" t="n">
-        <v>2424</v>
+        <v>2425</v>
       </c>
       <c r="U884" t="n">
-        <v>2449.6</v>
+        <v>2450</v>
       </c>
       <c r="V884" t="n">
         <v>-13942</v>
@@ -71002,79 +71002,79 @@
         <v>44714</v>
       </c>
       <c r="B885" t="n">
-        <v>1258</v>
+        <v>1423</v>
       </c>
       <c r="C885" t="n">
-        <v>130</v>
+        <v>213</v>
       </c>
       <c r="D885" t="n">
-        <v>6179534</v>
+        <v>6179616</v>
       </c>
       <c r="E885" t="n">
         <v>0</v>
       </c>
       <c r="F885" t="n">
-        <v>3798</v>
+        <v>3912</v>
       </c>
       <c r="G885" t="n">
-        <v>54</v>
+        <v>136</v>
       </c>
       <c r="H885" t="n">
         <v>0</v>
       </c>
       <c r="I885" t="n">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="J885" t="n">
-        <v>80160</v>
+        <v>83001</v>
       </c>
       <c r="K885" t="n">
-        <v>7626158</v>
+        <v>7859418</v>
       </c>
       <c r="L885" t="n">
-        <v>3597665</v>
+        <v>3782241</v>
       </c>
       <c r="M885" t="n">
         <v>0</v>
       </c>
       <c r="N885" t="n">
-        <v>-1642795</v>
+        <v>-1409558</v>
       </c>
       <c r="O885" t="n">
-        <v>-1704026</v>
+        <v>-1470789</v>
       </c>
       <c r="P885" t="n">
-        <v>-147903</v>
+        <v>36675</v>
       </c>
       <c r="Q885" t="n">
-        <v>-167848</v>
+        <v>16730</v>
       </c>
       <c r="R885" t="n">
-        <v>-229769</v>
+        <v>3449</v>
       </c>
       <c r="S885" t="n">
-        <v>-243432.3</v>
+        <v>-210112.7</v>
       </c>
       <c r="T885" t="n">
-        <v>-182640</v>
+        <v>1935</v>
       </c>
       <c r="U885" t="n">
-        <v>-23978.3</v>
+        <v>2390</v>
       </c>
       <c r="V885" t="n">
-        <v>-5089</v>
+        <v>-2248</v>
       </c>
       <c r="W885" t="n">
-        <v>-6</v>
+        <v>-2.6</v>
       </c>
       <c r="X885" t="n">
-        <v>-13856.3</v>
+        <v>-12909.3</v>
       </c>
       <c r="Y885" t="n">
-        <v>-5914.6</v>
+        <v>-5508.7</v>
       </c>
       <c r="Z885" t="n">
-        <v>-41402</v>
+        <v>-38561</v>
       </c>
     </row>
     <row r="886">
@@ -71082,79 +71082,79 @@
         <v>44715</v>
       </c>
       <c r="B886" t="n">
-        <v>4879</v>
+        <v>5036</v>
       </c>
       <c r="C886" t="n">
-        <v>686</v>
+        <v>770</v>
       </c>
       <c r="D886" t="n">
-        <v>6182414</v>
+        <v>6182487</v>
       </c>
       <c r="E886" t="n">
         <v>0</v>
       </c>
       <c r="F886" t="n">
-        <v>2503</v>
+        <v>2826</v>
       </c>
       <c r="G886" t="n">
-        <v>68</v>
+        <v>141</v>
       </c>
       <c r="H886" t="n">
         <v>0</v>
       </c>
       <c r="I886" t="n">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="J886" t="n">
-        <v>50587</v>
+        <v>55747</v>
       </c>
       <c r="K886" t="n">
-        <v>4660418</v>
+        <v>5323616</v>
       </c>
       <c r="L886" t="n">
-        <v>1127476</v>
+        <v>1312136</v>
       </c>
       <c r="M886" t="n">
         <v>0</v>
       </c>
       <c r="N886" t="n">
-        <v>-4630229</v>
+        <v>-3967054</v>
       </c>
       <c r="O886" t="n">
-        <v>-4684265</v>
+        <v>-4021090</v>
       </c>
       <c r="P886" t="n">
-        <v>-2622894</v>
+        <v>-2438232</v>
       </c>
       <c r="Q886" t="n">
-        <v>-2641563</v>
+        <v>-2456901</v>
       </c>
       <c r="R886" t="n">
-        <v>-2965740</v>
+        <v>-2535802</v>
       </c>
       <c r="S886" t="n">
-        <v>-669180.7</v>
+        <v>-574441.4</v>
       </c>
       <c r="T886" t="n">
-        <v>-2470189</v>
+        <v>-2470105</v>
       </c>
       <c r="U886" t="n">
-        <v>-377366.1</v>
+        <v>-350985.9</v>
       </c>
       <c r="V886" t="n">
-        <v>-29573</v>
+        <v>-27254</v>
       </c>
       <c r="W886" t="n">
-        <v>-36.9</v>
+        <v>-32.8</v>
       </c>
       <c r="X886" t="n">
-        <v>-16201.3</v>
+        <v>-14481.3</v>
       </c>
       <c r="Y886" t="n">
-        <v>-10153.3</v>
+        <v>-9416.1</v>
       </c>
       <c r="Z886" t="n">
-        <v>-71073</v>
+        <v>-65913</v>
       </c>
     </row>
     <row r="887">
@@ -71162,79 +71162,79 @@
         <v>44716</v>
       </c>
       <c r="B887" t="n">
-        <v>312</v>
+        <v>664</v>
       </c>
       <c r="C887" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="D887" t="n">
-        <v>6184290</v>
+        <v>6184314</v>
       </c>
       <c r="E887" t="n">
         <v>0</v>
       </c>
       <c r="F887" t="n">
-        <v>343</v>
+        <v>2408</v>
       </c>
       <c r="G887" t="n">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="H887" t="n">
         <v>0</v>
       </c>
       <c r="I887" t="n">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="J887" t="n">
-        <v>6939</v>
+        <v>46936</v>
       </c>
       <c r="K887" t="n">
-        <v>732597</v>
+        <v>4219999</v>
       </c>
       <c r="L887" t="n">
-        <v>0</v>
+        <v>947097</v>
       </c>
       <c r="M887" t="n">
         <v>0</v>
       </c>
       <c r="N887" t="n">
-        <v>-8559999</v>
+        <v>-5072620</v>
       </c>
       <c r="O887" t="n">
-        <v>-8614885</v>
+        <v>-5127507</v>
       </c>
       <c r="P887" t="n">
-        <v>-3751757</v>
+        <v>-2804658</v>
       </c>
       <c r="Q887" t="n">
-        <v>-3770167</v>
+        <v>-2823068</v>
       </c>
       <c r="R887" t="n">
-        <v>-3927821</v>
+        <v>-1103617</v>
       </c>
       <c r="S887" t="n">
-        <v>-1230697.9</v>
+        <v>-732501</v>
       </c>
       <c r="T887" t="n">
-        <v>-1127476</v>
+        <v>-365039</v>
       </c>
       <c r="U887" t="n">
-        <v>-538595.3</v>
+        <v>-403295.4</v>
       </c>
       <c r="V887" t="n">
-        <v>-43648</v>
+        <v>-8811</v>
       </c>
       <c r="W887" t="n">
-        <v>-86.3</v>
+        <v>-15.8</v>
       </c>
       <c r="X887" t="n">
-        <v>-26103.3</v>
+        <v>-12771</v>
       </c>
       <c r="Y887" t="n">
-        <v>-16393</v>
+        <v>-10679.1</v>
       </c>
       <c r="Z887" t="n">
-        <v>-114751</v>
+        <v>-74754</v>
       </c>
     </row>
     <row r="888">
@@ -71242,79 +71242,79 @@
         <v>44717</v>
       </c>
       <c r="B888" t="n">
-        <v>261</v>
+        <v>553</v>
       </c>
       <c r="C888" t="n">
         <v>0</v>
       </c>
       <c r="D888" t="n">
-        <v>6186151</v>
+        <v>6314784</v>
       </c>
       <c r="E888" t="n">
         <v>0</v>
       </c>
       <c r="F888" t="n">
-        <v>369</v>
+        <v>2381</v>
       </c>
       <c r="G888" t="n">
-        <v>39</v>
+        <v>128672</v>
       </c>
       <c r="H888" t="n">
         <v>0</v>
       </c>
       <c r="I888" t="n">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="J888" t="n">
-        <v>6939</v>
+        <v>44101</v>
       </c>
       <c r="K888" t="n">
-        <v>732861</v>
+        <v>3988828</v>
       </c>
       <c r="L888" t="n">
-        <v>0</v>
+        <v>762676</v>
       </c>
       <c r="M888" t="n">
         <v>0</v>
       </c>
       <c r="N888" t="n">
-        <v>-8563636</v>
+        <v>-5307692</v>
       </c>
       <c r="O888" t="n">
-        <v>-8617892</v>
+        <v>-5361952</v>
       </c>
       <c r="P888" t="n">
-        <v>-3752985</v>
+        <v>-2990307</v>
       </c>
       <c r="Q888" t="n">
-        <v>-3771350</v>
+        <v>-3008673</v>
       </c>
       <c r="R888" t="n">
-        <v>264</v>
+        <v>-231171</v>
       </c>
       <c r="S888" t="n">
-        <v>-1231127.4</v>
+        <v>-765993.1</v>
       </c>
       <c r="T888" t="n">
-        <v>0</v>
+        <v>-184421</v>
       </c>
       <c r="U888" t="n">
-        <v>-538764.3</v>
+        <v>-429810.4</v>
       </c>
       <c r="V888" t="n">
-        <v>0</v>
+        <v>-2835</v>
       </c>
       <c r="W888" t="n">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="X888" t="n">
-        <v>-24407</v>
+        <v>-12966.7</v>
       </c>
       <c r="Y888" t="n">
-        <v>-16395.9</v>
+        <v>-11087</v>
       </c>
       <c r="Z888" t="n">
-        <v>-114771</v>
+        <v>-77609</v>
       </c>
     </row>
     <row r="889">
@@ -71322,79 +71322,239 @@
         <v>44718</v>
       </c>
       <c r="B889" t="n">
-        <v>0</v>
+        <v>930</v>
       </c>
       <c r="C889" t="n">
         <v>0</v>
       </c>
       <c r="D889" t="n">
-        <v>0</v>
+        <v>128677</v>
       </c>
       <c r="E889" t="n">
         <v>0</v>
       </c>
       <c r="F889" t="n">
+        <v>2220</v>
+      </c>
+      <c r="G889" t="n">
+        <v>128677</v>
+      </c>
+      <c r="H889" t="n">
+        <v>0</v>
+      </c>
+      <c r="I889" t="n">
+        <v>64</v>
+      </c>
+      <c r="J889" t="n">
+        <v>41771</v>
+      </c>
+      <c r="K889" t="n">
+        <v>3685240</v>
+      </c>
+      <c r="L889" t="n">
+        <v>763322</v>
+      </c>
+      <c r="M889" t="n">
+        <v>0</v>
+      </c>
+      <c r="N889" t="n">
+        <v>-5616913</v>
+      </c>
+      <c r="O889" t="n">
+        <v>-5670411</v>
+      </c>
+      <c r="P889" t="n">
+        <v>-2993255</v>
+      </c>
+      <c r="Q889" t="n">
+        <v>-3011304</v>
+      </c>
+      <c r="R889" t="n">
+        <v>-303588</v>
+      </c>
+      <c r="S889" t="n">
+        <v>-810058.7</v>
+      </c>
+      <c r="T889" t="n">
+        <v>646</v>
+      </c>
+      <c r="U889" t="n">
+        <v>-430186.3</v>
+      </c>
+      <c r="V889" t="n">
+        <v>-2330</v>
+      </c>
+      <c r="W889" t="n">
+        <v>-5.3</v>
+      </c>
+      <c r="X889" t="n">
+        <v>-4658.7</v>
+      </c>
+      <c r="Y889" t="n">
+        <v>-11422.6</v>
+      </c>
+      <c r="Z889" t="n">
+        <v>-79958</v>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" s="1" t="n">
+        <v>44719</v>
+      </c>
+      <c r="B890" t="n">
+        <v>3802</v>
+      </c>
+      <c r="C890" t="n">
+        <v>0</v>
+      </c>
+      <c r="D890" t="n">
+        <v>0</v>
+      </c>
+      <c r="E890" t="n">
+        <v>0</v>
+      </c>
+      <c r="F890" t="n">
+        <v>1763</v>
+      </c>
+      <c r="G890" t="n">
+        <v>0</v>
+      </c>
+      <c r="H890" t="n">
+        <v>0</v>
+      </c>
+      <c r="I890" t="n">
+        <v>71</v>
+      </c>
+      <c r="J890" t="n">
+        <v>38257</v>
+      </c>
+      <c r="K890" t="n">
+        <v>2640470</v>
+      </c>
+      <c r="L890" t="n">
+        <v>764120</v>
+      </c>
+      <c r="M890" t="n">
+        <v>0</v>
+      </c>
+      <c r="N890" t="n">
+        <v>-6680061</v>
+      </c>
+      <c r="O890" t="n">
+        <v>-6727687</v>
+      </c>
+      <c r="P890" t="n">
+        <v>-2996379</v>
+      </c>
+      <c r="Q890" t="n">
+        <v>-3013761</v>
+      </c>
+      <c r="R890" t="n">
+        <v>-1044770</v>
+      </c>
+      <c r="S890" t="n">
+        <v>-961098.1</v>
+      </c>
+      <c r="T890" t="n">
+        <v>798</v>
+      </c>
+      <c r="U890" t="n">
+        <v>-430537.3</v>
+      </c>
+      <c r="V890" t="n">
+        <v>-3514</v>
+      </c>
+      <c r="W890" t="n">
+        <v>-8.4</v>
+      </c>
+      <c r="X890" t="n">
+        <v>-2893</v>
+      </c>
+      <c r="Y890" t="n">
+        <v>-8704.9</v>
+      </c>
+      <c r="Z890" t="n">
+        <v>-60934</v>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" s="1" t="n">
+        <v>44720</v>
+      </c>
+      <c r="B891" t="n">
+        <v>0</v>
+      </c>
+      <c r="C891" t="n">
+        <v>0</v>
+      </c>
+      <c r="D891" t="n">
+        <v>0</v>
+      </c>
+      <c r="E891" t="n">
+        <v>0</v>
+      </c>
+      <c r="F891" t="n">
         <v>200</v>
       </c>
-      <c r="G889" t="n">
-        <v>0</v>
-      </c>
-      <c r="H889" t="n">
-        <v>0</v>
-      </c>
-      <c r="I889" t="n">
+      <c r="G891" t="n">
+        <v>0</v>
+      </c>
+      <c r="H891" t="n">
+        <v>0</v>
+      </c>
+      <c r="I891" t="n">
         <v>10</v>
       </c>
-      <c r="J889" t="n">
+      <c r="J891" t="n">
         <v>4602</v>
       </c>
-      <c r="K889" t="n">
-        <v>427557</v>
-      </c>
-      <c r="L889" t="n">
-        <v>0</v>
-      </c>
-      <c r="M889" t="n">
-        <v>0</v>
-      </c>
-      <c r="N889" t="n">
-        <v>-8874573</v>
-      </c>
-      <c r="O889" t="n">
-        <v>-8928065</v>
-      </c>
-      <c r="P889" t="n">
-        <v>-3756579</v>
-      </c>
-      <c r="Q889" t="n">
-        <v>-3774626</v>
-      </c>
-      <c r="R889" t="n">
-        <v>-305304</v>
-      </c>
-      <c r="S889" t="n">
-        <v>-1275437.9</v>
-      </c>
-      <c r="T889" t="n">
-        <v>0</v>
-      </c>
-      <c r="U889" t="n">
-        <v>-539232.3</v>
-      </c>
-      <c r="V889" t="n">
-        <v>-2337</v>
-      </c>
-      <c r="W889" t="n">
-        <v>-33.7</v>
-      </c>
-      <c r="X889" t="n">
-        <v>-15328.3</v>
-      </c>
-      <c r="Y889" t="n">
-        <v>-16732.4</v>
-      </c>
-      <c r="Z889" t="n">
-        <v>-117127</v>
+      <c r="K891" t="n">
+        <v>0</v>
+      </c>
+      <c r="L891" t="n">
+        <v>0</v>
+      </c>
+      <c r="M891" t="n">
+        <v>0</v>
+      </c>
+      <c r="N891" t="n">
+        <v>-9326226</v>
+      </c>
+      <c r="O891" t="n">
+        <v>-7855969</v>
+      </c>
+      <c r="P891" t="n">
+        <v>-3763156</v>
+      </c>
+      <c r="Q891" t="n">
+        <v>-3780306</v>
+      </c>
+      <c r="R891" t="n">
+        <v>-2640470</v>
+      </c>
+      <c r="S891" t="n">
+        <v>-1122281.3</v>
+      </c>
+      <c r="T891" t="n">
+        <v>-764120</v>
+      </c>
+      <c r="U891" t="n">
+        <v>-540043.7</v>
+      </c>
+      <c r="V891" t="n">
+        <v>-33655</v>
+      </c>
+      <c r="W891" t="n">
+        <v>-88</v>
+      </c>
+      <c r="X891" t="n">
+        <v>-13166.3</v>
+      </c>
+      <c r="Y891" t="n">
+        <v>-11521</v>
+      </c>
+      <c r="Z891" t="n">
+        <v>-80647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualiza datos provincias 2022-06-20
</commit_message>
<xml_diff>
--- a/data/output/covid19-spain_consolidated.xlsx
+++ b/data/output/covid19-spain_consolidated.xlsx
@@ -71986,7 +71986,7 @@
         <v>197</v>
       </c>
       <c r="J897" t="n">
-        <v>69534</v>
+        <v>76450</v>
       </c>
       <c r="K897" t="n">
         <v>7196122</v>
@@ -72022,19 +72022,19 @@
         <v>2869.1</v>
       </c>
       <c r="V897" t="n">
-        <v>-52906</v>
+        <v>-45990</v>
       </c>
       <c r="W897" t="n">
-        <v>-43.2</v>
+        <v>-37.6</v>
       </c>
       <c r="X897" t="n">
-        <v>-17631.7</v>
+        <v>-15326.3</v>
       </c>
       <c r="Y897" t="n">
-        <v>-7533</v>
+        <v>-6545</v>
       </c>
       <c r="Z897" t="n">
-        <v>-52731</v>
+        <v>-45815</v>
       </c>
     </row>
     <row r="898">
@@ -72066,7 +72066,7 @@
         <v>147</v>
       </c>
       <c r="J898" t="n">
-        <v>65474</v>
+        <v>72390</v>
       </c>
       <c r="K898" t="n">
         <v>6542096</v>
@@ -72105,16 +72105,16 @@
         <v>-4060</v>
       </c>
       <c r="W898" t="n">
-        <v>-5.8</v>
+        <v>-5.3</v>
       </c>
       <c r="X898" t="n">
-        <v>-18987</v>
+        <v>-16681.7</v>
       </c>
       <c r="Y898" t="n">
-        <v>-8115.4</v>
+        <v>-7127.4</v>
       </c>
       <c r="Z898" t="n">
-        <v>-56808</v>
+        <v>-49892</v>
       </c>
     </row>
     <row r="899">
@@ -72146,7 +72146,7 @@
         <v>145</v>
       </c>
       <c r="J899" t="n">
-        <v>76733</v>
+        <v>83649</v>
       </c>
       <c r="K899" t="n">
         <v>6309827</v>
@@ -72185,16 +72185,16 @@
         <v>11259</v>
       </c>
       <c r="W899" t="n">
-        <v>17.2</v>
+        <v>15.6</v>
       </c>
       <c r="X899" t="n">
-        <v>-15235.7</v>
+        <v>-12930.3</v>
       </c>
       <c r="Y899" t="n">
-        <v>-6523.7</v>
+        <v>-5535.7</v>
       </c>
       <c r="Z899" t="n">
-        <v>-45666</v>
+        <v>-38750</v>
       </c>
     </row>
     <row r="900">
@@ -72226,7 +72226,7 @@
         <v>94</v>
       </c>
       <c r="J900" t="n">
-        <v>35239</v>
+        <v>42155</v>
       </c>
       <c r="K900" t="n">
         <v>3722083</v>
@@ -72265,16 +72265,16 @@
         <v>-41494</v>
       </c>
       <c r="W900" t="n">
-        <v>-54.1</v>
+        <v>-49.6</v>
       </c>
       <c r="X900" t="n">
         <v>-11431.7</v>
       </c>
       <c r="Y900" t="n">
-        <v>-12455.6</v>
+        <v>-11467.6</v>
       </c>
       <c r="Z900" t="n">
-        <v>-87189</v>
+        <v>-80273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualiza datos provincias 2022-07-04
</commit_message>
<xml_diff>
--- a/data/output/covid19-spain_consolidated.xlsx
+++ b/data/output/covid19-spain_consolidated.xlsx
@@ -71426,7 +71426,7 @@
         <v>194</v>
       </c>
       <c r="J890" t="n">
-        <v>122357</v>
+        <v>122356</v>
       </c>
       <c r="K890" t="n">
         <v>9418451</v>
@@ -71462,19 +71462,19 @@
         <v>2585.6</v>
       </c>
       <c r="V890" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="W890" t="n">
         <v>0.1</v>
       </c>
       <c r="X890" t="n">
-        <v>50.3</v>
+        <v>50</v>
       </c>
       <c r="Y890" t="n">
-        <v>68.4</v>
+        <v>68.3</v>
       </c>
       <c r="Z890" t="n">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="891">
@@ -71542,7 +71542,7 @@
         <v>2651.1</v>
       </c>
       <c r="V891" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="W891" t="n">
         <v>0</v>
@@ -71708,7 +71708,7 @@
         <v>0.1</v>
       </c>
       <c r="X893" t="n">
-        <v>86</v>
+        <v>86.3</v>
       </c>
       <c r="Y893" t="n">
         <v>62.3</v>
@@ -72031,10 +72031,10 @@
         <v>-7505.3</v>
       </c>
       <c r="Y897" t="n">
-        <v>-3177</v>
+        <v>-3176.9</v>
       </c>
       <c r="Z897" t="n">
-        <v>-22239</v>
+        <v>-22238</v>
       </c>
     </row>
     <row r="898">
@@ -72146,7 +72146,7 @@
         <v>185</v>
       </c>
       <c r="J899" t="n">
-        <v>100323</v>
+        <v>100324</v>
       </c>
       <c r="K899" t="n">
         <v>9478749</v>
@@ -72182,19 +72182,19 @@
         <v>3058.7</v>
       </c>
       <c r="V899" t="n">
-        <v>14321</v>
+        <v>14322</v>
       </c>
       <c r="W899" t="n">
         <v>16.7</v>
       </c>
       <c r="X899" t="n">
-        <v>-7449.3</v>
+        <v>-7449</v>
       </c>
       <c r="Y899" t="n">
-        <v>-3170.3</v>
+        <v>-3170.1</v>
       </c>
       <c r="Z899" t="n">
-        <v>-22192</v>
+        <v>-22191</v>
       </c>
     </row>
     <row r="900">
@@ -72226,7 +72226,7 @@
         <v>205</v>
       </c>
       <c r="J900" t="n">
-        <v>100390</v>
+        <v>100392</v>
       </c>
       <c r="K900" t="n">
         <v>9491372</v>
@@ -72262,19 +72262,19 @@
         <v>3110.3</v>
       </c>
       <c r="V900" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="W900" t="n">
         <v>0.1</v>
       </c>
       <c r="X900" t="n">
-        <v>90.7</v>
+        <v>91.3</v>
       </c>
       <c r="Y900" t="n">
-        <v>-3175</v>
+        <v>-3174.7</v>
       </c>
       <c r="Z900" t="n">
-        <v>-22225</v>
+        <v>-22223</v>
       </c>
     </row>
     <row r="901">
@@ -72306,7 +72306,7 @@
         <v>129</v>
       </c>
       <c r="J901" t="n">
-        <v>81588</v>
+        <v>81592</v>
       </c>
       <c r="K901" t="n">
         <v>7528551</v>
@@ -72342,19 +72342,19 @@
         <v>3179.1</v>
       </c>
       <c r="V901" t="n">
-        <v>-18802</v>
+        <v>-18800</v>
       </c>
       <c r="W901" t="n">
         <v>-18.7</v>
       </c>
       <c r="X901" t="n">
-        <v>-1471.3</v>
+        <v>-1470</v>
       </c>
       <c r="Y901" t="n">
-        <v>-5863.7</v>
+        <v>-5863.1</v>
       </c>
       <c r="Z901" t="n">
-        <v>-41046</v>
+        <v>-41042</v>
       </c>
     </row>
     <row r="902">
@@ -72386,7 +72386,7 @@
         <v>182</v>
       </c>
       <c r="J902" t="n">
-        <v>81618</v>
+        <v>81623</v>
       </c>
       <c r="K902" t="n">
         <v>7534506</v>
@@ -72422,19 +72422,19 @@
         <v>3271.6</v>
       </c>
       <c r="V902" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="W902" t="n">
         <v>0</v>
       </c>
       <c r="X902" t="n">
-        <v>-6235</v>
+        <v>-6233.7</v>
       </c>
       <c r="Y902" t="n">
-        <v>-5862.6</v>
+        <v>-5861.9</v>
       </c>
       <c r="Z902" t="n">
-        <v>-41038</v>
+        <v>-41033</v>
       </c>
     </row>
     <row r="903">
@@ -72466,7 +72466,7 @@
         <v>199</v>
       </c>
       <c r="J903" t="n">
-        <v>100471</v>
+        <v>100477</v>
       </c>
       <c r="K903" t="n">
         <v>9508060</v>
@@ -72502,19 +72502,19 @@
         <v>3557.3</v>
       </c>
       <c r="V903" t="n">
-        <v>18853</v>
+        <v>18854</v>
       </c>
       <c r="W903" t="n">
         <v>23.1</v>
       </c>
       <c r="X903" t="n">
-        <v>27</v>
+        <v>28.3</v>
       </c>
       <c r="Y903" t="n">
-        <v>-3171.4</v>
+        <v>-3170.6</v>
       </c>
       <c r="Z903" t="n">
-        <v>-22200</v>
+        <v>-22194</v>
       </c>
     </row>
     <row r="904">
@@ -72546,7 +72546,7 @@
         <v>200</v>
       </c>
       <c r="J904" t="n">
-        <v>100537</v>
+        <v>100543</v>
       </c>
       <c r="K904" t="n">
         <v>9093020</v>
@@ -72588,13 +72588,13 @@
         <v>0.1</v>
       </c>
       <c r="X904" t="n">
-        <v>6316.3</v>
+        <v>6317</v>
       </c>
       <c r="Y904" t="n">
-        <v>59.9</v>
+        <v>60.7</v>
       </c>
       <c r="Z904" t="n">
-        <v>419</v>
+        <v>425</v>
       </c>
     </row>
     <row r="905">
@@ -72626,7 +72626,7 @@
         <v>173</v>
       </c>
       <c r="J905" t="n">
-        <v>84004</v>
+        <v>84013</v>
       </c>
       <c r="K905" t="n">
         <v>7165945</v>
@@ -72662,19 +72662,19 @@
         <v>-10663.6</v>
       </c>
       <c r="V905" t="n">
-        <v>-16533</v>
+        <v>-16530</v>
       </c>
       <c r="W905" t="n">
         <v>-16.4</v>
       </c>
       <c r="X905" t="n">
-        <v>795.3</v>
+        <v>796.7</v>
       </c>
       <c r="Y905" t="n">
-        <v>-285.4</v>
+        <v>-284.1</v>
       </c>
       <c r="Z905" t="n">
-        <v>-1998</v>
+        <v>-1989</v>
       </c>
     </row>
     <row r="906">
@@ -72706,7 +72706,7 @@
         <v>212</v>
       </c>
       <c r="J906" t="n">
-        <v>98394</v>
+        <v>98408</v>
       </c>
       <c r="K906" t="n">
         <v>8709600</v>
@@ -72742,19 +72742,19 @@
         <v>-10669.7</v>
       </c>
       <c r="V906" t="n">
-        <v>14390</v>
+        <v>14395</v>
       </c>
       <c r="W906" t="n">
         <v>17.1</v>
       </c>
       <c r="X906" t="n">
-        <v>-692.3</v>
+        <v>-689.7</v>
       </c>
       <c r="Y906" t="n">
-        <v>-275.6</v>
+        <v>-273.7</v>
       </c>
       <c r="Z906" t="n">
-        <v>-1929</v>
+        <v>-1916</v>
       </c>
     </row>
     <row r="907">
@@ -72786,7 +72786,7 @@
         <v>223</v>
       </c>
       <c r="J907" t="n">
-        <v>92454</v>
+        <v>92474</v>
       </c>
       <c r="K907" t="n">
         <v>8088965</v>
@@ -72822,19 +72822,19 @@
         <v>-10384.4</v>
       </c>
       <c r="V907" t="n">
-        <v>-5940</v>
+        <v>-5934</v>
       </c>
       <c r="W907" t="n">
         <v>-6</v>
       </c>
       <c r="X907" t="n">
-        <v>-2694.3</v>
+        <v>-2689.7</v>
       </c>
       <c r="Y907" t="n">
-        <v>-1133.7</v>
+        <v>-1131.1</v>
       </c>
       <c r="Z907" t="n">
-        <v>-7936</v>
+        <v>-7918</v>
       </c>
     </row>
     <row r="908">
@@ -72866,7 +72866,7 @@
         <v>159</v>
       </c>
       <c r="J908" t="n">
-        <v>77139</v>
+        <v>77170</v>
       </c>
       <c r="K908" t="n">
         <v>7187388</v>
@@ -72902,19 +72902,19 @@
         <v>-10263.7</v>
       </c>
       <c r="V908" t="n">
-        <v>-15315</v>
+        <v>-15304</v>
       </c>
       <c r="W908" t="n">
-        <v>-16.6</v>
+        <v>-16.5</v>
       </c>
       <c r="X908" t="n">
-        <v>-2288.3</v>
+        <v>-2281</v>
       </c>
       <c r="Y908" t="n">
-        <v>-635.6</v>
+        <v>-631.7</v>
       </c>
       <c r="Z908" t="n">
-        <v>-4449</v>
+        <v>-4422</v>
       </c>
     </row>
     <row r="909">
@@ -72946,7 +72946,7 @@
         <v>196</v>
       </c>
       <c r="J909" t="n">
-        <v>77142</v>
+        <v>77177</v>
       </c>
       <c r="K909" t="n">
         <v>7194845</v>
@@ -72982,19 +72982,19 @@
         <v>-10176.6</v>
       </c>
       <c r="V909" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="W909" t="n">
         <v>0</v>
       </c>
       <c r="X909" t="n">
-        <v>-7084</v>
+        <v>-7077</v>
       </c>
       <c r="Y909" t="n">
-        <v>-639.4</v>
+        <v>-635.1</v>
       </c>
       <c r="Z909" t="n">
-        <v>-4476</v>
+        <v>-4446</v>
       </c>
     </row>
     <row r="910">
@@ -73002,34 +73002,34 @@
         <v>44739</v>
       </c>
       <c r="B910" t="n">
-        <v>2686</v>
+        <v>3813</v>
       </c>
       <c r="C910" t="n">
         <v>1029</v>
       </c>
       <c r="D910" t="n">
-        <v>129511</v>
+        <v>6378758</v>
       </c>
       <c r="E910" t="n">
         <v>0</v>
       </c>
       <c r="F910" t="n">
-        <v>5239</v>
+        <v>5655</v>
       </c>
       <c r="G910" t="n">
-        <v>129511</v>
+        <v>129579</v>
       </c>
       <c r="H910" t="n">
         <v>0</v>
       </c>
       <c r="I910" t="n">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="J910" t="n">
-        <v>87012</v>
+        <v>94185</v>
       </c>
       <c r="K910" t="n">
-        <v>7709381</v>
+        <v>8457059</v>
       </c>
       <c r="L910" t="n">
         <v>3501076</v>
@@ -73038,10 +73038,10 @@
         <v>0</v>
       </c>
       <c r="N910" t="n">
-        <v>-1742929</v>
+        <v>-995251</v>
       </c>
       <c r="O910" t="n">
-        <v>-1798679</v>
+        <v>-1051001</v>
       </c>
       <c r="P910" t="n">
         <v>-313612</v>
@@ -73050,10 +73050,10 @@
         <v>-338513</v>
       </c>
       <c r="R910" t="n">
-        <v>514536</v>
+        <v>1262214</v>
       </c>
       <c r="S910" t="n">
-        <v>-256954.1</v>
+        <v>-150143</v>
       </c>
       <c r="T910" t="n">
         <v>-261493</v>
@@ -73062,19 +73062,19 @@
         <v>-48359</v>
       </c>
       <c r="V910" t="n">
-        <v>9870</v>
+        <v>17008</v>
       </c>
       <c r="W910" t="n">
-        <v>12.8</v>
+        <v>22</v>
       </c>
       <c r="X910" t="n">
-        <v>-1814</v>
+        <v>570.3</v>
       </c>
       <c r="Y910" t="n">
-        <v>-1922.7</v>
+        <v>-898.9</v>
       </c>
       <c r="Z910" t="n">
-        <v>-13459</v>
+        <v>-6292</v>
       </c>
     </row>
     <row r="911">
@@ -73082,34 +73082,34 @@
         <v>44740</v>
       </c>
       <c r="B911" t="n">
-        <v>6718</v>
+        <v>8010</v>
       </c>
       <c r="C911" t="n">
         <v>553</v>
       </c>
       <c r="D911" t="n">
-        <v>382</v>
+        <v>6253777</v>
       </c>
       <c r="E911" t="n">
         <v>0</v>
       </c>
       <c r="F911" t="n">
-        <v>5544</v>
+        <v>5953</v>
       </c>
       <c r="G911" t="n">
-        <v>382</v>
+        <v>451</v>
       </c>
       <c r="H911" t="n">
         <v>0</v>
       </c>
       <c r="I911" t="n">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="J911" t="n">
-        <v>87054</v>
+        <v>94237</v>
       </c>
       <c r="K911" t="n">
-        <v>7724809</v>
+        <v>8473785</v>
       </c>
       <c r="L911" t="n">
         <v>3505443</v>
@@ -73118,10 +73118,10 @@
         <v>0</v>
       </c>
       <c r="N911" t="n">
-        <v>-1740969</v>
+        <v>-991993</v>
       </c>
       <c r="O911" t="n">
-        <v>-1368211</v>
+        <v>-619235</v>
       </c>
       <c r="P911" t="n">
         <v>-313298</v>
@@ -73130,10 +73130,10 @@
         <v>-339951</v>
       </c>
       <c r="R911" t="n">
-        <v>15428</v>
+        <v>16726</v>
       </c>
       <c r="S911" t="n">
-        <v>-195458.7</v>
+        <v>-88462.1</v>
       </c>
       <c r="T911" t="n">
         <v>4367</v>
@@ -73142,19 +73142,19 @@
         <v>-48564.4</v>
       </c>
       <c r="V911" t="n">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="W911" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="X911" t="n">
-        <v>3305</v>
+        <v>5689</v>
       </c>
       <c r="Y911" t="n">
-        <v>-1926.1</v>
+        <v>-900.9</v>
       </c>
       <c r="Z911" t="n">
-        <v>-13483</v>
+        <v>-6306</v>
       </c>
     </row>
     <row r="912">
@@ -73162,34 +73162,34 @@
         <v>44741</v>
       </c>
       <c r="B912" t="n">
-        <v>1986</v>
+        <v>3291</v>
       </c>
       <c r="C912" t="n">
         <v>275</v>
       </c>
       <c r="D912" t="n">
-        <v>287</v>
+        <v>6257495</v>
       </c>
       <c r="E912" t="n">
         <v>0</v>
       </c>
       <c r="F912" t="n">
-        <v>2517</v>
+        <v>2944</v>
       </c>
       <c r="G912" t="n">
-        <v>287</v>
+        <v>364</v>
       </c>
       <c r="H912" t="n">
         <v>0</v>
       </c>
       <c r="I912" t="n">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="J912" t="n">
-        <v>35986</v>
+        <v>43176</v>
       </c>
       <c r="K912" t="n">
-        <v>3137239</v>
+        <v>3887531</v>
       </c>
       <c r="L912" t="n">
         <v>970853</v>
@@ -73198,10 +73198,10 @@
         <v>0</v>
       </c>
       <c r="N912" t="n">
-        <v>-4803601</v>
+        <v>-4053309</v>
       </c>
       <c r="O912" t="n">
-        <v>-4028706</v>
+        <v>-3278414</v>
       </c>
       <c r="P912" t="n">
         <v>-2851361</v>
@@ -73210,10 +73210,10 @@
         <v>-2776716</v>
       </c>
       <c r="R912" t="n">
-        <v>-4587570</v>
+        <v>-4586254</v>
       </c>
       <c r="S912" t="n">
-        <v>-575529.4</v>
+        <v>-468344.9</v>
       </c>
       <c r="T912" t="n">
         <v>-2534590</v>
@@ -73222,19 +73222,19 @@
         <v>-396673.7</v>
       </c>
       <c r="V912" t="n">
-        <v>-51068</v>
+        <v>-51061</v>
       </c>
       <c r="W912" t="n">
-        <v>-58.7</v>
+        <v>-54.2</v>
       </c>
       <c r="X912" t="n">
-        <v>-13718.7</v>
+        <v>-11333.7</v>
       </c>
       <c r="Y912" t="n">
-        <v>-6859.7</v>
+        <v>-5833.9</v>
       </c>
       <c r="Z912" t="n">
-        <v>-48018</v>
+        <v>-40837</v>
       </c>
     </row>
     <row r="913">
@@ -73242,34 +73242,34 @@
         <v>44742</v>
       </c>
       <c r="B913" t="n">
-        <v>1446</v>
+        <v>2690</v>
       </c>
       <c r="C913" t="n">
         <v>0</v>
       </c>
       <c r="D913" t="n">
-        <v>0</v>
+        <v>6260776</v>
       </c>
       <c r="E913" t="n">
         <v>0</v>
       </c>
       <c r="F913" t="n">
-        <v>2395</v>
+        <v>3440</v>
       </c>
       <c r="G913" t="n">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="H913" t="n">
         <v>0</v>
       </c>
       <c r="I913" t="n">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="J913" t="n">
-        <v>33222</v>
+        <v>54676</v>
       </c>
       <c r="K913" t="n">
-        <v>2899282</v>
+        <v>5198214</v>
       </c>
       <c r="L913" t="n">
         <v>784468</v>
@@ -73278,10 +73278,10 @@
         <v>0</v>
       </c>
       <c r="N913" t="n">
-        <v>-6579467</v>
+        <v>-4280535</v>
       </c>
       <c r="O913" t="n">
-        <v>-5810318</v>
+        <v>-3511386</v>
       </c>
       <c r="P913" t="n">
         <v>-3041094</v>
@@ -73290,10 +73290,10 @@
         <v>-2966406</v>
       </c>
       <c r="R913" t="n">
-        <v>-237957</v>
+        <v>1310683</v>
       </c>
       <c r="S913" t="n">
-        <v>-830045.4</v>
+        <v>-501626.6</v>
       </c>
       <c r="T913" t="n">
         <v>-186385</v>
@@ -73302,19 +73302,19 @@
         <v>-423772.3</v>
       </c>
       <c r="V913" t="n">
-        <v>-2764</v>
+        <v>11500</v>
       </c>
       <c r="W913" t="n">
-        <v>-7.7</v>
+        <v>26.6</v>
       </c>
       <c r="X913" t="n">
-        <v>-17930</v>
+        <v>-13169.7</v>
       </c>
       <c r="Y913" t="n">
-        <v>-9310.3</v>
+        <v>-6247.4</v>
       </c>
       <c r="Z913" t="n">
-        <v>-65172</v>
+        <v>-43732</v>
       </c>
     </row>
     <row r="914">
@@ -73322,34 +73322,34 @@
         <v>44743</v>
       </c>
       <c r="B914" t="n">
-        <v>10456</v>
+        <v>11978</v>
       </c>
       <c r="C914" t="n">
         <v>0</v>
       </c>
       <c r="D914" t="n">
-        <v>0</v>
+        <v>6264540</v>
       </c>
       <c r="E914" t="n">
         <v>0</v>
       </c>
       <c r="F914" t="n">
-        <v>2516</v>
+        <v>3516</v>
       </c>
       <c r="G914" t="n">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="H914" t="n">
         <v>0</v>
       </c>
       <c r="I914" t="n">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="J914" t="n">
-        <v>33245</v>
+        <v>54729</v>
       </c>
       <c r="K914" t="n">
-        <v>2911568</v>
+        <v>5219010</v>
       </c>
       <c r="L914" t="n">
         <v>786338</v>
@@ -73358,10 +73358,10 @@
         <v>0</v>
       </c>
       <c r="N914" t="n">
-        <v>-6579804</v>
+        <v>-4272362</v>
       </c>
       <c r="O914" t="n">
-        <v>-5177397</v>
+        <v>-2869955</v>
       </c>
       <c r="P914" t="n">
         <v>-3043373</v>
@@ -73370,10 +73370,10 @@
         <v>-2970682</v>
       </c>
       <c r="R914" t="n">
-        <v>12286</v>
+        <v>20796</v>
       </c>
       <c r="S914" t="n">
-        <v>-739628.1</v>
+        <v>-409993.6</v>
       </c>
       <c r="T914" t="n">
         <v>1870</v>
@@ -73382,19 +73382,179 @@
         <v>-424383.1</v>
       </c>
       <c r="V914" t="n">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="W914" t="n">
         <v>0.1</v>
       </c>
       <c r="X914" t="n">
-        <v>-17936.3</v>
+        <v>-13169.3</v>
       </c>
       <c r="Y914" t="n">
-        <v>-8458.4</v>
+        <v>-5392.1</v>
       </c>
       <c r="Z914" t="n">
-        <v>-59209</v>
+        <v>-37745</v>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" s="1" t="n">
+        <v>44744</v>
+      </c>
+      <c r="B915" t="n">
+        <v>755</v>
+      </c>
+      <c r="C915" t="n">
+        <v>0</v>
+      </c>
+      <c r="D915" t="n">
+        <v>6267179</v>
+      </c>
+      <c r="E915" t="n">
+        <v>0</v>
+      </c>
+      <c r="F915" t="n">
+        <v>447</v>
+      </c>
+      <c r="G915" t="n">
+        <v>70</v>
+      </c>
+      <c r="H915" t="n">
+        <v>0</v>
+      </c>
+      <c r="I915" t="n">
+        <v>21</v>
+      </c>
+      <c r="J915" t="n">
+        <v>7193</v>
+      </c>
+      <c r="K915" t="n">
+        <v>753835</v>
+      </c>
+      <c r="L915" t="n">
+        <v>0</v>
+      </c>
+      <c r="M915" t="n">
+        <v>0</v>
+      </c>
+      <c r="N915" t="n">
+        <v>-6774716</v>
+      </c>
+      <c r="O915" t="n">
+        <v>-6433553</v>
+      </c>
+      <c r="P915" t="n">
+        <v>-3831682</v>
+      </c>
+      <c r="Q915" t="n">
+        <v>-3759836</v>
+      </c>
+      <c r="R915" t="n">
+        <v>-4465175</v>
+      </c>
+      <c r="S915" t="n">
+        <v>-919079</v>
+      </c>
+      <c r="T915" t="n">
+        <v>-786338</v>
+      </c>
+      <c r="U915" t="n">
+        <v>-537119.4</v>
+      </c>
+      <c r="V915" t="n">
+        <v>-47536</v>
+      </c>
+      <c r="W915" t="n">
+        <v>-86.9</v>
+      </c>
+      <c r="X915" t="n">
+        <v>-11994.3</v>
+      </c>
+      <c r="Y915" t="n">
+        <v>-9996.7</v>
+      </c>
+      <c r="Z915" t="n">
+        <v>-69977</v>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="B916" t="n">
+        <v>586</v>
+      </c>
+      <c r="C916" t="n">
+        <v>0</v>
+      </c>
+      <c r="D916" t="n">
+        <v>6268970</v>
+      </c>
+      <c r="E916" t="n">
+        <v>0</v>
+      </c>
+      <c r="F916" t="n">
+        <v>504</v>
+      </c>
+      <c r="G916" t="n">
+        <v>63</v>
+      </c>
+      <c r="H916" t="n">
+        <v>0</v>
+      </c>
+      <c r="I916" t="n">
+        <v>23</v>
+      </c>
+      <c r="J916" t="n">
+        <v>7193</v>
+      </c>
+      <c r="K916" t="n">
+        <v>754429</v>
+      </c>
+      <c r="L916" t="n">
+        <v>0</v>
+      </c>
+      <c r="M916" t="n">
+        <v>0</v>
+      </c>
+      <c r="N916" t="n">
+        <v>-6780077</v>
+      </c>
+      <c r="O916" t="n">
+        <v>-6440416</v>
+      </c>
+      <c r="P916" t="n">
+        <v>-3833805</v>
+      </c>
+      <c r="Q916" t="n">
+        <v>-3762569</v>
+      </c>
+      <c r="R916" t="n">
+        <v>594</v>
+      </c>
+      <c r="S916" t="n">
+        <v>-920059.4</v>
+      </c>
+      <c r="T916" t="n">
+        <v>0</v>
+      </c>
+      <c r="U916" t="n">
+        <v>-537509.9</v>
+      </c>
+      <c r="V916" t="n">
+        <v>0</v>
+      </c>
+      <c r="W916" t="n">
+        <v>0</v>
+      </c>
+      <c r="X916" t="n">
+        <v>-15827.7</v>
+      </c>
+      <c r="Y916" t="n">
+        <v>-9997.7</v>
+      </c>
+      <c r="Z916" t="n">
+        <v>-69984</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualiza datos provincias 2022-08-23
</commit_message>
<xml_diff>
--- a/data/output/covid19-spain_consolidated.xlsx
+++ b/data/output/covid19-spain_consolidated.xlsx
@@ -73642,10 +73642,10 @@
         <v>44747</v>
       </c>
       <c r="B918" t="n">
-        <v>13199</v>
+        <v>13198</v>
       </c>
       <c r="C918" t="n">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="D918" t="n">
         <v>6277508</v>
@@ -73669,37 +73669,37 @@
         <v>89819</v>
       </c>
       <c r="K918" t="n">
-        <v>8826262</v>
+        <v>8826261</v>
       </c>
       <c r="L918" t="n">
-        <v>3816150</v>
+        <v>3816149</v>
       </c>
       <c r="M918" t="n">
         <v>0</v>
       </c>
       <c r="N918" t="n">
-        <v>-700412</v>
+        <v>-700413</v>
       </c>
       <c r="O918" t="n">
-        <v>-344602</v>
+        <v>-344603</v>
       </c>
       <c r="P918" t="n">
-        <v>70618</v>
+        <v>70617</v>
       </c>
       <c r="Q918" t="n">
-        <v>36244</v>
+        <v>36243</v>
       </c>
       <c r="R918" t="n">
-        <v>24206</v>
+        <v>24205</v>
       </c>
       <c r="S918" t="n">
-        <v>-49228.9</v>
+        <v>-49229</v>
       </c>
       <c r="T918" t="n">
-        <v>6028</v>
+        <v>6027</v>
       </c>
       <c r="U918" t="n">
-        <v>5177.7</v>
+        <v>5177.6</v>
       </c>
       <c r="V918" t="n">
         <v>92</v>
@@ -73749,37 +73749,37 @@
         <v>75552</v>
       </c>
       <c r="K919" t="n">
-        <v>7282107</v>
+        <v>7282106</v>
       </c>
       <c r="L919" t="n">
-        <v>3825221</v>
+        <v>3825220</v>
       </c>
       <c r="M919" t="n">
         <v>0</v>
       </c>
       <c r="N919" t="n">
-        <v>-715696</v>
+        <v>-715697</v>
       </c>
       <c r="O919" t="n">
-        <v>83738</v>
+        <v>83737</v>
       </c>
       <c r="P919" t="n">
-        <v>75607</v>
+        <v>75606</v>
       </c>
       <c r="Q919" t="n">
-        <v>39804</v>
+        <v>39803</v>
       </c>
       <c r="R919" t="n">
         <v>-1544155</v>
       </c>
       <c r="S919" t="n">
-        <v>11962.6</v>
+        <v>11962.4</v>
       </c>
       <c r="T919" t="n">
         <v>9071</v>
       </c>
       <c r="U919" t="n">
-        <v>5686.3</v>
+        <v>5686.1</v>
       </c>
       <c r="V919" t="n">
         <v>-14267</v>
@@ -73829,37 +73829,37 @@
         <v>90051</v>
       </c>
       <c r="K920" t="n">
-        <v>8848568</v>
+        <v>8848567</v>
       </c>
       <c r="L920" t="n">
-        <v>3828059</v>
+        <v>3828058</v>
       </c>
       <c r="M920" t="n">
         <v>0</v>
       </c>
       <c r="N920" t="n">
-        <v>-261749</v>
+        <v>-261750</v>
       </c>
       <c r="O920" t="n">
-        <v>94418</v>
+        <v>94417</v>
       </c>
       <c r="P920" t="n">
-        <v>74854</v>
+        <v>74853</v>
       </c>
       <c r="Q920" t="n">
-        <v>37563</v>
+        <v>37562</v>
       </c>
       <c r="R920" t="n">
         <v>1566461</v>
       </c>
       <c r="S920" t="n">
-        <v>13488.3</v>
+        <v>13488.1</v>
       </c>
       <c r="T920" t="n">
         <v>2838</v>
       </c>
       <c r="U920" t="n">
-        <v>5366.1</v>
+        <v>5366</v>
       </c>
       <c r="V920" t="n">
         <v>14499</v>
@@ -73909,37 +73909,37 @@
         <v>90181</v>
       </c>
       <c r="K921" t="n">
-        <v>8872248</v>
+        <v>8872247</v>
       </c>
       <c r="L921" t="n">
-        <v>3831796</v>
+        <v>3831795</v>
       </c>
       <c r="M921" t="n">
         <v>0</v>
       </c>
       <c r="N921" t="n">
-        <v>382287</v>
+        <v>382286</v>
       </c>
       <c r="O921" t="n">
-        <v>92080</v>
+        <v>92079</v>
       </c>
       <c r="P921" t="n">
-        <v>72166</v>
+        <v>72165</v>
       </c>
       <c r="Q921" t="n">
-        <v>34754</v>
+        <v>34753</v>
       </c>
       <c r="R921" t="n">
         <v>23680</v>
       </c>
       <c r="S921" t="n">
-        <v>13154.3</v>
+        <v>13154.1</v>
       </c>
       <c r="T921" t="n">
         <v>3737</v>
       </c>
       <c r="U921" t="n">
-        <v>4964.9</v>
+        <v>4964.7</v>
       </c>
       <c r="V921" t="n">
         <v>130</v>
@@ -73989,37 +73989,37 @@
         <v>71190</v>
       </c>
       <c r="K922" t="n">
-        <v>7307997</v>
+        <v>7307996</v>
       </c>
       <c r="L922" t="n">
-        <v>3833891</v>
+        <v>3833890</v>
       </c>
       <c r="M922" t="n">
         <v>0</v>
       </c>
       <c r="N922" t="n">
-        <v>-280703</v>
+        <v>-280704</v>
       </c>
       <c r="O922" t="n">
-        <v>78248</v>
+        <v>78247</v>
       </c>
       <c r="P922" t="n">
-        <v>71134</v>
+        <v>71133</v>
       </c>
       <c r="Q922" t="n">
-        <v>33915</v>
+        <v>33914</v>
       </c>
       <c r="R922" t="n">
         <v>-1564251</v>
       </c>
       <c r="S922" t="n">
-        <v>11178.3</v>
+        <v>11178.1</v>
       </c>
       <c r="T922" t="n">
         <v>2095</v>
       </c>
       <c r="U922" t="n">
-        <v>4845</v>
+        <v>4844.9</v>
       </c>
       <c r="V922" t="n">
         <v>-18991</v>
@@ -74069,37 +74069,37 @@
         <v>71256</v>
       </c>
       <c r="K923" t="n">
-        <v>7313460</v>
+        <v>7313459</v>
       </c>
       <c r="L923" t="n">
-        <v>3835815</v>
+        <v>3835814</v>
       </c>
       <c r="M923" t="n">
         <v>0</v>
       </c>
       <c r="N923" t="n">
-        <v>-284566</v>
+        <v>-284567</v>
       </c>
       <c r="O923" t="n">
-        <v>76301</v>
+        <v>76300</v>
       </c>
       <c r="P923" t="n">
-        <v>69907</v>
+        <v>69906</v>
       </c>
       <c r="Q923" t="n">
-        <v>33101</v>
+        <v>33100</v>
       </c>
       <c r="R923" t="n">
         <v>5463</v>
       </c>
       <c r="S923" t="n">
-        <v>10900.1</v>
+        <v>10900</v>
       </c>
       <c r="T923" t="n">
         <v>1924</v>
       </c>
       <c r="U923" t="n">
-        <v>4728.7</v>
+        <v>4728.6</v>
       </c>
       <c r="V923" t="n">
         <v>66</v>
@@ -74149,37 +74149,37 @@
         <v>90355</v>
       </c>
       <c r="K924" t="n">
-        <v>8887646</v>
+        <v>8887645</v>
       </c>
       <c r="L924" t="n">
-        <v>3840042</v>
+        <v>3840041</v>
       </c>
       <c r="M924" t="n">
         <v>0</v>
       </c>
       <c r="N924" t="n">
-        <v>-264041</v>
+        <v>-264042</v>
       </c>
       <c r="O924" t="n">
-        <v>85590</v>
+        <v>85589</v>
       </c>
       <c r="P924" t="n">
-        <v>66835</v>
+        <v>66834</v>
       </c>
       <c r="Q924" t="n">
-        <v>29920</v>
+        <v>29919</v>
       </c>
       <c r="R924" t="n">
         <v>1574186</v>
       </c>
       <c r="S924" t="n">
-        <v>12227.1</v>
+        <v>12227</v>
       </c>
       <c r="T924" t="n">
         <v>4227</v>
       </c>
       <c r="U924" t="n">
-        <v>4274.3</v>
+        <v>4274.1</v>
       </c>
       <c r="V924" t="n">
         <v>19099</v>
@@ -74229,22 +74229,22 @@
         <v>90494</v>
       </c>
       <c r="K925" t="n">
-        <v>8908234</v>
+        <v>8908233</v>
       </c>
       <c r="L925" t="n">
-        <v>3845407</v>
+        <v>3845406</v>
       </c>
       <c r="M925" t="n">
         <v>0</v>
       </c>
       <c r="N925" t="n">
-        <v>-262630</v>
+        <v>-262631</v>
       </c>
       <c r="O925" t="n">
         <v>81972</v>
       </c>
       <c r="P925" t="n">
-        <v>65501</v>
+        <v>65500</v>
       </c>
       <c r="Q925" t="n">
         <v>29257</v>
@@ -74309,22 +74309,22 @@
         <v>76139</v>
       </c>
       <c r="K926" t="n">
-        <v>7343481</v>
+        <v>7343480</v>
       </c>
       <c r="L926" t="n">
-        <v>3848568</v>
+        <v>3848567</v>
       </c>
       <c r="M926" t="n">
         <v>0</v>
       </c>
       <c r="N926" t="n">
-        <v>145112</v>
+        <v>145111</v>
       </c>
       <c r="O926" t="n">
         <v>61374</v>
       </c>
       <c r="P926" t="n">
-        <v>63151</v>
+        <v>63150</v>
       </c>
       <c r="Q926" t="n">
         <v>23347</v>
@@ -74389,22 +74389,22 @@
         <v>90818</v>
       </c>
       <c r="K927" t="n">
-        <v>8920363</v>
+        <v>8920362</v>
       </c>
       <c r="L927" t="n">
-        <v>3851252</v>
+        <v>3851251</v>
       </c>
       <c r="M927" t="n">
         <v>0</v>
       </c>
       <c r="N927" t="n">
-        <v>166213</v>
+        <v>166212</v>
       </c>
       <c r="O927" t="n">
         <v>71795</v>
       </c>
       <c r="P927" t="n">
-        <v>60756</v>
+        <v>60755</v>
       </c>
       <c r="Q927" t="n">
         <v>23193</v>
@@ -74469,22 +74469,22 @@
         <v>90934</v>
       </c>
       <c r="K928" t="n">
-        <v>8932112</v>
+        <v>8932111</v>
       </c>
       <c r="L928" t="n">
-        <v>3855724</v>
+        <v>3855723</v>
       </c>
       <c r="M928" t="n">
         <v>0</v>
       </c>
       <c r="N928" t="n">
-        <v>151944</v>
+        <v>151943</v>
       </c>
       <c r="O928" t="n">
         <v>59864</v>
       </c>
       <c r="P928" t="n">
-        <v>58682</v>
+        <v>58681</v>
       </c>
       <c r="Q928" t="n">
         <v>23928</v>
@@ -74549,22 +74549,22 @@
         <v>71886</v>
       </c>
       <c r="K929" t="n">
-        <v>7363424</v>
+        <v>7363423</v>
       </c>
       <c r="L929" t="n">
-        <v>3857078</v>
+        <v>3857077</v>
       </c>
       <c r="M929" t="n">
         <v>0</v>
       </c>
       <c r="N929" t="n">
-        <v>133675</v>
+        <v>133674</v>
       </c>
       <c r="O929" t="n">
         <v>55427</v>
       </c>
       <c r="P929" t="n">
-        <v>57102</v>
+        <v>57101</v>
       </c>
       <c r="Q929" t="n">
         <v>23187</v>
@@ -74629,22 +74629,22 @@
         <v>62313</v>
       </c>
       <c r="K930" t="n">
-        <v>5858492</v>
+        <v>5858491</v>
       </c>
       <c r="L930" t="n">
-        <v>3858307</v>
+        <v>3858306</v>
       </c>
       <c r="M930" t="n">
         <v>0</v>
       </c>
       <c r="N930" t="n">
-        <v>-1378667</v>
+        <v>-1378668</v>
       </c>
       <c r="O930" t="n">
         <v>-1454968</v>
       </c>
       <c r="P930" t="n">
-        <v>55593</v>
+        <v>55592</v>
       </c>
       <c r="Q930" t="n">
         <v>22492</v>
@@ -74709,22 +74709,22 @@
         <v>67048</v>
       </c>
       <c r="K931" t="n">
-        <v>5862589</v>
+        <v>5862588</v>
       </c>
       <c r="L931" t="n">
-        <v>3860843</v>
+        <v>3860842</v>
       </c>
       <c r="M931" t="n">
         <v>0</v>
       </c>
       <c r="N931" t="n">
-        <v>-2939467</v>
+        <v>-2939468</v>
       </c>
       <c r="O931" t="n">
         <v>-3025057</v>
       </c>
       <c r="P931" t="n">
-        <v>50721</v>
+        <v>50720</v>
       </c>
       <c r="Q931" t="n">
         <v>20801</v>
@@ -74789,10 +74789,10 @@
         <v>81651</v>
       </c>
       <c r="K932" t="n">
-        <v>7448083</v>
+        <v>7448082</v>
       </c>
       <c r="L932" t="n">
-        <v>3864928</v>
+        <v>3864927</v>
       </c>
       <c r="M932" t="n">
         <v>0</v>
@@ -74869,10 +74869,10 @@
         <v>67148</v>
       </c>
       <c r="K933" t="n">
-        <v>5873012</v>
+        <v>5873011</v>
       </c>
       <c r="L933" t="n">
-        <v>3867021</v>
+        <v>3867020</v>
       </c>
       <c r="M933" t="n">
         <v>0</v>
@@ -74949,10 +74949,10 @@
         <v>81907</v>
       </c>
       <c r="K934" t="n">
-        <v>7455634</v>
+        <v>7455633</v>
       </c>
       <c r="L934" t="n">
-        <v>3868678</v>
+        <v>3868677</v>
       </c>
       <c r="M934" t="n">
         <v>0</v>
@@ -75029,10 +75029,10 @@
         <v>82011</v>
       </c>
       <c r="K935" t="n">
-        <v>7497304</v>
+        <v>7497303</v>
       </c>
       <c r="L935" t="n">
-        <v>3904915</v>
+        <v>3904914</v>
       </c>
       <c r="M935" t="n">
         <v>0</v>
@@ -75109,10 +75109,10 @@
         <v>60400</v>
       </c>
       <c r="K936" t="n">
-        <v>5503056</v>
+        <v>5503055</v>
       </c>
       <c r="L936" t="n">
-        <v>3905754</v>
+        <v>3905753</v>
       </c>
       <c r="M936" t="n">
         <v>0</v>
@@ -75189,10 +75189,10 @@
         <v>60420</v>
       </c>
       <c r="K937" t="n">
-        <v>5504115</v>
+        <v>5504114</v>
       </c>
       <c r="L937" t="n">
-        <v>3906564</v>
+        <v>3906563</v>
       </c>
       <c r="M937" t="n">
         <v>0</v>
@@ -75269,10 +75269,10 @@
         <v>65101</v>
       </c>
       <c r="K938" t="n">
-        <v>5506466</v>
+        <v>5506465</v>
       </c>
       <c r="L938" t="n">
-        <v>3907892</v>
+        <v>3907891</v>
       </c>
       <c r="M938" t="n">
         <v>0</v>
@@ -75349,10 +75349,10 @@
         <v>36976</v>
       </c>
       <c r="K939" t="n">
-        <v>2813761</v>
+        <v>2813760</v>
       </c>
       <c r="L939" t="n">
-        <v>1285795</v>
+        <v>1285794</v>
       </c>
       <c r="M939" t="n">
         <v>0</v>
@@ -75429,10 +75429,10 @@
         <v>36995</v>
       </c>
       <c r="K940" t="n">
-        <v>2815517</v>
+        <v>2815516</v>
       </c>
       <c r="L940" t="n">
-        <v>1286438</v>
+        <v>1286437</v>
       </c>
       <c r="M940" t="n">
         <v>0</v>
@@ -75509,10 +75509,10 @@
         <v>37250</v>
       </c>
       <c r="K941" t="n">
-        <v>2816924</v>
+        <v>2816923</v>
       </c>
       <c r="L941" t="n">
-        <v>1286920</v>
+        <v>1286919</v>
       </c>
       <c r="M941" t="n">
         <v>0</v>
@@ -75589,10 +75589,10 @@
         <v>37271</v>
       </c>
       <c r="K942" t="n">
-        <v>2816561</v>
+        <v>2816560</v>
       </c>
       <c r="L942" t="n">
-        <v>1285646</v>
+        <v>1285645</v>
       </c>
       <c r="M942" t="n">
         <v>0</v>
@@ -75669,10 +75669,10 @@
         <v>32619</v>
       </c>
       <c r="K943" t="n">
-        <v>2817129</v>
+        <v>2817128</v>
       </c>
       <c r="L943" t="n">
-        <v>1285941</v>
+        <v>1285940</v>
       </c>
       <c r="M943" t="n">
         <v>0</v>
@@ -75749,10 +75749,10 @@
         <v>32634</v>
       </c>
       <c r="K944" t="n">
-        <v>2817908</v>
+        <v>2817907</v>
       </c>
       <c r="L944" t="n">
-        <v>1286197</v>
+        <v>1286196</v>
       </c>
       <c r="M944" t="n">
         <v>0</v>
@@ -75829,10 +75829,10 @@
         <v>32663</v>
       </c>
       <c r="K945" t="n">
-        <v>2819070</v>
+        <v>2819069</v>
       </c>
       <c r="L945" t="n">
-        <v>1286630</v>
+        <v>1286629</v>
       </c>
       <c r="M945" t="n">
         <v>0</v>
@@ -75909,10 +75909,10 @@
         <v>37361</v>
       </c>
       <c r="K946" t="n">
-        <v>2821118</v>
+        <v>2821117</v>
       </c>
       <c r="L946" t="n">
-        <v>1287860</v>
+        <v>1287859</v>
       </c>
       <c r="M946" t="n">
         <v>0</v>
@@ -75986,13 +75986,13 @@
         <v>70</v>
       </c>
       <c r="J947" t="n">
-        <v>37372</v>
+        <v>37374</v>
       </c>
       <c r="K947" t="n">
-        <v>2822143</v>
+        <v>2822142</v>
       </c>
       <c r="L947" t="n">
-        <v>1288248</v>
+        <v>1288247</v>
       </c>
       <c r="M947" t="n">
         <v>0</v>
@@ -76022,19 +76022,19 @@
         <v>258.6</v>
       </c>
       <c r="V947" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="W947" t="n">
         <v>0</v>
       </c>
       <c r="X947" t="n">
-        <v>1579.3</v>
+        <v>1580</v>
       </c>
       <c r="Y947" t="n">
-        <v>53.9</v>
+        <v>54.1</v>
       </c>
       <c r="Z947" t="n">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="948">
@@ -76066,13 +76066,13 @@
         <v>67</v>
       </c>
       <c r="J948" t="n">
-        <v>37620</v>
+        <v>37622</v>
       </c>
       <c r="K948" t="n">
-        <v>2823004</v>
+        <v>2823003</v>
       </c>
       <c r="L948" t="n">
-        <v>1288577</v>
+        <v>1288576</v>
       </c>
       <c r="M948" t="n">
         <v>0</v>
@@ -76108,13 +76108,13 @@
         <v>0.7</v>
       </c>
       <c r="X948" t="n">
-        <v>1652.3</v>
+        <v>1653</v>
       </c>
       <c r="Y948" t="n">
-        <v>52.9</v>
+        <v>53.1</v>
       </c>
       <c r="Z948" t="n">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="949">
@@ -76146,13 +76146,13 @@
         <v>61</v>
       </c>
       <c r="J949" t="n">
-        <v>35630</v>
+        <v>35634</v>
       </c>
       <c r="K949" t="n">
-        <v>2521752</v>
+        <v>2521751</v>
       </c>
       <c r="L949" t="n">
-        <v>1010862</v>
+        <v>1010861</v>
       </c>
       <c r="M949" t="n">
         <v>0</v>
@@ -76182,19 +76182,19 @@
         <v>-39254.9</v>
       </c>
       <c r="V949" t="n">
-        <v>-1990</v>
+        <v>-1988</v>
       </c>
       <c r="W949" t="n">
         <v>-5.3</v>
       </c>
       <c r="X949" t="n">
-        <v>-577</v>
+        <v>-575.7</v>
       </c>
       <c r="Y949" t="n">
-        <v>-234.4</v>
+        <v>-233.9</v>
       </c>
       <c r="Z949" t="n">
-        <v>-1641</v>
+        <v>-1637</v>
       </c>
     </row>
     <row r="950">
@@ -76226,13 +76226,13 @@
         <v>42</v>
       </c>
       <c r="J950" t="n">
-        <v>30981</v>
+        <v>30986</v>
       </c>
       <c r="K950" t="n">
-        <v>2522119</v>
+        <v>2522118</v>
       </c>
       <c r="L950" t="n">
-        <v>1011060</v>
+        <v>1011059</v>
       </c>
       <c r="M950" t="n">
         <v>0</v>
@@ -76262,19 +76262,19 @@
         <v>-39268.7</v>
       </c>
       <c r="V950" t="n">
-        <v>-4649</v>
+        <v>-4648</v>
       </c>
       <c r="W950" t="n">
         <v>-13</v>
       </c>
       <c r="X950" t="n">
-        <v>-2130.3</v>
+        <v>-2129.3</v>
       </c>
       <c r="Y950" t="n">
-        <v>-234</v>
+        <v>-233.3</v>
       </c>
       <c r="Z950" t="n">
-        <v>-1638</v>
+        <v>-1633</v>
       </c>
     </row>
     <row r="951">
@@ -76306,13 +76306,13 @@
         <v>52</v>
       </c>
       <c r="J951" t="n">
-        <v>30986</v>
+        <v>30991</v>
       </c>
       <c r="K951" t="n">
-        <v>2522683</v>
+        <v>2522682</v>
       </c>
       <c r="L951" t="n">
-        <v>1011259</v>
+        <v>1011258</v>
       </c>
       <c r="M951" t="n">
         <v>0</v>
@@ -76348,13 +76348,13 @@
         <v>0</v>
       </c>
       <c r="X951" t="n">
-        <v>-2211.3</v>
+        <v>-2210.3</v>
       </c>
       <c r="Y951" t="n">
-        <v>-235.4</v>
+        <v>-234.7</v>
       </c>
       <c r="Z951" t="n">
-        <v>-1648</v>
+        <v>-1643</v>
       </c>
     </row>
     <row r="952">
@@ -76386,13 +76386,13 @@
         <v>66</v>
       </c>
       <c r="J952" t="n">
-        <v>35660</v>
+        <v>35665</v>
       </c>
       <c r="K952" t="n">
-        <v>2523459</v>
+        <v>2523458</v>
       </c>
       <c r="L952" t="n">
-        <v>1011581</v>
+        <v>1011580</v>
       </c>
       <c r="M952" t="n">
         <v>0</v>
@@ -76428,13 +76428,13 @@
         <v>15.1</v>
       </c>
       <c r="X952" t="n">
-        <v>10</v>
+        <v>10.3</v>
       </c>
       <c r="Y952" t="n">
-        <v>428.1</v>
+        <v>428.9</v>
       </c>
       <c r="Z952" t="n">
-        <v>2997</v>
+        <v>3002</v>
       </c>
     </row>
     <row r="953">
@@ -76442,13 +76442,13 @@
         <v>44782</v>
       </c>
       <c r="B953" t="n">
-        <v>715</v>
+        <v>726</v>
       </c>
       <c r="C953" t="n">
         <v>43</v>
       </c>
       <c r="D953" t="n">
-        <v>6367926</v>
+        <v>6367937</v>
       </c>
       <c r="E953" t="n">
         <v>0</v>
@@ -76457,7 +76457,7 @@
         <v>1239</v>
       </c>
       <c r="G953" t="n">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="H953" t="n">
         <v>0</v>
@@ -76466,22 +76466,22 @@
         <v>59</v>
       </c>
       <c r="J953" t="n">
-        <v>35675</v>
+        <v>35685</v>
       </c>
       <c r="K953" t="n">
-        <v>2524362</v>
+        <v>2524372</v>
       </c>
       <c r="L953" t="n">
-        <v>1012051</v>
+        <v>1012050</v>
       </c>
       <c r="M953" t="n">
         <v>0</v>
       </c>
       <c r="N953" t="n">
-        <v>-289399</v>
+        <v>-289388</v>
       </c>
       <c r="O953" t="n">
-        <v>-296756</v>
+        <v>-296745</v>
       </c>
       <c r="P953" t="n">
         <v>-273744</v>
@@ -76490,10 +76490,10 @@
         <v>-275809</v>
       </c>
       <c r="R953" t="n">
-        <v>903</v>
+        <v>914</v>
       </c>
       <c r="S953" t="n">
-        <v>-42393.7</v>
+        <v>-42392.1</v>
       </c>
       <c r="T953" t="n">
         <v>470</v>
@@ -76502,19 +76502,19 @@
         <v>-39401.3</v>
       </c>
       <c r="V953" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="W953" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="X953" t="n">
-        <v>1564.7</v>
+        <v>1566.3</v>
       </c>
       <c r="Y953" t="n">
-        <v>-240.9</v>
+        <v>-239.4</v>
       </c>
       <c r="Z953" t="n">
-        <v>-1686</v>
+        <v>-1676</v>
       </c>
     </row>
     <row r="954">
@@ -76546,22 +76546,22 @@
         <v>59</v>
       </c>
       <c r="J954" t="n">
-        <v>35684</v>
+        <v>35697</v>
       </c>
       <c r="K954" t="n">
-        <v>2525155</v>
+        <v>2525165</v>
       </c>
       <c r="L954" t="n">
-        <v>1012357</v>
+        <v>1012356</v>
       </c>
       <c r="M954" t="n">
         <v>0</v>
       </c>
       <c r="N954" t="n">
-        <v>-290362</v>
+        <v>-290351</v>
       </c>
       <c r="O954" t="n">
-        <v>-296988</v>
+        <v>-296977</v>
       </c>
       <c r="P954" t="n">
         <v>-274081</v>
@@ -76573,7 +76573,7 @@
         <v>793</v>
       </c>
       <c r="S954" t="n">
-        <v>-42426.9</v>
+        <v>-42425.3</v>
       </c>
       <c r="T954" t="n">
         <v>306</v>
@@ -76582,19 +76582,19 @@
         <v>-39413</v>
       </c>
       <c r="V954" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="W954" t="n">
         <v>0</v>
       </c>
       <c r="X954" t="n">
-        <v>1566</v>
+        <v>1568.7</v>
       </c>
       <c r="Y954" t="n">
-        <v>-241.1</v>
+        <v>-239.6</v>
       </c>
       <c r="Z954" t="n">
-        <v>-1688</v>
+        <v>-1677</v>
       </c>
     </row>
     <row r="955">
@@ -76602,13 +76602,13 @@
         <v>44784</v>
       </c>
       <c r="B955" t="n">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="C955" t="n">
         <v>42</v>
       </c>
       <c r="D955" t="n">
-        <v>6371390</v>
+        <v>6371392</v>
       </c>
       <c r="E955" t="n">
         <v>0</v>
@@ -76617,7 +76617,7 @@
         <v>1108</v>
       </c>
       <c r="G955" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H955" t="n">
         <v>0</v>
@@ -76626,22 +76626,22 @@
         <v>82</v>
       </c>
       <c r="J955" t="n">
-        <v>35867</v>
+        <v>35884</v>
       </c>
       <c r="K955" t="n">
-        <v>2525782</v>
+        <v>2525794</v>
       </c>
       <c r="L955" t="n">
-        <v>1012618</v>
+        <v>1012617</v>
       </c>
       <c r="M955" t="n">
         <v>0</v>
       </c>
       <c r="N955" t="n">
-        <v>-291142</v>
+        <v>-291129</v>
       </c>
       <c r="O955" t="n">
-        <v>-297222</v>
+        <v>-297209</v>
       </c>
       <c r="P955" t="n">
         <v>-274302</v>
@@ -76650,10 +76650,10 @@
         <v>-275959</v>
       </c>
       <c r="R955" t="n">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="S955" t="n">
-        <v>-42460.3</v>
+        <v>-42458.4</v>
       </c>
       <c r="T955" t="n">
         <v>261</v>
@@ -76662,19 +76662,19 @@
         <v>-39422.7</v>
       </c>
       <c r="V955" t="n">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="W955" t="n">
         <v>0.5</v>
       </c>
       <c r="X955" t="n">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="Y955" t="n">
-        <v>-250.4</v>
+        <v>-248.3</v>
       </c>
       <c r="Z955" t="n">
-        <v>-1753</v>
+        <v>-1738</v>
       </c>
     </row>
     <row r="956">
@@ -76682,10 +76682,10 @@
         <v>44785</v>
       </c>
       <c r="B956" t="n">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C956" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D956" t="n">
         <v>6372817</v>
@@ -76706,10 +76706,10 @@
         <v>81</v>
       </c>
       <c r="J956" t="n">
-        <v>35869</v>
+        <v>35897</v>
       </c>
       <c r="K956" t="n">
-        <v>2526616</v>
+        <v>2526629</v>
       </c>
       <c r="L956" t="n">
         <v>1013112</v>
@@ -76718,43 +76718,43 @@
         <v>0</v>
       </c>
       <c r="N956" t="n">
-        <v>-289945</v>
+        <v>-289931</v>
       </c>
       <c r="O956" t="n">
-        <v>4864</v>
+        <v>4878</v>
       </c>
       <c r="P956" t="n">
-        <v>-272534</v>
+        <v>-272533</v>
       </c>
       <c r="Q956" t="n">
-        <v>2250</v>
+        <v>2251</v>
       </c>
       <c r="R956" t="n">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="S956" t="n">
-        <v>694.9</v>
+        <v>696.9</v>
       </c>
       <c r="T956" t="n">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="U956" t="n">
-        <v>321.4</v>
+        <v>321.6</v>
       </c>
       <c r="V956" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="W956" t="n">
         <v>0</v>
       </c>
       <c r="X956" t="n">
-        <v>64.7</v>
+        <v>70.7</v>
       </c>
       <c r="Y956" t="n">
-        <v>34.1</v>
+        <v>37.6</v>
       </c>
       <c r="Z956" t="n">
-        <v>239</v>
+        <v>263</v>
       </c>
     </row>
     <row r="957">
@@ -76762,22 +76762,22 @@
         <v>44786</v>
       </c>
       <c r="B957" t="n">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C957" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D957" t="n">
-        <v>6373809</v>
+        <v>6373810</v>
       </c>
       <c r="E957" t="n">
         <v>0</v>
       </c>
       <c r="F957" t="n">
-        <v>579</v>
+        <v>775</v>
       </c>
       <c r="G957" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H957" t="n">
         <v>0</v>
@@ -76786,55 +76786,55 @@
         <v>41</v>
       </c>
       <c r="J957" t="n">
-        <v>27351</v>
+        <v>31249</v>
       </c>
       <c r="K957" t="n">
-        <v>1855434</v>
+        <v>2526858</v>
       </c>
       <c r="L957" t="n">
-        <v>1013250</v>
+        <v>1013251</v>
       </c>
       <c r="M957" t="n">
         <v>0</v>
       </c>
       <c r="N957" t="n">
-        <v>-961695</v>
+        <v>-290270</v>
       </c>
       <c r="O957" t="n">
-        <v>-666685</v>
+        <v>4740</v>
       </c>
       <c r="P957" t="n">
-        <v>-272691</v>
+        <v>-272689</v>
       </c>
       <c r="Q957" t="n">
-        <v>2190</v>
+        <v>2192</v>
       </c>
       <c r="R957" t="n">
-        <v>-671182</v>
+        <v>229</v>
       </c>
       <c r="S957" t="n">
-        <v>-95240.7</v>
+        <v>677.1</v>
       </c>
       <c r="T957" t="n">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="U957" t="n">
-        <v>312.9</v>
+        <v>313.1</v>
       </c>
       <c r="V957" t="n">
-        <v>-8518</v>
+        <v>-4648</v>
       </c>
       <c r="W957" t="n">
-        <v>-23.7</v>
+        <v>-12.9</v>
       </c>
       <c r="X957" t="n">
-        <v>-2777.7</v>
+        <v>-1482.7</v>
       </c>
       <c r="Y957" t="n">
-        <v>-518.6</v>
+        <v>37.6</v>
       </c>
       <c r="Z957" t="n">
-        <v>-3630</v>
+        <v>263</v>
       </c>
     </row>
     <row r="958">
@@ -76842,22 +76842,22 @@
         <v>44787</v>
       </c>
       <c r="B958" t="n">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C958" t="n">
         <v>18</v>
       </c>
       <c r="D958" t="n">
-        <v>6374656</v>
+        <v>6374660</v>
       </c>
       <c r="E958" t="n">
         <v>0</v>
       </c>
       <c r="F958" t="n">
-        <v>593</v>
+        <v>789</v>
       </c>
       <c r="G958" t="n">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H958" t="n">
         <v>0</v>
@@ -76866,55 +76866,55 @@
         <v>42</v>
       </c>
       <c r="J958" t="n">
-        <v>27353</v>
+        <v>31256</v>
       </c>
       <c r="K958" t="n">
-        <v>1855641</v>
+        <v>2527069</v>
       </c>
       <c r="L958" t="n">
-        <v>1013370</v>
+        <v>1013371</v>
       </c>
       <c r="M958" t="n">
         <v>0</v>
       </c>
       <c r="N958" t="n">
-        <v>-962267</v>
+        <v>-290838</v>
       </c>
       <c r="O958" t="n">
-        <v>-667042</v>
+        <v>4387</v>
       </c>
       <c r="P958" t="n">
-        <v>-272827</v>
+        <v>-272825</v>
       </c>
       <c r="Q958" t="n">
-        <v>2111</v>
+        <v>2113</v>
       </c>
       <c r="R958" t="n">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="S958" t="n">
-        <v>-95291.7</v>
+        <v>626.7</v>
       </c>
       <c r="T958" t="n">
         <v>120</v>
       </c>
       <c r="U958" t="n">
-        <v>301.6</v>
+        <v>301.9</v>
       </c>
       <c r="V958" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="W958" t="n">
         <v>0</v>
       </c>
       <c r="X958" t="n">
-        <v>-2838</v>
+        <v>-1542.7</v>
       </c>
       <c r="Y958" t="n">
-        <v>-519</v>
+        <v>37.9</v>
       </c>
       <c r="Z958" t="n">
-        <v>-3633</v>
+        <v>265</v>
       </c>
     </row>
     <row r="959">
@@ -76922,79 +76922,79 @@
         <v>44788</v>
       </c>
       <c r="B959" t="n">
-        <v>121</v>
+        <v>216</v>
       </c>
       <c r="C959" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D959" t="n">
-        <v>0</v>
+        <v>6375682</v>
       </c>
       <c r="E959" t="n">
         <v>0</v>
       </c>
       <c r="F959" t="n">
-        <v>319</v>
+        <v>816</v>
       </c>
       <c r="G959" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H959" t="n">
         <v>0</v>
       </c>
       <c r="I959" t="n">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="J959" t="n">
-        <v>16593</v>
+        <v>31258</v>
       </c>
       <c r="K959" t="n">
-        <v>820175</v>
+        <v>2527522</v>
       </c>
       <c r="L959" t="n">
-        <v>820175</v>
+        <v>1013511</v>
       </c>
       <c r="M959" t="n">
         <v>0</v>
       </c>
       <c r="N959" t="n">
-        <v>-1998895</v>
+        <v>-291547</v>
       </c>
       <c r="O959" t="n">
-        <v>-1703284</v>
+        <v>4064</v>
       </c>
       <c r="P959" t="n">
-        <v>-466455</v>
+        <v>-273118</v>
       </c>
       <c r="Q959" t="n">
-        <v>-191406</v>
+        <v>1931</v>
       </c>
       <c r="R959" t="n">
-        <v>-1035466</v>
+        <v>453</v>
       </c>
       <c r="S959" t="n">
-        <v>-243326.3</v>
+        <v>580.6</v>
       </c>
       <c r="T959" t="n">
-        <v>-193195</v>
+        <v>140</v>
       </c>
       <c r="U959" t="n">
-        <v>-27343.7</v>
+        <v>275.9</v>
       </c>
       <c r="V959" t="n">
-        <v>-10760</v>
+        <v>2</v>
       </c>
       <c r="W959" t="n">
-        <v>-39.3</v>
+        <v>0</v>
       </c>
       <c r="X959" t="n">
-        <v>-6425.3</v>
+        <v>-1546.3</v>
       </c>
       <c r="Y959" t="n">
-        <v>-2723.9</v>
+        <v>-629.6</v>
       </c>
       <c r="Z959" t="n">
-        <v>-19067</v>
+        <v>-4407</v>
       </c>
     </row>
     <row r="960">
@@ -77002,79 +77002,559 @@
         <v>44789</v>
       </c>
       <c r="B960" t="n">
-        <v>135</v>
+        <v>380</v>
       </c>
       <c r="C960" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="D960" t="n">
-        <v>0</v>
+        <v>6377760</v>
       </c>
       <c r="E960" t="n">
         <v>0</v>
       </c>
       <c r="F960" t="n">
-        <v>644</v>
+        <v>1137</v>
       </c>
       <c r="G960" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="H960" t="n">
         <v>0</v>
       </c>
       <c r="I960" t="n">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="J960" t="n">
-        <v>21251</v>
+        <v>35923</v>
       </c>
       <c r="K960" t="n">
-        <v>820492</v>
+        <v>2528225</v>
       </c>
       <c r="L960" t="n">
-        <v>820492</v>
+        <v>1013861</v>
       </c>
       <c r="M960" t="n">
         <v>0</v>
       </c>
       <c r="N960" t="n">
-        <v>-2000626</v>
+        <v>-292892</v>
       </c>
       <c r="O960" t="n">
-        <v>-1703870</v>
+        <v>3853</v>
       </c>
       <c r="P960" t="n">
-        <v>-467368</v>
+        <v>-273998</v>
       </c>
       <c r="Q960" t="n">
-        <v>-191559</v>
+        <v>1811</v>
       </c>
       <c r="R960" t="n">
-        <v>317</v>
+        <v>703</v>
       </c>
       <c r="S960" t="n">
-        <v>-243410</v>
+        <v>550.4</v>
       </c>
       <c r="T960" t="n">
-        <v>317</v>
+        <v>350</v>
       </c>
       <c r="U960" t="n">
-        <v>-27365.6</v>
+        <v>258.7</v>
       </c>
       <c r="V960" t="n">
+        <v>4665</v>
+      </c>
+      <c r="W960" t="n">
+        <v>14.9</v>
+      </c>
+      <c r="X960" t="n">
+        <v>1558</v>
+      </c>
+      <c r="Y960" t="n">
+        <v>34</v>
+      </c>
+      <c r="Z960" t="n">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" s="1" t="n">
+        <v>44790</v>
+      </c>
+      <c r="B961" t="n">
+        <v>450</v>
+      </c>
+      <c r="C961" t="n">
+        <v>29</v>
+      </c>
+      <c r="D961" t="n">
+        <v>6379706</v>
+      </c>
+      <c r="E961" t="n">
+        <v>0</v>
+      </c>
+      <c r="F961" t="n">
+        <v>1070</v>
+      </c>
+      <c r="G961" t="n">
+        <v>60</v>
+      </c>
+      <c r="H961" t="n">
+        <v>0</v>
+      </c>
+      <c r="I961" t="n">
+        <v>73</v>
+      </c>
+      <c r="J961" t="n">
+        <v>35933</v>
+      </c>
+      <c r="K961" t="n">
+        <v>2528835</v>
+      </c>
+      <c r="L961" t="n">
+        <v>1014125</v>
+      </c>
+      <c r="M961" t="n">
+        <v>0</v>
+      </c>
+      <c r="N961" t="n">
+        <v>-293307</v>
+      </c>
+      <c r="O961" t="n">
+        <v>3670</v>
+      </c>
+      <c r="P961" t="n">
+        <v>-274122</v>
+      </c>
+      <c r="Q961" t="n">
+        <v>1769</v>
+      </c>
+      <c r="R961" t="n">
+        <v>610</v>
+      </c>
+      <c r="S961" t="n">
+        <v>524.3</v>
+      </c>
+      <c r="T961" t="n">
+        <v>264</v>
+      </c>
+      <c r="U961" t="n">
+        <v>252.7</v>
+      </c>
+      <c r="V961" t="n">
+        <v>10</v>
+      </c>
+      <c r="W961" t="n">
+        <v>0</v>
+      </c>
+      <c r="X961" t="n">
+        <v>1559</v>
+      </c>
+      <c r="Y961" t="n">
+        <v>33.7</v>
+      </c>
+      <c r="Z961" t="n">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" s="1" t="n">
+        <v>44791</v>
+      </c>
+      <c r="B962" t="n">
+        <v>314</v>
+      </c>
+      <c r="C962" t="n">
+        <v>0</v>
+      </c>
+      <c r="D962" t="n">
+        <v>6381166</v>
+      </c>
+      <c r="E962" t="n">
+        <v>0</v>
+      </c>
+      <c r="F962" t="n">
+        <v>763</v>
+      </c>
+      <c r="G962" t="n">
+        <v>27</v>
+      </c>
+      <c r="H962" t="n">
+        <v>0</v>
+      </c>
+      <c r="I962" t="n">
+        <v>63</v>
+      </c>
+      <c r="J962" t="n">
+        <v>33017</v>
+      </c>
+      <c r="K962" t="n">
+        <v>2274226</v>
+      </c>
+      <c r="L962" t="n">
+        <v>820910</v>
+      </c>
+      <c r="M962" t="n">
+        <v>0</v>
+      </c>
+      <c r="N962" t="n">
+        <v>-548777</v>
+      </c>
+      <c r="O962" t="n">
+        <v>-251568</v>
+      </c>
+      <c r="P962" t="n">
+        <v>-467666</v>
+      </c>
+      <c r="Q962" t="n">
+        <v>-191707</v>
+      </c>
+      <c r="R962" t="n">
+        <v>-254609</v>
+      </c>
+      <c r="S962" t="n">
+        <v>-35938.3</v>
+      </c>
+      <c r="T962" t="n">
+        <v>-193215</v>
+      </c>
+      <c r="U962" t="n">
+        <v>-27386.7</v>
+      </c>
+      <c r="V962" t="n">
+        <v>-2916</v>
+      </c>
+      <c r="W962" t="n">
+        <v>-8.1</v>
+      </c>
+      <c r="X962" t="n">
+        <v>586.3</v>
+      </c>
+      <c r="Y962" t="n">
+        <v>-409.6</v>
+      </c>
+      <c r="Z962" t="n">
+        <v>-2867</v>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" s="1" t="n">
+        <v>44792</v>
+      </c>
+      <c r="B963" t="n">
+        <v>360</v>
+      </c>
+      <c r="C963" t="n">
+        <v>0</v>
+      </c>
+      <c r="D963" t="n">
+        <v>6382656</v>
+      </c>
+      <c r="E963" t="n">
+        <v>0</v>
+      </c>
+      <c r="F963" t="n">
+        <v>780</v>
+      </c>
+      <c r="G963" t="n">
+        <v>29</v>
+      </c>
+      <c r="H963" t="n">
+        <v>0</v>
+      </c>
+      <c r="I963" t="n">
+        <v>59</v>
+      </c>
+      <c r="J963" t="n">
+        <v>33019</v>
+      </c>
+      <c r="K963" t="n">
+        <v>2274858</v>
+      </c>
+      <c r="L963" t="n">
+        <v>821265</v>
+      </c>
+      <c r="M963" t="n">
+        <v>0</v>
+      </c>
+      <c r="N963" t="n">
+        <v>-246893</v>
+      </c>
+      <c r="O963" t="n">
+        <v>-251771</v>
+      </c>
+      <c r="P963" t="n">
+        <v>-189596</v>
+      </c>
+      <c r="Q963" t="n">
+        <v>-191847</v>
+      </c>
+      <c r="R963" t="n">
+        <v>632</v>
+      </c>
+      <c r="S963" t="n">
+        <v>-35967.3</v>
+      </c>
+      <c r="T963" t="n">
+        <v>355</v>
+      </c>
+      <c r="U963" t="n">
+        <v>-27406.7</v>
+      </c>
+      <c r="V963" t="n">
+        <v>2</v>
+      </c>
+      <c r="W963" t="n">
+        <v>0</v>
+      </c>
+      <c r="X963" t="n">
+        <v>-968</v>
+      </c>
+      <c r="Y963" t="n">
+        <v>-411.1</v>
+      </c>
+      <c r="Z963" t="n">
+        <v>-2878</v>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" s="1" t="n">
+        <v>44793</v>
+      </c>
+      <c r="B964" t="n">
+        <v>67</v>
+      </c>
+      <c r="C964" t="n">
+        <v>0</v>
+      </c>
+      <c r="D964" t="n">
+        <v>6383574</v>
+      </c>
+      <c r="E964" t="n">
+        <v>0</v>
+      </c>
+      <c r="F964" t="n">
+        <v>295</v>
+      </c>
+      <c r="G964" t="n">
+        <v>25</v>
+      </c>
+      <c r="H964" t="n">
+        <v>0</v>
+      </c>
+      <c r="I964" t="n">
+        <v>10</v>
+      </c>
+      <c r="J964" t="n">
+        <v>11631</v>
+      </c>
+      <c r="K964" t="n">
+        <v>1453663</v>
+      </c>
+      <c r="L964" t="n">
+        <v>0</v>
+      </c>
+      <c r="M964" t="n">
+        <v>0</v>
+      </c>
+      <c r="N964" t="n">
+        <v>-1068455</v>
+      </c>
+      <c r="O964" t="n">
+        <v>-1073195</v>
+      </c>
+      <c r="P964" t="n">
+        <v>-1011059</v>
+      </c>
+      <c r="Q964" t="n">
+        <v>-1013251</v>
+      </c>
+      <c r="R964" t="n">
+        <v>-821195</v>
+      </c>
+      <c r="S964" t="n">
+        <v>-153313.6</v>
+      </c>
+      <c r="T964" t="n">
+        <v>-821265</v>
+      </c>
+      <c r="U964" t="n">
+        <v>-144750.1</v>
+      </c>
+      <c r="V964" t="n">
+        <v>-21388</v>
+      </c>
+      <c r="W964" t="n">
+        <v>-64.8</v>
+      </c>
+      <c r="X964" t="n">
+        <v>-8100.7</v>
+      </c>
+      <c r="Y964" t="n">
+        <v>-2802.6</v>
+      </c>
+      <c r="Z964" t="n">
+        <v>-19618</v>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" s="1" t="n">
+        <v>44794</v>
+      </c>
+      <c r="B965" t="n">
+        <v>76</v>
+      </c>
+      <c r="C965" t="n">
+        <v>0</v>
+      </c>
+      <c r="D965" t="n">
+        <v>6384546</v>
+      </c>
+      <c r="E965" t="n">
+        <v>0</v>
+      </c>
+      <c r="F965" t="n">
+        <v>316</v>
+      </c>
+      <c r="G965" t="n">
+        <v>25</v>
+      </c>
+      <c r="H965" t="n">
+        <v>0</v>
+      </c>
+      <c r="I965" t="n">
+        <v>18</v>
+      </c>
+      <c r="J965" t="n">
+        <v>11631</v>
+      </c>
+      <c r="K965" t="n">
+        <v>1453898</v>
+      </c>
+      <c r="L965" t="n">
+        <v>0</v>
+      </c>
+      <c r="M965" t="n">
+        <v>0</v>
+      </c>
+      <c r="N965" t="n">
+        <v>-1068784</v>
+      </c>
+      <c r="O965" t="n">
+        <v>-1073171</v>
+      </c>
+      <c r="P965" t="n">
+        <v>-1011258</v>
+      </c>
+      <c r="Q965" t="n">
+        <v>-1013371</v>
+      </c>
+      <c r="R965" t="n">
+        <v>235</v>
+      </c>
+      <c r="S965" t="n">
+        <v>-153310.1</v>
+      </c>
+      <c r="T965" t="n">
+        <v>0</v>
+      </c>
+      <c r="U965" t="n">
+        <v>-144767.3</v>
+      </c>
+      <c r="V965" t="n">
+        <v>0</v>
+      </c>
+      <c r="W965" t="n">
+        <v>0</v>
+      </c>
+      <c r="X965" t="n">
+        <v>-7128.7</v>
+      </c>
+      <c r="Y965" t="n">
+        <v>-2803.6</v>
+      </c>
+      <c r="Z965" t="n">
+        <v>-19625</v>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" s="1" t="n">
+        <v>44795</v>
+      </c>
+      <c r="B966" t="n">
+        <v>0</v>
+      </c>
+      <c r="C966" t="n">
+        <v>0</v>
+      </c>
+      <c r="D966" t="n">
+        <v>0</v>
+      </c>
+      <c r="E966" t="n">
+        <v>0</v>
+      </c>
+      <c r="F966" t="n">
+        <v>322</v>
+      </c>
+      <c r="G966" t="n">
+        <v>0</v>
+      </c>
+      <c r="H966" t="n">
+        <v>0</v>
+      </c>
+      <c r="I966" t="n">
+        <v>22</v>
+      </c>
+      <c r="J966" t="n">
         <v>4658</v>
       </c>
-      <c r="W960" t="n">
-        <v>28.1</v>
-      </c>
-      <c r="X960" t="n">
-        <v>-2033.3</v>
-      </c>
-      <c r="Y960" t="n">
-        <v>-2060.6</v>
-      </c>
-      <c r="Z960" t="n">
-        <v>-14424</v>
+      <c r="K966" t="n">
+        <v>0</v>
+      </c>
+      <c r="L966" t="n">
+        <v>0</v>
+      </c>
+      <c r="M966" t="n">
+        <v>0</v>
+      </c>
+      <c r="N966" t="n">
+        <v>-2523458</v>
+      </c>
+      <c r="O966" t="n">
+        <v>-2527522</v>
+      </c>
+      <c r="P966" t="n">
+        <v>-1011580</v>
+      </c>
+      <c r="Q966" t="n">
+        <v>-1013511</v>
+      </c>
+      <c r="R966" t="n">
+        <v>-1453898</v>
+      </c>
+      <c r="S966" t="n">
+        <v>-361074.6</v>
+      </c>
+      <c r="T966" t="n">
+        <v>0</v>
+      </c>
+      <c r="U966" t="n">
+        <v>-144787.3</v>
+      </c>
+      <c r="V966" t="n">
+        <v>-6973</v>
+      </c>
+      <c r="W966" t="n">
+        <v>-60</v>
+      </c>
+      <c r="X966" t="n">
+        <v>-9453.7</v>
+      </c>
+      <c r="Y966" t="n">
+        <v>-3800</v>
+      </c>
+      <c r="Z966" t="n">
+        <v>-26600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>